<commit_message>
Finish the 3 routes at the same docking station.
& adjust to make them nearly the same length/time.
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Desktop/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5DBF2E7-F542-744D-AE62-4CABED1D408A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C861E7-4C08-514B-A983-8C22693249A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="28060" windowHeight="17500" xr2:uid="{211AF0F6-F836-F343-9553-311F059F951A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -83,9 +83,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>Walk bikes through Little Turnstile (70m)</t>
-  </si>
-  <si>
     <t>desc</t>
   </si>
   <si>
@@ -146,27 +143,6 @@
     <t>Walk through Tachbrook Street Market and from Howick Place to Ashley Place.</t>
   </si>
   <si>
-    <t>MultiLineString ((532425.86516154767014086 177642.33997085387818515, 532411.25822669372428209 177649.51064796402351931, 532407.54009782173670828 177671.5538405618572142, 532404.75150116789154708 177727.19298332382459193, 532429.18491946905851364 177794.11930301843676716, 532358.00930963514838368 177800.49323822744190693, 532344.59748763276729733 177875.45337209175340831, 532340.61377812712453306 177908.3853706716618035, 532327.99869802594184875 177961.36870709658251144, 532247.2621853785822168 177940.65341766728670336, 532213.93181584810372442 177940.5206273504300043, 532181.53097853565122932 177966.54752945387735963, 532131.07065813092049211 178059.50075125196599402, 531992.96872860239818692 177958.58011044265003875, 531978.40126691607292742 177969.69867078488459811, 531975.51999578601680696 177976.24701426242245361, 531956.66076657059602439 177991.70110486945486628, 531930.72932639950886369 178011.6080690412200056, 531893.66570231656078249 178019.07318060554098338, 531849.13696666923351586 178060.9825788619054947, 531859.09044875507242978 178130.13308598485309631, 531859.16702702990733087 178134.34492127480916679, 531819.8686971872812137 178155.9232769338414073, 531807.15032861998770386 178147.34909587725996971, 531804.22081675904337317 178166.85535778096527793, 531594.50186685402877629 178293.37287628170452081, 531621.63150816119741648 178357.4752960842452012, 531633.50392294430639595 178379.59179671431775205, 531588.61539335269480944 178402.98467423874535598, 531470.04583553783595562 178481.04854062185040675, 531567.95477312488947064 178566.74453142564743757, 531600.88228947878815234 178584.2162747971015051, 531772.37417057063430548 178639.05066937819356099, 531797.10340734256897122 178657.86639300896786153, 531837.96040722646284848 178713.77597179752774537, 531857.31372296100016683 178741.19316908807377331, 531868.06556503567844629 178749.79464274787460454, 531880.13844949356280267 178747.46484413990401663, 531893.87027424620464444 178732.70546787517378107, 531882.84744893456809223 178737.65639788802945986, 531874.82179012312553823 178745.74090769540634938, 531873.81108064437285066 178750.26503583858720958, 531928.47747769311536103 178812.55852085907827131, 531938.12053605390246958 178829.1566770619538147, 531932.74461501650512218 178852.9451276523177512, 531965.13453926669899374 178839.37092703295638785, 531981.7662949759978801 178846.35962438152637333, 532009.72108437039423734 178845.01564412217703648, 531981.39670040470082313 178850.0555700947297737, 531960.96820046263746917 178846.83001747232628986, 531933.5510031720623374 178860.26982006573234685, 531935.16377948329318315 178924.24328041044645943, 531930.32545054971706122 179009.45162885275203735, 531910.43454271147493273 179022.35383934245328419, 531885.70530593954026699 179057.83491818906622939, 531876.11210935655981302 179066.35873417466063984, 531831.93818780174478889 179086.51181359370821156, 531779.46893305156845599 179106.20686848048353568, 531672.18940927542280406 179157.81096578075084835, 531589.70353428379166871 179198.03799872964737006, 531556.67969205614645034 179124.41894058702746406, 531620.5699304185109213 179098.98690395732410252, 531635.7671230387641117 179139.9262799954158254, 531648.27035036904271692 179178.57474457612261176, 531695.00515957863535732 179157.60464692092500627, 531797.07743173581548035 179112.31386224390007555, 531810.86905931774526834 179106.1050852510088589, 531847.91815481544472277 179173.68914956544176675, 531891.07424407650250942 179215.21670715624350123, 531905.47685013443697244 179238.60377113270806149, 531919.96244928787928075 179292.40742513118311763, 531957.96748593868687749 179272.83832924981834367, 531967.94273236184380949 179364.63301262669847347, 531985.87575963942799717 179480.30103856680216268, 531979.93544435373041779 179495.99243743464467116, 531952.58757775544654578 179485.23262106810580008, 531939.54275271145161241 179490.46462862013140693, 531766.64450117154046893 179467.29959379057982005, 531761.71291867026593536 179464.16131401702295989, 531729.43346957070752978 179458.33308015181683004, 531718.67365320411045104 179473.57615333772264421, 531714.63872206665109843 179523.78862971480702981, 531716.09578053292352706 179527.48731659070472233, 531741.86680176388472319 179544.99216120038181543, 531751.2878118836088106 179549.55071448421222158, 531794.563677724217996 179583.10166665274300613, 531736.03185356059111655 179657.43647553340997547, 531711.23332369688432664 179690.98742770194076002, 531710.01770948793273419 179697.49096372016356327, 531768.36719152017030865 179689.71103278253576718, 531817.90347053715959191 179690.92664699154556729, 531827.62838420912157744 179689.71103278253576718, 531830.54585831076838076 179679.74299626867286861, 531848.91713031963445246 179689.19716539108776487, 531944.69973392877727747 179685.07748351542977616, 532042.54217847576364875 179713.40029641060391441, 532046.66186035145074129 179723.69950109976343811, 531964.78318307269364595 179783.43488829687703401, 531949.33437603886704892 179795.79393392385100015, 531887.02418766950722784 179851.66711936253705062, 531879.29978415265213698 179893.89385858806781471, 531869.00057946355082095 179984.52685985263087787, 531866.29703823267482221 180017.74179497518343851, 532058.37720568536315113 180022.37643708530231379, 532075.37089342251420021 180021.86147685084142722, 532105.01448292518034577 180034.50729168066754937, 532262.32514954556245357 180048.1606702930002939, 532325.92739683925174177 180055.68131635268218815, 532405.1537294692825526 180033.52798163625993766, 532464.76121906656771898 180011.84399723159731366, 532540.23274920228868723 179984.43393902308889665, 532591.95515356154646724 180078.2101313185703475, 532591.20419306261464953 180094.73126229355693795, 532607.72532403760123998 180147.29849721392383799, 532534.50667539855930954 180136.78505022986792028, 532536.55852291593328118 180144.94319960565189831, 532612.86246818082872778 180163.34207012850674801, 532665.91098826692905277 180179.77963973267469555, 532720.82741398992948234 180243.84880307616549544, 532752.20822868880350143 180305.86327021915349178, 532785.08336789719760418 180312.58773051179014146, 532914.34243796626105905 180285.68988934133085422, 532886.6974345410708338 180313.33489276652107947, 532846.35067278542555869 180329.77246237068902701, 532662.54875812062527984 180367.13057510743965395, 532637.89240371435880661 180305.86327021915349178, 532548.96951092616654932 180316.77607292827451602, 532545.8441308259498328 180272.49985484205535613, 532572.40986167767550796 180230.30722348930430599, 532516.1530198740074411 180204.2623893209383823, 532468.75142168754246086 180244.89233062358107418, 532463.02155817055609077 180284.4804785595042631, 532459.3752813870087266 180373.55381141533143818, 532372.69448957266286016 180390.68838654135470279, 532277.44368469482287765 180400.13795320072676986, 532203.73706475202925503 180422.18694207252701744, 532202.47712253080680966 180432.26647984248120338, 532156.80421701062005013 180436.991263172152685, 532083.72756817832123488 180361.39472989740897901, 532038.73218060249928385 180353.29513465752825141, 531941.74603957985527813 180343.19241163434344344, 531920.30576653964817524 180317.62579917337279767, 531909.74514889775309712 180270.76305838747066446, 531907.76503308990504593 180261.52251795082702301, 531948.6874264522921294 180252.28197751415427774, 531995.60517045494634658 180231.05073579659801908, 532076.78991857706569135 180211.68960345312370919, 532106.05162995983846486 180200.24893434107070789, 532099.67125680122990161 180191.66843250702368096, 531974.81395447254180908 180230.50070362773840316, 531904.40983685990795493 180254.70211905709584244, 531741.12336655741091818 180332.22967136604711413, 531739.7332929449621588 180345.2238377439789474, 531706.95472862606402487 180347.60832770192064345, 531644.49292385333683342 180395.90728139248676598, 531648.12442413077224046 180495.13802647482953034, 531518.84301425225567073 180495.13802647482953034, 531488.34336362790782005 180484.8074996504583396))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((531488.34336362790782005 180484.8074996504583396, 531473.81241081142798066 180479.88572530940291472, 531430.96070753701496869 180458.09672364447033033, 531451.29710909095592797 180386.19301815022481605, 531525.37971475173253566 180400.71901926017017104, 531538.45311575068626553 180381.83521781724994071, 531549.34761658310890198 180218.41770533029921353, 531569.5024431231431663 180215.87565513607114553, 531626.15384745202027261 180269.62185924287769012, 531643.585048783919774 180270.34815929835895076, 531647.21654906147159636 180203.52855419259867631, 531643.83931215479969978 180060.99850968600367196, 531625.11130755802150816 180053.36858188730548136, 531633.66547321295365691 180050.08258383703650907, 531634.2177775400923565 180047.32106220131390728, 531614.51892320532351732 180053.39640979986870661, 531602.36822800827212632 180051.73949681845260784, 531601.26361935399472713 180045.84825066229677759, 531592.78442665631882846 180051.56285102886613458, 531593.45052950282115489 180089.86376470435061492, 531513.85123934247530997 180096.19174174638465047, 531519.18006211472675204 180125.33374128208379261, 531513.35166220751125365 180149.81302089206292294, 531336.20963958697393537 180096.6219828424800653, 531238.11603961104992777 180067.39065219060285017, 531199.89045337401330471 180177.0081421350769233, 531177.40481441095471382 180218.60657421653741039, 531061.32270326465368271 180145.94985331749194302, 531060.76056229067035019 180124.58849630266195163, 531057.63696220016572624 180100.43033974233549088, 531037.72401162306778133 180082.46963922184659168, 530999.45991051418241113 180089.88818943683872931, 530975.4472348183626309 180111.55816506480914541, 530987.4871511091478169 180150.16886052410700358, 531011.03398508415557444 180159.51833872005227022, 531014.84303175657987595 180179.2561260225775186, 530958.39988561067730188 180262.36259887542109936, 530929.3741334832739085 180271.64266970381140709, 530943.43033389060292393 180263.83366947752074338, 530923.9078333250945434 180242.84698136936640367, 530866.90213167306501418 180188.57442979663028382, 530842.303780960268341 180151.09122871042927727, 530840.0206066551618278 180145.71054415201069787, 530822.22424072585999966 180117.54081000993028283, 530812.51550312107428908 180086.5150615772290621, 530820.11364559445064515 180120.49564319400815293, 530836.57628762000240386 180149.4107964952418115, 530859.76145922881551087 180140.51328725425992161, 530887.37670600018464029 180127.04054134621401317, 530942.97500607429537922 180058.23076402678270824, 531005.72952298959717155 180026.85350556910270825, 531037.65725966589525342 180016.94489763511228375, 531078.94312605750747025 180004.28389860835159197, 531103.36682528315577656 179997.4820276228711009, 531123.39294299448374659 179985.6610553627833724, 531156.49166532268282026 179963.68795398517977446, 531181.76768542011268437 179933.82261524567729793, 531212.01546737970784307 179888.97245578825823031, 531103.54066311055794358 179763.39200930739752948, 531108.54719253838993609 179756.71663673696457408, 531135.1701887323288247 179781.81394092956907116, 531167.34841385786421597 179808.82066558845690452, 531194.06783293525222689 179811.40641582175157964, 531236.87636457534972578 179792.73155302571831271, 531253.82739388255868107 179784.97430232583428733, 531249.51781016041059047 179751.07224371147458442, 531230.84294736431911588 179747.62457673373864964, 531216.47766829049214721 179768.31057860012515448, 531178.84063711692579091 179737.85618696350138634, 531127.12563245091587305 179702.51760044175898656, 531045.96180568356066942 179636.29366391123039648, 531013.78358055802527815 179596.07088250436936505, 530972.86260063934605569 179563.04264083271846175, 530945.78228133858647197 179595.62788598841871135, 530882.00223331130109727 179643.29507977730827406, 530842.39146664168220013 179630.53907017182791606, 530826.94998132972978055 179588.91419672238407657, 530809.49438923806883395 179516.40635264918091707, 530801.43796211876906455 179441.21303286953479983, 530771.22636042162775993 179379.44709162198705599, 530816.2080785040743649 179456.65451818142901175, 530938.3972231459338218 179398.91679049350204878, 530945.11091241205576807 179382.80393625498982146, 531051.18720281543210149 179331.77989783309749328, 531117.65272654918953776 179413.01553795216022991, 531106.23945479700341821 179449.94082891539437696, 531128.01335033809300512 179490.33879105054074898, 531145.9327949439175427 179489.53642785921692848, 531118.11753764539025724 179461.98862495779758319, 531170.3957165403990075 179433.66088251979090273, 531266.22342408250551671 179404.70195991088985465, 531313.87248040549457073 179407.3990763065230567, 531433.52216941397637129 179415.3352683637640439, 531469.58935155137442052 179427.35766240957309492, 531466.38337980583310127 179436.3744579438935034, 531357.78108692553360015 179511.91516719831270166, 531327.52472857688553631 179431.76587355969240889, 531318.50793304259423167 179389.48712116529350169, 531315.08669927902519703 179378.57198898226488382, 531298.67588855815120041 179338.66640459033078514, 531270.20679607603233308 179239.75740465606213547, 531274.79732766340021044 179226.52587243364541791, 531198.10844702739268541 179192.5019324331660755, 531219.62179134623147547 179127.21737543260678649, 531235.3105901419185102 179110.29808261376456358, 531240.33914468786679208 179077.35684370002127253, 531245.46363338397350162 178841.6303636806551367, 531233.0184465505881235 178844.00959057526779361, 531233.75051636435091496 178886.46963977129780687, 531226.42981822707224637 179085.22659419756382704, 531181.16885312169324607 179183.82010049920063466, 530988.59653849294409156 179108.14471807319205254, 530973.83061021461617202 179097.68551887612557039, 530832.78523280692752451 179038.00655875154188834, 530746.65065118379425257 179009.70519621824496426, 530660.53985221788752824 178980.90664574180846103, 530629.06085022771731019 178958.21248151632607915, 530637.84568799240514636 178901.11103604579693638, 530747.65616005111951381 178890.12998883993714117, 530829.64797918824478984 178865.23961517328280024, 530854.35533540148753673 178855.90572504830197431, 530871.92501093086320907 178861.03021374437958002, 530891.65204298356547952 178844.1667831186496187, 530965.44759355159476399 178788.4324741373420693, 530886.32739482226315886 178835.18531884101685137, 530876.4373699810821563 178823.49710766511270776, 530792.12940123490989208 178700.15787217835895717, 530743.08072371536400169 178626.95089080586330965, 530828.00082210742402822 178569.11737552162958309, 530830.19703154859598726 178562.52874719808460213, 530868.26466186228208244 178541.84777496033348143, 530837.15169477893505245 178458.75785110259312205, 530903.77004782785661519 178437.16179159769671969, 530958.67528385727200657 178408.9771037692844402, 530969.51906797324772924 178398.22482838027644902, 531033.78183673555031419 178376.20990525075467303, 531215.27667861443478614 178352.53666500566760078, 531252.47748471389058977 178318.71775036983308382, 531315.60612536745611578 178272.49856703419936821, 531294.18747943139169365 178255.58910971626755781, 531295.31477658601943403 178201.47884629893815145, 531322.36990829464048147 178189.07857759913895279, 531270.5142391863046214 178118.05885686387773603, 531219.78586723259650171 178146.24128572706831619, 531171.31208958791103214 178190.20587475365027785, 531094.65588307997677475 178130.45912556367693469, 530872.93878867325838655 178114.04592761132516898, 530864.83308461052365601 178128.09106711560161784, 530878.95511248987168074 178084.87972859182627872, 530943.32097328128293157 177890.14320068835513666, 530878.53382568154484034 177871.54188188168336637, 530847.7604888214264065 177818.14109144799294882, 530864.0522553944028914 177757.49951587078976445, 530876.72362939559388906 177733.06186601129593328, 530833.27891853428445756 177695.04774400766473264, 530829.65852596261538565 177662.46421086171176285, 530830.56362410553265363 177651.60303314638440497, 530804.31577796011697501 177646.17244428873527795, 530835.99421296315267682 177652.50813128933077678, 530839.61460553493816406 177696.85794029355747625, 530881.2149192038923502 177736.88257737495587207, 530903.80695161537732929 177711.30042302669608034, 530946.30642832547891885 177686.18709587972261943, 531019.71461537026334554 177674.59632950421655551, 531093.94195289048366249 177671.7781124759640079, 531118.76178659219294786 177709.00786302858614363, 531122.30747712100856006 177752.44257200666470453, 531115.21609606337733567 177786.12663203047122806, 531278.31786038912832737 177901.36157421718235128, 531294.66580769827123731 177906.02167873742291704, 531318.86828601313754916 177883.92376375428284518, 531341.04136397247202694 177863.066037877346389, 531340.89103802025783807 177853.74582883683615364, 531236.94064202811568975 177673.88082695021876134, 531241.75107250059954822 177597.21459129443974234, 531264.60061724507249892 177546.70507133298087865, 531288.65276960772462189 177480.86230424034874886, 531271.81626295391470194 177391.86934049872797914, 531241.75107250059954822 177314.90245293837506324))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((531236.84324939036741853 177318.54342519459896721, 531202.52396391110960394 177191.43496045682695694, 531023.30102863081265241 177159.65784427238395438, 530944.49378049338702112 177143.13374385648057796, 530915.25883360370062292 177148.21808244596468285, 530890.0134778693318367 177105.24807653366588056, 530798.05788532528094947 176955.03413150229607709, 530778.53778894036076963 176970.21642869058996439, 530846.85812628781422973 177061.31021182052791119, 530925.4432389655848965 177024.38350523461122066, 531189.53587636584416032 177001.13818751723738387, 531180.75431189488153905 176810.13916027281084098, 531181.01259320287499577 176679.19053713156608865, 531207.87384923174977303 176244.24481450865278021, 531207.48642726987600327 176156.30002914459328167, 531185.2742347844177857 176156.30002914459328167, 531209.55267773370724171 176148.55158990548807196, 531188.94265151466242969 175949.80426446883939207, 531154.94696310814470053 175823.53456467346404679, 531066.20655180979520082 175503.10660128630115651, 530998.72868066909722984 175231.84770217089680955, 531029.01404346199706197 175153.91027290970669128, 531021.65302618476562202 175139.83394162519834936, 531029.40146542387083173 175082.75377256359206513, 531032.75912242755293846 175056.73193078552139923, 531026.30208972818218172 175037.10255137970671058, 530966.8973888949258253 175050.27489808623795398, 530928.21976302622351795 175062.67240086884703487, 531062.91346513316966593 175558.95993413514224812, 530985.17079143389128149 175576.00650046131340787, 530873.33498508238699287 175582.33439250665833242, 530875.38815978192724288 175595.23469414943247102, 530797.41443990776315331 175600.27078763680765405, 530684.78446298860944808 175838.26282582237035967, 530601.53621917893178761 175966.56306039975606836, 530646.58820994652342051 176020.4295711001905147, 530665.19664091581944376 176035.12043765484122559, 530699.47532954334747046 176074.2960818005958572, 530719.25994543684646487 176118.95408105937531218, 530745.12009748979471624 176148.40592089734855108, 530716.86548691359348595 176127.43046423231135122, 530670.8918832641793415 176208.65049734638887458, 530598.10034415242262185 176165.74180060689104721, 530560.55523450532928109 176215.54653789382427931, 530483.93256175622809678 176177.23520151924458332, 530387.97902395331766456 176303.5319877928995993, 530379.94736301514785737 176309.76833628604072146, 530341.93712524976581335 176251.15764247826882638, 530303.51330139499623328 176202.36548520234646276, 530182.75271213706582785 176293.85078009468270466, 530305.95290925877634436 176211.51401469158008695, 530417.23728811659384519 176386.02025389933260158, 530494.13386454083956778 176495.22892708366271108, 530475.49227025615982711 176509.52081603524857201, 530501.92500291229225695 176509.08523381545091979, 530512.77645926724653691 176528.58107065639342181, 530498.98223508731462061 176613.64545309916138649, 530462.28959876869339496 176757.56519204287906177, 530434.33330443082377315 176909.11773503280710429, 530402.8200269922381267 177194.41969347806298174, 530347.79517984646372497 177352.39425463852239773, 530312.29527846199925989 177448.2439883763436228, 530321.17025380814447999 177524.56877635276759975, 530299.1076171655440703 177512.2877638345817104, 530112.49448222981300205 177489.69982631949824281, 530086.75473947997670621 177355.87942906434182078, 530025.81983827648218721 177182.92411681212252006, 530186.56190524436533451 177134.07113567480701022, 530174.47998517821542919 177096.77477373127476312, 530096.4836231010267511 176769.19463073462247849, 529884.42970881413202733 176831.87007454806007445, 529743.07660154439508915 176608.87987858781707473, 529771.98973712243605405 176569.9510816659021657, 529802.22569589677732438 176526.86484041254152544, 529830.94985673227347434 176534.42383010612684302, 529799.95799898868426681 176524.5971435044775717, 529740.99787937884684652 176599.43114147079177201, 529698.59198002424091101 176544.13718110171612352, 529597.32066152559127659 176436.11156106233829632, 529515.85195648483932018 176518.75130591302877292, 529470.99966809689067304 176555.56964268209412694, 529518.67451752966735512 176525.99916645159828477, 529605.23845730861648917 176434.94747649942291901, 529505.5353504242375493 176347.90575941736460663, 529255.71074105193838477 176177.45054182736203074, 529165.48091607249807566 176110.54161229194141924))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((529164.61925642273854464 176109.67995264215278439, 529001.12134455901104957 175987.36767307508853264, 528997.60493395722005516 175985.00944533024448901, 528925.98516327538527548 176086.5956472598190885, 528836.08586953231133521 176038.64935726355179213, 528804.92078103474341333 175988.30575276748277247, 528764.76576316286809742 175973.92186576858512126, 528736.1864626327296719 176029.69451619402389042, 528753.60289678350090981 176038.27722640830324963, 528557.00358154252171516 175913.29103869749815203, 528554.72205805755220354 175880.40056722576264292, 528529.4405931425280869 175873.17729153577238321, 528524.62507601594552398 175887.02190327495918609, 528445.1690434260526672 175861.74043835999327712, 528400.62551000446546823 175832.84733560003223829, 528350.06258017453365028 175846.09000769836711697, 528240.50956554315052927 176160.30250021276879124, 528416.27594066609162837 176261.42835987257421948, 528433.8382980921305716 176249.8060543195460923, 528444.64069186616688967 176225.97724452381953597, 528425.57764402963221073 176249.48833685560384765, 528405.06003338482696563 176243.23115157571737655, 528298.35011839854996651 176189.29952098953071982, 528242.99004875461105257 176148.69032720808172598, 528155.720433603040874 176103.8961748254369013, 528011.98040374473202974 176080.87730883390759118, 528002.26132699276786298 176073.71588385876384564, 528007.81933374144136906 176031.80425242587807588, 528024.69687239604536444 176034.07766336353961378, 528007.59572685486637056 176028.48092482279753312, 528028.97791927156504244 175838.52871152572333813, 528071.95822007348760962 175635.10030053602531552, 528066.13247264770325273 175627.8668870801338926, 527986.25385233573615551 175601.30841606299509294, 527783.6197062972933054 175545.97057698419666849, 527730.72324247192591429 175535.3912842191348318, 527705.49569818598683923 175645.25317062556860037, 527652.00888393050990999 175633.26453688892070204, 527667.81058392324484885 175521.98211052999249659, 527493.51585617032833397 175475.42110760780633427, 527372.37483971798792481 175449.05027409436297603, 527388.85661066381726414 175307.30704395961947739, 527363.30986569775268435 175304.0106897704245057, 527347.65218329906929284 175302.36251267584157176, 527392.9859605492092669 175304.87285213259747252, 527397.12063730170484632 175242.85270084580406547, 527416.99002535012550652 175173.88838360883528367, 527443.43270875024609268 175068.11765000826562755, 527450.48409099027048796 175080.4575689283083193, 527439.50107401434797794 175130.92109447572147474, 527503.88389773119706661 175132.10243069072021171, 527497.49056007748004049 175161.73309173848247156, 527475.35977589245885611 175220.01082342577865347, 527552.57162293803412467 175256.15777092802454717, 527519.86724186455830932 175235.87121875837328844, 527544.948797274264507 175170.46245661145076156, 527552.32572533597704023 175142.92192518117371947, 527701.83146738610230386 175159.64296212099725381, 527840.27181734365876764 175177.83938467313419096, 527917.36071558820549399 175188.16708395950263366, 527968.50741681596264243 175201.44555447052698582, 528779.72360599890816957 175221.85505544117768295, 529261.51673463499173522 175222.65933442555251531, 529351.25411826185882092 175215.8378031077736523, 529372.18678662180900574 175227.73136467591393739, 529365.05064968089573085 175241.05215363221941516, 529360.76896751637104899 175246.28532072220696136, 529382.68670980352908373 175224.25992501174914651, 529468.12816032278351486 175328.11548124635010026, 529698.30448176467325538 175447.99130945329670794, 529895.33541291893925518 175576.70590840361546725, 529955.73367966525256634 175634.15791823549079709, 529931.4270601209718734 175659.2011020083737094, 529925.47286403307225555 175678.95786343273357488, 529921.73475975845940411 175812.78199646400753409, 529619.1352187282172963 176067.34689756546868011, 529430.02734231401700526 175986.28361064163618721, 529289.88080719718709588 175972.14038232708116993, 529264.1658466252265498 175952.85416189813986421, 529130.44805165135767311 175948.99691781235742383, 529054.58891796413809061 175905.28148484011762775, 529001.12134455901104957 175987.36767307508853264, 528831.19019799574743956 176248.25477146793855354, 528752.75956825143657625 176391.9371136634144932, 528675.49066539527848363 176408.16534021744155325, 528705.96678335568867624 176534.67820903472602367, 528716.35159020742867142 176527.29953048215247691, 528719.63100289751309901 176506.25663238778361119, 528747.77929515356663615 176407.32768290513195097, 528744.77316685440018773 176389.5641975007893052, 528668.2535374202998355 176407.60096729596261866, 528714.38658874668180943 176593.66351471430971287, 528668.75400357856415212 176604.88464221468893811, 528606.66376474313437939 176705.1267145512974821, 528552.80235274136066437 176674.4556327169702854, 528522.08681564137805253 176737.87589794580708258, 528508.67160317418165505 176757.9432818841887638, 528487.60639351513236761 176746.19111228492693044, 528469.86726959166117013 176755.72589139378396794, 528197.11153506592381746 176662.46467340260278434, 528176.00199985504150391 176658.75310677211382426, 528137.95844189240597188 176788.65793883957667276, 527957.94746031321119517 176731.12865606683772057, 527939.38962716073729098 176738.55178932784474455))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((527940.77566473442129791 176739.55987936040037312, 527892.90263102832250297 176721.44575849862303585, 527636.93444367230404168 176695.61776634884881787, 527711.9710393245331943 176478.3039893300156109, 527834.02353440679144114 176550.01674702038872056, 527855.60682320327032357 176496.67211271909764037, 527890.17659236572217196 176414.29315516981296241, 527929.95724563486874104 176377.71143682854017243, 528044.29808945208787918 176288.20219040603842586, 528076.05943495687097311 176244.31378570853848942, 528028.70615620422177017 176220.05966732307570055, 527961.14111213048454374 176203.89025506612961181, 527797.13707352406345308 176203.89025506612961181, 527683.08496921148616821 176217.74975128637743182, 527584.33605864213313907 176217.1722722772101406, 527518.79219110053963959 176395.61328611301723868, 527483.2068727093283087 176504.61552287041558884, 527473.46186028700321913 176591.34613342949887738, 527389.6547534546116367 176724.85280361596960574, 527365.42176395864225924 176779.05610696220537648, 527516.26628560293465853 176817.18143791682086885, 527480.72110768430866301 176938.649287985637784, 527537.79039941774681211 176962.5634430730715394, 527483.56923695211298764 176947.51469569859909825, 527472.50587809423450381 177038.787406276416732, 527388.83922673121560365 177163.25019342801533639, 527190.55077449802774936 177069.79876631233491935, 527159.65929454017896205 177000.74722287710756063, 527099.77578929206356406 176863.97566198912682012, 526993.89284357777796686 176974.11520853615365922, 526965.6928630608599633 177009.76424051032518037, 526918.33817879669368267 176978.37180936889490113, 526881.62499661440961063 176915.05487198193441145, 526809.33459098706953228 176814.57045149418991059, 526803.78523573139682412 176782.81458185013616458, 526837.9906987837748602 176724.64684572990518063, 526829.14218303072266281 176698.07787916850065812, 526713.59169160143937916 176585.58887918625259772, 526702.01159683079458773 176498.87495989364106208, 526728.35331819928251207 176459.47930909239221364, 526759.08459305611904711 176456.02855037362314761, 526877.73335154261440039 176444.22870948346098885, 526952.37421362893655896 176459.79166246333625168, 526957.30744241294451058 176431.45683538325829431, 527038.82798124512191862 176435.9939717588131316, 527098.5913686784915626 176454.87681948934914544, 527051.24293423152994365 176594.92815045249881223, 527174.99744662863668054 176650.61612686808803119, 527153.14015064027626067 176640.28990523278480396, 527205.55905537132639438 176487.71942607063101605, 527102.71056710940320045 176449.37945362422033213, 527080.02346470882184803 176442.65865531019517221, 527118.21201132400892675 176315.62328595775761642, 527136.13724749034736305 176310.16777929847012274, 527123.4023648789152503 176243.66339232763857581, 527158.08696234272792935 176237.9932378021767363, 527169.22996887960471213 176208.6499966005794704, 527150.43826302816160023 176186.18838753091404215, 527118.65549396350979805 176157.02174997527617961, 527093.6976608419790864 176147.4813768335734494, 527018.22708262107335031 176131.11693114246008918, 526849.86647974920924753 176114.85084184003062546, 526845.07710992521606386 176097.65762165782507509, 526857.65365130186546594 176044.64240146498195827, 526893.8380195926874876 176044.15844629961065948, 526858.37810308812186122 176039.0902959554514382, 526874.83542804175522178 175886.27227852959185839, 527054.69047931989189237 175862.7618143102445174, 527176.94489326048642397 175856.8841982554004062, 527195.27535622008144855 175822.70450227480614558, 527223.9658216992393136 175795.75699128504493274, 527224.12844125344417989 175773.97201046324335039, 527243.25712752784602344 175756.61424477020045742, 527267.78618826356250793 175718.31265972839901224, 527222.48707379773259163 175682.39379150536842644, 527195.04935412993654609 175648.09664192068157718, 527009.0825874931178987 175569.97535675560357049, 526824.66230209683999419 175469.42516340431757271, 526795.48152648622635752 175473.6317607709497679, 526758.33231608534697443 175456.72367672127438709, 526790.20567167596891522 175381.68114836351014674, 526851.47655176091939211 175305.71711282295291312, 526851.47655176091939211 175278.90286315878620371, 526865.43143400084227324 175215.89678796651423909, 526877.77642672799993306 175178.34743508807150647, 526907.09578445507213473 175139.25495811874861829, 526889.09267006127629429 175116.10809675537166186, 526973.96449506049975753 174912.93009145429823548, 526885.95633615972474217 174859.8365453231963329, 526909.64957838621921837 174789.88203135458752513, 526922.28532687691040337 174784.41939029871718958, 526957.33885194035246968 174894.75840272463392466, 526938.1368365534581244 174894.58398754562949762, 526918.67389838397502899 174882.02661713416455314, 526881.00047726207412779 174863.13230195376672782, 526645.98297396756242961 174831.60109246335923672, 526609.50912189844530076 174827.05741743353428319, 526567.45242367009632289 174822.48189269431168213, 526532.3543359829345718 174820.95671778128598817, 526511.19253406394273043 174818.36392042905208655, 526475.19840611529070884 174928.17651417059823871, 526482.59550444374326617 174953.18938274509855546, 526621.9569095199694857 175008.21030497280298732, 526587.08526148088276386 175075.49314598224009387, 526608.94237426621839404 175084.53746851411415264, 526524.52869730209931731 175245.07419345498783514, 526473.27779452677350491 175229.8263443021569401, 526498.70052055746782571 175244.55399248545290902, 526476.25838999240659177 175289.43825361545896158, 526525.35055060335434973 175313.2830173407564871, 526502.38243260327726603 175360.27122821123339236, 526655.2694470772985369 175450.74106705139274709, 526548.66932689363602549 175611.34256390717928298, 526523.42193000798579305 175630.27811157138785347, 526498.17453312233556062 175591.70569966279435903, 526496.73523488116916269 175590.17850534588797018))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((526496.73523488116916269 175590.17850534588797018, 526406.30206112191081047 175494.22269502107519656, 526346.69015180855058134 175449.33843389106914401, 526380.35334765608422458 175404.45417276109219529, 526342.83291061769705266 175434.61078570786048658, 526304.6144535921048373 175412.13552230672212318, 526220.48104146879632026 175317.48543366795638576, 526212.83254945755470544 175223.7914065305958502, 526176.50221240427345037 175198.93380749414791353, 526071.33544725005049258 175206.58229950536042452, 526034.04904869536403567 175148.26254791987594217, 526009.19144965894520283 175110.97614936518948525, 526011.10357266175560653 175093.76704233995405957, 526011.20072534133214504 175093.52450637135189027, 526028.17182268667966127 175051.15715683341841213, 526084.52183982264250517 174972.04738347270176746, 526120.93744978227186948 174927.4696540392760653, 526209.46505330502986908 174784.94649092113832012, 526119.83870293013751507 174923.07466663033119403, 526053.28603645204566419 175005.32371671171858907, 526010.59187305101659149 175067.48139578086556867, 525994.89548944763373584 175089.45633282553171739, 525949.06204932602122426 175022.90366634743986651, 525855.51160305016674101 174953.83957849282887764, 525828.51382325252052397 174995.27803120561293326, 525855.66856688621919602 174947.56102505151648074, 525805.44013935560360551 174918.05182387726381421, 525814.23011417349334806 174839.56990586066967808, 525702.0009714097250253 174820.10639019258087501, 525698.8616946890251711 174722.78881185199134052, 525659.9346633527893573 174636.77262970581068657, 525565.36717306601349264 174664.02053710119798779, 525538.06676878000143915 174653.24728339188732207, 525493.99436724185943604 174553.83953325595939532, 525459.71583271224517375 174532.29302583733806387, 525496.93252734444104135 174407.42122147939517163, 525457.92714756459463388 174534.53035107266623527, 525490.77226448152214289 174556.32890400406904519, 525543.79577161197084934 174666.49996881955303252, 525536.72597066126763821 174676.51552016640198417, 525515.04797329346183687 174692.30743877869099379, 525500.11743205995298922 174748.58409419711097144, 525507.00845109077636153 174843.90985745683428831, 525596.59169849148020148 174873.7709399237355683, 525710.00638670718763024 174878.36495261095114984, 525777.76807384355925024 174928.89909217032254674, 525768.58004846912808716 175008.14581102479132824, 525713.45189622254110873 175119.55061868979828432, 525685.88782009924761951 175159.74822970293462276, 525595.15606952679809183 175150.56020432850345969, 525492.93928723619319499 175144.81768846948398277, 525471.69197855785023421 175159.74822970293462276, 525369.47519626724533737 175139.07517261046450585, 525386.70274384436197579 175104.62007745634764433, 525230.50631247903220356 175056.3829442405840382, 525197.19972049666102976 175054.0859378969471436, 525166.19013485801406205 175226.36141366756055504, 525089.24042234709486365 175214.8763819495216012, 525097.279944549780339 175086.24402670745621435, 525104.45808937354013324 175049.49192520976066589, 525199.78385263320524246 174985.17574758871342055, 525214.81787929905112833 174966.87071981595363468, 525190.62146005278918892 174953.39830346533562988, 525127.28929241502191871 174934.86312413716223091, 525064.65251295559573919 174957.45343804056756198, 525099.16753414331469685 174650.99683751305565238, 525102.00163976603653282 174620.04028388037113473, 524979.1647777232574299 174597.37606225861236453, 524937.07801401300821453 174585.3315757944365032, 524940.61593483120668679 174596.39404977264348418, 524962.98638330516405404 174622.83447105140658095, 524944.37760573695413768 174606.91934299230342731, 524890.5032964691054076 174612.08132202102569863, 524777.03524737863335758 174619.39787700184388086, 524680.01865243853535503 174723.03394835483049974, 524522.6853424928849563 174831.17963737441459671, 524475.66009829880204052 174858.21915278598316945, 524323.54649589885957539 174929.67139882530318573, 524302.64638736820779741 174931.76140967838000506, 524251.52485175657784566 174949.68193757452536374, 524272.59287336631678045 175049.00829122628783807, 524272.14576235634740442 175067.33352094312431291, 524042.01348253048490733 175122.84527774224989116, 524018.31376306770835072 175131.4362350333831273, 523987.54343810823047534 175136.79924140661023557, 523960.12279363907873631 175046.48958203330403194, 524000.25377948675304651 175034.22337187058292329, 523966.59409888373920694 175032.38559600326698273, 523951.98165977036114782 175045.27283976325998083, 524036.35662941134069115 175313.19315103691769764, 524059.98113962868228555 175307.65666737424908206, 524327.96859593223780394 175207.23306857905117795, 524341.93538261542562395 175220.81630157568724826, 524471.09094912011642009 175168.31033058575121686, 524509.24167378677520901 175273.27074366103624925, 524654.88253770291339606 175213.55327629734529182, 524711.1153041081270203 175194.90256357757607475, 524706.84647323249373585 175187.00979776872554794, 524628.75152248388621956 175210.13245730067137629, 524518.74834085872862488 175260.84737031435361132, 524477.97536607540678233 175285.99682499363552779, 524380.67268556274939328 175322.80957126850262284, 524218.49263602652354166 175448.51886382378870621, 524123.84486623620614409 175480.16830401346669532, 524107.50576417194679379 175492.16410046571400017, 524128.81952411436941475 175549.43083725060569122, 524093.59998840204207227 175564.60831672887434252, 524054.6833743552560918 175482.29967801991733722, 524045.09912176639772952 175488.11071598145645112))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((527656.7183093624189496 178369.34070502704707906, 527783.66874267382081598 178260.44675826572347432, 527701.29201637103687972 178172.63382336677750573, 527726.60529186681378633 178158.51739612722303718, 527707.29683605546597391 178172.78455480805132538, 527838.83275414002127945 178317.72066099435323849, 527870.91154732566792518 178356.61619773207348771, 527746.60622373130172491 178482.5254609857511241, 527869.90908503858372569 178585.97956900941790082, 527839.18433681316673756 178655.71945479151327163, 527835.94589031487703323 178664.7629006463685073, 527776.6708300617756322 178800.04388493386795744, 527853.03527260560076684 178816.77474871501908638, 527868.81008702784311026 178834.93968653454794548, 527956.28860336926300079 178854.53869839245453477, 527945.29403574171010405 178902.34116633859230205, 527960.59082548448350281 178906.64338845372549258, 528074.04253716359380633 178926.48126136808423325, 528075.63601999881211668 178916.12362293904880062, 528060.09956235531717539 178881.8637419814185705, 528072.05068361957091838 178818.12442857190035284, 528067.92073296045418829 178806.12665641392231919, 528040.501292280619964 178800.6427682779612951, 528050.44083952705841511 178741.0054847993014846, 528058.38286198873538524 178718.14782906166510656, 528102.34081977850291878 178746.40651621224242263, 528250.96058182965498418 178905.49245868952129968, 528307.84153715777210891 178965.57330830910359509, 528456.10630761610809714 179120.06087270937860012, 528453.06503982131835073 179134.64540692919399589, 528421.32784037000965327 179147.83876678114756942, 528276.90514995099510998 178992.9140435898443684, 528343.29222077992744744 178930.61010330502176657, 528508.60514012665953487 178773.42616898694541305, 528627.19860546640120447 178713.62781604222254828, 528688.83252045430708677 178852.26219280663644895, 528695.22035057423636317 178849.19359146716305986, 528631.00734287954401225 178710.50025443226331845, 528694.29413869057316333 178684.68859138496918604, 528704.07457833737134933 178673.90502972310059704, 528675.54235468478873372 178676.5972451399138663, 528566.76733427762519568 178496.98558549524750561, 528583.98656073305755854 178472.45039081721915863, 528590.69624376785941422 178461.60069059068337083, 528559.28921679628547281 178483.15733183023985475, 528530.16633724083658308 178495.29186497832415625, 528481.12854740128386766 178503.28638093473273329, 528322.66582040826324373 178458.74550632052705623, 528317.48233069677371532 178476.88772031053667888, 528318.63421729940455407 178485.81484148022718728, 528306.97136544866953045 178503.66908381960820407, 528286.37375599541701376 178488.37048086652066559, 528274.68490427918732166 178477.86123803912778385, 528230.34233377804048359 178459.68453743468853645, 528242.35289700934663415 178427.08443723549135029, 528172.00531236897222698 178397.91592653095722198, 528134.25782792770769447 178356.73685259514604695, 528536.36687937250826508 177976.28225404073600657, 528565.26066673942841589 177951.17037601495394483, 528618.5099502638913691 177941.48868810140993446, 528799.1956435035681352 177949.62260939209954813, 529089.81677403079811484 177901.90869243987253867, 529255.79840785474516451 177863.14847174196620472, 529358.25357655365951359 177883.68841009688912891, 529427.69813003926537931 177906.1845330570358783, 529433.56668385502416641 177888.57887160996324383, 529378.79351490852423012 177854.34564101841533557, 529295.6556691862642765 177852.38945641319151036, 529234.28037719719577581 177853.36754871581797488, 528956.5021632545394823 177913.03117917533381842, 528790.22647180990315974 177935.52730213548056781, 528692.90628769970498979 177932.5930252276302781, 528557.92954993876628578 177932.5930252276302781, 528554.01718072837684304 177894.44742542563471943, 528627.54724844382144511 177420.27802047552540898, 528632.27978818584233522 177383.89662120884167962, 528696.16907470289152116 177392.77013322510174476, 528706.22572165471501648 177407.55931991888792254, 528704.45101925148628652 177685.8918134956038557, 528709.77512646117247641 177687.66651589883258566, 528709.18355899350717664 177399.27737537038046867, 528698.53534457390196621 177388.62916095086256973, 528633.46292312140576541 177378.57251399909728207, 528658.30875676684081554 177201.69384114164859056, 528671.9148085251217708 177111.77558604351361282, 528696.37895216140896082 177096.46537706872913986, 528698.52647522534243762 177087.85737352253636345, 528707.54613430006429553 177045.9768067144905217, 528686.48968786001205444 177029.56326320749940351, 528651.63210264872759581 177034.21630194777389988, 528601.67845188046339899 177025.25386094400892034, 528636.23278523643966764 177061.25791369623038918, 528648.99903309403453022 177090.69567049364559352, 528683.61924763000570238 177095.42086361086694524, 528707.09237683820538223 177083.02097844227682799, 528717.31761167501099408 177070.66164703483809717, 528900.55563481082208455 177088.40867106735822745, 529012.84455444279592484 177200.88158813735935837, 529132.22997563553508371 177273.7439153409213759, 529136.69044820708222687 177251.27508732164278626, 529135.47952493233606219 177274.99521491886116564, 529192.11810795951168984 177297.59016217343742028, 529279.07078784692566842 177338.04844474766287021, 529379.56394133775029331 177459.42329247039742768, 529514.28841154393739998 177579.99861740384949371, 529522.47303623706102371 177587.32366964058019221, 530009.96149630157742649 177853.79645061693736352, 530094.68275518657173961 177878.00252458406612277, 530200.58432879275642335 177862.87372835460701026, 530315.37161932047456503 177998.80604608487919904))</t>
-  </si>
-  <si>
     <t>02 Shepherd's Bush</t>
   </si>
   <si>
@@ -197,9 +173,6 @@
     <t>12 Soho</t>
   </si>
   <si>
-    <t>MultiLineString ((522501.94230883487034589 178726.41802728205220774, 522509.3171643289970234 178692.11021129344590008, 522504.37178637820761651 178610.51147510507144034, 522674.06006731535308063 178577.74834618097520433, 522695.07792360632447526 178757.01829689781880006, 522871.25624804722610861 178766.46876867543323897, 523096.53894994757138193 178769.45924701925832778, 523146.56457700586179271 178764.79577539447927848, 523228.15499849966727197 178681.39223342304467224, 523341.47502835217164829 178625.18549861619248986, 523349.17238342546625063 178622.56512242107419297, 523338.6908786449348554 178607.66173281130613759, 523330.33842952299164608 178605.53267715277615935, 523318.05541610840009525 178608.31682686010026373, 523049.53108943597180769 178557.41122244377038442, 523044.84592751995660365 178556.49860799589077942, 523038.88646519993199036 178504.87752603454282507, 523045.46353330073179677 178491.7233898330014199, 523052.69884405157063156 178411.49882859381614253, 523054.4322625290369615 178375.4288675059506204, 523103.10630509618204087 178343.670138604065869, 523108.87300237617455423 178325.90583238122053444, 523119.7353025998454541 178318.10387213190551847, 523126.32058558438438922 178326.65065053338184953, 523136.96704334113746881 178320.71276599433622323, 523197.00493266043486074 178288.80073473454103805, 523242.30379059282131493 178263.10884516095393337, 523127.63683081179624423 178184.14008984004613012, 523181.18413750198669732 178115.4480903485964518, 523221.2093970482237637 178062.44166554414550774, 523237.43585362087469548 178040.26550822801073082, 523471.72365575307048857 178194.08150103568914346, 523504.52584943413967267 178070.048206178820692, 523533.22776890522800386 178030.07053262993576936, 523398.27638210507575423 177944.08385379810351878, 523374.85150622186483815 177922.22063630708726123, 523440.44115869491361082 177805.09625689091626555, 523462.30437618592986837 177764.4931386933021713, 523365.48155586858047172 177712.95841175017994829, 523424.82457477279240265 177581.77910680408240296, 523434.19452512607676908 177552.10759735197643749, 523498.16975758440094069 177350.68934009084478021, 523543.47255923581542447 177377.19986846460960805, 523720.65685013914480805 177494.3160001412325073, 523740.79142865084577352 177501.02752631180919707, 523763.52510854077991098 177520.51030919776530936, 523791.01839464512886479 177472.12212565407389775, 523850.40389263059478253 177270.87127137003699318, 523905.39046483935089782 177009.13518765641492791, 523950.85999103111680597 176923.03958886690088548, 524024.87041156162740663 176766.3116395082033705, 524158.7422016387572512 176861.0014422457315959, 524150.03509334108093753 176879.50404737834469415, 524347.03341857658233494 176991.60806671128375456, 524324.17725929513107985 177034.05521966257947497, 524476.55165450496133417 177106.97725165582960472, 524501.58459086087532341 177071.06042992777656764, 524552.73885210976004601 177093.91658920928603038, 524496.59686273266561329 177229.15389398331171833, 524449.34194107458461076 177318.12462787510594353, 524399.1698832738911733 177302.76348325112485327, 524404.66854049474932253 177329.1570379113254603, 524169.69941686512902379 177380.1700359427195508, 524119.83809645345900208 177460.02507976815104485, 523954.87837982719065621 177548.00359530214336701, 524125.23060610314132646 177470.69582927966257557, 524276.1069283313699998 177516.75281185458879918, 524264.62413314066361636 177545.0041890301508829, 524284.58432462147902697 177528.76640343241160735, 524401.59080314182210714 177544.16933234094176441, 524598.18210187566000968 177647.93601894256426021, 524702.78518042073119432 177684.64508786791702732, 524730.84316259669139981 177694.39206814055796713, 524743.63401176454499364 177685.64633391896495596, 524749.76929571013897657 177691.34065775718772784, 524785.28179647319484502 177706.26515992148779333, 524805.12269188673235476 177677.06875034020049497, 524890.26466468954458833 177733.9889697001199238, 524900.02326978160999715 177732.91675252851564437, 524914.16278953978326172 177714.11232543102232739, 524914.433173893019557 177703.10024843754945323, 524895.1238769325427711 177675.34173217235365883, 524920.4659545662580058 177628.80580489605199546, 524910.18844398378860205 177623.75821537460433319, 524917.57360786944627762 177620.23991505563026294, 524938.32413323107175529 177584.05164737423183396, 524950.20932233543135226 177593.41349562600953504, 524943.99898932594805956 177602.68904486036626622, 524939.81656498205848038 177602.46701134811155498, 524944.64205134124495089 177603.30154497240437195, 524951.62820201518479735 177594.10471880476688966, 524978.48803550400771201 177611.26339810941135511, 524991.338410071330145 177614.20456636406015605, 524996.90309547598008066 177616.60875923844287172, 525046.99662963894661516 177531.42582527716876939, 525239.41112284129485488 177643.52029113803291693, 525247.45787289727013558 177648.27282234595622867, 525259.52019177761394531 177658.21438176609808579, 525180.47252021881286055 177798.30595981661463156, 524957.03894217207562178 177697.24630155507475138, 524904.35931604239158332 177802.04137613053899258, 524828.42314845940563828 178030.7590969885350205, 524705.97326419106684625 178005.83836105518275872, 524533.05028670514002442 177972.15814960357965901, 524412.19303111883345991 177923.3538982339669019, 524347.32041661813855171 177918.60612411511829123, 524215.25543399516027421 177874.27527343999827281, 524153.58899412449682131 177868.02728649199707434, 524107.64839021116495132 177866.90650818648282439, 524077.78060873120557517 177856.69226100511150435, 524086.80756595288403332 177870.61416968662524596, 524045.25677349988836795 177910.08328927803086117, 523833.18216259987093508 177995.34252377698430791, 523819.950420176028274 177988.69269825710216537, 523786.25443879171507433 178026.36677837959723547, 523723.08611731143901125 178130.99483389721717685, 523834.20989532244857401 178190.30815001711016521, 523794.47597305721137673 178252.39056805544532835, 523924.27272151375655085 178295.13950059562921524, 524017.76622407609829679 178319.41152608778793365))</t>
-  </si>
-  <si>
     <t>Walk down/up the Richmond Way link. Use lift up on second visit to Westfield.</t>
   </si>
   <si>
@@ -218,48 +191,6 @@
     <t>01 Hammersmith</t>
   </si>
   <si>
-    <t>MultiLineString ((524019.5942947514122352 178316.91922095965128392, 524147.7133394600241445 178306.75905061210505664, 524166.91197717498289421 178284.19988717755768448, 524354.64446763973683119 178269.30031749303452671, 524399.84070607554167509 178273.06237215833971277, 524414.83044529519975185 178259.25790301198139787, 524410.00335248897317797 178275.08226800878765061, 524460.50269656255841255 178279.86024319374701008, 524545.15821839333511889 178304.07423270272556692, 524543.03650101134553552 178318.19322945724707097, 524606.41363690642174333 178341.00155929423635826, 524585.96807908453047276 178393.16329537253477611, 524641.53035025740973651 178409.4543690562422853, 524644.76698741316795349 178405.13885284864227287, 524586.18761726538650692 178398.75567615206819028, 524557.75235208170488477 178462.92715298544499092, 524533.38262645772192627 178466.85974151274422184, 524527.65925442636944354 178452.12205853176419623, 524496.18070825340691954 178442.39232607831945643, 524427.78641247749328613 178419.42729580210288987, 524292.65770760283339769 178428.95569482402061112, 524285.72796285967342556 178500.85179653487284668, 524141.93575943791074678 178524.23968504322692752, 524134.57290564820868894 178602.63242245087167248, 524072.20520295930327848 178751.62193443000433035, 523910.22241958661470562 178665.86634323271573521, 523905.02511102921562269 178451.91047428591991775, 523915.41972814401378855 178413.79687819821992889, 523895.92982105386909097 178448.44560191431082785, 523726.1510748450527899 178452.77669237882946618, 523708.82671298703644425 178632.95005570244393311, 523695.29205528547754511 178640.31290949208778329, 523686.62987435649847612 178648.54198137467028573, 523680.02150594454724342 178649.19214336172444746, 523900.87884802120970562 178671.65342459944076836, 523999.36567001842195168 178726.5068444459757302, 523959.47227376641239971 178773.2569181787839625, 523927.20931058085989207 178820.58665569889126346, 523850.2099083709763363 178872.39582184806931764, 523892.85029150103218853 178940.42065121117047966, 523998.51854862732579932 179080.1726343011832796, 524045.92328174656722695 179069.92708279716316611, 524108.31766754906857386 179070.02411880018189549, 524108.13091779133537784 179068.4773711011512205, 524042.70696497993776575 179065.09797074663219973, 523999.53327132220147178 179074.33729632402537391, 523939.45133300090674311 179101.74353711132425815, 523931.0548391982447356 179077.84969023033045232, 523832.73847269039833918 178950.01551744830794632, 523808.87133779458235949 178919.72486848966218531, 523809.41094240511301905 178912.73769014445133507, 523799.16029718943173066 178891.93745666136965156, 523586.12709654704667628 178975.25572723767254502, 523546.82854762935312465 178989.41042456653667614, 523455.77026956726331264 179026.61562438475084491, 523425.37385861721122637 179017.71911386278225109, 523394.55668384418822825 178968.1703076938574668, 523386.43806897010654211 178974.87698954631923698, 523390.32088477944489568 179020.23533786431653425, 523400.29266174440272152 179082.18389918576576747, 523455.35804958565859124 179075.1242340778990183, 523472.30124584451550618 179109.01062659561284818, 523504.09316043963190168 179333.90299656018032692, 523501.12058276316383854 179549.91030771631631069, 523489.23027205729158595 179569.72749222605489194, 523506.07487889059120789 179573.69092912800260819, 523514.99261191993718967 179520.18453095172299072, 523513.01089346897788346 179360.65619564833468758, 523525.6670606259140186 179357.86960204786737449, 523623.99278196529485285 179332.54146969801513478, 523808.35468181630130857 179496.79414100397843868, 523821.31694713741308078 179494.6065657127473969, 523820.82524603558704257 179440.88822034336044453, 523821.60161350667476654 179423.82347127312095836, 523978.71472944790730253 179559.94275737437419593, 523963.60412625916069373 179581.12237331917276606, 523932.02048844669479877 179605.1507095372362528, 523999.59877721423981711 179655.89870352283469401, 523910.11968204472213984 179798.0550079453678336, 523930.4073799456236884 179829.45350444715586491, 523864.14663150085834786 179860.29696010009502061, 523810.64023332454962656 179872.18727080593816936, 523789.8321895893313922 179869.21469312947010621, 523791.3184784275945276 179862.27867855108343065, 523810.64023332454962656 179862.77410816380870529, 523818.07167751574888825 179851.379227070719935, 523809.64937409909907728 179859.80153048736974597, 523790.32761920208577067 179859.80153048736974597, 523777.1597479346091859 179869.18618441122816876, 523706.58830350730568171 179852.08963036345085129, 523700.07543018303113058 179892.55552700196858495, 523753.57804833719274029 179905.68178868596442044, 523757.7367767600226216 180009.66353510232875124, 523767.00669973070034757 180023.23681901925010607, 523706.96914328029379249 180170.29134639311814681, 523632.6539854159927927 180440.35106004029512405, 523620.79229790804674849 180462.13728423725115135, 523548.03862911934265867 180463.75793557113502175, 523535.22499171097297221 180459.7186919086962007, 523506.46992536378093064 180432.00136401766212657, 523471.37248534307582304 180400.94759161036927253, 523441.88097540393937379 180396.77844605082646012, 523405.13739714992698282 180400.94492353178793564, 523354.80208993284031749 180427.03869174927240238, 523338.7929603232187219 180408.12326784816104919, 523328.15338179533137009 180424.15373995114350691, 523305.84850782883586362 180426.90513797110179439, 523301.15577980724629015 180523.14838607650017366, 523292.50651331816334277 180618.96054938790621236, 523284.62079987034667283 180674.33723709877813235, 523248.287612549145706 180823.73672169324709103, 523180.15017024852568284 181046.19415628933347762, 523195.18096548621542752 181051.93683565245009959, 523202.13110555708408356 181048.79546767444116995, 523198.1975192311219871 181025.29501264891587198, 523215.94951775739900768 180948.18024191819131374, 523266.44380770833231509 180772.14566253469092771, 523290.08581532444804907 180672.17699802399147302, 523301.87572635652031749 180592.6180390000808984, 523321.93386030138935894 180594.37743679818231612, 523345.83390644547762349 180595.59365976107073948, 523343.46150832128478214 180548.75618748448323458, 523354.87576299742795527 180537.93592937797075137, 523380.31128285668091848 180514.1939573377603665, 523406.97587942460086197 180529.63057361770188436, 523484.37468678108416498 180575.0080605911789462, 523509.171474092931021 180541.68172154412604868, 523535.32422105281148106 180470.54419238591799513, 523633.30356490309350193 180465.74028088501654565, 523653.83785533590707928 180470.43274004379054531, 523657.69995753932744265 180447.81861192517681047, 523665.83561170572647825 180442.37385650910437107, 523675.93876430939417332 180435.46308627870166674, 523682.85951727599604055 180423.24514195055235177, 523686.44381641852669418 180412.04702033923240378, 523712.49482848419575021 180418.87395834788912907, 523706.73923687369097024 180445.57087515294551849, 523721.2475296090124175 180427.75734292989363894, 523719.41961515875300393 180446.1546540999552235, 523728.11535413248930126 180423.38281483261380345, 523734.61995970364660025 180436.75314993946813047, 523743.92085290589602664 180445.78751291986554861, 523769.65134543011663482 180443.11091388569911942, 523795.20135089615359902 180453.50444708927534521, 523818.04303102707490325 180456.12513331841910258, 523822.22505310841370374 180471.36572253954363987, 523842.84258654178120196 180463.33524113963358104, 523866.60769404500024393 180445.05963141279062256, 523881.3551514504943043 180423.12364392634481192, 523912.52049187803640962 180435.65034075808944181))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((523912.23182315297890455 180434.71100018959259614, 523933.4534212714061141 180352.53366981475846842, 524001.52344168594572693 180143.68549420178169385, 523913.53053296857979149 180113.67887586844153702, 523902.62098808796145022 180137.80206676595844328, 523916.00450257491320372 180117.34166811924660578, 523997.87116536882240325 180145.33954628632636741, 523923.79085326276253909 180363.22947150381514803, 523872.72131736180745065 180542.85840179145452566, 523835.97818674857262522 180523.79079492119490169, 523763.34026239992817864 180654.77233878360129893, 523744.63108860928332433 180677.45673540118150413, 523650.93208653811598197 180844.88014607870718464, 523635.86034783296054229 180877.92901890238863416, 523672.90413934946991503 180906.25662417968851514, 523670.72509278968209401 180920.78360124499886297, 523773.86662995326332748 180929.49978748415014707, 523780.94853127264650539 181260.35169014619896188, 523974.53005634632427245 181333.20707353367470205, 524028.53397912753280252 181282.74034599942388013, 524026.59334985166788101 181290.30040013694087975, 524233.11923408636357635 181385.62614455129369162, 524217.87981449643848464 181424.35966934243333526, 524259.1864618023391813 181439.65405084792291746, 524180.57548385200789198 181646.75296914129285142, 524246.61444996122736484 181674.13497947927680798, 524310.64003295754082501 181756.68368711578659713, 524324.73458955099340528 181770.25499738051439635, 524357.15467388625256717 181768.32267447313643061, 524362.52223751798737794 181772.61672537846607156, 524428.21140558586921543 181747.88693608297035098, 524470.84714648721273988 181712.35715199852711521, 524536.93254488427191973 181586.58171633951133117, 524554.69743692653719336 181598.66184292820980772, 524669.10334167850669473 181744.33395767453475855, 524692.55299917422235012 181756.41408426326233894, 524751.53244075446855277 181674.69558086898177862, 524688.64472292503342032 181633.30338241058052517, 524641.74540793348569423 181580.71930196558241732, 524662.35268270247615874 181547.32130492618307471, 524660.22089565743226558 181540.92594379096408375, 524672.30102224613074213 181535.95177401913679205, 524799.49764926848001778 181620.51266014017164707, 524921.00951083737891167 181697.25699376262491569, 524922.43070220074150711 181707.20533330627949908, 524928.82606333598960191 181697.96758944430621341, 524901.8234274317510426 181673.80733626688015647, 525026.17767172737512738 181464.89220585022121668, 524920.29891515569761395 181419.41408222209429368, 524786.99264362745452672 181364.56044746178667992, 524835.49713539250660688 181262.62477866216795519, 524810.03188311751000583 181242.69948545226361603, 524652.8294552881270647 181191.18254679589881562, 524402.65496118809096515 181094.42998001689556986, 524304.52021488372702152 181022.55664469531620853, 524231.26470003672875464 180918.89318028924753889, 524209.14982763008447364 180870.5168968997313641, 524198.09239142679143697 180881.5743331030535046, 524164.92008281679591164 180965.88728415334480815, 524142.45342317444738001 180993.90335134317865595, 524123.2956079263240099 180993.85086294135544449, 524084.75367034279042855 180953.44766842460376211, 524118.6821531155728735 180877.17565803986508399, 524106.36578986316453665 180874.40456134342821315, 524049.16254756337730214 180876.73670476407278329, 524019.75422611943213269 180856.76255305705126375, 523997.69997150875860825 180847.04886512237135321, 523980.05357129260664806 180839.417857577878749, 523960.7030579368583858 180839.417857577878749, 523944.11690363183151931 180782.74849703587824479, 523930.29510837770067155 180767.54452225632849149, 523993.87536654679570347 180622.41567208780907094, 523990.55990376364206895 180643.74445799872046337, 524173.57321334740845487 180692.2783743524341844, 524192.01128995302133262 180618.89747461018851027, 524220.32912637857953086 180551.10990497015882283, 524220.5789011872257106 180534.90904957352904603, 524231.74438736715819687 180521.31105254049180076, 524218.06263667164603248 180517.35405082762008533, 524270.64104605483589694 180417.25284834808553569, 524303.3120032858569175 180383.15005364664830267, 524374.44817258138209581 180271.11154306019307114, 524456.19647553935647011 180149.77631248842226341, 524431.26476303639356047 180136.00103032620972954, 524459.56523167877458036 180144.27347500628093258, 524525.75418626563623548 180172.10854396742070094, 524641.63642226834781468 180229.18827888066880405, 524630.52720418258104473 180253.81709120800951496, 524616.84224711218848825 180281.94728074161685072, 524603.91244324017316103 180308.93155401269905269, 524598.58000010333489627 180313.8827607449493371, 524587.42772607307415456 180310.60648767265956849, 524592.46009993064217269 180317.89068621123442426, 524603.82116770057473332 180322.09606592508498579, 524614.00544641900341958 180322.34570301411440596, 524754.85509058670140803 180388.94884889174136333, 524708.14623816998209804 180493.35138344980077818, 524691.32313322799745947 180486.98523136778385378, 524705.02864181320182979 180499.13329579585115425, 524601.37547879898920655 180711.38724282311159186, 524596.0233205872355029 180713.76597980610677041, 524663.75182977877557278 180627.27976981503888965, 524868.74748395150527358 180735.9867015402414836, 524880.61112230643630028 180756.5456591853289865, 524875.5653715591179207 180764.13213197357254103, 524891.28976369893644005 180780.379913758370094, 524899.00831162196118385 180777.91579997690860182, 524896.38319139555096626 180788.82128840731456876, 524908.52099283307325095 180806.57090083844377659, 524918.36612558737397194 180815.52170617721276358, 524987.54607934912201017 180862.98865713539998978, 524898.15788384573534131 180986.02517464658012614, 524884.03555789380334318 181013.55537098314380273, 524928.2247080490924418 181024.21138646424515173, 524940.22894107585307211 181020.27645458056940697, 525054.89033654436934739 181049.24941641179611906, 524998.89522997406311333 181305.53165977715980262, 525260.98247081786394119 181375.88277569483034313, 525445.8561063768574968 181437.37408240092918277, 525452.05563839036040008 181443.14992468082346022, 525454.73027244885452092 181463.24714800907531753, 525525.30599382147192955 181466.04417678515892476, 525646.34203849150799215 181437.3191127959289588, 525749.25431174924597144 181463.62342599901603535, 525755.4399772712495178 181450.57309592515230179, 525777.37221961934119463 181420.22921704116743058, 525815.13287177938036621 181442.1180841151799541, 525815.54239428753498942 181442.27739287109579891))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((525815.54239428753498942 181442.27739287109579891, 525938.4894992244662717 181490.10516775862197392, 525950.2033640209119767 181472.33594733368954621, 525943.13234854943584651 181373.34173073348938487, 525962.06789837975520641 181288.70267443344346248, 526084.9407700706506148 181347.92177145567256957, 526141.85119377286173403 181374.63645114144310355, 526247.90762806567363441 181264.37710280925966799, 526196.01242155989166349 181214.6880689833778888, 526166.16735107859130949 181192.64317541586933658, 526182.74869802431203425 181210.14127948944224045, 526289.24206442979630083 181085.57761354133253917, 526304.73383384314365685 181090.14411224401555955, 526312.97320597257930785 181086.63195823784917593, 526405.64829471055418253 180975.33631497254827991, 526406.50096082710660994 180959.79253581800730899, 526425.68278948625084013 180965.84515120310243219, 526594.1189202640671283 181126.22767907357774675, 526481.37747424189001322 181247.68218424991937354, 526436.7998225896153599 181292.98168183141387999, 526364.50886605237610638 181370.49790682113962248, 526315.65099693823140115 181327.24125062092207372, 526174.19306422164663672 181474.26841948175569996, 526118.98830004595220089 181451.55415104021085426, 526093.47386830300092697 181427.99858194089028984, 526147.53385363647248596 181372.97566176933469251, 526117.64916966739110649 181356.75464216282125562, 525896.63604345871135592 181252.18492163851624355, 525804.47871884633786976 181202.92109834335860796, 525674.52415049879346043 181177.43981043208623305, 525417.28142454475164413 181124.71832773357164115, 525450.65898510219994932 180968.90288878511637449, 525448.5728875674540177 180995.38028057347401045, 525580.7993774680653587 181023.62283181439852342, 525598.13003391132224351 180945.3139397373306565, 525607.75236547156237066 180908.16104843508219346, 525612.56353125174064189 180883.21426290841191076, 525623.07681943802163005 180835.94901390164159238, 525631.27362039673607796 180829.35593486961442977, 525630.06616769870743155 180815.88719046339974739, 525532.28454484208486974 180779.59350092764361762, 525501.02729750447906554 180764.22108420424046926, 525485.39867383567616343 180754.48522027939907275, 525448.1205632813507691 180741.67487300987704657, 525428.64883543166797608 180743.98073551838751882, 525274.54035777947865427 180702.73141731056966819, 525225.9229351548710838 180690.87681836728006601, 525208.01717880030628294 180709.67786253962549381, 525200.18341039516963065 180722.65953589673154056, 525163.92425377701874822 180720.42131635241094045, 525171.53420022781938314 180675.88074742027674802, 525177.80121495190542191 180667.82315706068766303, 525205.21940436994191259 180529.83692215289920568, 525202.53354091674555093 180499.39713635004591197, 525217.75343381811399013 180446.57515510389930569, 525265.20368815783876926 180455.52803328121080995, 525259.78516155341640115 180477.87945552368182689, 525268.52280582929961383 180452.9590315387758892, 525421.26921318552922457 180497.63403710661805235, 525446.30735667480621487 180398.85467028760467656, 525445.17935181641951203 180398.21167875776882283, 525420.12320177466608584 180383.9290343812899664, 525372.9962905184365809 180352.34950992788071744, 525364.52507656568195671 180327.99476981372572482, 525324.28681029006838799 180312.46421090036164969, 525076.87950780324172229 180213.18165121536003426, 525092.47997789632063359 180166.629184607823845, 525087.99899180571082979 180164.96956012982991524, 525131.2729772892780602 180055.01999166997848079, 525400.28327040141448379 180165.03473592712543905, 525457.11612049920950085 180186.51174571155570447, 525519.24511377036105841 180025.31955409917281941, 525538.98347847280092537 179972.22863600350683555, 525571.77124779403675348 179895.67673749651294202, 525617.60380089143291116 179797.21516905541648157, 525673.47756801324430853 179662.45056660982663743, 525613.02575635176617652 179620.2152606945601292, 525630.83745085913687944 179599.70482459513004869, 525606.00902821240015328 179617.51651910252985545, 525492.79681842681020498 179534.3952780679683201, 525517.08549275505356491 179489.05641932183061726, 525484.7005936506902799 179530.0772915207198821, 525429.82762361585628241 179495.93095825402997434, 525313.85690457350574434 179430.39389928575837985, 525309.06791018566582352 179437.57739086757646874, 525356.47895462566521019 179468.7058543887687847, 525353.60555799293797463 179482.35448839422315359, 525368.93034003407228738 179476.12879568999051116, 525425.4404738110024482 179506.29946033359738067, 525375.64614801947027445 179589.0921119402628392, 525370.77017299830913544 179596.45324670110130683, 525434.41614770900923759 179634.6992497275932692, 525421.80133750266395509 179659.47227550984825939, 525427.39915714180096984 179662.39022623706841841, 525471.61650676012504846 179597.89238431974081323, 525184.72663602349348366 179419.83259478391846642, 525208.6187529000453651 179388.72964811127167195, 525215.80224448186345398 179373.88376550885732286, 525148.79085531854070723 179337.39614326649461873, 525140.3769248811295256 179332.81476808225852437, 524984.62089585815556347 179676.87027474676142447, 524980.50617997418157756 179688.6684670404647477, 524951.26898805412929505 179685.32707367819966748, 524820.95464692520909011 179634.37082490339525975, 524810.93046683829743415 179609.31037468629074283, 524843.03832464327570051 179508.38986770567134954, 524807.60560298000928015 179485.20549427167861722, 524703.27592252695467323 179431.83769127260893583, 524617.75620542606338859 179575.09962145454483107, 524498.60092300793621689 179796.83555421329219826, 524464.29486135952174664 179922.3455358539649751, 524391.49907200783491135 180100.98807638921425678, 524197.37696707027498633 180024.84535419387975708, 524130.02899053593864664 180004.79501412331592292, 524164.57578076719073579 179943.56385594073799439, 524201.82267002947628498 179912.52478155549033545, 524273.21254111552843824 179881.48570717024267651, 524284.59353505680337548 179876.31252810603473336, 524445.73806290689390153 179568.50837378573487513, 524454.16972204064950347 179535.7185882649209816, 524373.44439292512834072 179453.58798262715572491, 524353.45823794102761894 179411.11740328592713922, 524346.40296634018886834 179381.5818728904123418, 524337.00973276444710791 179379.3654919343534857, 524274.6872111193370074 179445.0653559887141455, 524249.97718396421987563 179422.31644209986552596))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((524249.97718396421987563 179422.31644209986552596, 524248.09063964674714953 179420.57962352185859345, 524231.20392760063987225 179398.62689786194823682, 524232.82265402289340273 179395.01589276641607285, 524385.38761930819600821 179221.87442430757801048, 524385.38761930819600821 179212.90917027732939459, 524438.18300415284465998 179156.12922808589064516, 524570.28329039399977773 179006.69620745387510397, 524700.98101851902902126 179091.39982051457627676, 524711.83193899260368198 179097.007949031481985, 524716.87237500911578536 179099.99616585933836177, 524718.76718895498197526 179092.8934059570892714, 524696.23571698309388012 179080.07131011568708345, 524678.74982980021741241 179058.15524498705053702, 524674.25436888239346445 179080.97733096149750054, 524709.50849799939896911 179105.50707113670068793, 525019.12328359950333834 179286.75246481280191801, 525126.9951293395133689 179333.83938160410616547, 525163.80853701278101653 179265.3493208167492412, 525215.17608260328415781 179142.92333715932909399, 525235.29503795958589762 179146.66888735865359195, 525236.12335093319416046 179146.99713273279485293, 525405.392016846453771 179214.0752280225569848, 525471.53291914879810065 179049.24790006288094446, 525514.57699842483270913 179075.49428986536804587, 525574.28753522550687194 179077.06907325351494364, 525574.28753522550687194 179051.87253904313547537, 525588.45396603550761938 179007.86059112328803167, 525591.26759051892440766 178988.16521973989438266, 525607.21146259119268507 178989.57203198154456913, 525588.32020733586978167 178982.91982687110430561, 525478.29455103096552193 178974.53093041834654287, 525357.75664400029927492 178938.75233156332978979, 525307.44793495535850525 178907.14925625239266083, 525106.8280279291793704 178791.05139943258836865, 525141.39902080979663879 178737.10666269203647971, 525174.15424077014904469 178734.65491616009967402, 525128.42563297669403255 178713.73651046739541925, 525133.77685303764883429 178695.25047752965474501, 525158.10058058728463948 178705.95291765150614083, 525190.20790095289703459 178651.46776794025208801, 525228.10579012299422175 178583.51367086486425251, 525201.60606543626636267 178566.21796919498592615, 525295.95426285627763718 178496.51634551520692185, 525326.84208016830962151 178536.51844553701812401, 525376.93699422583449632 178484.23081163188908249, 525324.76084575697313994 178418.86686161754187196, 525360.27136073401197791 178473.38879090908449143, 525431.60036567493807524 178549.65587991260690615, 525344.89456077455542982 178653.32112459669588134, 525439.16125242365524173 178700.23684167736792006, 525483.30881792632862926 178634.92763320647645742, 525530.49711275601293892 178590.84330049104755744, 525577.51932919700630009 178544.81350922945421189, 525597.16444525693077594 178525.40052273799665272, 525588.47622809757012874 178508.78139137243852019, 525604.47783662029542029 178512.66683010943233967, 525628.09064453258179128 178492.11954176213475876, 525659.47355236567091197 178452.53428301808889955, 525713.59123718016780913 178344.12060141284018755, 525732.49230667052324861 178352.32295232376782224, 525715.0922296498902142 178341.20492456736974418, 525745.51348978653550148 178292.14412009407533333, 525752.42284710763487965 178243.77861884664162062, 525830.72889674629550427 178141.28981858419138007, 525896.00242686306592077 178181.89303810551064089, 525949.38357987010385841 178108.33855643015704118, 526063.55754208331927657 177998.47304562115459703, 526240.20404965861234814 178164.34842468574061058, 526283.28856370132416487 178114.80123353656381369, 526385.55490465881302953 178199.05475307532469742, 526458.76830784429330379 178251.35004106492851861, 526375.67690581630449742 178464.30807493376778439, 526315.2467952505685389 178444.552077248779824, 526238.25651015469338745 178432.64037276225280948, 526149.93557932786643505 178441.93731284930254333, 526090.66758627293165773 178434.96460778400069103, 526034.88594575074966997 178408.235905033769086, 525976.78007020673248917 178517.4749510565015953, 525940.18563409615308046 178593.45575471699703485, 525837.99324970017187297 178546.41155678656650707, 525802.4071329872822389 178609.5827689859434031, 525711.1127249967539683 178737.73127572966041043, 525805.68154822511132807 178613.01432153128553182, 526021.35517114016693085 178721.26253662595991045, 526270.76997553906403482 178813.45403372519649565, 526143.33955579355824739 178767.74135057261446491, 526097.32672476547304541 178890.71894277923274785, 526093.0574930205475539 178933.8856193107785657, 526074.55748879280872643 178941.00100555224344134, 526093.58066659071482718 178941.13121456975932233, 526088.69760579953435808 178993.13581199539476074, 526211.31028287101071328 179003.57347023714100942, 526199.34856594784650952 179056.81849040847737342, 526206.62047603982500732 179066.37049779869266786, 526188.0618779466021806 179102.36209072399651632, 526167.3646381531143561 179197.54278659154078923, 526167.3646381531143561 179228.3240159587294329, 526167.7310813597869128 179308.57507823742344044, 526167.11127823567949235 179411.66888013994321227, 526089.31039173016324639 179406.55787299721851014, 526074.16666686290409416 179647.34309838674380444, 526071.96742292866110802 179673.52631873372592963, 526121.07215822767466307 179661.16662345439544879, 526116.72956258896738291 179684.54983073959010653, 526120.07002077263314277 179690.89670128843863495, 525859.68130536109674722 180557.24453120492398739, 525846.31947262666653842 180594.65766286122379825, 525879.7240544626256451 180598.66621268156450242, 525882.55008484877180308 180599.07834211288718507))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((525882.55008484877180308 180599.07834211288718507, 526144.10206235200166702 180628.87880492309341207, 526211.97706139634829015 180640.08887598145520315, 526394.68412689818069339 180685.65199389134068042, 526375.25024652888532728 180751.41157924372237176, 526543.08072616113349795 180799.48524305276805535, 526566.20990454801358283 180735.24582871556049213, 526773.2086006454192102 180792.2867543384199962, 526781.81037810200359672 180804.0292009754339233, 526876.82089265179820359 180898.32528518006438389, 526893.50918447971343994 180930.32612565089948475, 526924.34248529304750264 180944.76673002715688199, 526972.18770328722894192 180987.68083861388731748, 526822.07183925563003868 181156.94281222127028741, 526922.36106670461595058 181052.43190333811799064, 527056.51731256174389273 181181.75928882521111518, 527072.0604500574991107 181194.33582109218696132, 527105.36620856204535812 181208.59860649338224903, 527134.84456199198029935 181207.65720116312149912, 527141.67895267263520509 181237.20603345840936527, 527126.8461934340884909 181257.45282692171167582, 527004.39505052170716226 181384.53058732440695167, 526985.91159781138412654 181369.18001979179098271, 526928.28958167461678386 181432.30053406039951369, 526997.63798668433446437 181498.45083301386330277, 526991.12956032424699515 181511.24325723896618001, 526678.53803907369729131 181414.39224837144138291, 526667.31783640081994236 181399.6772284725739155, 526656.64944697415921837 181395.44666025164769962, 526645.98105754749849439 181403.90779669350013137, 526619.08016179490368813 181431.82035006419755518, 526630.85217771399766207 181442.85661498832632788, 526625.70192074938677251 181459.04313687709509395, 526679.9176372914807871 181475.29189143585972488, 526705.68373186374083161 181482.08222587691852823, 526706.45631411974318326 181479.08550615585409105, 526686.25770194770302624 181472.89795374975074083, 526671.31848243589047343 181522.68559793970780447, 526666.90397646627388895 181521.94984694477170706, 526673.52573542075697333 181504.29182306613074616, 526671.31848243589047343 181502.8203210762294475, 526664.32884798396844417 181521.58197144727455452, 526672.42210892832372338 181534.0897383613337297, 526664.69672348140738904 181552.11563773744273931, 526615.76928231760393828 181537.7684933360433206, 526607.67602137324865907 181540.71149731581681408, 526667.6397274611517787 181562.3241827923047822, 526633.05943069886416197 181671.21533004395314492, 526634.16305719129741192 181721.7062420719594229, 526742.32487509062048048 181719.08851347386371344, 526749.72303723508957773 181718.96316810802090913, 526747.44774530804716051 181725.1558509673923254, 526745.80791060253977776 181720.21680638659745455, 526614.1888072743313387 181722.68839901124010794, 526608.25850433309096843 181744.71523850716766901, 526605.99934130790643394 181752.33991371729644015, 526446.30086804460734129 181920.76268879341660067, 526376.42578245303593576 181996.86867373716086149, 526253.96636714844498783 181892.34601317506167106, 526219.61745367909315974 181921.09456031789886765, 526171.9210004648193717 181960.76382179747452028, 526080.54168990370817482 182039.16895036882488057, 526092.26835894433315843 182054.09146642521955073, 526106.13131886860355735 182090.02748875319957733, 526381.77541522704996169 182309.68137803877471015, 526390.42294119927100837 182322.36665932871983387, 526288.06584389437921345 182450.834574355132645, 526191.83267548796720803 182572.23641757547738962, 526248.36124993639532477 182619.61274663705262356, 526103.13665034133009613 182779.77704090779297985, 526036.37909575458616018 182871.56867846462409943, 526166.79859251785092056 182977.49245963362045586, 526362.76431727269664407 182717.9993845462158788, 526568.42065479012671858 182878.4328625048219692, 526567.34392003866378218 182903.1977617870143149, 526584.30249237327370793 182884.75867916931747459, 526641.10025050956755877 182928.09725291316863149, 526696.1483146749669686 183016.25491068401606753, 526738.14096997957676649 183080.85899576800875366, 526799.24566712148953229 183168.34369431925006211, 526821.85709690093062818 183181.26451133604859933, 526845.63949992938432842 183154.3195547133218497, 526846.27791611000429839 183154.20463980082422495, 526851.96460711781401187 183153.18103541940217838, 527089.65806536294985563 182846.11161946220090613, 527159.99787061079405248 182839.75561296389787458, 527206.71119945566169918 182882.25472003052709624, 527209.41581725038122386 182908.01976323217968456, 527213.6862663998035714 182915.9912683111615479, 527203.90023362345527858 182922.97789460717467591, 527163.95716502459254116 182973.89433370024198666, 527185.46497119322884828 183029.63905581075232476, 527126.6477053442504257 183105.13584481080761179, 527112.16285629197955132 183116.54815012478502467, 527123.57516160595696419 183143.7621089503809344, 527053.78452526277396828 183235.06055146208382212, 527149.31445503246504813 183306.12010162867954932, 527157.71220760734286159 183299.49029696427169256, 527157.7350565199740231 183299.47225834906566888, 527372.2451753921341151 183478.31646749860374257, 527603.46507797553204 183601.90996593536692671, 527662.58712028060108423 183506.32227007864275947, 527655.90415950608439744 183492.21379733242793009))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((527655.90415950608439744 183492.21379733242793009, 527654.68629352480638772 183489.6427469274494797, 527558.99850281549151987 183445.7492649506602902, 527464.80590493814088404 183378.65690534905297682, 527529.78861410322133452 183281.50301839754683897, 527962.42357370757963508 183483.62205357951461338, 527973.56080347381066531 183488.82516092201694846, 528248.28510450641624629 183588.52026548737194389, 528303.09698454267345369 183598.97112996794749051, 528344.76732492458540946 183589.8908444368862547, 528360.00343477982096374 183621.74180270021315664, 528384.43865157361142337 183633.31768803694285452, 528392.23448110034223646 183625.76139408763265237, 528384.47060682089067996 183632.05436160630779341, 528361.53645626234356314 183620.09746778081171215, 528348.20271571911871433 183580.91116915637394413, 528292.58456641039811075 183591.77239997015567496, 528257.98622214375063777 183557.36140638464712538, 528521.85076717485208064 182678.38405832633725367, 528341.94312283548060805 182630.40868650248739868, 528329.949279879569076 182503.61663239658810198, 528247.70578532433137298 182419.65973170485813171, 528153.46844781318213791 182414.51951329517760314, 528153.46844781318213791 182339.12964328628731892, 528192.87678895425051451 182330.56261260344763286, 528194.59019509085919708 182289.44086532585788518, 528239.13875464152079076 182184.92309099534759298, 528055.80429802893195301 182126.66728235210757703, 527857.0491861873306334 182243.17889963858760893, 527835.18695252947509289 182239.66741698305122554, 527838.772610142827034 182227.64257323095807806, 527823.08229359821416438 182224.95575459097744897, 527811.03382629505358636 182221.05085970158688724, 527781.70427009277045727 182243.19124876931891777, 527668.77023004030343145 182337.87599429336842149, 527639.32060709642246366 182349.04721267713466659, 527584.9030367435188964 182332.47174584548338316, 527408.28049158933572471 182270.47011755546554923, 527357.30311246565543115 182249.0471085372264497, 527366.05996286729350686 182222.77655733237043023, 527350.84845480835065246 182220.83466268656775355, 527361.52887536038178951 182227.30764483928214759, 527348.90656016254797578 182272.61851990822469816, 527335.63694674952421337 182287.83002796708024107, 527307.47947438526898623 182274.23676544640329666, 527292.26796632644254714 182256.1124154188146349, 527242.83056513511110097 182307.89627264047157951, 527172.35597194754518569 182242.92371428263140842, 526900.49072153388988227 182418.98882883627084084, 526755.78376343683339655 182547.31084604043280706, 526721.96971074212342501 182518.14893207367276773, 526721.42847167002037168 182510.27474968624301255, 526639.36008041724562645 182453.71151223586639389, 526728.61123994365334511 182341.94567091023782268, 526635.31149883137550205 182260.91681474831420928, 526629.98235425702296197 182258.85755792172858492, 526577.14322044944856316 182220.11298631975660101, 526583.50453914981335402 182213.9761393434018828, 526612.02737233357038349 182233.3108826142270118, 526628.28531093138735741 182249.45831946312682703, 526730.51656499120872468 182139.8360750732535962, 526693.837565878755413 182097.80319830903317779, 526684.65127594629302621 182088.79316362290410325, 526699.03030984883662313 182072.19530309486435726, 526716.57443575479555875 182074.75238155253464356, 526722.84627124748658389 182066.73337691847700626, 526798.51334596984088421 181991.13818491756683215, 526866.75974808703176677 182069.62223492347402498, 526882.31688596680760384 182087.82361979689449072, 526934.9228784617735073 182045.90755342398188077, 526939.83839354338124394 182039.90649309137370437, 526939.83839354338124394 182025.22802654595579952, 526953.29365454334765673 182027.91907874596654437, 527063.01316396985203028 181911.23626593552762643, 527121.54787396104075015 181813.50358696334296837, 527023.0907087258528918 181748.39970547880511731, 527054.7895969923119992 181712.22981796885142103, 527075.97658408165443689 181714.24235780647723004, 527080.78246395441237837 181701.94142769221798517, 527079.6564745232462883 181686.00343252817401662, 527105.82488133199512959 181658.69750754616688937, 527442.20734915044158697 181314.52695137952105142, 527459.12822526623494923 181326.29444383695954457, 527468.89448804350104183 181332.78180451109074056, 527419.56431302148848772 181385.23810306136147119, 527473.52474095020443201 181423.3884920031123329, 527541.4968345935922116 181469.99792764431913383, 527513.48277443449478596 181503.55932644888525829, 527548.78461593028623611 181469.69239985276362859, 527597.29704240849241614 181303.15504638879792765, 527520.45864899968728423 181278.72603273176355287, 527493.44284569495357573 181267.15421134524513036, 527387.01661669730674475 181170.06974426365923136, 527429.41461164352949709 181120.02025737526128069, 527508.38860920432489365 181143.15408535901224241, 527552.0115922475233674 181044.38326500484254211, 527617.38904907600954175 181065.27134975808439776, 527665.90049312810879201 181080.65138910515815951, 527891.34266930283047259 181143.2742158203618601, 527899.13187455991283059 181119.94490523042622954, 527904.33462368953041732 181097.01015329896472394, 527820.96005753811914474 181078.33706724832882173, 527844.18837801553308964 181002.66209630461526103, 527853.80389859748538584 180991.36529486137442291, 527884.2926319494144991 180989.82570853206561878, 527897.81294143584091216 180972.85507457796484232, 527908.1319633579114452 180946.21514748636400327, 527918.58895030023995787 180920.68108835321618244, 527941.45521559938788414 180855.90905671450309455, 527959.02194552542641759 180867.80684457015013322, 527979.60677813622169197 180868.6474805666366592, 528095.75816618301905692 180907.32333309669047594, 528218.68883095902856439 180948.86776828416623175, 528232.99101356463506818 180949.5488245987216942, 528249.33636511373333633 180901.53435442302725278, 528274.28005263407249004 180832.49227053558570333, 528413.89659711671993136 180874.71776203761692159, 528440.4577933840919286 180872.67459309397963807, 528441.88889231265056878 180868.47956919606076553, 528480.12932370661292225 180756.38422738478402607, 528315.31369558570440859 180703.26183484998182394, 528079.46642620186321437 180632.41520988091360778))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526692.80084780836477876 179647.72075017780298367, 526544.65379679470788687 179640.67684462433680892, 526514.23908054397907108 179631.71659103041747585, 526459.01828505133744329 179636.29050092305988073, 526411.9174515149788931 179628.55661391041940078, 526397.78921595867723227 179626.15454808797221631, 526395.30093265138566494 179643.52499421581160277, 526402.44541665085125715 179662.16024893836583942, 526431.23864846909418702 179657.35777275226428173, 526403.68164814496412873 179659.45682299701729789, 526399.58064635645132512 179645.06697337637888268, 526397.66759617673233151 179639.57072356637218036, 526399.69519630237482488 179630.99646285979542881, 526407.86559560417663306 179609.58792857639491558, 526407.1355080088833347 179595.46081518297432922, 526405.31812318519223481 179578.4985568281263113, 526414.70794477441813797 179560.47615732613485307, 526438.29747225344181061 179421.98284034681273624, 526447.2566591496579349 179400.3794134950148873, 526443.27324291132390499 179425.80230685905553401, 526661.83190965442918241 179456.92559352092212066, 526673.60955778870265931 179451.2058947991754394, 526704.50509979214984924 179464.53338350655394606, 526797.19172580249141902 179477.86087221393245272, 526803.85547015618067235 179464.53338350655394606, 526815.97136898105964065 179467.18373637451441027, 526825.3611905702855438 179410.5419093681848608, 526856.86252751504071057 179206.38901416890439577, 526873.82478586991783231 179087.65320568502647802, 526866.85814404557459056 179082.8068461550574284, 526876.24796563480049372 179074.02281950702308677, 526883.21460745914373547 179027.98240397247718647, 526875.03637575230095536 179024.65053179563255981, 526886.56871603394392878 178986.79712720314273611, 526902.37576597684528679 178869.52358519978588447, 526856.64449148019775748 178854.26221120113041252, 526815.01278510922566056 178840.01978533738292754, 526811.13741514587309211 178827.26046769024105743, 526810.19336951395962387 178822.06821671460056677, 526763.22709932515863329 178814.75186306712566875, 526748.59439203015062958 178818.29203418685938232, 526534.17802787688560784 178780.17619179750909097, 526556.36310022731777281 178626.76877660810714588, 526549.1273886983981356 178624.33518190018367022, 526544.750046381726861 178654.78625888586975634, 526525.05200595653150231 178786.96296492687542923, 526529.61966750444844365 178803.71105726901441813, 526515.91668286081403494 178835.68468810399645008, 526497.6460366693791002 178969.6694268410501536, 526535.70988290151581168 178952.9213344989111647, 526864.20087588473688811 179005.0688038369116839, 526904.39858746575191617 179011.78256420639809221, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527770.03632687916979194 179164.03159300866536796, 527739.41564339946489781 179158.49662950204219669, 527737.28947808116208762 179153.9753308377112262, 527736.19962250639218837 179161.69230536534450948, 527771.59785052062943578 179169.64108689734712243, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528282.42500657623168081 179806.61658668008749373, 528307.96808183658868074 179740.1390959385316819, 528324.99679867678787559 179729.00493492765235715, 528282.03859719191677868 179662.78071852284483612, 528265.95217516226693988 179622.08936450752662495, 528267.10970970639027655 179566.52770638960646465, 528306.18395167891867459 179499.6337649634515401, 528343.33046841598115861 179469.3338732514239382, 528348.40521787817124277 179448.48920341735356487, 528386.22882526856847107 179444.91777596104657277, 528521.88698721944820136 179589.55984161066589877, 528355.56430925149470568 179756.63511088167433627, 528333.7391614638036117 179823.61573685068287887, 528366.82284218922723085 179832.14097995104384609, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528527.81361586402636021 179811.23436799447517842, 528529.98316993506159633 179822.87106710238731466, 528536.09736777131911367 179823.8572280437219888, 528543.93099439248908311 179824.1739670438983012))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((528533.86825586541090161 179825.01659448479767889, 528599.09828376933000982 179804.26158560626208782, 529067.56848417001310736 179787.9540786303114146, 529126.86850953719113022 179829.46409638732438907, 529184.68603427021298558 179833.91159828985109925, 529236.57355646649375558 179804.26158560626208782, 529461.54302770318463445 179967.33665536600165069, 529365.1804864815203473 180130.41172512577031739, 529332.56547252961900085 180117.06921941813197918, 529176.88434407091699541 180335.52529085575952195, 528968.42684971622657031 180655.33458768369746394, 528933.41540621093008667 180638.92297354058246128, 528917.00379206787329167 180629.07600505475420505, 528956.39166601130273193 180565.6177637014479842, 528889.09824919363018125 180520.36887541532632895, 529037.60859426553361118 180322.19037864034180529, 528980.81174594059120864 180277.24678561804466881, 528985.75060231669340283 180264.89964467784739099, 528967.47683372523169965 180262.43021648982539773, 528869.68747747887391597 180180.56867205633898266, 528753.13046700344420969 180299.10122508218046278, 528749.46897789079230279 180304.32965189014794305, 528768.29435105295851827 180318.41158448159694672, 528778.68045006087049842 180329.09107490163296461, 528777.89595665864180773 180339.10883718938566744, 528786.29993801447562873 180331.19731133786262944, 528766.49707728379871696 180311.67933983076363802, 528735.71864135982468724 180290.81664662051480263, 528713.38623358681797981 180285.77175626676762477, 528668.77996420615818352 180275.46013541670981795, 528678.81986454653088003 180236.4348891912959516, 528685.54394682915881276 180209.20438540610484779, 528648.68728152720723301 180200.38155767129501328, 528657.51626427297014743 180164.64456824841909111, 528561.08355491538532078 180139.08601459197234362, 528473.16496016969904304 180096.57592482483596541, 528471.71575256390497088 180078.58159705405705608, 528455.77446890133433044 180078.09852785218390636, 528452.87605368986260146 180092.59060390916420147, 528456.2575381031492725 180107.5657491680176463, 528445.63001566135790199 180136.06683208007598296, 528434.51942401775158942 180130.75307085920940153, 528435.00249321956653148 180119.15941001361352392, 528434.03635481582023203 180138.48217808958725072, 528458.18981491075828671 180158.28801536746323109, 528508.42901190835982561 180176.64464503963245079, 528492.97079744748771191 180232.19760325804236345, 528463.50357613165397197 180225.43463443146902137, 528442.73160045000258833 180280.1422215465863701, 528368.29083982005249709 180530.61085074103903025, 528399.42485451779793948 180540.37256290816003457, 528373.18561336421407759 180528.66321234643692151, 528398.20391442335676402 180451.73774791724281386, 528402.87839129334315658 180453.56406502836034633, 528495.6276780579937622 180483.51435554612544365, 528631.8531929935561493 180596.55254879055428319, 528664.70189872267656028 180554.04245902341790497, 528713.73342271556612104 180597.76022179532446899, 528701.17362346616573632 180617.08298987129819579, 528701.17362346616573632 180635.4396195434674155, 528716.6318379269214347 180666.35604846503701992, 528751.41282046365085989 180679.88198611821280792, 528786.19380300038028508 180647.03328038906329311, 528882.80764338024891913 180721.42593748154467903, 528908.89338028279598802 180749.44395119170076214, 528941.25901681010145694 180770.21592687338124961, 528984.08419391023926437 180821.70737133437069133, 528974.05492355371825397 180859.35868258221307769, 528989.1841545554343611 180829.86192138504702598, 529040.11857240251265466 180898.90430847753304988, 529064.22407606989145279 180876.05281915218802169, 529116.11744003393687308 180788.13860499695874751, 529191.0602760020410642 180677.82465982373105362, 529192.20589897234458476 180667.51405309184337966, 529243.27595739718526602 180675.42673247310449369, 529253.40125929773785174 180655.48501190464594401, 529245.96676619641948491 180680.13564787179348059, 529287.00160038517788053 180692.91698966833064333, 529105.37200643471442163 181014.1322900807717815, 529080.35383750754408538 181057.74321855726884678, 529150.25737489317543805 181094.96458261978114024, 529105.31938657385762781 181161.35024718247586861, 529063.5588317719521001 181143.64740329908090644, 529046.76382603647653013 181133.20726459860452451, 529038.72230120946187526 181129.90637958364095539, 529016.40501055552158505 181225.42438358269282617, 528860.85349469736684114 181191.94844760172418319, 528730.96686309122014791 181161.59693231229903176, 528681.95751262735575438 181150.4457873418868985, 528719.83069236215669662 181094.50466865097405389, 528670.49132059747353196 181063.23323584237368777, 528656.24544565135147423 181091.03006500555784442, 528636.09274450805969536 181115.69975088789942674, 528619.76210737472865731 181137.24229348936933093, 528607.94845498027279973 181141.41181786387460306, 528598.91448550228960812 181161.91197937171091326, 528542.97336681128945202 181222.54381298396037892, 528630.5333786754636094 181247.56095923084649257, 528643.38941216340754181 181213.50984350591897964, 528660.41497002588585019 181220.80651116126682609, 528688.33952496037818491 181230.55820254873833619, 528679.86120436212513596 181260.31371245899936184, 528667.46310047351289541 181267.8903315020725131, 528633.75722163496538997 181366.41482741927029565, 528463.70207082328852266 181314.08507524349261075, 528428.78978234506212175 181348.55440134933451191, 528409.40016961458604783 181407.56676936079747975, 528378.71507131354883313 181399.79127068642992526, 528367.57113712374120951 181397.15591765905264765, 528327.16320699045900255 181385.98296514025423676, 528308.22175984270870686 181356.13857025865581818, 528284.80718849156983197 181340.66114173838286661, 528256.63033144187647849 181343.0422845876601059, 528236.78747436462435871 181362.88514166491222568, 528124.47690330736804754 181327.56485606741625816, 528100.04183234507218003 181315.23161206592340022, 528077.21998848498333246 181309.38646938232704997, 528120.39353655825834721 181328.79462172722560354, 528099.23992964578792453 181396.49718135065631941, 528083.2094619075069204 181447.06752287576091476, 527892.05577444343362004 181391.53930473059881479, 527886.54702264338266104 181381.62355149036739022, 527894.36945019953418523 181395.8361311347107403, 528096.21011615579482168 181454.44925028792931698, 528174.43439171742647886 181477.365657776419539, 528210.57180352613795549 181486.17966065660584718, 528186.33329560561105609 181562.09026046219514683, 528058.53025384293869138 181521.54584721333230846, 528025.91844318632502109 181610.126576159207616, 528008.71294296334963292 181668.53094684361713007, 528092.33064007223583758 181691.78074555195053108, 528060.10723484493792057 181786.81939641226199456, 528111.16470766742713749 181801.12569479394005612, 528229.73017954116221517 181814.84780309765483253, 528238.68286890105810016 181821.33241880481364205, 528233.97450602473691106 181880.77550011838320643, 528312.01526012923568487 181886.28911337567842565, 528336.83830706239677966 181958.7224278392677661, 528346.83872474473901093 181961.95785708940820768))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((528346.83872474473901093 181961.95785708940820768, 528351.42447949468623847 181963.4414836261421442, 528343.88806465221568942 181967.13308218619204126, 528356.90300176513846964 182021.63313134637428448, 528360.15673604339826852 182079.38691478478722274, 528255.16213896812405437 182063.02837978929164819, 528103.70979977981187403 182011.23638814975856803, 527993.06327218632213771 181982.20148374579730444, 528054.27198957849759609 181792.29751440085237846, 528047.20944526395760477 181784.45024294030736201, 527955.99687798251397908 181751.91292813932523131, 527952.44751808664295822 181758.68897884970647283, 527941.10340294241905212 181748.7705221853684634, 527752.98447521112393588 181691.77686399561935104, 527549.82001883175689727 181624.62000102378078736, 527503.58740099950227886 181751.36114301218185574, 527479.05319745594169945 181810.98149478450068273, 527449.22437855799216777 181845.582924706133781, 527393.44448721886146814 181959.82730108534451574, 527344.62620919058099389 181935.31162831617984921, 527346.5051257333252579 181939.60629469942068681, 527396.22930995177011937 181966.38085543247871101, 527419.84997505962383002 181915.38169213145738468, 527486.41730399988591671 181949.20218989948625676, 527482.96182583621703088 181958.41679833593661897, 527528.6399562283186242 181968.15795582588179968, 527569.11841471691150218 181981.09131695271935314, 527585.04652358556631953 181978.72184621190535836, 527591.99038922868203372 181992.01720981305697933, 527591.46384017518721521 181998.99398477206705138, 527600.46228416555095464 181983.46020101421163417, 527671.37066017126198858 182008.93864325288450345, 527672.00585366494487971 182009.53293042359291576, 527672.91207058762665838 182009.79258584204944782, 527742.12486925080884248 182029.11416199523955584, 527811.41948285070247948 182045.82072442839853466, 527815.11899438232649118 182051.27116669819224626, 527820.06026732875034213 182037.87445605464745313, 527847.26226369361393154 181951.43140346015570685, 527927.21323233155999333 181975.30975012294948101, 528269.95467810390982777 182084.54117023901198991, 528507.92312907101586461 182120.20857272588182241, 528831.99491885420866311 182222.19505171180935577, 528823.07806823251303285 182344.80174776044441387, 528847.59940744226332754 182369.32308697016560473, 528823.07806823251303285 182398.30285149076371454, 528816.39043026615399867 182670.266795453208033, 528800.78594167821574956 182841.91616992131457664, 528606.84444065578281879 183463.86650078624370508, 528658.11633173062000424 183599.84847276745131239, 528633.59499252098612487 183633.28666259889723733, 528604.24853495263960212 183671.01782232944970019, 528627.80092093267012388 183660.77765451229061, 528647.1594083410454914 183636.01462974661262706, 528664.55382729053962976 183620.91758688475238159, 528702.78872932109516114 183664.2395359665970318, 528761.45386870275251567 183741.77597892552148551, 528769.94595531257800758 183759.78576646986766718, 528818.92929546756204218 183815.98943147188401781, 528876.9750076774507761 183846.2940231827669777, 528923.7981087981024757 183868.95036243469803594, 528962.26051460986491293 183871.43938000165508129, 528970.91118134488351643 183879.29152365346089937, 528993.43618665123358369 183886.51150319766020402, 529035.75791006267536432 183811.45033337359200232, 528956.97029918350744992 183772.32270229508867487, 528928.22346818703226745 183829.55018992690020241, 528922.63380660430993885 183889.97176989167928696, 528941.92318019969388843 184098.53460018764599226, 528863.38120412628632039 184095.51375495406682603, 528708.33693763334304094 184000.71587241004453972, 528724.42232338106259704 183964.10698729282012209, 528701.76598412916064262 184001.86755271273432299, 528789.37049590330570936 184060.77403476776089519, 528689.63087926781736314 184162.2935707290598657, 528691.49826807086355984 184184.03894319324172102, 528710.63466808956582099 184213.17846140338224359, 528791.45426438504364341 184306.83684223380987532, 528956.13032546907197684 184285.44605525681981817, 529003.7386343190446496 184310.71759315161034465, 529085.40256406948901713 184166.4398523555137217, 529106.88706586312036961 184179.02949331066338345, 529160.12714608758687973 184168.68103781942045316, 529164.48439050489105284 184164.86844895425019786, 529180.99500393983907998 184154.38365939242066815, 529137.3034288139315322 184069.37328925836482085, 529098.63988687307573855 184040.28537339897593483, 529197.46968787396326661 183851.66075099032605067, 529231.8759383208816871 183807.63561239538830705, 529366.40293027937877923 183902.40006897028069943, 529470.80148133041802794 183700.60958103262237273, 529532.41350877098739147 183585.44640055124182254, 529538.36414308042731136 183573.78315730480244383, 529529.43819161620922387 183570.68882746392046101, 529518.60803717316593975 183578.90070281090447679, 529450.281529710162431 183705.0832505801517982, 529321.97175762639380991 183640.23852705396711826, 529418.54900543135590851 183463.64013106780475937, 529410.27095561951864511 183361.54418338829418644, 529378.53843134071212262 183277.38401030114619061, 529300.0293472099583596 183204.18649908609222621, 529248.55052252893801779 183171.68790031166281551, 529171.72482365590985864 183152.15465962985763326, 529162.35992088436614722 183162.69077780697261915, 529164.55778478819411248 183210.37992642441531643, 529162.58233259071130306 183288.01632287859683856, 529163.35543786408379674 183347.00887900387169793, 529165.64832443615887314 183368.61479538556886837, 529209.96307325642555952 183366.53984011086868122, 529238.56352939270436764 183320.99361840856727213, 529307.53664107876829803 183228.71848092431901023, 529332.4133849231293425 183210.28397338639479131, 529655.02802976139355451 182747.87247683008899912))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((529655.02802976139355451 182747.87247683008899912, 529725.18133759195916355 182647.32001716547529213, 529758.11947344534564763 182602.45964416163042188, 529772.86156971787568182 182573.57162642496405169, 529786.14614357193931937 182535.41119721299037337, 529721.72104365052655339 182498.97087032342096791, 529662.05603224551305175 182458.96742579058627598, 529465.69317875348497182 182347.95250755702727474, 529447.2254714909940958 182321.03347663194290362, 529485.62160862435121089 182274.29035316518275067, 529327.0288682907121256 182182.47350349830230698, 529281.95514209056273103 182262.60457229847088456, 529271.27928321424406022 182255.78608057467499748, 529184.98289716511499137 182225.79025960189756006, 529254.93800170661415905 182123.0347249869373627, 529194.03950407542288303 182072.44127056252909824, 529292.80413319286890328 181924.86280826764414087, 529215.98652011051308364 181870.62796054553473368, 529193.31721052876673639 181845.4344820223050192, 529136.51610650331713259 181827.80988931999308988, 529055.08064286154694855 181793.40041071106679738, 529048.18442968558520079 181784.34046519559342414, 529038.80868799472227693 181788.7224668295821175, 529002.77593848691321909 181776.43501262343488634, 529014.08187095657922328 181735.5730537639465183, 529044.40527507243677974 181648.47109775303397328, 529115.73285259760450572 181668.03016941447276622, 529137.29936532687861472 181681.75431387854041532, 529179.25603554560802877 181720.57403679116396233, 529160.24231672799214721 181743.47910360060632229, 529140.96079503151122481 181821.17043695540633053, 528996.20386221027001739 181782.66523825988406315, 528957.45751267555169761 181764.97831311973277479, 528992.17077459231950343 181659.57102250630850904, 529022.32355210115201771 181563.27666852626134641, 528964.93600781005807221 181545.76860416625277139, 528936.72857078560627997 181511.7251456884550862, 528878.36835625220555812 181539.93258271290687844, 528856.96961092331912369 181541.87792319734580815, 528842.37955728999804705 181597.32012700402992778, 528805.67882148048374802 181719.06924707361031324, 528596.42409515334293246 181654.20028191219898872, 528551.78308687021490186 181642.34251408698037267, 528507.37306858669035137 181777.43956236285157502, 528766.16571141825988889 181854.68164780738879927, 528777.9935695423046127 181857.12154139997437596, 528783.85590929095633328 181838.53742159798275679, 528772.98604363994672894 181835.13982246746309102, 528765.42155704949982464 181856.89868191126151942, 528912.88206116098444909 181899.58461731197894551, 528933.9016505628824234 181842.99341507619828917, 528977.55772085906937718 181853.66489892636309378, 528886.68841898324899375 182145.02874586603138596, 528881.19098790897987783 182154.40671652223682031, 528855.96748062665574253 182141.14820628412417136, 528840.44532229914329946 182149.23266374639933929, 528839.79856570216361433 182207.44075747462920845, 528841.09207889623939991 182274.70344356057466939, 528907.70800838526338339 182267.58912099379813299, 528901.34845087071880698 182218.96412019734270871, 528914.49795431364327669 182199.37284149171318859, 528944.79199275141581893 182201.06235859365551732, 529116.82618026225827634 182275.25592555687762797, 529236.03349617577623576 182330.91525820962851867, 529228.61333048343658447 182366.16104524824186228, 529249.75958250637631863 182377.47901842225110158, 529260.6965834874426946 182345.48021171212894842, 529391.5315474170492962 182398.66071800183271989, 529324.89775743579957634 182506.92984195848111995, 529307.95238226593937725 182527.55765377206262201, 529395.9228944230126217 182579.30535354110179469, 529313.15534203872084618 182528.16323932801606134, 529338.0299911656184122 182494.00108638301026076, 529401.06366170477122068 182399.72070142376469448, 529437.38091082300525159 182410.7247426172834821, 529515.77390267443843186 182460.22066143920528702, 529694.98193959216587245 182559.66469046362908557, 529753.83678528945893049 182587.3854519649175927, 529779.14153369213454425 182575.72735903057036921, 529858.90584623115137219 182464.89736771275056526, 529886.78703951300121844 182424.94217844444210641, 529760.35582555131986737 182335.00857195170829073, 529745.32829435018356889 182335.50571294111432508, 529754.22227583988569677 182333.09009388764388859, 529844.24740195064805448 182214.70289386285003275, 529902.10613867023494095 182253.63458346226252615, 529904.80511579709127545 182251.14619939160184003, 529941.11181005125399679 182198.01181227143388242, 529940.89537670253776014 182188.48874492605682462, 529972.6108493892243132 182165.00088953139493242, 530056.9588389479322359 182048.7881039172061719, 529981.98284822911955416 181992.5561108780966606, 529951.05525205750018358 182016.92330786169623025, 529819.2849761457182467 181928.86637559026712552, 529799.05698917480185628 181958.56732936628395692, 529803.05725013604387641 181964.66939977870788425, 529801.62453686981461942 181960.81469362112693489, 529828.71775786660145968 181919.54642597923520952, 529924.09649344824720174 181787.99958944245008752, 529857.85091200319584459 181729.57684998650802299, 529698.32181283622048795 181616.30609073047526181, 529685.48704050190281123 181617.03950629243627191, 529635.51744967524427921 181690.38779020583024248, 529688.40668625489342958 181726.48536033323034644, 529692.63985970325302333 181722.80896518367808312, 529644.80728511966299266 181691.31286854337668046, 529645.71116362931206822 181681.09080057707615197, 529586.96591395325958729 181646.48816596489632502, 529515.04247384704649448 181599.24059515440603718, 529543.51227790850680321 181551.4553936262964271, 529539.00726222933735698 181538.53999719221610576, 529525.71878347580786794 181533.37225545474211685, 529491.7593377724988386 181561.79483501086360775, 529437.12892511917743832 181617.90174530341755599, 529480.68560547789093107 181649.27732013809145428, 529452.0052509990055114 181692.96711596235400066, 529415.66898023779504001 181743.18504027591552585, 529422.12033342942595482 181756.496664849226363, 529410.79081194649916142 181745.6821476363693364, 529411.79279640805907547 181742.27344958332832903, 529417.83336036605760455 181734.97711012425133958, 529445.56671970279421657 181695.34609987842850387, 529414.95451968535780907 181675.21360844530863687, 529316.29792853817343712 181612.14346808032132685, 529210.36666346830315888 181540.84275432795402594, 529292.45281272125430405 181467.24829591458546929, 529338.54938403982669115 181401.53055816600681283, 529381.24053801142144948 181306.35028045883518644, 529665.55224183772224933 181363.5063766969833523, 529664.71503826801199466 181384.86775368836242706, 529672.3439009505091235 181401.4207107936963439, 529766.81024347490165383 181438.92780598934041336, 529794.06817890249658376 181452.26089733641128987, 529984.75397409894503653 181524.94074914953671396, 529992.18142025219276547 181529.49952054413734004, 529997.79784449038561434 181531.55623927924898453))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((535514.30680333590134978 179524.80755477515049279, 535499.36235546763055027 179481.84226715381373651, 535492.82415952521841973 179444.48114748310763389, 535463.86929178040008992 179400.58183186998940073, 535399.42136034846771508 179366.95682416635099798, 535321.89703703171107918 179295.27017579812672921, 535279.8657774020684883 179283.12781190514215268, 535101.46643097442574799 179497.95425001182593405, 535066.20687428512610495 179530.64522972371196374, 535040.98811850743368268 179543.72162160844891332, 535039.12006252387072891 179587.62093722156714648, 535044.7242304744431749 179592.29107718038721941, 535036.31797854858450592 179582.95079726271796972, 535038.18603453214745969 179547.4577335755166132, 535007.3631108037661761 179563.33620943559799343, 534947.1183053347049281 179556.79801349321496673, 534869.5939820179482922 179546.52370558376424015, 534718.28144735156092793 179513.83272587187821046, 534612.26927028584759682 179486.74591411059373058, 534612.26927028584759682 179455.92299038224155083, 534527.27272303495556116 179439.11048653040779755, 534514.19633115013130009 179463.39521431637695059, 534497.3838272982975468 179460.5931303410907276, 534488.97757537243887782 179473.66952222582767718, 534374.0921323848888278 179452.18687841517385095, 534301.70496302295941859 179452.18687841517385095, 534232.58689163206145167 179457.79104636577540077, 534155.99659630702808499 179483.0098021435260307, 534136.38200847990810871 179501.69036197889363393, 534117.70144864462781698 179504.49244595417985693, 534038.3090693443082273 179541.85356562491506338, 533971.05905393697321415 179587.62093722156714648, 533905.91060151113197207 179646.46470070295617916, 533868.78298883838579059 179677.05411743334843777, 533814.60936531575862318 179702.27287321106996387, 533764.17185376037377864 179719.08537706290371716, 533735.21698601555544883 179744.30413284065434709, 533662.8298166535096243 179797.89398886833805591, 533678.24127851764205843 179824.51378663373179734, 533699.25690833246335387 179872.14921421391773038, 533728.21177607728168368 179852.41787288780324161, 533759.03469980566296726 179897.71823048856458627, 533730.91986712557263672 179854.01778862628270872, 533658.8310093138134107 179905.21964279739768244, 533619.01806616468820721 179928.97897983799339272, 533566.71249862562399358 179955.36527060542721301, 533544.2958268232177943 179960.03541056427638978, 533484.63478884904179722 179977.43168191093718633, 533469.22332698479294777 179969.49244398091104813, 533411.78060549113433808 180001.71640969690633938, 533390.76497567631304264 180012.4577316022478044, 533382.82573774631600827 180031.60530543350614607, 533351.06878602621145546 180030.67127744172466919, 533300.6312744707101956 180049.35183727709227242, 533240.85348299751058221 179885.89693871766212396, 533173.60346759017556906 179908.31361052009742707, 533147.45068382075987756 179897.1052746188652236, 533121.29790005122777075 179875.62263080821139738, 533109.15553615824319422 179875.62263080821139738, 533085.33782236813567579 179864.88130890289903618, 533063.38816456159111112 179863.01325291936518624, 533056.84996861917898059 179775.6816356890485622, 533052.97625329520087689 179769.77504887530812994, 533049.84475868125446141 179753.95276029917295091, 533085.77453898952808231 179746.86569354109815322, 533111.65057343174703419 179737.6360252050217241, 533122.52839682786725461 179734.66934609701274894, 533143.9132087315665558 179736.4823166630230844, 533227.63518259371630847 179755.64490078343078494, 533235.51463751657865942 179725.05407578885206021, 533246.17507652984932065 179690.29177465863176621, 533261.35461469017900527 179692.60926140064839274, 533329.02522755693644285 179684.26630912939435802, 533382.2115482862573117 179671.75188072252785787, 533410.02138919045682997 179667.11690723849460483, 533450.22978416446130723 179668.97089663209044375, 533452.54727090639062226 179679.63133564536110498, 533461.3537205260945484 179717.17462086598970927, 533453.93776295159477741 179668.97089663209044375, 533451.94869960669893771 179660.89830636882106774, 533430.31913536891806871 179658.49502145350561477, 533401.47971638524904847 179663.3015912841365207, 533327.77897898247465491 179679.32349071951466613, 533262.89028626913204789 179686.53334546543192118, 533246.06729186198208481 179683.32896557834465057, 533293.98835750482976437 179526.55448060017079115, 533297.79979026620276272 179471.92394435431924649, 533277.47214887232985348 179409.67054258575080894, 533267.30832817545160651 179398.23624430174822919, 533261.0353450890397653 179395.85409882574458607, 533255.47700564551632851 179411.57625896626268514, 533142.40450039238203317 179443.3381986441090703, 533048.38915894599631429 179483.99348143170936964, 532974.70145889348350465 179533.54210732915089466, 532794.61126092006452382 179654.87271689844783396, 532708.53640439314767718 179706.00943977979477495, 532693.2906733478885144 179712.36182771535823122, 532685.9464436424896121 179717.96226352726807818, 532658.78351692855358124 179728.82743421287159435, 532607.27455960412044078 179737.47932938844314776, 532548.11974142713006586 179741.40286324714543298, 532534.03526090865489095 179738.18355341436108574, 532548.52215515612624586 179713.23390221039880998, 532555.76560227992013097 179695.93011185922659934, 532523.17009022308047861 179679.43114896627957933, 532492.98906054079998285 179664.94425471880822442, 532479.7094074806664139 179651.26218792953295633, 532484.41954601428005844 179673.02428334188880399, 532449.79857150348834693 179748.49007901950972155, 532378.32551233028061688 179682.61488870403263718, 532357.40633448015432805 179686.00104389677289873, 532361.9146399162709713 179664.21872470591915771, 532197.54445065301842988 179511.6966937497491017, 532242.98194478405639529 179474.83317379461368546, 532244.69978968834038824 179458.70721855689771473, 532258.3818564775865525 179462.12773525423835963, 532327.39026551635470241 179384.03927239449694753, 532343.62657718255650252 179360.62614285058225505, 532356.44643774325959384 179329.55894946909393184, 532412.07767790672369301 179270.75782656238880008, 532414.88226228312123567 179257.70878397024353035, 532428.03560322884004563 179250.60044720803853124, 532448.61292798642534763 179227.50345003115944564, 532496.48670395300723612 179169.1310389841964934, 532506.14544822706375271 179101.51982906644116156, 532494.38697693694848567 178997.79331447216100059, 532483.8883418565383181 178999.47309608501382172, 532498.58643096906598657 179109.07884632432251237, 532488.92768669512588531 179168.71109358099056408, 532445.25697034073527902 179214.06497424640110694, 532606.87226027122233063 179362.21232334937667474, 532626.11217573913745582 179400.69215428520692512, 532679.98393904929980636 179385.30022191087482497, 532719.58761149924248457 179333.93767049448797479, 532820.3977558920159936 179207.26369896886171773, 532909.74552235088776797 179116.74030400396441109, 532941.48410618293564767 179098.9765160133538302, 532963.40215328731574118 179080.1896184952929616, 532976.27465714234858751 179080.88542951448471285, 532985.58112952392548323 179071.40500437797163613, 533037.41905045346356928 179058.18459501341567375, 533056.55385348107665777 179066.18642173407715745, 533060.32914265117142349 179065.0439605139545165, 533066.32706405699718744 179059.61726971823372878, 533052.61752941517625004 179038.19612184033030644, 533040.33607129845768213 178975.07513942685909569, 533032.33884275739546865 178967.93475680088158697, 533022.34230708109680563 178935.44601585279451683, 533014.34507853991817683 178938.30216890317387879, 533009.7752336593111977 178929.16247914195992053, 533004.63415816868655384 178922.59332712605828419, 533008.63277243915945292 178907.74133126405649818, 532948.08232777111697942 178850.76107790888636373, 532929.23171763855498284 178851.90353912903810851, 532820.69790172390639782 178835.33785143680870533, 532628.47880143311340362 178740.51357016403926536, 532649.04310339584480971 178706.81096416953369044, 532649.61433400597888976 178688.53158464707667008, 532680.4607869500759989 178677.10697244553011842, 532646.72988178418017924 178686.93224038934567943, 532644.91513582807965577 178705.68461526944884099, 532577.46707779157441109 178826.97013667138526216, 532558.10978759278077632 178818.50132220939849503, 532477.21695213438943028 178782.04142910346854478, 532465.16113808494992554 178762.56665256191627122, 532448.46847247786354274 178772.14947911410126835, 532425.90246156463399529 178760.71191193890990689, 532423.12035063013900071 178744.32836976903490722, 532352.79476867453195155 178710.47935339916148223, 532245.37437425879761577 178647.41817221697419882, 532184.94074229244142771 178616.19670506301918067, 532251.30818086618091911 178452.11467546166386455, 532511.10399071127176285 178585.03346189408330247, 532598.70955449633765966 178413.85017633717507124, 532702.58256901206914335 178176.74428570797317661, 532815.09900265594478697 177890.48924129054648802, 532856.91221495741046965 177792.91708755856961943, 532858.8989350259071216 177769.61827948209247552, 532770.30928106070496142 177726.3168125337397214, 532588.16317295876797289 177673.66873071744339541, 532472.21096532221417874 177646.21587158855982125, 532427.41945832245983183 177643.32609694340499118))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((524044.91210958641022444 175488.04344289214350283, 524085.52461603935807943 175461.19657479849411175, 524103.28008306899573654 175495.27063632552744821, 524138.79455675766803324 175591.48109126661438495, 524129.17100038880016655 175633.29742638493189588, 523976.51973626675317064 175725.69477560109226033, 524005.3036557876621373 175719.74511276691919193, 524151.31351847440237179 175627.49342679663095623, 524325.26564783230423927 175881.45175875423592515, 524265.40427828562678769 175894.51242120077949949, 524182.68674945743987337 175922.81052316830027848, 523924.7386661380296573 176107.83657449448946863, 523885.55667879834072664 176168.78633257842739113, 524033.5775198593037203 176344.0168870696797967, 524088.59564563841558993 176404.0004238125984557, 524217.18918832298368216 176480.86513136423309334, 524234.28227358422009274 176458.37422970472835004, 524314.94964086962863803 176518.34996746337856166, 524328.14430317643564194 176505.15530515648424625, 524406.35059385467320681 176563.87137158666155301, 524530.42688709695357829 176645.50051187761710025, 524556.54821199004072696 176598.69980477745411918, 524615.32119299960322678 176566.04814866106607951, 524656.19633344910107553 176622.45522326184436679, 524673.86358512495644391 176669.64518129741190933, 524687.07387990888673812 176707.38888068028609268, 524697.76792806736193597 176718.08292883876129054, 524791.82018601219169796 176798.60282085544895381, 524894.62324445182457566 176690.62037168533424847, 524947.35885916277766228 176642.90719647065270692, 524977.49349614046514034 176666.13597914096317254, 524900.58739135367795825 176605.86670518555911258, 524870.45275437599048018 176633.49012241512537003, 524732.33566822810098529 176495.37303626732318662, 524628.43395114876329899 176566.94279908936005086, 524566.90906731935683638 176469.00522891184664331, 524555.92248092114459723 176450.17108080073376186, 524611.16931538027711213 176409.99156483047408983, 524670.51981275726575404 176371.66103527450468391, 524673.61098449560813606 176338.27638049997040071, 524636.5169236350338906 176296.23644485796103254, 524565.41997365222778171 176214.62951096461620182, 524571.60231712902896106 176203.50129270643810742, 524604.68284478283021599 176174.72198301905882545, 524588.03502420790027827 176155.80400509302853607, 524535.064686015015468 176062.22307428557542153, 524514.25491029641125351 176016.81992726307362318, 524478.18463238410186023 176002.69450374494772404, 524412.60230890719685704 175996.64075080861221068, 524397.46792656637262553 175964.35406848150887527, 524407.55751479358877987 175947.20176849522977136, 524409.57543243898544461 175893.72695089096669108, 524410.77357104083057493 175873.16941487803705968, 524408.75565339543391019 175849.71112224974785931, 524414.93552618462126702 175841.26109210946015082, 524437.00650043168570846 175835.45957887879922055, 524651.41025026002898812 175810.99232742778258398, 524731.11799725505989045 175799.89378037783899345, 524754.32405017770361155 175993.61387434042990208, 524753.31509135500527918 176084.42016838540439494, 524796.70032073196489364 176103.59038601713837124, 525047.12265628203749657 176180.61843837762717158, 524992.33966347749810666 176361.30496533127734438, 525128.8617562991566956 176407.8115966334589757, 525215.05184906325303018 176421.69970128277782351, 525318.75507486017886549 176515.06803950533503667, 525329.99290352826938033 176505.92964351741829887, 525213.53843648789916188 176411.26652987388661131, 525090.62899151816964149 176387.06088406970957294, 525061.77148157625924796 176376.93670005700550973, 525085.56370682967826724 176240.99830333300633356, 525104.72513684059958905 176197.52988835732685402, 525071.38045466400217265 176177.87953445233870298, 525184.4233297451864928 175922.32358751614810899, 525232.21329014201182872 175831.17452397785382345, 525394.0406293993582949 175972.00136882782680914, 525380.45207419455982745 175992.38420163505361415, 525579.64794026513118297 175772.49667195708025247, 525789.04116105276625603 175920.79213703639106825, 525794.67906692263204604 175913.40021600711042993, 525796.36541037389542907 175924.88107120373751968, 525831.44916197401471436 175948.5820945069717709, 525842.88386619929224253 175956.48243560802075081, 525966.89843111461959779 175827.58213343276293017, 526037.0428866392467171 175909.39836246441700496, 526083.99901098641566932 175909.39836246441700496, 526183.90565853379666805 175950.36008795883390121, 526213.87765279808081686 175990.32274697776301764, 526258.58368871151469648 176103.28294610444572754, 526151.85186089854687452 176147.91625591710908338, 526151.49614943633787334 176179.64869351152447052, 526047.38884781103115529 176231.98070609322167002, 526018.99594736774452031 176239.218112088565249, 526012.31526491045951843 176231.42398255510488525, 525961.23868289159145206 176229.001861541881226, 525788.46569891297258437 176403.76074188807979226, 525739.81123790750280023 176436.52803195299929939, 525728.0358450491912663 176477.41611387868761085, 525702.36593637219630182 176520.02743093523895368, 525681.16035963909234852 176514.67023260265705176, 525672.11343565175775439 176513.5143718154868111, 525598.1237177683506161 176794.07800558168673888, 525590.47065528121311218 176803.15163323399610817, 525576.05627165164332837 176800.20250201458111405, 525603.30556521995458752 176824.95719950424972922, 525545.77949344262015074 176885.87943373149028048, 525467.20725123130250722 176931.41561955848010257, 525439.5283931796438992 176951.95154650005861185, 525403.81373762898147106 177049.27398287542746402, 525403.81373762898147106 177092.13156953614088707, 525397.56367290765047073 177140.34635452943621203, 525389.52787540876306593 177153.73935036090551876, 525384.84032686776481569 177171.15024494181852788, 525401.57936285785399377 177193.54199610272189602, 525396.49806739354971796 177201.56509420418296941, 525394.6260111698647961 177214.66948776991921477, 525487.42651254346128553 177227.50644473225111142, 525492.50780800764914602 177223.22745907813077793, 525498.9792741967830807 177209.83568196554551832))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((525498.9792741967830807 177209.83568196554551832, 525499.70685131091158837 177208.33006480569019914, 525546.48938673955854028 177091.50102327833883464, 525607.1780920778401196 177105.30195335522876121, 525641.23937251162715256 177033.56127417489187792, 525704.87392115953844041 176980.53248363500460982, 525742.65693441918119788 176954.01808836506097578, 525749.9179498142329976 176950.09361684083705768, 525759.91741443739738315 176949.90844157003448345, 525789.17510722379665822 176925.28013055364135653, 525823.06218178023118526 176907.87365509843220934, 525834.31157948146574199 176917.87311972162569873, 525840.02393209061119705 176917.83761663141194731, 525839.83007433160673827 176904.55402936117025092, 525831.35577882663346827 176898.87676776724401861, 525816.50067409395705909 176887.31365200405707583, 525759.91843862924724817 176830.72846091576502658, 525971.4164017754374072 176713.56057522911578417, 525990.28241726732812822 176704.62404157503624447, 525990.28241726732812822 176695.68750792095670477, 526044.89456737553700805 176673.8426478776964359, 526231.32058888114988804 176565.61129584512673318, 526246.21481163799762726 176558.66065855862689205, 526279.02310593228321522 176632.42519633183837868, 526283.16126619779970497 176641.72923013736726716, 526326.25483707862440497 176694.1716895958816167, 526240.12421508901752532 176797.52843598343315534, 526248.73727728798985481 176850.9294216169801075, 526278.02168876444920897 176885.38167041284032166, 526272.85385144501924515 176930.16959384744404815, 526251.69148790801409632 176959.08371336333220825, 526325.95375438174232841 177013.98570174560882151, 526319.56678607675712556 177036.69492238553357311, 526331.39291572826914489 177017.30782459620968439, 526465.45469694142229855 177118.89621701225405559, 526531.37082942517008632 177192.56718861166154966, 526549.98244330286979675 177194.89364034638856538, 526607.62827024597208947 177274.30958925650338642, 526607.62827024597208947 177288.8285534702881705, 526641.02188793767709285 177312.0588962123147212, 526727.77269911498297006 177419.49923139426391572, 526755.35873112105764449 177438.37388487218413502, 526797.46372734103351831 177454.34474550731829368, 526929.58630168635863811 177497.90163814864354208, 527031.94499939354136586 177545.81422005410422571, 527131.79582655231934041 177579.02292893503908999, 527156.87407868099398911 177613.12935183010995388, 527095.68314348696731031 177730.49557179247494787, 527136.81147697800770402 177756.57695400633383542, 527102.70505408302415162 177810.74597860436188057, 527125.77704604144673795 177823.78666971129132435, 527048.53602948493789881 177964.22488163207890466, 527053.25930870475713164 177974.33477002254221588, 527098.19096869986969978 178015.38451597469975241, 526908.94946135848294944 178337.4750089393928647, 526940.62272087635938078 178361.92182539845816791, 526883.33841691690031439 178439.4463433051132597, 526910.62494222086388618 178467.51928232313366607, 526887.60617866518441588 178499.03289314155699685, 526918.00911059393547475 178465.09473867359338328, 526914.67600807105191052 178462.40279670694144443, 526758.43816197034902871 178293.39700141816865653, 526769.00779414852149785 178281.43285661714617163, 526783.34981272195000201 178251.05608661123551428, 526764.73600135685410351 178280.00450905179604888, 526756.2519320712890476 178288.05494963173987344, 526526.90699357143603265 178031.40025283378781751, 526505.86243384412955493 178042.24138966298778541, 526524.99385177798103541 178024.38539959135232493, 526373.21793616958893836 177872.60948398287291639, 526378.31964761856943369 177863.68148894709884189, 526365.56536899600178003 177863.68148894709884189, 526501.56836159329395741 177739.12724830291699618, 526619.97851843247190118 177577.92520181008148938, 526630.38032632856629789 177565.05702568762353621, 526471.97642374865245074 177464.09629657075856812, 526468.49501929641701281 177439.7264654046157375, 526426.7181658687768504 177443.20786985690938309, 526252.64794325339607894 177363.13556745389360003, 526212.61179205193184316 177333.54362960928119719, 526188.24196088581811637 177333.54362960928119719, 526111.65106293500866741 177425.80084759538294747, 526189.54348884453065693 177335.32316621133941226, 526248.99693555117119104 177371.07838590905885212, 526381.31203635118436068 177439.0548791715700645, 526462.80067659239284694 177473.97858213211293332, 526636.94032988674007356 177583.86839270126074553, 526670.26410251285415143 177616.99946092290338129, 526688.55747073027305305 177690.17293379263719544, 526822.43166541238315403 177811.57437741738976911, 527046.55382472439669073 177968.52284097846131772, 527133.60565806506201625 178026.52744588098721579, 527152.05848008545581251 178036.42819022812182084, 527291.56621869676746428 177804.21605766733409837, 527319.9554854022571817 177819.83015435532433912, 527360.1001912277424708 177839.80410252374713309, 527353.88239083020016551 177859.14837042734143324, 527412.6060612517176196 177890.23737241525668651, 527367.00885833613574505 177998.70344601754914038, 527429.8777290228754282 178039.46458195726154372, 527368.39059175783768296 178154.83932266797637567, 527356.64585767348762602 178166.58405675229732879, 527244.18394927959889174 178092.28198195234290324, 527187.99826812464743853 178202.51293736099614762, 527130.47483265656046569 178327.19163935232791118, 527130.47483265656046569 178336.82347040742752142, 527106.47640507481992245 178384.55715666484320536, 527164.85215369169600308 178410.35007031389977783, 527154.54868436977267265 178430.37184342864202335, 527245.21691735507920384 178618.75959407596383244, 527293.66525488265324384 178710.58556358556961641, 527279.48398153169546276 178728.96806519792880863, 527296.81704342004377395 178719.65596891054883599, 527313.62467651721090078 178762.66981539080734365, 527337.94203093100804836 178751.72700590462773107, 527419.45399717660620809 178711.76451556503889151, 527479.39759952831082046 178777.611654511973029, 527424.4321250639623031 178709.32203599691274576, 527552.51673102448694408 178625.85540736871189438, 527527.96637719089630991 178599.2435734422178939, 527515.02121530997101218 178586.53641387179959565, 527538.98158421937841922 178566.8297592174494639, 527641.03992576699238271 178487.17096276683150791, 527636.13838343927636743 178480.70983878933475353, 527628.56327256909571588 178478.25906762547674589, 527637.92076246754731983 178448.62701628042850643, 527645.05027858063112944 178430.5804286191414576, 527663.09686624188907444 178407.4095012515608687, 527665.10204264870844781 178405.84991960183833726, 527659.53210818534716964 178400.50278251702548005, 527674.67989808064885437 178389.84342098905472085, 527652.43348332692403346 178373.39041538978926837, 527656.76978971192147583 178369.27718900417676196))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((530315.37161932047456503 177998.80604608487919904, 530315.56318013661075383 177999.03289441973902285, 530312.13405959820374846 178036.68039025971665978, 530327.5800858890870586 178073.0888808025047183, 530359.94318859372287989 178068.67573043366428465, 530382.17224571469705552 178064.30687938295886852, 530409.71792252280283719 178051.83336535666603595, 530457.53305962367448956 178047.15579759678803384, 530484.55909291654825211 178044.27656433341326192, 530481.82446864934172481 178176.08545401293667965, 530480.73061894241254777 178201.7909221246954985, 530453.93130112381186336 178202.88477183159557171, 530434.6485230919206515 178208.30226855166256428, 530510.72968812065664679 178204.59099220877396874, 530560.83191874937620014 178250.05412740889005363, 530576.60484320647083223 178299.22853895186563022, 530595.16122492088470608 178402.68036700924858451, 530413.80008803645614535 178436.11341032542986795, 530418.27724980388302356 178499.91296551114646718, 530508.93977559404447675 178869.27881132310722023, 530512.99918529542628676 178904.58935879755881615, 530537.61080370028503239 178893.65086172873270698, 530445.72742832207586616 178500.95881695748539641, 530401.85479763883631676 178248.42200085142394528, 530398.61737529921811074 178112.52069049383862875, 530397.05111636582296342 178067.79433303145924583, 530372.89449547010008246 178077.41707417467841879, 530341.8666145202005282 178078.87150609420496039, 530263.00199223437812179 178102.06698323713499121, 530128.67393126524984837 178193.75180186820216477, 530016.07499924581497908 178268.64121385099133477, 529986.7336030377773568 178290.67374241168727167, 529976.07911414559930563 178274.75468253748840652, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529225.49949584668502212 178821.69789721473352984, 529270.770087662152946 178758.30559268582146615, 529337.70783226401545107 178657.27980173568357714, 529306.5308305585058406 178711.19551833867444657, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529620.80678689747583121 178938.51310259819729254, 529633.90588229265995324 178955.7253200063132681, 529712.89748927822802216 179004.92786699859425426, 529720.95868967950809747 179007.69887060293694958, 529744.56234859698452055 178988.58683275303337723, 529762.83693021174985915 178665.01042368449270725, 529752.2592964896466583 178761.09022093558451161, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530189.61440031998790801 178792.12452214764198288, 530183.93791116797365248 178891.73339131372631527, 530174.20678690751083195 178981.20567270851461217, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529764.82379545003641397 178980.39474568678997457, 529726.8608069175388664 178986.4645860674791038, 529708.5995219451142475 179019.31924272864125669, 529662.33663572394289076 179123.12740439243498258, 529642.51702948904130608 179154.93664896697737277, 529570.58282343833707273 179120.13400562520837411, 529529.60315316671039909 179076.01919454638846219, 529561.16543161950539798 179129.58498098282143474, 529516.00091436528600752 179150.95722108607878909, 529517.0294774059439078 179259.9849033905484248, 529490.5439791101962328 179316.29872986389091238, 529420.08741082856431603 179303.95597337657818571, 529384.60198592755477875 179291.8703576494299341, 529375.15206299198325723 179284.92755712530924939, 529252.36735001939814538 179242.24219094007275999, 529261.78258011117577553 179194.57754063030006364, 529269.58965256006922573 179174.62613326087011956, 529296.33848912897519767 179174.14417224159114994, 529301.68539485009387136 179174.04783159797079861, 529296.33972956647630781 179174.13921049170312472, 529267.85474757140036672 179174.62613326087011956, 529239.58119475841522217 179148.36465595476329327, 529195.2201183628058061 179118.48233969206921756, 529148.38958095852285624 179107.35710484313312918, 529204.08223160775378346 179134.07865458953892812, 529185.22284631489310414 179175.21252341114450246, 529078.4996979859424755 179150.77853555406909436, 528999.59170996560715139 179155.74130209622671828, 529004.55447650782298297 179178.57002819015178829, 529008.00452898163348436 179232.70877502896473743, 528944.69158343283925205 179232.70877502896473743, 528973.09685089520644397 179300.47073837311472744, 528996.36863628611899912 179297.04841699209646322, 529001.91040330554824322 179304.25271411731955595, 529003.21327904821373522 179305.94645258274977095, 529003.64613620459567755 179307.80479111763997935, 529030.28640920133329928 179422.17657674243673682, 529184.34559951478149742 179359.33850391051964834, 529283.96327179321087897 179424.30655104867764749, 529302.73181874421425164 179444.51883238056325354, 529335.78186670539434999 179437.48325416501029395, 529384.02287575032096356 179413.93252533991471864, 529384.73062578472308815 179413.58700957507244311, 529384.76409676810726523 179413.5639608106284868))</t>
-  </si>
-  <si>
     <t>LineString (537677.74915669474285096 185252.76164181722560897, 537643.00114871666301042 185239.7001480043400079, 537316.95739506953395903 185031.778326699975878, 537229.96213505661580712 185184.60276563980733044, 537201.04272982059046626 185166.52813736733514816, 537232.9745731019647792 185196.65251782146515325, 537381.55745029193349183 184941.75541837234050035, 537351.62029182142578065 184925.45972019206965342, 537377.43642238166648895 184919.42450584482867271, 537451.04292529029771686 184780.09048736712429672, 537410.21722342562861741 184755.88968471533735283, 537356.76501582947093993 184755.25835942875710316, 537356.76501582947093993 184747.05113070338848047, 537411.69031576090492308 184747.68245598993962631, 537448.0967406197451055 184770.19972454421804287, 537473.55352781643159688 184785.3385604316717945, 537747.60077800450380892 184961.0985148370382376, 537758.58534546149894595 184966.78314978542039171, 537804.51481488952413201 184996.98240664083277807, 537864.35811839380767196 184906.36238933156710118, 537888.28139535372611135 184870.65235785552067682, 537902.61249206471256912 184864.98165376979159191, 537907.4644952624803409 184835.48672166577307507, 537967.46757289220113307 184838.46378766733687371, 538011.82434299273882061 184870.64293947687838227, 538078.40289423160720617 184929.68653100670780987, 538087.9936144461389631 184924.56079820176819339, 538119.73315815057139844 184948.990714373474475, 538135.54168771498370916 184938.64766800281358883, 538198.23536510684061795 184991.52666786056943238, 538217.03544040443375707 184970.49224639392923564, 538219.97872249479405582 184911.99294450273737311, 538277.44748879398684949 184908.84473496669670567, 538457.97480364586226642 184911.07213344739284366, 538505.90271932515315711 184912.79847530333790928, 538515.10912559076678008 184897.09912988185533322, 538525.09080817364156246 184843.70197354088304564, 538526.32566582434810698 184663.7970501403324306, 538535.63319873600266874 184619.60857876110821962, 538536.262393569923006 184571.81602369761094451, 538515.46818044490646571 184517.37803845322923735, 538477.49967075069434941 184449.00327367073623464, 538457.15434100909624249 184427.57313958508893847, 538425.17171020386740565 184374.84922809444833547, 538353.79349812655709684 184318.35783824842656031, 538316.48486082209274173 184324.74894653976662084, 538190.98032854299526662 184445.91087261610664427, 538114.62453358469065279 184373.80012300860835239, 538061.91426858631893992 184325.90183424047427252, 537967.65557023207657039 184278.89492702769348398, 537901.19514178577810526 184215.13547579868463799, 537977.30053500854410231 184073.08899729140102863, 537952.37116555206011981 184095.98202858777949587, 537924.70485076669137925 184145.06449046015040949, 537858.05490487033966929 184162.7840894281398505, 537783.67563862353563309 184141.90954871260328218, 537716.38640219438821077 184208.09989124414278194, 537652.52806460822466761 184222.53044708562083542, 537589.67334013665094972 184199.95114084909437224, 537529.27968590334057808 184136.36056276527233422, 537466.31568435055669397 184167.65469237719662488, 537441.44360490585677326 184163.61488125869072974, 537340.45030948391649872 184140.68196232168702409, 537305.82299475627951324 184147.8273495165631175, 537292.6933565727667883 184134.00420770817436278, 537293.64353717770427465 184173.76163395500043407, 537329.91342148836702108 184205.7187055399408564, 537299.37220923521090299 184236.54379842459456995, 537060.04192334006074816 184042.19927089911652729, 537029.58205211441963911 183969.99358210602076724, 536973.11503039160743356 184035.81513554195407778, 536881.89676296338438988 184157.26752178772585467, 536840.94333374209236354 184298.92676470399601385, 536804.17421305226162076 184360.56232096807798371, 536787.11574887309689075 184417.34081984456861392, 536781.21086306986398995 184436.03648271708516404, 536746.07112654484808445 184412.19589463999727741, 536728.29071210836991668 184395.55630067101446912, 536629.15679720137268305 184535.64480583346448839, 536503.18433391104917973 184625.85561704222345725, 536213.61207215348258615 184309.68219968944322318, 536153.73730594327207655 184326.93248854571720585, 536139.37114563805516809 184333.95485085935797542, 536114.35501550161279738 184335.30487016192637384, 536144.87662159639876336 184330.06202568946173415, 536135.06113926612306386 184271.20040344842709601, 535894.41512988414615393 184028.71740162841160782, 535626.21423393173608929 183916.66086290855309926, 535049.39860839024186134 183732.96161910553928465, 534847.32944020687136799 183620.90508038568077609, 534843.65545533073600382 183426.18388195446459576, 534865.6993645871989429 183304.94238104444229975, 535372.70927748351823539 183418.83591220233938657, 535729.61131596809718758 183230.43964716198388487, 535597.45816457970067859 183171.78773763249046169, 535507.29320245317649096 183158.26299331351765431, 535493.76845813426189125 183165.1987596309336368)</t>
   </si>
   <si>
@@ -326,19 +257,91 @@
     <t>E12 Holborn</t>
   </si>
   <si>
-    <t>LineString (530248.37173048651311547 182901.4726771293208003, 530247.19071921310387552 182900.21293177100596949, 530251.05921820166986436 182893.88266069884411991, 530184.08185019285883754 182852.74914162818458863, 530085.83308541483711451 182787.51840435751364566, 530111.18260209145955741 182744.29519918368896469, 529990.56694557412993163 182662.18936071105417795, 529961.50293195550329983 182710.87158352226833813, 529962.22953229595441371 182727.58339135299320333, 529962.59283246623817831 182727.22009118273854256, 529972.76523723278660327 182752.65110309905139729, 529932.80478152283467352 182814.59110673272516578, 529979.07706384977791458 182754.49032623908715323, 529993.03934241353999823 182732.28046154495677911, 529968.62376257998403162 182714.22668772435281426, 530013.09155612858012319 182629.12904521985910833, 530018.17775851185433567 182621.49974164497689344, 530100.32880480831954628 182494.38274551162612624, 530104.0113532249815762 182482.84132467227755114, 530220.50368910923134536 182556.47051627180189826, 530255.09743770561181009 182478.63458192982943729, 530272.39431200386025012 182483.35191128388396464, 530279.47030603489838541 182470.7723663397191558, 530137.95042541308794171 182415.73685720900539309, 530133.8373461066512391 182413.51172491264878772, 530186.21162480069324374 182272.1011724385607522, 530075.7495097367791459 182226.86884083910263143, 530075.1733111577341333 182226.46204725949792191, 530187.16388441331218928 182265.91148495653760619, 530233.22869966924190521 182154.23642371431924403, 530357.8921046924078837 182201.72724467553780414, 530348.98757576220668852 182228.44083146619959734, 530358.86895656702108681 182231.0766534095746465, 530394.74696868821047246 182125.29837629428948276, 530508.99968287569936365 182165.49652313266415149, 530513.72136097133625299 182167.0985210579528939, 530567.86575565708335489 182188.16529536261805333, 530573.45622016047127545 182150.89553200689260848, 530664.76714038196951151 181926.34520778860314749, 530694.76100652059540153 181850.76066511913086288, 530759.06664636044297367 181869.87285391447949223, 530674.73822676041163504 181825.22436629422008991, 530573.75377231650054455 181777.63399121144902892, 530599.29007114132400602 181730.04361612870707177, 530646.88044622412417084 181748.21467864664737135, 530657.97477119497489184 181732.12790743884397671, 530724.74751764547545463 181760.6236275052651763, 530741.12779784575104713 181707.06197263259673491, 530773.19373494503088295 181600.7954151411249768, 530782.75100370426662266 181575.85406711159157567, 530688.89235894195735455 181552.28991476428927854, 530627.95015930733643472 181539.24596229381859303, 530599.01706093887332827 181486.621268884598976, 530600.06536160444375128 181482.63772635560599156, 530608.87108719476964325 181476.34792236247449182, 530639.82865497504826635 181423.25654537187074311, 530713.75870660948567092 181269.28719607146922499, 530693.84197932516690344 181263.16111494251526892, 530680.6315366072813049 181248.85744669524137862, 530660.53410572255961597 181232.36456035793526098, 530708.91471134126186371 181117.72636383789358661, 530738.96049951435998082 181054.31545012778951786, 530780.90824702754616737 181058.58881666694651358, 530775.76585162139963359 181090.30025500498595648)</t>
-  </si>
-  <si>
-    <t>MultiLineString ((529997.79784449038561434 181531.55623927924898453, 530052.96381539374124259 181551.7578624269226566, 530212.19656886300072074 181656.20085126161575317, 530209.62829864572267979 181680.17137328925309703, 530219.94612751191016287 181663.94489138040808029, 530214.47685644379816949 181646.0454587938147597, 530280.60531572205945849 181554.06226355716353282, 530282.5352925822371617 181541.31063073134282604, 530320.75503214134369045 181490.63379023759625852, 530439.40590576594695449 181519.28956287557957694, 530446.77953103894833475 181528.09228405426256359, 530452.47980525041930377 181521.3478456501616165, 530415.45271119684912264 181496.96883923502173275, 530453.46287902258336544 181405.91857528948457912, 530484.62340791756287217 181368.68222978565609083, 530453.29358863539528102 181346.97811556659871712, 530395.29544163832906634 181277.22392895829398185, 530367.43655410828068852 181235.61759427358629182, 530392.94670032931026071 181209.0107060651644133, 530366.14074424654245377 181232.85823050834005699, 530356.76784806651994586 181243.06795197643805295, 530233.45040496217552572 181368.96061311141238548, 530208.70179800654295832 181365.30212338751880452, 530089.44054251117631793 181304.94443834689445794, 529993.94726804597303271 181289.97907443816075101, 529966.154449358349666 181292.82961994459037669, 529944.77535806014202535 181334.87516616433276795, 529944.77535806014202535 181344.13943906020722352, 529926.36038226482924074 181394.46298536835820414, 529818.3114558468805626 181372.26115117289009504, 529660.9002180868992582 181353.18405782332411036, 529658.19050382054410875 181346.70498227514326572, 529687.50564937863964587 181285.67399781054700725, 529721.54846181173343211 181300.10519003760418855, 529759.29157994396518916 181225.35901491285767406, 529693.52337177516892552 181197.2517148221086245, 529775.50000859634019434 181018.70994359909673221, 529775.97546259185764939 181007.7745017017587088, 529781.20545654278248549 181022.98902955889934674, 529838.73539000260643661 181058.17262522855889983, 529856.80264183296822011 181056.27080924643087201, 529884.37897357402835041 181053.41808527320972644, 529884.37897357402835041 181040.5808273937436752, 529841.11265998031012714 181013.00449565265444107, 529793.09180643118452281 180981.03021445288322866, 529813.06087424361612648 180938.71480885017081164, 529693.24646736856084317 180862.64216956440941431, 529636.19198790425434709 180936.81299286801367998, 529544.71261489775497466 181110.32049908270710148, 529500.67028855415992439 181087.15450479803257622, 529497.70719626196660101 181077.45711184164974838, 529472.11685373820364475 181065.06599861959693953, 529327.24100357142742723 180987.63423189727473073, 529363.68890629184897989 180934.36422022906481288, 529341.2594276947202161 180918.74369049177039415, 529369.35465322365052998 180880.94103444411302917, 529373.59544198273215443 180864.11040405652602203, 529474.45649861427955329 180734.88892437299364246, 529586.06983813573606312 180745.40322447285871021, 529628.95491681678686291 180674.37020755160483532, 529698.51421969395596534 180685.57043428605538793, 529764.5366088654845953 180707.3814021373691503, 529796.95831783371977508 180641.94849858339875937, 529758.90263750497251749 180615.22934820654336363, 529701.21620745782274753 180576.41469456732738763, 529752.221008560503833 180488.99246547726215795, 529736.71554902533534914 180486.13619661549455486, 529630.94052359636407346 180420.23669079795945436, 529553.29336541274096817 180371.4960196012398228, 529600.89540751581080258 180294.5100008912559133, 529603.18077846488449723 180280.48510687495581806, 529627.5501629994250834 180237.51849304826464504, 529651.26990355167072266 180199.75792183651356027, 529755.13459132704883814 180264.05033537332201377, 529757.49669685761909932 180282.93852961267111823, 529750.75456156919244677 180263.42270937078865245, 529741.05953626392874867 180258.27485075587173924, 529692.10561535775195807 180344.68907300592400134, 529714.50048789544962347 180362.21963196148863062, 529818.38248662056867033 180418.31933547760127112, 529825.45121432386804372 180416.40886853076517582, 529886.37351822550408542 180465.18994148258934729, 529853.88177636556793004 180532.38877123859128915, 529886.33526469033677131 180548.33083567884750664, 529890.60546052257996053 180565.19810921599855646, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530050.41157349967397749 180610.86616918962681666, 530070.07637521636206657 180510.97958763028145768, 530188.07669850694946945 180525.82471146847819909, 530198.33220224641263485 180523.73919493536232039, 530176.7395676999585703 180498.66072197334142402, 530147.27407653350383043 180475.71472900768276304, 530145.39805810165125877 180460.62154763849684969, 530097.86113173386547714 180432.84690278727794066, 530092.62034017115365714 180436.74164287745952606, 530183.20679586019832641 180517.71444849349791184, 530183.54491803026758134 180518.12750223511829972, 530278.19829585729166865 180603.40918027592124417, 530268.53268745890818536 180617.5672072812449187, 530235.09162783063948154 180613.78033897408749908, 530272.91186433425173163 180628.17850733728846535, 530231.35642782167997211 180685.7212082612386439, 530271.80877493182197213 180714.15635758946882561, 530279.1604463669937104 180713.85645559715339914, 530406.94488804508000612 180799.17112492027808912, 530444.13386487518437207 180752.09647070491337217, 530401.44239147310145199 180811.87520614813547581, 530473.6967024392215535 180867.95744204666698352, 530505.41823465214110911 180898.08767154935048893, 530524.12640605843625963 180911.90581873711198568, 530566.90231333044357598 180885.25091369968140498, 530583.1249414641642943 180878.67467777145793661, 530613.2015811363235116 180832.95796116237761453, 530621.62208804569672793 180863.95207658049184829, 530628.92289129947312176 180938.48514510347740725, 530661.53606858651619405 180994.88196303881704807, 530688.01616593403741717 181020.94359625864308327, 530721.15283389366231859 181041.38081424048868939, 530656.38647651602514088 181175.61041465913876891, 530656.38647651602514088 181175.61041465913876891))</t>
-  </si>
-  <si>
-    <t>MultiLineString ((529384.76409676810726523 179413.5639608106284868, 529488.89725268981419504 179341.85586195762152784, 529507.48609744769055396 179304.67817244172329083, 529527.17355776752810925 179312.97107102791778743, 529529.5510069637093693 179300.78664389729965478, 529534.45449593081139028 179283.84731837426079437, 529628.36373918130993843 179315.94288252317346632, 529728.8134611037094146 179371.58312865174957551, 529746.30872093141078949 179339.90252301786676981, 529747.72725551202893257 179333.28269497497240081, 529759.07553215697407722 179336.11976413620868698, 529797.66349294758401811 179363.07587449543643743, 529903.46462748944759369 179375.02742007101187482, 529922.34603962791152298 179322.73916143921087496, 529942.10454290267080069 179279.78589345078216866, 529950.30449442740064114 179210.40749376593157649, 530008.30646530282683671 179214.88170591468224302, 530029.01860685972496867 179098.38756920979358256, 530058.40054170438088477 179101.96558558152173646, 530074.08929685712791979 179102.65520119262509979, 530077.42243897751905024 179093.34539044267148711, 530077.13509913976304233 179130.46969750721473247, 530117.59254832461010665 179137.82559735901304521, 530104.71972358389757574 179220.57947069173678756, 530152.21009681595023721 179221.90492982690921053, 530207.71678659250028431 179224.85872263100463897, 530184.66079276066739112 179293.78055472593405284, 530187.28638636425603181 179405.36828287967364304, 530159.7176535262260586 179577.34466391659225337, 530083.57543902134057134 179577.34466391659225337, 529950.98296203871723264 179502.51524621350108646, 529931.29101001156959683 179516.95601103341323324, 529918.16304199350997806 179629.85653598894714378, 529922.10143239889293909 179699.43476648480282165, 530057.3195029852213338 179688.93239207033184357, 530088.82662622863426805 179667.92764324138988741, 530323.81725375237874687 179657.42526882691890933, 530325.13005055417306721 179730.94188972821575589, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530310.70194406423252076 180314.97494861029554158, 530322.77280297817196697 180317.23823465663008392, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530887.07347942178603262 180750.79246864788001403, 530877.94206235243473202 180786.27454640308860689, 530909.77157327998429537 180806.88545921674813144, 531001.73798804986290634 180835.84509620812605135, 530983.51015721820294857 180883.61690484962309711, 530971.57197559298947453 180910.01476331148296595, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530933.97294215473812073 181004.14973056968301535, 530987.43905753502622247 181017.50046930427197367, 531017.77227606379892677 181055.46117654372937977, 531043.15823628788348287 181082.8842570090200752, 531133.24576505646109581 181116.43755003809928894, 531080.85005751345306635 181269.00233420182485133, 531047.05935273109935224 181249.54233780177310109, 530921.40490906045306474 181207.63958008401095867, 530856.85412047430872917 181253.56449276715284213, 530816.26180326705798507 181237.64866236463421956))</t>
-  </si>
-  <si>
-    <t>LineString (533114.38557692908216268 180650.94499810261186212, 532993.2912894997280091 180672.05200613249326125, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531662.09765580005478114 180911.36713150818832219, 531644.95713887771125883 180910.93905784812523052, 531621.9483896060846746 180876.42593394074356183, 531595.00393322226591408 180858.26113188423914835, 531572.22224397643003613 180843.12379683717153966, 531551.33272161148488522 180836.46336941645131446, 531511.58714895439334214 180836.14345619000960141, 531510.64536264294292778 180916.21691724128322676, 531435.75916852697264403 180912.37710467760916799, 531466.5541653853142634 180913.61106873201788403, 531465.03699818823952228 180989.25269041734281927, 531387.01125662168487906 180986.86857053614221513, 531389.17863833182491362 181128.18185803995584138, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531110.30965442163869739 181356.39285153028322384, 531197.1542466712417081 181376.88721254793927073, 531286.93602178571745753 181375.08379181567579508, 531305.25734407640993595 181583.75572135805850849, 531325.21203300100751221 181586.18808011634973809, 531388.88918386655859649 181572.61640889989212155, 531390.49493819230701774 181599.32936576748033985, 531367.26279260986484587 181685.65545662579825148, 531395.89248193160165101 181593.61920236010337248, 531412.32238542404957116 181591.09869188832817599, 531419.12145480117760599 181581.94767167716054246, 531385.41458384564612061 181534.11455342586850747, 531374.38023236603476107 181529.41130202304339036, 531413.36951656360179186 181525.26491641241591424, 531471.93530321691650897 181443.00015478587010875, 531489.86913823755457997 181396.66486753628123552, 531500.42645009863190353 181343.75654840667266399, 531561.43261282751336694 181271.18043218745151535, 531499.01550433901138604 181334.88368744595209137, 531566.52648988855071366 181353.74707860476337373, 531590.37191976455505937 181360.8123911606380716, 531583.52515332715120167 181463.7283773985109292, 531566.74728090583812445 181537.16921628548880108, 531557.91564021108206362 181566.97600363052333705, 531578.66999584389850497 181574.92448025586782023, 531607.15203708468470722 181582.43137484646285884, 531674.27250636543612927 181614.50127011956647038, 531688.84471351187676191 181590.65584024353302084, 531676.92199857381638139 181529.27593741449527442, 531692.81895182456355542 181520.00271468493156135, 531744.15286336338613182 181527.39921376685379073, 531827.17028589476831257 181517.68440900254063308, 531837.76825472852215171 181595.40284711701679043, 531873.09481750777922571 181627.19675361836561933, 531892.79980997554957867 181649.86393449633033015, 531906.87584316555876285 181666.05597267561824992, 532031.40197696257382631 181539.76351073960540816, 532080.85916485369671136 181575.09007351889158599, 532117.06889170245267451 181580.38905793579760939, 532140.91432157845702022 181599.81866746442392468, 532170.05873587145470083 181590.98702676958055235, 532184.18936098308768123 181559.19312026820261963, 532149.74596227332949638 181529.16554190579336137, 532138.2648293700767681 181394.04143927496625111, 532132.82734409463591874 181370.85496780133689754, 532125.90053239720873535 181323.38831371636479162, 532096.75611810432747006 181293.36073535395553336, 532017.27135185094084591 181313.67350895205163397, 532018.15451592043973505 181340.1684310365235433, 532031.40197696257382631 181369.31284532946301624, 532033.16830510157160461 181389.62561892755911686, 532057.23452599509619176 181405.74336319562280551, 532119.69996919808909297 181395.70321314127068035, 532140.79753599606920034 181364.76011517079314217, 532132.3034719011047855 181288.28254195442423224, 532160.56472212448716164 181242.35801034132600762, 532384.22602272103540599 181180.09494344278937206, 532424.85156991728581488 181173.91279495641356334, 532670.78084617818240076 181110.13770430514705367, 532818.19047775026410818 181176.80775713562616147, 532780.99707011831924319 181260.68462679820368066, 532688.27519202104303986 181257.87865509698167443, 532650.54560429917182773 181265.88190097737242468, 532436.45877699879929423 181308.18477205943781883, 532413.59236019768286496 181321.90462214010767639, 532414.73568103776779026 181427.0901394252141472, 532338.13318475405685604 181459.10312294677714817, 532350.7097139946417883 181509.40923990920418873, 532405.30328410735819489 181674.61910129722673446, 532528.63901972828898579 181635.46036252533667721, 532616.67472441249992698 181609.7356436240952462, 532609.81479937222320586 181581.72428304271306843, 532720.71692085755057633 181553.71292246135999449, 532855.62877998419571668 181525.1299014599644579, 533071.32848995237145573 181469.8718779842602089, 533186.19458453194238245 181444.03007418513880111, 533181.16196181264240295 181435.64236965295276605, 533152.08458610100205988 181436.48114010615972802, 533186.47417468298226595 181432.28728784006671049, 533189.54966634477023035 181438.99745146580971777, 533246.78843064326792955 181526.30952275943127461, 533260.0739210395840928 181527.98328532904270105, 533340.41452438081614673 181492.83427136726095341, 533338.70870435202959925 181483.54382457892643288, 533339.90022310265339911 181474.30955426144646481, 533358.96452311298344284 181468.35196050821105018, 533371.7733496823348105 181461.2028480043518357, 533421.18748124549165368 181431.14743276051012799, 533457.81188699707854539 181401.60169366677291691, 533466.42939423269126564 181399.13954874229966663, 533532.90730719361454248 181489.9311428323853761, 533627.23823461274150759 181537.48131668634596281, 533600.77017667470499873 181593.49511371820699424, 533571.96468304062727839 181647.30677931586978957, 533565.79550759738776833 181677.67810457508312538, 533566.74461151170544326 181709.94763766299001873, 533571.49013108352664858 181761.67380099510774016, 533438.61558307439554483 181753.13186576595762745, 533368.85644536965992302 181739.84441096504451707, 533363.63351622002664953 181744.60156841060961597, 533362.33726643316913396 181745.78222090430790558, 533349.36948162270709872 181755.27449376182630658, 533376.01579060044605285 181931.55007622967241332, 533386.24188510165549815 181988.51551208973978646, 533386.32651571999303997 181988.9869550303556025, 533395.4760166349587962 182035.56623241596389562, 533318.95291807304602116 182051.36991581466281787, 533232.44854578538797796 182077.1548729388450738, 533173.13606239529326558 181928.21060169869451784, 533081.3675638793502003 181840.45443919772515073, 533032.44119917706120759 181849.24923483061138541)</t>
-  </si>
-  <si>
     <t>LineString (532697.1052455990575254 182632.05932354778633453, 532655.33205056318547577 182614.85859618009999394, 532626.86352182505652308 182629.09286054916447029, 532587.82842075009830296 182620.02757512527750805, 532516.08383130398578942 182600.83475501867360435, 532535.27665141061879694 182498.93001969077158719, 532546.70094909309409559 182441.35155937095987611, 532622.55828570493031293 182456.43163231186917983, 532600.79276104434393346 182442.18386507811374031, 532613.40521086833905429 182384.24542369923437946, 532563.74368968640919775 182375.57436444525956176, 532570.5496154772117734 182349.89332451421068981, 532613.77773230266757309 182221.77954575628973544, 532622.15411480166949332 182179.14974196642288007, 532625.14567997993435711 182043.93099591019563377, 532622.15411480166949332 181975.12499681077315472, 532620.957488730433397 181933.54224083331064321, 532705.76836153340991586 181922.69781706220237538, 532699.78523117688018829 181866.15723519353196025, 532694.25083559716586024 181810.14017723107826896, 532743.61166103801224381 181788.00259491213364527, 532732.54286987858358771 181747.31730848812730983, 532740.62009585974738002 181786.80596884083934128, 532620.35917569464072585 181837.96173338868538849, 532603.1576759199379012 181792.48994267950183712, 532540.33480717707425356 181814.02921196279930882, 532518.79553789377678186 181824.20053356880089268, 532460.75917343597393483 181843.6457072273187805, 532437.12580852792598307 181862.64214610910858028, 532441.91231281310319901 181949.99584931359277107, 532338.88065859954804182 181920.13854406692553312, 532334.11378894187510014 181934.43915304006077349, 532298.27399114507716149 182038.20684345928020775, 532289.60576192860025913 182079.62583160575013608, 532259.53832987882196903 182167.63571083481656387, 532288.66615467704832554 182063.33930591211537831, 532281.46249908185563982 182058.01486481996835209, 532220.90932479011826217 182025.71317250368883833, 532158.87452575471252203 182016.26025074589415453, 532107.4742636966984719 182011.53378986698226072, 532104.52022564737126231 181924.09426360743236728, 532086.79599735140800476 181928.63609710824675858, 532087.97761257109232247 181975.30989828731981106, 532092.70407344994600862 182022.86991088121430948, 532079.11549842311069369 182099.67490016322699375, 532046.62107988074421883 182161.70969919872004539, 532014.12666133837774396 182194.20411774111562409, 531972.17932103818748146 182188.88684925236157142, 531913.68936766183469445 182151.07516222121194005, 531908.60801759164314717 182163.45413967911736108, 531953.17571160080842674 182184.55127293791156262, 531987.59041022916790098 182199.51705184334423393, 532004.99554516770876944 182204.79133515805006027, 531983.10726941167376935 182243.55731752107385546, 531968.33927613054402173 182281.13658613828010857, 531944.07757288287393749 182371.59054498534533195, 531937.94260709825903177 182398.64015493713668548, 532011.93064753827638924 182423.87109960327506997, 532068.52979368122760206 182445.01053972897352651, 532086.94156411325093359 182440.23711776512209326, 532158.88385228300467134 182467.76953373529249802, 532152.40563676052261144 182502.8882810408831574, 532121.55289627402089536 182643.03526213087025099, 532075.0642949640750885 182863.25497264647856355, 532069.45360170258209109 182883.29316286626271904, 532082.41561907751020044 182888.00662372991791926, 532062.29523281508591026 182889.32744172037928365, 532066.95640396035742015 182915.35964283399516717, 531884.43796249642036855 182981.6259192216093652, 531767.99498561583459377 183028.33115369590814225, 531728.68198287941049784 182918.06297528900904581, 531725.87449492723681033 182910.13609254563925788, 531809.84689899394288659 182817.65547132669598795, 531837.40510237636044621 182760.1590255610353779, 531828.71498920442536473 182755.52429853595094755, 531814.23146725108381361 182767.69045697676483542, 531569.74961667892057449 182693.53482457570498809, 531563.95620789751410484 182754.94495765783358365, 531565.11488965386524796 182687.74141579438582994, 531616.09688692959025502 182577.66664894908899441, 531609.14479639194905758 182564.92114963015774265, 531628.84238624852150679 182534.7954239672399126, 531625.36634097970090806 182476.86133615393191576, 531747.02792538760695606 182513.93915235446183942, 531632.89777239540126175 182463.5364959568833001, 531625.94568185787647963 182421.82395273129804991, 531681.5624061586568132 182312.90786764226504602, 531703.57735952769871801 182270.0366426604159642, 531683.80043675052002072 182250.5687343017780222, 531595.88583471847232431 182183.28084469723398797, 531580.06645999138709158 182164.89640980056719854, 531555.2433897431474179 182143.27140381743083708, 531526.61310013174079359 182118.90519989278982393, 531515.64830836560577154 182136.41840896362555213, 531466.00216786901000887 182107.48354180311434902, 531411.63507536228280514 182149.7436767349136062, 531394.57873261498752981 182161.31762359911226667, 531354.5267849137308076 182200.07511671676184051, 531330.16058098908979446 182208.29871054133400321, 531333.2063564796699211 182193.06983308843336999, 531354.79575750709045678 182159.67430333484662697, 531334.90127811359707266 182155.04768022007192485, 531291.87368314596824348 182150.88371941674267873, 531265.96459370316006243 182135.15320082646212541, 531248.34037534287199378 182041.19192783226026222, 531270.21593675261829048 182040.14943936991039664, 531272.14963821833953261 182027.69603843480581418, 531291.66027387382928282 182000.88878809078596532, 531269.86458137142471969 182026.02942997106583789, 531260.89388385554775596 182036.66077076771762222, 531156.26423942053224891 182028.00196012531523593, 530992.96919284970499575 181971.66516905839671381, 530937.44887701561674476 182060.66096943948650733, 530881.5203235651133582 182170.88512587477453053, 530778.6444442254723981 182309.68591545993695036, 530773.74559282837435603 182337.44607337698107585, 530858.50592793908435851 182423.17597282669157721, 530936.88755029300227761 182449.3031802780169528, 531037.31400393415242434 182542.38135682337451726, 531094.36521082976832986 182594.22753410961013287, 531155.37121963454410434 182521.76535719376988709, 531166.80187289451714605 182513.19236724881920964, 531203.95149598934222013 182472.57272441431996413, 531259.88004943984560668 182529.52187190589029342, 531326.62689972575753927 182604.63759332848712802, 531370.30832468345761299 182662.60733486112440005, 531384.59664125845301896 182683.83569091532262973, 531369.90008706704247743 182687.50982946317526512, 531339.69050345139112324 182687.10159184673102573, 531257.94092076190281659 182652.80963206687010825, 531233.85490139271132648 182679.95743355926242657, 531204.76797122228890657 182711.18761121592251584, 531182.72313993528950959 182813.24701532270410098, 531203.13502075662836432 182831.20947044549393468, 531268.45303938491269946 182871.21675685534137301, 531362.55180997133720666 182909.59109279947006144, 531365.40947328635957092 182920.61350844299886376, 531354.79529525921680033 182956.13018107216339558, 531445.73022431845311075 182985.52328945489716716, 531448.01767393574118614 182986.57650366716552526)</t>
+  </si>
+  <si>
+    <t>LineString (535514.30680333590134978 179524.80755477515049279, 535499.36235546763055027 179481.84226715381373651, 535492.82415952521841973 179444.48114748310763389, 535463.86929178040008992 179400.58183186998940073, 535399.42136034846771508 179366.95682416635099798, 535321.89703703171107918 179295.27017579812672921, 535279.8657774020684883 179283.12781190514215268, 535101.46643097442574799 179497.95425001182593405, 535066.20687428512610495 179530.64522972371196374, 535040.98811850743368268 179543.72162160844891332, 535039.12006252387072891 179587.62093722156714648, 535044.7242304744431749 179592.29107718038721941, 535036.31797854858450592 179582.95079726271796972, 535038.18603453214745969 179547.4577335755166132, 535007.3631108037661761 179563.33620943559799343, 534947.1183053347049281 179556.79801349321496673, 534869.5939820179482922 179546.52370558376424015, 534718.28144735156092793 179513.83272587187821046, 534612.26927028584759682 179486.74591411059373058, 534612.26927028584759682 179455.92299038224155083, 534527.27272303495556116 179439.11048653040779755, 534514.19633115013130009 179463.39521431637695059, 534497.3838272982975468 179460.5931303410907276, 534488.97757537243887782 179473.66952222582767718, 534374.0921323848888278 179452.18687841517385095, 534301.70496302295941859 179452.18687841517385095, 534232.58689163206145167 179457.79104636577540077, 534155.99659630702808499 179483.0098021435260307, 534136.38200847990810871 179501.69036197889363393, 534117.70144864462781698 179504.49244595417985693, 534038.3090693443082273 179541.85356562491506338, 533971.05905393697321415 179587.62093722156714648, 533905.91060151113197207 179646.46470070295617916, 533868.78298883838579059 179677.05411743334843777, 533814.60936531575862318 179702.27287321106996387, 533764.17185376037377864 179719.08537706290371716, 533735.21698601555544883 179744.30413284065434709, 533662.8298166535096243 179797.89398886833805591, 533678.24127851764205843 179824.51378663373179734, 533699.25690833246335387 179872.14921421391773038, 533728.21177607728168368 179852.41787288780324161, 533759.03469980566296726 179897.71823048856458627, 533730.91986712557263672 179854.01778862628270872, 533658.8310093138134107 179905.21964279739768244, 533619.01806616468820721 179928.97897983799339272, 533566.71249862562399358 179955.36527060542721301, 533544.2958268232177943 179960.03541056427638978, 533484.63478884904179722 179977.43168191093718633, 533469.22332698479294777 179969.49244398091104813, 533411.78060549113433808 180001.71640969690633938, 533390.76497567631304264 180012.4577316022478044, 533382.82573774631600827 180031.60530543350614607, 533351.06878602621145546 180030.67127744172466919, 533300.6312744707101956 180049.35183727709227242, 533240.85348299751058221 179885.89693871766212396, 533173.60346759017556906 179908.31361052009742707, 533147.45068382075987756 179897.1052746188652236, 533121.29790005122777075 179875.62263080821139738, 533109.15553615824319422 179875.62263080821139738, 533085.33782236813567579 179864.88130890289903618, 533063.38816456159111112 179863.01325291936518624, 533056.84996861917898059 179775.6816356890485622, 533052.97625329520087689 179769.77504887530812994, 533049.84475868125446141 179753.95276029917295091, 533085.77453898952808231 179746.86569354109815322, 533111.65057343174703419 179737.6360252050217241, 533122.52839682786725461 179734.66934609701274894, 533143.9132087315665558 179736.4823166630230844, 533227.63518259371630847 179755.64490078343078494, 533235.51463751657865942 179725.05407578885206021, 533246.17507652984932065 179690.29177465863176621, 533261.35461469017900527 179692.60926140064839274, 533329.02522755693644285 179684.26630912939435802, 533382.2115482862573117 179671.75188072252785787, 533410.02138919045682997 179667.11690723849460483, 533450.22978416446130723 179668.97089663209044375, 533452.54727090639062226 179679.63133564536110498, 533461.3537205260945484 179717.17462086598970927, 533453.93776295159477741 179668.97089663209044375, 533451.94869960669893771 179660.89830636882106774, 533430.31913536891806871 179658.49502145350561477, 533401.47971638524904847 179663.3015912841365207, 533327.77897898247465491 179679.32349071951466613, 533262.89028626913204789 179686.53334546543192118, 533246.06729186198208481 179683.32896557834465057, 533293.98835750482976437 179526.55448060017079115, 533297.79979026620276272 179471.92394435431924649, 533277.47214887232985348 179409.67054258575080894, 533267.30832817545160651 179398.23624430174822919, 533261.0353450890397653 179395.85409882574458607, 533255.47700564551632851 179411.57625896626268514, 533142.40450039238203317 179443.3381986441090703, 533048.38915894599631429 179483.99348143170936964, 532974.70145889348350465 179533.54210732915089466, 532794.61126092006452382 179654.87271689844783396, 532708.53640439314767718 179706.00943977979477495, 532693.2906733478885144 179712.36182771535823122, 532685.9464436424896121 179717.96226352726807818, 532658.78351692855358124 179728.82743421287159435, 532607.27455960412044078 179737.47932938844314776, 532548.11974142713006586 179741.40286324714543298, 532534.03526090865489095 179738.18355341436108574, 532548.52215515612624586 179713.23390221039880998, 532555.76560227992013097 179695.93011185922659934, 532523.17009022308047861 179679.43114896627957933, 532492.98906054079998285 179664.94425471880822442, 532479.7094074806664139 179651.26218792953295633, 532484.41954601428005844 179673.02428334188880399, 532449.79857150348834693 179748.49007901950972155, 532378.32551233028061688 179682.61488870403263718, 532357.40633448015432805 179686.00104389677289873, 532361.9146399162709713 179664.21872470591915771, 532197.54445065301842988 179511.6966937497491017, 532242.98194478405639529 179474.83317379461368546, 532244.69978968834038824 179458.70721855689771473, 532258.3818564775865525 179462.12773525423835963, 532327.39026551635470241 179384.03927239449694753, 532343.62657718255650252 179360.62614285058225505, 532356.44643774325959384 179329.55894946909393184, 532412.07767790672369301 179270.75782656238880008, 532414.88226228312123567 179257.70878397024353035, 532428.03560322884004563 179250.60044720803853124, 532448.61292798642534763 179227.50345003115944564, 532496.48670395300723612 179169.1310389841964934, 532506.14544822706375271 179101.51982906644116156, 532494.38697693694848567 178997.79331447216100059, 532483.8883418565383181 178999.47309608501382172, 532498.58643096906598657 179109.07884632432251237, 532488.92768669512588531 179168.71109358099056408, 532445.25697034073527902 179214.06497424640110694, 532606.87226027122233063 179362.21232334937667474, 532626.11217573913745582 179400.69215428520692512, 532679.98393904929980636 179385.30022191087482497, 532719.58761149924248457 179333.93767049448797479, 532820.3977558920159936 179207.26369896886171773, 532909.74552235088776797 179116.74030400396441109, 532941.48410618293564767 179098.9765160133538302, 532963.40215328731574118 179080.1896184952929616, 532976.27465714234858751 179080.88542951448471285, 532985.58112952392548323 179071.40500437797163613, 533037.41905045346356928 179058.18459501341567375, 533056.55385348107665777 179066.18642173407715745, 533060.32914265117142349 179065.0439605139545165, 533066.32706405699718744 179059.61726971823372878, 533052.61752941517625004 179038.19612184033030644, 533040.33607129845768213 178975.07513942685909569, 533032.33884275739546865 178967.93475680088158697, 533022.34230708109680563 178935.44601585279451683, 533014.34507853991817683 178938.30216890317387879, 533009.7752336593111977 178929.16247914195992053, 533004.63415816868655384 178922.59332712605828419, 533008.63277243915945292 178907.74133126405649818, 532948.08232777111697942 178850.76107790888636373, 532929.23171763855498284 178851.90353912903810851, 532820.69790172390639782 178835.33785143680870533, 532628.47880143311340362 178740.51357016403926536, 532649.04310339584480971 178706.81096416953369044, 532649.61433400597888976 178688.53158464707667008, 532680.4607869500759989 178677.10697244553011842, 532646.72988178418017924 178686.93224038934567943, 532644.91513582807965577 178705.68461526944884099, 532577.46707779157441109 178826.97013667138526216, 532558.10978759278077632 178818.50132220939849503, 532477.21695213438943028 178782.04142910346854478, 532465.16113808494992554 178762.56665256191627122, 532448.46847247786354274 178772.14947911410126835, 532425.90246156463399529 178760.71191193890990689, 532423.12035063013900071 178744.32836976903490722, 532352.79476867453195155 178710.47935339916148223, 532245.37437425879761577 178647.41817221697419882, 532184.94074229244142771 178616.19670506301918067, 532251.30818086618091911 178452.11467546166386455, 532511.10399071127176285 178585.03346189408330247, 532598.70955449633765966 178413.85017633717507124, 532702.58256901206914335 178176.74428570797317661, 532815.09900265594478697 177890.48924129054648802, 532856.91221495741046965 177792.91708755856961943, 532858.8989350259071216 177769.61827948209247552, 532770.30928106070496142 177726.3168125337397214, 532588.16317295876797289 177673.66873071744339541, 532472.21096532221417874 177646.21587158855982125, 532427.41945832245983183 177643.32609694340499118)</t>
+  </si>
+  <si>
+    <t>LineString (532425.86516154767014086 177642.33997085387818515, 532411.25822669372428209 177649.51064796402351931, 532407.54009782173670828 177671.5538405618572142, 532404.75150116789154708 177727.19298332382459193, 532429.18491946905851364 177794.11930301843676716, 532358.00930963514838368 177800.49323822744190693, 532344.59748763276729733 177875.45337209175340831, 532340.61377812712453306 177908.3853706716618035, 532327.99869802594184875 177961.36870709658251144, 532247.2621853785822168 177940.65341766728670336, 532213.93181584810372442 177940.5206273504300043, 532181.53097853565122932 177966.54752945387735963, 532131.07065813092049211 178059.50075125196599402, 531992.96872860239818692 177958.58011044265003875, 531978.40126691607292742 177969.69867078488459811, 531975.51999578601680696 177976.24701426242245361, 531956.66076657059602439 177991.70110486945486628, 531930.72932639950886369 178011.6080690412200056, 531893.66570231656078249 178019.07318060554098338, 531849.13696666923351586 178060.9825788619054947, 531859.09044875507242978 178130.13308598485309631, 531859.16702702990733087 178134.34492127480916679, 531819.8686971872812137 178155.9232769338414073, 531807.15032861998770386 178147.34909587725996971, 531804.22081675904337317 178166.85535778096527793, 531594.50186685402877629 178293.37287628170452081, 531621.63150816119741648 178357.4752960842452012, 531633.50392294430639595 178379.59179671431775205, 531588.61539335269480944 178402.98467423874535598, 531470.04583553783595562 178481.04854062185040675, 531567.95477312488947064 178566.74453142564743757, 531600.88228947878815234 178584.2162747971015051, 531772.37417057063430548 178639.05066937819356099, 531797.10340734256897122 178657.86639300896786153, 531837.96040722646284848 178713.77597179752774537, 531857.31372296100016683 178741.19316908807377331, 531868.06556503567844629 178749.79464274787460454, 531880.13844949356280267 178747.46484413990401663, 531893.87027424620464444 178732.70546787517378107, 531882.84744893456809223 178737.65639788802945986, 531874.82179012312553823 178745.74090769540634938, 531873.81108064437285066 178750.26503583858720958, 531928.47747769311536103 178812.55852085907827131, 531938.12053605390246958 178829.1566770619538147, 531932.74461501650512218 178852.9451276523177512, 531965.13453926669899374 178839.37092703295638785, 531981.7662949759978801 178846.35962438152637333, 532009.72108437039423734 178845.01564412217703648, 531981.39670040470082313 178850.0555700947297737, 531960.96820046263746917 178846.83001747232628986, 531933.5510031720623374 178860.26982006573234685, 531935.16377948329318315 178924.24328041044645943, 531930.32545054971706122 179009.45162885275203735, 531910.43454271147493273 179022.35383934245328419, 531885.70530593954026699 179057.83491818906622939, 531876.11210935655981302 179066.35873417466063984, 531831.93818780174478889 179086.51181359370821156, 531779.46893305156845599 179106.20686848048353568, 531672.18940927542280406 179157.81096578075084835, 531589.70353428379166871 179198.03799872964737006, 531556.67969205614645034 179124.41894058702746406, 531620.5699304185109213 179098.98690395732410252, 531635.7671230387641117 179139.9262799954158254, 531648.27035036904271692 179178.57474457612261176, 531695.00515957863535732 179157.60464692092500627, 531797.07743173581548035 179112.31386224390007555, 531810.86905931774526834 179106.1050852510088589, 531847.91815481544472277 179173.68914956544176675, 531891.07424407650250942 179215.21670715624350123, 531905.47685013443697244 179238.60377113270806149, 531919.96244928787928075 179292.40742513118311763, 531957.96748593868687749 179272.83832924981834367, 531967.94273236184380949 179364.63301262669847347, 531985.87575963942799717 179480.30103856680216268, 531979.93544435373041779 179495.99243743464467116, 531952.58757775544654578 179485.23262106810580008, 531939.54275271145161241 179490.46462862013140693, 531766.64450117154046893 179467.29959379057982005, 531761.71291867026593536 179464.16131401702295989, 531729.43346957070752978 179458.33308015181683004, 531718.67365320411045104 179473.57615333772264421, 531714.63872206665109843 179523.78862971480702981, 531716.09578053292352706 179527.48731659070472233, 531741.86680176388472319 179544.99216120038181543, 531751.2878118836088106 179549.55071448421222158, 531794.563677724217996 179583.10166665274300613, 531736.03185356059111655 179657.43647553340997547, 531711.23332369688432664 179690.98742770194076002, 531710.01770948793273419 179697.49096372016356327, 531768.36719152017030865 179689.71103278253576718, 531817.90347053715959191 179690.92664699154556729, 531827.62838420912157744 179689.71103278253576718, 531830.54585831076838076 179679.74299626867286861, 531848.91713031963445246 179689.19716539108776487, 531944.69973392877727747 179685.07748351542977616, 532042.54217847576364875 179713.40029641060391441, 532046.66186035145074129 179723.69950109976343811, 531964.78318307269364595 179783.43488829687703401, 531949.33437603886704892 179795.79393392385100015, 531887.02418766950722784 179851.66711936253705062, 531879.29978415265213698 179893.89385858806781471, 531869.00057946355082095 179984.52685985263087787, 531866.29703823267482221 180017.74179497518343851, 532058.37720568536315113 180022.37643708530231379, 532075.37089342251420021 180021.86147685084142722, 532105.01448292518034577 180034.50729168066754937, 532262.32514954556245357 180048.1606702930002939, 532325.92739683925174177 180055.68131635268218815, 532405.1537294692825526 180033.52798163625993766, 532464.76121906656771898 180011.84399723159731366, 532540.23274920228868723 179984.43393902308889665, 532591.95515356154646724 180078.2101313185703475, 532591.20419306261464953 180094.73126229355693795, 532607.72532403760123998 180147.29849721392383799, 532534.50667539855930954 180136.78505022986792028, 532536.55852291593328118 180144.94319960565189831, 532612.86246818082872778 180163.34207012850674801, 532665.91098826692905277 180179.77963973267469555, 532720.82741398992948234 180243.84880307616549544, 532752.20822868880350143 180305.86327021915349178, 532785.08336789719760418 180312.58773051179014146, 532914.34243796626105905 180285.68988934133085422, 532886.6974345410708338 180313.33489276652107947, 532846.35067278542555869 180329.77246237068902701, 532662.54875812062527984 180367.13057510743965395, 532637.89240371435880661 180305.86327021915349178, 532548.96951092616654932 180316.77607292827451602, 532545.8441308259498328 180272.49985484205535613, 532572.40986167767550796 180230.30722348930430599, 532516.1530198740074411 180204.2623893209383823, 532468.75142168754246086 180244.89233062358107418, 532463.02155817055609077 180284.4804785595042631, 532459.3752813870087266 180373.55381141533143818, 532372.69448957266286016 180390.68838654135470279, 532277.44368469482287765 180400.13795320072676986, 532203.73706475202925503 180422.18694207252701744, 532202.47712253080680966 180432.26647984248120338, 532156.80421701062005013 180436.991263172152685, 532083.72756817832123488 180361.39472989740897901, 532038.73218060249928385 180353.29513465752825141, 531941.74603957985527813 180343.19241163434344344, 531920.30576653964817524 180317.62579917337279767, 531909.74514889775309712 180270.76305838747066446, 531907.76503308990504593 180261.52251795082702301, 531948.6874264522921294 180252.28197751415427774, 531995.60517045494634658 180231.05073579659801908, 532076.78991857706569135 180211.68960345312370919, 532106.05162995983846486 180200.24893434107070789, 532099.67125680122990161 180191.66843250702368096, 531974.81395447254180908 180230.50070362773840316, 531904.40983685990795493 180254.70211905709584244, 531741.12336655741091818 180332.22967136604711413, 531739.7332929449621588 180345.2238377439789474, 531706.95472862606402487 180347.60832770192064345, 531644.49292385333683342 180395.90728139248676598, 531648.12442413077224046 180495.13802647482953034, 531518.84301425225567073 180495.13802647482953034, 531488.34336362790782005 180484.8074996504583396)</t>
+  </si>
+  <si>
+    <t>LineString (531488.34336362790782005 180484.8074996504583396, 531473.81241081142798066 180479.88572530940291472, 531430.96070753701496869 180458.09672364447033033, 531451.29710909095592797 180386.19301815022481605, 531525.37971475173253566 180400.71901926017017104, 531538.45311575068626553 180381.83521781724994071, 531549.34761658310890198 180218.41770533029921353, 531569.5024431231431663 180215.87565513607114553, 531626.15384745202027261 180269.62185924287769012, 531643.585048783919774 180270.34815929835895076, 531647.21654906147159636 180203.52855419259867631, 531643.83931215479969978 180060.99850968600367196, 531625.11130755802150816 180053.36858188730548136, 531633.66547321295365691 180050.08258383703650907, 531634.2177775400923565 180047.32106220131390728, 531614.51892320532351732 180053.39640979986870661, 531602.36822800827212632 180051.73949681845260784, 531601.26361935399472713 180045.84825066229677759, 531592.78442665631882846 180051.56285102886613458, 531593.45052950282115489 180089.86376470435061492, 531513.85123934247530997 180096.19174174638465047, 531519.18006211472675204 180125.33374128208379261, 531513.35166220751125365 180149.81302089206292294, 531336.20963958697393537 180096.6219828424800653, 531238.11603961104992777 180067.39065219060285017, 531199.89045337401330471 180177.0081421350769233, 531177.40481441095471382 180218.60657421653741039, 531061.32270326465368271 180145.94985331749194302, 531060.76056229067035019 180124.58849630266195163, 531057.63696220016572624 180100.43033974233549088, 531037.72401162306778133 180082.46963922184659168, 530999.45991051418241113 180089.88818943683872931, 530975.4472348183626309 180111.55816506480914541, 530987.4871511091478169 180150.16886052410700358, 531011.03398508415557444 180159.51833872005227022, 531014.84303175657987595 180179.2561260225775186, 530958.39988561067730188 180262.36259887542109936, 530929.3741334832739085 180271.64266970381140709, 530943.43033389060292393 180263.83366947752074338, 530923.9078333250945434 180242.84698136936640367, 530866.90213167306501418 180188.57442979663028382, 530842.303780960268341 180151.09122871042927727, 530840.0206066551618278 180145.71054415201069787, 530822.22424072585999966 180117.54081000993028283, 530812.51550312107428908 180086.5150615772290621, 530820.11364559445064515 180120.49564319400815293, 530836.57628762000240386 180149.4107964952418115, 530859.76145922881551087 180140.51328725425992161, 530887.37670600018464029 180127.04054134621401317, 530942.97500607429537922 180058.23076402678270824, 531005.72952298959717155 180026.85350556910270825, 531037.65725966589525342 180016.94489763511228375, 531078.94312605750747025 180004.28389860835159197, 531103.36682528315577656 179997.4820276228711009, 531123.39294299448374659 179985.6610553627833724, 531156.49166532268282026 179963.68795398517977446, 531181.76768542011268437 179933.82261524567729793, 531212.01546737970784307 179888.97245578825823031, 531103.54066311055794358 179763.39200930739752948, 531108.54719253838993609 179756.71663673696457408, 531135.1701887323288247 179781.81394092956907116, 531167.34841385786421597 179808.82066558845690452, 531194.06783293525222689 179811.40641582175157964, 531236.87636457534972578 179792.73155302571831271, 531253.82739388255868107 179784.97430232583428733, 531249.51781016041059047 179751.07224371147458442, 531230.84294736431911588 179747.62457673373864964, 531216.47766829049214721 179768.31057860012515448, 531178.84063711692579091 179737.85618696350138634, 531127.12563245091587305 179702.51760044175898656, 531045.96180568356066942 179636.29366391123039648, 531013.78358055802527815 179596.07088250436936505, 530972.86260063934605569 179563.04264083271846175, 530945.78228133858647197 179595.62788598841871135, 530882.00223331130109727 179643.29507977730827406, 530842.39146664168220013 179630.53907017182791606, 530826.94998132972978055 179588.91419672238407657, 530809.49438923806883395 179516.40635264918091707, 530801.43796211876906455 179441.21303286953479983, 530771.22636042162775993 179379.44709162198705599, 530816.2080785040743649 179456.65451818142901175, 530938.3972231459338218 179398.91679049350204878, 530945.11091241205576807 179382.80393625498982146, 531051.18720281543210149 179331.77989783309749328, 531117.65272654918953776 179413.01553795216022991, 531106.23945479700341821 179449.94082891539437696, 531128.01335033809300512 179490.33879105054074898, 531145.9327949439175427 179489.53642785921692848, 531118.11753764539025724 179461.98862495779758319, 531170.3957165403990075 179433.66088251979090273, 531266.22342408250551671 179404.70195991088985465, 531313.87248040549457073 179407.3990763065230567, 531433.52216941397637129 179415.3352683637640439, 531469.58935155137442052 179427.35766240957309492, 531466.38337980583310127 179436.3744579438935034, 531357.78108692553360015 179511.91516719831270166, 531327.52472857688553631 179431.76587355969240889, 531318.50793304259423167 179389.48712116529350169, 531315.08669927902519703 179378.57198898226488382, 531298.67588855815120041 179338.66640459033078514, 531270.20679607603233308 179239.75740465606213547, 531274.79732766340021044 179226.52587243364541791, 531198.10844702739268541 179192.5019324331660755, 531219.62179134623147547 179127.21737543260678649, 531235.3105901419185102 179110.29808261376456358, 531240.33914468786679208 179077.35684370002127253, 531245.46363338397350162 178841.6303636806551367, 531233.0184465505881235 178844.00959057526779361, 531233.75051636435091496 178886.46963977129780687, 531226.42981822707224637 179085.22659419756382704, 531181.16885312169324607 179183.82010049920063466, 530988.59653849294409156 179108.14471807319205254, 530973.83061021461617202 179097.68551887612557039, 530832.78523280692752451 179038.00655875154188834, 530746.65065118379425257 179009.70519621824496426, 530660.53985221788752824 178980.90664574180846103, 530629.06085022771731019 178958.21248151632607915, 530637.84568799240514636 178901.11103604579693638, 530747.65616005111951381 178890.12998883993714117, 530829.64797918824478984 178865.23961517328280024, 530854.35533540148753673 178855.90572504830197431, 530871.92501093086320907 178861.03021374437958002, 530891.65204298356547952 178844.1667831186496187, 530965.44759355159476399 178788.4324741373420693, 530886.32739482226315886 178835.18531884101685137, 530876.4373699810821563 178823.49710766511270776, 530792.12940123490989208 178700.15787217835895717, 530743.08072371536400169 178626.95089080586330965, 530828.00082210742402822 178569.11737552162958309, 530830.19703154859598726 178562.52874719808460213, 530868.26466186228208244 178541.84777496033348143, 530837.15169477893505245 178458.75785110259312205, 530903.77004782785661519 178437.16179159769671969, 530958.67528385727200657 178408.9771037692844402, 530969.51906797324772924 178398.22482838027644902, 531033.78183673555031419 178376.20990525075467303, 531215.27667861443478614 178352.53666500566760078, 531252.47748471389058977 178318.71775036983308382, 531315.60612536745611578 178272.49856703419936821, 531294.18747943139169365 178255.58910971626755781, 531295.31477658601943403 178201.47884629893815145, 531322.36990829464048147 178189.07857759913895279, 531270.5142391863046214 178118.05885686387773603, 531219.78586723259650171 178146.24128572706831619, 531171.31208958791103214 178190.20587475365027785, 531094.65588307997677475 178130.45912556367693469, 530872.93878867325838655 178114.04592761132516898, 530864.83308461052365601 178128.09106711560161784, 530878.95511248987168074 178084.87972859182627872, 530943.32097328128293157 177890.14320068835513666, 530878.53382568154484034 177871.54188188168336637, 530847.7604888214264065 177818.14109144799294882, 530864.0522553944028914 177757.49951587078976445, 530876.72362939559388906 177733.06186601129593328, 530833.27891853428445756 177695.04774400766473264, 530829.65852596261538565 177662.46421086171176285, 530830.56362410553265363 177651.60303314638440497, 530804.31577796011697501 177646.17244428873527795, 530835.99421296315267682 177652.50813128933077678, 530839.61460553493816406 177696.85794029355747625, 530881.2149192038923502 177736.88257737495587207, 530903.80695161537732929 177711.30042302669608034, 530946.30642832547891885 177686.18709587972261943, 531019.71461537026334554 177674.59632950421655551, 531093.94195289048366249 177671.7781124759640079, 531118.76178659219294786 177709.00786302858614363, 531122.30747712100856006 177752.44257200666470453, 531115.21609606337733567 177786.12663203047122806, 531278.31786038912832737 177901.36157421718235128, 531294.66580769827123731 177906.02167873742291704, 531318.86828601313754916 177883.92376375428284518, 531341.04136397247202694 177863.066037877346389, 531340.89103802025783807 177853.74582883683615364, 531236.94064202811568975 177673.88082695021876134, 531241.75107250059954822 177597.21459129443974234, 531264.60061724507249892 177546.70507133298087865, 531288.65276960772462189 177480.86230424034874886, 531271.81626295391470194 177391.86934049872797914, 531241.75107250059954822 177314.90245293837506324)</t>
+  </si>
+  <si>
+    <t>LineString (531236.84324939036741853 177318.54342519459896721, 531202.52396391110960394 177191.43496045682695694, 531023.30102863081265241 177159.65784427238395438, 530944.49378049338702112 177143.13374385648057796, 530915.25883360370062292 177148.21808244596468285, 530890.0134778693318367 177105.24807653366588056, 530798.05788532528094947 176955.03413150229607709, 530778.53778894036076963 176970.21642869058996439, 530846.85812628781422973 177061.31021182052791119, 530925.4432389655848965 177024.38350523461122066, 531189.53587636584416032 177001.13818751723738387, 531180.75431189488153905 176810.13916027281084098, 531181.01259320287499577 176679.19053713156608865, 531207.87384923174977303 176244.24481450865278021, 531207.48642726987600327 176156.30002914459328167, 531185.2742347844177857 176156.30002914459328167, 531209.55267773370724171 176148.55158990548807196, 531188.94265151466242969 175949.80426446883939207, 531154.94696310814470053 175823.53456467346404679, 531066.20655180979520082 175503.10660128630115651, 530998.72868066909722984 175231.84770217089680955, 531029.01404346199706197 175153.91027290970669128, 531021.65302618476562202 175139.83394162519834936, 531029.40146542387083173 175082.75377256359206513, 531032.75912242755293846 175056.73193078552139923, 531026.30208972818218172 175037.10255137970671058, 530966.8973888949258253 175050.27489808623795398, 530928.21976302622351795 175062.67240086884703487, 531062.91346513316966593 175558.95993413514224812, 530985.17079143389128149 175576.00650046131340787, 530873.33498508238699287 175582.33439250665833242, 530875.38815978192724288 175595.23469414943247102, 530797.41443990776315331 175600.27078763680765405, 530684.78446298860944808 175838.26282582237035967, 530601.53621917893178761 175966.56306039975606836, 530646.58820994652342051 176020.4295711001905147, 530665.19664091581944376 176035.12043765484122559, 530699.47532954334747046 176074.2960818005958572, 530719.25994543684646487 176118.95408105937531218, 530745.12009748979471624 176148.40592089734855108, 530716.86548691359348595 176127.43046423231135122, 530670.8918832641793415 176208.65049734638887458, 530598.10034415242262185 176165.74180060689104721, 530560.55523450532928109 176215.54653789382427931, 530483.93256175622809678 176177.23520151924458332, 530387.97902395331766456 176303.5319877928995993, 530379.94736301514785737 176309.76833628604072146, 530341.93712524976581335 176251.15764247826882638, 530303.51330139499623328 176202.36548520234646276, 530182.75271213706582785 176293.85078009468270466, 530305.95290925877634436 176211.51401469158008695, 530417.23728811659384519 176386.02025389933260158, 530494.13386454083956778 176495.22892708366271108, 530475.49227025615982711 176509.52081603524857201, 530501.92500291229225695 176509.08523381545091979, 530512.77645926724653691 176528.58107065639342181, 530498.98223508731462061 176613.64545309916138649, 530462.28959876869339496 176757.56519204287906177, 530434.33330443082377315 176909.11773503280710429, 530402.8200269922381267 177194.41969347806298174, 530347.79517984646372497 177352.39425463852239773, 530312.29527846199925989 177448.2439883763436228, 530321.17025380814447999 177524.56877635276759975, 530299.1076171655440703 177512.2877638345817104, 530112.49448222981300205 177489.69982631949824281, 530086.75473947997670621 177355.87942906434182078, 530025.81983827648218721 177182.92411681212252006, 530186.56190524436533451 177134.07113567480701022, 530174.47998517821542919 177096.77477373127476312, 530096.4836231010267511 176769.19463073462247849, 529884.42970881413202733 176831.87007454806007445, 529743.07660154439508915 176608.87987858781707473, 529771.98973712243605405 176569.9510816659021657, 529802.22569589677732438 176526.86484041254152544, 529830.94985673227347434 176534.42383010612684302, 529799.95799898868426681 176524.5971435044775717, 529740.99787937884684652 176599.43114147079177201, 529698.59198002424091101 176544.13718110171612352, 529597.32066152559127659 176436.11156106233829632, 529515.85195648483932018 176518.75130591302877292, 529470.99966809689067304 176555.56964268209412694, 529518.67451752966735512 176525.99916645159828477, 529605.23845730861648917 176434.94747649942291901, 529505.5353504242375493 176347.90575941736460663, 529255.71074105193838477 176177.45054182736203074, 529165.48091607249807566 176110.54161229194141924)</t>
+  </si>
+  <si>
+    <t>LineString (529164.61925642273854464 176109.67995264215278439, 529001.12134455901104957 175987.36767307508853264, 528997.60493395722005516 175985.00944533024448901, 528925.98516327538527548 176086.5956472598190885, 528836.08586953231133521 176038.64935726355179213, 528804.92078103474341333 175988.30575276748277247, 528764.76576316286809742 175973.92186576858512126, 528736.1864626327296719 176029.69451619402389042, 528753.60289678350090981 176038.27722640830324963, 528557.00358154252171516 175913.29103869749815203, 528554.72205805755220354 175880.40056722576264292, 528529.4405931425280869 175873.17729153577238321, 528524.62507601594552398 175887.02190327495918609, 528445.1690434260526672 175861.74043835999327712, 528400.62551000446546823 175832.84733560003223829, 528350.06258017453365028 175846.09000769836711697, 528240.50956554315052927 176160.30250021276879124, 528416.27594066609162837 176261.42835987257421948, 528433.8382980921305716 176249.8060543195460923, 528444.64069186616688967 176225.97724452381953597, 528425.57764402963221073 176249.48833685560384765, 528405.06003338482696563 176243.23115157571737655, 528298.35011839854996651 176189.29952098953071982, 528242.99004875461105257 176148.69032720808172598, 528155.720433603040874 176103.8961748254369013, 528011.98040374473202974 176080.87730883390759118, 528002.26132699276786298 176073.71588385876384564, 528007.81933374144136906 176031.80425242587807588, 528024.69687239604536444 176034.07766336353961378, 528007.59572685486637056 176028.48092482279753312, 528028.97791927156504244 175838.52871152572333813, 528071.95822007348760962 175635.10030053602531552, 528066.13247264770325273 175627.8668870801338926, 527986.25385233573615551 175601.30841606299509294, 527783.6197062972933054 175545.97057698419666849, 527730.72324247192591429 175535.3912842191348318, 527705.49569818598683923 175645.25317062556860037, 527652.00888393050990999 175633.26453688892070204, 527667.81058392324484885 175521.98211052999249659, 527493.51585617032833397 175475.42110760780633427, 527372.37483971798792481 175449.05027409436297603, 527388.85661066381726414 175307.30704395961947739, 527363.30986569775268435 175304.0106897704245057, 527347.65218329906929284 175302.36251267584157176, 527392.9859605492092669 175304.87285213259747252, 527397.12063730170484632 175242.85270084580406547, 527416.99002535012550652 175173.88838360883528367, 527443.43270875024609268 175068.11765000826562755, 527450.48409099027048796 175080.4575689283083193, 527439.50107401434797794 175130.92109447572147474, 527503.88389773119706661 175132.10243069072021171, 527497.49056007748004049 175161.73309173848247156, 527475.35977589245885611 175220.01082342577865347, 527552.57162293803412467 175256.15777092802454717, 527519.86724186455830932 175235.87121875837328844, 527544.948797274264507 175170.46245661145076156, 527552.32572533597704023 175142.92192518117371947, 527701.83146738610230386 175159.64296212099725381, 527840.27181734365876764 175177.83938467313419096, 527917.36071558820549399 175188.16708395950263366, 527968.50741681596264243 175201.44555447052698582, 528779.72360599890816957 175221.85505544117768295, 529261.51673463499173522 175222.65933442555251531, 529351.25411826185882092 175215.8378031077736523, 529372.18678662180900574 175227.73136467591393739, 529365.05064968089573085 175241.05215363221941516, 529360.76896751637104899 175246.28532072220696136, 529382.68670980352908373 175224.25992501174914651, 529468.12816032278351486 175328.11548124635010026, 529698.30448176467325538 175447.99130945329670794, 529895.33541291893925518 175576.70590840361546725, 529955.73367966525256634 175634.15791823549079709, 529931.4270601209718734 175659.2011020083737094, 529925.47286403307225555 175678.95786343273357488, 529921.73475975845940411 175812.78199646400753409, 529619.1352187282172963 176067.34689756546868011, 529430.02734231401700526 175986.28361064163618721, 529289.88080719718709588 175972.14038232708116993, 529264.1658466252265498 175952.85416189813986421, 529130.44805165135767311 175948.99691781235742383, 529054.58891796413809061 175905.28148484011762775, 529001.12134455901104957 175987.36767307508853264, 528831.19019799574743956 176248.25477146793855354, 528752.75956825143657625 176391.9371136634144932, 528675.49066539527848363 176408.16534021744155325, 528705.96678335568867624 176534.67820903472602367, 528716.35159020742867142 176527.29953048215247691, 528719.63100289751309901 176506.25663238778361119, 528747.77929515356663615 176407.32768290513195097, 528744.77316685440018773 176389.5641975007893052, 528668.2535374202998355 176407.60096729596261866, 528714.38658874668180943 176593.66351471430971287, 528668.75400357856415212 176604.88464221468893811, 528606.66376474313437939 176705.1267145512974821, 528552.80235274136066437 176674.4556327169702854, 528522.08681564137805253 176737.87589794580708258, 528508.67160317418165505 176757.9432818841887638, 528487.60639351513236761 176746.19111228492693044, 528469.86726959166117013 176755.72589139378396794, 528197.11153506592381746 176662.46467340260278434, 528176.00199985504150391 176658.75310677211382426, 528137.95844189240597188 176788.65793883957667276, 527957.94746031321119517 176731.12865606683772057, 527939.38962716073729098 176738.55178932784474455)</t>
+  </si>
+  <si>
+    <t>LineString (527940.77566473442129791 176739.55987936040037312, 527892.90263102832250297 176721.44575849862303585, 527636.93444367230404168 176695.61776634884881787, 527711.9710393245331943 176478.3039893300156109, 527834.02353440679144114 176550.01674702038872056, 527855.60682320327032357 176496.67211271909764037, 527890.17659236572217196 176414.29315516981296241, 527929.95724563486874104 176377.71143682854017243, 528044.29808945208787918 176288.20219040603842586, 528076.05943495687097311 176244.31378570853848942, 528028.70615620422177017 176220.05966732307570055, 527961.14111213048454374 176203.89025506612961181, 527797.13707352406345308 176203.89025506612961181, 527683.08496921148616821 176217.74975128637743182, 527584.33605864213313907 176217.1722722772101406, 527518.79219110053963959 176395.61328611301723868, 527483.2068727093283087 176504.61552287041558884, 527473.46186028700321913 176591.34613342949887738, 527389.6547534546116367 176724.85280361596960574, 527365.42176395864225924 176779.05610696220537648, 527516.26628560293465853 176817.18143791682086885, 527480.72110768430866301 176938.649287985637784, 527537.79039941774681211 176962.5634430730715394, 527483.56923695211298764 176947.51469569859909825, 527472.50587809423450381 177038.787406276416732, 527388.83922673121560365 177163.25019342801533639, 527190.55077449802774936 177069.79876631233491935, 527159.65929454017896205 177000.74722287710756063, 527099.77578929206356406 176863.97566198912682012, 526993.89284357777796686 176974.11520853615365922, 526965.6928630608599633 177009.76424051032518037, 526918.33817879669368267 176978.37180936889490113, 526881.62499661440961063 176915.05487198193441145, 526809.33459098706953228 176814.57045149418991059, 526803.78523573139682412 176782.81458185013616458, 526837.9906987837748602 176724.64684572990518063, 526829.14218303072266281 176698.07787916850065812, 526713.59169160143937916 176585.58887918625259772, 526702.01159683079458773 176498.87495989364106208, 526728.35331819928251207 176459.47930909239221364, 526759.08459305611904711 176456.02855037362314761, 526877.73335154261440039 176444.22870948346098885, 526952.37421362893655896 176459.79166246333625168, 526957.30744241294451058 176431.45683538325829431, 527038.82798124512191862 176435.9939717588131316, 527098.5913686784915626 176454.87681948934914544, 527051.24293423152994365 176594.92815045249881223, 527174.99744662863668054 176650.61612686808803119, 527153.14015064027626067 176640.28990523278480396, 527205.55905537132639438 176487.71942607063101605, 527102.71056710940320045 176449.37945362422033213, 527080.02346470882184803 176442.65865531019517221, 527118.21201132400892675 176315.62328595775761642, 527136.13724749034736305 176310.16777929847012274, 527123.4023648789152503 176243.66339232763857581, 527158.08696234272792935 176237.9932378021767363, 527169.22996887960471213 176208.6499966005794704, 527150.43826302816160023 176186.18838753091404215, 527118.65549396350979805 176157.02174997527617961, 527093.6976608419790864 176147.4813768335734494, 527018.22708262107335031 176131.11693114246008918, 526849.86647974920924753 176114.85084184003062546, 526845.07710992521606386 176097.65762165782507509, 526857.65365130186546594 176044.64240146498195827, 526893.8380195926874876 176044.15844629961065948, 526858.37810308812186122 176039.0902959554514382, 526874.83542804175522178 175886.27227852959185839, 527054.69047931989189237 175862.7618143102445174, 527176.94489326048642397 175856.8841982554004062, 527195.27535622008144855 175822.70450227480614558, 527223.9658216992393136 175795.75699128504493274, 527224.12844125344417989 175773.97201046324335039, 527243.25712752784602344 175756.61424477020045742, 527267.78618826356250793 175718.31265972839901224, 527222.48707379773259163 175682.39379150536842644, 527195.04935412993654609 175648.09664192068157718, 527009.0825874931178987 175569.97535675560357049, 526824.66230209683999419 175469.42516340431757271, 526795.48152648622635752 175473.6317607709497679, 526758.33231608534697443 175456.72367672127438709, 526790.20567167596891522 175381.68114836351014674, 526851.47655176091939211 175305.71711282295291312, 526851.47655176091939211 175278.90286315878620371, 526865.43143400084227324 175215.89678796651423909, 526877.77642672799993306 175178.34743508807150647, 526907.09578445507213473 175139.25495811874861829, 526889.09267006127629429 175116.10809675537166186, 526973.96449506049975753 174912.93009145429823548, 526885.95633615972474217 174859.8365453231963329, 526909.64957838621921837 174789.88203135458752513, 526922.28532687691040337 174784.41939029871718958, 526957.33885194035246968 174894.75840272463392466, 526938.1368365534581244 174894.58398754562949762, 526918.67389838397502899 174882.02661713416455314, 526881.00047726207412779 174863.13230195376672782, 526645.98297396756242961 174831.60109246335923672, 526609.50912189844530076 174827.05741743353428319, 526567.45242367009632289 174822.48189269431168213, 526532.3543359829345718 174820.95671778128598817, 526511.19253406394273043 174818.36392042905208655, 526475.19840611529070884 174928.17651417059823871, 526482.59550444374326617 174953.18938274509855546, 526621.9569095199694857 175008.21030497280298732, 526587.08526148088276386 175075.49314598224009387, 526608.94237426621839404 175084.53746851411415264, 526524.52869730209931731 175245.07419345498783514, 526473.27779452677350491 175229.8263443021569401, 526498.70052055746782571 175244.55399248545290902, 526476.25838999240659177 175289.43825361545896158, 526525.35055060335434973 175313.2830173407564871, 526502.38243260327726603 175360.27122821123339236, 526655.2694470772985369 175450.74106705139274709, 526548.66932689363602549 175611.34256390717928298, 526523.42193000798579305 175630.27811157138785347, 526498.17453312233556062 175591.70569966279435903, 526496.73523488116916269 175590.17850534588797018)</t>
+  </si>
+  <si>
+    <t>LineString (526496.73523488116916269 175590.17850534588797018, 526406.30206112191081047 175494.22269502107519656, 526346.69015180855058134 175449.33843389106914401, 526380.35334765608422458 175404.45417276109219529, 526342.83291061769705266 175434.61078570786048658, 526304.6144535921048373 175412.13552230672212318, 526220.48104146879632026 175317.48543366795638576, 526212.83254945755470544 175223.7914065305958502, 526176.50221240427345037 175198.93380749414791353, 526071.33544725005049258 175206.58229950536042452, 526034.04904869536403567 175148.26254791987594217, 526009.19144965894520283 175110.97614936518948525, 526011.10357266175560653 175093.76704233995405957, 526011.20072534133214504 175093.52450637135189027, 526028.17182268667966127 175051.15715683341841213, 526084.52183982264250517 174972.04738347270176746, 526120.93744978227186948 174927.4696540392760653, 526209.46505330502986908 174784.94649092113832012, 526119.83870293013751507 174923.07466663033119403, 526053.28603645204566419 175005.32371671171858907, 526010.59187305101659149 175067.48139578086556867, 525994.89548944763373584 175089.45633282553171739, 525949.06204932602122426 175022.90366634743986651, 525855.51160305016674101 174953.83957849282887764, 525828.51382325252052397 174995.27803120561293326, 525855.66856688621919602 174947.56102505151648074, 525805.44013935560360551 174918.05182387726381421, 525814.23011417349334806 174839.56990586066967808, 525702.0009714097250253 174820.10639019258087501, 525698.8616946890251711 174722.78881185199134052, 525659.9346633527893573 174636.77262970581068657, 525565.36717306601349264 174664.02053710119798779, 525538.06676878000143915 174653.24728339188732207, 525493.99436724185943604 174553.83953325595939532, 525459.71583271224517375 174532.29302583733806387, 525496.93252734444104135 174407.42122147939517163, 525457.92714756459463388 174534.53035107266623527, 525490.77226448152214289 174556.32890400406904519, 525543.79577161197084934 174666.49996881955303252, 525536.72597066126763821 174676.51552016640198417, 525515.04797329346183687 174692.30743877869099379, 525500.11743205995298922 174748.58409419711097144, 525507.00845109077636153 174843.90985745683428831, 525596.59169849148020148 174873.7709399237355683, 525710.00638670718763024 174878.36495261095114984, 525777.76807384355925024 174928.89909217032254674, 525768.58004846912808716 175008.14581102479132824, 525713.45189622254110873 175119.55061868979828432, 525685.88782009924761951 175159.74822970293462276, 525595.15606952679809183 175150.56020432850345969, 525492.93928723619319499 175144.81768846948398277, 525471.69197855785023421 175159.74822970293462276, 525369.47519626724533737 175139.07517261046450585, 525386.70274384436197579 175104.62007745634764433, 525230.50631247903220356 175056.3829442405840382, 525197.19972049666102976 175054.0859378969471436, 525166.19013485801406205 175226.36141366756055504, 525089.24042234709486365 175214.8763819495216012, 525097.279944549780339 175086.24402670745621435, 525104.45808937354013324 175049.49192520976066589, 525199.78385263320524246 174985.17574758871342055, 525214.81787929905112833 174966.87071981595363468, 525190.62146005278918892 174953.39830346533562988, 525127.28929241502191871 174934.86312413716223091, 525064.65251295559573919 174957.45343804056756198, 525099.16753414331469685 174650.99683751305565238, 525102.00163976603653282 174620.04028388037113473, 524979.1647777232574299 174597.37606225861236453, 524937.07801401300821453 174585.3315757944365032, 524940.61593483120668679 174596.39404977264348418, 524962.98638330516405404 174622.83447105140658095, 524944.37760573695413768 174606.91934299230342731, 524890.5032964691054076 174612.08132202102569863, 524777.03524737863335758 174619.39787700184388086, 524680.01865243853535503 174723.03394835483049974, 524522.6853424928849563 174831.17963737441459671, 524475.66009829880204052 174858.21915278598316945, 524323.54649589885957539 174929.67139882530318573, 524302.64638736820779741 174931.76140967838000506, 524251.52485175657784566 174949.68193757452536374, 524272.59287336631678045 175049.00829122628783807, 524272.14576235634740442 175067.33352094312431291, 524042.01348253048490733 175122.84527774224989116, 524018.31376306770835072 175131.4362350333831273, 523987.54343810823047534 175136.79924140661023557, 523960.12279363907873631 175046.48958203330403194, 524000.25377948675304651 175034.22337187058292329, 523966.59409888373920694 175032.38559600326698273, 523951.98165977036114782 175045.27283976325998083, 524036.35662941134069115 175313.19315103691769764, 524059.98113962868228555 175307.65666737424908206, 524327.96859593223780394 175207.23306857905117795, 524341.93538261542562395 175220.81630157568724826, 524471.09094912011642009 175168.31033058575121686, 524509.24167378677520901 175273.27074366103624925, 524654.88253770291339606 175213.55327629734529182, 524711.1153041081270203 175194.90256357757607475, 524706.84647323249373585 175187.00979776872554794, 524628.75152248388621956 175210.13245730067137629, 524518.74834085872862488 175260.84737031435361132, 524477.97536607540678233 175285.99682499363552779, 524380.67268556274939328 175322.80957126850262284, 524218.49263602652354166 175448.51886382378870621, 524123.84486623620614409 175480.16830401346669532, 524107.50576417194679379 175492.16410046571400017, 524128.81952411436941475 175549.43083725060569122, 524093.59998840204207227 175564.60831672887434252, 524054.6833743552560918 175482.29967801991733722, 524045.09912176639772952 175488.11071598145645112)</t>
+  </si>
+  <si>
+    <t>LineString (524044.91210958641022444 175488.04344289214350283, 524085.52461603935807943 175461.19657479849411175, 524103.28008306899573654 175495.27063632552744821, 524138.79455675766803324 175591.48109126661438495, 524129.17100038880016655 175633.29742638493189588, 523976.51973626675317064 175725.69477560109226033, 524005.3036557876621373 175719.74511276691919193, 524151.31351847440237179 175627.49342679663095623, 524325.26564783230423927 175881.45175875423592515, 524265.40427828562678769 175894.51242120077949949, 524182.68674945743987337 175922.81052316830027848, 523924.7386661380296573 176107.83657449448946863, 523885.55667879834072664 176168.78633257842739113, 524033.5775198593037203 176344.0168870696797967, 524088.59564563841558993 176404.0004238125984557, 524217.18918832298368216 176480.86513136423309334, 524234.28227358422009274 176458.37422970472835004, 524314.94964086962863803 176518.34996746337856166, 524328.14430317643564194 176505.15530515648424625, 524406.35059385467320681 176563.87137158666155301, 524530.42688709695357829 176645.50051187761710025, 524556.54821199004072696 176598.69980477745411918, 524615.32119299960322678 176566.04814866106607951, 524656.19633344910107553 176622.45522326184436679, 524673.86358512495644391 176669.64518129741190933, 524687.07387990888673812 176707.38888068028609268, 524697.76792806736193597 176718.08292883876129054, 524791.82018601219169796 176798.60282085544895381, 524894.62324445182457566 176690.62037168533424847, 524947.35885916277766228 176642.90719647065270692, 524977.49349614046514034 176666.13597914096317254, 524900.58739135367795825 176605.86670518555911258, 524870.45275437599048018 176633.49012241512537003, 524732.33566822810098529 176495.37303626732318662, 524628.43395114876329899 176566.94279908936005086, 524566.90906731935683638 176469.00522891184664331, 524555.92248092114459723 176450.17108080073376186, 524611.16931538027711213 176409.99156483047408983, 524670.51981275726575404 176371.66103527450468391, 524673.61098449560813606 176338.27638049997040071, 524636.5169236350338906 176296.23644485796103254, 524565.41997365222778171 176214.62951096461620182, 524571.60231712902896106 176203.50129270643810742, 524604.68284478283021599 176174.72198301905882545, 524588.03502420790027827 176155.80400509302853607, 524535.064686015015468 176062.22307428557542153, 524514.25491029641125351 176016.81992726307362318, 524478.18463238410186023 176002.69450374494772404, 524412.60230890719685704 175996.64075080861221068, 524397.46792656637262553 175964.35406848150887527, 524407.55751479358877987 175947.20176849522977136, 524409.57543243898544461 175893.72695089096669108, 524410.77357104083057493 175873.16941487803705968, 524408.75565339543391019 175849.71112224974785931, 524414.93552618462126702 175841.26109210946015082, 524437.00650043168570846 175835.45957887879922055, 524651.41025026002898812 175810.99232742778258398, 524731.11799725505989045 175799.89378037783899345, 524754.32405017770361155 175993.61387434042990208, 524753.31509135500527918 176084.42016838540439494, 524796.70032073196489364 176103.59038601713837124, 525047.12265628203749657 176180.61843837762717158, 524992.33966347749810666 176361.30496533127734438, 525128.8617562991566956 176407.8115966334589757, 525215.05184906325303018 176421.69970128277782351, 525318.75507486017886549 176515.06803950533503667, 525329.99290352826938033 176505.92964351741829887, 525213.53843648789916188 176411.26652987388661131, 525090.62899151816964149 176387.06088406970957294, 525061.77148157625924796 176376.93670005700550973, 525085.56370682967826724 176240.99830333300633356, 525104.72513684059958905 176197.52988835732685402, 525071.38045466400217265 176177.87953445233870298, 525184.4233297451864928 175922.32358751614810899, 525232.21329014201182872 175831.17452397785382345, 525394.0406293993582949 175972.00136882782680914, 525380.45207419455982745 175992.38420163505361415, 525579.64794026513118297 175772.49667195708025247, 525789.04116105276625603 175920.79213703639106825, 525794.67906692263204604 175913.40021600711042993, 525796.36541037389542907 175924.88107120373751968, 525831.44916197401471436 175948.5820945069717709, 525842.88386619929224253 175956.48243560802075081, 525966.89843111461959779 175827.58213343276293017, 526037.0428866392467171 175909.39836246441700496, 526083.99901098641566932 175909.39836246441700496, 526183.90565853379666805 175950.36008795883390121, 526213.87765279808081686 175990.32274697776301764, 526258.58368871151469648 176103.28294610444572754, 526151.85186089854687452 176147.91625591710908338, 526151.49614943633787334 176179.64869351152447052, 526047.38884781103115529 176231.98070609322167002, 526018.99594736774452031 176239.218112088565249, 526012.31526491045951843 176231.42398255510488525, 525961.23868289159145206 176229.001861541881226, 525788.46569891297258437 176403.76074188807979226, 525739.81123790750280023 176436.52803195299929939, 525728.0358450491912663 176477.41611387868761085, 525702.36593637219630182 176520.02743093523895368, 525681.16035963909234852 176514.67023260265705176, 525672.11343565175775439 176513.5143718154868111, 525598.1237177683506161 176794.07800558168673888, 525590.47065528121311218 176803.15163323399610817, 525576.05627165164332837 176800.20250201458111405, 525603.30556521995458752 176824.95719950424972922, 525545.77949344262015074 176885.87943373149028048, 525467.20725123130250722 176931.41561955848010257, 525439.5283931796438992 176951.95154650005861185, 525403.81373762898147106 177049.27398287542746402, 525403.81373762898147106 177092.13156953614088707, 525397.56367290765047073 177140.34635452943621203, 525389.52787540876306593 177153.73935036090551876, 525384.84032686776481569 177171.15024494181852788, 525401.57936285785399377 177193.54199610272189602, 525396.49806739354971796 177201.56509420418296941, 525394.6260111698647961 177214.66948776991921477, 525487.42651254346128553 177227.50644473225111142, 525492.50780800764914602 177223.22745907813077793, 525498.9792741967830807 177209.83568196554551832)</t>
+  </si>
+  <si>
+    <t>LineString (525498.9792741967830807 177209.83568196554551832, 525499.70685131091158837 177208.33006480569019914, 525546.48938673955854028 177091.50102327833883464, 525607.1780920778401196 177105.30195335522876121, 525641.23937251162715256 177033.56127417489187792, 525704.87392115953844041 176980.53248363500460982, 525742.65693441918119788 176954.01808836506097578, 525749.9179498142329976 176950.09361684083705768, 525759.91741443739738315 176949.90844157003448345, 525789.17510722379665822 176925.28013055364135653, 525823.06218178023118526 176907.87365509843220934, 525834.31157948146574199 176917.87311972162569873, 525840.02393209061119705 176917.83761663141194731, 525839.83007433160673827 176904.55402936117025092, 525831.35577882663346827 176898.87676776724401861, 525816.50067409395705909 176887.31365200405707583, 525759.91843862924724817 176830.72846091576502658, 525971.4164017754374072 176713.56057522911578417, 525990.28241726732812822 176704.62404157503624447, 525990.28241726732812822 176695.68750792095670477, 526044.89456737553700805 176673.8426478776964359, 526231.32058888114988804 176565.61129584512673318, 526246.21481163799762726 176558.66065855862689205, 526279.02310593228321522 176632.42519633183837868, 526283.16126619779970497 176641.72923013736726716, 526326.25483707862440497 176694.1716895958816167, 526240.12421508901752532 176797.52843598343315534, 526248.73727728798985481 176850.9294216169801075, 526278.02168876444920897 176885.38167041284032166, 526272.85385144501924515 176930.16959384744404815, 526251.69148790801409632 176959.08371336333220825, 526325.95375438174232841 177013.98570174560882151, 526319.56678607675712556 177036.69492238553357311, 526331.39291572826914489 177017.30782459620968439, 526465.45469694142229855 177118.89621701225405559, 526531.37082942517008632 177192.56718861166154966, 526549.98244330286979675 177194.89364034638856538, 526607.62827024597208947 177274.30958925650338642, 526607.62827024597208947 177288.8285534702881705, 526641.02188793767709285 177312.0588962123147212, 526727.77269911498297006 177419.49923139426391572, 526755.35873112105764449 177438.37388487218413502, 526797.46372734103351831 177454.34474550731829368, 526929.58630168635863811 177497.90163814864354208, 527031.94499939354136586 177545.81422005410422571, 527131.79582655231934041 177579.02292893503908999, 527156.87407868099398911 177613.12935183010995388, 527095.68314348696731031 177730.49557179247494787, 527136.81147697800770402 177756.57695400633383542, 527102.70505408302415162 177810.74597860436188057, 527125.77704604144673795 177823.78666971129132435, 527048.53602948493789881 177964.22488163207890466, 527053.25930870475713164 177974.33477002254221588, 527098.19096869986969978 178015.38451597469975241, 526908.94946135848294944 178337.4750089393928647, 526940.62272087635938078 178361.92182539845816791, 526883.33841691690031439 178439.4463433051132597, 526910.62494222086388618 178467.51928232313366607, 526887.60617866518441588 178499.03289314155699685, 526918.00911059393547475 178465.09473867359338328, 526914.67600807105191052 178462.40279670694144443, 526758.43816197034902871 178293.39700141816865653, 526769.00779414852149785 178281.43285661714617163, 526783.34981272195000201 178251.05608661123551428, 526764.73600135685410351 178280.00450905179604888, 526756.2519320712890476 178288.05494963173987344, 526526.90699357143603265 178031.40025283378781751, 526505.86243384412955493 178042.24138966298778541, 526524.99385177798103541 178024.38539959135232493, 526373.21793616958893836 177872.60948398287291639, 526378.31964761856943369 177863.68148894709884189, 526365.56536899600178003 177863.68148894709884189, 526501.56836159329395741 177739.12724830291699618, 526619.97851843247190118 177577.92520181008148938, 526630.38032632856629789 177565.05702568762353621, 526471.97642374865245074 177464.09629657075856812, 526468.49501929641701281 177439.7264654046157375, 526426.7181658687768504 177443.20786985690938309, 526252.64794325339607894 177363.13556745389360003, 526212.61179205193184316 177333.54362960928119719, 526188.24196088581811637 177333.54362960928119719, 526111.65106293500866741 177425.80084759538294747, 526189.54348884453065693 177335.32316621133941226, 526248.99693555117119104 177371.07838590905885212, 526381.31203635118436068 177439.0548791715700645, 526462.80067659239284694 177473.97858213211293332, 526636.94032988674007356 177583.86839270126074553, 526670.26410251285415143 177616.99946092290338129, 526688.55747073027305305 177690.17293379263719544, 526822.43166541238315403 177811.57437741738976911, 527046.55382472439669073 177968.52284097846131772, 527133.60565806506201625 178026.52744588098721579, 527152.05848008545581251 178036.42819022812182084, 527291.56621869676746428 177804.21605766733409837, 527319.9554854022571817 177819.83015435532433912, 527360.1001912277424708 177839.80410252374713309, 527353.88239083020016551 177859.14837042734143324, 527412.6060612517176196 177890.23737241525668651, 527367.00885833613574505 177998.70344601754914038, 527429.8777290228754282 178039.46458195726154372, 527368.39059175783768296 178154.83932266797637567, 527356.64585767348762602 178166.58405675229732879, 527244.18394927959889174 178092.28198195234290324, 527187.99826812464743853 178202.51293736099614762, 527130.47483265656046569 178327.19163935232791118, 527130.47483265656046569 178336.82347040742752142, 527106.47640507481992245 178384.55715666484320536, 527164.85215369169600308 178410.35007031389977783, 527154.54868436977267265 178430.37184342864202335, 527245.21691735507920384 178618.75959407596383244, 527293.66525488265324384 178710.58556358556961641, 527279.48398153169546276 178728.96806519792880863, 527296.81704342004377395 178719.65596891054883599, 527313.62467651721090078 178762.66981539080734365, 527337.94203093100804836 178751.72700590462773107, 527419.45399717660620809 178711.76451556503889151, 527479.39759952831082046 178777.611654511973029, 527424.4321250639623031 178709.32203599691274576, 527552.51673102448694408 178625.85540736871189438, 527527.96637719089630991 178599.2435734422178939, 527515.02121530997101218 178586.53641387179959565, 527538.98158421937841922 178566.8297592174494639, 527641.03992576699238271 178487.17096276683150791, 527636.13838343927636743 178480.70983878933475353, 527628.56327256909571588 178478.25906762547674589, 527637.92076246754731983 178448.62701628042850643, 527645.05027858063112944 178430.5804286191414576, 527663.09686624188907444 178407.4095012515608687, 527665.10204264870844781 178405.84991960183833726, 527659.53210818534716964 178400.50278251702548005, 527674.67989808064885437 178389.84342098905472085, 527652.43348332692403346 178373.39041538978926837, 527656.76978971192147583 178369.27718900417676196)</t>
+  </si>
+  <si>
+    <t>LineString (527656.7183093624189496 178369.34070502704707906, 527783.66874267382081598 178260.44675826572347432, 527701.29201637103687972 178172.63382336677750573, 527726.60529186681378633 178158.51739612722303718, 527707.29683605546597391 178172.78455480805132538, 527838.83275414002127945 178317.72066099435323849, 527870.91154732566792518 178356.61619773207348771, 527746.60622373130172491 178482.5254609857511241, 527869.90908503858372569 178585.97956900941790082, 527839.18433681316673756 178655.71945479151327163, 527835.94589031487703323 178664.7629006463685073, 527776.6708300617756322 178800.04388493386795744, 527853.03527260560076684 178816.77474871501908638, 527868.81008702784311026 178834.93968653454794548, 527956.28860336926300079 178854.53869839245453477, 527945.29403574171010405 178902.34116633859230205, 527960.59082548448350281 178906.64338845372549258, 528074.04253716359380633 178926.48126136808423325, 528075.63601999881211668 178916.12362293904880062, 528060.09956235531717539 178881.8637419814185705, 528072.05068361957091838 178818.12442857190035284, 528067.92073296045418829 178806.12665641392231919, 528040.501292280619964 178800.6427682779612951, 528050.44083952705841511 178741.0054847993014846, 528058.38286198873538524 178718.14782906166510656, 528102.34081977850291878 178746.40651621224242263, 528250.96058182965498418 178905.49245868952129968, 528307.84153715777210891 178965.57330830910359509, 528456.10630761610809714 179120.06087270937860012, 528453.06503982131835073 179134.64540692919399589, 528421.32784037000965327 179147.83876678114756942, 528276.90514995099510998 178992.9140435898443684, 528343.29222077992744744 178930.61010330502176657, 528508.60514012665953487 178773.42616898694541305, 528627.19860546640120447 178713.62781604222254828, 528688.83252045430708677 178852.26219280663644895, 528695.22035057423636317 178849.19359146716305986, 528631.00734287954401225 178710.50025443226331845, 528694.29413869057316333 178684.68859138496918604, 528704.07457833737134933 178673.90502972310059704, 528675.54235468478873372 178676.5972451399138663, 528566.76733427762519568 178496.98558549524750561, 528583.98656073305755854 178472.45039081721915863, 528590.69624376785941422 178461.60069059068337083, 528559.28921679628547281 178483.15733183023985475, 528530.16633724083658308 178495.29186497832415625, 528481.12854740128386766 178503.28638093473273329, 528322.66582040826324373 178458.74550632052705623, 528317.48233069677371532 178476.88772031053667888, 528318.63421729940455407 178485.81484148022718728, 528306.97136544866953045 178503.66908381960820407, 528286.37375599541701376 178488.37048086652066559, 528274.68490427918732166 178477.86123803912778385, 528230.34233377804048359 178459.68453743468853645, 528242.35289700934663415 178427.08443723549135029, 528172.00531236897222698 178397.91592653095722198, 528134.25782792770769447 178356.73685259514604695, 528536.36687937250826508 177976.28225404073600657, 528565.26066673942841589 177951.17037601495394483, 528618.5099502638913691 177941.48868810140993446, 528799.1956435035681352 177949.62260939209954813, 529089.81677403079811484 177901.90869243987253867, 529255.79840785474516451 177863.14847174196620472, 529358.25357655365951359 177883.68841009688912891, 529427.69813003926537931 177906.1845330570358783, 529433.56668385502416641 177888.57887160996324383, 529378.79351490852423012 177854.34564101841533557, 529295.6556691862642765 177852.38945641319151036, 529234.28037719719577581 177853.36754871581797488, 528956.5021632545394823 177913.03117917533381842, 528790.22647180990315974 177935.52730213548056781, 528692.90628769970498979 177932.5930252276302781, 528557.92954993876628578 177932.5930252276302781, 528554.01718072837684304 177894.44742542563471943, 528627.54724844382144511 177420.27802047552540898, 528632.27978818584233522 177383.89662120884167962, 528696.16907470289152116 177392.77013322510174476, 528706.22572165471501648 177407.55931991888792254, 528704.45101925148628652 177685.8918134956038557, 528709.77512646117247641 177687.66651589883258566, 528709.18355899350717664 177399.27737537038046867, 528698.53534457390196621 177388.62916095086256973, 528633.46292312140576541 177378.57251399909728207, 528658.30875676684081554 177201.69384114164859056, 528671.9148085251217708 177111.77558604351361282, 528696.37895216140896082 177096.46537706872913986, 528698.52647522534243762 177087.85737352253636345, 528707.54613430006429553 177045.9768067144905217, 528686.48968786001205444 177029.56326320749940351, 528651.63210264872759581 177034.21630194777389988, 528601.67845188046339899 177025.25386094400892034, 528636.23278523643966764 177061.25791369623038918, 528648.99903309403453022 177090.69567049364559352, 528683.61924763000570238 177095.42086361086694524, 528707.09237683820538223 177083.02097844227682799, 528717.31761167501099408 177070.66164703483809717, 528900.55563481082208455 177088.40867106735822745, 529012.84455444279592484 177200.88158813735935837, 529132.22997563553508371 177273.7439153409213759, 529136.69044820708222687 177251.27508732164278626, 529135.47952493233606219 177274.99521491886116564, 529192.11810795951168984 177297.59016217343742028, 529279.07078784692566842 177338.04844474766287021, 529379.56394133775029331 177459.42329247039742768, 529514.28841154393739998 177579.99861740384949371, 529522.47303623706102371 177587.32366964058019221, 530009.96149630157742649 177853.79645061693736352, 530094.68275518657173961 177878.00252458406612277, 530200.58432879275642335 177862.87372835460701026, 530315.37161932047456503 177998.80604608487919904)</t>
+  </si>
+  <si>
+    <t>LineString (533114.38557692908216268 180650.94499810261186212, 532993.2912894997280091 180672.05200613249326125, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531662.09765580005478114 180911.36713150818832219, 531644.95713887771125883 180910.93905784812523052, 531621.9483896060846746 180876.42593394074356183, 531595.00393322226591408 180858.26113188423914835, 531572.22224397643003613 180843.12379683717153966, 531551.33272161148488522 180836.46336941645131446, 531511.58714895439334214 180836.14345619000960141, 531510.64536264294292778 180916.21691724128322676, 531435.75916852697264403 180912.37710467760916799, 531466.5541653853142634 180913.61106873201788403, 531465.03699818823952228 180989.25269041734281927, 531387.01125662168487906 180986.86857053614221513, 531389.17863833182491362 181128.18185803995584138, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531132.9760996779659763 181281.26323102368041873, 531047.80579616781324148 181254.33936599228763953, 531131.03878337366040796 181286.03806058526970446, 531110.30965442163869739 181356.39285153028322384, 531197.1542466712417081 181376.88721254793927073, 531286.93602178571745753 181375.08379181567579508, 531305.25734407640993595 181583.75572135805850849, 531325.21203300100751221 181586.18808011634973809, 531388.88918386655859649 181572.61640889989212155, 531390.49493819230701774 181599.32936576748033985, 531367.26279260986484587 181685.65545662579825148, 531395.89248193160165101 181593.61920236010337248, 531412.32238542404957116 181591.09869188832817599, 531419.12145480117760599 181581.94767167716054246, 531385.41458384564612061 181534.11455342586850747, 531374.38023236603476107 181529.41130202304339036, 531413.36951656360179186 181525.26491641241591424, 531471.93530321691650897 181443.00015478587010875, 531489.86913823755457997 181396.66486753628123552, 531500.42645009863190353 181343.75654840667266399, 531561.43261282751336694 181271.18043218745151535, 531499.01550433901138604 181334.88368744595209137, 531566.52648988855071366 181353.74707860476337373, 531590.37191976455505937 181360.8123911606380716, 531583.52515332715120167 181463.7283773985109292, 531566.74728090583812445 181537.16921628548880108, 531557.91564021108206362 181566.97600363052333705, 531578.66999584389850497 181574.92448025586782023, 531607.15203708468470722 181582.43137484646285884, 531674.27250636543612927 181614.50127011956647038, 531688.84471351187676191 181590.65584024353302084, 531676.92199857381638139 181529.27593741449527442, 531692.81895182456355542 181520.00271468493156135, 531744.15286336338613182 181527.39921376685379073, 531827.17028589476831257 181517.68440900254063308, 531837.76825472852215171 181595.40284711701679043, 531873.09481750777922571 181627.19675361836561933, 531892.79980997554957867 181649.86393449633033015, 531906.87584316555876285 181666.05597267561824992, 532031.40197696257382631 181539.76351073960540816, 532080.85916485369671136 181575.09007351889158599, 532117.06889170245267451 181580.38905793579760939, 532140.91432157845702022 181599.81866746442392468, 532170.05873587145470083 181590.98702676958055235, 532184.18936098308768123 181559.19312026820261963, 532149.74596227332949638 181529.16554190579336137, 532138.2648293700767681 181394.04143927496625111, 532132.82734409463591874 181370.85496780133689754, 532125.90053239720873535 181323.38831371636479162, 532096.75611810432747006 181293.36073535395553336, 532017.27135185094084591 181313.67350895205163397, 532018.15451592043973505 181340.1684310365235433, 532031.40197696257382631 181369.31284532946301624, 532033.16830510157160461 181389.62561892755911686, 532057.23452599509619176 181405.74336319562280551, 532119.69996919808909297 181395.70321314127068035, 532140.79753599606920034 181364.76011517079314217, 532132.3034719011047855 181288.28254195442423224, 532160.56472212448716164 181242.35801034132600762, 532384.22602272103540599 181180.09494344278937206, 532424.85156991728581488 181173.91279495641356334, 532670.78084617818240076 181110.13770430514705367, 532818.19047775026410818 181176.80775713562616147, 532780.99707011831924319 181260.68462679820368066, 532688.27519202104303986 181257.87865509698167443, 532650.54560429917182773 181265.88190097737242468, 532436.45877699879929423 181308.18477205943781883, 532413.59236019768286496 181321.90462214010767639, 532414.73568103776779026 181427.0901394252141472, 532338.13318475405685604 181459.10312294677714817, 532350.7097139946417883 181509.40923990920418873, 532405.30328410735819489 181674.61910129722673446, 532528.63901972828898579 181635.46036252533667721, 532616.67472441249992698 181609.7356436240952462, 532609.81479937222320586 181581.72428304271306843, 532720.71692085755057633 181553.71292246135999449, 532855.62877998419571668 181525.1299014599644579, 533071.32848995237145573 181469.8718779842602089, 533186.19458453194238245 181444.03007418513880111, 533181.16196181264240295 181435.64236965295276605, 533152.08458610100205988 181436.48114010615972802, 533186.47417468298226595 181432.28728784006671049, 533189.54966634477023035 181438.99745146580971777, 533246.78843064326792955 181526.30952275943127461, 533260.0739210395840928 181527.98328532904270105, 533340.41452438081614673 181492.83427136726095341, 533338.70870435202959925 181483.54382457892643288, 533339.90022310265339911 181474.30955426144646481, 533358.96452311298344284 181468.35196050821105018, 533371.7733496823348105 181461.2028480043518357, 533421.18748124549165368 181431.14743276051012799, 533457.81188699707854539 181401.60169366677291691, 533466.42939423269126564 181399.13954874229966663, 533532.90730719361454248 181489.9311428323853761, 533627.23823461274150759 181537.48131668634596281, 533600.77017667470499873 181593.49511371820699424, 533571.96468304062727839 181647.30677931586978957, 533565.79550759738776833 181677.67810457508312538, 533566.74461151170544326 181709.94763766299001873, 533571.49013108352664858 181761.67380099510774016, 533438.61558307439554483 181753.13186576595762745, 533368.85644536965992302 181739.84441096504451707, 533363.63351622002664953 181744.60156841060961597, 533362.33726643316913396 181745.78222090430790558, 533349.36948162270709872 181755.27449376182630658, 533376.01579060044605285 181931.55007622967241332, 533386.24188510165549815 181988.51551208973978646, 533386.32651571999303997 181988.9869550303556025, 533395.4760166349587962 182035.56623241596389562, 533318.95291807304602116 182051.36991581466281787, 533232.44854578538797796 182077.1548729388450738, 533173.13606239529326558 181928.21060169869451784, 533081.3675638793502003 181840.45443919772515073, 533032.44119917706120759 181849.24923483061138541)</t>
+  </si>
+  <si>
+    <t>LineString (530248.37173048651311547 182901.4726771293208003, 530247.19071921310387552 182900.21293177100596949, 530251.05921820166986436 182893.88266069884411991, 530184.08185019285883754 182852.74914162818458863, 530085.83308541483711451 182787.51840435751364566, 530111.18260209145955741 182744.29519918368896469, 529990.56694557412993163 182662.18936071105417795, 529961.50293195550329983 182710.87158352226833813, 529962.22953229595441371 182727.58339135299320333, 529962.59283246623817831 182727.22009118273854256, 529972.76523723278660327 182752.65110309905139729, 529932.80478152283467352 182814.59110673272516578, 529979.07706384977791458 182754.49032623908715323, 529993.03934241353999823 182732.28046154495677911, 529968.62376257998403162 182714.22668772435281426, 530013.09155612858012319 182629.12904521985910833, 530018.17775851185433567 182621.49974164497689344, 530100.32880480831954628 182494.38274551162612624, 530104.0113532249815762 182482.84132467227755114, 530220.50368910923134536 182556.47051627180189826, 530255.09743770561181009 182478.63458192982943729, 530272.39431200386025012 182483.35191128388396464, 530279.47030603489838541 182470.7723663397191558, 530137.95042541308794171 182415.73685720900539309, 530133.8373461066512391 182413.51172491264878772, 530186.21162480069324374 182272.1011724385607522, 530075.7495097367791459 182226.86884083910263143, 530075.1733111577341333 182226.46204725949792191, 530187.16388441331218928 182265.91148495653760619, 530233.22869966924190521 182154.23642371431924403, 530357.8921046924078837 182201.72724467553780414, 530348.98757576220668852 182228.44083146619959734, 530358.86895656702108681 182231.0766534095746465, 530394.74696868821047246 182125.29837629428948276, 530508.99968287569936365 182165.49652313266415149, 530513.72136097133625299 182167.0985210579528939, 530567.86575565708335489 182188.16529536261805333, 530573.45622016047127545 182150.89553200689260848, 530664.76714038196951151 181926.34520778860314749, 530694.76100652059540153 181850.76066511913086288, 530759.06664636044297367 181869.87285391447949223, 530674.73822676041163504 181825.22436629422008991, 530573.75377231650054455 181777.63399121144902892, 530599.29007114132400602 181730.04361612870707177, 530646.88044622412417084 181748.21467864664737135, 530657.97477119497489184 181732.12790743884397671, 530724.74751764547545463 181760.6236275052651763, 530741.12779784575104713 181707.06197263259673491, 530773.19373494503088295 181600.7954151411249768, 530782.75100370426662266 181575.85406711159157567, 530688.89235894195735455 181552.28991476428927854, 530627.95015930733643472 181539.24596229381859303, 530599.01706093887332827 181486.621268884598976, 530600.06536160444375128 181482.63772635560599156, 530608.87108719476964325 181476.34792236247449182, 530639.82865497504826635 181423.25654537187074311, 530713.75870660948567092 181269.28719607146922499, 530693.84197932516690344 181263.16111494251526892, 530717.14176355150993913 181259.05196211650036275, 530725.90888015425298363 181237.15531960281077772, 530777.48901169560849667 181216.35996013710973784, 530818.8762664794921875 181237.42591273161815479, 530793.81802459026221186 181220.82747317798202857, 530815.62781070545315742 181198.7895409248303622, 530811.81109403807204217 181182.0243397920858115, 530813.52439235441852361 181170.48626728833187371, 530798.10321753786411136 181142.40510449395515025, 530780.39245925494469702 181104.23634472012054175, 530781.57594784977845848 181091.27197462657932192)</t>
+  </si>
+  <si>
+    <t>Walk bikes through Little Turnstile (70m) and John Watkins plaza</t>
+  </si>
+  <si>
+    <t>LineString (522501.94230883487034589 178726.41802728205220774, 522509.3171643289970234 178692.11021129344590008, 522504.37178637820761651 178610.51147510507144034, 522674.06006731535308063 178577.74834618097520433, 522695.07792360632447526 178757.01829689781880006, 522871.25624804722610861 178766.46876867543323897, 523096.53894994757138193 178769.45924701925832778, 523146.56457700586179271 178764.79577539447927848, 523228.15499849966727197 178681.39223342304467224, 523341.47502835217164829 178625.18549861619248986, 523349.17238342546625063 178622.56512242107419297, 523338.6908786449348554 178607.66173281130613759, 523330.33842952299164608 178605.53267715277615935, 523318.05541610840009525 178608.31682686010026373, 523049.53108943597180769 178557.41122244377038442, 523044.84592751995660365 178556.49860799589077942, 523038.88646519993199036 178504.87752603454282507, 523045.46353330073179677 178491.7233898330014199, 523052.69884405157063156 178411.49882859381614253, 523054.4322625290369615 178375.4288675059506204, 523103.10630509618204087 178343.670138604065869, 523108.87300237617455423 178325.90583238122053444, 523119.7353025998454541 178318.10387213190551847, 523126.32058558438438922 178326.65065053338184953, 523136.96704334113746881 178320.71276599433622323, 523197.00493266043486074 178288.80073473454103805, 523242.30379059282131493 178263.10884516095393337, 523127.63683081179624423 178184.14008984004613012, 523181.18413750198669732 178115.4480903485964518, 523221.2093970482237637 178062.44166554414550774, 523237.43585362087469548 178040.26550822801073082, 523471.72365575307048857 178194.08150103568914346, 523504.52584943413967267 178070.048206178820692, 523533.22776890522800386 178030.07053262993576936, 523398.27638210507575423 177944.08385379810351878, 523374.85150622186483815 177922.22063630708726123, 523440.44115869491361082 177805.09625689091626555, 523462.30437618592986837 177764.4931386933021713, 523365.48155586858047172 177712.95841175017994829, 523424.82457477279240265 177581.77910680408240296, 523434.19452512607676908 177552.10759735197643749, 523498.16975758440094069 177350.68934009084478021, 523543.47255923581542447 177377.19986846460960805, 523720.65685013914480805 177494.3160001412325073, 523740.79142865084577352 177501.02752631180919707, 523763.52510854077991098 177520.51030919776530936, 523791.01839464512886479 177472.12212565407389775, 523850.40389263059478253 177270.87127137003699318, 523905.39046483935089782 177009.13518765641492791, 523950.85999103111680597 176923.03958886690088548, 524024.87041156162740663 176766.3116395082033705, 524158.7422016387572512 176861.0014422457315959, 524150.03509334108093753 176879.50404737834469415, 524347.03341857658233494 176991.60806671128375456, 524324.17725929513107985 177034.05521966257947497, 524476.55165450496133417 177106.97725165582960472, 524501.58459086087532341 177071.06042992777656764, 524552.73885210976004601 177093.91658920928603038, 524496.59686273266561329 177229.15389398331171833, 524449.34194107458461076 177318.12462787510594353, 524399.1698832738911733 177302.76348325112485327, 524404.66854049474932253 177329.1570379113254603, 524169.69941686512902379 177380.1700359427195508, 524119.83809645345900208 177460.02507976815104485, 523954.87837982719065621 177548.00359530214336701, 524125.23060610314132646 177470.69582927966257557, 524276.1069283313699998 177516.75281185458879918, 524264.62413314066361636 177545.0041890301508829, 524284.58432462147902697 177528.76640343241160735, 524401.59080314182210714 177544.16933234094176441, 524598.18210187566000968 177647.93601894256426021, 524702.78518042073119432 177684.64508786791702732, 524730.84316259669139981 177694.39206814055796713, 524743.63401176454499364 177685.64633391896495596, 524749.76929571013897657 177691.34065775718772784, 524785.28179647319484502 177706.26515992148779333, 524805.12269188673235476 177677.06875034020049497, 524890.26466468954458833 177733.9889697001199238, 524900.02326978160999715 177732.91675252851564437, 524914.16278953978326172 177714.11232543102232739, 524914.433173893019557 177703.10024843754945323, 524895.1238769325427711 177675.34173217235365883, 524920.4659545662580058 177628.80580489605199546, 524910.18844398378860205 177623.75821537460433319, 524917.57360786944627762 177620.23991505563026294, 524938.32413323107175529 177584.05164737423183396, 524950.20932233543135226 177593.41349562600953504, 524943.99898932594805956 177602.68904486036626622, 524939.81656498205848038 177602.46701134811155498, 524944.64205134124495089 177603.30154497240437195, 524951.62820201518479735 177594.10471880476688966, 524978.48803550400771201 177611.26339810941135511, 524991.338410071330145 177614.20456636406015605, 524996.90309547598008066 177616.60875923844287172, 525046.99662963894661516 177531.42582527716876939, 525239.41112284129485488 177643.52029113803291693, 525247.45787289727013558 177648.27282234595622867, 525259.52019177761394531 177658.21438176609808579, 525180.47252021881286055 177798.30595981661463156, 524957.03894217207562178 177697.24630155507475138, 524904.35931604239158332 177802.04137613053899258, 524828.42314845940563828 178030.7590969885350205, 524705.97326419106684625 178005.83836105518275872, 524533.05028670514002442 177972.15814960357965901, 524412.19303111883345991 177923.3538982339669019, 524347.32041661813855171 177918.60612411511829123, 524215.25543399516027421 177874.27527343999827281, 524153.58899412449682131 177868.02728649199707434, 524107.64839021116495132 177866.90650818648282439, 524077.78060873120557517 177856.69226100511150435, 524086.80756595288403332 177870.61416968662524596, 524045.25677349988836795 177910.08328927803086117, 523833.18216259987093508 177995.34252377698430791, 523819.950420176028274 177988.69269825710216537, 523786.25443879171507433 178026.36677837959723547, 523723.08611731143901125 178130.99483389721717685, 523834.20989532244857401 178190.30815001711016521, 523794.47597305721137673 178252.39056805544532835, 523924.27272151375655085 178295.13950059562921524, 524017.76622407609829679 178319.41152608778793365)</t>
+  </si>
+  <si>
+    <t>LineString (524019.5942947514122352 178316.91922095965128392, 524147.7133394600241445 178306.75905061210505664, 524166.91197717498289421 178284.19988717755768448, 524354.64446763973683119 178269.30031749303452671, 524399.84070607554167509 178273.06237215833971277, 524414.83044529519975185 178259.25790301198139787, 524410.00335248897317797 178275.08226800878765061, 524460.50269656255841255 178279.86024319374701008, 524545.15821839333511889 178304.07423270272556692, 524543.03650101134553552 178318.19322945724707097, 524606.41363690642174333 178341.00155929423635826, 524585.96807908453047276 178393.16329537253477611, 524641.53035025740973651 178409.4543690562422853, 524644.76698741316795349 178405.13885284864227287, 524586.18761726538650692 178398.75567615206819028, 524557.75235208170488477 178462.92715298544499092, 524533.38262645772192627 178466.85974151274422184, 524527.65925442636944354 178452.12205853176419623, 524496.18070825340691954 178442.39232607831945643, 524427.78641247749328613 178419.42729580210288987, 524292.65770760283339769 178428.95569482402061112, 524285.72796285967342556 178500.85179653487284668, 524141.93575943791074678 178524.23968504322692752, 524134.57290564820868894 178602.63242245087167248, 524072.20520295930327848 178751.62193443000433035, 523910.22241958661470562 178665.86634323271573521, 523905.02511102921562269 178451.91047428591991775, 523915.41972814401378855 178413.79687819821992889, 523895.92982105386909097 178448.44560191431082785, 523726.1510748450527899 178452.77669237882946618, 523708.82671298703644425 178632.95005570244393311, 523695.29205528547754511 178640.31290949208778329, 523686.62987435649847612 178648.54198137467028573, 523680.02150594454724342 178649.19214336172444746, 523900.87884802120970562 178671.65342459944076836, 523999.36567001842195168 178726.5068444459757302, 523959.47227376641239971 178773.2569181787839625, 523927.20931058085989207 178820.58665569889126346, 523850.2099083709763363 178872.39582184806931764, 523892.85029150103218853 178940.42065121117047966, 523998.51854862732579932 179080.1726343011832796, 524045.92328174656722695 179069.92708279716316611, 524108.31766754906857386 179070.02411880018189549, 524108.13091779133537784 179068.4773711011512205, 524042.70696497993776575 179065.09797074663219973, 523999.53327132220147178 179074.33729632402537391, 523939.45133300090674311 179101.74353711132425815, 523931.0548391982447356 179077.84969023033045232, 523832.73847269039833918 178950.01551744830794632, 523808.87133779458235949 178919.72486848966218531, 523809.41094240511301905 178912.73769014445133507, 523799.16029718943173066 178891.93745666136965156, 523586.12709654704667628 178975.25572723767254502, 523546.82854762935312465 178989.41042456653667614, 523455.77026956726331264 179026.61562438475084491, 523425.37385861721122637 179017.71911386278225109, 523394.55668384418822825 178968.1703076938574668, 523386.43806897010654211 178974.87698954631923698, 523390.32088477944489568 179020.23533786431653425, 523400.29266174440272152 179082.18389918576576747, 523455.35804958565859124 179075.1242340778990183, 523472.30124584451550618 179109.01062659561284818, 523504.09316043963190168 179333.90299656018032692, 523501.12058276316383854 179549.91030771631631069, 523489.23027205729158595 179569.72749222605489194, 523506.07487889059120789 179573.69092912800260819, 523514.99261191993718967 179520.18453095172299072, 523513.01089346897788346 179360.65619564833468758, 523525.6670606259140186 179357.86960204786737449, 523623.99278196529485285 179332.54146969801513478, 523808.35468181630130857 179496.79414100397843868, 523821.31694713741308078 179494.6065657127473969, 523820.82524603558704257 179440.88822034336044453, 523821.60161350667476654 179423.82347127312095836, 523978.71472944790730253 179559.94275737437419593, 523963.60412625916069373 179581.12237331917276606, 523932.02048844669479877 179605.1507095372362528, 523999.59877721423981711 179655.89870352283469401, 523910.11968204472213984 179798.0550079453678336, 523930.4073799456236884 179829.45350444715586491, 523864.14663150085834786 179860.29696010009502061, 523810.64023332454962656 179872.18727080593816936, 523789.8321895893313922 179869.21469312947010621, 523791.3184784275945276 179862.27867855108343065, 523810.64023332454962656 179862.77410816380870529, 523818.07167751574888825 179851.379227070719935, 523809.64937409909907728 179859.80153048736974597, 523790.32761920208577067 179859.80153048736974597, 523777.1597479346091859 179869.18618441122816876, 523706.58830350730568171 179852.08963036345085129, 523700.07543018303113058 179892.55552700196858495, 523753.57804833719274029 179905.68178868596442044, 523757.7367767600226216 180009.66353510232875124, 523767.00669973070034757 180023.23681901925010607, 523706.96914328029379249 180170.29134639311814681, 523632.6539854159927927 180440.35106004029512405, 523620.79229790804674849 180462.13728423725115135, 523548.03862911934265867 180463.75793557113502175, 523535.22499171097297221 180459.7186919086962007, 523506.46992536378093064 180432.00136401766212657, 523471.37248534307582304 180400.94759161036927253, 523441.88097540393937379 180396.77844605082646012, 523405.13739714992698282 180400.94492353178793564, 523354.80208993284031749 180427.03869174927240238, 523338.7929603232187219 180408.12326784816104919, 523328.15338179533137009 180424.15373995114350691, 523305.84850782883586362 180426.90513797110179439, 523301.15577980724629015 180523.14838607650017366, 523292.50651331816334277 180618.96054938790621236, 523284.62079987034667283 180674.33723709877813235, 523248.287612549145706 180823.73672169324709103, 523180.15017024852568284 181046.19415628933347762, 523195.18096548621542752 181051.93683565245009959, 523202.13110555708408356 181048.79546767444116995, 523198.1975192311219871 181025.29501264891587198, 523215.94951775739900768 180948.18024191819131374, 523266.44380770833231509 180772.14566253469092771, 523290.08581532444804907 180672.17699802399147302, 523301.87572635652031749 180592.6180390000808984, 523321.93386030138935894 180594.37743679818231612, 523345.83390644547762349 180595.59365976107073948, 523343.46150832128478214 180548.75618748448323458, 523354.87576299742795527 180537.93592937797075137, 523380.31128285668091848 180514.1939573377603665, 523406.97587942460086197 180529.63057361770188436, 523484.37468678108416498 180575.0080605911789462, 523509.171474092931021 180541.68172154412604868, 523535.32422105281148106 180470.54419238591799513, 523633.30356490309350193 180465.74028088501654565, 523653.83785533590707928 180470.43274004379054531, 523657.69995753932744265 180447.81861192517681047, 523665.83561170572647825 180442.37385650910437107, 523675.93876430939417332 180435.46308627870166674, 523682.85951727599604055 180423.24514195055235177, 523686.44381641852669418 180412.04702033923240378, 523712.49482848419575021 180418.87395834788912907, 523706.73923687369097024 180445.57087515294551849, 523721.2475296090124175 180427.75734292989363894, 523719.41961515875300393 180446.1546540999552235, 523728.11535413248930126 180423.38281483261380345, 523734.61995970364660025 180436.75314993946813047, 523743.92085290589602664 180445.78751291986554861, 523769.65134543011663482 180443.11091388569911942, 523795.20135089615359902 180453.50444708927534521, 523818.04303102707490325 180456.12513331841910258, 523822.22505310841370374 180471.36572253954363987, 523842.84258654178120196 180463.33524113963358104, 523866.60769404500024393 180445.05963141279062256, 523881.3551514504943043 180423.12364392634481192, 523912.52049187803640962 180435.65034075808944181)</t>
+  </si>
+  <si>
+    <t>LineString (523912.23182315297890455 180434.71100018959259614, 523933.4534212714061141 180352.53366981475846842, 524001.52344168594572693 180143.68549420178169385, 523913.53053296857979149 180113.67887586844153702, 523902.62098808796145022 180137.80206676595844328, 523916.00450257491320372 180117.34166811924660578, 523997.87116536882240325 180145.33954628632636741, 523923.79085326276253909 180363.22947150381514803, 523872.72131736180745065 180542.85840179145452566, 523835.97818674857262522 180523.79079492119490169, 523763.34026239992817864 180654.77233878360129893, 523744.63108860928332433 180677.45673540118150413, 523650.93208653811598197 180844.88014607870718464, 523635.86034783296054229 180877.92901890238863416, 523672.90413934946991503 180906.25662417968851514, 523670.72509278968209401 180920.78360124499886297, 523773.86662995326332748 180929.49978748415014707, 523780.94853127264650539 181260.35169014619896188, 523974.53005634632427245 181333.20707353367470205, 524028.53397912753280252 181282.74034599942388013, 524026.59334985166788101 181290.30040013694087975, 524233.11923408636357635 181385.62614455129369162, 524217.87981449643848464 181424.35966934243333526, 524259.1864618023391813 181439.65405084792291746, 524180.57548385200789198 181646.75296914129285142, 524246.61444996122736484 181674.13497947927680798, 524310.64003295754082501 181756.68368711578659713, 524324.73458955099340528 181770.25499738051439635, 524357.15467388625256717 181768.32267447313643061, 524362.52223751798737794 181772.61672537846607156, 524428.21140558586921543 181747.88693608297035098, 524470.84714648721273988 181712.35715199852711521, 524536.93254488427191973 181586.58171633951133117, 524554.69743692653719336 181598.66184292820980772, 524669.10334167850669473 181744.33395767453475855, 524692.55299917422235012 181756.41408426326233894, 524751.53244075446855277 181674.69558086898177862, 524688.64472292503342032 181633.30338241058052517, 524641.74540793348569423 181580.71930196558241732, 524662.35268270247615874 181547.32130492618307471, 524660.22089565743226558 181540.92594379096408375, 524672.30102224613074213 181535.95177401913679205, 524799.49764926848001778 181620.51266014017164707, 524921.00951083737891167 181697.25699376262491569, 524922.43070220074150711 181707.20533330627949908, 524928.82606333598960191 181697.96758944430621341, 524901.8234274317510426 181673.80733626688015647, 525026.17767172737512738 181464.89220585022121668, 524920.29891515569761395 181419.41408222209429368, 524786.99264362745452672 181364.56044746178667992, 524835.49713539250660688 181262.62477866216795519, 524810.03188311751000583 181242.69948545226361603, 524652.8294552881270647 181191.18254679589881562, 524402.65496118809096515 181094.42998001689556986, 524304.52021488372702152 181022.55664469531620853, 524231.26470003672875464 180918.89318028924753889, 524209.14982763008447364 180870.5168968997313641, 524198.09239142679143697 180881.5743331030535046, 524164.92008281679591164 180965.88728415334480815, 524142.45342317444738001 180993.90335134317865595, 524123.2956079263240099 180993.85086294135544449, 524084.75367034279042855 180953.44766842460376211, 524118.6821531155728735 180877.17565803986508399, 524106.36578986316453665 180874.40456134342821315, 524049.16254756337730214 180876.73670476407278329, 524019.75422611943213269 180856.76255305705126375, 523997.69997150875860825 180847.04886512237135321, 523980.05357129260664806 180839.417857577878749, 523960.7030579368583858 180839.417857577878749, 523944.11690363183151931 180782.74849703587824479, 523930.29510837770067155 180767.54452225632849149, 523993.87536654679570347 180622.41567208780907094, 523990.55990376364206895 180643.74445799872046337, 524173.57321334740845487 180692.2783743524341844, 524192.01128995302133262 180618.89747461018851027, 524220.32912637857953086 180551.10990497015882283, 524220.5789011872257106 180534.90904957352904603, 524231.74438736715819687 180521.31105254049180076, 524218.06263667164603248 180517.35405082762008533, 524270.64104605483589694 180417.25284834808553569, 524303.3120032858569175 180383.15005364664830267, 524374.44817258138209581 180271.11154306019307114, 524456.19647553935647011 180149.77631248842226341, 524431.26476303639356047 180136.00103032620972954, 524459.56523167877458036 180144.27347500628093258, 524525.75418626563623548 180172.10854396742070094, 524641.63642226834781468 180229.18827888066880405, 524630.52720418258104473 180253.81709120800951496, 524616.84224711218848825 180281.94728074161685072, 524603.91244324017316103 180308.93155401269905269, 524598.58000010333489627 180313.8827607449493371, 524587.42772607307415456 180310.60648767265956849, 524592.46009993064217269 180317.89068621123442426, 524603.82116770057473332 180322.09606592508498579, 524614.00544641900341958 180322.34570301411440596, 524754.85509058670140803 180388.94884889174136333, 524708.14623816998209804 180493.35138344980077818, 524691.32313322799745947 180486.98523136778385378, 524705.02864181320182979 180499.13329579585115425, 524601.37547879898920655 180711.38724282311159186, 524596.0233205872355029 180713.76597980610677041, 524663.75182977877557278 180627.27976981503888965, 524868.74748395150527358 180735.9867015402414836, 524880.61112230643630028 180756.5456591853289865, 524875.5653715591179207 180764.13213197357254103, 524891.28976369893644005 180780.379913758370094, 524899.00831162196118385 180777.91579997690860182, 524896.38319139555096626 180788.82128840731456876, 524908.52099283307325095 180806.57090083844377659, 524918.36612558737397194 180815.52170617721276358, 524987.54607934912201017 180862.98865713539998978, 524898.15788384573534131 180986.02517464658012614, 524884.03555789380334318 181013.55537098314380273, 524928.2247080490924418 181024.21138646424515173, 524940.22894107585307211 181020.27645458056940697, 525054.89033654436934739 181049.24941641179611906, 524998.89522997406311333 181305.53165977715980262, 525260.98247081786394119 181375.88277569483034313, 525445.8561063768574968 181437.37408240092918277, 525452.05563839036040008 181443.14992468082346022, 525454.73027244885452092 181463.24714800907531753, 525525.30599382147192955 181466.04417678515892476, 525646.34203849150799215 181437.3191127959289588, 525749.25431174924597144 181463.62342599901603535, 525755.4399772712495178 181450.57309592515230179, 525777.37221961934119463 181420.22921704116743058, 525815.13287177938036621 181442.1180841151799541, 525815.54239428753498942 181442.27739287109579891)</t>
+  </si>
+  <si>
+    <t>LineString (525815.54239428753498942 181442.27739287109579891, 525938.4894992244662717 181490.10516775862197392, 525950.2033640209119767 181472.33594733368954621, 525943.13234854943584651 181373.34173073348938487, 525962.06789837975520641 181288.70267443344346248, 526084.9407700706506148 181347.92177145567256957, 526141.85119377286173403 181374.63645114144310355, 526247.90762806567363441 181264.37710280925966799, 526196.01242155989166349 181214.6880689833778888, 526166.16735107859130949 181192.64317541586933658, 526182.74869802431203425 181210.14127948944224045, 526289.24206442979630083 181085.57761354133253917, 526304.73383384314365685 181090.14411224401555955, 526312.97320597257930785 181086.63195823784917593, 526405.64829471055418253 180975.33631497254827991, 526406.50096082710660994 180959.79253581800730899, 526425.68278948625084013 180965.84515120310243219, 526594.1189202640671283 181126.22767907357774675, 526481.37747424189001322 181247.68218424991937354, 526436.7998225896153599 181292.98168183141387999, 526364.50886605237610638 181370.49790682113962248, 526315.65099693823140115 181327.24125062092207372, 526174.19306422164663672 181474.26841948175569996, 526118.98830004595220089 181451.55415104021085426, 526093.47386830300092697 181427.99858194089028984, 526147.53385363647248596 181372.97566176933469251, 526117.64916966739110649 181356.75464216282125562, 525896.63604345871135592 181252.18492163851624355, 525804.47871884633786976 181202.92109834335860796, 525674.52415049879346043 181177.43981043208623305, 525417.28142454475164413 181124.71832773357164115, 525450.65898510219994932 180968.90288878511637449, 525448.5728875674540177 180995.38028057347401045, 525580.7993774680653587 181023.62283181439852342, 525598.13003391132224351 180945.3139397373306565, 525607.75236547156237066 180908.16104843508219346, 525612.56353125174064189 180883.21426290841191076, 525623.07681943802163005 180835.94901390164159238, 525631.27362039673607796 180829.35593486961442977, 525630.06616769870743155 180815.88719046339974739, 525532.28454484208486974 180779.59350092764361762, 525501.02729750447906554 180764.22108420424046926, 525485.39867383567616343 180754.48522027939907275, 525448.1205632813507691 180741.67487300987704657, 525428.64883543166797608 180743.98073551838751882, 525274.54035777947865427 180702.73141731056966819, 525225.9229351548710838 180690.87681836728006601, 525208.01717880030628294 180709.67786253962549381, 525200.18341039516963065 180722.65953589673154056, 525163.92425377701874822 180720.42131635241094045, 525171.53420022781938314 180675.88074742027674802, 525177.80121495190542191 180667.82315706068766303, 525205.21940436994191259 180529.83692215289920568, 525202.53354091674555093 180499.39713635004591197, 525217.75343381811399013 180446.57515510389930569, 525265.20368815783876926 180455.52803328121080995, 525259.78516155341640115 180477.87945552368182689, 525268.52280582929961383 180452.9590315387758892, 525421.26921318552922457 180497.63403710661805235, 525446.30735667480621487 180398.85467028760467656, 525445.17935181641951203 180398.21167875776882283, 525420.12320177466608584 180383.9290343812899664, 525372.9962905184365809 180352.34950992788071744, 525364.52507656568195671 180327.99476981372572482, 525324.28681029006838799 180312.46421090036164969, 525076.87950780324172229 180213.18165121536003426, 525092.47997789632063359 180166.629184607823845, 525087.99899180571082979 180164.96956012982991524, 525131.2729772892780602 180055.01999166997848079, 525400.28327040141448379 180165.03473592712543905, 525457.11612049920950085 180186.51174571155570447, 525519.24511377036105841 180025.31955409917281941, 525538.98347847280092537 179972.22863600350683555, 525571.77124779403675348 179895.67673749651294202, 525617.60380089143291116 179797.21516905541648157, 525673.47756801324430853 179662.45056660982663743, 525613.02575635176617652 179620.2152606945601292, 525630.83745085913687944 179599.70482459513004869, 525606.00902821240015328 179617.51651910252985545, 525492.79681842681020498 179534.3952780679683201, 525517.08549275505356491 179489.05641932183061726, 525484.7005936506902799 179530.0772915207198821, 525429.82762361585628241 179495.93095825402997434, 525313.85690457350574434 179430.39389928575837985, 525309.06791018566582352 179437.57739086757646874, 525356.47895462566521019 179468.7058543887687847, 525353.60555799293797463 179482.35448839422315359, 525368.93034003407228738 179476.12879568999051116, 525425.4404738110024482 179506.29946033359738067, 525375.64614801947027445 179589.0921119402628392, 525370.77017299830913544 179596.45324670110130683, 525434.41614770900923759 179634.6992497275932692, 525421.80133750266395509 179659.47227550984825939, 525427.39915714180096984 179662.39022623706841841, 525471.61650676012504846 179597.89238431974081323, 525184.72663602349348366 179419.83259478391846642, 525208.6187529000453651 179388.72964811127167195, 525215.80224448186345398 179373.88376550885732286, 525148.79085531854070723 179337.39614326649461873, 525140.3769248811295256 179332.81476808225852437, 524984.62089585815556347 179676.87027474676142447, 524980.50617997418157756 179688.6684670404647477, 524951.26898805412929505 179685.32707367819966748, 524820.95464692520909011 179634.37082490339525975, 524810.93046683829743415 179609.31037468629074283, 524843.03832464327570051 179508.38986770567134954, 524807.60560298000928015 179485.20549427167861722, 524703.27592252695467323 179431.83769127260893583, 524617.75620542606338859 179575.09962145454483107, 524498.60092300793621689 179796.83555421329219826, 524464.29486135952174664 179922.3455358539649751, 524391.49907200783491135 180100.98807638921425678, 524197.37696707027498633 180024.84535419387975708, 524130.02899053593864664 180004.79501412331592292, 524164.57578076719073579 179943.56385594073799439, 524201.82267002947628498 179912.52478155549033545, 524273.21254111552843824 179881.48570717024267651, 524284.59353505680337548 179876.31252810603473336, 524445.73806290689390153 179568.50837378573487513, 524454.16972204064950347 179535.7185882649209816, 524373.44439292512834072 179453.58798262715572491, 524353.45823794102761894 179411.11740328592713922, 524346.40296634018886834 179381.5818728904123418, 524337.00973276444710791 179379.3654919343534857, 524274.6872111193370074 179445.0653559887141455, 524249.97718396421987563 179422.31644209986552596)</t>
+  </si>
+  <si>
+    <t>LineString (524249.97718396421987563 179422.31644209986552596, 524248.09063964674714953 179420.57962352185859345, 524231.20392760063987225 179398.62689786194823682, 524232.82265402289340273 179395.01589276641607285, 524385.38761930819600821 179221.87442430757801048, 524385.38761930819600821 179212.90917027732939459, 524438.18300415284465998 179156.12922808589064516, 524570.28329039399977773 179006.69620745387510397, 524700.98101851902902126 179091.39982051457627676, 524711.83193899260368198 179097.007949031481985, 524716.87237500911578536 179099.99616585933836177, 524718.76718895498197526 179092.8934059570892714, 524696.23571698309388012 179080.07131011568708345, 524678.74982980021741241 179058.15524498705053702, 524674.25436888239346445 179080.97733096149750054, 524709.50849799939896911 179105.50707113670068793, 525019.12328359950333834 179286.75246481280191801, 525126.9951293395133689 179333.83938160410616547, 525163.80853701278101653 179265.3493208167492412, 525215.17608260328415781 179142.92333715932909399, 525235.29503795958589762 179146.66888735865359195, 525236.12335093319416046 179146.99713273279485293, 525405.392016846453771 179214.0752280225569848, 525471.53291914879810065 179049.24790006288094446, 525514.57699842483270913 179075.49428986536804587, 525574.28753522550687194 179077.06907325351494364, 525574.28753522550687194 179051.87253904313547537, 525588.45396603550761938 179007.86059112328803167, 525591.26759051892440766 178988.16521973989438266, 525607.21146259119268507 178989.57203198154456913, 525588.32020733586978167 178982.91982687110430561, 525478.29455103096552193 178974.53093041834654287, 525357.75664400029927492 178938.75233156332978979, 525307.44793495535850525 178907.14925625239266083, 525106.8280279291793704 178791.05139943258836865, 525141.39902080979663879 178737.10666269203647971, 525174.15424077014904469 178734.65491616009967402, 525128.42563297669403255 178713.73651046739541925, 525133.77685303764883429 178695.25047752965474501, 525158.10058058728463948 178705.95291765150614083, 525190.20790095289703459 178651.46776794025208801, 525228.10579012299422175 178583.51367086486425251, 525201.60606543626636267 178566.21796919498592615, 525295.95426285627763718 178496.51634551520692185, 525326.84208016830962151 178536.51844553701812401, 525376.93699422583449632 178484.23081163188908249, 525324.76084575697313994 178418.86686161754187196, 525360.27136073401197791 178473.38879090908449143, 525431.60036567493807524 178549.65587991260690615, 525344.89456077455542982 178653.32112459669588134, 525439.16125242365524173 178700.23684167736792006, 525483.30881792632862926 178634.92763320647645742, 525530.49711275601293892 178590.84330049104755744, 525577.51932919700630009 178544.81350922945421189, 525597.16444525693077594 178525.40052273799665272, 525588.47622809757012874 178508.78139137243852019, 525604.47783662029542029 178512.66683010943233967, 525628.09064453258179128 178492.11954176213475876, 525659.47355236567091197 178452.53428301808889955, 525713.59123718016780913 178344.12060141284018755, 525732.49230667052324861 178352.32295232376782224, 525715.0922296498902142 178341.20492456736974418, 525745.51348978653550148 178292.14412009407533333, 525752.42284710763487965 178243.77861884664162062, 525830.72889674629550427 178141.28981858419138007, 525896.00242686306592077 178181.89303810551064089, 525949.38357987010385841 178108.33855643015704118, 526063.55754208331927657 177998.47304562115459703, 526240.20404965861234814 178164.34842468574061058, 526283.28856370132416487 178114.80123353656381369, 526385.55490465881302953 178199.05475307532469742, 526458.76830784429330379 178251.35004106492851861, 526375.67690581630449742 178464.30807493376778439, 526315.2467952505685389 178444.552077248779824, 526238.25651015469338745 178432.64037276225280948, 526149.93557932786643505 178441.93731284930254333, 526090.66758627293165773 178434.96460778400069103, 526034.88594575074966997 178408.235905033769086, 525976.78007020673248917 178517.4749510565015953, 525940.18563409615308046 178593.45575471699703485, 525837.99324970017187297 178546.41155678656650707, 525802.4071329872822389 178609.5827689859434031, 525711.1127249967539683 178737.73127572966041043, 525805.68154822511132807 178613.01432153128553182, 526021.35517114016693085 178721.26253662595991045, 526270.76997553906403482 178813.45403372519649565, 526143.33955579355824739 178767.74135057261446491, 526097.32672476547304541 178890.71894277923274785, 526093.0574930205475539 178933.8856193107785657, 526074.55748879280872643 178941.00100555224344134, 526093.58066659071482718 178941.13121456975932233, 526088.69760579953435808 178993.13581199539476074, 526211.31028287101071328 179003.57347023714100942, 526199.34856594784650952 179056.81849040847737342, 526206.62047603982500732 179066.37049779869266786, 526188.0618779466021806 179102.36209072399651632, 526167.3646381531143561 179197.54278659154078923, 526167.3646381531143561 179228.3240159587294329, 526167.7310813597869128 179308.57507823742344044, 526167.11127823567949235 179411.66888013994321227, 526089.31039173016324639 179406.55787299721851014, 526074.16666686290409416 179647.34309838674380444, 526071.96742292866110802 179673.52631873372592963, 526121.07215822767466307 179661.16662345439544879, 526116.72956258896738291 179684.54983073959010653, 526120.07002077263314277 179690.89670128843863495, 525859.68130536109674722 180557.24453120492398739, 525846.31947262666653842 180594.65766286122379825, 525879.7240544626256451 180598.66621268156450242, 525882.55008484877180308 180599.07834211288718507)</t>
+  </si>
+  <si>
+    <t>LineString (525882.55008484877180308 180599.07834211288718507, 526144.10206235200166702 180628.87880492309341207, 526211.97706139634829015 180640.08887598145520315, 526394.68412689818069339 180685.65199389134068042, 526375.25024652888532728 180751.41157924372237176, 526543.08072616113349795 180799.48524305276805535, 526566.20990454801358283 180735.24582871556049213, 526773.2086006454192102 180792.2867543384199962, 526781.81037810200359672 180804.0292009754339233, 526876.82089265179820359 180898.32528518006438389, 526893.50918447971343994 180930.32612565089948475, 526924.34248529304750264 180944.76673002715688199, 526972.18770328722894192 180987.68083861388731748, 526822.07183925563003868 181156.94281222127028741, 526922.36106670461595058 181052.43190333811799064, 527056.51731256174389273 181181.75928882521111518, 527072.0604500574991107 181194.33582109218696132, 527105.36620856204535812 181208.59860649338224903, 527134.84456199198029935 181207.65720116312149912, 527141.67895267263520509 181237.20603345840936527, 527126.8461934340884909 181257.45282692171167582, 527004.39505052170716226 181384.53058732440695167, 526985.91159781138412654 181369.18001979179098271, 526928.28958167461678386 181432.30053406039951369, 526997.63798668433446437 181498.45083301386330277, 526991.12956032424699515 181511.24325723896618001, 526678.53803907369729131 181414.39224837144138291, 526667.31783640081994236 181399.6772284725739155, 526656.64944697415921837 181395.44666025164769962, 526645.98105754749849439 181403.90779669350013137, 526619.08016179490368813 181431.82035006419755518, 526630.85217771399766207 181442.85661498832632788, 526625.70192074938677251 181459.04313687709509395, 526679.9176372914807871 181475.29189143585972488, 526705.68373186374083161 181482.08222587691852823, 526706.45631411974318326 181479.08550615585409105, 526686.25770194770302624 181472.89795374975074083, 526671.31848243589047343 181522.68559793970780447, 526666.90397646627388895 181521.94984694477170706, 526673.52573542075697333 181504.29182306613074616, 526671.31848243589047343 181502.8203210762294475, 526664.32884798396844417 181521.58197144727455452, 526672.42210892832372338 181534.0897383613337297, 526664.69672348140738904 181552.11563773744273931, 526615.76928231760393828 181537.7684933360433206, 526607.67602137324865907 181540.71149731581681408, 526667.6397274611517787 181562.3241827923047822, 526633.05943069886416197 181671.21533004395314492, 526634.16305719129741192 181721.7062420719594229, 526742.32487509062048048 181719.08851347386371344, 526749.72303723508957773 181718.96316810802090913, 526747.44774530804716051 181725.1558509673923254, 526745.80791060253977776 181720.21680638659745455, 526614.1888072743313387 181722.68839901124010794, 526608.25850433309096843 181744.71523850716766901, 526605.99934130790643394 181752.33991371729644015, 526446.30086804460734129 181920.76268879341660067, 526376.42578245303593576 181996.86867373716086149, 526253.96636714844498783 181892.34601317506167106, 526219.61745367909315974 181921.09456031789886765, 526171.9210004648193717 181960.76382179747452028, 526080.54168990370817482 182039.16895036882488057, 526092.26835894433315843 182054.09146642521955073, 526106.13131886860355735 182090.02748875319957733, 526381.77541522704996169 182309.68137803877471015, 526390.42294119927100837 182322.36665932871983387, 526288.06584389437921345 182450.834574355132645, 526191.83267548796720803 182572.23641757547738962, 526248.36124993639532477 182619.61274663705262356, 526103.13665034133009613 182779.77704090779297985, 526036.37909575458616018 182871.56867846462409943, 526166.79859251785092056 182977.49245963362045586, 526362.76431727269664407 182717.9993845462158788, 526568.42065479012671858 182878.4328625048219692, 526567.34392003866378218 182903.1977617870143149, 526584.30249237327370793 182884.75867916931747459, 526641.10025050956755877 182928.09725291316863149, 526696.1483146749669686 183016.25491068401606753, 526738.14096997957676649 183080.85899576800875366, 526799.24566712148953229 183168.34369431925006211, 526821.85709690093062818 183181.26451133604859933, 526845.63949992938432842 183154.3195547133218497, 526846.27791611000429839 183154.20463980082422495, 526851.96460711781401187 183153.18103541940217838, 527089.65806536294985563 182846.11161946220090613, 527159.99787061079405248 182839.75561296389787458, 527206.71119945566169918 182882.25472003052709624, 527209.41581725038122386 182908.01976323217968456, 527213.6862663998035714 182915.9912683111615479, 527203.90023362345527858 182922.97789460717467591, 527163.95716502459254116 182973.89433370024198666, 527185.46497119322884828 183029.63905581075232476, 527126.6477053442504257 183105.13584481080761179, 527112.16285629197955132 183116.54815012478502467, 527123.57516160595696419 183143.7621089503809344, 527053.78452526277396828 183235.06055146208382212, 527149.31445503246504813 183306.12010162867954932, 527157.71220760734286159 183299.49029696427169256, 527157.7350565199740231 183299.47225834906566888, 527372.2451753921341151 183478.31646749860374257, 527603.46507797553204 183601.90996593536692671, 527662.58712028060108423 183506.32227007864275947, 527655.90415950608439744 183492.21379733242793009)</t>
+  </si>
+  <si>
+    <t>LineString (527655.90415950608439744 183492.21379733242793009, 527654.68629352480638772 183489.6427469274494797, 527558.99850281549151987 183445.7492649506602902, 527464.80590493814088404 183378.65690534905297682, 527529.78861410322133452 183281.50301839754683897, 527962.42357370757963508 183483.62205357951461338, 527973.56080347381066531 183488.82516092201694846, 528248.28510450641624629 183588.52026548737194389, 528303.09698454267345369 183598.97112996794749051, 528344.76732492458540946 183589.8908444368862547, 528360.00343477982096374 183621.74180270021315664, 528384.43865157361142337 183633.31768803694285452, 528392.23448110034223646 183625.76139408763265237, 528384.47060682089067996 183632.05436160630779341, 528361.53645626234356314 183620.09746778081171215, 528348.20271571911871433 183580.91116915637394413, 528292.58456641039811075 183591.77239997015567496, 528257.98622214375063777 183557.36140638464712538, 528521.85076717485208064 182678.38405832633725367, 528341.94312283548060805 182630.40868650248739868, 528329.949279879569076 182503.61663239658810198, 528247.70578532433137298 182419.65973170485813171, 528153.46844781318213791 182414.51951329517760314, 528153.46844781318213791 182339.12964328628731892, 528192.87678895425051451 182330.56261260344763286, 528194.59019509085919708 182289.44086532585788518, 528239.13875464152079076 182184.92309099534759298, 528055.80429802893195301 182126.66728235210757703, 527857.0491861873306334 182243.17889963858760893, 527835.18695252947509289 182239.66741698305122554, 527838.772610142827034 182227.64257323095807806, 527823.08229359821416438 182224.95575459097744897, 527811.03382629505358636 182221.05085970158688724, 527781.70427009277045727 182243.19124876931891777, 527668.77023004030343145 182337.87599429336842149, 527639.32060709642246366 182349.04721267713466659, 527584.9030367435188964 182332.47174584548338316, 527408.28049158933572471 182270.47011755546554923, 527357.30311246565543115 182249.0471085372264497, 527366.05996286729350686 182222.77655733237043023, 527350.84845480835065246 182220.83466268656775355, 527361.52887536038178951 182227.30764483928214759, 527348.90656016254797578 182272.61851990822469816, 527335.63694674952421337 182287.83002796708024107, 527307.47947438526898623 182274.23676544640329666, 527292.26796632644254714 182256.1124154188146349, 527242.83056513511110097 182307.89627264047157951, 527172.35597194754518569 182242.92371428263140842, 526900.49072153388988227 182418.98882883627084084, 526755.78376343683339655 182547.31084604043280706, 526721.96971074212342501 182518.14893207367276773, 526721.42847167002037168 182510.27474968624301255, 526639.36008041724562645 182453.71151223586639389, 526728.61123994365334511 182341.94567091023782268, 526635.31149883137550205 182260.91681474831420928, 526629.98235425702296197 182258.85755792172858492, 526577.14322044944856316 182220.11298631975660101, 526583.50453914981335402 182213.9761393434018828, 526612.02737233357038349 182233.3108826142270118, 526628.28531093138735741 182249.45831946312682703, 526730.51656499120872468 182139.8360750732535962, 526693.837565878755413 182097.80319830903317779, 526684.65127594629302621 182088.79316362290410325, 526699.03030984883662313 182072.19530309486435726, 526716.57443575479555875 182074.75238155253464356, 526722.84627124748658389 182066.73337691847700626, 526798.51334596984088421 181991.13818491756683215, 526866.75974808703176677 182069.62223492347402498, 526882.31688596680760384 182087.82361979689449072, 526934.9228784617735073 182045.90755342398188077, 526939.83839354338124394 182039.90649309137370437, 526939.83839354338124394 182025.22802654595579952, 526953.29365454334765673 182027.91907874596654437, 527063.01316396985203028 181911.23626593552762643, 527121.54787396104075015 181813.50358696334296837, 527023.0907087258528918 181748.39970547880511731, 527054.7895969923119992 181712.22981796885142103, 527075.97658408165443689 181714.24235780647723004, 527080.78246395441237837 181701.94142769221798517, 527079.6564745232462883 181686.00343252817401662, 527105.82488133199512959 181658.69750754616688937, 527442.20734915044158697 181314.52695137952105142, 527459.12822526623494923 181326.29444383695954457, 527468.89448804350104183 181332.78180451109074056, 527419.56431302148848772 181385.23810306136147119, 527473.52474095020443201 181423.3884920031123329, 527541.4968345935922116 181469.99792764431913383, 527513.48277443449478596 181503.55932644888525829, 527548.78461593028623611 181469.69239985276362859, 527597.29704240849241614 181303.15504638879792765, 527520.45864899968728423 181278.72603273176355287, 527493.44284569495357573 181267.15421134524513036, 527387.01661669730674475 181170.06974426365923136, 527429.41461164352949709 181120.02025737526128069, 527508.38860920432489365 181143.15408535901224241, 527552.0115922475233674 181044.38326500484254211, 527617.38904907600954175 181065.27134975808439776, 527665.90049312810879201 181080.65138910515815951, 527891.34266930283047259 181143.2742158203618601, 527899.13187455991283059 181119.94490523042622954, 527904.33462368953041732 181097.01015329896472394, 527820.96005753811914474 181078.33706724832882173, 527844.18837801553308964 181002.66209630461526103, 527853.80389859748538584 180991.36529486137442291, 527884.2926319494144991 180989.82570853206561878, 527897.81294143584091216 180972.85507457796484232, 527908.1319633579114452 180946.21514748636400327, 527918.58895030023995787 180920.68108835321618244, 527941.45521559938788414 180855.90905671450309455, 527959.02194552542641759 180867.80684457015013322, 527979.60677813622169197 180868.6474805666366592, 528095.75816618301905692 180907.32333309669047594, 528218.68883095902856439 180948.86776828416623175, 528232.99101356463506818 180949.5488245987216942, 528249.33636511373333633 180901.53435442302725278, 528274.28005263407249004 180832.49227053558570333, 528413.89659711671993136 180874.71776203761692159, 528440.4577933840919286 180872.67459309397963807, 528441.88889231265056878 180868.47956919606076553, 528480.12932370661292225 180756.38422738478402607, 528315.31369558570440859 180703.26183484998182394, 528079.46642620186321437 180632.41520988091360778)</t>
+  </si>
+  <si>
+    <t>LineString (528533.86825586541090161 179825.01659448479767889, 528599.09828376933000982 179804.26158560626208782, 529067.56848417001310736 179787.9540786303114146, 529126.86850953719113022 179829.46409638732438907, 529184.68603427021298558 179833.91159828985109925, 529236.57355646649375558 179804.26158560626208782, 529461.54302770318463445 179967.33665536600165069, 529365.1804864815203473 180130.41172512577031739, 529332.56547252961900085 180117.06921941813197918, 529176.88434407091699541 180335.52529085575952195, 528968.42684971622657031 180655.33458768369746394, 528933.41540621093008667 180638.92297354058246128, 528917.00379206787329167 180629.07600505475420505, 528956.39166601130273193 180565.6177637014479842, 528889.09824919363018125 180520.36887541532632895, 529037.60859426553361118 180322.19037864034180529, 528980.81174594059120864 180277.24678561804466881, 528985.75060231669340283 180264.89964467784739099, 528967.47683372523169965 180262.43021648982539773, 528869.68747747887391597 180180.56867205633898266, 528753.13046700344420969 180299.10122508218046278, 528749.46897789079230279 180304.32965189014794305, 528768.29435105295851827 180318.41158448159694672, 528778.68045006087049842 180329.09107490163296461, 528777.89595665864180773 180339.10883718938566744, 528786.29993801447562873 180331.19731133786262944, 528766.49707728379871696 180311.67933983076363802, 528735.71864135982468724 180290.81664662051480263, 528713.38623358681797981 180285.77175626676762477, 528668.77996420615818352 180275.46013541670981795, 528678.81986454653088003 180236.4348891912959516, 528685.54394682915881276 180209.20438540610484779, 528648.68728152720723301 180200.38155767129501328, 528657.51626427297014743 180164.64456824841909111, 528561.08355491538532078 180139.08601459197234362, 528473.16496016969904304 180096.57592482483596541, 528471.71575256390497088 180078.58159705405705608, 528455.77446890133433044 180078.09852785218390636, 528452.87605368986260146 180092.59060390916420147, 528456.2575381031492725 180107.5657491680176463, 528445.63001566135790199 180136.06683208007598296, 528434.51942401775158942 180130.75307085920940153, 528435.00249321956653148 180119.15941001361352392, 528434.03635481582023203 180138.48217808958725072, 528458.18981491075828671 180158.28801536746323109, 528508.42901190835982561 180176.64464503963245079, 528492.97079744748771191 180232.19760325804236345, 528463.50357613165397197 180225.43463443146902137, 528442.73160045000258833 180280.1422215465863701, 528368.29083982005249709 180530.61085074103903025, 528399.42485451779793948 180540.37256290816003457, 528373.18561336421407759 180528.66321234643692151, 528398.20391442335676402 180451.73774791724281386, 528402.87839129334315658 180453.56406502836034633, 528495.6276780579937622 180483.51435554612544365, 528631.8531929935561493 180596.55254879055428319, 528664.70189872267656028 180554.04245902341790497, 528713.73342271556612104 180597.76022179532446899, 528701.17362346616573632 180617.08298987129819579, 528701.17362346616573632 180635.4396195434674155, 528716.6318379269214347 180666.35604846503701992, 528751.41282046365085989 180679.88198611821280792, 528786.19380300038028508 180647.03328038906329311, 528882.80764338024891913 180721.42593748154467903, 528908.89338028279598802 180749.44395119170076214, 528941.25901681010145694 180770.21592687338124961, 528984.08419391023926437 180821.70737133437069133, 528974.05492355371825397 180859.35868258221307769, 528989.1841545554343611 180829.86192138504702598, 529040.11857240251265466 180898.90430847753304988, 529064.22407606989145279 180876.05281915218802169, 529116.11744003393687308 180788.13860499695874751, 529191.0602760020410642 180677.82465982373105362, 529192.20589897234458476 180667.51405309184337966, 529243.27595739718526602 180675.42673247310449369, 529253.40125929773785174 180655.48501190464594401, 529245.96676619641948491 180680.13564787179348059, 529287.00160038517788053 180692.91698966833064333, 529105.37200643471442163 181014.1322900807717815, 529080.35383750754408538 181057.74321855726884678, 529150.25737489317543805 181094.96458261978114024, 529105.31938657385762781 181161.35024718247586861, 529063.5588317719521001 181143.64740329908090644, 529046.76382603647653013 181133.20726459860452451, 529038.72230120946187526 181129.90637958364095539, 529016.40501055552158505 181225.42438358269282617, 528860.85349469736684114 181191.94844760172418319, 528730.96686309122014791 181161.59693231229903176, 528681.95751262735575438 181150.4457873418868985, 528719.83069236215669662 181094.50466865097405389, 528670.49132059747353196 181063.23323584237368777, 528656.24544565135147423 181091.03006500555784442, 528636.09274450805969536 181115.69975088789942674, 528619.76210737472865731 181137.24229348936933093, 528607.94845498027279973 181141.41181786387460306, 528598.91448550228960812 181161.91197937171091326, 528542.97336681128945202 181222.54381298396037892, 528630.5333786754636094 181247.56095923084649257, 528643.38941216340754181 181213.50984350591897964, 528660.41497002588585019 181220.80651116126682609, 528688.33952496037818491 181230.55820254873833619, 528679.86120436212513596 181260.31371245899936184, 528667.46310047351289541 181267.8903315020725131, 528633.75722163496538997 181366.41482741927029565, 528463.70207082328852266 181314.08507524349261075, 528428.78978234506212175 181348.55440134933451191, 528409.40016961458604783 181407.56676936079747975, 528378.71507131354883313 181399.79127068642992526, 528367.57113712374120951 181397.15591765905264765, 528327.16320699045900255 181385.98296514025423676, 528308.22175984270870686 181356.13857025865581818, 528284.80718849156983197 181340.66114173838286661, 528256.63033144187647849 181343.0422845876601059, 528236.78747436462435871 181362.88514166491222568, 528124.47690330736804754 181327.56485606741625816, 528100.04183234507218003 181315.23161206592340022, 528077.21998848498333246 181309.38646938232704997, 528120.39353655825834721 181328.79462172722560354, 528099.23992964578792453 181396.49718135065631941, 528083.2094619075069204 181447.06752287576091476, 527892.05577444343362004 181391.53930473059881479, 527886.54702264338266104 181381.62355149036739022, 527894.36945019953418523 181395.8361311347107403, 528096.21011615579482168 181454.44925028792931698, 528174.43439171742647886 181477.365657776419539, 528210.57180352613795549 181486.17966065660584718, 528186.33329560561105609 181562.09026046219514683, 528058.53025384293869138 181521.54584721333230846, 528025.91844318632502109 181610.126576159207616, 528008.71294296334963292 181668.53094684361713007, 528092.33064007223583758 181691.78074555195053108, 528060.10723484493792057 181786.81939641226199456, 528111.16470766742713749 181801.12569479394005612, 528229.73017954116221517 181814.84780309765483253, 528238.68286890105810016 181821.33241880481364205, 528233.97450602473691106 181880.77550011838320643, 528312.01526012923568487 181886.28911337567842565, 528336.83830706239677966 181958.7224278392677661, 528346.83872474473901093 181961.95785708940820768)</t>
+  </si>
+  <si>
+    <t>LineString (528346.83872474473901093 181961.95785708940820768, 528351.42447949468623847 181963.4414836261421442, 528343.88806465221568942 181967.13308218619204126, 528356.90300176513846964 182021.63313134637428448, 528360.15673604339826852 182079.38691478478722274, 528255.16213896812405437 182063.02837978929164819, 528103.70979977981187403 182011.23638814975856803, 527993.06327218632213771 181982.20148374579730444, 528054.27198957849759609 181792.29751440085237846, 528047.20944526395760477 181784.45024294030736201, 527955.99687798251397908 181751.91292813932523131, 527952.44751808664295822 181758.68897884970647283, 527941.10340294241905212 181748.7705221853684634, 527752.98447521112393588 181691.77686399561935104, 527549.82001883175689727 181624.62000102378078736, 527503.58740099950227886 181751.36114301218185574, 527479.05319745594169945 181810.98149478450068273, 527449.22437855799216777 181845.582924706133781, 527393.44448721886146814 181959.82730108534451574, 527344.62620919058099389 181935.31162831617984921, 527346.5051257333252579 181939.60629469942068681, 527396.22930995177011937 181966.38085543247871101, 527419.84997505962383002 181915.38169213145738468, 527486.41730399988591671 181949.20218989948625676, 527482.96182583621703088 181958.41679833593661897, 527528.6399562283186242 181968.15795582588179968, 527569.11841471691150218 181981.09131695271935314, 527585.04652358556631953 181978.72184621190535836, 527591.99038922868203372 181992.01720981305697933, 527591.46384017518721521 181998.99398477206705138, 527600.46228416555095464 181983.46020101421163417, 527671.37066017126198858 182008.93864325288450345, 527672.00585366494487971 182009.53293042359291576, 527672.91207058762665838 182009.79258584204944782, 527742.12486925080884248 182029.11416199523955584, 527811.41948285070247948 182045.82072442839853466, 527815.11899438232649118 182051.27116669819224626, 527820.06026732875034213 182037.87445605464745313, 527847.26226369361393154 181951.43140346015570685, 527927.21323233155999333 181975.30975012294948101, 528269.95467810390982777 182084.54117023901198991, 528507.92312907101586461 182120.20857272588182241, 528831.99491885420866311 182222.19505171180935577, 528823.07806823251303285 182344.80174776044441387, 528847.59940744226332754 182369.32308697016560473, 528823.07806823251303285 182398.30285149076371454, 528816.39043026615399867 182670.266795453208033, 528800.78594167821574956 182841.91616992131457664, 528606.84444065578281879 183463.86650078624370508, 528658.11633173062000424 183599.84847276745131239, 528633.59499252098612487 183633.28666259889723733, 528604.24853495263960212 183671.01782232944970019, 528627.80092093267012388 183660.77765451229061, 528647.1594083410454914 183636.01462974661262706, 528664.55382729053962976 183620.91758688475238159, 528702.78872932109516114 183664.2395359665970318, 528761.45386870275251567 183741.77597892552148551, 528769.94595531257800758 183759.78576646986766718, 528818.92929546756204218 183815.98943147188401781, 528876.9750076774507761 183846.2940231827669777, 528923.7981087981024757 183868.95036243469803594, 528962.26051460986491293 183871.43938000165508129, 528970.91118134488351643 183879.29152365346089937, 528993.43618665123358369 183886.51150319766020402, 529035.75791006267536432 183811.45033337359200232, 528956.97029918350744992 183772.32270229508867487, 528928.22346818703226745 183829.55018992690020241, 528922.63380660430993885 183889.97176989167928696, 528941.92318019969388843 184098.53460018764599226, 528863.38120412628632039 184095.51375495406682603, 528708.33693763334304094 184000.71587241004453972, 528724.42232338106259704 183964.10698729282012209, 528701.76598412916064262 184001.86755271273432299, 528789.37049590330570936 184060.77403476776089519, 528689.63087926781736314 184162.2935707290598657, 528691.49826807086355984 184184.03894319324172102, 528710.63466808956582099 184213.17846140338224359, 528791.45426438504364341 184306.83684223380987532, 528956.13032546907197684 184285.44605525681981817, 529003.7386343190446496 184310.71759315161034465, 529085.40256406948901713 184166.4398523555137217, 529106.88706586312036961 184179.02949331066338345, 529160.12714608758687973 184168.68103781942045316, 529164.48439050489105284 184164.86844895425019786, 529180.99500393983907998 184154.38365939242066815, 529137.3034288139315322 184069.37328925836482085, 529098.63988687307573855 184040.28537339897593483, 529197.46968787396326661 183851.66075099032605067, 529231.8759383208816871 183807.63561239538830705, 529366.40293027937877923 183902.40006897028069943, 529470.80148133041802794 183700.60958103262237273, 529532.41350877098739147 183585.44640055124182254, 529538.36414308042731136 183573.78315730480244383, 529529.43819161620922387 183570.68882746392046101, 529518.60803717316593975 183578.90070281090447679, 529450.281529710162431 183705.0832505801517982, 529321.97175762639380991 183640.23852705396711826, 529418.54900543135590851 183463.64013106780475937, 529410.27095561951864511 183361.54418338829418644, 529378.53843134071212262 183277.38401030114619061, 529300.0293472099583596 183204.18649908609222621, 529248.55052252893801779 183171.68790031166281551, 529171.72482365590985864 183152.15465962985763326, 529162.35992088436614722 183162.69077780697261915, 529164.55778478819411248 183210.37992642441531643, 529162.58233259071130306 183288.01632287859683856, 529163.35543786408379674 183347.00887900387169793, 529165.64832443615887314 183368.61479538556886837, 529209.96307325642555952 183366.53984011086868122, 529238.56352939270436764 183320.99361840856727213, 529307.53664107876829803 183228.71848092431901023, 529332.4133849231293425 183210.28397338639479131, 529655.02802976139355451 182747.87247683008899912)</t>
+  </si>
+  <si>
+    <t>LineString (529655.02802976139355451 182747.87247683008899912, 529725.18133759195916355 182647.32001716547529213, 529758.11947344534564763 182602.45964416163042188, 529772.86156971787568182 182573.57162642496405169, 529786.14614357193931937 182535.41119721299037337, 529721.72104365052655339 182498.97087032342096791, 529662.05603224551305175 182458.96742579058627598, 529465.69317875348497182 182347.95250755702727474, 529447.2254714909940958 182321.03347663194290362, 529485.62160862435121089 182274.29035316518275067, 529327.0288682907121256 182182.47350349830230698, 529281.95514209056273103 182262.60457229847088456, 529271.27928321424406022 182255.78608057467499748, 529184.98289716511499137 182225.79025960189756006, 529254.93800170661415905 182123.0347249869373627, 529194.03950407542288303 182072.44127056252909824, 529292.80413319286890328 181924.86280826764414087, 529215.98652011051308364 181870.62796054553473368, 529193.31721052876673639 181845.4344820223050192, 529136.51610650331713259 181827.80988931999308988, 529055.08064286154694855 181793.40041071106679738, 529048.18442968558520079 181784.34046519559342414, 529038.80868799472227693 181788.7224668295821175, 529002.77593848691321909 181776.43501262343488634, 529014.08187095657922328 181735.5730537639465183, 529044.40527507243677974 181648.47109775303397328, 529115.73285259760450572 181668.03016941447276622, 529137.29936532687861472 181681.75431387854041532, 529179.25603554560802877 181720.57403679116396233, 529160.24231672799214721 181743.47910360060632229, 529140.96079503151122481 181821.17043695540633053, 528996.20386221027001739 181782.66523825988406315, 528957.45751267555169761 181764.97831311973277479, 528992.17077459231950343 181659.57102250630850904, 529022.32355210115201771 181563.27666852626134641, 528964.93600781005807221 181545.76860416625277139, 528936.72857078560627997 181511.7251456884550862, 528878.36835625220555812 181539.93258271290687844, 528856.96961092331912369 181541.87792319734580815, 528842.37955728999804705 181597.32012700402992778, 528805.67882148048374802 181719.06924707361031324, 528596.42409515334293246 181654.20028191219898872, 528551.78308687021490186 181642.34251408698037267, 528507.37306858669035137 181777.43956236285157502, 528766.16571141825988889 181854.68164780738879927, 528777.9935695423046127 181857.12154139997437596, 528783.85590929095633328 181838.53742159798275679, 528772.98604363994672894 181835.13982246746309102, 528765.42155704949982464 181856.89868191126151942, 528912.88206116098444909 181899.58461731197894551, 528933.9016505628824234 181842.99341507619828917, 528977.55772085906937718 181853.66489892636309378, 528886.68841898324899375 182145.02874586603138596, 528881.19098790897987783 182154.40671652223682031, 528855.96748062665574253 182141.14820628412417136, 528840.44532229914329946 182149.23266374639933929, 528839.79856570216361433 182207.44075747462920845, 528841.09207889623939991 182274.70344356057466939, 528907.70800838526338339 182267.58912099379813299, 528901.34845087071880698 182218.96412019734270871, 528914.49795431364327669 182199.37284149171318859, 528944.79199275141581893 182201.06235859365551732, 529116.82618026225827634 182275.25592555687762797, 529236.03349617577623576 182330.91525820962851867, 529228.61333048343658447 182366.16104524824186228, 529249.75958250637631863 182377.47901842225110158, 529260.6965834874426946 182345.48021171212894842, 529391.5315474170492962 182398.66071800183271989, 529324.89775743579957634 182506.92984195848111995, 529307.95238226593937725 182527.55765377206262201, 529395.9228944230126217 182579.30535354110179469, 529313.15534203872084618 182528.16323932801606134, 529338.0299911656184122 182494.00108638301026076, 529401.06366170477122068 182399.72070142376469448, 529437.38091082300525159 182410.7247426172834821, 529515.77390267443843186 182460.22066143920528702, 529694.98193959216587245 182559.66469046362908557, 529753.83678528945893049 182587.3854519649175927, 529779.14153369213454425 182575.72735903057036921, 529858.90584623115137219 182464.89736771275056526, 529886.78703951300121844 182424.94217844444210641, 529760.35582555131986737 182335.00857195170829073, 529745.32829435018356889 182335.50571294111432508, 529754.22227583988569677 182333.09009388764388859, 529844.24740195064805448 182214.70289386285003275, 529902.10613867023494095 182253.63458346226252615, 529904.80511579709127545 182251.14619939160184003, 529941.11181005125399679 182198.01181227143388242, 529940.89537670253776014 182188.48874492605682462, 529972.6108493892243132 182165.00088953139493242, 530056.9588389479322359 182048.7881039172061719, 529981.98284822911955416 181992.5561108780966606, 529951.05525205750018358 182016.92330786169623025, 529819.2849761457182467 181928.86637559026712552, 529799.05698917480185628 181958.56732936628395692, 529803.05725013604387641 181964.66939977870788425, 529801.62453686981461942 181960.81469362112693489, 529828.71775786660145968 181919.54642597923520952, 529924.09649344824720174 181787.99958944245008752, 529857.85091200319584459 181729.57684998650802299, 529698.32181283622048795 181616.30609073047526181, 529685.48704050190281123 181617.03950629243627191, 529635.51744967524427921 181690.38779020583024248, 529688.40668625489342958 181726.48536033323034644, 529692.63985970325302333 181722.80896518367808312, 529644.80728511966299266 181691.31286854337668046, 529645.71116362931206822 181681.09080057707615197, 529586.96591395325958729 181646.48816596489632502, 529515.04247384704649448 181599.24059515440603718, 529543.51227790850680321 181551.4553936262964271, 529539.00726222933735698 181538.53999719221610576, 529525.71878347580786794 181533.37225545474211685, 529491.7593377724988386 181561.79483501086360775, 529437.12892511917743832 181617.90174530341755599, 529480.68560547789093107 181649.27732013809145428, 529452.0052509990055114 181692.96711596235400066, 529415.66898023779504001 181743.18504027591552585, 529422.12033342942595482 181756.496664849226363, 529410.79081194649916142 181745.6821476363693364, 529411.79279640805907547 181742.27344958332832903, 529417.83336036605760455 181734.97711012425133958, 529445.56671970279421657 181695.34609987842850387, 529414.95451968535780907 181675.21360844530863687, 529316.29792853817343712 181612.14346808032132685, 529210.36666346830315888 181540.84275432795402594, 529292.45281272125430405 181467.24829591458546929, 529338.54938403982669115 181401.53055816600681283, 529381.24053801142144948 181306.35028045883518644, 529665.55224183772224933 181363.5063766969833523, 529664.71503826801199466 181384.86775368836242706, 529672.3439009505091235 181401.4207107936963439, 529766.81024347490165383 181438.92780598934041336, 529794.06817890249658376 181452.26089733641128987, 529984.75397409894503653 181524.94074914953671396, 529992.18142025219276547 181529.49952054413734004, 529997.79784449038561434 181531.55623927924898453)</t>
+  </si>
+  <si>
+    <t>[-2] Final dock visited by all.</t>
+  </si>
+  <si>
+    <t>LineString (528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526692.80084780836477876 179647.72075017780298367, 526544.65379679470788687 179640.67684462433680892, 526514.23908054397907108 179631.71659103041747585, 526459.01828505133744329 179636.29050092305988073, 526411.9174515149788931 179628.55661391041940078, 526397.78921595867723227 179626.15454808797221631, 526395.30093265138566494 179643.52499421581160277, 526402.44541665085125715 179662.16024893836583942, 526431.23864846909418702 179657.35777275226428173, 526403.68164814496412873 179659.45682299701729789, 526399.58064635645132512 179645.06697337637888268, 526397.66759617673233151 179639.57072356637218036, 526399.69519630237482488 179630.99646285979542881, 526407.86559560417663306 179609.58792857639491558, 526407.1355080088833347 179595.46081518297432922, 526405.31812318519223481 179578.4985568281263113, 526414.70794477441813797 179560.47615732613485307, 526438.29747225344181061 179421.98284034681273624, 526447.2566591496579349 179400.3794134950148873, 526443.27324291132390499 179425.80230685905553401, 526661.83190965442918241 179456.92559352092212066, 526673.60955778870265931 179451.2058947991754394, 526704.50509979214984924 179464.53338350655394606, 526797.19172580249141902 179477.86087221393245272, 526803.85547015618067235 179464.53338350655394606, 526815.97136898105964065 179467.18373637451441027, 526825.3611905702855438 179410.5419093681848608, 526856.86252751504071057 179206.38901416890439577, 526873.82478586991783231 179087.65320568502647802, 526866.85814404557459056 179082.8068461550574284, 526876.24796563480049372 179074.02281950702308677, 526883.21460745914373547 179027.98240397247718647, 526875.03637575230095536 179024.65053179563255981, 526886.56871603394392878 178986.79712720314273611, 526902.37576597684528679 178869.52358519978588447, 526856.64449148019775748 178854.26221120113041252, 526815.01278510922566056 178840.01978533738292754, 526811.13741514587309211 178827.26046769024105743, 526810.19336951395962387 178822.06821671460056677, 526763.22709932515863329 178814.75186306712566875, 526748.59439203015062958 178818.29203418685938232, 526534.17802787688560784 178780.17619179750909097, 526556.36310022731777281 178626.76877660810714588, 526549.1273886983981356 178624.33518190018367022, 526544.750046381726861 178654.78625888586975634, 526525.05200595653150231 178786.96296492687542923, 526529.61966750444844365 178803.71105726901441813, 526515.91668286081403494 178835.68468810399645008, 526497.6460366693791002 178969.6694268410501536, 526535.70988290151581168 178952.9213344989111647, 526864.20087588473688811 179005.0688038369116839, 526904.39858746575191617 179011.78256420639809221, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527770.03632687916979194 179164.03159300866536796, 527739.41564339946489781 179158.49662950204219669, 527737.28947808116208762 179153.9753308377112262, 527736.19962250639218837 179161.69230536534450948, 527771.59785052062943578 179169.64108689734712243, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528282.42500657623168081 179806.61658668008749373, 528307.96808183658868074 179740.1390959385316819, 528324.99679867678787559 179729.00493492765235715, 528282.03859719191677868 179662.78071852284483612, 528265.95217516226693988 179622.08936450752662495, 528267.10970970639027655 179566.52770638960646465, 528306.18395167891867459 179499.6337649634515401, 528343.33046841598115861 179469.3338732514239382, 528348.40521787817124277 179448.48920341735356487, 528386.22882526856847107 179444.91777596104657277, 528521.88698721944820136 179589.55984161066589877, 528355.56430925149470568 179756.63511088167433627, 528333.7391614638036117 179823.61573685068287887, 528366.82284218922723085 179832.14097995104384609, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528527.81361586402636021 179811.23436799447517842, 528529.98316993506159633 179822.87106710238731466, 528533.85478600137867033 179825.13354498089756817)</t>
+  </si>
+  <si>
+    <t>LineString (529997.79784449038561434 181531.55623927924898453, 530052.96381539374124259 181551.7578624269226566, 530212.19656886300072074 181656.20085126161575317, 530209.62829864572267979 181680.17137328925309703, 530219.94612751191016287 181663.94489138040808029, 530214.47685644379816949 181646.0454587938147597, 530280.60531572205945849 181554.06226355716353282, 530282.5352925822371617 181541.31063073134282604, 530320.75503214134369045 181490.63379023759625852, 530439.40590576594695449 181519.28956287557957694, 530446.77953103894833475 181528.09228405426256359, 530452.47980525041930377 181521.3478456501616165, 530415.45271119684912264 181496.96883923502173275, 530453.46287902258336544 181405.91857528948457912, 530484.62340791756287217 181368.68222978565609083, 530453.29358863539528102 181346.97811556659871712, 530395.29544163832906634 181277.22392895829398185, 530367.43655410828068852 181235.61759427358629182, 530392.94670032931026071 181209.0107060651644133, 530366.14074424654245377 181232.85823050834005699, 530356.76784806651994586 181243.06795197643805295, 530233.45040496217552572 181368.96061311141238548, 530208.70179800654295832 181365.30212338751880452, 530089.44054251117631793 181304.94443834689445794, 529993.94726804597303271 181289.97907443816075101, 529966.154449358349666 181292.82961994459037669, 529944.77535806014202535 181334.87516616433276795, 529944.77535806014202535 181344.13943906020722352, 529926.36038226482924074 181394.46298536835820414, 529818.3114558468805626 181372.26115117289009504, 529660.9002180868992582 181353.18405782332411036, 529658.19050382054410875 181346.70498227514326572, 529687.50564937863964587 181285.67399781054700725, 529721.54846181173343211 181300.10519003760418855, 529759.29157994396518916 181225.35901491285767406, 529693.52337177516892552 181197.2517148221086245, 529775.50000859634019434 181018.70994359909673221, 529775.97546259185764939 181007.7745017017587088, 529781.20545654278248549 181022.98902955889934674, 529838.73539000260643661 181058.17262522855889983, 529856.80264183296822011 181056.27080924643087201, 529884.37897357402835041 181053.41808527320972644, 529884.37897357402835041 181040.5808273937436752, 529841.11265998031012714 181013.00449565265444107, 529793.09180643118452281 180981.03021445288322866, 529813.06087424361612648 180938.71480885017081164, 529693.24646736856084317 180862.64216956440941431, 529636.19198790425434709 180936.81299286801367998, 529544.71261489775497466 181110.32049908270710148, 529500.67028855415992439 181087.15450479803257622, 529497.70719626196660101 181077.45711184164974838, 529472.11685373820364475 181065.06599861959693953, 529327.24100357142742723 180987.63423189727473073, 529363.68890629184897989 180934.36422022906481288, 529341.2594276947202161 180918.74369049177039415, 529369.35465322365052998 180880.94103444411302917, 529373.59544198273215443 180864.11040405652602203, 529474.45649861427955329 180734.88892437299364246, 529586.06983813573606312 180745.40322447285871021, 529628.95491681678686291 180674.37020755160483532, 529698.51421969395596534 180685.57043428605538793, 529764.5366088654845953 180707.3814021373691503, 529796.95831783371977508 180641.94849858339875937, 529758.90263750497251749 180615.22934820654336363, 529701.21620745782274753 180576.41469456732738763, 529752.221008560503833 180488.99246547726215795, 529736.71554902533534914 180486.13619661549455486, 529630.94052359636407346 180420.23669079795945436, 529553.29336541274096817 180371.4960196012398228, 529600.89540751581080258 180294.5100008912559133, 529603.18077846488449723 180280.48510687495581806, 529627.5501629994250834 180237.51849304826464504, 529651.26990355167072266 180199.75792183651356027, 529755.13459132704883814 180264.05033537332201377, 529757.49669685761909932 180282.93852961267111823, 529750.75456156919244677 180263.42270937078865245, 529741.05953626392874867 180258.27485075587173924, 529692.10561535775195807 180344.68907300592400134, 529714.50048789544962347 180362.21963196148863062, 529818.38248662056867033 180418.31933547760127112, 529825.45121432386804372 180416.40886853076517582, 529886.37351822550408542 180465.18994148258934729, 529853.88177636556793004 180532.38877123859128915, 529886.33526469033677131 180548.33083567884750664, 529890.60546052257996053 180565.19810921599855646, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530050.41157349967397749 180610.86616918962681666, 530235.09162783063948154 180613.78033897408749908, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530444.13386487518437207 180752.09647070491337217, 530456.53883401595521718 180738.17460338707314804, 530549.71892086556181312 180796.16773621237371117, 530512.65642931591719389 180852.13211276050424203, 530566.90231333044357598 180885.25091369968140498, 530583.1249414641642943 180878.67467777145793661, 530524.64255371654871851 180911.98733362223720178, 530505.54892795660998672 180897.67947467043995857, 530523.40039052930660546 180917.79939073801506311, 530561.34779101354070008 180950.63630880584241822, 530621.1334050502628088 180918.0341914298478514, 530628.92289129947312176 180938.48514510347740725, 530661.53606858651619405 180994.88196303881704807, 530688.01616593403741717 181020.94359625864308327, 530721.15283389366231859 181041.38081424048868939, 530656.38647651602514088 181175.61041465913876891, 530656.38647651602514088 181175.61041465913876891, 530598.19786890340037644 181315.67702762898989022, 530608.5923467124812305 181319.8971903805504553, 530706.48800598783418536 181115.20450672687729821, 530736.81760364526417106 181050.18089281633729115, 530777.92077549907844514 181058.54980300978058949, 530775.52353065914940089 181090.80832662503235042)</t>
+  </si>
+  <si>
+    <t>LineString (530315.37161932047456503 177998.80604608487919904, 530315.56318013661075383 177999.03289441973902285, 530312.13405959820374846 178036.68039025971665978, 530327.5800858890870586 178073.0888808025047183, 530359.94318859372287989 178068.67573043366428465, 530382.17224571469705552 178064.30687938295886852, 530409.71792252280283719 178051.83336535666603595, 530457.53305962367448956 178047.15579759678803384, 530484.55909291654825211 178044.27656433341326192, 530481.82446864934172481 178176.08545401293667965, 530480.73061894241254777 178201.7909221246954985, 530453.93130112381186336 178202.88477183159557171, 530434.6485230919206515 178208.30226855166256428, 530510.72968812065664679 178204.59099220877396874, 530560.83191874937620014 178250.05412740889005363, 530576.60484320647083223 178299.22853895186563022, 530595.16122492088470608 178402.68036700924858451, 530413.80008803645614535 178436.11341032542986795, 530418.27724980388302356 178499.91296551114646718, 530508.93977559404447675 178869.27881132310722023, 530512.99918529542628676 178904.58935879755881615, 530537.61080370028503239 178893.65086172873270698, 530445.72742832207586616 178500.95881695748539641, 530401.85479763883631676 178248.42200085142394528, 530398.61737529921811074 178112.52069049383862875, 530397.05111636582296342 178067.79433303145924583, 530372.89449547010008246 178077.41707417467841879, 530341.8666145202005282 178078.87150609420496039, 530263.00199223437812179 178102.06698323713499121, 530128.67393126524984837 178193.75180186820216477, 530016.07499924581497908 178268.64121385099133477, 529986.7336030377773568 178290.67374241168727167, 529976.07911414559930563 178274.75468253748840652, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529225.49949584668502212 178821.69789721473352984, 529270.770087662152946 178758.30559268582146615, 529337.70783226401545107 178657.27980173568357714, 529306.5308305585058406 178711.19551833867444657, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529620.80678689747583121 178938.51310259819729254, 529633.90588229265995324 178955.7253200063132681, 529712.89748927822802216 179004.92786699859425426, 529720.95868967950809747 179007.69887060293694958, 529744.56234859698452055 178988.58683275303337723, 529762.83693021174985915 178665.01042368449270725, 529752.2592964896466583 178761.09022093558451161, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530236.91407839476596564 179040.03534455323824659, 530198.04067157465033233 179295.67006986140040681, 530178.82171383546665311 179293.91705343726789579, 530203.9075888644438237 179301.97881107561988756, 530227.05203155928757042 179124.50007814407581463, 530147.65676901047118008 179116.53179329342674464, 530141.78222267993260175 179084.47633569216122851, 530118.88753060693852603 179077.95465337141649798, 530090.59497993404511362 179077.31045524863293394, 530078.73141084762755781 179089.52513436280423775, 530077.11848901340272278 179102.71359217830467969, 530025.22613055759575218 179097.06148806744022295, 530039.08963760850019753 179034.0295733317034319, 530124.90864512417465448 179031.64245610794750974, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529764.82379545003641397 178980.39474568678997457, 529726.8608069175388664 178986.4645860674791038, 529708.5995219451142475 179019.31924272864125669, 529662.33663572394289076 179123.12740439243498258, 529642.51702948904130608 179154.93664896697737277, 529570.58282343833707273 179120.13400562520837411, 529529.60315316671039909 179076.01919454638846219, 529561.16543161950539798 179129.58498098282143474, 529516.00091436528600752 179150.95722108607878909, 529517.0294774059439078 179259.9849033905484248, 529490.5439791101962328 179316.29872986389091238, 529420.08741082856431603 179303.95597337657818571, 529384.60198592755477875 179291.8703576494299341, 529375.15206299198325723 179284.92755712530924939, 529252.36735001939814538 179242.24219094007275999, 529261.78258011117577553 179194.57754063030006364, 529269.58965256006922573 179174.62613326087011956, 529296.33848912897519767 179174.14417224159114994, 529301.68539485009387136 179174.04783159797079861, 529296.33972956647630781 179174.13921049170312472, 529267.85474757140036672 179174.62613326087011956, 529239.58119475841522217 179148.36465595476329327, 529195.2201183628058061 179118.48233969206921756, 529148.38958095852285624 179107.35710484313312918, 529204.08223160775378346 179134.07865458953892812, 529185.22284631489310414 179175.21252341114450246, 529078.4996979859424755 179150.77853555406909436, 528999.59170996560715139 179155.74130209622671828, 529004.55447650782298297 179178.57002819015178829, 529008.00452898163348436 179232.70877502896473743, 528944.69158343283925205 179232.70877502896473743, 528973.09685089520644397 179300.47073837311472744, 528996.36863628611899912 179297.04841699209646322, 529001.91040330554824322 179304.25271411731955595, 529003.21327904821373522 179305.94645258274977095, 529003.64613620459567755 179307.80479111763997935, 529030.28640920133329928 179422.17657674243673682, 529184.34559951478149742 179359.33850391051964834, 529283.96327179321087897 179424.30655104867764749, 529302.73181874421425164 179444.51883238056325354, 529335.78186670539434999 179437.48325416501029395, 529384.02287575032096356 179413.93252533991471864, 529384.73062578472308815 179413.58700957507244311, 529384.76409676810726523 179413.5639608106284868)</t>
+  </si>
+  <si>
+    <t>LineString (529384.76409676810726523 179413.5639608106284868, 529488.89725268981419504 179341.85586195762152784, 529507.48609744769055396 179304.67817244172329083, 529527.17355776752810925 179312.97107102791778743, 529529.5510069637093693 179300.78664389729965478, 529534.45449593081139028 179283.84731837426079437, 529628.36373918130993843 179315.94288252317346632, 529728.8134611037094146 179371.58312865174957551, 529741.16611664625816047 179340.74701443157391623, 529747.72725551202893257 179333.28269497497240081, 529732.54637435323093086 179372.60836770420428365, 529934.28882346954196692 179505.42975160863716155, 529918.16304199350997806 179629.85653598894714378, 529922.10143239889293909 179699.43476648480282165, 530057.3195029852213338 179688.93239207033184357, 530088.82662622863426805 179667.92764324138988741, 530323.81725375237874687 179657.42526882691890933, 530325.13005055417306721 179730.94188972821575589, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530192.40161589626222849 180341.40615362935932353, 530196.23630858049727976 180369.52140639838762581, 530158.12951031571719795 180404.89178596111014485, 530182.56527195440139621 180428.99094872875139117, 530154.47698763408698142 180458.55987566290423274, 530183.92752438690513372 180435.08348239044426009, 530293.34787298541050404 180342.47797329718014225, 530293.65838375233579427 180330.37039344478398561, 530322.77280297817196697 180317.23823465663008392, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530887.07347942178603262 180750.79246864788001403, 530877.94206235243473202 180786.27454640308860689, 530909.77157327998429537 180806.88545921674813144, 531001.73798804986290634 180835.84509620812605135, 530983.51015721820294857 180883.61690484962309711, 530971.57197559298947453 180910.01476331148296595, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530839.96893899887800217 180962.59428733977256343, 530825.31875263038091362 180987.98871232249075547, 530828.8466102258535102 181060.02426798728993163, 530784.76249950716737658 181057.81600592558970675, 530782.85777297907043248 181089.98073848168132827)</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +728,8 @@
     <col min="7" max="7" width="14.1640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="4"/>
     <col min="9" max="9" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="4"/>
+    <col min="10" max="10" width="10.83203125" style="4"/>
+    <col min="11" max="11" width="13" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -733,19 +737,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -764,7 +768,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -776,7 +780,7 @@
         <v>9992.6263998460909</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="G2" s="6">
         <f t="shared" ref="G2:G13" si="0">IF(B2=1,K$1+(C2*K$2)/86400+D2/1000/K$3/24,G1+(C2*K$2)/86400+D2/1000/K$3/24)</f>
@@ -795,7 +799,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -807,7 +811,7 @@
         <v>10887.8491666108</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -829,7 +833,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -841,7 +845,7 @@
         <v>10102.0951141726</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -857,13 +861,13 @@
         <v>8</v>
       </c>
       <c r="K4" s="2">
-        <f>C14+C29+C44</f>
+        <f>C14+C29+C44-2</f>
         <v>789</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -875,7 +879,7 @@
         <v>10944.401411074199</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -887,10 +891,13 @@
       <c r="H5" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="J5" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -902,7 +909,7 @@
         <v>10095.084299316801</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="0"/>
@@ -914,7 +921,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -926,7 +933,7 @@
         <v>10046.5421778538</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
@@ -938,7 +945,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -950,10 +957,10 @@
         <v>10548.867796274901</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
@@ -965,23 +972,23 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9">
-        <v>10437.9228677547</v>
+        <v>10611.294807914701</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="0"/>
-        <v>0.71226796410967974</v>
+        <v>0.71319309279910192</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>14</v>
@@ -989,7 +996,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1001,11 +1008,11 @@
         <v>9917.6186015727999</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>0.75504891500381122</v>
+        <v>0.7559740436932334</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>14</v>
@@ -1013,7 +1020,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1025,11 +1032,11 @@
         <v>8839.9771304433798</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>0.7938905054386225</v>
+        <v>0.79481563412804468</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>14</v>
@@ -1037,7 +1044,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1049,11 +1056,11 @@
         <v>9403.1546556121302</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>0.83322046540177408</v>
+        <v>0.83414559409119626</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>14</v>
@@ -1061,7 +1068,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1070,17 +1077,17 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>4195.7036937358298</v>
+        <v>4207.7000846856199</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
-        <v>0.85206725549200457</v>
+        <v>0.85303237215125938</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>14</v>
@@ -1089,15 +1096,15 @@
     <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C14" s="2">
         <f>SUM(C2:C13)</f>
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D14" s="2">
         <f>SUM(D2:D13)</f>
-        <v>115411.84331426804</v>
+        <v>115597.21164537784</v>
       </c>
       <c r="G14" s="3">
         <f>G13-K$1</f>
-        <v>0.47706725549200457</v>
+        <v>0.47803237215125938</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>14</v>
@@ -1111,19 +1118,19 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>6</v>
@@ -1134,7 +1141,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1146,7 +1153,7 @@
         <v>10431.583680433399</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G17" s="6">
         <f t="shared" ref="G17:G28" si="1">IF(B17=1,K$1+(C17*K$2)/86400+D17/1000/K$3/24,G16+(C17*K$2)/86400+D17/1000/K$3/24)</f>
@@ -1158,7 +1165,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1170,10 +1177,10 @@
         <v>9598.5794537826896</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="1"/>
@@ -1185,7 +1192,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1197,7 +1204,7 @@
         <v>10045.637819464901</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="1"/>
@@ -1209,7 +1216,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1221,7 +1228,7 @@
         <v>10467.777384413201</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>
@@ -1236,7 +1243,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1248,7 +1255,7 @@
         <v>9551.6573628486094</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="1"/>
@@ -1260,7 +1267,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -1272,7 +1279,7 @@
         <v>8539.3878200574109</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G22" s="6">
         <f t="shared" si="1"/>
@@ -1284,7 +1291,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B23">
         <v>7</v>
@@ -1296,7 +1303,7 @@
         <v>10161.2218843683</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G23" s="6">
         <f t="shared" si="1"/>
@@ -1308,7 +1315,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -1317,17 +1324,17 @@
         <v>27</v>
       </c>
       <c r="D24">
-        <v>10047.346638979299</v>
+        <v>10038.4748637967</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G24" s="6">
         <f t="shared" si="1"/>
-        <v>0.69753286237004808</v>
+        <v>0.6975032897861061</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>4</v>
@@ -1335,7 +1342,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="B25">
         <v>9</v>
@@ -1347,14 +1354,14 @@
         <v>9563.4170463354603</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="1"/>
-        <v>0.73704980808005516</v>
+        <v>0.73702023549611317</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>4</v>
@@ -1362,7 +1369,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B26">
         <v>10</v>
@@ -1374,14 +1381,14 @@
         <v>10131.2822821796</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>0.7777651934650982</v>
+        <v>0.77773562088115622</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>4</v>
@@ -1389,7 +1396,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -1401,11 +1408,11 @@
         <v>9935.6153135720906</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" si="1"/>
-        <v>0.8192172445103385</v>
+        <v>0.81918767192639652</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>4</v>
@@ -1413,23 +1420,23 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28">
         <v>12</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D28">
-        <v>7488.6714860751799</v>
+        <v>7510.26180699628</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" si="1"/>
-        <v>0.85286003835281132</v>
+        <v>0.85324965572749523</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>4</v>
@@ -1438,15 +1445,15 @@
     <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C29" s="2">
         <f>SUM(C17:C28)</f>
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D29" s="2">
         <f>SUM(D17:D28)</f>
-        <v>115962.17817251016</v>
+        <v>115974.89671824865</v>
       </c>
       <c r="G29" s="3">
         <f>G28-K$1</f>
-        <v>0.47786003835281132</v>
+        <v>0.47824965572749523</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>4</v>
@@ -1460,19 +1467,19 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
       <c r="D31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>6</v>
@@ -1483,7 +1490,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1495,7 +1502,7 @@
         <v>10745.2726174831</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G32" s="6">
         <f t="shared" ref="G32:G43" si="2">IF(B32=1,K$1+(C32*K$2)/86400+D32/1000/K$3/24,G31+(C32*K$2)/86400+D32/1000/K$3/24)</f>
@@ -1507,7 +1514,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1519,7 +1526,7 @@
         <v>9112.8127969055804</v>
       </c>
       <c r="E33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G33" s="6">
         <f t="shared" si="2"/>
@@ -1531,7 +1538,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1543,10 +1550,10 @@
         <v>10846.765699108901</v>
       </c>
       <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
         <v>22</v>
-      </c>
-      <c r="F34" t="s">
-        <v>23</v>
       </c>
       <c r="G34" s="6">
         <f t="shared" si="2"/>
@@ -1558,7 +1565,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -1570,7 +1577,7 @@
         <v>10067.9823020771</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" si="2"/>
@@ -1582,7 +1589,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1594,10 +1601,10 @@
         <v>10534.2462617441</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="6">
         <f t="shared" si="2"/>
@@ -1609,7 +1616,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -1621,7 +1628,7 @@
         <v>9776.0011247831208</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37" s="6">
         <f t="shared" si="2"/>
@@ -1633,7 +1640,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B38">
         <v>7</v>
@@ -1645,10 +1652,10 @@
         <v>9000.7159530542594</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G38" s="6">
         <f t="shared" si="2"/>
@@ -1660,7 +1667,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -1672,7 +1679,7 @@
         <v>10057.201629004699</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G39" s="6">
         <f t="shared" si="2"/>
@@ -1684,7 +1691,7 @@
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B40">
         <v>9</v>
@@ -1696,7 +1703,7 @@
         <v>9882.94922301921</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G40" s="6">
         <f t="shared" si="2"/>
@@ -1708,7 +1715,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -1720,7 +1727,7 @@
         <v>10569.3243713347</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G41" s="6">
         <f t="shared" si="2"/>
@@ -1732,7 +1739,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="B42">
         <v>11</v>
@@ -1741,17 +1748,17 @@
         <v>28</v>
       </c>
       <c r="D42">
-        <v>10650.070893766</v>
+        <v>11539.134278147199</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G42" s="6">
         <f t="shared" si="2"/>
-        <v>0.83122780957426934</v>
+        <v>0.83419135418887336</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>5</v>
@@ -1759,7 +1766,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B43">
         <v>12</v>
@@ -1768,14 +1775,14 @@
         <v>14</v>
       </c>
       <c r="D43">
-        <v>5231.8590340946903</v>
+        <v>4065.9771499308299</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G43" s="6">
         <f t="shared" si="2"/>
-        <v>0.85352845079902939</v>
+        <v>0.85260572246642052</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>5</v>
@@ -1788,11 +1795,11 @@
       </c>
       <c r="D44" s="2">
         <f>SUM(D32:D43)</f>
-        <v>116475.20190637547</v>
+        <v>116198.38340659281</v>
       </c>
       <c r="G44" s="3">
         <f>G43-K$1</f>
-        <v>0.47852845079902939</v>
+        <v>0.47760572246642052</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Fix S dock numbering so each route finishes with a docking station.
Also sync up the summary route dock counts with reality.
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Desktop/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9563FC3-2E9A-A147-A448-7148F0C8735F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D30BA-E5D6-A94B-BCE1-F295D8FC3CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="28060" windowHeight="17500" xr2:uid="{211AF0F6-F836-F343-9553-311F059F951A}"/>
+    <workbookView xWindow="6380" yWindow="520" windowWidth="28060" windowHeight="17500" xr2:uid="{211AF0F6-F836-F343-9553-311F059F951A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:F28"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1171,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18">
         <v>9622.4267540258297</v>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="G18" s="6">
         <f t="shared" si="1"/>
-        <v>0.45434670144819739</v>
+        <v>0.45469392367041961</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>4</v>
@@ -1198,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19">
         <v>10047.1885802253</v>
@@ -1222,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20">
         <v>10468.802652468101</v>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="G20" s="6">
         <f t="shared" si="1"/>
-        <v>0.5390527833349531</v>
+        <v>0.53940000555717527</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>4</v>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="G21" s="6">
         <f t="shared" si="1"/>
-        <v>0.57848656705725754</v>
+        <v>0.5788337892794797</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>4</v>
@@ -1273,7 +1273,7 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22">
         <v>8539.0048141119696</v>
@@ -1544,7 +1544,7 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D34">
         <v>10846.765699108901</v>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="G34" s="6">
         <f t="shared" si="2"/>
-        <v>0.50616894815610314</v>
+        <v>0.5065161703783253</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>5</v>
@@ -1574,14 +1574,14 @@
         <v>18</v>
       </c>
       <c r="D35">
-        <v>10067.9823020771</v>
+        <v>10066.99824741</v>
       </c>
       <c r="E35" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" si="2"/>
-        <v>0.54597888916302684</v>
+        <v>0.54632283120302527</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>5</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="G36" s="6">
         <f t="shared" si="2"/>
-        <v>0.5869958211466183</v>
+        <v>0.58733976318661674</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>5</v>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="G37" s="6">
         <f t="shared" si="2"/>
-        <v>0.62617971378478432</v>
+        <v>0.62652365582478275</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>5</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="G38" s="6">
         <f t="shared" si="2"/>
-        <v>0.66277932251718741</v>
+        <v>0.66312326455718584</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>5</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="G39" s="6">
         <f t="shared" si="2"/>
-        <v>0.70324777239164749</v>
+        <v>0.70359171443164592</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>5</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="G40" s="6">
         <f t="shared" si="2"/>
-        <v>0.74348260313504488</v>
+        <v>0.74382654517504332</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>5</v>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="G41" s="6">
         <f t="shared" si="2"/>
-        <v>0.78600535103949387</v>
+        <v>0.78634929307949231</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>5</v>
@@ -1745,7 +1745,7 @@
         <v>11</v>
       </c>
       <c r="C42">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D42">
         <v>11539.134278147199</v>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="G42" s="6">
         <f t="shared" si="2"/>
-        <v>0.83419135418887336</v>
+        <v>0.83522974067331623</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>5</v>
@@ -1772,7 +1772,7 @@
         <v>12</v>
       </c>
       <c r="C43">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D43">
         <v>4065.9771499308299</v>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="G43" s="6">
         <f t="shared" si="2"/>
-        <v>0.85260572246642052</v>
+        <v>0.85260244228419679</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>5</v>
@@ -1795,11 +1795,11 @@
       </c>
       <c r="D44" s="2">
         <f>SUM(D32:D43)</f>
-        <v>116198.38340659281</v>
+        <v>116197.39935192571</v>
       </c>
       <c r="G44" s="3">
         <f>G43-K$1</f>
-        <v>0.47760572246642052</v>
+        <v>0.47760244228419679</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add docking station per-stage counts
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Documents/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5483CCF-8A9B-9448-818F-44E27BF42835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E058D532-6B1F-044D-8FBE-158DCD298F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
+    <workbookView xWindow="1300" yWindow="4080" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B222A62-E78F-E448-B4C7-291D829E11A4}">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,60 +654,72 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>36</v>
+      </c>
       <c r="D2">
-        <v>10275.7603419072</v>
+        <v>10387.633383793</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
       <c r="D3">
-        <v>10176.9320304295</v>
+        <v>10135.874484428899</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
       <c r="D4">
-        <v>10601.066552067599</v>
+        <v>10889.6786160784</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
       <c r="D5">
-        <v>11162.543933425801</v>
+        <v>10373.492909434601</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -716,16 +728,19 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
       <c r="D6">
-        <v>10261.913579423001</v>
+        <v>10047.75961035</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -734,16 +749,19 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
       <c r="D7">
-        <v>10185.2940832533</v>
+        <v>10347.2332512455</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -752,16 +770,19 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
       <c r="D8">
-        <v>9096.5507719182897</v>
+        <v>10260.484070139</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -770,11 +791,12 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
+        <f>SUM(C2:C8)</f>
         <v>162</v>
       </c>
       <c r="D9" s="1">
         <f>SUM(D2:D8)</f>
-        <v>71760.061292424696</v>
+        <v>72442.156325469405</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -782,39 +804,27 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>10130.800646047501</v>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -823,476 +833,577 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>10240.7485129782</v>
+        <v>10396.40561819</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>10322.5536861458</v>
+        <v>10050.3586120912</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
       </c>
       <c r="D14">
-        <v>10086.2297192444</v>
+        <v>10040.0307021154</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>10197.200793621199</v>
+        <v>10328.5537327765</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
       </c>
       <c r="D16">
-        <v>10503.889210624</v>
+        <v>10468.1416395172</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>10473.764647815</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18">
         <v>7</v>
       </c>
-      <c r="D17">
-        <v>11221.3477004749</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C18">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="1">
+      <c r="D18">
+        <v>8970.4012079409804</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="1">
+        <f>SUM(C12:C18)</f>
         <v>162</v>
       </c>
-      <c r="D18" s="1">
-        <f>SUM(D11:D17)</f>
-        <v>72702.770269136003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>10029.895474594299</v>
-      </c>
-      <c r="E20" t="s">
-        <v>31</v>
+      <c r="D19" s="1">
+        <f>SUM(D12:D18)</f>
+        <v>70727.656160446277</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
         <v>2</v>
       </c>
-      <c r="D21">
-        <v>10369.6417108937</v>
+      <c r="D21" t="s">
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
       </c>
       <c r="D22">
-        <v>10147.9934740517</v>
+        <v>10130.800646047501</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
       </c>
       <c r="D23">
-        <v>10428.3463445986</v>
+        <v>10240.7485129782</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
       </c>
       <c r="D24">
-        <v>10263.725203550401</v>
+        <v>10322.5536861458</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>10123.7166457228</v>
+        <v>10086.2297192444</v>
       </c>
       <c r="E25" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>10830.2986615384</v>
+        <v>10197.200793621199</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C27" s="1">
-        <v>162</v>
-      </c>
-      <c r="D27" s="1">
-        <f>SUM(D20:D26)</f>
-        <v>72193.617514949903</v>
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>10503.889210624</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>3</v>
+        <v>71</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>31</v>
+      </c>
+      <c r="D28">
+        <v>11221.3477004749</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>10387.633383793</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>10135.874484428899</v>
-      </c>
-      <c r="E30" t="s">
-        <v>45</v>
+      <c r="C29" s="1">
+        <f>SUM(C22:C28)</f>
+        <v>162</v>
+      </c>
+      <c r="D29" s="1">
+        <f>SUM(D22:D28)</f>
+        <v>72702.770269136003</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="D31">
-        <v>10889.6786160784</v>
-      </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>32</v>
       </c>
       <c r="D32">
-        <v>10373.492909434601</v>
+        <v>10029.895474594299</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
       </c>
       <c r="D33">
-        <v>10047.75961035</v>
+        <v>10369.6417108937</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>19</v>
       </c>
       <c r="D34">
-        <v>10347.2332512455</v>
+        <v>10147.9934740517</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>16</v>
       </c>
       <c r="D35">
-        <v>10260.484070139</v>
+        <v>10428.3463445986</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C36" s="1">
-        <v>162</v>
-      </c>
-      <c r="D36" s="1">
-        <f>SUM(D29:D35)</f>
-        <v>72442.156325469405</v>
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36">
+        <v>10263.725203550401</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>10123.7166457228</v>
       </c>
       <c r="E37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>28</v>
       </c>
       <c r="D38">
-        <v>10396.40561819</v>
+        <v>10830.2986615384</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="D39">
-        <v>10050.3586120912</v>
-      </c>
-      <c r="E39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="D40">
-        <v>10040.0307021154</v>
-      </c>
-      <c r="E40" t="s">
-        <v>60</v>
+      <c r="C39" s="1">
+        <f>SUM(C32:C38)</f>
+        <v>162</v>
+      </c>
+      <c r="D39" s="1">
+        <f>SUM(D32:D38)</f>
+        <v>72193.617514949903</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
         <v>4</v>
       </c>
-      <c r="D41">
-        <v>10328.5537327765</v>
-      </c>
-      <c r="E41" t="s">
-        <v>62</v>
+      <c r="F41" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>29</v>
       </c>
       <c r="D42">
-        <v>10468.1416395172</v>
+        <v>10275.7603419072</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
       </c>
       <c r="D43">
-        <v>10473.764647815</v>
+        <v>10176.9320304295</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>23</v>
+      </c>
+      <c r="D44">
+        <v>10601.066552067599</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>17</v>
+      </c>
+      <c r="D45">
+        <v>11162.543933425801</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <v>10261.913579423001</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>24</v>
+      </c>
+      <c r="D47">
+        <v>10185.2940832533</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48">
         <v>7</v>
       </c>
-      <c r="D44">
-        <v>8970.4012079409804</v>
-      </c>
-      <c r="E44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C45" s="1">
+      <c r="C48">
+        <v>25</v>
+      </c>
+      <c r="D48">
+        <v>9096.5507719182897</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="1">
         <v>162</v>
       </c>
-      <c r="D45" s="1">
-        <f>SUM(D38:D44)</f>
-        <v>70727.656160446277</v>
+      <c r="D49" s="1">
+        <f>SUM(D42:D48)</f>
+        <v>71760.061292424696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20230706 update (ATD2 v2)
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Documents/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E058D532-6B1F-044D-8FBE-158DCD298F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C5AD75-5DB4-5C47-9368-89836ECFD5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="4080" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
+    <workbookView xWindow="5620" yWindow="10140" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -56,6 +56,21 @@
     <t>cmt</t>
   </si>
   <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>LineString (528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526810.75304763286840171 179467.00080663594417274, 526668.71815055573824793 179454.61404235597001389, 526438.77076674299314618 179425.46686823663185351, 526444.83039404929149896 179401.22835901146754622, 526429.857896420173347 179399.29642383340978995, 526400.95936604985035956 179579.61037377678439952, 526395.80753890855703503 179617.60509894342976622, 526400.31538765714503825 179630.4846667965175584, 526396.45151730126235634 179663.00557562557514757, 526429.93839371926151216 179670.41132714110426605, 526431.87032889726106077 179659.14170526966336183, 526400.31538765714503825 179655.59982411004602909, 526404.17925801302772015 179629.51869920754688792, 526481.13467593537643552 179644.97418063125223853, 526512.36762797913979739 179646.26213741654646583, 526515.90950913866981864 179639.17837509737000801, 526505.28386565984692425 179635.63649393775267527, 526386.30885761685203761 179621.30797470119432546, 526318.94980677636340261 179621.48525741521734744, 526215.34960218577180058 179626.84875574553734623, 526121.02660867478698492 179655.6876124200061895, 526113.32453510130289942 179686.26937513795564882, 526116.04291400965303183 179658.17945975257316604, 526072.0957883259980008 179674.03667005078750663, 526077.53254614258185029 179626.23850758047774434, 526092.24883591232355684 179409.14943758773733862, 526170.58646800776477903 179414.55203290464123711, 526170.91200886678416282 179254.77395809174049646, 526170.02756560104899108 179226.2506627686379943, 526170.69089805032126606 179197.28514581263880245, 526191.0330931645585224 179103.75527045089984313, 526208.50084766466170549 179068.1564290011592675, 526205.1700667041586712 179050.55107881623553112, 526215.6382354375673458 179000.58936440671095625, 526094.3026433001505211 178987.74206641569617204, 526096.78229620109777898 178934.34904740183264948, 526076.51597697660326958 178943.73160259836004116, 526090.02685645967721939 178944.10690480621997267, 526079.61222019151318818 179075.18120090151205659, 525857.43331313808448613 179086.440267137310002, 525822.15490559919271618 179081.18603622727096081, 525774.11622299312148243 179039.15218894690042362, 525789.9340731572592631 179008.44695039271027781, 525609.81218133552465588 178989.52756098052486777, 525584.06940557796042413 178987.97679135657381266, 525578.79678885661996901 179053.72942341200541705, 525579.54627333593089134 178986.48593813352636062, 525473.92217159015126526 178976.91720417744363658, 525356.52116651367396116 178940.85043772764038295, 525101.93763904797378927 178795.75530841300496832, 525143.89285716298036277 178740.55107405106537044, 525178.48751069651916623 178739.81501759291859344, 525136.90032081049866974 178734.29459415673045442, 525073.96749363793060184 178845.07109110968303867, 525050.22967286221683025 178837.15848418447421864, 524920.68373622617218643 178769.44129003383568488, 524812.24932546948548406 178896.28909129649400711, 524699.21156708616763353 179025.31069560500327498, 524681.6391244096448645 179051.25509521568892524, 524679.63010795961599797 179077.09913740976480767, 524788.97600055101793259 179149.0372246410115622, 524957.31112467218190432 179248.31178502010880038, 524889.31033757049590349 179366.96949636968201958, 524837.84125263791065663 179392.39398410747526214, 524751.64603811223059893 179345.88577483102562837, 524614.60184811090584844 179570.98550772908492945, 524703.84473427385091782 179436.35361285935505293, 524844.32857223774772137 179505.77558726171264425, 524810.43752961605787277 179598.63431089642108418, 524822.46338344959076494 179627.87900090057519265, 524845.42183167708572 179640.99811417344608344, 524954.20114589820150286 179688.82821464753942564, 524980.43937244394328445 179689.64815922707202844, 525145.27674076042603701 179339.90930881092208438, 525213.61852516769431531 179374.56420798628823832, 525206.26161919755395502 179390.0524310814216733, 525222.23384926444850862 179385.21236136413062923, 525351.1733065313892439 179466.91273819096386433, 525352.72212884086184204 179482.01375570870004594, 525369.8851592862047255 179479.95885097398422658, 525422.48737169418018311 179507.45546200548415072, 525366.53774576925206929 179596.40102116821799427, 525283.64405398862436414 179742.1564941595424898, 525384.085012789350003 179740.24697022794862278, 525418.45644355763215572 179681.43363313551526517, 525419.82130964624229819 179656.85948007801198401)</t>
   </si>
   <si>
@@ -92,9 +107,6 @@
     <t>W7 Marylebone</t>
   </si>
   <si>
-    <t>LineString (530577.23797894886229187 180877.97880632089800201, 530617.74819760688114911 180823.78270298111601733, 530460.08680607296992093 180724.14946249785134569, 530317.89046422939281911 180623.28449239319888875, 530146.54318801360204816 180467.81284240834065713, 530072.77626957895699888 180399.24656015267828479, 530035.55066324456129223 180349.42993991106050089, 529890.48028561775572598 180246.51208710417267866, 529825.74567924335133284 180200.98946149481344037, 529919.54799574031494558 180130.36585574291530065, 529957.12143912480678409 179966.409011882962659, 529911.86251868435647339 179845.57623372576199472, 529906.73886731371749192 179702.96793724340386689, 529926.37953090108931065 179692.72063450215500779, 529923.81770521576981992 179643.19200458613340743, 529919.54799574031494558 179631.23681805469095707, 529921.4103331834776327 179584.29027873513405211, 529930.04384519555605948 179550.71550979930907488, 529930.52348475181497633 179516.66110130725428462, 529941.07555498881265521 179505.62939151405589655, 529912.29718161525670439 179479.72885547782061622, 529902.96647088008467108 179374.86438768959487788, 529800.47367502108681947 179363.00662448359071277, 529739.62031473114620894 179333.45689976593712345, 529740.46023528114892542 179272.14269961469108239, 529760.61832848156336695 179193.19016791306785308, 529641.34961037908215076 179153.71390206224168651, 529568.27652252756524831 179120.95700061158277094, 529550.34316133812535554 179093.66307770530693233, 529526.79745115165133029 179077.07363828388042748, 529564.38437103840988129 179130.25138729959144257, 529513.81095916836056858 179152.52902801893651485, 529512.12165939807891846 179263.45971292795729823, 529524.55590479262173176 179301.70093485678080469, 529448.61280135076958686 179371.58212878205813468, 529385.91768299601972103 179410.16374007728882134, 529333.16189551877323538 179435.02868727562599815, 529281.9714767278637737 179374.53091961363679729, 529220.891999761457555 179328.57588456268422306, 529164.02991525223478675 179367.55040796031244099, 529081.42719402140937746 179391.9821987469040323, 529060.48565906146541238 179415.83228022902039811, 529027.32822870835661888 179419.32253605569712818, 528999.98789139953441918 179308.21605890721548349, 529003.47814722615294158 179297.74529142724350095, 529055.25027532153762877 179270.40495411845040508, 529084.33574054366908967 179209.47090447816299275, 529104.11385689466260374 179164.09757873168564402, 529351.77659326093271375 179225.75876500256708823, 529383.05599977204110473 179235.19909444704535417, 529373.87950731569435447 179284.14038754784269258, 529392.23249222850427032 179227.24613431817851961, 529266.2086624939693138 179192.37546298385132104, 529269.26749331271275878 179176.46954272608854808, 529304.13816464703995734 179174.63424423482501879, 529268.04396098526194692 179166.06951794217457063, 529196.15887484396807849 179120.03240704443305731, 529149.98932790081016719 179107.75948950258316472, 529203.17197058210149407 179134.6430231656995602, 529187.39250517124310136 179174.383899015490897, 529058.81908330414444208 179141.07169425903703086, 529011.0423685876885429 179146.33151606269530021, 529005.19812213920522481 179177.89044688461581245, 528990.58750601788051426 179149.25363928693695925, 528858.21532395936083049 179161.52655682878685184, 528770.55162723187822849 179211.78707628592383116, 528715.03128597105387598 179321.6589095177478157, 528618.60121957084629685 179477.9925020151422359, 528491.34275315469130874 179622.19928313192212954, 528388.04569717741105705 179719.06766801583580673, 528360.57773886946961284 179750.62659883772721514, 528302.13527438452001661 179698.61280544605688192, 528281.73319864494260401 179662.65391637163702399, 528262.13372618111316115 179565.91304187983041629, 528297.16959096642676741 179504.60027850553160533, 528354.10287124256137758 179445.47725668028579094, 528571.1610022954409942 179230.06143178927595727, 528461.67392484133597463 179117.28974201151868328, 528427.73293083056341857 179154.51534834591438994, 528270.83738425537012517 178995.94010165525833145, 528307.81268304819241166 178962.03991528681945056, 528251.02088932693004608 178905.98091890395153314, 528237.09773989859968424 178880.69941073132213205, 528445.48698298842646182 178680.18773902862449177, 528506.68087698111776263 178769.79506966570625082, 528622.96355511201545596 178714.21878967669908889, 528690.51011079095769674 178852.7319798031821847, 528629.80371264915447682 178709.94369121600175276, 528706.32797509559895843 178677.88045276078628376, 528675.97477602458093315 178675.74290353045216762, 528565.03597096959128976 178505.16647494878270663, 528591.54158142581582069 178459.85043126542586833, 528535.96530143683776259 178489.77612049027811736, 528478.67898206354584545 178502.6014158723410219, 528322.21037840214557946 178459.85043126542586833, 528311.95014209649525583 178498.3263174116727896, 528292.28468917729333043 178492.34117956669069827, 528227.69070692639797926 178577.5864321083354298, 528109.89053357648663223 178750.95101042950409465, 528057.58673679200001061 178714.85402391621028073, 528050.95667804463300854 178736.21754654651158489, 528039.90658013243228197 178798.09809485499863513, 528075.26689345156773925 178816.51492470869561657, 528057.36634973983746022 178881.49318986901198514, 528077.50150927738286555 178927.95894264802336693, 527957.20683819404803216 178903.17720783254480921, 527893.18735658738296479 178892.33519885077839717, 527838.97731167858000845 178884.59090672095771879, 527827.61901655478868634 178890.78634042482008226, 527761.01810423820279539 178875.29775616514962167, 527777.55729742196854204 178801.08342777710640803, 527839.85880704678129405 178661.95543657644884661, 527875.91507322294637561 178584.04074644856154919, 527702.52480672812089324 178435.08524715233943425, 527673.89863282348960638 178393.55225022041122429)</t>
-  </si>
-  <si>
     <t>P1 Westminster</t>
   </si>
   <si>
@@ -146,9 +158,6 @@
     <t>S3 Bermondsey</t>
   </si>
   <si>
-    <t>LineString (532680.96280913078226149 178677.48286417848430574, 532646.72988178418017924 178686.93224038934567943, 532644.91513582807965577 178705.68461526944884099, 532577.46707779157441109 178826.97013667138526216, 532558.10978759278077632 178818.50132220939849503, 532477.21695213438943028 178782.04142910346854478, 532465.16113808494992554 178762.56665256191627122, 532448.46847247786354274 178772.14947911410126835, 532425.90246156463399529 178760.71191193890990689, 532423.12035063013900071 178744.32836976903490722, 532352.79476867453195155 178710.47935339916148223, 532245.37437425879761577 178647.41817221697419882, 532184.94074229244142771 178616.19670506301918067, 532251.30818086618091911 178452.11467546166386455, 532511.10399071127176285 178585.03346189408330247, 532598.70955449633765966 178413.85017633717507124, 532702.58256901206914335 178176.74428570797317661, 532815.09900265594478697 177890.48924129054648802, 532856.91221495741046965 177792.91708755856961943, 532858.8989350259071216 177769.61827948209247552, 532770.30928106070496142 177726.3168125337397214, 532588.16317295876797289 177673.66873071744339541, 532472.21096532221417874 177646.21587158855982125, 532425.64025696949101985 177642.10992637852905318, 532411.25822669372428209 177649.51064796402351931, 532407.54009782173670828 177671.5538405618572142, 532404.75150116789154708 177727.19298332382459193, 532429.18491946905851364 177794.11930301843676716, 532358.00930963514838368 177800.49323822744190693, 532344.59748763276729733 177875.45337209175340831, 532340.61377812712453306 177908.3853706716618035, 532327.99869802594184875 177961.36870709658251144, 532247.2621853785822168 177940.65341766728670336, 532213.93181584810372442 177940.5206273504300043, 532181.53097853565122932 177966.54752945387735963, 532131.07065813092049211 178059.50075125196599402, 531992.96872860239818692 177958.58011044265003875, 531978.40126691607292742 177969.69867078488459811, 531975.51999578601680696 177976.24701426242245361, 531956.66076657059602439 177991.70110486945486628, 531930.72932639950886369 178011.6080690412200056, 531893.66570231656078249 178019.07318060554098338, 531849.13696666923351586 178060.9825788619054947, 531859.09044875507242978 178130.13308598485309631, 531859.16702702990733087 178134.34492127480916679, 531819.8686971872812137 178155.9232769338414073, 531814.8917296277359128 178147.84576965900487266, 531807.24648775579407811 178147.84155853773700073, 531681.84718574595171958 177939.97077090424136259, 531528.1577946882462129 178035.11182251141872257, 531487.49922562530264258 177974.93714029833790846, 531424.07185788720380515 178019.66156626751762815, 531347.63374804891645908 177870.85120349729550071, 531277.70100926072336733 177896.05951631630887277, 531112.62721886532381177 177774.89698050887091085, 531123.19844682177063078 177739.93061111477436498, 531112.62721886532381177 177703.33789895815425552, 531087.41890604631043971 177667.55835818278137594, 530999.59639687044546008 177661.05298713271622546, 530915.83974460093304515 177696.01935652681277134, 530878.43386106321122497 177734.03511860055732541, 530837.77529200038406998 177695.81606368144275621, 530831.67650664085522294 177668.57482240931130946, 530831.67650664085522294 177655.15749461855739355, 530794.67720879369881004 177645.80602373406873085, 530835.33577785652596503 177653.53115185603382997, 530871.92849001311697066 177554.32424334256211296, 531069.12254996818955988 177399.4150952129275538, 530896.22850016714073718 177112.81085585197433829, 530778.53778894036076963 176970.21642869058996439, 530859.93520509428344667 177058.15468442905694246, 530925.4432389655848965 177024.38350523461122066, 531189.53587636584416032 177001.13818751723738387, 531180.75431189488153905 176810.13916027281084098, 531181.01259320287499577 176679.19053713156608865, 531173.18175361305475235 176619.08758663863409311, 530892.20482224225997925 176554.68621974403504282, 530879.22067569091450423 176529.75665836548432708, 530804.95135741727426648 176476.78134043602040038, 530799.75769879668951035 176407.18631492089480162, 530703.67501431691925973 176400.43455871418700553, 530602.39867121644783765 176331.35889906110242009, 530719.7753560405690223 176120.36651760194217786, 530745.14145082631148398 176154.77223921977565624, 530808.30562182224821299 176214.79391414625570178, 530927.40622285439167172 176269.47334575466811657, 530985.69952494266908616 176293.35631588246906176, 531191.53301749157253653 176335.15151360613526776, 531198.76075845130253583 176235.22013859765138477, 531207.48642726987600327 176156.30002914459328167, 531185.2742347844177857 176156.30002914459328167, 531209.55267773370724171 176148.55158990548807196, 531188.94265151466242969 175949.80426446883939207, 531154.94696310814470053 175823.53456467346404679, 531066.20655180979520082 175503.10660128630115651, 530998.72868066909722984 175231.84770217089680955, 531029.01404346199706197 175153.91027290970669128, 531021.65302618476562202 175139.83394162519834936, 531029.40146542387083173 175082.75377256359206513, 531032.75912242755293846 175056.73193078552139923, 531026.30208972818218172 175037.10255137970671058, 530966.8973888949258253 175050.27489808623795398, 530928.21976302622351795 175062.67240086884703487, 531062.91346513316966593 175558.95993413514224812, 530985.123753986437805 175577.28249899740330875)</t>
-  </si>
-  <si>
     <t>S4 Brixton</t>
   </si>
   <si>
@@ -158,15 +167,9 @@
     <t>S5 Clapham</t>
   </si>
   <si>
-    <t>LineString (530319.24822289927396923 177532.86330300656845793, 530283.00367995072156191 177511.02849130801041611, 530184.84259889076929539 177499.21280562478932552, 530113.65853050712030381 177494.05278513085795566, 530069.67329359170980752 177299.41811178030911833, 530023.48879483062773943 177179.55834118591155857, 530191.73232603189535439 177132.27421150187728927, 530094.96480481803882867 176769.12109921933733858, 529881.66167348786257207 176830.25587819798965938, 529842.9543123907642439 176768.22780633534421213, 529745.09127103956416249 176816.94227156793931499, 529690.3932994834613055 176733.5929815776180476, 529531.50871543935500085 176823.45393484842497855, 529513.38458597532007843 176824.64773978322045878, 529499.05892675823997706 176851.56261467593139969, 529271.26506909728050232 177111.75961302706855349, 529136.28157614718656987 177252.8598545910208486, 529045.9358032428426668 177206.80840826532221399, 528896.89055745047517121 177069.65020661591552198, 528719.06074102083221078 177058.62250209698686376, 528714.32951614784542471 177068.97205650678370148, 528710.55932132713496685 177045.83340986201073974, 528687.79030162561684847 177026.31710726069286466, 528651.71471196867059916 177031.34403368830680847, 528597.30562592856585979 177022.47298705135472119, 528633.38121558562852442 177062.39269691769732162, 528645.80068087729159743 177093.14565859251888469, 528659.99435549648478627 177110.29634875731426291, 528636.63393268582876772 177251.93739339418243617, 528532.66370314673986286 177925.4865684756077826, 528554.77845204086042941 177948.92160088589298539, 528617.49191905430052429 177943.97053770063212141, 528827.74706898862496018 177946.61110473275766708, 528860.91919232998043299 177944.30060857962234877, 529088.99816973123233765 177901.39139430731302127, 529260.80006226000841707 177863.10317234124522656, 529404.71096551173832268 177897.76061463812948205, 529417.25365891447290778 177885.54799211447243579, 529376.32486991619225591 177854.85140036582015455, 529293.80715016182512045 177856.50175476088770665, 529251.55807764746714383 177854.19125860778149217, 529020.1783914560219273 177904.03196133946767077, 528852.00727859640028328 177934.72855308811995201, 528754.63636928622145206 177937.03904924125527032, 528579.45125024754088372 177935.38869484615861438, 528555.02600520011037588 177929.77748990285908803, 528554.69593432114925236 177897.76061463812948205, 528587.94057327986229211 177658.03592232000664808, 528599.48983881680760533 177670.76972791197476909, 528612.2236444087466225 177688.53782873795717023, 528710.54046897927764803 177690.61077383431256749, 528765.9177165535511449 177685.87261361404671334, 528789.90465266862884164 177690.01850380678661168, 528858.015705834957771 177683.20739849016536027, 528903.546464201528579 177615.09634532386553474, 528963.06960196862928569 177621.01904559918330051, 529007.48985403357073665 177597.03210948410560377, 529033.5497352450620383 177566.23406805237755179, 529046.80177711113356054 177501.01033127031405456, 529029.92208132648374885 177443.56013859962695278, 529030.81048636778723449 177437.933573338057613, 529046.80177711113356054 177434.08381815909524448, 529055.38969251036178321 177424.31136270478600636, 529129.12731093820184469 177415.4273122918093577, 529252.541577925439924 177354.34946570245665498, 529274.1594339304137975 177332.1393396699859295, 529378.18414042412769049 177463.05533711041789502, 529514.28841154393739998 177579.99861740384949371, 529522.47303623706102371 177587.32366964058019221, 530009.96149630157742649 177853.79645061693736352, 530094.68275518657173961 177878.00252458406612277, 530200.58432879275642335 177862.87372835460701026, 530315.37161932047456503 177998.80604608487919904, 530315.56318013661075383 177999.03289441973902285, 530312.13405959820374846 178036.68039025971665978, 530327.5800858890870586 178073.0888808025047183, 530359.94318859372287989 178068.67573043366428465, 530382.17224571469705552 178064.30687938295886852, 530409.71792252280283719 178051.83336535666603595, 530457.53305962367448956 178047.15579759678803384, 530484.55909291654825211 178044.27656433341326192, 530481.82446864934172481 178176.08545401293667965, 530480.73061894241254777 178201.7909221246954985, 530453.93130112381186336 178202.88477183159557171, 530434.6485230919206515 178208.30226855166256428, 530510.72968812065664679 178204.59099220877396874, 530560.83191874937620014 178250.05412740889005363, 530576.60484320647083223 178299.22853895186563022, 530595.16122492088470608 178402.68036700924858451, 530423.46094173076562583 178433.51663268019910902, 530418.27724980388302356 178499.91296551114646718, 530412.79759553028270602 178422.85328647977439687, 530401.85479763883631676 178248.42200085142394528, 530398.61737529921811074 178112.52069049383862875, 530397.05111636582296342 178067.79433303145924583, 530372.89449547010008246 178077.41707417467841879, 530341.8666145202005282 178078.87150609420496039, 530263.00199223437812179 178102.06698323713499121, 530128.67393126524984837 178193.75180186820216477, 530016.07499924581497908 178268.64121385099133477, 530002.24668997840490192 178279.27173925217357464, 529972.73623576539102942 178260.44271802250295877)</t>
-  </si>
-  <si>
     <t>S6 Battersea Power Station</t>
   </si>
   <si>
-    <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529225.49949584668502212 178821.69789721473352984, 529270.770087662152946 178758.30559268582146615, 529337.70783226401545107 178657.27980173568357714, 529306.5308305585058406 178711.19551833867444657, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529616.82995180855505168 178944.1724078263505362, 529717.92404021020047367 179004.65221903027850203, 529727.10921454057097435 178992.59667772171087563, 529745.47956320131197572 178982.4273775702167768, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529877.37348464445676655 178984.43081074606743641, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530208.48382428544573486 179227.08777841698611155, 530200.14624832582194358 179282.94953734712908044, 530185.47211463667917997 179294.62214369073626585, 530196.47771490353625268 179309.6297804182395339, 530192.14217540447134525 179370.16058188583701849, 530171.13148398592602462 179464.20843871153192595, 530148.2424291695933789 179574.15693386044586077, 530133.06942986708600074 179585.28380001557525247, 530072.88319930084981024 179599.95103267458034679, 530076.42356580472551286 179662.66609645792050287, 530120.93103042512666434 179669.24106282231514342, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530887.07347942178603262 180750.79246864788001403, 530912.25232304760720581 180759.71698828696389683, 531106.04388992069289088 180804.06853912054793909, 531363.93330286943819374 180808.82664637052221224, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531469.1157709649996832 180836.43344559159595519, 531398.75209977955091745 180833.40343104291241616, 531375.85865652305074036 180811.85666091914754361, 531102.54545270372182131 180807.29027070096344687, 530885.10598675487563014 180755.68535418406827375, 530875.96761612175032496 180785.2506709385488648, 530899.35109391843434423 180802.98986099121975712, 530995.84153678070288152 180837.66191427601734176, 530981.05887840350624174 180885.83994180549052544, 530971.57197559298947453 180910.01476331148296595, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530841.84631613304372877 180962.22017306523048319, 530581.45210872450843453 180805.03124651397229172, 530573.32594334834720939 180811.05062827406800352, 530606.733512117061764 180830.61361899445182644, 530580.57139824447222054 180878.84452221845276654, 530580.57139824447222054 180878.84452221845276654)</t>
-  </si>
-  <si>
     <t>S7 Westminster</t>
   </si>
   <si>
@@ -264,6 +267,33 @@
   </si>
   <si>
     <t>LineString (534494.76712749910075217 180197.82926488673547283, 534477.08958587038796395 180204.9261592309048865, 534466.10449469194281846 180201.48237478407099843, 534446.35375012725125998 180105.42193530994700268, 534275.77913797693327069 180170.50961626204662025, 534224.15787377348169684 180196.54468864286900498, 534203.5093680921709165 180212.25550818303599954, 534185.55414576060138643 180210.4599859498848673, 534171.14064759924076498 180237.33092047309037298, 534155.10926930524874479 180232.7692223628400825, 534110.10282780381385237 180227.94574123568600044, 534059.63022310636006296 180244.41244702640688047, 534045.56321658962406218 180253.93444574531167746, 534018.52404629567172378 180285.19719793670810759, 534005.14660858130082488 180295.44406237191287801, 533989.44804280833341181 180338.41282897180644795, 534003.21356487192679197 180354.3808345656725578, 534155.73554933757986873 180422.10720311899785884, 534135.36257668328471482 180462.85314842750085518, 534160.69113728043157607 180481.57425843409146182, 534211.8988793573807925 180382.46249957560212351, 534228.96812671632505953 180379.70939516284852289, 534265.3091049644863233 180416.35643082388560288, 534271.73921295220497996 180462.74348229306633584, 534252.4929513584356755 180455.64950213933479972, 534269.62446292664390057 180472.076978985540336, 534255.40823154035024345 180562.17560434373444878, 534234.92044681450352073 180597.79788426094455644, 534256.13046408852096647 180604.31816759763751179, 534251.89312430669087917 180626.73219362733652815, 534379.78553101746365428 180633.41155169066041708, 534352.34416242560837418 180636.5838860665098764, 534344.23650324332993478 180704.43507658550515771, 534297.84553046221844852 180708.00611733732512221, 534240.14221260114572942 180695.98651926324237138, 534189.34860979067161679 180672.75587819167412817, 534160.54824850801378489 180757.54946950945304707, 534160.5841055567143485 180757.22253176767844707, 534127.8658005315810442 180858.10397226159693673, 534111.99208847992122173 180939.00866548559861258, 534085.5094500295817852 180985.32051877162302844, 534070.93534209730569273 180988.37091345511726104, 534075.68040049390401691 180998.87782847607741132, 534054.99797940440475941 181035.08444935575244017, 534068.56281289900653064 181030.73750628152629361, 534096.52225887367967516 180994.37437144466093741, 534118.50570094562135637 180998.44537923578172922, 534120.13410406210459769 181012.28680572554003447, 534190.96963962737936527 181035.08444935575244017, 534233.56329029169864953 181041.4142344745923765, 534230.7365170813864097 181061.51134635950438678, 534425.65412626438774168 181087.91946370297227986, 534428.68984542321413755 181124.52763081435114145, 534418.41545121860690415 181314.94640340618207119, 534244.43570935411844403 181318.37120147436507978, 534082.24461821641307324 181331.92378598402137868, 534008.65777000458911061 181337.21434369860799052, 534003.03775836550630629 181356.73341751954285428, 533970.61429565714206547 181390.91446260787779465, 533908.72647818853147328 181354.13541679794434458, 533820.00587128894403577 181301.66338870135950856, 533762.7596401305636391 181265.19378197882906534, 533763.82057414436712861 181254.40761950571322814, 533775.00675160356331617 181229.54225989809492603, 533765.23515282932203263 181236.37174127201433294, 533750.68025846313685179 181246.3013364469516091, 533738.92612418869975954 181260.82114937415462919, 533558.01058455463498831 181157.44207860867027193, 533549.5142814606660977 181141.84867783010122366, 533537.31101294630207121 181133.86961764763691463, 533483.72784082207363099 181114.99530462495749816, 533375.88864138023927808 181117.98406295705353841, 533381.80025942670181394 181168.40668747131712735, 533323.37956343777477741 181201.44220008412958123, 533277.55680660111829638 181222.13016911473823711, 533325.81375910399947315 181204.22413798831985332, 533380.40929047460667789 181174.66604775583255105, 533399.53511356632225215 181212.91769393908907659, 533422.13835903815925121 181229.95706360254553147, 533476.03840593271888793 181291.15969749572104774, 533522.51176960719749331 181254.94408223693608306, 533527.5245621653739363 181246.81990119433612563, 533527.00599741796031594 181236.96717099371016957, 533512.83189432229846716 181222.62021298229228705, 533521.10348163370508701 181215.37559709040215239, 533538.7190823903074488 181185.9681870742351748, 533548.10621201666072011 181170.94877967197680846, 533562.65626293770037591 181116.50342783879023045, 533565.78408725361805409 181068.52103992408956401, 533568.11593338451348245 181052.2709871992119588, 533565.98876765870954841 181030.01686012774007395, 533550.6638780701905489 180995.96154993091477081, 533517.88564200571272522 180943.17581912584137172, 533527.8685909277992323 180932.10417117548058741, 533519.96954229823313653 180930.1110331111412961, 533540.88975644903257489 180852.93240523023996502, 533549.08821875147987157 180816.53405966371065006, 533554.74233068409375846 180784.02291605086065829, 533498.69594615150708705 180775.96580654679564759, 533473.25244245456997305 180751.37041963971569203, 533450.91870032052975148 180721.12092079993453808, 533451.20140591717790812 180708.11646335478872061, 533482.01631595019716769 180701.33152903561131097, 533556.93329905800055712 180708.68187454805593006, 533574.10766405356116593 180706.42022977498709224, 533632.91042815323453397 180723.09985997635521926, 533664.85616057284642011 180736.10431742150103673, 533657.22310946369543672 180723.94797676627058536, 533653.26523111085407436 180708.11646335478872061, 533628.66984420374501497 180717.16304244706407189, 533572.27007767534814775 180700.55408864485798404, 533556.72126986051443964 180706.77361177079728805, 533481.23887555941473693 180699.42326625832356513, 533449.2931431399192661 180706.77361177079728805, 533440.52926964417565614 180711.01419572028680705, 533410.70382919942494482 180714.40666287989006378, 533368.01528410776518285 180716.38560205633984879, 533344.26801399048417807 180714.68936847653822042, 533317.41098231042269617 180704.51196699772845022, 533298.32835453760344535 180707.05631736741634086, 533274.0156732271425426 180725.43218114858609624, 533214.36479233752470464 180758.22603035805514082, 533150.04926910332869738 180796.6033151010342408, 533131.95611091877799481 180803.10554382362170145, 533112.94415954523719847 180814.13106209231773391, 533032.09035890805535018 180821.19870200814330019, 533006.17641249333973974 180714.80543799756560475, 532992.55450278345961124 180708.59827885474078357, 533019.41655259137041867 180701.98867611197056249, 533047.67523066280409694 180678.44941610301611945, 533062.18958536896388978 180672.97919573029503226, 533115.1629428390879184 180663.2515109057421796, 533114.02687698940280825 180650.64306823158403859, 532992.54919304675422609 180668.21878358686808497, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531644.05815143184736371 180909.64867640155716799, 531643.0989445325685665 180988.84512792871100828, 531556.3810018397634849 180988.02673437033081427, 531388.22242831636685878 180986.58758923810091801, 531389.17863833182491362 181128.18185803995584138, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531133.39463505509775132 181279.42110962877632119, 531076.29551051347516477 181260.61487964406842366, 531131.04354967980179936 181113.15854730040882714, 531036.5176723989425227 181074.07573265538667329, 530995.61705242155585438 181020.45047535176854581, 530934.72057378862518817 181004.99913002699031495, 530807.47420052578672767 181052.26206866747816093, 530678.41002193070016801 181020.45047535176854581, 530547.98248933651484549 181092.25378597865346819, 530470.12182414066046476 180975.54759959221701138, 530510.45278707984834909 180923.94229928601998836, 530504.58646519773174077 180903.04352758117602207, 530525.67277607112191617 180907.31886370456777513, 530582.29576928459573537 180878.9198528709821403)</t>
+  </si>
+  <si>
+    <t>Initial Draft</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>v1 20230703</t>
+  </si>
+  <si>
+    <t>v2 20230706</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>LineString (530577.23797894886229187 180877.97880632089800201, 530617.74819760688114911 180823.78270298111601733, 530460.08680607296992093 180724.14946249785134569, 530317.89046422939281911 180623.28449239319888875, 530146.54318801360204816 180467.81284240834065713, 530072.77626957895699888 180399.24656015267828479, 530035.55066324456129223 180349.42993991106050089, 529890.48028561775572598 180246.51208710417267866, 529825.74567924335133284 180200.98946149481344037, 529919.54799574031494558 180130.36585574291530065, 529957.12143912480678409 179966.409011882962659, 529911.86251868435647339 179845.57623372576199472, 529906.73886731371749192 179702.96793724340386689, 529926.37953090108931065 179692.72063450215500779, 529923.81770521576981992 179643.19200458613340743, 529919.54799574031494558 179631.23681805469095707, 529921.4103331834776327 179584.29027873513405211, 529930.04384519555605948 179550.71550979930907488, 529930.52348475181497633 179516.66110130725428462, 529941.07555498881265521 179505.62939151405589655, 529912.29718161525670439 179479.72885547782061622, 529902.96647088008467108 179374.86438768959487788, 529800.47367502108681947 179363.00662448359071277, 529739.62031473114620894 179333.45689976593712345, 529740.46023528114892542 179272.14269961469108239, 529760.61832848156336695 179193.19016791306785308, 529641.34961037908215076 179153.71390206224168651, 529568.27652252756524831 179120.95700061158277094, 529550.34316133812535554 179093.66307770530693233, 529617.62970972212497145 178970.86160351810394786, 529616.82995180855505168 178944.1724078263505362, 529593.97022081958130002 178995.33693686561309732, 529513.20162077283021063 179036.94500355634954758, 529526.79745115165133029 179077.07363828388042748, 529564.38437103840988129 179130.25138729959144257, 529513.81095916836056858 179152.52902801893651485, 529512.12165939807891846 179263.45971292795729823, 529524.55590479262173176 179301.70093485678080469, 529448.61280135076958686 179371.58212878205813468, 529385.91768299601972103 179410.16374007728882134, 529333.16189551877323538 179435.02868727562599815, 529281.9714767278637737 179374.53091961363679729, 529220.891999761457555 179328.57588456268422306, 529164.02991525223478675 179367.55040796031244099, 529081.42719402140937746 179391.9821987469040323, 529060.48565906146541238 179415.83228022902039811, 529027.32822870835661888 179419.32253605569712818, 528999.98789139953441918 179308.21605890721548349, 529003.47814722615294158 179297.74529142724350095, 529055.25027532153762877 179270.40495411845040508, 529084.33574054366908967 179209.47090447816299275, 529104.11385689466260374 179164.09757873168564402, 529351.77659326093271375 179225.75876500256708823, 529383.05599977204110473 179235.19909444704535417, 529373.87950731569435447 179284.14038754784269258, 529392.23249222850427032 179227.24613431817851961, 529266.2086624939693138 179192.37546298385132104, 529269.26749331271275878 179176.46954272608854808, 529304.13816464703995734 179174.63424423482501879, 529268.04396098526194692 179166.06951794217457063, 529196.15887484396807849 179120.03240704443305731, 529149.98932790081016719 179107.75948950258316472, 529203.17197058210149407 179134.6430231656995602, 529187.39250517124310136 179174.383899015490897, 529058.81908330414444208 179141.07169425903703086, 529011.0423685876885429 179146.33151606269530021, 528858.21532395936083049 179161.52655682878685184, 528770.55162723187822849 179211.78707628592383116, 528715.03128597105387598 179321.6589095177478157, 528618.60121957084629685 179477.9925020151422359, 528491.34275315469130874 179622.19928313192212954, 528388.04569717741105705 179719.06766801583580673, 528360.57773886946961284 179750.62659883772721514, 528302.13527438452001661 179698.61280544605688192, 528281.73319864494260401 179662.65391637163702399, 528262.13372618111316115 179565.91304187983041629, 528297.16959096642676741 179504.60027850553160533, 528354.10287124256137758 179445.47725668028579094, 528571.1610022954409942 179230.06143178927595727, 528461.67392484133597463 179117.28974201151868328, 528427.73293083056341857 179154.51534834591438994, 528270.83738425537012517 178995.94010165525833145, 528307.81268304819241166 178962.03991528681945056, 528251.02088932693004608 178905.98091890395153314, 528237.09773989859968424 178880.69941073132213205, 528445.48698298842646182 178680.18773902862449177, 528506.68087698111776263 178769.79506966570625082, 528622.96355511201545596 178714.21878967669908889, 528690.51011079095769674 178852.7319798031821847, 528629.80371264915447682 178709.94369121600175276, 528706.32797509559895843 178677.88045276078628376, 528675.97477602458093315 178675.74290353045216762, 528565.03597096959128976 178505.16647494878270663, 528591.54158142581582069 178459.85043126542586833, 528535.96530143683776259 178489.77612049027811736, 528478.67898206354584545 178502.6014158723410219, 528322.21037840214557946 178459.85043126542586833, 528311.95014209649525583 178498.3263174116727896, 528292.28468917729333043 178492.34117956669069827, 528227.69070692639797926 178577.5864321083354298, 528109.89053357648663223 178750.95101042950409465, 528057.58673679200001061 178714.85402391621028073, 528050.95667804463300854 178736.21754654651158489, 528039.90658013243228197 178798.09809485499863513, 528075.26689345156773925 178816.51492470869561657, 528057.36634973983746022 178881.49318986901198514, 528077.50150927738286555 178927.95894264802336693, 527957.20683819404803216 178903.17720783254480921, 527893.18735658738296479 178892.33519885077839717, 527838.97731167858000845 178884.59090672095771879, 527827.61901655478868634 178890.78634042482008226, 527761.01810423820279539 178875.29775616514962167, 527777.55729742196854204 178801.08342777710640803, 527839.85880704678129405 178661.95543657644884661, 527875.91507322294637561 178584.04074644856154919, 527702.52480672812089324 178435.08524715233943425, 527673.89863282348960638 178393.55225022041122429)</t>
+  </si>
+  <si>
+    <t>LineString (532680.96280913078226149 178677.48286417848430574, 532646.72988178418017924 178686.93224038934567943, 532644.91513582807965577 178705.68461526944884099, 532577.46707779157441109 178826.97013667138526216, 532558.10978759278077632 178818.50132220939849503, 532477.21695213438943028 178782.04142910346854478, 532465.16113808494992554 178762.56665256191627122, 532448.46847247786354274 178772.14947911410126835, 532425.90246156463399529 178760.71191193890990689, 532423.12035063013900071 178744.32836976903490722, 532352.79476867453195155 178710.47935339916148223, 532245.37437425879761577 178647.41817221697419882, 532184.94074229244142771 178616.19670506301918067, 532251.30818086618091911 178452.11467546166386455, 532511.10399071127176285 178585.03346189408330247, 532598.70955449633765966 178413.85017633717507124, 532702.58256901206914335 178176.74428570797317661, 532815.09900265594478697 177890.48924129054648802, 532856.91221495741046965 177792.91708755856961943, 532858.8989350259071216 177769.61827948209247552, 532770.30928106070496142 177726.3168125337397214, 532588.16317295876797289 177673.66873071744339541, 532472.21096532221417874 177646.21587158855982125, 532425.64025696949101985 177642.10992637852905318, 532411.25822669372428209 177649.51064796402351931, 532407.54009782173670828 177671.5538405618572142, 532404.75150116789154708 177727.19298332382459193, 532429.18491946905851364 177794.11930301843676716, 532358.00930963514838368 177800.49323822744190693, 532344.59748763276729733 177875.45337209175340831, 532340.61377812712453306 177908.3853706716618035, 532327.99869802594184875 177961.36870709658251144, 532247.2621853785822168 177940.65341766728670336, 532213.93181584810372442 177940.5206273504300043, 532181.53097853565122932 177966.54752945387735963, 532131.07065813092049211 178059.50075125196599402, 531992.96872860239818692 177958.58011044265003875, 531978.40126691607292742 177969.69867078488459811, 531975.51999578601680696 177976.24701426242245361, 531956.66076657059602439 177991.70110486945486628, 531930.72932639950886369 178011.6080690412200056, 531893.66570231656078249 178019.07318060554098338, 531849.13696666923351586 178060.9825788619054947, 531859.09044875507242978 178130.13308598485309631, 531859.16702702990733087 178134.34492127480916679, 531819.8686971872812137 178155.9232769338414073, 531814.8917296277359128 178147.84576965900487266, 531807.24648775579407811 178147.84155853773700073, 531681.84718574595171958 177939.97077090424136259, 531528.1577946882462129 178035.11182251141872257, 531487.49922562530264258 177974.93714029833790846, 531424.07185788720380515 178019.66156626751762815, 531347.63374804891645908 177870.85120349729550071, 531277.70100926072336733 177896.05951631630887277, 531112.62721886532381177 177774.89698050887091085, 531123.19844682177063078 177739.93061111477436498, 531112.62721886532381177 177703.33789895815425552, 531087.41890604631043971 177667.55835818278137594, 530999.59639687044546008 177661.05298713271622546, 530915.83974460093304515 177696.01935652681277134, 530878.43386106321122497 177734.03511860055732541, 530837.77529200038406998 177695.81606368144275621, 530831.67650664085522294 177668.57482240931130946, 530831.67650664085522294 177655.15749461855739355, 530794.67720879369881004 177645.80602373406873085, 530835.33577785652596503 177653.53115185603382997, 530871.92849001311697066 177554.32424334256211296, 531069.12254996818955988 177399.4150952129275538, 531020.61008431122172624 177322.7039789414848201, 531091.09575783216860145 177289.02749048147234134, 531153.74968985083978623 177288.24431633122731, 531216.40362186951097101 177277.2798782279714942, 531239.84660494257695973 177317.72826233872910962, 531211.70457696809899062 177219.32499111071228981, 531201.52331301511730999 177187.4106444887293037, 530917.23109648050740361 177149.81828527752077207, 530896.22850016714073718 177112.81085585197433829, 530778.53778894036076963 176970.21642869058996439, 530805.62878007220569998 176973.21251439995830879, 530899.60967810009606183 176912.9081048319931142, 530892.56111074797809124 176812.07443298946600407, 530912.92363865405786783 176700.86370365635957569, 530991.2410536773968488 176720.63885094976285473, 531176.07015313243027776 176705.75854209534008987, 531181.01259320287499577 176679.19053713156608865, 531173.18175361305475235 176619.08758663863409311, 530892.20482224225997925 176554.68621974403504282, 530879.22067569091450423 176529.75665836548432708, 530895.8881946955807507 176444.7932273649785202, 530920.42121049202978611 176275.10653477313462645, 530798.92437035741750151 176217.86283124817418866, 530745.23294417129363865 176147.84827024937840179, 530808.30562182224821299 176214.79391414625570178, 530927.40622285439167172 176269.47334575466811657, 530985.69952494266908616 176293.35631588246906176, 531191.53301749157253653 176335.15151360613526776, 531198.76075845130253583 176235.22013859765138477, 531207.48642726987600327 176156.30002914459328167, 531185.2742347844177857 176156.30002914459328167, 531209.55267773370724171 176148.55158990548807196, 531188.94265151466242969 175949.80426446883939207, 531154.94696310814470053 175823.53456467346404679, 531066.20655180979520082 175503.10660128630115651, 530998.72868066909722984 175231.84770217089680955, 531029.01404346199706197 175153.91027290970669128, 531021.65302618476562202 175139.83394162519834936, 531029.40146542387083173 175082.75377256359206513, 531032.75912242755293846 175056.73193078552139923, 531026.30208972818218172 175037.10255137970671058, 530966.8973888949258253 175050.27489808623795398, 530928.21976302622351795 175062.67240086884703487, 531062.91346513316966593 175558.95993413514224812, 530985.123753986437805 175577.28249899740330875)</t>
+  </si>
+  <si>
+    <t>LineString (530319.24822289927396923 177532.86330300656845793, 530283.00367995072156191 177511.02849130801041611, 530184.84259889076929539 177499.21280562478932552, 530113.65853050712030381 177494.05278513085795566, 530069.67329359170980752 177299.41811178030911833, 530023.48879483062773943 177179.55834118591155857, 530191.73232603189535439 177132.27421150187728927, 530094.96480481803882867 176769.12109921933733858, 529881.66167348786257207 176830.25587819798965938, 529842.9543123907642439 176768.22780633534421213, 529745.09127103956416249 176816.94227156793931499, 529690.3932994834613055 176733.5929815776180476, 529531.50871543935500085 176823.45393484842497855, 529513.38458597532007843 176824.64773978322045878, 529499.05892675823997706 176851.56261467593139969, 529271.26506909728050232 177111.75961302706855349, 529136.28157614718656987 177252.8598545910208486, 529045.9358032428426668 177206.80840826532221399, 528896.89055745047517121 177069.65020661591552198, 528719.06074102083221078 177058.62250209698686376, 528714.32951614784542471 177068.97205650678370148, 528710.55932132713496685 177045.83340986201073974, 528687.79030162561684847 177026.31710726069286466, 528651.71471196867059916 177031.34403368830680847, 528597.30562592856585979 177022.47298705135472119, 528633.38121558562852442 177062.39269691769732162, 528645.80068087729159743 177093.14565859251888469, 528659.99435549648478627 177110.29634875731426291, 528636.63393268582876772 177251.93739339418243617, 528627.29656225664075464 177420.25810052070301026, 528532.66370314673986286 177925.4865684756077826, 528554.77845204086042941 177948.92160088589298539, 528617.49191905430052429 177943.97053770063212141, 528827.74706898862496018 177946.61110473275766708, 528860.91919232998043299 177944.30060857962234877, 529088.99816973123233765 177901.39139430731302127, 529260.80006226000841707 177863.10317234124522656, 529404.71096551173832268 177897.76061463812948205, 529417.25365891447290778 177885.54799211447243579, 529376.32486991619225591 177854.85140036582015455, 529293.80715016182512045 177856.50175476088770665, 529251.55807764746714383 177854.19125860778149217, 529020.1783914560219273 177904.03196133946767077, 528852.00727859640028328 177934.72855308811995201, 528754.63636928622145206 177937.03904924125527032, 528579.45125024754088372 177935.38869484615861438, 528555.02600520011037588 177929.77748990285908803, 528554.69593432114925236 177897.76061463812948205, 528587.94057327986229211 177658.03592232000664808, 528599.48983881680760533 177670.76972791197476909, 528612.2236444087466225 177688.53782873795717023, 528710.54046897927764803 177690.61077383431256749, 528765.9177165535511449 177685.87261361404671334, 528789.90465266862884164 177690.01850380678661168, 528858.015705834957771 177683.20739849016536027, 528903.546464201528579 177615.09634532386553474, 528963.06960196862928569 177621.01904559918330051, 529007.48985403357073665 177597.03210948410560377, 529033.5497352450620383 177566.23406805237755179, 529046.80177711113356054 177501.01033127031405456, 529029.92208132648374885 177443.56013859962695278, 529030.81048636778723449 177437.933573338057613, 529046.80177711113356054 177434.08381815909524448, 529055.38969251036178321 177424.31136270478600636, 529129.12731093820184469 177415.4273122918093577, 529252.541577925439924 177354.34946570245665498, 529274.1594339304137975 177332.1393396699859295, 529378.18414042412769049 177463.05533711041789502, 529514.28841154393739998 177579.99861740384949371, 529522.47303623706102371 177587.32366964058019221, 530009.96149630157742649 177853.79645061693736352, 530094.68275518657173961 177878.00252458406612277, 530200.58432879275642335 177862.87372835460701026, 530315.37161932047456503 177998.80604608487919904, 530315.56318013661075383 177999.03289441973902285, 530312.13405959820374846 178036.68039025971665978, 530327.5800858890870586 178073.0888808025047183, 530359.94318859372287989 178068.67573043366428465, 530382.17224571469705552 178064.30687938295886852, 530409.71792252280283719 178051.83336535666603595, 530457.53305962367448956 178047.15579759678803384, 530484.55909291654825211 178044.27656433341326192, 530481.82446864934172481 178176.08545401293667965, 530480.73061894241254777 178201.7909221246954985, 530453.93130112381186336 178202.88477183159557171, 530434.6485230919206515 178208.30226855166256428, 530510.72968812065664679 178204.59099220877396874, 530560.83191874937620014 178250.05412740889005363, 530576.60484320647083223 178299.22853895186563022, 530595.16122492088470608 178402.68036700924858451, 530423.46094173076562583 178433.51663268019910902, 530418.27724980388302356 178499.91296551114646718, 530412.79759553028270602 178422.85328647977439687, 530401.85479763883631676 178248.42200085142394528, 530398.61737529921811074 178112.52069049383862875, 530397.05111636582296342 178067.79433303145924583, 530372.89449547010008246 178077.41707417467841879, 530341.8666145202005282 178078.87150609420496039, 530263.00199223437812179 178102.06698323713499121, 530128.67393126524984837 178193.75180186820216477, 530016.07499924581497908 178268.64121385099133477, 530002.24668997840490192 178279.27173925217357464, 529972.73623576539102942 178260.44271802250295877)</t>
+  </si>
+  <si>
+    <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529225.49949584668502212 178821.69789721473352984, 529270.770087662152946 178758.30559268582146615, 529337.70783226401545107 178657.27980173568357714, 529306.5308305585058406 178711.19551833867444657, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529684.84245063865091652 178849.14101684212801047, 529657.52491406002081931 178773.00064893162925728, 529696.44831980823073536 178755.84746999081107788, 529755.07401005295105278 178759.51157563112792559, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529877.37348464445676655 178984.43081074606743641, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530208.48382428544573486 179227.08777841698611155, 530200.14624832582194358 179282.94953734712908044, 530185.47211463667917997 179294.62214369073626585, 530196.47771490353625268 179309.6297804182395339, 530192.14217540447134525 179370.16058188583701849, 530171.13148398592602462 179464.20843871153192595, 530148.2424291695933789 179574.15693386044586077, 530133.06942986708600074 179585.28380001557525247, 530072.88319930084981024 179599.95103267458034679, 530076.42356580472551286 179662.66609645792050287, 530120.93103042512666434 179669.24106282231514342, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530887.07347942178603262 180750.79246864788001403, 530912.25232304760720581 180759.71698828696389683, 531106.04388992069289088 180804.06853912054793909, 531363.93330286943819374 180808.82664637052221224, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531469.1157709649996832 180836.43344559159595519, 531398.75209977955091745 180833.40343104291241616, 531375.85865652305074036 180811.85666091914754361, 531102.54545270372182131 180807.29027070096344687, 530885.10598675487563014 180755.68535418406827375, 530875.96761612175032496 180785.2506709385488648, 530899.35109391843434423 180802.98986099121975712, 530995.84153678070288152 180837.66191427601734176, 530981.05887840350624174 180885.83994180549052544, 530971.57197559298947453 180910.01476331148296595, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530841.84631613304372877 180962.22017306523048319, 530822.39289369573816657 180996.15798742827610113, 530834.18258258642163128 181050.89582870650338009, 530803.86623972468078136 181055.9485525168129243, 530670.81117938680108637 181018.05312393954955041, 530540.28248095407616347 181088.79125728373765014, 530466.175865069613792 180976.78921282212832011, 530516.46695041528437287 180923.52303003016277216, 530508.37677010952029377 180901.19154505711048841, 530529.67934027465526015 180911.15398420437122695, 530580.2603085950249806 180875.74680006815469824, 530580.2603085950249806 180875.74680006815469824)</t>
   </si>
 </sst>
 </file>
@@ -624,15 +654,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B222A62-E78F-E448-B4C7-291D829E11A4}">
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,10 +681,22 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -666,12 +708,24 @@
         <v>10387.633383793</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>76.3</v>
+      </c>
+      <c r="K2">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="L2">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -683,12 +737,24 @@
         <v>10135.874484428899</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>64.7</v>
+      </c>
+      <c r="K3">
+        <v>70.7</v>
+      </c>
+      <c r="L3">
+        <v>70.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -700,14 +766,26 @@
         <v>10889.6786160784</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="K4">
+        <v>72.7</v>
+      </c>
+      <c r="L4">
+        <v>73</v>
+      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -719,16 +797,26 @@
         <v>10373.492909434601</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>70.2</v>
+      </c>
+      <c r="K5">
+        <v>72.2</v>
+      </c>
+      <c r="L5">
+        <v>72.5</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -740,16 +828,28 @@
         <v>10047.75961035</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="K6">
+        <v>71.8</v>
+      </c>
+      <c r="L6">
+        <v>71.8</v>
+      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -761,16 +861,31 @@
         <v>10347.2332512455</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7">
+        <f>AVERAGE(J2:J6)</f>
+        <v>71.88</v>
+      </c>
+      <c r="K7">
+        <f>AVERAGE(K2:K6)</f>
+        <v>71.960000000000008</v>
+      </c>
+      <c r="L7">
+        <f>AVERAGE(L2:L6)</f>
+        <v>72.080000000000013</v>
+      </c>
+      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -782,14 +897,14 @@
         <v>10260.484070139</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
         <v>162</v>
@@ -798,16 +913,16 @@
         <f>SUM(D2:D8)</f>
         <v>72442.156325469405</v>
       </c>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -826,14 +941,14 @@
       <c r="F11" t="s">
         <v>5</v>
       </c>
+      <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -845,12 +960,12 @@
         <v>10396.40561819</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -862,12 +977,12 @@
         <v>10050.3586120912</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -879,12 +994,12 @@
         <v>10040.0307021154</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -896,12 +1011,12 @@
         <v>10328.5537327765</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -913,12 +1028,12 @@
         <v>10468.1416395172</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -930,12 +1045,12 @@
         <v>10473.764647815</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -947,7 +1062,7 @@
         <v>8970.4012079409804</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -982,7 +1097,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -991,15 +1106,15 @@
         <v>24</v>
       </c>
       <c r="D22">
-        <v>10130.800646047501</v>
+        <v>10414.387040997</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1011,12 +1126,12 @@
         <v>10240.7485129782</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1028,12 +1143,12 @@
         <v>10322.5536861458</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -1045,12 +1160,12 @@
         <v>10086.2297192444</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -1062,12 +1177,12 @@
         <v>10197.200793621199</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -1079,12 +1194,12 @@
         <v>10503.889210624</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B28">
         <v>7</v>
@@ -1096,7 +1211,7 @@
         <v>11221.3477004749</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1106,7 +1221,7 @@
       </c>
       <c r="D29" s="1">
         <f>SUM(D22:D28)</f>
-        <v>72702.770269136003</v>
+        <v>72986.356664085499</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1131,7 +1246,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1143,12 +1258,12 @@
         <v>10029.895474594299</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1160,12 +1275,12 @@
         <v>10369.6417108937</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1177,12 +1292,12 @@
         <v>10147.9934740517</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -1191,15 +1306,15 @@
         <v>16</v>
       </c>
       <c r="D35">
-        <v>10428.3463445986</v>
+        <v>10587.4904613938</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1211,12 +1326,12 @@
         <v>10263.725203550401</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -1225,15 +1340,15 @@
         <v>17</v>
       </c>
       <c r="D37">
-        <v>10123.7166457228</v>
+        <v>10124.7844637862</v>
       </c>
       <c r="E37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B38">
         <v>7</v>
@@ -1242,10 +1357,10 @@
         <v>28</v>
       </c>
       <c r="D38">
-        <v>10830.2986615384</v>
+        <v>11007.39364301</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1255,7 +1370,7 @@
       </c>
       <c r="D39" s="1">
         <f>SUM(D32:D38)</f>
-        <v>72193.617514949903</v>
+        <v>72530.924431280087</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1280,7 +1395,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1292,12 +1407,12 @@
         <v>10275.7603419072</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1309,12 +1424,12 @@
         <v>10176.9320304295</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -1326,12 +1441,12 @@
         <v>10601.066552067599</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -1343,12 +1458,12 @@
         <v>11162.543933425801</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -1360,12 +1475,12 @@
         <v>10261.913579423001</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B47">
         <v>6</v>
@@ -1377,12 +1492,12 @@
         <v>10185.2940832533</v>
       </c>
       <c r="E47" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B48">
         <v>7</v>
@@ -1394,7 +1509,7 @@
         <v>9096.5507719182897</v>
       </c>
       <c r="E48" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix minor numbering error. No routing changes.
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Documents/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C5AD75-5DB4-5C47-9368-89836ECFD5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0662FEB3-670A-C847-9738-33F5CC3E2929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="10140" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
+    <workbookView xWindow="2460" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529225.49949584668502212 178821.69789721473352984, 529270.770087662152946 178758.30559268582146615, 529337.70783226401545107 178657.27980173568357714, 529306.5308305585058406 178711.19551833867444657, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529684.84245063865091652 178849.14101684212801047, 529657.52491406002081931 178773.00064893162925728, 529696.44831980823073536 178755.84746999081107788, 529755.07401005295105278 178759.51157563112792559, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529877.37348464445676655 178984.43081074606743641, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530208.48382428544573486 179227.08777841698611155, 530200.14624832582194358 179282.94953734712908044, 530185.47211463667917997 179294.62214369073626585, 530196.47771490353625268 179309.6297804182395339, 530192.14217540447134525 179370.16058188583701849, 530171.13148398592602462 179464.20843871153192595, 530148.2424291695933789 179574.15693386044586077, 530133.06942986708600074 179585.28380001557525247, 530072.88319930084981024 179599.95103267458034679, 530076.42356580472551286 179662.66609645792050287, 530120.93103042512666434 179669.24106282231514342, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530887.07347942178603262 180750.79246864788001403, 530912.25232304760720581 180759.71698828696389683, 531106.04388992069289088 180804.06853912054793909, 531363.93330286943819374 180808.82664637052221224, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531469.1157709649996832 180836.43344559159595519, 531398.75209977955091745 180833.40343104291241616, 531375.85865652305074036 180811.85666091914754361, 531102.54545270372182131 180807.29027070096344687, 530885.10598675487563014 180755.68535418406827375, 530875.96761612175032496 180785.2506709385488648, 530899.35109391843434423 180802.98986099121975712, 530995.84153678070288152 180837.66191427601734176, 530981.05887840350624174 180885.83994180549052544, 530971.57197559298947453 180910.01476331148296595, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530841.84631613304372877 180962.22017306523048319, 530822.39289369573816657 180996.15798742827610113, 530834.18258258642163128 181050.89582870650338009, 530803.86623972468078136 181055.9485525168129243, 530670.81117938680108637 181018.05312393954955041, 530540.28248095407616347 181088.79125728373765014, 530466.175865069613792 180976.78921282212832011, 530516.46695041528437287 180923.52303003016277216, 530508.37677010952029377 180901.19154505711048841, 530529.67934027465526015 180911.15398420437122695, 530580.2603085950249806 180875.74680006815469824, 530580.2603085950249806 180875.74680006815469824)</t>
+  </si>
+  <si>
+    <t>OSRM Raw</t>
   </si>
 </sst>
 </file>
@@ -654,15 +657,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B222A62-E78F-E448-B4C7-291D829E11A4}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,8 +696,11 @@
       <c r="L1" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -722,8 +728,11 @@
       <c r="L2">
         <v>72.400000000000006</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>77.400000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -751,8 +760,11 @@
       <c r="L3">
         <v>70.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -780,10 +792,13 @@
       <c r="L4">
         <v>73</v>
       </c>
+      <c r="M4">
+        <v>86.2</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -811,10 +826,11 @@
       <c r="L5">
         <v>72.5</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -842,12 +858,13 @@
       <c r="L6">
         <v>71.8</v>
       </c>
+      <c r="M6">
+        <v>79.5</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -878,12 +895,14 @@
         <f>AVERAGE(L2:L6)</f>
         <v>72.080000000000013</v>
       </c>
+      <c r="M7">
+        <f>AVERAGE(M2:M6)</f>
+        <v>80.16</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -901,10 +920,8 @@
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
         <v>162</v>
@@ -915,14 +932,12 @@
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -943,10 +958,8 @@
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -963,7 +976,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -980,7 +993,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -997,7 +1010,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1014,7 +1027,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1303,7 +1316,7 @@
         <v>4</v>
       </c>
       <c r="C35">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D35">
         <v>10587.4904613938</v>
@@ -1354,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D38">
         <v>11007.39364301</v>

</xml_diff>

<commit_message>
ATD2 V3 (Friday evening) - 2 more removals. Plus TSP based rerouting.
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Documents/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0662FEB3-670A-C847-9738-33F5CC3E2929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4601FF9A-9B59-3B4E-BA1C-E17141DD65ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>W5 Notting Hill</t>
   </si>
   <si>
-    <t>LineString (525813.62879803299438208 181444.3455462628044188, 525938.4894992244662717 181490.10516775862197392, 525950.2033640209119767 181472.33594733368954621, 525943.13234854943584651 181373.34173073348938487, 525962.06789837975520641 181288.70267443344346248, 526084.9407700706506148 181347.92177145567256957, 526141.85119377286173403 181374.63645114144310355, 526247.90762806567363441 181264.37710280925966799, 526196.01242155989166349 181214.6880689833778888, 526166.16735107859130949 181192.64317541586933658, 526187.1327016269788146 181205.25580382536281832, 526289.24206442979630083 181085.57761354133253917, 526304.73383384314365685 181090.14411224401555955, 526312.97320597257930785 181086.63195823784917593, 526405.64829471055418253 180975.33631497254827991, 526406.50096082710660994 180959.79253581800730899, 526425.68278948625084013 180965.84515120310243219, 526594.1189202640671283 181126.22767907357774675, 526481.37747424189001322 181247.68218424991937354, 526436.7998225896153599 181292.98168183141387999, 526364.50886605237610638 181370.49790682113962248, 526315.65099693823140115 181327.24125062092207372, 526174.19306422164663672 181474.26841948175569996, 526118.98830004595220089 181451.55415104021085426, 526093.47386830300092697 181427.99858194089028984, 526147.53385363647248596 181372.97566176933469251, 526117.64916966739110649 181356.75464216282125562, 525896.63604345871135592 181252.18492163851624355, 525804.47871884633786976 181202.92109834335860796, 525674.52415049879346043 181177.43981043208623305, 525808.02069279435090721 181198.8358115378941875, 525864.59372291236650199 181229.60359984767274, 525899.00071198993828148 181072.78713039786089212, 525914.79815168655477464 180998.59706019930308685, 526038.20014135900419205 181021.09393767311121337, 526034.23010415781755 181034.3273950106522534, 526110.653320282115601 181059.4709639519569464, 526191.52032900520134717 180703.23102329159155488, 526415.88937359000556171 180762.15805877896491438, 526543.08072616113349795 180799.48524305276805535, 526566.20990454801358283 180735.24582871556049213, 526773.2086006454192102 180792.2867543384199962, 526781.81037810200359672 180804.0292009754339233, 526876.82089265179820359 180898.32528518006438389, 526893.50918447971343994 180930.32612565089948475, 526924.34248529304750264 180944.76673002715688199, 526972.18770328722894192 180987.68083861388731748, 526822.07183925563003868 181156.94281222127028741, 526922.36106670461595058 181052.43190333811799064, 527056.51731256174389273 181181.75928882521111518, 527072.0604500574991107 181194.33582109218696132, 527105.36620856204535812 181208.59860649338224903, 527134.84456199198029935 181207.65720116312149912, 527141.67895267263520509 181237.20603345840936527, 527126.8461934340884909 181257.45282692171167582, 527004.39505052170716226 181384.53058732440695167, 526985.91159781138412654 181369.18001979179098271, 526928.28958167461678386 181432.30053406039951369, 526997.63798668433446437 181498.45083301386330277, 526991.12956032424699515 181511.24325723896618001, 526678.53803907369729131 181414.39224837144138291, 526667.31783640081994236 181399.6772284725739155, 526656.64944697415921837 181395.44666025164769962, 526645.98105754749849439 181403.90779669350013137, 526619.08016179490368813 181431.82035006419755518, 526630.85217771399766207 181442.85661498832632788, 526625.70192074938677251 181459.04313687709509395, 526679.9176372914807871 181475.29189143585972488, 526706.84188712364993989 181479.03970802802359685, 526704.67241586744785309 181483.81254479169729166, 526684.71328031027223915 181478.02728810845292173, 526671.31848243589047343 181522.68559793970780447, 526666.90397646627388895 181521.94984694477170706, 526673.52573542075697333 181504.29182306613074616, 526671.31848243589047343 181502.8203210762294475, 526664.32884798396844417 181521.58197144727455452, 526672.42210892832372338 181534.0897383613337297, 526664.69672348140738904 181552.11563773744273931, 526615.76928231760393828 181537.7684933360433206, 526607.67602137324865907 181540.71149731581681408, 526667.6397274611517787 181562.3241827923047822, 526633.51603102358058095 181673.21107818573364057, 526634.14788983517792076 181721.54827727310475893, 526750.40991116955410689 181719.96863024411140941, 526763.6789462132146582 181717.44119499769294634, 527047.06762321561109275 181716.49340678029693663, 527075.50126973760779947 181704.80401876571704634, 527090.57778861722908914 181720.29356452525826171, 527188.46480982354842126 181748.64203353796619922, 527263.33384336996823549 181773.11378883954603225, 527341.77672236878424883 181800.06906386234913953, 527457.35124988225288689 181828.41753287505707704, 527478.70498486375436187 181813.3316481038054917, 527501.72297252365387976 181756.39241547140409239, 527552.19019862043205649 181634.29178817657520995, 527576.96563832846004516 181539.9116470152803231, 527502.86533335037529469 181515.28355731410556473, 527511.7228042078204453 181503.83365596178919077, 527545.64043651556130499 181469.26791603030869737, 527474.56463378143962473 181422.82020299739087932, 527381.22077847318723798 181367.63679676040192135, 527435.71565961930900812 181312.86944120863336138, 527464.59794662659987807 181334.12244485557312146, 527517.74514231248758733 181280.34209467822802253, 527383.21302771475166082 181171.51255586085608229, 527413.66733776684850454 181131.1336214438197203, 527429.41461164352949709 181120.02025737526128069, 527508.38860920432489365 181143.15408535901224241, 527552.0115922475233674 181044.38326500484254211, 527617.38904907600954175 181065.27134975808439776, 527665.90049312810879201 181080.65138910515815951, 527880.71712640451733023 181139.95635454953298904, 527892.84981061285361648 181124.42310436989646405, 527898.57802572846412659 181147.61365187869523652, 528147.61506407021079212 181224.24573191639501601, 528390.99835214088670909 181293.8688241028576158, 528368.25337566784583032 181399.05101017700508237, 528327.16320699045900255 181385.98296514025423676, 528308.22175984270870686 181356.13857025865581818, 528284.80718849156983197 181340.66114173838286661, 528256.63033144187647849 181343.0422845876601059, 528236.78747436462435871 181362.88514166491222568, 528124.47690330736804754 181327.56485606741625816, 528078.36375248804688454 181310.06427945720497519)</t>
-  </si>
-  <si>
     <t>W6 Paddington</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>P5 Fulham</t>
   </si>
   <si>
-    <t>LineString (525578.32314166694413871 175779.89375719579402357, 525779.26792031072545797 175913.87857735189027153, 525794.67906692263204604 175913.40021600711042993, 525796.36541037389542907 175924.88107120373751968, 525831.44916197401471436 175948.5820945069717709, 525842.88386619929224253 175956.48243560802075081, 525966.89843111461959779 175827.58213343276293017, 526037.0428866392467171 175909.39836246441700496, 526083.99901098641566932 175909.39836246441700496, 526183.90565853379666805 175950.36008795883390121, 526213.87765279808081686 175990.32274697776301764, 526258.58368871151469648 176103.28294610444572754, 526151.85186089854687452 176147.91625591710908338, 526151.49614943633787334 176179.64869351152447052, 526047.38884781103115529 176231.98070609322167002, 526018.99594736774452031 176239.218112088565249, 526012.31526491045951843 176231.42398255510488525, 525961.23868289159145206 176229.001861541881226, 525788.46569891297258437 176403.76074188807979226, 525739.81123790750280023 176436.52803195299929939, 525728.0358450491912663 176477.41611387868761085, 525702.36593637219630182 176520.02743093523895368, 525681.16035963909234852 176514.67023260265705176, 525672.11343565175775439 176513.5143718154868111, 525598.1237177683506161 176794.07800558168673888, 525590.47065528121311218 176803.15163323399610817, 525576.05627165164332837 176800.20250201458111405, 525603.30556521995458752 176824.95719950424972922, 525545.77949344262015074 176885.87943373149028048, 525467.20725123130250722 176931.41561955848010257, 525439.5283931796438992 176951.95154650005861185, 525403.81373762898147106 177049.27398287542746402, 525403.81373762898147106 177092.13156953614088707, 525397.56367290765047073 177140.34635452943621203, 525389.52787540876306593 177153.73935036090551876, 525384.84032686776481569 177171.15024494181852788, 525401.57936285785399377 177193.54199610272189602, 525396.49806739354971796 177201.56509420418296941, 525394.6260111698647961 177214.66948776991921477, 525487.42651254346128553 177227.50644473225111142, 525492.50780800764914602 177223.22745907813077793, 525498.9792741967830807 177209.83568196554551832, 525499.70685131091158837 177208.33006480569019914, 525546.48938673955854028 177091.50102327833883464, 525607.1780920778401196 177105.30195335522876121, 525641.23937251162715256 177033.56127417489187792, 525704.87392115953844041 176980.53248363500460982, 525742.65693441918119788 176954.01808836506097578, 525749.9179498142329976 176950.09361684083705768, 525759.91741443739738315 176949.90844157003448345, 525789.17510722379665822 176925.28013055364135653, 525823.06218178023118526 176907.87365509843220934, 525834.31157948146574199 176917.87311972162569873, 525840.02393209061119705 176917.83761663141194731, 525839.83007433160673827 176904.55402936117025092, 525831.35577882663346827 176898.87676776724401861, 525816.50067409395705909 176887.31365200405707583, 525759.91843862924724817 176830.72846091576502658, 525971.4164017754374072 176713.56057522911578417, 525990.28241726732812822 176704.62404157503624447, 525990.28241726732812822 176695.68750792095670477, 526044.89456737553700805 176673.8426478776964359, 526231.32058888114988804 176565.61129584512673318, 526246.21481163799762726 176558.66065855862689205, 526279.02310593228321522 176632.42519633183837868, 526283.16126619779970497 176641.72923013736726716, 526326.25483707862440497 176694.1716895958816167, 526240.12421508901752532 176797.52843598343315534, 526248.73727728798985481 176850.9294216169801075, 526278.02168876444920897 176885.38167041284032166, 526272.85385144501924515 176930.16959384744404815, 526251.69148790801409632 176959.08371336333220825, 526325.95375438174232841 177013.98570174560882151, 526319.56678607675712556 177036.69492238553357311, 526331.39291572826914489 177017.30782459620968439, 526465.45469694142229855 177118.89621701225405559, 526531.37082942517008632 177192.56718861166154966, 526549.98244330286979675 177194.89364034638856538, 526607.62827024597208947 177274.30958925650338642, 526607.62827024597208947 177288.8285534702881705, 526641.02188793767709285 177312.0588962123147212, 526727.77269911498297006 177419.49923139426391572, 526755.35873112105764449 177438.37388487218413502, 526797.46372734103351831 177454.34474550731829368, 526929.58630168635863811 177497.90163814864354208, 527031.94499939354136586 177545.81422005410422571, 527131.79582655231934041 177579.02292893503908999, 527156.87407868099398911 177613.12935183010995388, 527095.68314348696731031 177730.49557179247494787, 527136.81147697800770402 177756.57695400633383542, 527102.70505408302415162 177810.74597860436188057, 527125.77704604144673795 177823.78666971129132435, 527048.53602948493789881 177964.22488163207890466, 527026.87337462871801108 177950.0097189677762799, 526946.35645452653989196 177896.54735731321852654, 526834.03755092830397189 177803.64159754675347358, 526824.94913852983154356 177797.93363960826536641, 526784.72778616880532354 177851.09168424911331385, 526706.87674400769174099 177973.44731176737695932, 526634.32416085619479418 177927.33338179817656055, 526512.58338573749642819 178040.46622332264087163, 526519.31304050667677075 178017.6128924343502149, 526371.94527612451929599 177875.96814802818698809, 526400.17261434311512858 177844.21239253226667643, 526508.84786648489534855 177733.42009002406848595, 526626.69700354768428952 177566.1731110785913188, 526460.89075782534200698 177464.74579751139390282, 526454.46574496384710073 177446.82339321335894056, 526426.39858351601287723 177448.17602750001242384, 526367.89715061872266233 177423.8286103404534515, 526275.22880457423161715 177381.16762834310065955, 526209.74243830097839236 177335.0968178995535709, 526189.01057360135018826 177332.13512294244719669, 526113.32281358691398054 177425.59305269937613048, 526030.51900099997874349 177531.11546100955456495, 526193.47004954458680004 177728.49897465461981483, 526270.35714144632220268 177793.47398189548403025, 526039.15440734755247831 178025.89499738009180874, 525946.02356363565195352 178113.06979876160039566, 525928.76722545002121478 178136.49907633577822708, 526006.53529266326222569 178197.5254068571375683, 525909.86526466929353774 178347.12092503774329089, 526031.45418893126770854 178419.44031195042771287, 525979.57233337289653718 178520.5659626150445547, 525986.60716124519240111 178488.0298837055452168, 525783.34360698144882917 178376.24297001594095491, 525732.83573407854419202 178350.98903356451774016, 525778.65115257329307497 178377.8639997206046246, 525731.46603016031440347 178455.16984871673048474, 525568.58136916358489543 178364.83045690337894484, 525496.7204893120797351 178324.45148632011841983, 525454.97274006495717913 178276.20203841981128789, 525308.00674845476169139 178392.76418910655775107, 525327.85414873412810266 178420.77501689142081887)</t>
-  </si>
-  <si>
     <t>P6 Chelsea</t>
   </si>
   <si>
@@ -146,15 +140,9 @@
     <t>S1 Lambeth</t>
   </si>
   <si>
-    <t>LineString (531565.23039256664924324 178567.62021348648704588, 531600.88228947878815234 178584.2162747971015051, 531772.37417057063430548 178639.05066937819356099, 531797.10340734256897122 178657.86639300896786153, 531837.96040722646284848 178713.77597179752774537, 531857.31372296100016683 178741.19316908807377331, 531868.06556503567844629 178749.79464274787460454, 531880.13844949356280267 178747.46484413990401663, 531893.87027424620464444 178732.70546787517378107, 531882.84744893456809223 178737.65639788802945986, 531874.82179012312553823 178745.74090769540634938, 531873.81108064437285066 178750.26503583858720958, 531928.47747769311536103 178812.55852085907827131, 531938.12053605390246958 178829.1566770619538147, 531932.74461501650512218 178852.9451276523177512, 531965.13453926669899374 178839.37092703295638785, 531981.7662949759978801 178846.35962438152637333, 532009.72108437039423734 178845.01564412217703648, 531981.39670040470082313 178850.0555700947297737, 531960.96820046263746917 178846.83001747232628986, 531933.5510031720623374 178860.26982006573234685, 531935.16377948329318315 178924.24328041044645943, 531930.32545054971706122 179009.45162885275203735, 531910.43454271147493273 179022.35383934245328419, 531885.70530593954026699 179057.83491818906622939, 531876.11210935655981302 179066.35873417466063984, 531831.93818780174478889 179086.51181359370821156, 531779.46893305156845599 179106.20686848048353568, 531672.18940927542280406 179157.81096578075084835, 531589.70353428379166871 179198.03799872964737006, 531556.67969205614645034 179124.41894058702746406, 531620.5699304185109213 179098.98690395732410252, 531635.7671230387641117 179139.9262799954158254, 531648.27035036904271692 179178.57474457612261176, 531695.00515957863535732 179157.60464692092500627, 531797.07743173581548035 179112.31386224390007555, 531810.86905931774526834 179106.1050852510088589, 531847.91815481544472277 179173.68914956544176675, 531891.07424407650250942 179215.21670715624350123, 531905.47685013443697244 179238.60377113270806149, 531919.96244928787928075 179292.40742513118311763, 531957.96748593868687749 179272.83832924981834367, 531967.94273236184380949 179364.63301262669847347, 531985.87575963942799717 179480.30103856680216268, 531979.93544435373041779 179495.99243743464467116, 531952.58757775544654578 179485.23262106810580008, 531939.54275271145161241 179490.46462862013140693, 531766.64450117154046893 179467.29959379057982005, 531761.71291867026593536 179464.16131401702295989, 531729.43346957070752978 179458.33308015181683004, 531718.67365320411045104 179473.57615333772264421, 531714.63872206665109843 179523.78862971480702981, 531716.09578053292352706 179527.48731659070472233, 531741.86680176388472319 179544.99216120038181543, 531751.2878118836088106 179549.55071448421222158, 531794.563677724217996 179583.10166665274300613, 531736.03185356059111655 179657.43647553340997547, 531711.23332369688432664 179690.98742770194076002, 531710.01770948793273419 179697.49096372016356327, 531768.36719152017030865 179689.71103278253576718, 531817.90347053715959191 179690.92664699154556729, 531827.62838420912157744 179689.71103278253576718, 531830.54585831076838076 179679.74299626867286861, 531848.91713031963445246 179689.19716539108776487, 531944.69973392877727747 179685.07748351542977616, 532042.54217847576364875 179713.40029641060391441, 532046.66186035145074129 179723.69950109976343811, 531964.78318307269364595 179783.43488829687703401, 531949.33437603886704892 179795.79393392385100015, 531887.02418766950722784 179851.66711936253705062, 531879.29978415265213698 179893.89385858806781471, 531869.00057946355082095 179984.52685985263087787, 531866.29703823267482221 180017.74179497518343851, 532058.37720568536315113 180022.37643708530231379, 532033.20136249682400376 180178.89389132228097878, 532106.75421455432660878 180190.50749954185448587, 532075.78459263534750789 180204.27177595027023926, 531950.18557040859013796 180250.7262088286515791, 531904.68540677125565708 180257.29303465684643015, 531860.20923614560160786 180140.37888149343780242, 531754.9771151402965188 180133.48226009897189215, 531747.77637041220441461 180141.38065216020913795, 531745.96566537232138216 180174.87869539731764235, 531651.80900330049917102 180172.16263783755130135, 531644.11350688117090613 180200.22856595515622757, 531643.83931215479969978 180060.99850968600367196, 531625.11130755802150816 180053.36858188730548136, 531633.66547321295365691 180050.08258383703650907, 531634.2177775400923565 180047.32106220131390728, 531614.51892320532351732 180053.39640979986870661, 531602.36822800827212632 180051.73949681845260784, 531601.26361935399472713 180045.84825066229677759, 531592.78442665631882846 180051.56285102886613458, 531593.45052950282115489 180089.86376470435061492, 531513.85123934247530997 180096.19174174638465047, 531519.18006211472675204 180125.33374128208379261, 531513.35166220751125365 180149.81302089206292294, 531422.67299250164069235 180461.56490609078900889, 531482.45439605577848852 180488.13441878146841191, 531433.30079757794737816 180454.25829010084271431, 531451.23521864414215088 180385.84179492230759934, 531522.97290290903765708 180398.46231345040723681, 531658.47741763154044747 180391.81993527771555819, 531739.51443133817519993 180345.32328806901932694, 531899.45102110982406884 180269.32835973758483306, 531920.25482747599016875 180313.4964409458625596, 531942.65892663970589638 180340.70141850170330144, 532095.40687415155116469 180361.34519558821921237, 532152.37729773903265595 180433.03831291184178554, 532202.94655013689771295 180431.75807867391267791, 532256.71638812962919474 180407.43362815340515226, 532374.97802585770841688 180393.35105153627227992, 532459.60804447636473924 180370.57185269574983977, 532461.19814912823494524 180285.76627126333187334, 532465.92665053717792034 180247.43457141483668238, 532493.4954023661557585 180222.92901423358125612, 532452.90807328466325998 180147.11494670400861651, 532527.19054349034558982 180142.52015473254141398, 532537.91172475717030466 180135.62796677529695444, 532616.02318827249109745 180158.60192663274938241, 532674.98968523996882141 180186.1706784616690129, 532751.56955143145751208 180296.44568577737663873, 532775.30930995079688728 180316.35645098716486245, 532914.68466641928534955 180285.72450451058102772, 532895.53969987132586539 180311.76165901566855609, 532839.63639755162876099 180333.20402154928888194, 532901.66608916665427387 180315.59065232524881139, 532923.87425036216154695 180282.66130986291682348, 533132.17148640297818929 180152.47553733742097393, 533126.72782159631606191 180120.77814802477951162, 533177.19047552125994116 179911.81100420773145743, 533177.19047552125994116 179911.81100420773145743, 533144.89093221118673682 179901.35225368669489399, 533108.5248437209520489 179872.42468329664552584, 533066.37324115261435509 179864.98616519634379074, 533049.84320092969574034 179750.92888765849056654, 533107.84760892775375396 179739.26681170516530983, 533140.86942005890887231 179734.16034606634639204, 533223.25373236555606127 179757.30965696240309626, 533248.27541399584151804 179688.03193979547359049, 533327.25541587651241571 179685.30849145477986895, 533413.72490069409832358 179664.20176681425073184, 533458.66179831593763083 179668.28693932530586608, 533462.74697082699276507 179714.58556111744837835, 533492.70490257488563657 179792.88470091295312159, 533373.55403766862582415 179881.39677198612480424, 533374.91576183901634067 179946.07867007807362825, 533387.17127937218174338 180014.16487859591143206, 533381.72438269073609263 180029.14384446982876398, 533406.23541775718331337 180008.03711982929962687, 533486.57714380824472755 179980.80263642215868458, 533569.64231819997075945 179956.29160135574056767, 533665.64387221017386764 179901.82263454148778692, 533728.9640461317030713 179852.80056440862244926, 533763.00715039065107703 179912.03556581915472634, 533731.00663238728884608 179845.99194355684448965, 533697.6443902135360986 179868.46039236773503944, 533658.83525135833770037 179792.88470091295312159, 533729.64490821689832956 179746.58607912081060931, 533777.98611626459751278 179715.60685424524126574, 533886.92404989304486662 179672.03168079382157885, 534054.41612284700386226 179527.68891873603570275, 534134.50261897931341082 179505.72398318111663684)</t>
-  </si>
-  <si>
     <t>S2 Bankside</t>
   </si>
   <si>
-    <t>LineString (534134.50261897931341082 179505.72398318111663684, 534161.12046731344889849 179478.51866212062304839, 534268.20681759295985103 179451.43236519605852664, 534371.78454269852954894 179453.52622194297146052, 534488.53814230323769152 179477.87973351695109159, 534494.98466007283423096 179461.40529921691631898, 534512.17537412513047457 179461.40529921691631898, 534522.20329065551050007 179445.64714466902660206, 534511.62516024080105126 179466.71508290435303934, 534496.16740915493573993 179464.36707008117809892, 534493.03672539070248604 179476.8898051381111145, 534702.1627230066806078 179526.04097460908815265, 534896.44344984879717231 179566.88705734140239656, 534992.27464395156130195 179584.69176007088390179, 535029.45505259244237095 179577.88407961549819447, 535044.64141668530646712 179593.07044370827497914, 535083.91649623564444482 179599.35445643632556312, 535105.91054078377783298 179581.02608597950893454, 535104.33953760180156678 179542.27467415656428784, 535130.5229239686159417 179493.57357551416498609, 535254.89400921121705323 179351.92145526938838884, 535306.21344649035017937 179301.64935344501282088, 535425.60968832322396338 179398.00421527508297004, 535482.16580287565011531 179449.32365255415788852, 535506.25451833324041218 179531.01581801878637634, 535495.78116378642152995 179448.01448323580552824, 535436.08304287004284561 179386.22169140999903902, 535314.5921301277121529 179290.91416503459913656, 535342.87018740398343652 179238.54739230085397139, 535185.76986920274794102 179129.62450501468265429, 535141.78178010636474937 179126.48249865067191422, 535084.17833009921014309 179183.03861320309806615, 535030.76422191085293889 179175.70726502037723549, 534880.99525189236737788 179072.02105500755715184, 534803.49242824641987681 179131.71917592402314767, 534766.83568733278661966 179183.03861320309806615, 534641.15543277177494019 179161.04456865493557416, 534665.24414822936523706 179156.85522683622548357, 534776.26170642487704754 178818.56587497628061101, 534718.65825641772244126 178795.5244949734187685, 534768.61604381597135216 178661.29493365884991363, 534831.21432475326582789 178556.21924779983237386, 534951.93958084657788277 178435.49399170652031898, 534952.41323877044487745 178422.29324807948432863, 534920.77471851953305304 178358.38970222626812756, 534947.40119595837313682 178345.85959519623429514, 534914.50966500455979258 178355.2571754687523935, 534945.52167990384623408 178429.81131229753373191, 534821.94349932007025927 178554.01599823284777813, 534758.03995346685405821 178664.43756643508095294, 534705.41350394068285823 178797.25670095355599187, 534598.28108883381355554 178810.41331333509879187, 534492.71493710565846413 178796.94344827780150808, 534245.87182861380279064 178820.75065163488034159, 534072.95635159919038415 178852.07591921000857837, 533911.31797091162297875 178832.02774796192534268, 533807.94458791369106621 178906.58188479070668109, 533667.60738917719572783 179024.36489087314112112, 533584.90868277894333005 179119.59370430145645514, 533452.08954826043918729 179157.18402539161616005, 533214.01751468959264457 179290.00315991009119898, 533260.27816641773097217 179401.55670898006064817, 533255.47700564551632851 179411.57625896626268514, 533142.40450039238203317 179443.3381986441090703, 533048.38915894599631429 179483.99348143170936964, 532974.70145889348350465 179533.54210732915089466, 532794.61126092006452382 179654.87271689844783396, 532708.53640439314767718 179706.00943977979477495, 532693.2906733478885144 179712.36182771535823122, 532685.9464436424896121 179717.96226352726807818, 532658.78351692855358124 179728.82743421287159435, 532607.27455960412044078 179737.47932938844314776, 532548.11974142713006586 179741.40286324714543298, 532534.03526090865489095 179738.18355341436108574, 532548.52215515612624586 179713.23390221039880998, 532555.76560227992013097 179695.93011185922659934, 532523.17009022308047861 179679.43114896627957933, 532492.98906054079998285 179664.94425471880822442, 532479.7094074806664139 179651.26218792953295633, 532484.41954601428005844 179673.02428334188880399, 532449.79857150348834693 179748.49007901950972155, 532378.32551233028061688 179682.61488870403263718, 532357.40633448015432805 179686.00104389677289873, 532361.9146399162709713 179664.21872470591915771, 532197.54445065301842988 179511.6966937497491017, 532242.98194478405639529 179474.83317379461368546, 532244.69978968834038824 179458.70721855689771473, 532258.3818564775865525 179462.12773525423835963, 532327.39026551635470241 179384.03927239449694753, 532343.62657718255650252 179360.62614285058225505, 532356.44643774325959384 179329.55894946909393184, 532412.07767790672369301 179270.75782656238880008, 532414.88226228312123567 179257.70878397024353035, 532428.03560322884004563 179250.60044720803853124, 532448.61292798642534763 179227.50345003115944564, 532485.17324555455707014 179162.59509741654619575, 532492.73745000781491399 179103.45677169098053128, 532484.96392502961680293 179000.80637084558838978, 532493.42510495812166482 179058.75919992162380368, 532498.58643096906598657 179109.07884632432251237, 532488.92768669512588531 179168.71109358099056408, 532459.73001239355653524 179226.54700779423001222, 532606.87226027122233063 179362.21232334937667474, 532626.11217573913745582 179400.69215428520692512, 532679.98393904929980636 179385.30022191087482497, 532719.58761149924248457 179333.93767049448797479, 532820.3977558920159936 179207.26369896886171773, 532909.74552235088776797 179116.74030400396441109, 532941.48410618293564767 179098.9765160133538302, 532963.40215328731574118 179080.1896184952929616, 532976.27465714234858751 179080.88542951448471285, 532985.58112952392548323 179071.40500437797163613, 533037.41905045346356928 179058.18459501341567375, 533056.55385348107665777 179066.18642173407715745, 533060.32914265117142349 179065.0439605139545165, 533066.32706405699718744 179059.61726971823372878, 533052.61752941517625004 179038.19612184033030644, 533040.33607129845768213 178975.07513942685909569, 533032.33884275739546865 178967.93475680088158697, 533022.34230708109680563 178935.44601585279451683, 533014.34507853991817683 178938.30216890317387879, 533009.7752336593111977 178929.16247914195992053, 533004.63415816868655384 178922.59332712605828419, 533008.63277243915945292 178907.74133126405649818, 532948.08232777111697942 178850.76107790888636373, 532929.23171763855498284 178851.90353912903810851, 532820.69790172390639782 178835.33785143680870533, 532628.47880143311340362 178740.51357016403926536, 532649.04310339584480971 178706.81096416953369044, 532649.61433400597888976 178688.53158464707667008, 532680.96280913078226149 178677.48286417848430574)</t>
-  </si>
-  <si>
     <t>S3 Bermondsey</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
     <t>E3 Bow</t>
   </si>
   <si>
-    <t>LineString (538057.11912127735558897 181862.36995379574364051, 538053.62050980445928872 181858.87134232284734026, 538078.00283839902840555 181725.81349199247779325, 537941.46179826941806823 181703.52107727742986754, 537993.7096452577970922 181642.91357477093697526, 538053.69201395311392844 181543.8893257146992255, 537933.4239803443197161 181488.67192663639434613, 538057.85222895222250372 181541.24191616984899156, 538066.94687634671572596 181538.87918232899392024, 538082.506038723513484 181524.15319597572670318, 538090.42530879157129675 181509.20216024381807074, 538125.44152047054376453 181443.09396750494488515, 538174.66927109437528998 181352.78140245075337589, 538212.79301781801041216 181233.2282937929558102, 538225.66242323035839945 181199.85061172995483503, 538241.47548658237792552 181194.25015179277397692, 538274.4193685658974573 181215.99311390187358484, 538284.63197198079433292 181249.59587352504604496, 538292.94811339187435806 181286.28655660181539133, 538290.81553514266852289 181260.73360870234319009, 538312.43949847598560154 181260.35753977482090704, 538331.80704824393615127 181267.31481493418687023, 538327.67029004113283008 181291.66527799205505289, 538335.56773751927539706 181269.47721126751275733, 538339.14039233094081283 181284.1438994413765613, 538474.63447606388945132 181330.39465194242075086, 538488.79537792666815221 181288.87746238996624015, 538509.7148920422187075 181224.50972664973232895, 538727.43854908808134496 181286.78539811534574255, 538725.63448648143094033 181293.36210534413112327, 538740.65893888392020017 181246.83476887160213664, 538834.19827158399857581 181277.85299318662146106, 538849.22272398648783565 181237.14157377314404584, 538854.06932153576053679 181230.84099695915938355, 538845.34544594713952392 181225.02507990010781214, 538848.7380642315838486 181208.06198847782798111, 538853.10000202595256269 181204.18471043845056556, 538858.91591908503323793 181204.18471043845056556, 538863.76251663418952376 181189.1602580358448904, 538857.47811150143388659 181180.36061177065130323, 538866.26599859318230301 181169.53650693810777739, 538882.66424707614351064 181115.4919752876739949, 538880.72560805652756244 181101.4368423949345015, 538892.84210192947648466 181091.25898754157242365, 538908.35121408698614687 181035.03845597061445005, 538902.05063727300148457 181020.01400356800877489, 538883.63356658595148474 181017.59070479340152815, 538879.75628854660317302 181008.38216944987652823, 538886.05686536058783531 180993.3577170472999569, 538882.17958732123952359 180981.24122317423461936, 538888.48016413522418588 180965.73211101672495715, 538895.26540070411283523 180943.92242204523063265, 538857.46193982020486146 180934.71388670170563273, 538842.92214717250317335 180928.89796964265406132, 538824.50507648545317352 180928.89796964265406132, 538774.10046197345945984 180907.57294042606372386, 538717.87993040238507092 180854.26036738461698405, 538729.99642427545040846 180840.20523449187749065, 538707.07831848983187228 180830.60309832252096385, 538703.25330118928104639 180837.43348635928123258, 538663.36383505456615239 180847.26924513219273649, 538663.91026609751861542 180852.73355556160095148, 538660.24865216040052474 180844.65553881169762462, 538640.96016229398082942 180837.16027083780500107, 538544.24186769349034876 180802.73511513255652972, 538450.80215935071464628 180793.71900292404461652, 538430.0377797189867124 180786.06896832288475707, 538416.10378812404815108 180768.30995942730805837, 538405.72159830818418413 180775.6867785069916863, 538415.28414155961945653 180756.83490752556826919, 538418.01629677438177168 180719.40438108413945884, 538406.54124487261287868 180719.40438108413945884, 538409.000184565782547 180685.25244090033811517, 538395.33940849232021719 180678.69526838505407795, 538382.49827898317016661 180675.41668212742661126, 538362.28033039439469576 180657.65767323184991255, 538356.81601996498648077 180676.23632869182620198, 538348.34633879945613444 180663.94163022565771826, 538323.75694186717737466 180621.86643991924938746, 538322.93729530274868011 180593.17881016488536261, 538328.4016057321568951 180552.46969746579998173, 538322.6640797812724486 180530.61245574819622561, 538329.76768333942163736 180524.87492979731177911, 538343.42845941300038248 180540.99464556406019256, 538349.98563192831352353 180540.99464556406019256, 538343.97489045595284551 180555.74828372345655225, 538352.71778714295942336 180560.93937863138853572, 538365.01248560915701091 180534.98390409172861837, 538371.84287364582996815 180527.88030053349211812, 538376.48753751092590392 180495.36765347851905972, 538383.86435659055132419 180427.33698863245081156, 538397.2519171426538378 180335.26335789696895517, 538386.32329628383740783 180280.34703808143967763, 538356.54280444351024926 180181.98945035215001553, 538349.86702627711929381 180158.3111812362622004, 538333.93950255436357111 180158.96128424536436796, 538325.81321494071744382 180125.48097927699564025, 538338.16517211345490068 180121.9054127269773744, 538312.80498378432821482 180015.22765528378658928, 538309.48158343171235174 179915.05087322887266055, 538303.30955420562531799 179855.22966688327142037, 538278.62143730116076767 179762.64922849129652604, 538277.6718943432206288 179740.33496898142038845, 538278.14666582213249058 179706.15142249822383747, 538284.31869504833593965 179692.38304960916866548, 538274.34849399072118104 179684.31193446728866547, 538260.58012110169511288 179479.68542704707942903, 538283.84392356942407787 179380.45818795004743151, 538276.46764299820642918 179373.42610627005342394, 538286.21778096398338675 179367.16458653993322514, 538328.94721406803000718 179194.82253968715667725, 538373.10096160881221294 179125.98067524185171351, 538412.337829110911116 179066.10921436137869023, 538405.98546794115100056 179059.09686761553166434, 538415.39026240026578307 179061.24182073780684732, 538432.44739647547248751 179038.1479516392282676, 538557.31229543488007039 178855.83570372880785726, 538560.63569578749593347 178836.37007309254840948, 538544.49346550367772579 178770.85160899977199733, 538392.56659224512986839 178811.6819561880256515, 538328.48941097827628255 178579.7348779343010392, 538315.17884117900393903 178559.57830087453476153, 538294.47845585108734667 178453.40847317627049051, 538304.19587160169612616 178433.00190009997459128, 538253.66530969843734056 178404.8213944231683854, 538283.78929852542933077 178333.88425944367190823, 538307.11109632684383541 178343.60167519428068772, 538318.77199522766750306 178346.5168999194575008, 538335.11924329411704093 178348.77976422818028368, 538281.84581537533085793 178321.25161896785721183, 538252.69356812338810414 178330.96903471846599132, 538232.28699504712130874 178316.39291109255282208, 538044.79800434643402696 178261.3466268312477041, 538019.15639011771418154 178253.05674019930302165, 538025.32914176001213491 178211.08202903144410811, 537920.39236384036485106 178207.37837804603623226, 537794.46823033690452576 178227.13118330150609836, 537698.17330471647437662 178260.46404217008966953, 537658.66769420565105975 178275.27864611166296527, 537636.4457882932620123 178285.15504873939789832, 537613.32763770420569927 178298.05650823522591963, 537459.7524428729666397 178375.6691471713129431, 537456.14730042521841824 178381.81708270622766577, 537556.97021414036862552 178513.66243141060112976, 537678.42049946112092584 178674.65567737040692009, 537642.61853993555996567 178704.28488525358261541, 537655.49145826080348343 178726.26947054677293636, 537656.62345710769295692 178743.01280580330058001, 537645.11526750994380563 178749.34231008208007552, 537658.54148870729841292 178753.46607802127255127, 537643.36394558555912226 178764.38451038327184506, 537846.50558974756859243 178742.98746254466823302, 537864.34695504221599549 178732.03885750484187156, 537921.10559516295325011 178705.15133090259041637, 537929.97295804345048964 178681.03210386767750606, 537934.22929222602397203 178722.8860566635557916, 537931.391736104269512 178762.2571478528843727, 537923.27317417750600725 178793.5180244478979148, 537919.38620787719264627 178840.16162005084333941, 537924.24491575255524367 178882.91824935356271453, 537923.94315128470771015 178917.25865100373630412, 537939.79278095357585698 179148.20369934543850832, 537945.62323040387127548 179326.0324075817479752, 537596.7680049566552043 179354.21291325855418108, 537587.05058920604642481 179321.17369970644358546, 537583.16362290584947914 179361.01510428398614749, 537578.30491503048688173 179418.34785721261869185, 537345.08693701564334333 179405.71521673683309928, 537341.19997071544639766 179448.9577168270770926, 537339.25648756534792483 179477.62409329140791669, 537446.14806082216091454 179485.39802589188911952, 537438.37412822165060788 179644.76364420205936767, 537455.86547657276969403 179648.650610502314521, 537520.97216210188344121 179645.73538577710860409, 537523.7159856699872762 179645.73538577710860409, 537550.12440935370977968 179645.73538577710860409, 537546.72331384103745222 179683.14743641699897125, 537621.06154433323536068 179697.72356004291214049, 537630.77896008384414017 179799.27055463689612225, 537550.12440935370977968 179816.76190298801520839, 537528.26022391486912966 179825.02170637605013326, 537537.97763966547790915 179912.96431891914107837, 537544.29395990341436118 179930.94153805778478272, 537492.79165642510633916 179940.65895380839356221, 537507.85365083860233426 179979.04274602336226963, 537506.88190926343668252 180020.8276337510033045, 537501.05145981314126402 180022.28524611360626295, 537502.02320138819050044 180025.68634162630769424, 537416.05443968356121331 180037.57935224322136492, 537411.13920003117527813 180046.84167782287113369)</t>
-  </si>
-  <si>
     <t>E4 Isle of Dogs</t>
   </si>
   <si>
@@ -239,36 +224,9 @@
     <t>N6 Shoreditch</t>
   </si>
   <si>
-    <t>N7A Kings Cross</t>
-  </si>
-  <si>
-    <t>LineString (533064.46897248667664826 183210.39921171619789675, 533076.87953593488782644 183044.4026491524418816, 533070.12536461430136114 182985.15014620366855524, 533045.871749417623505 182926.97217051047482528, 533058.76607648422941566 182947.23468447223422118, 533080.25662159512285143 182941.70854430084000342, 533168.98187212459743023 182947.23468447223422118, 533189.95457557367626578 182949.67927450055140071, 533190.07185356423724443 182932.90852184614050202, 533256.30459875019732863 182938.06875343210413121, 533270.02612364920787513 182934.78496969558182172, 533273.77901934809051454 182943.58081898986711167, 533263.22400019492488354 182991.66479513191734441, 533262.98944421380292624 183071.82430170045699924, 533364.55218406510539353 183067.83685002036509104, 533378.15643097355496138 183087.01180148191633634, 533393.87168171268422157 183066.6054311191837769, 533558.68779758946038783 183057.05841860847431235, 533558.68779758946038783 183104.32901793727069162, 533562.10755929746665061 183050.22677661170018837, 533642.96578439825680107 183054.08632424913230352, 533689.65670660801697522 183029.44389308284735307, 533695.6545603577978909 183019.57997865247307345, 533704.33502684440463781 183018.39627867707167752, 533731.16547348327003419 182971.580515898327576, 533679.00828732317313552 182905.35815865072072484, 533656.73604574415367097 182842.7174792095029261, 533666.46468460059259087 182784.81158445819164626, 533584.38219428097363561 182771.602907855034573, 533559.38005642499774694 182775.37681545593659393, 533489.0910273581976071 182693.88399819895857945, 533450.88021289906464517 182666.99490654253168032, 533423.99112124263774604 182625.95366138272220269, 533418.28455447813030332 182579.59432971687056124, 533451.54715791763737798 182502.91214257484534755, 533464.75749999412801117 182467.34583698387723416, 533337.93821605830453336 182452.71284268359886482, 533337.78902459214441478 182368.47306541417492554, 533484.07380397082306445 182386.01211906579555944, 533489.36575981404166669 182293.32729244133224711, 533472.43150111590512097 182205.93442166002932936, 533583.10897760698571801 182063.8076075866993051, 533609.71995556121692061 182037.80142458603950217, 533610.24870057171210647 182016.33477542886976153, 533584.88456065976060927 182052.1574076684191823, 533535.1852201041765511 182057.86061068301205523, 533518.26287293271161616 181970.58373815898085013, 533484.19519956270232797 181975.12609460830572061, 533475.45617014251183718 181918.25283637543907389, 533396.87044996197801083 181921.33462932368274778, 533362.97072753123939037 181745.67243127315305173, 533383.00238169485237449 181921.33462932368274778, 533385.57218187116086483 181991.15361790888709947, 533400.75257761764805764 182035.04779862469877116, 533331.49939815502148122 182048.89843451723572798, 533234.54494690720457584 182081.48816602909937501, 533073.65851616964209825 182090.02078689282643609, 533085.33284421800635755 182215.89180190846673213, 533090.14230673655401915 182227.52340018114773557, 533155.84606537700165063 182220.5149992594961077, 533149.99286592833232135 182319.05148053923039697, 533156.54641778930090368 182323.96664443501504138, 533151.53487813088577241 182385.64713253875379451, 532980.57106288510840386 182377.64146055665332824, 532778.65285523270722479 182361.72131757129682228, 532755.6968509522266686 182366.02556837382144295, 532572.76619184156879783 182348.80856516343192197, 532552.88329151901416481 182350.97523911585449241, 532244.88995379093103111 182215.8126952207821887, 532262.60291642148513347 182168.39960261050146073, 532295.2441410442115739 182069.11680604351568036, 532305.37037298001814634 182028.61187830017297529, 532288.80017526680603623 182059.91114064730936661, 532220.90932479011826217 182025.71317250368883833, 532158.87452575471252203 182016.26025074589415453, 532107.4742636966984719 182011.53378986698226072, 532104.52022564737126231 181924.09426360743236728, 532086.79599735140800476 181928.63609710824675858, 532087.97761257109232247 181975.30989828731981106, 532092.70407344994600862 182022.86991088121430948, 532079.11549842311069369 182099.67490016322699375, 532046.62107988074421883 182161.70969919872004539, 532014.12666133837774396 182194.20411774111562409, 531972.17932103818748146 182188.88684925236157142, 531913.68936766183469445 182151.07516222121194005, 531908.60801759164314717 182163.45413967911736108, 531953.17571160080842674 182184.55127293791156262, 531987.59041022916790098 182199.51705184334423393, 532004.99554516770876944 182204.79133515805006027, 531983.10726941167376935 182243.55731752107385546, 531968.33927613054402173 182281.13658613828010857, 531944.07757288287393749 182371.59054498534533195, 531937.94260709825903177 182398.64015493713668548, 532011.93064753827638924 182423.87109960327506997, 532068.52979368122760206 182445.01053972897352651, 532086.94156411325093359 182440.23711776512209326, 532158.88385228300467134 182467.76953373529249802, 532152.40563676052261144 182502.8882810408831574, 532121.55289627402089536 182643.03526213087025099, 532075.0642949640750885 182863.25497264647856355, 532069.45360170258209109 182883.29316286626271904, 532082.41561907751020044 182888.00662372991791926, 532062.29523281508591026 182889.32744172037928365, 532066.95640396035742015 182915.35964283399516717, 531884.43796249642036855 182981.6259192216093652, 531767.99498561583459377 183028.33115369590814225, 531728.68198287941049784 182918.06297528900904581, 531725.87449492723681033 182910.13609254563925788, 531809.84689899394288659 182817.65547132669598795, 531837.40510237636044621 182760.1590255610353779, 531828.71498920442536473 182755.52429853595094755, 531814.23146725108381361 182767.69045697676483542, 531569.74961667892057449 182693.53482457570498809, 531563.95620789751410484 182754.94495765783358365, 531565.11488965386524796 182687.74141579438582994, 531616.09688692959025502 182577.66664894908899441, 531609.14479639194905758 182564.92114963015774265, 531628.84238624852150679 182534.7954239672399126, 531625.36634097970090806 182476.86133615393191576, 531747.02792538760695606 182513.93915235446183942, 531632.89777239540126175 182463.5364959568833001, 531625.94568185787647963 182421.82395273129804991, 531681.5624061586568132 182312.90786764226504602, 531703.57735952769871801 182270.0366426604159642, 531683.80043675052002072 182250.5687343017780222, 531595.88583471847232431 182183.28084469723398797, 531580.06645999138709158 182164.89640980056719854, 531555.2433897431474179 182143.27140381743083708, 531526.61310013174079359 182118.90519989278982393, 531515.64830836560577154 182136.41840896362555213, 531466.00216786901000887 182107.48354180311434902, 531411.63507536228280514 182149.7436767349136062, 531394.57873261498752981 182161.31762359911226667, 531354.5267849137308076 182200.07511671676184051, 531330.16058098908979446 182208.29871054133400321, 531333.2063564796699211 182193.06983308843336999, 531354.79575750709045678 182159.67430333484662697, 531334.90127811359707266 182155.04768022007192485, 531291.87368314596824348 182150.88371941674267873, 531265.96459370316006243 182135.15320082646212541, 531248.34037534287199378 182041.19192783226026222, 531270.21593675261829048 182040.14943936991039664, 531272.14963821833953261 182027.69603843480581418, 531291.66027387382928282 182000.88878809078596532, 531269.86458137142471969 182026.02942997106583789, 531260.89388385554775596 182036.66077076771762222, 531156.26423942053224891 182028.00196012531523593, 530992.96919284970499575 181971.66516905839671381, 530937.44887701561674476 182060.66096943948650733, 530881.5203235651133582 182170.88512587477453053, 530784.23736255615949631 182302.13991453754715621)</t>
-  </si>
-  <si>
-    <t>LineString (530784.23736255615949631 182302.13991453754715621, 530778.6444442254723981 182309.68591545993695036, 530773.74559282837435603 182337.44607337698107585, 530858.50592793908435851 182423.17597282669157721, 530936.88755029300227761 182449.3031802780169528, 531037.31400393415242434 182542.38135682337451726, 531094.36521082976832986 182594.22753410961013287, 531155.37121963454410434 182521.76535719376988709, 531166.80187289451714605 182513.19236724881920964, 531203.95149598934222013 182472.57272441431996413, 531259.88004943984560668 182529.52187190589029342, 531326.62689972575753927 182604.63759332848712802, 531370.30832468345761299 182662.60733486112440005, 531384.59664125845301896 182683.83569091532262973, 531369.90008706704247743 182687.50982946317526512, 531339.69050345139112324 182687.10159184673102573, 531257.94092076190281659 182652.80963206687010825, 531233.85490139271132648 182679.95743355926242657, 531204.76797122228890657 182711.18761121592251584, 531182.72313993528950959 182813.24701532270410098, 531203.13502075662836432 182831.20947044549393468, 531268.45303938491269946 182871.21675685534137301, 531362.55180997133720666 182909.59109279947006144, 531365.40947328635957092 182920.61350844299886376, 531354.79529525921680033 182956.13018107216339558, 531444.90684366086497903 182988.57858534331899136, 531474.10273866006173193 182998.58689318058895878, 531486.5355991879478097 183012.4143484897504095, 531547.55104103893972933 183034.71440845559118316, 531569.85110100475139916 183061.97003730272990651, 531517.81762775115203112 183110.59655695044784807, 531527.72876551374793053 183131.65772469594958238, 531497.95239027438219637 183140.93648922778083943, 531508.4095920140389353 183177.7640257888706401, 531495.22442460327874869 183139.57250639220001176, 531524.09539462334942073 183130.25195701562915929, 531519.54878517135512084 183120.02208574867108837, 531516.59348902758210897 183111.38352778987609781, 531448.32344150589779019 183136.55978571731247939, 531241.26357583678327501 183121.43743597742286511, 531197.64141312555875629 183108.64160158214508556, 530715.12526052596513182 183043.21945667950785719, 530703.01725020399317145 183063.42695543030276895, 530695.13352120853960514 183041.84071603690972552, 530546.28326243243645877 183024.95802384099806659, 530541.22589214832987636 183004.5417986634420231, 530703.18488589045591652 182946.11745994322700426, 530775.51721857010852545 182908.57789488162961788, 530786.04660877038259059 182895.30170723787159659, 530795.49963942251633853 182875.6843990063352976, 530804.3135183157864958 182802.06196081181406043, 530806.59301448101177812 182793.73684438230702654, 530819.8735573566518724 182794.33149555584532209, 530807.31673856556881219 182782.83954266682849266, 530812.03824553836602718 182733.95805871355696581, 530761.76808306365273893 182714.23882370966020972, 530770.16958811797667295 182659.52488996647298336, 530712.95603303634561598 182638.97244784975191578, 530630.19079316093120724 182601.20039206769433804, 530615.74853653833270073 182603.42227770193130709, 530555.75762441393453628 182723.95957335943239741, 530539.09348215709906071 182717.29391645672149025, 530547.14781758119352162 182730.62523026211420074, 530461.60522066289559007 182906.15419536712579429, 530437.90885532670654356 182917.93718825542600825, 530382.0339413866167888 182876.71421071342774667, 530325.26406243664678186 182961.75723386157187633, 530268.29162278701551259 182922.72056224985863082, 530249.18178586428985 182908.73221319253207184, 530252.98490572301670909 182894.20538857823703438, 530184.08185019285883754 182852.74914162818458863, 530085.83308541483711451 182787.51840435751364566, 530111.18260209145955741 182744.29519918368896469, 529999.02136356220580637 182666.39424455061089247, 529961.66046464198734611 182715.15181299234973267, 529988.72742143063805997 182735.23374867427628487, 529986.10803851566743106 182740.763557050464442, 529932.80478152283467352 182814.59110673272516578, 529984.94386833114549518 182734.94270612817490473, 529957.00378390413243324 182716.02494063068297692, 530013.09155612858012319 182629.12904521985910833, 530018.17775851185433567 182621.49974164497689344, 530100.32880480831954628 182494.38274551162612624, 530104.0113532249815762 182482.84132467227755114, 530220.50368910923134536 182556.47051627180189826, 530255.09743770561181009 182478.63458192982943729, 530272.39431200386025012 182483.35191128388396464, 530279.47030603489838541 182470.7723663397191558, 530137.95042541308794171 182415.73685720900539309, 530133.8373461066512391 182413.51172491264878772, 530186.21162480069324374 182272.1011724385607522, 530075.7495097367791459 182226.86884083910263143, 530075.1733111577341333 182226.46204725949792191, 530187.16388441331218928 182265.91148495653760619, 530233.22869966924190521 182154.23642371431924403, 530357.8921046924078837 182201.72724467553780414, 530348.98757576220668852 182228.44083146619959734, 530358.86895656702108681 182231.0766534095746465, 530394.74696868821047246 182125.29837629428948276, 530508.99968287569936365 182165.49652313266415149, 530513.72136097133625299 182167.0985210579528939, 530567.86575565708335489 182188.16529536261805333, 530573.45622016047127545 182150.89553200689260848, 530664.76714038196951151 181926.34520778860314749, 530694.76100652059540153 181850.76066511913086288, 530759.06664636044297367 181869.87285391447949223, 530674.73822676041163504 181825.22436629422008991, 530573.75377231650054455 181777.63399121144902892, 530599.29007114132400602 181730.04361612870707177, 530646.88044622412417084 181748.21467864664737135, 530657.97477119497489184 181732.12790743884397671, 530724.74751764547545463 181760.6236275052651763, 530741.12779784575104713 181707.06197263259673491, 530773.19373494503088295 181600.7954151411249768, 530782.75100370426662266 181575.85406711159157567, 530688.89235894195735455 181552.28991476428927854, 530627.95015930733643472 181539.24596229381859303, 530599.01706093887332827 181486.621268884598976, 530600.06536160444375128 181482.63772635560599156, 530608.87108719476964325 181476.34792236247449182, 530639.82865497504826635 181423.25654537187074311, 530713.75870660948567092 181269.28719607146922499, 530693.84197932516690344 181263.16111494251526892, 530645.94210892508272082 181237.73285941511858255, 530707.03671619179658592 181120.0358954158728011, 530733.0917692908551544 181051.75368729417095892, 530735.53599696443416178 181033.12102656494244002, 530686.68588671088218689 181005.64283954733400606, 530652.70320131711196154 180951.48293470105272718, 530637.30479699815623462 180860.15446770534617826, 530634.11892024241387844 180839.31352392872213386, 530578.89705647761002183 180803.20692069784854539, 530573.58726188482251018 180813.82650988339446485, 530606.733512117061764 180830.61361899445182644, 530579.45680101704783738 180882.17122962352004834)</t>
-  </si>
-  <si>
-    <t>LineString (534150.19790721382014453 181658.82599177915835753, 534188.4078070386312902 181677.32008704933105037, 534295.39330477884504944 181748.67556176203652285, 534458.90044428419787437 181864.5233750130282715, 534483.31045287544839084 181802.6053044400177896, 534553.56364833330735564 181831.18287547372165136, 534581.15801056486088783 181763.96769404891529121, 534626.35794776398688555 181776.75086198319331743, 534797.74285306176170707 181843.92396450418164022, 535287.18371127475984395 182016.74360227302531712, 535232.17579299991484731 182019.72173797580762766, 535207.64996956521645188 182091.8977326549065765, 535091.50267715682275593 182197.53395787699264474, 535042.14986233541276306 182197.81197882973356172, 535028.73974128148984164 182224.41747152400785126, 535036.47778976988047361 182425.60673222184414044, 535003.97798611875623465 182543.22506924520712346, 534994.72957604483235627 182519.28562053974019364, 534911.66025196714326739 182500.88847403886029497, 534924.30123606591951102 182412.06298755903844722, 534860.19338813633657992 182410.70859640560229309, 534794.73114905343391001 182370.9797892379865516, 534781.76486209139693528 182416.81556864531012252, 534775.89833489886950701 182439.80761461149086244, 534733.01554672734346241 182433.42887881567003205, 534738.45721302484162152 182649.24169926377362572, 534730.12317419145256281 182691.18073339309194125, 534802.97880399296991527 182703.14411171845858917, 534809.85073587717488408 182706.20718782997573726, 534878.44964922510553151 182728.92067172401584685, 534874.50866161868907511 182753.88025989828747697, 534886.18912552238907665 182730.73464611344388686, 534960.41568882705178112 182744.27007824546308257, 534951.68315196770709008 182818.06001470709452406, 534939.02097352163400501 182880.93428009451599792, 534963.03544988483190536 182888.35693642497062683, 534944.24135854840278625 182963.83128923355252482, 534899.9714611767558381 182951.04220777060254477, 534891.78288685239385813 182949.51981309754773974, 534883.95649775443598628 182942.20384067995473742, 534838.18913542130030692 182939.14134059820207767, 534833.59538529859855771 182956.15522994138882495, 534728.87489639106206596 182935.52588911273051053, 534732.14552768925204873 182871.83970818307716399, 534649.52294641232583672 182862.46408719307510182, 534628.55294301128014922 182955.48487151082372293, 534493.18888259516097605 182880.20793622478959151, 534302.84577480040024966 182816.22254123163293116, 534284.02654097892809659 182859.77562521857907996, 534295.78345685871317983 182819.58610184054123238, 534296.67217820382211357 182816.26452868265914731, 534176.80159754795022309 182772.97793011250905693, 534076.9094470014097169 182756.3292383547523059, 534124.19173159345518798 182555.3795288386172615, 534016.13174477114807814 182513.80254928936483338, 534017.00426228798460215 182506.70794914639554918, 534125.32640601880848408 182535.96195105163496919, 534168.1666928093181923 182311.53897498786682263, 534269.44489237654488534 182341.85239916807040572, 534307.17684069508686662 182340.19748915411764756, 534331.33852689899504185 182328.77861005775048397, 534411.72237405984196812 182320.70818523829802871, 534383.0651157310931012 182118.86140918426099233, 534448.45756019873078912 182114.30714349748450331, 534385.02715628384612501 182112.14474336401326582, 534401.94695855455938727 182029.46270526901935227, 534197.29156851791776717 182037.41563493365538307, 534198.35195913992356509 182073.99911139099276625, 534075.34664699353743345 182084.07282229952397756, 533877.15337622561492026 182102.89926247851690277, 533881.96351368981413543 182166.63358387906919234, 533889.17871988611295819 182271.25407372525660321, 533665.51229002187028527 182282.44098327826941386, 533645.62510754854883999 182286.76606867561349645, 533618.20713596616405994 182449.44603339742752723, 533631.91612175735644996 182517.07702996715670452, 533611.80960926366969943 182537.18354246084345505, 533613.63747403584420681 182570.9990407457225956, 533636.48578368767630309 182581.96622937865322456, 533661.16195811179932207 182576.48263506218791008, 533674.87094390299171209 182558.2039873406465631, 533694.06352401059120893 182568.25724358748993836, 533708.19324949278961867 182577.78883584373397753, 533744.78147669287864119 182600.35388822320965119, 533727.40999601525254548 182690.08309506479417905, 533748.53494538308586925 182713.30995750919100828, 533738.36664293019566685 182797.78821624990087003, 533887.88424544327426702 182820.57441884058061987, 533896.32165873644407839 182796.25481581923668273, 533994.96494650165550411 182805.68486597036826424, 533958.97602709801867604 182864.08820365733117796, 534162.58751859271433204 183101.90006286397692747, 534151.45251515158452094 183143.85516511532478034, 534224.62539490743074566 183157.37624072236940265, 534242.12325745774433017 183214.64197270525619388, 534235.76864853664301336 183146.50009479920845479, 534422.34790956706274301 183189.51548639123211615, 534554.33143426640890539 183222.22614488427643664, 534560.58397974201943725 183245.53360263974172994, 534585.38740086904726923 183236.13562777847982943, 534839.23427885014098138 183312.35428325369139202, 534883.15689386974554509 183313.64612487191334367, 535342.64082826022058725 183415.18309037722065113, 535377.02339462761301547 183414.03198869159677997, 535729.61131596809718758 183230.43964716198388487, 535597.45816457970067859 183171.78773763249046169, 535493.01945444208104163 183163.06486600026255473)</t>
-  </si>
-  <si>
-    <t>LineString (527158.31216002732980996 177000.8693951431196183, 527099.77578929206356406 176863.97566198912682012, 526993.89284357777796686 176974.11520853615365922, 526965.6928630608599633 177009.76424051032518037, 526918.33817879669368267 176978.37180936889490113, 526881.62499661440961063 176915.05487198193441145, 526809.33459098706953228 176814.57045149418991059, 526803.78523573139682412 176782.81458185013616458, 526837.9906987837748602 176724.64684572990518063, 526829.14218303072266281 176698.07787916850065812, 526713.59169160143937916 176585.58887918625259772, 526702.01159683079458773 176498.87495989364106208, 526728.35331819928251207 176459.47930909239221364, 526759.08459305611904711 176456.02855037362314761, 526877.73335154261440039 176444.22870948346098885, 526952.37421362893655896 176459.79166246333625168, 526957.30744241294451058 176431.45683538325829431, 527038.82798124512191862 176435.9939717588131316, 527098.5913686784915626 176454.87681948934914544, 527051.24293423152994365 176594.92815045249881223, 527174.99744662863668054 176650.61612686808803119, 527153.14015064027626067 176640.28990523278480396, 527205.55905537132639438 176487.71942607063101605, 527102.71056710940320045 176449.37945362422033213, 527080.02346470882184803 176442.65865531019517221, 527118.21201132400892675 176315.62328595775761642, 527136.13724749034736305 176310.16777929847012274, 527123.4023648789152503 176243.66339232763857581, 527158.08696234272792935 176237.9932378021767363, 527169.22996887960471213 176208.6499966005794704, 527150.43826302816160023 176186.18838753091404215, 527118.65549396350979805 176157.02174997527617961, 527093.6976608419790864 176147.4813768335734494, 527018.22708262107335031 176131.11693114246008918, 526849.86647974920924753 176114.85084184003062546, 526845.07710992521606386 176097.65762165782507509, 526857.65365130186546594 176044.64240146498195827, 526893.8380195926874876 176044.15844629961065948, 526858.37810308812186122 176039.0902959554514382, 526874.83542804175522178 175886.27227852959185839, 527054.69047931989189237 175862.7618143102445174, 527176.94489326048642397 175856.8841982554004062, 527195.27535622008144855 175822.70450227480614558, 527223.9658216992393136 175795.75699128504493274, 527224.12844125344417989 175773.97201046324335039, 527243.25712752784602344 175756.61424477020045742, 527267.78618826356250793 175718.31265972839901224, 527222.48707379773259163 175682.39379150536842644, 527195.04935412993654609 175648.09664192068157718, 527009.0825874931178987 175569.97535675560357049, 526824.66230209683999419 175469.42516340431757271, 526795.48152648622635752 175473.6317607709497679, 526758.33231608534697443 175456.72367672127438709, 526790.20567167596891522 175381.68114836351014674, 526851.47655176091939211 175305.71711282295291312, 526851.47655176091939211 175278.90286315878620371, 526865.43143400084227324 175215.89678796651423909, 526877.77642672799993306 175178.34743508807150647, 526907.09578445507213473 175139.25495811874861829, 526889.09267006127629429 175116.10809675537166186, 526973.96449506049975753 174912.93009145429823548, 526885.95633615972474217 174859.8365453231963329, 526909.64957838621921837 174789.88203135458752513, 526922.28532687691040337 174784.41939029871718958, 526957.33885194035246968 174894.75840272463392466, 526938.1368365534581244 174894.58398754562949762, 526918.67389838397502899 174882.02661713416455314, 526881.00047726207412779 174863.13230195376672782, 526645.98297396756242961 174831.60109246335923672, 526609.50912189844530076 174827.05741743353428319, 526567.45242367009632289 174822.48189269431168213, 526532.3543359829345718 174820.95671778128598817, 526511.19253406394273043 174818.36392042905208655, 526475.19840611529070884 174928.17651417059823871, 526482.59550444374326617 174953.18938274509855546, 526621.9569095199694857 175008.21030497280298732, 526587.08526148088276386 175075.49314598224009387, 526608.94237426621839404 175084.53746851411415264, 526524.52869730209931731 175245.07419345498783514, 526473.27779452677350491 175229.8263443021569401, 526498.70052055746782571 175244.55399248545290902, 526476.25838999240659177 175289.43825361545896158, 526525.35055060335434973 175313.2830173407564871, 526502.38243260327726603 175360.27122821123339236, 526655.2694470772985369 175450.74106705139274709, 526548.66932689363602549 175611.34256390717928298, 526523.42193000798579305 175630.27811157138785347, 526494.29995637480169535 175591.88974311901256442, 526406.30206112191081047 175494.22269502107519656, 526346.69015180855058134 175449.33843389106914401, 526380.35334765608422458 175404.45417276109219529, 526342.83291061769705266 175434.61078570786048658, 526304.6144535921048373 175412.13552230672212318, 526220.48104146879632026 175317.48543366795638576, 526212.83254945755470544 175223.7914065305958502, 526176.50221240427345037 175198.93380749414791353, 526071.33544725005049258 175206.58229950536042452, 526034.04904869536403567 175148.26254791987594217, 526009.19144965894520283 175110.97614936518948525, 526011.10357266175560653 175093.76704233995405957, 526011.20072534133214504 175093.52450637135189027, 526028.17182268667966127 175051.15715683341841213, 526084.52183982264250517 174972.04738347270176746, 526120.93744978227186948 174927.4696540392760653, 526209.46505330502986908 174784.94649092113832012, 526160.02340298215858638 174854.23032570173381828, 526058.27785727987065911 174801.38573994935723022, 526004.64454636699520051 174887.35678244201699272, 525960.47593737987335771 174865.27247794848517515, 525890.07368513778783381 174975.67681796516990289, 525855.51160305016674101 174953.83957849282887764, 525828.51382325252052397 174995.27803120561293326, 525849.7215751651674509 174948.58325841222540475, 525805.44013935560360551 174918.05182387726381421, 525814.23011417349334806 174839.56990586066967808, 525702.0009714097250253 174820.10639019258087501, 525698.8616946890251711 174722.78881185199134052, 525659.9346633527893573 174636.77262970581068657, 525565.36717306601349264 174664.02053710119798779, 525538.06676878000143915 174653.24728339188732207, 525493.99436724185943604 174553.83953325595939532, 525459.71583271224517375 174532.29302583733806387, 525496.93252734444104135 174407.42122147939517163, 525457.92714756459463388 174534.53035107266623527, 525490.77226448152214289 174556.32890400406904519, 525543.79577161197084934 174666.49996881955303252, 525536.72597066126763821 174676.51552016640198417, 525515.04797329346183687 174692.30743877869099379, 525500.11743205995298922 174748.58409419711097144, 525507.00845109077636153 174843.90985745683428831, 525596.59169849148020148 174873.7709399237355683, 525710.00638670718763024 174878.36495261095114984, 525777.76807384355925024 174928.89909217032254674, 525768.58004846912808716 175008.14581102479132824, 525718.31548450421541929 175117.9094939905917272, 525718.31548450421541929 175117.9094939905917272)</t>
-  </si>
-  <si>
-    <t>LineString (525327.85414873412810266 178420.77501689142081887, 525434.3555114408954978 178547.73350585880689323, 525347.43806628719903529 178651.24739231160492636, 525430.2491754493676126 178706.68292819705675356, 525486.36910066672135144 178623.18742970289895311, 525558.91436985018663108 178563.64555782591924071, 525601.34650842915289104 178515.0539152596029453, 525591.59441469295416027 178508.14618219647672959, 525612.31761388236191124 178515.8665897376195062, 525739.09483245271258056 178641.42479659095988609, 525767.53843918326310813 178664.58601921438821591, 525708.21320228814147413 178737.72672223576228134, 525731.62045715074054897 178716.68428954426781274, 525769.37393091234844178 178666.83504263576469384, 525806.39432751352433115 178612.95387134497286752, 526026.40911028429400176 178722.27400289245997556, 526144.43453311175107956 178765.52555535719147883, 526255.77580733434297144 178814.4714835460181348, 526271.20979337661992759 178817.35269416749360971, 526312.78246261400636286 178730.88154215391841717, 526431.85428454133216292 178507.28957353180157952, 526371.81847308482974768 178458.83962042655912228, 526552.97916730435099453 178570.48516453863703646, 526555.08568700461182743 178631.57423584524076432, 526525.59441120142582804 178796.93603231309680268, 526496.81081177107989788 178977.54604629526147619, 526531.73185393039602786 178797.25923736946424469, 526578.25740370713174343 178795.88277246299549006, 526808.88298217917326838 178842.85059796637506224, 526867.58985495707020164 178857.72481234182487242, 526887.47400313417892903 178869.08718272874830291, 526862.61881791288033128 179084.26207193068694323, 526876.82178089639637619 179026.0299236977880355, 526893.15518832765519619 179011.11681256498559378, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527768.86287219019141048 179171.7344985579547938, 527738.35830124607309699 179152.01631094136973843, 527772.52151037787552923 179165.95770141950924881, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528513.98412839835509658 179812.26687349064741284, 528529.45710146625060588 179823.30889789306093007, 528599.09828376933000982 179804.26158560626208782, 529067.56848417001310736 179787.9540786303114146, 529126.86850953719113022 179829.46409638732438907, 529184.68603427021298558 179833.91159828985109925, 529236.57355646649375558 179804.26158560626208782, 529461.54302770318463445 179967.33665536600165069, 529365.1804864815203473 180130.41172512577031739, 529330.03977657249197364 180104.57000673143193126, 529326.57823726569768041 180122.37220888037700206, 529506.08377560100052506 180233.14146669604815543, 529430.42441646789666265 180361.7129266606643796, 529518.94092159741558135 180419.07557802950032055, 529552.56730343436356634 180373.58106142663746141, 529648.71743816568050534 180427.49491339456290007, 529608.480220987345092 180501.82199512678198516, 529569.44679091090802103 180572.25595415246789344, 529667.74284364131744951 180629.72475247565307654, 529730.9295924516627565 180529.48919386579655111, 529787.31384936452377588 180567.2724588074197527, 529763.12702995492145419 180622.33490404754411429, 529706.82561028259806335 180576.71049719117581844, 529752.5037739867111668 180495.92673939117230475, 529740.29997511499095708 180487.27313655486796051, 529754.05698475218378007 180486.60747479822020978, 529655.30026389332488179 180435.30486135667888448, 529710.55415456288028508 180348.79930473779677413, 529762.78538142039906234 180271.69259134616004303, 529740.02540547132957727 180257.68645230054971762, 529689.83674055791925639 180345.80841046242858283, 529824.728592021856457 180415.94968910259194672, 529890.00781108462251723 180459.31649564448161982, 529865.28168949380051345 180503.69017882505431771, 529855.61934717127587646 180535.74483229906763881, 529894.55648332042619586 180548.55958596843993291, 529890.50570647965651006 180564.17520972224883735, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530050.41157349967397749 180610.86616918962681666, 530235.09162783063948154 180613.78033897408749908, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530441.01278525067027658 180758.81861569813918322, 530400.55581117747351527 180811.16401171206962317, 530508.37677010952029377 180901.19154505711048841, 530524.57064777321647853 180911.87319211009889841, 530583.04193836136255413 180879.49776674556778744)</t>
-  </si>
-  <si>
-    <t>LineString (530577.55627936229575425 180873.29039143532281741, 530508.03351007960736752 180921.27411260729422793, 530398.23249808500986546 181052.05378589619067498, 530335.04888452554587275 181096.60453780728857964, 530313.7541854988085106 181095.4837641742778942, 530277.88942924339789897 181128.54658634730731137, 530208.96185081487055868 181204.75919339017127641, 530146.19852736778557301 181259.11671458987984806, 530115.37725246080663055 181311.23268852362525649, 530089.44054251117631793 181304.94443834689445794, 529993.94726804597303271 181289.97907443816075101, 529966.154449358349666 181292.82961994459037669, 529944.77535806014202535 181334.87516616433276795, 529944.77535806014202535 181344.13943906020722352, 529926.36038226482924074 181394.46298536835820414, 529818.3114558468805626 181372.26115117289009504, 529660.9002180868992582 181353.18405782332411036, 529658.19050382054410875 181346.70498227514326572, 529687.50564937863964587 181285.67399781054700725, 529721.54846181173343211 181300.10519003760418855, 529759.29157994396518916 181225.35901491285767406, 529693.52337177516892552 181197.2517148221086245, 529775.50000859634019434 181018.70994359909673221, 529775.97546259185764939 181007.7745017017587088, 529781.20545654278248549 181022.98902955889934674, 529838.73539000260643661 181058.17262522855889983, 529856.80264183296822011 181056.27080924643087201, 529884.37897357402835041 181053.41808527320972644, 529884.37897357402835041 181040.5808273937436752, 529841.11265998031012714 181013.00449565265444107, 529793.09180643118452281 180981.03021445288322866, 529813.06087424361612648 180938.71480885017081164, 529693.24646736856084317 180862.64216956440941431, 529636.19198790425434709 180936.81299286801367998, 529544.71261489775497466 181110.32049908270710148, 529503.09825374488718808 181088.19581229900359176, 529492.28510446683503687 181074.0035538716474548, 529470.90163615171331912 181063.04265502601629123, 529432.46901320235338062 181041.241028774617007, 529404.33170837664511055 181030.67362469981890172, 529429.55946595408022404 180980.22139381090528332, 529341.93906022026203573 180918.15693974946043454, 529376.73622655984945595 180868.47114977936143987, 529404.34578149160370231 180829.45268785100779496, 529357.79744094552006572 180794.99778872131719254, 529292.81591668562032282 180885.3186391938070301, 529219.30587300169281662 180833.15022109559504315, 529297.55850014905445278 180694.72606625544722192, 529251.79900507966522127 180679.08758315991144627, 529252.95472623594105244 180654.80634892109083012, 529237.65350798552390188 180675.84590674249920994, 529186.38057327619753778 180657.79299018002348021, 529111.49788893118966371 180613.026168017211603, 529033.15595014626160264 180735.32098674381268211, 528988.79609909397549927 180702.76329789814190008, 529001.00523241108749062 180683.22868459072196856, 528968.42684971622657031 180655.33458768369746394, 528933.41540621093008667 180638.92297354058246128, 528917.00379206787329167 180629.07600505475420505, 528956.39166601130273193 180565.6177637014479842, 528889.09824919363018125 180520.36887541532632895, 529037.60859426553361118 180322.19037864034180529, 528980.81174594059120864 180277.24678561804466881, 528985.75060231669340283 180264.89964467784739099, 528967.47683372523169965 180262.43021648982539773, 528869.68747747887391597 180180.56867205633898266, 528753.13046700344420969 180299.10122508218046278, 528754.16503672057297081 180299.4973738573025912, 528770.91830490494612604 180309.96816647247760557, 528791.62720585486385971 180329.97901458147680387, 528777.89595665864180773 180339.10883718938566744, 528784.87936172517947853 180328.35022461912012659, 528766.49707728379871696 180311.67933983076363802, 528735.71864135982468724 180290.81664662051480263, 528713.38623358681797981 180285.77175626676762477, 528668.77996420615818352 180275.46013541670981795, 528678.81986454653088003 180236.4348891912959516, 528685.54394682915881276 180209.20438540610484779, 528648.68728152720723301 180200.38155767129501328, 528657.51626427297014743 180164.64456824841909111, 528561.08355491538532078 180139.08601459197234362, 528473.16496016969904304 180096.57592482483596541, 528471.71575256390497088 180078.58159705405705608, 528455.77446890133433044 180078.09852785218390636, 528452.87605368986260146 180092.59060390916420147, 528456.2575381031492725 180107.5657491680176463, 528445.63001566135790199 180136.06683208007598296, 528434.51942401775158942 180130.75307085920940153, 528435.00249321956653148 180119.15941001361352392, 528434.03635481582023203 180138.48217808958725072, 528458.18981491075828671 180158.28801536746323109, 528508.42901190835982561 180176.64464503963245079, 528492.97079744748771191 180232.19760325804236345, 528463.50357613165397197 180225.43463443146902137, 528442.73160045000258833 180280.1422215465863701, 528368.29083982005249709 180530.61085074103903025, 528399.42485451779793948 180540.37256290816003457, 528373.18561336421407759 180528.66321234643692151, 528398.20391442335676402 180451.73774791724281386, 528402.87839129334315658 180453.56406502836034633, 528495.6276780579937622 180483.51435554612544365, 528631.8531929935561493 180596.55254879055428319, 528664.70189872267656028 180554.04245902341790497, 528713.73342271556612104 180597.76022179532446899, 528701.17362346616573632 180617.08298987129819579, 528701.17362346616573632 180635.4396195434674155, 528716.6318379269214347 180666.35604846503701992, 528751.41282046365085989 180679.88198611821280792, 528786.19380300038028508 180647.03328038906329311, 528882.80764338024891913 180721.42593748154467903, 528908.89338028279598802 180749.44395119170076214, 528941.25901681010145694 180770.21592687338124961, 528984.08419391023926437 180821.70737133437069133, 528974.05492355371825397 180859.35868258221307769, 528989.1841545554343611 180829.86192138504702598, 529040.11857240251265466 180898.90430847753304988, 529112.31183115229941905 180989.06747418479062617, 529080.35383750754408538 181057.74321855726884678, 529150.25737489317543805 181094.96458261978114024, 529105.31938657385762781 181161.35024718247586861, 529063.5588317719521001 181143.64740329908090644, 529046.76382603647653013 181133.20726459860452451, 529038.72230120946187526 181129.90637958364095539, 529016.40501055552158505 181225.42438358269282617, 528860.85349469736684114 181191.94844760172418319, 528825.25553268182557076 181309.48477439771522768, 528674.92537136201281101 181261.00874411704717204, 528689.63158279552590102 181226.14957627476542257, 528640.0662035197019577 181213.07738833394250832, 528719.58868015988264233 181095.42769686627434567, 528668.38927739160135388 181063.29190151169314049, 528617.73454912076704204 181139.00165666910470463, 528598.12626720953267068 181160.78863657053443603, 528611.19845515035558492 181136.82295867896755226, 528206.1428879996528849 181051.66365116246743128, 528237.1932889255695045 180958.33994615747360513, 528214.42299491330049932 180950.7498481533548329, 527957.73968059255275875 180869.32879683657665737, 527979.60677813622169197 180868.6474805666366592, 527980.52286685828585178 180863.87237577338237315, 528002.11622184654697776 180796.95082105748588219, 528147.20215247070882469 180846.02662784914718941, 528143.09763044805731624 180858.87556635460350662, 528222.86812366941012442 180886.3580181579454802, 528226.97264569206163287 180877.07822923734784126, 528255.5258423708146438 180886.00110319946543314, 528274.28005263407249004 180832.49227053558570333, 528413.89659711671993136 180874.71776203761692159, 528440.4577933840919286 180872.67459309397963807, 528441.88889231265056878 180868.47956919606076553, 528480.12932370661292225 180756.38422738478402607, 528315.31369558570440859 180703.26183484998182394, 528079.46642620186321437 180632.41520988091360778)</t>
-  </si>
-  <si>
-    <t>LineString (528078.36375248804688454 181310.06427945720497519, 528120.39353655825834721 181328.79462172722560354, 528099.23992964578792453 181396.49718135065631941, 528083.2094619075069204 181447.06752287576091476, 527892.05577444343362004 181391.53930473059881479, 527886.54702264338266104 181381.62355149036739022, 527894.36945019953418523 181395.8361311347107403, 528096.21011615579482168 181454.44925028792931698, 528174.43439171742647886 181477.365657776419539, 528210.57180352613795549 181486.17966065660584718, 528186.33329560561105609 181562.09026046219514683, 528058.53025384293869138 181521.54584721333230846, 528025.91844318632502109 181610.126576159207616, 528008.71294296334963292 181668.53094684361713007, 527974.16629928222391754 181658.69760866125579923, 527946.58959034748841077 181751.49542285426286981, 527954.90637558174785227 181756.52926654869224876, 528111.16470766742713749 181801.12569479394005612, 528175.52004705951549113 181808.29031149361981079, 528172.01824275031685829 181825.36160750081762671, 528149.81553756294306368 182021.61447876173770055, 528104.60850979876704514 182012.27041250278125517, 528152.75831904984079301 182029.34170851000817493, 528168.07871290249750018 181874.8245933678408619, 528216.66624769219197333 181878.76412321566022001, 528233.97450602473691106 181880.77550011838320643, 528312.01526012923568487 181886.28911337567842565, 528336.83830706239677966 181958.7224278392677661, 528364.07657583232503384 181967.85795997321838513, 528398.32810312346555293 181877.94770083410548978, 528435.48417966347187757 181756.45373819654923864, 528556.93269398633856326 181793.33950502122752368, 528601.07048073236364871 181658.00311254803091288, 528462.81105602439492941 181615.32684191930457018, 528543.19771087332628667 181342.55578955341479741, 528848.09397080901544541 181432.12983202037867159, 528821.39401584293227643 181512.22969691874459386, 528869.62619255587924272 181528.59418544638901949, 528825.70046019228175282 181657.78751592763001099, 528781.18706770276185125 181829.79148424055892974, 528840.64356546348426491 181663.36835393149522133, 528928.19383570738136768 181689.65520411299075931, 528953.17121293372474611 181619.02951678325189278, 528997.95823416719213128 181634.5327164409973193, 529113.40120173222385347 181668.62010940056643449, 529255.4526879689656198 181785.48692165815737098, 529207.81271354551427066 181851.48813622404122725, 529209.79771247983444482 181862.901880096324021, 529201.85771674255374819 181846.52563888826989569, 529049.81566479301545769 181789.52457975188735873, 528954.52870295522734523 181766.80601999314967543, 529040.88659724884200841 181487.92052047938341275, 529208.07499765011016279 181542.65362748788902536, 529285.99421999289188534 181467.49755145219387487, 529296.60062423895578831 181467.17206752439960837, 529335.06877524114679545 181403.05848252086434513, 529397.35054353030864149 181423.20846637911745347, 529313.08697466843295842 181608.2219545322295744, 529347.89149224187713116 181631.11966346204280853, 529360.003021250362508 181638.69174143215059303, 529446.90093042538501322 181699.64433337154332548, 529416.11189753527287394 181753.80004300863947719, 529422.43464536091778427 181758.47337835803045891, 529443.87700755218975246 181711.74002486409153789, 529454.04838448914233595 181691.12236891090287827, 529472.12319620803464204 181661.08931673903134651, 529548.27107219526078552 181551.40338706798502244, 529523.80478713079355657 181530.78573111479636282, 529435.81869453191757202 181616.70519618046819232, 529478.4459440337959677 181645.69480029397527687, 529548.02589098876342177 181547.71293349421466701, 529541.20248039334546775 181540.13136616605333984, 529645.94890438881702721 181356.4556775517121423, 529665.98890690342523158 181359.0756422930280678, 529673.67560427926946431 181405.95077004205086268, 529767.56312223034910858 181439.16828370295115747, 529790.27442454162519425 181451.8257157189946156, 530012.95905668172053993 181535.92978279336239211, 530061.70118646346963942 181447.04707554430933669, 530133.46244322671554983 181459.83858795103151351, 530142.41057766624726355 181451.52960597147466615, 530121.31854648748412728 181417.01537313338485546, 530163.50260884512681514 181331.36894349814974703, 530208.22465636255219579 181366.63554168166592717, 530234.10646259249188006 181373.52784813527250662, 530191.7715905592776835 181481.05309050341020338, 530283.50257032876834273 181549.71721571101807058, 530311.93380967248231173 181491.24542158891563304, 530426.19520552584435791 181514.31227615085663274, 530446.77953103894833475 181528.09228405426256359, 530452.47980525041930377 181521.3478456501616165, 530415.45271119684912264 181496.96883923502173275, 530453.46287902258336544 181405.91857528948457912, 530484.62340791756287217 181368.68222978565609083, 530453.29358863539528102 181346.97811556659871712, 530395.29544163832906634 181277.22392895829398185, 530367.43655410828068852 181235.61759427358629182, 530392.94670032931026071 181209.0107060651644133, 530410.88688604242634028 181193.34473685521516018, 530334.12094446760602295 181103.43394227110547945, 530405.62894483865238726 181057.16405967809259892, 530487.65282761713024229 180959.89214740874012932, 530516.46695041528437287 180923.52303003016277216, 530505.78459265665151179 180899.06605305644916371, 530529.67934027465526015 180911.15398420437122695, 530582.29576928459573537 180878.9198528709821403, 530582.29576928459573537 180878.9198528709821403)</t>
-  </si>
-  <si>
     <t>LineString (530580.2603085950249806 180875.74680006815469824, 530531.28659617097582668 180919.46416819942533039, 530563.88801023468840867 180944.97831833627424203, 530620.69896473211701959 180923.3214464345946908, 530631.52323099854402244 180940.26917490593041293, 530672.45004481147043407 181008.75894496028195135, 530717.5530641155783087 181038.41000394721049815, 530783.43270573788322508 181058.76900571642909199, 530778.00363859941717237 181104.28964556960272603, 530801.95612234645523131 181156.06284796763793565, 530751.4015138226095587 181178.39113339898176491, 530780.09174134500790387 181213.18420375051209703, 530814.09418500657193363 181239.43468773260246962, 530853.48855285136960447 181252.44053536702995189, 530912.3730502761900425 181206.08465441560838372, 531047.80579616781324148 181254.33936599228763953, 531131.03878337366040796 181286.03806058526970446, 531110.30965442163869739 181356.39285153028322384, 531197.1542466712417081 181376.88721254793927073, 531286.93602178571745753 181375.08379181567579508, 531305.25734407640993595 181583.75572135805850849, 531325.21203300100751221 181586.18808011634973809, 531388.88918386655859649 181572.61640889989212155, 531390.49493819230701774 181599.32936576748033985, 531367.26279260986484587 181685.65545662579825148, 531395.89248193160165101 181593.61920236010337248, 531412.32238542404957116 181591.09869188832817599, 531419.12145480117760599 181581.94767167716054246, 531385.41458384564612061 181534.11455342586850747, 531374.38023236603476107 181529.41130202304339036, 531413.36951656360179186 181525.26491641241591424, 531471.93530321691650897 181443.00015478587010875, 531489.86913823755457997 181396.66486753628123552, 531500.42645009863190353 181343.75654840667266399, 531561.43261282751336694 181271.18043218745151535, 531510.99066478840541095 181339.18317034683423117, 531566.52648988855071366 181353.74707860476337373, 531590.37191976455505937 181360.8123911606380716, 531583.52515332715120167 181463.7283773985109292, 531566.74728090583812445 181537.16921628548880108, 531557.91564021108206362 181566.97600363052333705, 531578.66999584389850497 181574.92448025586782023, 531607.15203708468470722 181582.43137484646285884, 531674.27250636543612927 181614.50127011956647038, 531688.84471351187676191 181590.65584024353302084, 531676.92199857381638139 181529.27593741449527442, 531692.81895182456355542 181520.00271468493156135, 531744.15286336338613182 181527.39921376685379073, 531827.17028589476831257 181517.68440900254063308, 531837.76825472852215171 181595.40284711701679043, 531873.09481750777922571 181627.19675361836561933, 531892.79980997554957867 181649.86393449633033015, 531906.87584316555876285 181666.05597267561824992, 532031.40197696257382631 181539.76351073960540816, 532080.85916485369671136 181575.09007351889158599, 532117.06889170245267451 181580.38905793579760939, 532140.91432157845702022 181599.81866746442392468, 532170.05873587145470083 181590.98702676958055235, 532184.18936098308768123 181559.19312026820261963, 532149.74596227332949638 181529.16554190579336137, 532138.2648293700767681 181394.04143927496625111, 532132.82734409463591874 181370.85496780133689754, 532125.90053239720873535 181323.38831371636479162, 532096.75611810432747006 181293.36073535395553336, 532017.27135185094084591 181313.67350895205163397, 532018.15451592043973505 181340.1684310365235433, 532031.40197696257382631 181369.31284532946301624, 532033.16830510157160461 181389.62561892755911686, 532057.23452599509619176 181405.74336319562280551, 532119.69996919808909297 181395.70321314127068035, 532140.79753599606920034 181364.76011517079314217, 532132.3034719011047855 181288.28254195442423224, 532160.56472212448716164 181242.35801034132600762, 532384.22602272103540599 181180.09494344278937206, 532424.85156991728581488 181173.91279495641356334, 532670.78084617818240076 181110.13770430514705367, 532818.19047775026410818 181176.80775713562616147, 532780.99707011831924319 181260.68462679820368066, 532688.27519202104303986 181257.87865509698167443, 532650.54560429917182773 181265.88190097737242468, 532436.45877699879929423 181308.18477205943781883, 532413.59236019768286496 181321.90462214010767639, 532414.73568103776779026 181427.0901394252141472, 532338.13318475405685604 181459.10312294677714817, 532350.7097139946417883 181509.40923990920418873, 532405.30328410735819489 181674.61910129722673446, 532528.63901972828898579 181635.46036252533667721, 532616.67472441249992698 181609.7356436240952462, 532545.63823982118628919 181643.35478146860259585, 532594.42826642119325697 181790.64542780804913491, 532462.787251255242154 181845.87942018534522504, 532437.01138814585283399 181871.65528329473454505, 532445.2964870025170967 181957.26797147953766398, 532616.5218633720651269 181942.53890684561338276, 532701.21398501726798713 181920.44530989468330517, 532802.42052498331759125 181910.09618882910581306, 532815.01476064522285014 182025.01858924416592345, 532915.61185974825639278 182009.02176296585821547, 532912.46310028480365872 181963.04987479909323156, 532924.13200544030405581 182009.18769421585602686, 532982.27383896452374756 182001.80460424453485757, 533061.71429885365068913 181990.75895807769848034, 533064.2333064244594425 181966.82838615524815395, 533035.89447125315200537 181858.51106061163591221, 532947.72920627577695996 181893.14741470987792127, 532880.60253748437389731 181721.24718533383565955, 532784.00711035938002169 181767.39149765466572717, 532747.24231199838686734 181784.20146203070180491, 532733.93556229211390018 181745.29988511741976254, 532713.1074947752058506 181674.74374392238678411, 532748.93080092582385987 181661.89110736449947581, 532742.91467317531351 181642.74888270380324684, 532713.65441547974478453 181552.64369662242825143, 532855.62877998419571668 181525.1299014599644579, 533071.32848995237145573 181469.8718779842602089, 533186.19458453194238245 181444.03007418513880111, 533181.16196181264240295 181435.64236965295276605, 533152.08458610100205988 181436.48114010615972802, 533186.47417468298226595 181432.28728784006671049, 533189.54966634477023035 181438.99745146580971777, 533257.37403261545114219 181533.14433782830019481, 533340.41452438081614673 181492.83427136726095341, 533338.70870435202959925 181483.54382457892643288, 533339.90022310265339911 181474.30955426144646481, 533358.96452311298344284 181468.35196050821105018, 533371.7733496823348105 181461.2028480043518357, 533421.18748124549165368 181431.14743276051012799, 533457.81188699707854539 181401.60169366677291691, 533466.42939423269126564 181399.13954874229966663, 533532.90730719361454248 181489.9311428323853761, 533627.23823461274150759 181537.48131668634596281, 533600.77017667470499873 181593.49511371820699424, 533571.96468304062727839 181647.30677931586978957, 533565.79550759738776833 181677.67810457508312538, 533571.43902549741324037 181761.11675010700128041, 533688.88424648460932076 181775.70174559103907086, 533695.46948461106512696 181806.18034129549050704, 533711.03833596489857882 181690.5134740429057274, 533774.42839107918553054 181698.56300485107931308, 533904.80115716229192913 181714.28477588956593536, 533897.61435122019611299 181746.38584243066725321, 534052.37023917213082314 181783.27811293312697671, 534085.0618540165014565 181674.51498261015512981, 534131.12462164927273989 181691.05033509369241074, 534139.47207866376265883 181655.85994260499137454, 534150.19790721382014453 181658.82599177915835753)</t>
   </si>
   <si>
-    <t>LineString (534494.76712749910075217 180197.82926488673547283, 534477.08958587038796395 180204.9261592309048865, 534466.10449469194281846 180201.48237478407099843, 534446.35375012725125998 180105.42193530994700268, 534275.77913797693327069 180170.50961626204662025, 534224.15787377348169684 180196.54468864286900498, 534203.5093680921709165 180212.25550818303599954, 534185.55414576060138643 180210.4599859498848673, 534171.14064759924076498 180237.33092047309037298, 534155.10926930524874479 180232.7692223628400825, 534110.10282780381385237 180227.94574123568600044, 534059.63022310636006296 180244.41244702640688047, 534045.56321658962406218 180253.93444574531167746, 534018.52404629567172378 180285.19719793670810759, 534005.14660858130082488 180295.44406237191287801, 533989.44804280833341181 180338.41282897180644795, 534003.21356487192679197 180354.3808345656725578, 534155.73554933757986873 180422.10720311899785884, 534135.36257668328471482 180462.85314842750085518, 534160.69113728043157607 180481.57425843409146182, 534211.8988793573807925 180382.46249957560212351, 534228.96812671632505953 180379.70939516284852289, 534265.3091049644863233 180416.35643082388560288, 534271.73921295220497996 180462.74348229306633584, 534252.4929513584356755 180455.64950213933479972, 534269.62446292664390057 180472.076978985540336, 534255.40823154035024345 180562.17560434373444878, 534234.92044681450352073 180597.79788426094455644, 534256.13046408852096647 180604.31816759763751179, 534251.89312430669087917 180626.73219362733652815, 534379.78553101746365428 180633.41155169066041708, 534352.34416242560837418 180636.5838860665098764, 534344.23650324332993478 180704.43507658550515771, 534297.84553046221844852 180708.00611733732512221, 534240.14221260114572942 180695.98651926324237138, 534189.34860979067161679 180672.75587819167412817, 534160.54824850801378489 180757.54946950945304707, 534160.5841055567143485 180757.22253176767844707, 534127.8658005315810442 180858.10397226159693673, 534111.99208847992122173 180939.00866548559861258, 534085.5094500295817852 180985.32051877162302844, 534070.93534209730569273 180988.37091345511726104, 534075.68040049390401691 180998.87782847607741132, 534054.99797940440475941 181035.08444935575244017, 534068.56281289900653064 181030.73750628152629361, 534096.52225887367967516 180994.37437144466093741, 534118.50570094562135637 180998.44537923578172922, 534120.13410406210459769 181012.28680572554003447, 534190.96963962737936527 181035.08444935575244017, 534233.56329029169864953 181041.4142344745923765, 534230.7365170813864097 181061.51134635950438678, 534425.65412626438774168 181087.91946370297227986, 534428.68984542321413755 181124.52763081435114145, 534418.41545121860690415 181314.94640340618207119, 534244.43570935411844403 181318.37120147436507978, 534082.24461821641307324 181331.92378598402137868, 534008.65777000458911061 181337.21434369860799052, 534003.03775836550630629 181356.73341751954285428, 533970.61429565714206547 181390.91446260787779465, 533908.72647818853147328 181354.13541679794434458, 533820.00587128894403577 181301.66338870135950856, 533762.7596401305636391 181265.19378197882906534, 533763.82057414436712861 181254.40761950571322814, 533775.00675160356331617 181229.54225989809492603, 533765.23515282932203263 181236.37174127201433294, 533750.68025846313685179 181246.3013364469516091, 533738.92612418869975954 181260.82114937415462919, 533558.01058455463498831 181157.44207860867027193, 533549.5142814606660977 181141.84867783010122366, 533537.31101294630207121 181133.86961764763691463, 533483.72784082207363099 181114.99530462495749816, 533375.88864138023927808 181117.98406295705353841, 533381.80025942670181394 181168.40668747131712735, 533323.37956343777477741 181201.44220008412958123, 533277.55680660111829638 181222.13016911473823711, 533325.81375910399947315 181204.22413798831985332, 533380.40929047460667789 181174.66604775583255105, 533399.53511356632225215 181212.91769393908907659, 533422.13835903815925121 181229.95706360254553147, 533476.03840593271888793 181291.15969749572104774, 533522.51176960719749331 181254.94408223693608306, 533527.5245621653739363 181246.81990119433612563, 533527.00599741796031594 181236.96717099371016957, 533512.83189432229846716 181222.62021298229228705, 533521.10348163370508701 181215.37559709040215239, 533538.7190823903074488 181185.9681870742351748, 533548.10621201666072011 181170.94877967197680846, 533562.65626293770037591 181116.50342783879023045, 533565.78408725361805409 181068.52103992408956401, 533568.11593338451348245 181052.2709871992119588, 533565.98876765870954841 181030.01686012774007395, 533550.6638780701905489 180995.96154993091477081, 533517.88564200571272522 180943.17581912584137172, 533527.8685909277992323 180932.10417117548058741, 533519.96954229823313653 180930.1110331111412961, 533540.88975644903257489 180852.93240523023996502, 533549.08821875147987157 180816.53405966371065006, 533554.74233068409375846 180784.02291605086065829, 533498.69594615150708705 180775.96580654679564759, 533473.25244245456997305 180751.37041963971569203, 533450.91870032052975148 180721.12092079993453808, 533451.20140591717790812 180708.11646335478872061, 533482.01631595019716769 180701.33152903561131097, 533556.93329905800055712 180708.68187454805593006, 533574.10766405356116593 180706.42022977498709224, 533632.91042815323453397 180723.09985997635521926, 533664.85616057284642011 180736.10431742150103673, 533657.22310946369543672 180723.94797676627058536, 533653.26523111085407436 180708.11646335478872061, 533628.66984420374501497 180717.16304244706407189, 533572.27007767534814775 180700.55408864485798404, 533556.72126986051443964 180706.77361177079728805, 533481.23887555941473693 180699.42326625832356513, 533449.2931431399192661 180706.77361177079728805, 533440.52926964417565614 180711.01419572028680705, 533410.70382919942494482 180714.40666287989006378, 533368.01528410776518285 180716.38560205633984879, 533344.26801399048417807 180714.68936847653822042, 533317.41098231042269617 180704.51196699772845022, 533298.32835453760344535 180707.05631736741634086, 533274.0156732271425426 180725.43218114858609624, 533214.36479233752470464 180758.22603035805514082, 533150.04926910332869738 180796.6033151010342408, 533131.95611091877799481 180803.10554382362170145, 533112.94415954523719847 180814.13106209231773391, 533032.09035890805535018 180821.19870200814330019, 533006.17641249333973974 180714.80543799756560475, 532992.55450278345961124 180708.59827885474078357, 533019.41655259137041867 180701.98867611197056249, 533047.67523066280409694 180678.44941610301611945, 533062.18958536896388978 180672.97919573029503226, 533115.1629428390879184 180663.2515109057421796, 533114.02687698940280825 180650.64306823158403859, 532992.54919304675422609 180668.21878358686808497, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531644.05815143184736371 180909.64867640155716799, 531643.0989445325685665 180988.84512792871100828, 531556.3810018397634849 180988.02673437033081427, 531388.22242831636685878 180986.58758923810091801, 531389.17863833182491362 181128.18185803995584138, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531133.39463505509775132 181279.42110962877632119, 531076.29551051347516477 181260.61487964406842366, 531131.04354967980179936 181113.15854730040882714, 531036.5176723989425227 181074.07573265538667329, 530995.61705242155585438 181020.45047535176854581, 530934.72057378862518817 181004.99913002699031495, 530807.47420052578672767 181052.26206866747816093, 530678.41002193070016801 181020.45047535176854581, 530547.98248933651484549 181092.25378597865346819, 530470.12182414066046476 180975.54759959221701138, 530510.45278707984834909 180923.94229928601998836, 530504.58646519773174077 180903.04352758117602207, 530525.67277607112191617 180907.31886370456777513, 530582.29576928459573537 180878.9198528709821403)</t>
-  </si>
-  <si>
     <t>Initial Draft</t>
   </si>
   <si>
@@ -284,19 +242,61 @@
     <t>Team</t>
   </si>
   <si>
-    <t>LineString (530577.23797894886229187 180877.97880632089800201, 530617.74819760688114911 180823.78270298111601733, 530460.08680607296992093 180724.14946249785134569, 530317.89046422939281911 180623.28449239319888875, 530146.54318801360204816 180467.81284240834065713, 530072.77626957895699888 180399.24656015267828479, 530035.55066324456129223 180349.42993991106050089, 529890.48028561775572598 180246.51208710417267866, 529825.74567924335133284 180200.98946149481344037, 529919.54799574031494558 180130.36585574291530065, 529957.12143912480678409 179966.409011882962659, 529911.86251868435647339 179845.57623372576199472, 529906.73886731371749192 179702.96793724340386689, 529926.37953090108931065 179692.72063450215500779, 529923.81770521576981992 179643.19200458613340743, 529919.54799574031494558 179631.23681805469095707, 529921.4103331834776327 179584.29027873513405211, 529930.04384519555605948 179550.71550979930907488, 529930.52348475181497633 179516.66110130725428462, 529941.07555498881265521 179505.62939151405589655, 529912.29718161525670439 179479.72885547782061622, 529902.96647088008467108 179374.86438768959487788, 529800.47367502108681947 179363.00662448359071277, 529739.62031473114620894 179333.45689976593712345, 529740.46023528114892542 179272.14269961469108239, 529760.61832848156336695 179193.19016791306785308, 529641.34961037908215076 179153.71390206224168651, 529568.27652252756524831 179120.95700061158277094, 529550.34316133812535554 179093.66307770530693233, 529617.62970972212497145 178970.86160351810394786, 529616.82995180855505168 178944.1724078263505362, 529593.97022081958130002 178995.33693686561309732, 529513.20162077283021063 179036.94500355634954758, 529526.79745115165133029 179077.07363828388042748, 529564.38437103840988129 179130.25138729959144257, 529513.81095916836056858 179152.52902801893651485, 529512.12165939807891846 179263.45971292795729823, 529524.55590479262173176 179301.70093485678080469, 529448.61280135076958686 179371.58212878205813468, 529385.91768299601972103 179410.16374007728882134, 529333.16189551877323538 179435.02868727562599815, 529281.9714767278637737 179374.53091961363679729, 529220.891999761457555 179328.57588456268422306, 529164.02991525223478675 179367.55040796031244099, 529081.42719402140937746 179391.9821987469040323, 529060.48565906146541238 179415.83228022902039811, 529027.32822870835661888 179419.32253605569712818, 528999.98789139953441918 179308.21605890721548349, 529003.47814722615294158 179297.74529142724350095, 529055.25027532153762877 179270.40495411845040508, 529084.33574054366908967 179209.47090447816299275, 529104.11385689466260374 179164.09757873168564402, 529351.77659326093271375 179225.75876500256708823, 529383.05599977204110473 179235.19909444704535417, 529373.87950731569435447 179284.14038754784269258, 529392.23249222850427032 179227.24613431817851961, 529266.2086624939693138 179192.37546298385132104, 529269.26749331271275878 179176.46954272608854808, 529304.13816464703995734 179174.63424423482501879, 529268.04396098526194692 179166.06951794217457063, 529196.15887484396807849 179120.03240704443305731, 529149.98932790081016719 179107.75948950258316472, 529203.17197058210149407 179134.6430231656995602, 529187.39250517124310136 179174.383899015490897, 529058.81908330414444208 179141.07169425903703086, 529011.0423685876885429 179146.33151606269530021, 528858.21532395936083049 179161.52655682878685184, 528770.55162723187822849 179211.78707628592383116, 528715.03128597105387598 179321.6589095177478157, 528618.60121957084629685 179477.9925020151422359, 528491.34275315469130874 179622.19928313192212954, 528388.04569717741105705 179719.06766801583580673, 528360.57773886946961284 179750.62659883772721514, 528302.13527438452001661 179698.61280544605688192, 528281.73319864494260401 179662.65391637163702399, 528262.13372618111316115 179565.91304187983041629, 528297.16959096642676741 179504.60027850553160533, 528354.10287124256137758 179445.47725668028579094, 528571.1610022954409942 179230.06143178927595727, 528461.67392484133597463 179117.28974201151868328, 528427.73293083056341857 179154.51534834591438994, 528270.83738425537012517 178995.94010165525833145, 528307.81268304819241166 178962.03991528681945056, 528251.02088932693004608 178905.98091890395153314, 528237.09773989859968424 178880.69941073132213205, 528445.48698298842646182 178680.18773902862449177, 528506.68087698111776263 178769.79506966570625082, 528622.96355511201545596 178714.21878967669908889, 528690.51011079095769674 178852.7319798031821847, 528629.80371264915447682 178709.94369121600175276, 528706.32797509559895843 178677.88045276078628376, 528675.97477602458093315 178675.74290353045216762, 528565.03597096959128976 178505.16647494878270663, 528591.54158142581582069 178459.85043126542586833, 528535.96530143683776259 178489.77612049027811736, 528478.67898206354584545 178502.6014158723410219, 528322.21037840214557946 178459.85043126542586833, 528311.95014209649525583 178498.3263174116727896, 528292.28468917729333043 178492.34117956669069827, 528227.69070692639797926 178577.5864321083354298, 528109.89053357648663223 178750.95101042950409465, 528057.58673679200001061 178714.85402391621028073, 528050.95667804463300854 178736.21754654651158489, 528039.90658013243228197 178798.09809485499863513, 528075.26689345156773925 178816.51492470869561657, 528057.36634973983746022 178881.49318986901198514, 528077.50150927738286555 178927.95894264802336693, 527957.20683819404803216 178903.17720783254480921, 527893.18735658738296479 178892.33519885077839717, 527838.97731167858000845 178884.59090672095771879, 527827.61901655478868634 178890.78634042482008226, 527761.01810423820279539 178875.29775616514962167, 527777.55729742196854204 178801.08342777710640803, 527839.85880704678129405 178661.95543657644884661, 527875.91507322294637561 178584.04074644856154919, 527702.52480672812089324 178435.08524715233943425, 527673.89863282348960638 178393.55225022041122429)</t>
-  </si>
-  <si>
-    <t>LineString (532680.96280913078226149 178677.48286417848430574, 532646.72988178418017924 178686.93224038934567943, 532644.91513582807965577 178705.68461526944884099, 532577.46707779157441109 178826.97013667138526216, 532558.10978759278077632 178818.50132220939849503, 532477.21695213438943028 178782.04142910346854478, 532465.16113808494992554 178762.56665256191627122, 532448.46847247786354274 178772.14947911410126835, 532425.90246156463399529 178760.71191193890990689, 532423.12035063013900071 178744.32836976903490722, 532352.79476867453195155 178710.47935339916148223, 532245.37437425879761577 178647.41817221697419882, 532184.94074229244142771 178616.19670506301918067, 532251.30818086618091911 178452.11467546166386455, 532511.10399071127176285 178585.03346189408330247, 532598.70955449633765966 178413.85017633717507124, 532702.58256901206914335 178176.74428570797317661, 532815.09900265594478697 177890.48924129054648802, 532856.91221495741046965 177792.91708755856961943, 532858.8989350259071216 177769.61827948209247552, 532770.30928106070496142 177726.3168125337397214, 532588.16317295876797289 177673.66873071744339541, 532472.21096532221417874 177646.21587158855982125, 532425.64025696949101985 177642.10992637852905318, 532411.25822669372428209 177649.51064796402351931, 532407.54009782173670828 177671.5538405618572142, 532404.75150116789154708 177727.19298332382459193, 532429.18491946905851364 177794.11930301843676716, 532358.00930963514838368 177800.49323822744190693, 532344.59748763276729733 177875.45337209175340831, 532340.61377812712453306 177908.3853706716618035, 532327.99869802594184875 177961.36870709658251144, 532247.2621853785822168 177940.65341766728670336, 532213.93181584810372442 177940.5206273504300043, 532181.53097853565122932 177966.54752945387735963, 532131.07065813092049211 178059.50075125196599402, 531992.96872860239818692 177958.58011044265003875, 531978.40126691607292742 177969.69867078488459811, 531975.51999578601680696 177976.24701426242245361, 531956.66076657059602439 177991.70110486945486628, 531930.72932639950886369 178011.6080690412200056, 531893.66570231656078249 178019.07318060554098338, 531849.13696666923351586 178060.9825788619054947, 531859.09044875507242978 178130.13308598485309631, 531859.16702702990733087 178134.34492127480916679, 531819.8686971872812137 178155.9232769338414073, 531814.8917296277359128 178147.84576965900487266, 531807.24648775579407811 178147.84155853773700073, 531681.84718574595171958 177939.97077090424136259, 531528.1577946882462129 178035.11182251141872257, 531487.49922562530264258 177974.93714029833790846, 531424.07185788720380515 178019.66156626751762815, 531347.63374804891645908 177870.85120349729550071, 531277.70100926072336733 177896.05951631630887277, 531112.62721886532381177 177774.89698050887091085, 531123.19844682177063078 177739.93061111477436498, 531112.62721886532381177 177703.33789895815425552, 531087.41890604631043971 177667.55835818278137594, 530999.59639687044546008 177661.05298713271622546, 530915.83974460093304515 177696.01935652681277134, 530878.43386106321122497 177734.03511860055732541, 530837.77529200038406998 177695.81606368144275621, 530831.67650664085522294 177668.57482240931130946, 530831.67650664085522294 177655.15749461855739355, 530794.67720879369881004 177645.80602373406873085, 530835.33577785652596503 177653.53115185603382997, 530871.92849001311697066 177554.32424334256211296, 531069.12254996818955988 177399.4150952129275538, 531020.61008431122172624 177322.7039789414848201, 531091.09575783216860145 177289.02749048147234134, 531153.74968985083978623 177288.24431633122731, 531216.40362186951097101 177277.2798782279714942, 531239.84660494257695973 177317.72826233872910962, 531211.70457696809899062 177219.32499111071228981, 531201.52331301511730999 177187.4106444887293037, 530917.23109648050740361 177149.81828527752077207, 530896.22850016714073718 177112.81085585197433829, 530778.53778894036076963 176970.21642869058996439, 530805.62878007220569998 176973.21251439995830879, 530899.60967810009606183 176912.9081048319931142, 530892.56111074797809124 176812.07443298946600407, 530912.92363865405786783 176700.86370365635957569, 530991.2410536773968488 176720.63885094976285473, 531176.07015313243027776 176705.75854209534008987, 531181.01259320287499577 176679.19053713156608865, 531173.18175361305475235 176619.08758663863409311, 530892.20482224225997925 176554.68621974403504282, 530879.22067569091450423 176529.75665836548432708, 530895.8881946955807507 176444.7932273649785202, 530920.42121049202978611 176275.10653477313462645, 530798.92437035741750151 176217.86283124817418866, 530745.23294417129363865 176147.84827024937840179, 530808.30562182224821299 176214.79391414625570178, 530927.40622285439167172 176269.47334575466811657, 530985.69952494266908616 176293.35631588246906176, 531191.53301749157253653 176335.15151360613526776, 531198.76075845130253583 176235.22013859765138477, 531207.48642726987600327 176156.30002914459328167, 531185.2742347844177857 176156.30002914459328167, 531209.55267773370724171 176148.55158990548807196, 531188.94265151466242969 175949.80426446883939207, 531154.94696310814470053 175823.53456467346404679, 531066.20655180979520082 175503.10660128630115651, 530998.72868066909722984 175231.84770217089680955, 531029.01404346199706197 175153.91027290970669128, 531021.65302618476562202 175139.83394162519834936, 531029.40146542387083173 175082.75377256359206513, 531032.75912242755293846 175056.73193078552139923, 531026.30208972818218172 175037.10255137970671058, 530966.8973888949258253 175050.27489808623795398, 530928.21976302622351795 175062.67240086884703487, 531062.91346513316966593 175558.95993413514224812, 530985.123753986437805 175577.28249899740330875)</t>
-  </si>
-  <si>
-    <t>LineString (530319.24822289927396923 177532.86330300656845793, 530283.00367995072156191 177511.02849130801041611, 530184.84259889076929539 177499.21280562478932552, 530113.65853050712030381 177494.05278513085795566, 530069.67329359170980752 177299.41811178030911833, 530023.48879483062773943 177179.55834118591155857, 530191.73232603189535439 177132.27421150187728927, 530094.96480481803882867 176769.12109921933733858, 529881.66167348786257207 176830.25587819798965938, 529842.9543123907642439 176768.22780633534421213, 529745.09127103956416249 176816.94227156793931499, 529690.3932994834613055 176733.5929815776180476, 529531.50871543935500085 176823.45393484842497855, 529513.38458597532007843 176824.64773978322045878, 529499.05892675823997706 176851.56261467593139969, 529271.26506909728050232 177111.75961302706855349, 529136.28157614718656987 177252.8598545910208486, 529045.9358032428426668 177206.80840826532221399, 528896.89055745047517121 177069.65020661591552198, 528719.06074102083221078 177058.62250209698686376, 528714.32951614784542471 177068.97205650678370148, 528710.55932132713496685 177045.83340986201073974, 528687.79030162561684847 177026.31710726069286466, 528651.71471196867059916 177031.34403368830680847, 528597.30562592856585979 177022.47298705135472119, 528633.38121558562852442 177062.39269691769732162, 528645.80068087729159743 177093.14565859251888469, 528659.99435549648478627 177110.29634875731426291, 528636.63393268582876772 177251.93739339418243617, 528627.29656225664075464 177420.25810052070301026, 528532.66370314673986286 177925.4865684756077826, 528554.77845204086042941 177948.92160088589298539, 528617.49191905430052429 177943.97053770063212141, 528827.74706898862496018 177946.61110473275766708, 528860.91919232998043299 177944.30060857962234877, 529088.99816973123233765 177901.39139430731302127, 529260.80006226000841707 177863.10317234124522656, 529404.71096551173832268 177897.76061463812948205, 529417.25365891447290778 177885.54799211447243579, 529376.32486991619225591 177854.85140036582015455, 529293.80715016182512045 177856.50175476088770665, 529251.55807764746714383 177854.19125860778149217, 529020.1783914560219273 177904.03196133946767077, 528852.00727859640028328 177934.72855308811995201, 528754.63636928622145206 177937.03904924125527032, 528579.45125024754088372 177935.38869484615861438, 528555.02600520011037588 177929.77748990285908803, 528554.69593432114925236 177897.76061463812948205, 528587.94057327986229211 177658.03592232000664808, 528599.48983881680760533 177670.76972791197476909, 528612.2236444087466225 177688.53782873795717023, 528710.54046897927764803 177690.61077383431256749, 528765.9177165535511449 177685.87261361404671334, 528789.90465266862884164 177690.01850380678661168, 528858.015705834957771 177683.20739849016536027, 528903.546464201528579 177615.09634532386553474, 528963.06960196862928569 177621.01904559918330051, 529007.48985403357073665 177597.03210948410560377, 529033.5497352450620383 177566.23406805237755179, 529046.80177711113356054 177501.01033127031405456, 529029.92208132648374885 177443.56013859962695278, 529030.81048636778723449 177437.933573338057613, 529046.80177711113356054 177434.08381815909524448, 529055.38969251036178321 177424.31136270478600636, 529129.12731093820184469 177415.4273122918093577, 529252.541577925439924 177354.34946570245665498, 529274.1594339304137975 177332.1393396699859295, 529378.18414042412769049 177463.05533711041789502, 529514.28841154393739998 177579.99861740384949371, 529522.47303623706102371 177587.32366964058019221, 530009.96149630157742649 177853.79645061693736352, 530094.68275518657173961 177878.00252458406612277, 530200.58432879275642335 177862.87372835460701026, 530315.37161932047456503 177998.80604608487919904, 530315.56318013661075383 177999.03289441973902285, 530312.13405959820374846 178036.68039025971665978, 530327.5800858890870586 178073.0888808025047183, 530359.94318859372287989 178068.67573043366428465, 530382.17224571469705552 178064.30687938295886852, 530409.71792252280283719 178051.83336535666603595, 530457.53305962367448956 178047.15579759678803384, 530484.55909291654825211 178044.27656433341326192, 530481.82446864934172481 178176.08545401293667965, 530480.73061894241254777 178201.7909221246954985, 530453.93130112381186336 178202.88477183159557171, 530434.6485230919206515 178208.30226855166256428, 530510.72968812065664679 178204.59099220877396874, 530560.83191874937620014 178250.05412740889005363, 530576.60484320647083223 178299.22853895186563022, 530595.16122492088470608 178402.68036700924858451, 530423.46094173076562583 178433.51663268019910902, 530418.27724980388302356 178499.91296551114646718, 530412.79759553028270602 178422.85328647977439687, 530401.85479763883631676 178248.42200085142394528, 530398.61737529921811074 178112.52069049383862875, 530397.05111636582296342 178067.79433303145924583, 530372.89449547010008246 178077.41707417467841879, 530341.8666145202005282 178078.87150609420496039, 530263.00199223437812179 178102.06698323713499121, 530128.67393126524984837 178193.75180186820216477, 530016.07499924581497908 178268.64121385099133477, 530002.24668997840490192 178279.27173925217357464, 529972.73623576539102942 178260.44271802250295877)</t>
-  </si>
-  <si>
-    <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529225.49949584668502212 178821.69789721473352984, 529270.770087662152946 178758.30559268582146615, 529337.70783226401545107 178657.27980173568357714, 529306.5308305585058406 178711.19551833867444657, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529684.84245063865091652 178849.14101684212801047, 529657.52491406002081931 178773.00064893162925728, 529696.44831980823073536 178755.84746999081107788, 529755.07401005295105278 178759.51157563112792559, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529877.37348464445676655 178984.43081074606743641, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530208.48382428544573486 179227.08777841698611155, 530200.14624832582194358 179282.94953734712908044, 530185.47211463667917997 179294.62214369073626585, 530196.47771490353625268 179309.6297804182395339, 530192.14217540447134525 179370.16058188583701849, 530171.13148398592602462 179464.20843871153192595, 530148.2424291695933789 179574.15693386044586077, 530133.06942986708600074 179585.28380001557525247, 530072.88319930084981024 179599.95103267458034679, 530076.42356580472551286 179662.66609645792050287, 530120.93103042512666434 179669.24106282231514342, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530887.07347942178603262 180750.79246864788001403, 530912.25232304760720581 180759.71698828696389683, 531106.04388992069289088 180804.06853912054793909, 531363.93330286943819374 180808.82664637052221224, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531469.1157709649996832 180836.43344559159595519, 531398.75209977955091745 180833.40343104291241616, 531375.85865652305074036 180811.85666091914754361, 531102.54545270372182131 180807.29027070096344687, 530885.10598675487563014 180755.68535418406827375, 530875.96761612175032496 180785.2506709385488648, 530899.35109391843434423 180802.98986099121975712, 530995.84153678070288152 180837.66191427601734176, 530981.05887840350624174 180885.83994180549052544, 530971.57197559298947453 180910.01476331148296595, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530841.84631613304372877 180962.22017306523048319, 530822.39289369573816657 180996.15798742827610113, 530834.18258258642163128 181050.89582870650338009, 530803.86623972468078136 181055.9485525168129243, 530670.81117938680108637 181018.05312393954955041, 530540.28248095407616347 181088.79125728373765014, 530466.175865069613792 180976.78921282212832011, 530516.46695041528437287 180923.52303003016277216, 530508.37677010952029377 180901.19154505711048841, 530529.67934027465526015 180911.15398420437122695, 530580.2603085950249806 180875.74680006815469824, 530580.2603085950249806 180875.74680006815469824)</t>
-  </si>
-  <si>
-    <t>OSRM Raw</t>
+    <t>LineString (530319.24822289927396923 177532.86330300656845793, 530283.00367995072156191 177511.02849130801041611, 530186.53159918775781989 177500.75693363504251465, 530191.28202805644832551 177442.68187571264570579, 530228.60428188741207123 177420.49186220247065648, 530205.81630437565036118 177311.74978444981388748, 530190.99136274226475507 177305.01601308811223134, 530190.99136274226475507 177289.17268055406748317, 530236.84007037524133921 177280.49666444247122854, 530175.25996776495594531 177097.85946075979154557, 530094.96480481803882867 176769.12109921933733858, 529881.66167348786257207 176830.25587819798965938, 529842.9543123907642439 176768.22780633534421213, 529745.09127103956416249 176816.94227156793931499, 529690.3932994834613055 176733.5929815776180476, 529531.50871543935500085 176823.45393484842497855, 529513.38458597532007843 176824.64773978322045878, 529499.05892675823997706 176851.56261467593139969, 529271.26506909728050232 177111.75961302706855349, 529136.28157614718656987 177252.8598545910208486, 529045.9358032428426668 177206.80840826532221399, 528896.89055745047517121 177069.65020661591552198, 528719.06074102083221078 177058.62250209698686376, 528714.32951614784542471 177068.97205650678370148, 528710.55932132713496685 177045.83340986201073974, 528687.79030162561684847 177026.31710726069286466, 528651.71471196867059916 177031.34403368830680847, 528597.30562592856585979 177022.47298705135472119, 528633.38121558562852442 177062.39269691769732162, 528645.80068087729159743 177093.14565859251888469, 528659.99435549648478627 177110.29634875731426291, 528636.63393268582876772 177251.93739339418243617, 528627.29656225664075464 177420.25810052070301026, 528532.66370314673986286 177925.4865684756077826, 528554.77845204086042941 177948.92160088589298539, 528617.49191905430052429 177943.97053770063212141, 528827.74706898862496018 177946.61110473275766708, 528860.91919232998043299 177944.30060857962234877, 529088.99816973123233765 177901.39139430731302127, 529260.80006226000841707 177863.10317234124522656, 529404.71096551173832268 177897.76061463812948205, 529417.25365891447290778 177885.54799211447243579, 529376.32486991619225591 177854.85140036582015455, 529293.80715016182512045 177856.50175476088770665, 529251.55807764746714383 177854.19125860778149217, 529020.1783914560219273 177904.03196133946767077, 528852.00727859640028328 177934.72855308811995201, 528754.63636928622145206 177937.03904924125527032, 528579.45125024754088372 177935.38869484615861438, 528555.02600520011037588 177929.77748990285908803, 528554.69593432114925236 177897.76061463812948205, 528587.94057327986229211 177658.03592232000664808, 528599.48983881680760533 177670.76972791197476909, 528612.2236444087466225 177688.53782873795717023, 528710.54046897927764803 177690.61077383431256749, 528765.9177165535511449 177685.87261361404671334, 528789.90465266862884164 177690.01850380678661168, 528858.015705834957771 177683.20739849016536027, 528903.546464201528579 177615.09634532386553474, 528963.06960196862928569 177621.01904559918330051, 529007.48985403357073665 177597.03210948410560377, 529033.5497352450620383 177566.23406805237755179, 529046.80177711113356054 177501.01033127031405456, 529029.92208132648374885 177443.56013859962695278, 529030.81048636778723449 177437.933573338057613, 529046.80177711113356054 177434.08381815909524448, 529055.38969251036178321 177424.31136270478600636, 529129.12731093820184469 177415.4273122918093577, 529252.541577925439924 177354.34946570245665498, 529274.1594339304137975 177332.1393396699859295, 529378.18414042412769049 177463.05533711041789502, 529514.28841154393739998 177579.99861740384949371, 529522.47303623706102371 177587.32366964058019221, 530009.96149630157742649 177853.79645061693736352, 530094.68275518657173961 177878.00252458406612277, 530200.58432879275642335 177862.87372835460701026, 530315.37161932047456503 177998.80604608487919904, 530315.56318013661075383 177999.03289441973902285, 530312.13405959820374846 178036.68039025971665978, 530327.5800858890870586 178073.0888808025047183, 530359.94318859372287989 178068.67573043366428465, 530382.17224571469705552 178064.30687938295886852, 530409.71792252280283719 178051.83336535666603595, 530457.53305962367448956 178047.15579759678803384, 530484.55909291654825211 178044.27656433341326192, 530481.82446864934172481 178176.08545401293667965, 530480.73061894241254777 178201.7909221246954985, 530453.93130112381186336 178202.88477183159557171, 530434.6485230919206515 178208.30226855166256428, 530510.72968812065664679 178204.59099220877396874, 530560.83191874937620014 178250.05412740889005363, 530576.60484320647083223 178299.22853895186563022, 530595.16122492088470608 178402.68036700924858451, 530423.46094173076562583 178433.51663268019910902, 530418.27724980388302356 178499.91296551114646718, 530412.79759553028270602 178422.85328647977439687, 530401.85479763883631676 178248.42200085142394528, 530398.61737529921811074 178112.52069049383862875, 530397.05111636582296342 178067.79433303145924583, 530372.89449547010008246 178077.41707417467841879, 530341.8666145202005282 178078.87150609420496039, 530263.00199223437812179 178102.06698323713499121, 530128.67393126524984837 178193.75180186820216477, 530016.07499924581497908 178268.64121385099133477, 530002.24668997840490192 178279.27173925217357464, 529972.73623576539102942 178260.44271802250295877)</t>
+  </si>
+  <si>
+    <t>LineString (534134.50261897931341082 179505.72398318111663684, 534161.12046731344889849 179478.51866212062304839, 534268.20681759295985103 179451.43236519605852664, 534371.78454269852954894 179453.52622194297146052, 534488.53814230323769152 179477.87973351695109159, 534494.98466007283423096 179461.40529921691631898, 534512.17537412513047457 179461.40529921691631898, 534518.69754681340418756 179450.22317049890989438, 534511.62516024080105126 179466.71508290435303934, 534496.16740915493573993 179464.36707008117809892, 534493.03672539070248604 179476.8898051381111145, 534702.1627230066806078 179526.04097460908815265, 534896.44344984879717231 179566.88705734140239656, 534992.27464395156130195 179584.69176007088390179, 535029.45505259244237095 179577.88407961549819447, 535044.64141668530646712 179593.07044370827497914, 535083.91649623564444482 179599.35445643632556312, 535105.91054078377783298 179581.02608597950893454, 535104.33953760180156678 179542.27467415656428784, 535130.5229239686159417 179493.57357551416498609, 535254.89400921121705323 179351.92145526938838884, 535306.21344649035017937 179301.64935344501282088, 535425.60968832322396338 179398.00421527508297004, 535482.16580287565011531 179449.32365255415788852, 535506.25451833324041218 179531.01581801878637634, 535495.78116378642152995 179448.01448323580552824, 535436.08304287004284561 179386.22169140999903902, 535314.5921301277121529 179290.91416503459913656, 535342.87018740398343652 179238.54739230085397139, 535185.76986920274794102 179129.62450501468265429, 535141.78178010636474937 179126.48249865067191422, 535084.17833009921014309 179183.03861320309806615, 535030.76422191085293889 179175.70726502037723549, 534880.99525189236737788 179072.02105500755715184, 534803.49242824641987681 179131.71917592402314767, 534766.83568733278661966 179183.03861320309806615, 534649.38990060472860932 179164.91539512970484793, 534665.24414822936523706 179156.85522683622548357, 534776.26170642487704754 178818.56587497628061101, 534718.65825641772244126 178795.5244949734187685, 534768.61604381597135216 178661.29493365884991363, 534831.21432475326582789 178556.21924779983237386, 534951.93958084657788277 178435.49399170652031898, 534952.41323877044487745 178422.29324807948432863, 534920.77471851953305304 178358.38970222626812756, 534943.4089064939180389 178356.70942969765746966, 534914.50966500455979258 178355.2571754687523935, 534945.52167990384623408 178429.81131229753373191, 534821.94349932007025927 178554.01599823284777813, 534758.03995346685405821 178664.43756643508095294, 534705.41350394068285823 178797.25670095355599187, 534598.28108883381355554 178810.41331333509879187, 534492.71493710565846413 178796.94344827780150808, 534245.87182861380279064 178820.75065163488034159, 534072.95635159919038415 178852.07591921000857837, 533911.31797091162297875 178832.02774796192534268, 533807.94458791369106621 178906.58188479070668109, 533667.60738917719572783 179024.36489087314112112, 533584.90868277894333005 179119.59370430145645514, 533452.08954826043918729 179157.18402539161616005, 533416.03695482644252479 179198.34173780240234919, 533214.01751468959264457 179290.00315991009119898, 533260.27816641773097217 179401.55670898006064817, 533255.47700564551632851 179411.57625896626268514, 533142.40450039238203317 179443.3381986441090703, 533048.38915894599631429 179483.99348143170936964, 532974.70145889348350465 179533.54210732915089466, 532794.61126092006452382 179654.87271689844783396, 532708.53640439314767718 179706.00943977979477495, 532693.2906733478885144 179712.36182771535823122, 532685.9464436424896121 179717.96226352726807818, 532658.78351692855358124 179728.82743421287159435, 532607.27455960412044078 179737.47932938844314776, 532548.11974142713006586 179741.40286324714543298, 532534.03526090865489095 179738.18355341436108574, 532548.52215515612624586 179713.23390221039880998, 532555.76560227992013097 179695.93011185922659934, 532523.17009022308047861 179679.43114896627957933, 532492.98906054079998285 179664.94425471880822442, 532479.7094074806664139 179651.26218792953295633, 532484.41954601428005844 179673.02428334188880399, 532449.79857150348834693 179748.49007901950972155, 532378.32551233028061688 179682.61488870403263718, 532357.40633448015432805 179686.00104389677289873, 532361.9146399162709713 179664.21872470591915771, 532197.54445065301842988 179511.6966937497491017, 532242.98194478405639529 179474.83317379461368546, 532244.69978968834038824 179458.70721855689771473, 532258.3818564775865525 179462.12773525423835963, 532327.39026551635470241 179384.03927239449694753, 532343.62657718255650252 179360.62614285058225505, 532356.44643774325959384 179329.55894946909393184, 532412.07767790672369301 179270.75782656238880008, 532414.88226228312123567 179257.70878397024353035, 532428.03560322884004563 179250.60044720803853124, 532448.61292798642534763 179227.50345003115944564, 532485.17324555455707014 179162.59509741654619575, 532492.73745000781491399 179103.45677169098053128, 532484.96392502961680293 179000.80637084558838978, 532493.42510495812166482 179058.75919992162380368, 532498.58643096906598657 179109.07884632432251237, 532488.92768669512588531 179168.71109358099056408, 532459.73001239355653524 179226.54700779423001222, 532606.87226027122233063 179362.21232334937667474, 532626.11217573913745582 179400.69215428520692512, 532679.98393904929980636 179385.30022191087482497, 532719.58761149924248457 179333.93767049448797479, 532820.3977558920159936 179207.26369896886171773, 532909.74552235088776797 179116.74030400396441109, 532941.48410618293564767 179098.9765160133538302, 532963.40215328731574118 179080.1896184952929616, 532976.27465714234858751 179080.88542951448471285, 532985.58112952392548323 179071.40500437797163613, 533037.41905045346356928 179058.18459501341567375, 533056.55385348107665777 179066.18642173407715745, 533060.32914265117142349 179065.0439605139545165, 533066.32706405699718744 179059.61726971823372878, 533052.61752941517625004 179038.19612184033030644, 533040.33607129845768213 178975.07513942685909569, 533032.33884275739546865 178967.93475680088158697, 533022.34230708109680563 178935.44601585279451683, 533014.34507853991817683 178938.30216890317387879, 533009.7752336593111977 178929.16247914195992053, 533004.63415816868655384 178922.59332712605828419, 533008.63277243915945292 178907.74133126405649818, 532948.08232777111697942 178850.76107790888636373, 532929.23171763855498284 178851.90353912903810851, 532820.69790172390639782 178835.33785143680870533, 532628.47880143311340362 178740.51357016403926536, 532649.04310339584480971 178706.81096416953369044, 532649.61433400597888976 178688.53158464707667008, 532680.96280913078226149 178677.48286417848430574)</t>
+  </si>
+  <si>
+    <t>LineString (532680.96280913078226149 178677.48286417848430574, 532646.72988178418017924 178686.93224038934567943, 532644.91513582807965577 178705.68461526944884099, 532577.46707779157441109 178826.97013667138526216, 532558.10978759278077632 178818.50132220939849503, 532477.21695213438943028 178782.04142910346854478, 532465.16113808494992554 178762.56665256191627122, 532448.46847247786354274 178772.14947911410126835, 532425.90246156463399529 178760.71191193890990689, 532423.12035063013900071 178744.32836976903490722, 532352.79476867453195155 178710.47935339916148223, 532245.37437425879761577 178647.41817221697419882, 532184.94074229244142771 178616.19670506301918067, 532251.30818086618091911 178452.11467546166386455, 532511.10399071127176285 178585.03346189408330247, 532598.70955449633765966 178413.85017633717507124, 532702.58256901206914335 178176.74428570797317661, 532815.09900265594478697 177890.48924129054648802, 532856.91221495741046965 177792.91708755856961943, 532858.8989350259071216 177769.61827948209247552, 532770.30928106070496142 177726.3168125337397214, 532588.16317295876797289 177673.66873071744339541, 532472.21096532221417874 177646.21587158855982125, 532425.64025696949101985 177642.10992637852905318, 532411.25822669372428209 177649.51064796402351931, 532407.54009782173670828 177671.5538405618572142, 532404.75150116789154708 177727.19298332382459193, 532429.18491946905851364 177794.11930301843676716, 532358.00930963514838368 177800.49323822744190693, 532344.59748763276729733 177875.45337209175340831, 532340.61377812712453306 177908.3853706716618035, 532327.99869802594184875 177961.36870709658251144, 532247.2621853785822168 177940.65341766728670336, 532213.93181584810372442 177940.5206273504300043, 532181.53097853565122932 177966.54752945387735963, 532131.07065813092049211 178059.50075125196599402, 531992.96872860239818692 177958.58011044265003875, 531978.40126691607292742 177969.69867078488459811, 531975.51999578601680696 177976.24701426242245361, 531956.66076657059602439 177991.70110486945486628, 531930.72932639950886369 178011.6080690412200056, 531893.66570231656078249 178019.07318060554098338, 531849.13696666923351586 178060.9825788619054947, 531859.09044875507242978 178130.13308598485309631, 531859.16702702990733087 178134.34492127480916679, 531819.8686971872812137 178155.9232769338414073, 531814.8917296277359128 178147.84576965900487266, 531807.24648775579407811 178147.84155853773700073, 531681.84718574595171958 177939.97077090424136259, 531528.1577946882462129 178035.11182251141872257, 531487.49922562530264258 177974.93714029833790846, 531424.07185788720380515 178019.66156626751762815, 531347.63374804891645908 177870.85120349729550071, 531277.70100926072336733 177896.05951631630887277, 531112.62721886532381177 177774.89698050887091085, 531123.19844682177063078 177739.93061111477436498, 531112.62721886532381177 177703.33789895815425552, 531087.41890604631043971 177667.55835818278137594, 530999.59639687044546008 177661.05298713271622546, 530915.83974460093304515 177696.01935652681277134, 530878.43386106321122497 177734.03511860055732541, 530837.77529200038406998 177695.81606368144275621, 530831.67650664085522294 177668.57482240931130946, 530831.67650664085522294 177655.15749461855739355, 530794.67720879369881004 177645.80602373406873085, 530835.33577785652596503 177653.53115185603382997, 530871.92849001311697066 177554.32424334256211296, 531069.12254996818955988 177399.4150952129275538, 531020.61008431122172624 177322.7039789414848201, 531091.09575783216860145 177289.02749048147234134, 531153.74968985083978623 177288.24431633122731, 531216.40362186951097101 177277.2798782279714942, 531239.84660494257695973 177317.72826233872910962, 531211.70457696809899062 177219.32499111071228981, 531201.52331301511730999 177187.4106444887293037, 530917.23109648050740361 177149.81828527752077207, 530896.22850016714073718 177112.81085585197433829, 530778.53778894036076963 176970.21642869058996439, 530805.62878007220569998 176973.21251439995830879, 530899.60967810009606183 176912.9081048319931142, 530892.56111074797809124 176812.07443298946600407, 530912.92363865405786783 176700.86370365635957569, 530991.2410536773968488 176720.63885094976285473, 531176.07015313243027776 176705.75854209534008987, 531181.01259320287499577 176679.19053713156608865, 531173.18175361305475235 176619.08758663863409311, 530892.20482224225997925 176554.68621974403504282, 530879.22067569091450423 176529.75665836548432708, 530895.8881946955807507 176444.7932273649785202, 530920.42121049202978611 176275.10653477313462645, 530798.92437035741750151 176217.86283124817418866, 530745.23294417129363865 176147.84827024937840179, 530808.30562182224821299 176214.79391414625570178, 530927.40622285439167172 176269.47334575466811657, 530985.69952494266908616 176293.35631588246906176, 531137.60294202796649188 176324.69043263891944662, 531143.68991781480144709 176256.46724120562430471, 531197.37760446465108544 176259.01963003000128083, 531201.64722321007866412 176158.07364397635683417, 531185.2742347844177857 176156.30002914459328167, 531202.25716874515637755 176148.72114577199681662, 531188.94265151466242969 175949.80426446883939207, 531154.94696310814470053 175823.53456467346404679, 531066.20655180979520082 175503.10660128630115651, 530998.72868066909722984 175231.84770217089680955, 531029.01404346199706197 175153.91027290970669128, 531021.65302618476562202 175139.83394162519834936, 531029.40146542387083173 175082.75377256359206513, 531032.75912242755293846 175056.73193078552139923, 531026.30208972818218172 175037.10255137970671058, 530966.8973888949258253 175050.27489808623795398, 530928.21976302622351795 175062.67240086884703487, 531062.91346513316966593 175558.95993413514224812, 530985.123753986437805 175577.28249899740330875)</t>
+  </si>
+  <si>
+    <t>v3 20230707</t>
+  </si>
+  <si>
+    <t>LineString (530577.23797894886229187 180877.97880632089800201, 530617.74819760688114911 180823.78270298111601733, 530460.08680607296992093 180724.14946249785134569, 530317.89046422939281911 180623.28449239319888875, 530146.54318801360204816 180467.81284240834065713, 530072.77626957895699888 180399.24656015267828479, 530035.55066324456129223 180349.42993991106050089, 529890.48028561775572598 180246.51208710417267866, 529825.74567924335133284 180200.98946149481344037, 529919.54799574031494558 180130.36585574291530065, 529957.12143912480678409 179966.409011882962659, 529911.86251868435647339 179845.57623372576199472, 529906.73886731371749192 179702.96793724340386689, 529926.37953090108931065 179692.72063450215500779, 529923.81770521576981992 179643.19200458613340743, 529919.54799574031494558 179631.23681805469095707, 529921.4103331834776327 179584.29027873513405211, 529930.04384519555605948 179550.71550979930907488, 529930.52348475181497633 179516.66110130725428462, 529941.07555498881265521 179505.62939151405589655, 529912.29718161525670439 179479.72885547782061622, 529902.96647088008467108 179374.86438768959487788, 529800.47367502108681947 179363.00662448359071277, 529739.62031473114620894 179333.45689976593712345, 529740.46023528114892542 179272.14269961469108239, 529760.61832848156336695 179193.19016791306785308, 529641.34961037908215076 179153.71390206224168651, 529568.27652252756524831 179120.95700061158277094, 529550.34316133812535554 179093.66307770530693233, 529617.62970972212497145 178970.86160351810394786, 529616.82995180855505168 178944.1724078263505362, 529593.97022081958130002 178995.33693686561309732, 529513.20162077283021063 179036.94500355634954758, 529526.79745115165133029 179077.07363828388042748, 529564.38437103840988129 179130.25138729959144257, 529513.81095916836056858 179152.52902801893651485, 529512.12165939807891846 179263.45971292795729823, 529524.55590479262173176 179301.70093485678080469, 529448.61280135076958686 179371.58212878205813468, 529385.91768299601972103 179410.16374007728882134, 529333.16189551877323538 179435.02868727562599815, 529281.9714767278637737 179374.53091961363679729, 529220.891999761457555 179328.57588456268422306, 529164.02991525223478675 179367.55040796031244099, 529081.42719402140937746 179391.9821987469040323, 529060.48565906146541238 179415.83228022902039811, 529027.32822870835661888 179419.32253605569712818, 528999.98789139953441918 179308.21605890721548349, 529003.47814722615294158 179297.74529142724350095, 529055.25027532153762877 179270.40495411845040508, 529084.33574054366908967 179209.47090447816299275, 529104.11385689466260374 179164.09757873168564402, 529351.77659326093271375 179225.75876500256708823, 529383.05599977204110473 179235.19909444704535417, 529373.87950731569435447 179284.14038754784269258, 529392.23249222850427032 179227.24613431817851961, 529266.2086624939693138 179192.37546298385132104, 529269.26749331271275878 179176.46954272608854808, 529304.13816464703995734 179174.63424423482501879, 529268.04396098526194692 179166.06951794217457063, 529196.15887484396807849 179120.03240704443305731, 529149.98932790081016719 179107.75948950258316472, 529203.17197058210149407 179134.6430231656995602, 529187.39250517124310136 179174.383899015490897, 529058.81908330414444208 179141.07169425903703086, 529011.0423685876885429 179146.33151606269530021, 528858.21532395936083049 179161.52655682878685184, 528770.55162723187822849 179211.78707628592383116, 528715.03128597105387598 179321.6589095177478157, 528618.60121957084629685 179477.9925020151422359, 528491.34275315469130874 179622.19928313192212954, 528388.04569717741105705 179719.06766801583580673, 528360.57773886946961284 179750.62659883772721514, 528302.13527438452001661 179698.61280544605688192, 528281.73319864494260401 179662.65391637163702399, 528262.13372618111316115 179565.91304187983041629, 528297.16959096642676741 179504.60027850553160533, 528354.10287124256137758 179445.47725668028579094, 528571.1610022954409942 179230.06143178927595727, 528461.67392484133597463 179117.28974201151868328, 528427.73293083056341857 179154.51534834591438994, 528270.83738425537012517 178995.94010165525833145, 528307.81268304819241166 178962.03991528681945056, 528251.02088932693004608 178905.98091890395153314, 528237.09773989859968424 178880.69941073132213205, 528445.48698298842646182 178680.18773902862449177, 528506.68087698111776263 178769.79506966570625082, 528622.96355511201545596 178714.21878967669908889, 528690.51011079095769674 178852.7319798031821847, 528629.80371264915447682 178709.94369121600175276, 528706.32797509559895843 178677.88045276078628376, 528675.97477602458093315 178675.74290353045216762, 528565.03597096959128976 178505.16647494878270663, 528591.54158142581582069 178459.85043126542586833, 528535.96530143683776259 178489.77612049027811736, 528478.67898206354584545 178502.6014158723410219, 528322.21037840214557946 178459.85043126542586833, 528311.95014209649525583 178498.3263174116727896, 528292.28468917729333043 178492.34117956669069827, 528227.69070692639797926 178577.5864321083354298, 528109.89053357648663223 178750.95101042950409465, 528057.58673679200001061 178714.85402391621028073, 528050.95667804463300854 178736.21754654651158489, 528039.90658013243228197 178798.09809485499863513, 528075.26689345156773925 178816.51492470869561657, 528057.36634973983746022 178881.49318986901198514, 528077.50150927738286555 178927.95894264802336693, 527957.20683819404803216 178903.17720783254480921, 527893.18735658738296479 178892.33519885077839717, 527901.3675460263621062 178842.38277947145979851, 527870.26802183757536113 178834.76434196019545197, 527853.8672185888281092 178819.73012841463787481, 527876.57178353331983089 178723.1521395173331257, 527822.2081079538911581 178692.29039585794089362, 527839.85880704678129405 178661.95543657644884661, 527875.91507322294637561 178584.04074644856154919, 527702.52480672812089324 178435.08524715233943425, 527673.89863282348960638 178393.55225022041122429)</t>
+  </si>
+  <si>
+    <t>LineString (527158.31216002732980996 177000.8693951431196183, 527099.77578929206356406 176863.97566198912682012, 526993.89284357777796686 176974.11520853615365922, 526965.6928630608599633 177009.76424051032518037, 526918.33817879669368267 176978.37180936889490113, 526881.62499661440961063 176915.05487198193441145, 526809.33459098706953228 176814.57045149418991059, 526803.78523573139682412 176782.81458185013616458, 526837.9906987837748602 176724.64684572990518063, 526829.14218303072266281 176698.07787916850065812, 526713.59169160143937916 176585.58887918625259772, 526702.01159683079458773 176498.87495989364106208, 526728.35331819928251207 176459.47930909239221364, 526759.08459305611904711 176456.02855037362314761, 526877.73335154261440039 176444.22870948346098885, 526952.37421362893655896 176459.79166246333625168, 526957.30744241294451058 176431.45683538325829431, 527038.82798124512191862 176435.9939717588131316, 527098.5913686784915626 176454.87681948934914544, 527051.24293423152994365 176594.92815045249881223, 527174.99744662863668054 176650.61612686808803119, 527153.14015064027626067 176640.28990523278480396, 527205.55905537132639438 176487.71942607063101605, 527102.71056710940320045 176449.37945362422033213, 527080.02346470882184803 176442.65865531019517221, 527118.21201132400892675 176315.62328595775761642, 527136.13724749034736305 176310.16777929847012274, 527123.4023648789152503 176243.66339232763857581, 527158.08696234272792935 176237.9932378021767363, 527169.22996887960471213 176208.6499966005794704, 527150.43826302816160023 176186.18838753091404215, 527118.65549396350979805 176157.02174997527617961, 527093.6976608419790864 176147.4813768335734494, 527018.22708262107335031 176131.11693114246008918, 526849.86647974920924753 176114.85084184003062546, 526845.07710992521606386 176097.65762165782507509, 526857.65365130186546594 176044.64240146498195827, 526893.8380195926874876 176044.15844629961065948, 526858.37810308812186122 176039.0902959554514382, 526874.83542804175522178 175886.27227852959185839, 527054.69047931989189237 175862.7618143102445174, 527176.94489326048642397 175856.8841982554004062, 527195.27535622008144855 175822.70450227480614558, 527223.9658216992393136 175795.75699128504493274, 527224.12844125344417989 175773.97201046324335039, 527243.25712752784602344 175756.61424477020045742, 527267.78618826356250793 175718.31265972839901224, 527222.48707379773259163 175682.39379150536842644, 527195.04935412993654609 175648.09664192068157718, 527009.0825874931178987 175569.97535675560357049, 526824.66230209683999419 175469.42516340431757271, 526795.48152648622635752 175473.6317607709497679, 526758.33231608534697443 175456.72367672127438709, 526739.00449527858290821 175494.1876375125721097, 526659.79678197088651359 175453.90485760179581121, 526520.33526839537080377 175632.5364698740595486, 526494.29995637480169535 175591.88974311901256442, 526417.63095546839758754 175510.29328765845275484, 526347.42756016622297466 175447.95712626643944532, 526377.84023331629578024 175401.53346697887172922, 526474.02092083648312837 175290.30347386049106717, 526498.70052055746782571 175244.55399248562753201, 526475.29657367873005569 175230.89727244031382725, 526816.41278782673180103 175345.56198925705393776, 526851.47655176091939211 175305.71711282295291312, 526851.47655176091939211 175278.90286315878620371, 526865.43143400084227324 175215.89678796651423909, 526877.77642672799993306 175178.34743508807150647, 526907.09578445507213473 175139.25495811874861829, 526889.09267006127629429 175116.10809675537166186, 526973.96449506049975753 174912.93009145429823548, 526885.95633615972474217 174859.8365453231963329, 526909.64957838621921837 174789.88203135458752513, 526922.28532687691040337 174784.41939029871718958, 526957.33885194035246968 174894.75840272463392466, 526938.1368365534581244 174894.58398754562949762, 526918.67389838397502899 174882.02661713416455314, 526881.00047726207412779 174863.13230195376672782, 526645.98297396756242961 174831.60109246335923672, 526609.50912189844530076 174827.05741743353428319, 526567.45242367009632289 174822.48189269431168213, 526532.3543359829345718 174820.95671778128598817, 526511.19253406394273043 174818.36392042905208655, 526475.19840611529070884 174928.17651417059823871, 526482.59550444374326617 174953.18938274509855546, 526532.22763051942456514 174964.2464009866816923, 526571.62909553560893983 174894.99534126126673073, 526580.38497665035538375 174835.29615184283466078, 526489.64220873429439962 174815.59541933474247344, 526246.86550509929656982 174761.46815426199464127, 526221.64969290501903743 174759.09444567150785588, 526209.46505330502986908 174784.94649092113832012, 526160.02340298215858638 174854.23032570173381828, 526124.6438850344857201 174921.36244024016195908, 526014.36327163595706224 175074.63272621412761509, 526017.3072057357057929 175100.90490151091944426, 525993.2115238078404218 175089.59430634311866015, 525977.26344060234259814 175063.01416766727925278, 525818.40223485918249935 175038.85706352663692087, 525828.51382325252052397 174995.27803120561293326, 525849.7215751651674509 174948.58325841222540475, 525805.44013935560360551 174918.05182387726381421, 525814.23011417349334806 174839.56990586066967808, 525702.0009714097250253 174820.10639019258087501, 525698.8616946890251711 174722.78881185199134052, 525659.9346633527893573 174636.77262970581068657, 525565.36717306601349264 174664.02053710119798779, 525538.06676878000143915 174653.24728339188732207, 525493.99436724185943604 174553.83953325595939532, 525459.71583271224517375 174532.29302583733806387, 525496.93252734444104135 174407.42122147939517163, 525457.92714756459463388 174534.53035107266623527, 525490.77226448152214289 174556.32890400406904519, 525543.79577161197084934 174666.49996881955303252, 525536.72597066126763821 174676.51552016640198417, 525515.04797329346183687 174692.30743877869099379, 525500.11743205995298922 174748.58409419711097144, 525507.00845109077636153 174843.90985745683428831, 525596.59169849148020148 174873.7709399237355683, 525710.00638670718763024 174878.36495261095114984, 525777.76807384355925024 174928.89909217032254674, 525768.58004846912808716 175008.14581102479132824, 525718.31548450421541929 175117.9094939905917272, 525718.31548450421541929 175117.9094939905917272)</t>
+  </si>
+  <si>
+    <t>LineString (525578.32314166694413871 175779.89375719579402357, 525779.26792031072545797 175913.87857735189027153, 525794.67906692263204604 175913.40021600711042993, 525796.36541037389542907 175924.88107120373751968, 525831.44916197401471436 175948.5820945069717709, 525842.88386619929224253 175956.48243560802075081, 525966.89843111461959779 175827.58213343276293017, 526037.0428866392467171 175909.39836246441700496, 526083.99901098641566932 175909.39836246441700496, 526183.90565853379666805 175950.36008795883390121, 526213.87765279808081686 175990.32274697776301764, 526258.58368871151469648 176103.28294610444572754, 526151.85186089854687452 176147.91625591710908338, 526151.49614943633787334 176179.64869351152447052, 526047.38884781103115529 176231.98070609322167002, 526018.99594736774452031 176239.218112088565249, 526012.31526491045951843 176231.42398255510488525, 525961.23868289159145206 176229.001861541881226, 525788.46569891297258437 176403.76074188807979226, 525739.81123790750280023 176436.52803195299929939, 525728.0358450491912663 176477.41611387868761085, 525702.36593637219630182 176520.02743093523895368, 525681.16035963909234852 176514.67023260265705176, 525672.11343565175775439 176513.5143718154868111, 525598.1237177683506161 176794.07800558168673888, 525590.47065528121311218 176803.15163323399610817, 525576.05627165164332837 176800.20250201458111405, 525603.30556521995458752 176824.95719950424972922, 525545.77949344262015074 176885.87943373149028048, 525467.20725123130250722 176931.41561955848010257, 525439.5283931796438992 176951.95154650005861185, 525403.81373762898147106 177049.27398287542746402, 525403.81373762898147106 177092.13156953614088707, 525397.56367290765047073 177140.34635452943621203, 525389.52787540876306593 177153.73935036090551876, 525384.84032686776481569 177171.15024494181852788, 525401.57936285785399377 177193.54199610272189602, 525396.49806739354971796 177201.56509420418296941, 525394.6260111698647961 177214.66948776991921477, 525487.42651254346128553 177227.50644473225111142, 525492.50780800764914602 177223.22745907813077793, 525498.9792741967830807 177209.83568196554551832, 525499.70685131091158837 177208.33006480569019914, 525546.48938673955854028 177091.50102327833883464, 525607.1780920778401196 177105.30195335522876121, 525641.23937251162715256 177033.56127417489187792, 525704.87392115953844041 176980.53248363500460982, 525742.65693441918119788 176954.01808836506097578, 525749.9179498142329976 176950.09361684083705768, 525759.91741443739738315 176949.90844157003448345, 525789.17510722379665822 176925.28013055364135653, 525823.06218178023118526 176907.87365509843220934, 525834.31157948146574199 176917.87311972162569873, 525840.02393209061119705 176917.83761663141194731, 525839.83007433160673827 176904.55402936117025092, 525831.35577882663346827 176898.87676776724401861, 525816.50067409395705909 176887.31365200405707583, 525759.91843862924724817 176830.72846091576502658, 525971.4164017754374072 176713.56057522911578417, 525990.28241726732812822 176704.62404157503624447, 525990.28241726732812822 176695.68750792095670477, 526044.89456737553700805 176673.8426478776964359, 526231.32058888114988804 176565.61129584512673318, 526246.21481163799762726 176558.66065855862689205, 526279.02310593228321522 176632.42519633183837868, 526283.16126619779970497 176641.72923013736726716, 526326.25483707862440497 176694.1716895958816167, 526240.12421508901752532 176797.52843598343315534, 526248.73727728798985481 176850.9294216169801075, 526278.02168876444920897 176885.38167041284032166, 526272.85385144501924515 176930.16959384744404815, 526251.69148790801409632 176959.08371336333220825, 526325.95375438174232841 177013.98570174560882151, 526319.56678607675712556 177036.69492238553357311, 526275.62785452837124467 177115.78894070326350629, 526363.26278312434442341 177163.23261577691300772, 526280.99105564062483609 177311.16054981428897008, 526272.44164539803750813 177335.69364007547846995, 526250.13883606973104179 177367.10342987961485051, 526211.67648397688753903 177335.63154804351506755, 526185.76781282899901271 177337.73524490388808772, 526109.33917043660767376 177428.8673888374469243, 526184.45384267240297049 177332.04137422563508153, 526279.49768399423919618 177388.10410090390359983, 526392.28012242901604623 177439.78692706045694649, 526426.88133655081037432 177450.73667836480308324, 526443.39773776999209076 177459.56620775593910366, 526456.33326861797831953 177441.86628668761113659, 526426.8099234257824719 177445.81657967285718769, 526370.02369851002003998 177422.19351010789978318, 526421.35844583390280604 177339.17204928098362871, 526477.91752585000358522 177269.49535130927688442, 526501.99488521425519139 177262.22671452004578896, 526586.49278788908850402 177278.12685749647789635, 526586.49278788908850402 177263.58958391801570542, 526567.41261631727684289 177235.53718880962696858, 526548.32683216617442667 177195.86831152276135981, 526590.83281695051118731 177261.11110615459620021, 526601.66294423129875213 177281.92901748322765343, 526641.02188793767709285 177312.0588962123147212, 526727.77269911498297006 177419.49923139426391572, 526755.35873112105764449 177438.37388487218413502, 526797.46372734103351831 177454.34474550731829368, 526929.58630168635863811 177497.90163814864354208, 527031.94499939354136586 177545.81422005410422571, 527131.79582655231934041 177579.02292893503908999, 527156.87407868099398911 177613.12935183010995388, 527095.68314348696731031 177730.49557179247494787, 527136.81147697800770402 177756.57695400633383542, 527102.70505408302415162 177810.74597860436188057, 527125.77704604144673795 177823.78666971129132435, 527048.53602948493789881 177964.22488163207890466, 527026.87337462871801108 177950.0097189677762799, 526946.35645452653989196 177896.54735731321852654, 526834.03755092830397189 177803.64159754675347358, 526824.94913852983154356 177797.93363960826536641, 526784.72778616880532354 177851.09168424911331385, 526706.87674400769174099 177973.44731176737695932, 526634.32416085619479418 177927.33338179817656055, 526512.58338573749642819 178040.46622332264087163, 526519.31304050667677075 178017.6128924343502149, 526371.94527612451929599 177875.96814802818698809, 526382.33424909575842321 177860.83739275019615889, 526363.02973012148868293 177861.26396422297693789, 526282.97132645780220628 177789.13300047253142111, 526039.15440734755247831 178025.89499738009180874, 525946.02356363565195352 178113.06979876160039566, 525928.76722545002121478 178136.49907633577822708, 526006.53529266326222569 178197.5254068571375683, 525909.86526466929353774 178347.12092503774329089, 526031.45418893126770854 178419.44031195042771287, 525979.57233337289653718 178520.5659626150445547, 525986.60716124519240111 178488.0298837055452168, 525783.34360698144882917 178376.24297001594095491, 525732.83573407854419202 178350.98903356451774016, 525778.65115257329307497 178377.8639997206046246, 525731.46603016031440347 178455.16984871673048474, 525568.58136916358489543 178364.83045690337894484, 525496.7204893120797351 178324.45148632011841983, 525454.97274006495717913 178276.20203841981128789, 525308.00674845476169139 178392.76418910655775107, 525327.85414873412810266 178420.77501689142081887)</t>
+  </si>
+  <si>
+    <t>LineString (538057.11912127735558897 181862.36995379574364051, 538053.62050980445928872 181858.87134232284734026, 538078.00283839902840555 181725.81349199247779325, 537941.46179826941806823 181703.52107727742986754, 537993.7096452577970922 181642.91357477093697526, 538053.69201395311392844 181543.8893257146992255, 537933.4239803443197161 181488.67192663639434613, 538057.85222895222250372 181541.24191616984899156, 538066.94687634671572596 181538.87918232899392024, 538082.506038723513484 181524.15319597572670318, 538090.42530879157129675 181509.20216024381807074, 538125.44152047054376453 181443.09396750494488515, 538174.66927109437528998 181352.78140245075337589, 538212.79301781801041216 181233.2282937929558102, 538225.66242323035839945 181199.85061172995483503, 538241.47548658237792552 181194.25015179277397692, 538274.4193685658974573 181215.99311390187358484, 538284.63197198079433292 181249.59587352504604496, 538292.94811339187435806 181286.28655660181539133, 538290.81553514266852289 181260.73360870234319009, 538312.43949847598560154 181260.35753977482090704, 538331.80704824393615127 181267.31481493418687023, 538327.67029004113283008 181291.66527799205505289, 538335.56773751927539706 181269.47721126751275733, 538339.14039233094081283 181284.1438994413765613, 538474.63447606388945132 181330.39465194242075086, 538488.79537792666815221 181288.87746238996624015, 538509.7148920422187075 181224.50972664973232895, 538549.53403901937417686 181124.09031605365453288, 538569.65582116693258286 181131.19212151752435602, 538573.00177168450318277 181118.41270654619438574, 538582.57363540562801063 181121.34447346715023741, 538588.59396907058544457 181104.41239674753160216, 538561.66629002010449767 181093.31582571024773642, 538598.21099730290006846 180963.41196743381442502, 538615.37369384057819843 180937.37201406632084399, 538635.46388516668230295 180855.08748821140034124, 538664.80175754404626787 180853.98271477461094037, 538664.80175754404626787 180848.70435279875528067, 538705.12598798738326877 180838.79208001849474385, 538708.31755569379311055 180833.63647064674296416, 538729.99642427545040846 180840.20523449187749065, 538707.07831848983187228 180830.60309832252096385, 538703.25330118928104639 180837.43348635928123258, 538663.36383505456615239 180847.26924513219273649, 538663.91026609751861542 180852.73355556160095148, 538660.24865216040052474 180844.65553881169762462, 538640.96016229398082942 180837.16027083780500107, 538544.24186769349034876 180802.73511513255652972, 538450.80215935071464628 180793.71900292404461652, 538430.0377797189867124 180786.06896832288475707, 538416.10378812404815108 180768.30995942730805837, 538405.72159830818418413 180775.6867785069916863, 538415.28414155961945653 180756.83490752556826919, 538418.01629677438177168 180719.40438108413945884, 538406.54124487261287868 180719.40438108413945884, 538409.000184565782547 180685.25244090033811517, 538395.33940849232021719 180678.69526838505407795, 538382.49827898317016661 180675.41668212742661126, 538362.28033039439469576 180657.65767323184991255, 538356.81601996498648077 180676.23632869182620198, 538348.34633879945613444 180663.94163022565771826, 538323.75694186717737466 180621.86643991924938746, 538322.93729530274868011 180593.17881016488536261, 538328.4016057321568951 180552.46969746579998173, 538322.6640797812724486 180530.61245574819622561, 538329.76768333942163736 180524.87492979731177911, 538343.42845941300038248 180540.99464556406019256, 538349.98563192831352353 180540.99464556406019256, 538343.97489045595284551 180555.74828372345655225, 538352.71778714295942336 180560.93937863138853572, 538365.01248560915701091 180534.98390409172861837, 538371.84287364582996815 180527.88030053349211812, 538376.48753751092590392 180495.36765347851905972, 538383.86435659055132419 180427.33698863245081156, 538397.2519171426538378 180335.26335789696895517, 538386.32329628383740783 180280.34703808143967763, 538356.54280444351024926 180181.98945035215001553, 538349.86702627711929381 180158.3111812362622004, 538333.93950255436357111 180158.96128424536436796, 538325.81321494071744382 180125.48097927699564025, 538338.16517211345490068 180121.9054127269773744, 538312.80498378432821482 180015.22765528378658928, 538309.48158343171235174 179915.05087322887266055, 538303.30955420562531799 179855.22966688327142037, 538278.62143730116076767 179762.64922849129652604, 538277.6718943432206288 179740.33496898142038845, 538278.14666582213249058 179706.15142249822383747, 538284.31869504833593965 179692.38304960916866548, 538274.34849399072118104 179684.31193446728866547, 538260.58012110169511288 179479.68542704707942903, 538283.84392356942407787 179380.45818795004743151, 538276.46764299820642918 179373.42610627005342394, 538286.21778096398338675 179367.16458653993322514, 538328.94721406803000718 179194.82253968715667725, 538373.10096160881221294 179125.98067524185171351, 538412.337829110911116 179066.10921436137869023, 538405.98546794115100056 179059.09686761553166434, 538415.39026240026578307 179061.24182073780684732, 538432.44739647547248751 179038.1479516392282676, 538557.31229543488007039 178855.83570372880785726, 538560.63569578749593347 178836.37007309254840948, 538544.49346550367772579 178770.85160899977199733, 538392.56659224512986839 178811.6819561880256515, 538328.48941097827628255 178579.7348779343010392, 538315.17884117900393903 178559.57830087453476153, 538294.47845585108734667 178453.40847317627049051, 538304.19587160169612616 178433.00190009997459128, 538253.66530969843734056 178404.8213944231683854, 538283.78929852542933077 178333.88425944367190823, 538307.11109632684383541 178343.60167519428068772, 538318.77199522766750306 178346.5168999194575008, 538335.11924329411704093 178348.77976422818028368, 538281.84581537533085793 178321.25161896785721183, 538252.69356812338810414 178330.96903471846599132, 538232.28699504712130874 178316.39291109255282208, 538044.79800434643402696 178261.3466268312477041, 538019.15639011771418154 178253.05674019930302165, 538025.32914176001213491 178211.08202903144410811, 537920.39236384036485106 178207.37837804603623226, 537794.46823033690452576 178227.13118330150609836, 537698.17330471647437662 178260.46404217008966953, 537658.66769420565105975 178275.27864611166296527, 537636.4457882932620123 178285.15504873939789832, 537613.32763770420569927 178298.05650823522591963, 537459.7524428729666397 178375.6691471713129431, 537456.14730042521841824 178381.81708270622766577, 537556.97021414036862552 178513.66243141060112976, 537678.42049946112092584 178674.65567737040692009, 537642.61853993555996567 178704.28488525358261541, 537655.49145826080348343 178726.26947054677293636, 537656.62345710769295692 178743.01280580330058001, 537645.11526750994380563 178749.34231008208007552, 537658.54148870729841292 178753.46607802127255127, 537643.36394558555912226 178764.38451038327184506, 537846.50558974756859243 178742.98746254466823302, 537864.34695504221599549 178732.03885750484187156, 537921.10559516295325011 178705.15133090259041637, 537929.97295804345048964 178681.03210386767750606, 537934.22929222602397203 178722.8860566635557916, 537931.391736104269512 178762.2571478528843727, 537923.27317417750600725 178793.5180244478979148, 537919.38620787719264627 178840.16162005084333941, 537924.24491575255524367 178882.91824935356271453, 537923.94315128470771015 178917.25865100373630412, 537939.79278095357585698 179148.20369934543850832, 537945.62323040387127548 179326.0324075817479752, 537596.7680049566552043 179354.21291325855418108, 537587.05058920604642481 179321.17369970644358546, 537583.16362290584947914 179361.01510428398614749, 537578.30491503048688173 179418.34785721261869185, 537345.08693701564334333 179405.71521673683309928, 537341.19997071544639766 179448.9577168270770926, 537339.25648756534792483 179477.62409329140791669, 537446.14806082216091454 179485.39802589188911952, 537438.37412822165060788 179644.76364420205936767, 537455.86547657276969403 179648.650610502314521, 537520.97216210188344121 179645.73538577710860409, 537523.7159856699872762 179645.73538577710860409, 537550.12440935370977968 179645.73538577710860409, 537546.72331384103745222 179683.14743641699897125, 537621.06154433323536068 179697.72356004291214049, 537630.77896008384414017 179799.27055463689612225, 537550.12440935370977968 179816.76190298801520839, 537528.26022391486912966 179825.02170637605013326, 537537.97763966547790915 179912.96431891914107837, 537544.29395990341436118 179930.94153805778478272, 537492.79165642510633916 179940.65895380839356221, 537507.85365083860233426 179979.04274602336226963, 537506.88190926343668252 180020.8276337510033045, 537501.05145981314126402 180022.28524611360626295, 537502.02320138819050044 180025.68634162630769424, 537416.05443968356121331 180037.57935224322136492, 537411.13920003117527813 180046.84167782287113369)</t>
+  </si>
+  <si>
+    <t>LineString (525327.85414873412810266 178420.77501689142081887, 525434.3555114408954978 178547.73350585880689323, 525347.43806628719903529 178651.24739231160492636, 525430.2491754493676126 178706.68292819705675356, 525486.36910066672135144 178623.18742970289895311, 525558.91436985018663108 178563.64555782591924071, 525601.34650842915289104 178515.0539152596029453, 525591.59441469295416027 178508.14618219647672959, 525612.31761388236191124 178515.8665897376195062, 525739.09483245271258056 178641.42479659095988609, 525767.53843918326310813 178664.58601921438821591, 525708.21320228814147413 178737.72672223576228134, 525731.62045715074054897 178716.68428954426781274, 525769.37393091234844178 178666.83504263576469384, 525806.39432751352433115 178612.95387134497286752, 526026.40911028429400176 178722.27400289245997556, 526144.43453311175107956 178765.52555535719147883, 526255.77580733434297144 178814.4714835460181348, 526271.20979337661992759 178817.35269416749360971, 526312.78246261400636286 178730.88154215391841717, 526431.85428454133216292 178507.28957353180157952, 526371.81847308482974768 178458.83962042655912228, 526552.97916730435099453 178570.48516453863703646, 526555.08568700461182743 178631.57423584524076432, 526525.59441120142582804 178796.93603231309680268, 526496.81081177107989788 178977.54604629526147619, 526531.73185393039602786 178797.25923736946424469, 526578.25740370713174343 178795.88277246299549006, 526808.88298217917326838 178842.85059796637506224, 526867.58985495707020164 178857.72481234182487242, 526887.47400313417892903 178869.08718272874830291, 526862.61881791288033128 179084.26207193068694323, 526876.82178089639637619 179026.0299236977880355, 526893.15518832765519619 179011.11681256498559378, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527768.86287219019141048 179171.7344985579547938, 527738.35830124607309699 179152.01631094136973843, 527772.52151037787552923 179165.95770141950924881, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528513.98412839835509658 179812.26687349064741284, 528529.45710146625060588 179823.30889789306093007, 528599.09828376933000982 179804.26158560626208782, 529067.56848417001310736 179787.9540786303114146, 529126.86850953719113022 179829.46409638732438907, 529184.68603427021298558 179833.91159828985109925, 529236.57355646649375558 179804.26158560626208782, 529461.54302770318463445 179967.33665536600165069, 529365.1804864815203473 180130.41172512577031739, 529330.03977657249197364 180104.57000673143193126, 529326.57823726569768041 180122.37220888037700206, 529506.08377560100052506 180233.14146669604815543, 529430.42441646789666265 180361.7129266606643796, 529518.94092159741558135 180419.07557802950032055, 529552.56730343436356634 180373.58106142663746141, 529648.71743816568050534 180427.49491339456290007, 529608.480220987345092 180501.82199512678198516, 529569.44679091090802103 180572.25595415246789344, 529667.74284364131744951 180629.72475247565307654, 529730.9295924516627565 180529.48919386579655111, 529787.31384936452377588 180567.2724588074197527, 529763.12702995492145419 180622.33490404754411429, 529706.82561028259806335 180576.71049719117581844, 529752.5037739867111668 180495.92673939117230475, 529740.29997511499095708 180487.27313655486796051, 529754.05698475218378007 180486.60747479822020978, 529800.36167021188884974 180412.51190174778457731, 529824.728592021856457 180415.94968910259194672, 529890.00781108462251723 180459.31649564448161982, 529865.28168949380051345 180503.69017882505431771, 529855.61934717127587646 180535.74483229906763881, 529894.55648332042619586 180548.55958596843993291, 529890.50570647965651006 180564.17520972224883735, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530050.41157349967397749 180610.86616918962681666, 530235.09162783063948154 180613.78033897408749908, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530441.01278525067027658 180758.81861569813918322, 530400.55581117747351527 180811.16401171206962317, 530508.37677010952029377 180901.19154505711048841, 530524.57064777321647853 180911.87319211009889841, 530583.04193836136255413 180879.49776674556778744)</t>
+  </si>
+  <si>
+    <t>LineString (531565.23039256664924324 178567.62021348648704588, 531600.88228947878815234 178584.2162747971015051, 531772.37417057063430548 178639.05066937819356099, 531797.10340734256897122 178657.86639300896786153, 531837.96040722646284848 178713.77597179752774537, 531857.31372296100016683 178741.19316908807377331, 531868.06556503567844629 178749.79464274787460454, 531880.13844949356280267 178747.46484413990401663, 531893.87027424620464444 178732.70546787517378107, 531882.84744893456809223 178737.65639788802945986, 531874.82179012312553823 178745.74090769540634938, 531873.81108064437285066 178750.26503583858720958, 531928.47747769311536103 178812.55852085907827131, 531938.12053605390246958 178829.1566770619538147, 531932.74461501650512218 178852.9451276523177512, 531965.13453926669899374 178839.37092703295638785, 531981.7662949759978801 178846.35962438152637333, 532009.72108437039423734 178845.01564412217703648, 531981.39670040470082313 178850.0555700947297737, 531960.96820046263746917 178846.83001747232628986, 531933.5510031720623374 178860.26982006573234685, 531935.16377948329318315 178924.24328041044645943, 531930.32545054971706122 179009.45162885275203735, 531910.43454271147493273 179022.35383934245328419, 531885.70530593954026699 179057.83491818906622939, 531876.11210935655981302 179066.35873417466063984, 531831.93818780174478889 179086.51181359370821156, 531779.46893305156845599 179106.20686848048353568, 531672.18940927542280406 179157.81096578075084835, 531589.70353428379166871 179198.03799872964737006, 531556.67969205614645034 179124.41894058702746406, 531620.5699304185109213 179098.98690395732410252, 531635.7671230387641117 179139.9262799954158254, 531648.27035036904271692 179178.57474457612261176, 531695.00515957863535732 179157.60464692092500627, 531797.07743173581548035 179112.31386224390007555, 531810.86905931774526834 179106.1050852510088589, 531847.91815481544472277 179173.68914956544176675, 531891.07424407650250942 179215.21670715624350123, 531905.47685013443697244 179238.60377113270806149, 531919.96244928787928075 179292.40742513118311763, 531957.96748593868687749 179272.83832924981834367, 531967.94273236184380949 179364.63301262669847347, 531985.87575963942799717 179480.30103856680216268, 531979.93544435373041779 179495.99243743464467116, 531952.58757775544654578 179485.23262106810580008, 531939.54275271145161241 179490.46462862013140693, 531766.64450117154046893 179467.29959379057982005, 531761.71291867026593536 179464.16131401702295989, 531729.43346957070752978 179458.33308015181683004, 531718.67365320411045104 179473.57615333772264421, 531714.63872206665109843 179523.78862971480702981, 531716.09578053292352706 179527.48731659070472233, 531741.86680176388472319 179544.99216120038181543, 531751.2878118836088106 179549.55071448421222158, 531794.563677724217996 179583.10166665274300613, 531736.03185356059111655 179657.43647553340997547, 531711.23332369688432664 179690.98742770194076002, 531710.01770948793273419 179697.49096372016356327, 531768.36719152017030865 179689.71103278253576718, 531817.90347053715959191 179690.92664699154556729, 531827.62838420912157744 179689.71103278253576718, 531830.54585831076838076 179679.74299626867286861, 531848.91713031963445246 179689.19716539108776487, 531944.69973392877727747 179685.07748351542977616, 532042.54217847576364875 179713.40029641060391441, 532046.66186035145074129 179723.69950109976343811, 531964.78318307269364595 179783.43488829687703401, 531949.33437603886704892 179795.79393392385100015, 531887.02418766950722784 179851.66711936253705062, 531644.24913323228247464 179809.83732716954546049, 531648.01059164851903915 180039.80038389487890527, 531634.26440454111434519 180047.81851008319063112, 531623.9049881329992786 180054.69994857980054803, 531597.20816948893480003 180046.74794410250615329, 531509.86933764221612364 180049.32525078213075176, 531523.18559562193695456 180126.19637639203574508, 531515.31689772487152368 180157.06588352672406472, 531576.1272732806392014 180172.41316700863535516, 531565.55550737539306283 180212.44941103307064623, 531546.7916893131332472 180213.05469548667315394, 531534.08071578713133931 180378.90263577894074842, 531523.7637067319592461 180401.07970175734953955, 531452.49236999533604831 180382.73106677527539432, 531430.23252644832246006 180461.2673656364204362, 531482.0090381617192179 180489.08967605925863609, 531642.51904925843700767 180503.81476687197573483, 531641.9708823268301785 180395.39141782445949502, 531740.48138779681175947 180345.31959500885568559, 531899.45102110982406884 180269.32835973758483306, 531947.79937211831565946 180253.32166861725272611, 532077.03169044503010809 180211.29727531352546066, 532099.03156049200333655 180191.19724142824998125, 532036.57553188200108707 180178.45843636387144215, 532057.05969537724740803 180033.36227827219408937, 532071.14023115881718695 180019.57570919854333624, 532207.19135398743674159 180042.54381057742284611, 532098.64082088705617934 180352.62898129189852625, 532040.88056060869712383 180356.72434775123838335, 532096.3210087432526052 180363.38491236304980703, 532152.37729773903265595 180433.03831291184178554, 532202.94655013689771295 180431.75807867391267791, 532256.71638812962919474 180407.43362815340515226, 532374.97802585770841688 180393.35105153627227992, 532459.60804447636473924 180370.57185269574983977, 532461.19814912823494524 180285.76627126333187334, 532465.92665053717792034 180247.43457141483668238, 532493.4954023661557585 180222.92901423358125612, 532452.90807328466325998 180147.11494670400861651, 532527.19054349034558982 180142.52015473254141398, 532537.91172475717030466 180135.62796677529695444, 532618.38267560245003551 180157.40526832704199478, 532552.64666788431350142 180254.39529883849900216, 532628.93604597891680896 180260.83616025268565863, 532642.84987088851630688 180321.27857628939091228, 532664.46415251330472529 180368.25469532946590334, 532702.02634320827201009 180359.40188057228806429, 532839.63639755162876099 180333.20402154928888194, 532901.66608916665427387 180315.59065232524881139, 532923.87425036216154695 180282.66130986291682348, 533132.17148640297818929 180152.47553733742097393, 533126.72782159631606191 180120.77814802477951162, 533177.19047552125994116 179911.81100420773145743, 533177.19047552125994116 179911.81100420773145743, 533144.89093221118673682 179901.35225368669489399, 533108.5248437209520489 179872.42468329664552584, 533066.37324115261435509 179864.98616519634379074, 533049.84320092969574034 179750.92888765849056654, 533107.84760892775375396 179739.26681170516530983, 533140.86942005890887231 179734.16034606634639204, 533223.25373236555606127 179757.30965696240309626, 533248.27541399584151804 179688.03193979547359049, 533327.25541587651241571 179685.30849145477986895, 533413.72490069409832358 179664.20176681425073184, 533458.66179831593763083 179668.28693932530586608, 533460.88135104614775628 179717.44317431433591992, 533457.67475742171518505 179745.3986485997447744, 533465.68402344128116965 179805.36506646597990766, 533373.55403766862582415 179881.39677198612480424, 533374.91576183901634067 179946.07867007807362825, 533387.17127937218174338 180014.16487859591143206, 533381.73899602494202554 180032.14720059430692345, 533433.43858268216717988 179996.43141658138483763, 533486.57714380824472755 179980.80263642215868458, 533569.64231819997075945 179956.29160135574056767, 533665.64387221017386764 179901.82263454148778692, 533728.9640461317030713 179852.80056440862244926, 533763.00715039065107703 179912.03556581915472634, 533731.00663238728884608 179845.99194355684448965, 533825.00356353784445673 179775.30611803027568385, 533788.87545132858213037 179712.8257357390539255, 533730.70547138899564743 179746.56884022831218317, 533777.98611626459751278 179715.60685424524126574, 533886.92404989304486662 179672.03168079382157885, 534054.41612284700386226 179527.68891873603570275, 534134.50261897931341082 179505.72398318111663684)</t>
+  </si>
+  <si>
+    <t>LineString (530784.23736255615949631 182302.13991453754715621, 530778.6444442254723981 182309.68591545993695036, 530773.74559282837435603 182337.44607337698107585, 530858.50592793908435851 182423.17597282669157721, 530936.88755029300227761 182449.3031802780169528, 531037.31400393415242434 182542.38135682337451726, 531094.36521082976832986 182594.22753410961013287, 531155.37121963454410434 182521.76535719376988709, 531166.80187289451714605 182513.19236724881920964, 531203.95149598934222013 182472.57272441431996413, 531259.88004943984560668 182529.52187190589029342, 531326.62689972575753927 182604.63759332848712802, 531370.30832468345761299 182662.60733486112440005, 531384.59664125845301896 182683.83569091532262973, 531369.90008706704247743 182687.50982946317526512, 531339.69050345139112324 182687.10159184673102573, 531257.94092076190281659 182652.80963206687010825, 531233.85490139271132648 182679.95743355926242657, 531204.76797122228890657 182711.18761121592251584, 531182.72313993528950959 182813.24701532270410098, 531203.13502075662836432 182831.20947044549393468, 531268.45303938491269946 182871.21675685534137301, 531362.55180997133720666 182909.59109279947006144, 531365.40947328635957092 182920.61350844299886376, 531354.79529525921680033 182956.13018107216339558, 531444.90684366086497903 182988.57858534331899136, 531474.10273866006173193 182998.58689318058895878, 531486.5355991879478097 183012.4143484897504095, 531547.55104103893972933 183034.71440845559118316, 531569.85110100475139916 183061.97003730272990651, 531517.81762775115203112 183110.59655695044784807, 531527.72876551374793053 183131.65772469594958238, 531497.95239027438219637 183140.93648922778083943, 531508.4095920140389353 183177.7640257888706401, 531495.22442460327874869 183139.57250639220001176, 531524.09539462334942073 183130.25195701562915929, 531519.54878517135512084 183120.02208574867108837, 531516.59348902758210897 183111.38352778987609781, 531448.32344150589779019 183136.55978571731247939, 531241.26357583678327501 183121.43743597742286511, 531197.64141312555875629 183108.64160158214508556, 530715.12526052596513182 183043.21945667950785719, 530703.01725020399317145 183063.42695543030276895, 530695.13352120853960514 183041.84071603690972552, 530546.28326243243645877 183024.95802384099806659, 530541.22589214832987636 183004.5417986634420231, 530703.18488589045591652 182946.11745994322700426, 530775.51721857010852545 182908.57789488162961788, 530786.04660877038259059 182895.30170723787159659, 530795.49963942251633853 182875.6843990063352976, 530804.3135183157864958 182802.06196081181406043, 530806.59301448101177812 182793.73684438230702654, 530819.8735573566518724 182794.33149555584532209, 530807.31673856556881219 182782.83954266682849266, 530812.03824553836602718 182733.95805871355696581, 530761.76808306365273893 182714.23882370966020972, 530770.16958811797667295 182659.52488996647298336, 530712.95603303634561598 182638.97244784975191578, 530630.19079316093120724 182601.20039206769433804, 530615.74853653833270073 182603.42227770193130709, 530555.75762441393453628 182723.95957335943239741, 530539.09348215709906071 182717.29391645672149025, 530547.14781758119352162 182730.62523026211420074, 530461.60522066289559007 182906.15419536712579429, 530437.90885532670654356 182917.93718825542600825, 530382.0339413866167888 182876.71421071342774667, 530325.26406243664678186 182961.75723386157187633, 530268.29162278701551259 182922.72056224985863082, 530249.18178586428985 182908.73221319253207184, 530252.98490572301670909 182894.20538857823703438, 530184.08185019285883754 182852.74914162818458863, 530085.83308541483711451 182787.51840435751364566, 530111.18260209145955741 182744.29519918368896469, 529999.02136356220580637 182666.39424455061089247, 529961.66046464198734611 182715.15181299234973267, 529988.72742143063805997 182735.23374867427628487, 529986.10803851566743106 182740.763557050464442, 529932.80478152283467352 182814.59110673272516578, 529984.94386833114549518 182734.94270612817490473, 529957.00378390413243324 182716.02494063068297692, 530013.09155612858012319 182629.12904521985910833, 530018.17775851185433567 182621.49974164497689344, 530100.32880480831954628 182494.38274551162612624, 530104.0113532249815762 182482.84132467227755114, 530220.50368910923134536 182556.47051627180189826, 530255.09743770561181009 182478.63458192982943729, 530272.39431200386025012 182483.35191128388396464, 530279.47030603489838541 182470.7723663397191558, 530137.95042541308794171 182415.73685720900539309, 530133.8373461066512391 182413.51172491264878772, 530186.21162480069324374 182272.1011724385607522, 530075.7495097367791459 182226.86884083910263143, 530075.1733111577341333 182226.46204725949792191, 530187.16388441331218928 182265.91148495653760619, 530233.22869966924190521 182154.23642371431924403, 530357.8921046924078837 182201.72724467553780414, 530348.98757576220668852 182228.44083146619959734, 530358.86895656702108681 182231.0766534095746465, 530394.74696868821047246 182125.29837629428948276, 530508.99968287569936365 182165.49652313266415149, 530513.72136097133625299 182167.0985210579528939, 530567.86575565708335489 182188.16529536261805333, 530573.45622016047127545 182150.89553200689260848, 530664.76714038196951151 181926.34520778860314749, 530694.76100652059540153 181850.76066511913086288, 530759.06664636044297367 181869.87285391447949223, 530674.73822676041163504 181825.22436629422008991, 530573.75377231650054455 181777.63399121144902892, 530599.29007114132400602 181730.04361612870707177, 530646.88044622412417084 181748.21467864664737135, 530657.97477119497489184 181732.12790743884397671, 530724.74751764547545463 181760.6236275052651763, 530741.12779784575104713 181707.06197263259673491, 530773.19373494503088295 181600.7954151411249768, 530782.75100370426662266 181575.85406711159157567, 530688.89235894195735455 181552.28991476428927854, 530627.95015930733643472 181539.24596229381859303, 530599.01706093887332827 181486.621268884598976, 530600.06536160444375128 181482.63772635560599156, 530608.87108719476964325 181476.34792236247449182, 530639.82865497504826635 181423.25654537187074311, 530713.75870660948567092 181269.28719607146922499, 530693.84197932516690344 181263.16111494251526892, 530645.94210892508272082 181237.73285941511858255, 530707.03671619179658592 181120.0358954158728011, 530733.0917692908551544 181051.75368729417095892, 530735.53599696443416178 181033.12102656494244002, 530692.8715660268208012 181009.95126327298930846, 530547.98248933651484549 181092.25378597865346819, 530472.93963134801015258 180978.161691593733849, 530516.46695041528437287 180923.52303003016277216, 530552.73794393055140972 180906.14858023868873715, 530579.45680101704783738 180882.17122962352004834)</t>
+  </si>
+  <si>
+    <t>N7 Kings Cross</t>
+  </si>
+  <si>
+    <t>LineString (530577.55627936229575425 180873.29039143532281741, 530508.03351007960736752 180921.27411260729422793, 530398.23249808500986546 181052.05378589619067498, 530335.04888452554587275 181096.60453780728857964, 530313.7541854988085106 181095.4837641742778942, 530277.88942924339789897 181128.54658634730731137, 530208.96185081487055868 181204.75919339017127641, 530146.19852736778557301 181259.11671458987984806, 530115.37725246080663055 181311.23268852362525649, 530089.44054251117631793 181304.94443834689445794, 529993.94726804597303271 181289.97907443816075101, 529966.154449358349666 181292.82961994459037669, 529944.77535806014202535 181334.87516616433276795, 529944.77535806014202535 181344.13943906020722352, 529926.36038226482924074 181394.46298536835820414, 529818.3114558468805626 181372.26115117289009504, 529660.9002180868992582 181353.18405782332411036, 529658.19050382054410875 181346.70498227514326572, 529687.50564937863964587 181285.67399781054700725, 529721.54846181173343211 181300.10519003760418855, 529759.29157994396518916 181225.35901491285767406, 529693.52337177516892552 181197.2517148221086245, 529775.50000859634019434 181018.70994359909673221, 529775.97546259185764939 181007.7745017017587088, 529781.20545654278248549 181022.98902955889934674, 529838.73539000260643661 181058.17262522855889983, 529856.80264183296822011 181056.27080924643087201, 529884.37897357402835041 181053.41808527320972644, 529884.37897357402835041 181040.5808273937436752, 529841.11265998031012714 181013.00449565265444107, 529793.09180643118452281 180981.03021445288322866, 529813.06087424361612648 180938.71480885017081164, 529693.24646736856084317 180862.64216956440941431, 529636.19198790425434709 180936.81299286801367998, 529605.88993830105755478 180991.46413140607182868, 529541.23135347885545343 180948.44746960292104632, 529492.06945427530445158 181030.20584545240853913, 529469.24634072056505829 181064.96606145869009197, 529432.46901320235338062 181041.241028774617007, 529404.33170837664511055 181030.67362469981890172, 529429.55946595408022404 180980.22139381090528332, 529341.93906022026203573 180918.15693974946043454, 529376.73622655984945595 180868.47114977936143987, 529404.34578149160370231 180829.45268785100779496, 529357.79744094552006572 180794.99778872131719254, 529292.81591668562032282 180885.3186391938070301, 529219.30587300169281662 180833.15022109559504315, 529297.55850014905445278 180694.72606625544722192, 529251.79900507966522127 180679.08758315991144627, 529252.95472623594105244 180654.80634892109083012, 529237.65350798552390188 180675.84590674249920994, 529186.38057327619753778 180657.79299018002348021, 529111.49788893118966371 180613.026168017211603, 529033.15595014626160264 180735.32098674381268211, 528988.79609909397549927 180702.76329789814190008, 529001.00523241108749062 180683.22868459072196856, 528968.42684971622657031 180655.33458768369746394, 528933.41540621093008667 180638.92297354058246128, 528917.00379206787329167 180629.07600505475420505, 528956.39166601130273193 180565.6177637014479842, 528889.09824919363018125 180520.36887541532632895, 529037.60859426553361118 180322.19037864034180529, 528980.81174594059120864 180277.24678561804466881, 528985.75060231669340283 180264.89964467784739099, 528967.47683372523169965 180262.43021648982539773, 528869.68747747887391597 180180.56867205633898266, 528753.13046700344420969 180299.10122508218046278, 528754.16503672057297081 180299.4973738573025912, 528770.91830490494612604 180309.96816647247760557, 528791.62720585486385971 180329.97901458147680387, 528777.89595665864180773 180339.10883718938566744, 528784.87936172517947853 180328.35022461912012659, 528766.49707728379871696 180311.67933983076363802, 528735.71864135982468724 180290.81664662051480263, 528713.38623358681797981 180285.77175626676762477, 528668.77996420615818352 180275.46013541670981795, 528678.81986454653088003 180236.4348891912959516, 528685.54394682915881276 180209.20438540610484779, 528648.68728152720723301 180200.38155767129501328, 528657.51626427297014743 180164.64456824841909111, 528561.08355491538532078 180139.08601459197234362, 528473.16496016969904304 180096.57592482483596541, 528471.71575256390497088 180078.58159705405705608, 528455.77446890133433044 180078.09852785218390636, 528452.87605368986260146 180092.59060390916420147, 528456.2575381031492725 180107.5657491680176463, 528445.63001566135790199 180136.06683208007598296, 528434.51942401775158942 180130.75307085920940153, 528435.00249321956653148 180119.15941001361352392, 528434.03635481582023203 180138.48217808958725072, 528458.18981491075828671 180158.28801536746323109, 528508.42901190835982561 180176.64464503963245079, 528492.97079744748771191 180232.19760325804236345, 528463.50357613165397197 180225.43463443146902137, 528442.73160045000258833 180280.1422215465863701, 528368.29083982005249709 180530.61085074103903025, 528399.42485451779793948 180540.37256290816003457, 528373.18561336421407759 180528.66321234643692151, 528398.20391442335676402 180451.73774791724281386, 528402.87839129334315658 180453.56406502836034633, 528495.6276780579937622 180483.51435554612544365, 528631.8531929935561493 180596.55254879055428319, 528664.70189872267656028 180554.04245902341790497, 528713.73342271556612104 180597.76022179532446899, 528701.17362346616573632 180617.08298987129819579, 528701.17362346616573632 180635.4396195434674155, 528716.6318379269214347 180666.35604846503701992, 528751.41282046365085989 180679.88198611821280792, 528786.19380300038028508 180647.03328038906329311, 528882.80764338024891913 180721.42593748154467903, 528908.89338028279598802 180749.44395119170076214, 528941.25901681010145694 180770.21592687338124961, 528984.08419391023926437 180821.70737133437069133, 528974.05492355371825397 180859.35868258221307769, 528989.1841545554343611 180829.86192138504702598, 529040.11857240251265466 180898.90430847753304988, 529112.31183115229941905 180989.06747418479062617, 529080.35383750754408538 181057.74321855726884678, 529150.25737489317543805 181094.96458261978114024, 529105.31938657385762781 181161.35024718247586861, 529063.5588317719521001 181143.64740329908090644, 529046.76382603647653013 181133.20726459860452451, 529038.72230120946187526 181129.90637958364095539, 529016.40501055552158505 181225.42438358269282617, 528860.85349469736684114 181191.94844760172418319, 528825.25553268182557076 181309.48477439771522768, 528674.92537136201281101 181261.00874411704717204, 528689.63158279552590102 181226.14957627476542257, 528640.0662035197019577 181213.07738833394250832, 528719.58868015988264233 181095.42769686627434567, 528668.38927739160135388 181063.29190151169314049, 528617.73454912076704204 181139.00165666910470463, 528598.12626720953267068 181160.78863657053443603, 528611.19845515035558492 181136.82295867896755226, 528206.1428879996528849 181051.66365116246743128, 528237.1932889255695045 180958.33994615747360513, 528214.42299491330049932 180950.7498481533548329, 527957.73968059255275875 180869.32879683657665737, 527979.60677813622169197 180868.6474805666366592, 527980.52286685828585178 180863.87237577338237315, 528002.11622184654697776 180796.95082105748588219, 528147.20215247070882469 180846.02662784914718941, 528143.09763044805731624 180858.87556635460350662, 528222.86812366941012442 180886.3580181579454802, 528226.97264569206163287 180877.07822923734784126, 528255.5258423708146438 180886.00110319946543314, 528274.28005263407249004 180832.49227053558570333, 528413.89659711671993136 180874.71776203761692159, 528440.4577933840919286 180872.67459309397963807, 528441.88889231265056878 180868.47956919606076553, 528480.12932370661292225 180756.38422738478402607, 528315.31369558570440859 180703.26183484998182394, 528079.46642620186321437 180632.41520988091360778)</t>
+  </si>
+  <si>
+    <t>LineString (525813.62879803299438208 181444.3455462628044188, 525938.4894992244662717 181490.10516775862197392, 525950.2033640209119767 181472.33594733368954621, 525943.13234854943584651 181373.34173073348938487, 525962.06789837975520641 181288.70267443344346248, 526084.9407700706506148 181347.92177145567256957, 526141.85119377286173403 181374.63645114144310355, 526247.90762806567363441 181264.37710280925966799, 526196.01242155989166349 181214.6880689833778888, 526166.16735107859130949 181192.64317541586933658, 526187.1327016269788146 181205.25580382536281832, 526289.24206442979630083 181085.57761354133253917, 526304.73383384314365685 181090.14411224401555955, 526312.97320597257930785 181086.63195823784917593, 526423.70250916026998311 181197.57224821968702599, 526423.40014027606230229 181210.76514542126096785, 526440.61190727609209716 181208.4950954697560519, 526481.37747424189001322 181247.68218424991937354, 526436.7998225896153599 181292.98168183141387999, 526364.50886605237610638 181370.49790682113962248, 526315.65099693823140115 181327.24125062092207372, 526174.19306422164663672 181474.26841948175569996, 526118.98830004595220089 181451.55415104021085426, 526093.47386830300092697 181427.99858194089028984, 526147.53385363647248596 181372.97566176933469251, 526117.64916966739110649 181356.75464216282125562, 525896.63604345871135592 181252.18492163851624355, 525804.47871884633786976 181202.92109834335860796, 525674.52415049879346043 181177.43981043208623305, 525808.02069279435090721 181198.8358115378941875, 525864.59372291236650199 181229.60359984767274, 525899.00071198993828148 181072.78713039786089212, 525914.79815168655477464 180998.59706019930308685, 526038.20014135900419205 181021.09393767311121337, 526034.23010415781755 181034.3273950106522534, 526110.653320282115601 181059.4709639519569464, 526164.81034232175443321 180824.94568032599636354, 526232.31997911655344069 180857.46556634301668964, 526385.03995015844702721 180939.3827475757279899, 526403.75872426724527031 180965.03631317696999758, 526518.00100311415735632 180845.93953079267521389, 526544.3462272291071713 180802.71689747890923172, 526415.88937359000556171 180762.15805877896491438, 526543.08072616113349795 180799.48524305276805535, 526566.20990454801358283 180735.24582871556049213, 526773.2086006454192102 180792.2867543384199962, 526781.81037810200359672 180804.0292009754339233, 526876.82089265179820359 180898.32528518006438389, 526893.50918447971343994 180930.32612565089948475, 526924.34248529304750264 180944.76673002715688199, 526972.18770328722894192 180987.68083861388731748, 526822.07183925563003868 181156.94281222127028741, 526922.36106670461595058 181052.43190333811799064, 527056.51731256174389273 181181.75928882521111518, 527072.0604500574991107 181194.33582109218696132, 527105.36620856204535812 181208.59860649338224903, 527134.84456199198029935 181207.65720116312149912, 527141.67895267263520509 181237.20603345840936527, 527126.8461934340884909 181257.45282692171167582, 527004.39505052170716226 181384.53058732440695167, 526985.91159781138412654 181369.18001979179098271, 526928.28958167461678386 181432.30053406039951369, 526997.63798668433446437 181498.45083301386330277, 526991.12956032424699515 181511.24325723896618001, 526678.53803907369729131 181414.39224837144138291, 526667.31783640081994236 181399.6772284725739155, 526656.64944697415921837 181395.44666025164769962, 526645.98105754749849439 181403.90779669350013137, 526619.08016179490368813 181431.82035006419755518, 526630.85217771399766207 181442.85661498832632788, 526625.70192074938677251 181459.04313687709509395, 526679.9176372914807871 181475.29189143585972488, 526706.84188712364993989 181479.03970802802359685, 526704.67241586744785309 181483.81254479169729166, 526684.71328031027223915 181478.02728810845292173, 526671.31848243589047343 181522.68559793970780447, 526666.90397646627388895 181521.94984694477170706, 526673.52573542075697333 181504.29182306613074616, 526671.31848243589047343 181502.8203210762294475, 526664.32884798396844417 181521.58197144727455452, 526672.42210892832372338 181534.0897383613337297, 526664.69672348140738904 181552.11563773744273931, 526615.76928231760393828 181537.7684933360433206, 526607.67602137324865907 181540.71149731581681408, 526667.6397274611517787 181562.3241827923047822, 526633.51603102358058095 181673.21107818573364057, 526634.14788983517792076 181721.54827727310475893, 526750.40991116955410689 181719.96863024411140941, 526763.6789462132146582 181717.44119499769294634, 527047.06762321561109275 181716.49340678029693663, 527075.50126973760779947 181704.80401876571704634, 527090.57778861722908914 181720.29356452525826171, 527188.46480982354842126 181748.64203353796619922, 527263.33384336996823549 181773.11378883954603225, 527341.77672236878424883 181800.06906386234913953, 527457.35124988225288689 181828.41753287505707704, 527478.70498486375436187 181813.3316481038054917, 527501.72297252365387976 181756.39241547140409239, 527552.19019862043205649 181634.29178817657520995, 527576.96563832846004516 181539.9116470152803231, 527502.86533335037529469 181515.28355731410556473, 527511.7228042078204453 181503.83365596178919077, 527545.64043651556130499 181469.26791603030869737, 527474.56463378143962473 181422.82020299739087932, 527381.22077847318723798 181367.63679676040192135, 527435.71565961930900812 181312.86944120863336138, 527464.59794662659987807 181334.12244485557312146, 527517.74514231248758733 181280.34209467822802253, 527383.21302771475166082 181171.51255586085608229, 527413.66733776684850454 181131.1336214438197203, 527429.41461164352949709 181120.02025737526128069, 527508.38860920432489365 181143.15408535901224241, 527552.0115922475233674 181044.38326500484254211, 527617.38904907600954175 181065.27134975808439776, 527665.90049312810879201 181080.65138910515815951, 527880.71712640451733023 181139.95635454953298904, 527892.84981061285361648 181124.42310436989646405, 527898.57802572846412659 181147.61365187869523652, 528147.61506407021079212 181224.24573191639501601, 528390.99835214088670909 181293.8688241028576158, 528368.25337566784583032 181399.05101017700508237, 528327.16320699045900255 181385.98296514025423676, 528308.22175984270870686 181356.13857025865581818, 528284.80718849156983197 181340.66114173838286661, 528256.63033144187647849 181343.0422845876601059, 528236.78747436462435871 181362.88514166491222568, 528124.47690330736804754 181327.56485606741625816, 528078.36375248804688454 181310.06427945720497519)</t>
+  </si>
+  <si>
+    <t>LineString (528078.36375248804688454 181310.06427945720497519, 528120.39353655825834721 181328.79462172722560354, 528099.23992964578792453 181396.49718135065631941, 528083.2094619075069204 181447.06752287576091476, 527892.05577444343362004 181391.53930473059881479, 527886.54702264338266104 181381.62355149036739022, 527894.36945019953418523 181395.8361311347107403, 528096.21011615579482168 181454.44925028792931698, 528174.43439171742647886 181477.365657776419539, 528210.57180352613795549 181486.17966065660584718, 528186.33329560561105609 181562.09026046219514683, 528058.53025384293869138 181521.54584721333230846, 528025.91844318632502109 181610.126576159207616, 528008.71294296334963292 181668.53094684361713007, 527974.16629928222391754 181658.69760866125579923, 527946.58959034748841077 181751.49542285426286981, 527954.90637558174785227 181756.52926654869224876, 528111.16470766742713749 181801.12569479394005612, 528175.52004705951549113 181808.29031149361981079, 528172.01824275031685829 181825.36160750081762671, 528149.81553756294306368 182021.61447876173770055, 528104.60850979876704514 182012.27041250278125517, 528152.75831904984079301 182029.34170851000817493, 528168.07871290249750018 181874.8245933678408619, 528216.66624769219197333 181878.76412321566022001, 528233.97450602473691106 181880.77550011838320643, 528312.01526012923568487 181886.28911337567842565, 528336.83830706239677966 181958.7224278392677661, 528364.07657583232503384 181967.85795997321838513, 528398.32810312346555293 181877.94770083410548978, 528435.48417966347187757 181756.45373819654923864, 528556.93269398633856326 181793.33950502122752368, 528601.07048073236364871 181658.00311254803091288, 528462.81105602439492941 181615.32684191930457018, 528543.19771087332628667 181342.55578955341479741, 528848.09397080901544541 181432.12983202037867159, 528821.39401584293227643 181512.22969691874459386, 528869.62619255587924272 181528.59418544638901949, 528825.70046019228175282 181657.78751592763001099, 528781.18706770276185125 181829.79148424055892974, 528840.64356546348426491 181663.36835393149522133, 528928.19383570738136768 181689.65520411299075931, 528953.17121293372474611 181619.02951678325189278, 528997.95823416719213128 181634.5327164409973193, 529113.40120173222385347 181668.62010940056643449, 529255.4526879689656198 181785.48692165815737098, 529207.81271354551427066 181851.48813622404122725, 529209.79771247983444482 181862.901880096324021, 529201.85771674255374819 181846.52563888826989569, 529049.81566479301545769 181789.52457975188735873, 528954.52870295522734523 181766.80601999314967543, 529040.88659724884200841 181487.92052047938341275, 529208.07499765011016279 181542.65362748788902536, 529285.99421999289188534 181467.49755145219387487, 529296.60062423895578831 181467.17206752439960837, 529335.06877524114679545 181403.05848252086434513, 529397.35054353030864149 181423.20846637911745347, 529313.08697466843295842 181608.2219545322295744, 529347.89149224187713116 181631.11966346204280853, 529360.003021250362508 181638.69174143215059303, 529446.90093042538501322 181699.64433337154332548, 529416.11189753527287394 181753.80004300863947719, 529422.43464536091778427 181758.47337835803045891, 529443.87700755218975246 181711.74002486409153789, 529454.04838448914233595 181691.12236891090287827, 529472.12319620803464204 181661.08931673903134651, 529548.27107219526078552 181551.40338706798502244, 529523.80478713079355657 181530.78573111479636282, 529435.81869453191757202 181616.70519618046819232, 529478.4459440337959677 181645.69480029397527687, 529548.02589098876342177 181547.71293349421466701, 529541.20248039334546775 181540.13136616605333984, 529645.94890438881702721 181356.4556775517121423, 529665.98890690342523158 181359.0756422930280678, 529673.67560427926946431 181405.95077004205086268, 529767.56312223034910858 181439.16828370295115747, 529790.27442454162519425 181451.8257157189946156, 530012.95905668172053993 181535.92978279336239211, 530061.70118646346963942 181447.04707554430933669, 530133.46244322671554983 181459.83858795103151351, 530142.41057766624726355 181451.52960597147466615, 530121.31854648748412728 181417.01537313338485546, 530163.50260884512681514 181331.36894349814974703, 530208.22465636255219579 181366.63554168166592717, 530234.10646259249188006 181373.52784813527250662, 530191.7715905592776835 181481.05309050341020338, 530283.50257032876834273 181549.71721571101807058, 530311.93380967248231173 181491.24542158891563304, 530426.19520552584435791 181514.31227615085663274, 530446.77953103894833475 181528.09228405426256359, 530452.47980525041930377 181521.3478456501616165, 530415.45271119684912264 181496.96883923502173275, 530453.46287902258336544 181405.91857528948457912, 530484.62340791756287217 181368.68222978565609083, 530453.29358863539528102 181346.97811556659871712, 530395.29544163832906634 181277.22392895829398185, 530367.43655410828068852 181235.61759427358629182, 530392.94670032931026071 181209.0107060651644133, 530410.88688604242634028 181193.34473685521516018, 530334.12094446760602295 181103.43394227110547945, 530405.62894483865238726 181057.16405967809259892, 530486.81822421168908477 180959.05754400324076414, 530519.31806703854817897 180916.11851573517196812, 530582.29576928459573537 180878.9198528709821403, 530582.29576928459573537 180878.9198528709821403)</t>
+  </si>
+  <si>
+    <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529270.770087662152946 178758.30559268582146615, 529304.71750739659182727 178689.86743865112657659, 529337.70783226401545107 178657.27980173568357714, 529305.00792290433309972 178707.29236911991029046, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529684.84245063865091652 178849.14101684212801047, 529657.52491406002081931 178773.00064893162925728, 529696.44831980823073536 178755.84746999081107788, 529755.07401005295105278 178759.51157563112792559, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529877.37348464445676655 178984.43081074606743641, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530137.16457231086678803 179220.90265564562287182, 530137.2566814114106819 179287.56575694994535297, 530164.29013196483720094 179289.33844223213964142, 530181.6477391414809972 179297.81860453309491277, 530196.47771490353625268 179309.6297804182395339, 530192.14217540447134525 179370.16058188583701849, 530171.13148398592602462 179464.20843871153192595, 530148.2424291695933789 179574.15693386044586077, 530133.06942986708600074 179585.28380001557525247, 530072.88319930084981024 179599.95103267458034679, 530076.42356580472551286 179662.66609645792050287, 530120.93103042512666434 179669.24106282231514342, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530871.2405794725054875 180748.77793378444039263, 530884.09205942158587277 180795.04326160132768564, 530994.61478698416613042 180838.09571943094488233, 530982.23648845416028053 180885.78941204195143655, 531002.32567495363764465 180840.66601542077842169, 531087.78801661543548107 180857.37293935465277173, 531104.77522879175376147 180851.00402391061652452, 531115.93421733961440623 180802.8298538378730882, 531377.42735681601334363 180810.11179436542443, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531465.94281411881092936 180989.74318283077445813, 531389.47650842147413641 180987.01224334159633145, 531387.55785732087679207 181129.37252376566175371, 531386.90621243161149323 181168.05746712500695139, 531290.5201128131011501 181159.06143116063321941, 531142.08551940054167062 181108.94065935898106545, 531043.74918007606174797 181071.66004718522890471, 530997.40789101168047637 181015.41131011385004967, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530843.16896641999483109 180955.15571484464453533, 530745.85037270176690072 180904.40675493027083576, 530583.45370097586419433 180805.89406803768360987, 530578.08028169081080705 180813.05862708439235575, 530607.33556446491274983 180828.58183835234376602, 530580.2603085950249806 180875.74680006815469824, 530580.2603085950249806 180875.74680006815469824)</t>
+  </si>
+  <si>
+    <t>LineString (534494.76712749910075217 180197.82926488673547283, 534477.08958587038796395 180204.9261592309048865, 534466.10449469194281846 180201.48237478407099843, 534446.35375012725125998 180105.42193530994700268, 534275.77913797693327069 180170.50961626204662025, 534224.15787377348169684 180196.54468864286900498, 534203.5093680921709165 180212.25550818303599954, 534185.55414576060138643 180210.4599859498848673, 534171.14064759924076498 180237.33092047309037298, 534155.10926930524874479 180232.7692223628400825, 534110.10282780381385237 180227.94574123568600044, 534059.63022310636006296 180244.41244702640688047, 534045.56321658962406218 180253.93444574531167746, 534018.52404629567172378 180285.19719793670810759, 534005.14660858130082488 180295.44406237191287801, 533989.44804280833341181 180338.41282897180644795, 534003.21356487192679197 180354.3808345656725578, 534155.73554933757986873 180422.10720311899785884, 534135.36257668328471482 180462.85314842750085518, 534160.69113728043157607 180481.57425843409146182, 534211.8988793573807925 180382.46249957560212351, 534228.96812671632505953 180379.70939516284852289, 534265.3091049644863233 180416.35643082388560288, 534271.73921295220497996 180462.74348229306633584, 534252.4929513584356755 180455.64950213933479972, 534269.62446292664390057 180472.076978985540336, 534255.40823154035024345 180562.17560434373444878, 534234.92044681450352073 180597.79788426094455644, 534256.13046408852096647 180604.31816759763751179, 534251.89312430669087917 180626.73219362733652815, 534379.78553101746365428 180633.41155169066041708, 534352.34416242560837418 180636.5838860665098764, 534344.23650324332993478 180704.43507658550515771, 534297.84553046221844852 180708.00611733732512221, 534240.14221260114572942 180695.98651926324237138, 534189.34860979067161679 180672.75587819167412817, 534160.54824850801378489 180757.54946950945304707, 534160.5841055567143485 180757.22253176767844707, 534127.8658005315810442 180858.10397226159693673, 534111.99208847992122173 180939.00866548559861258, 534085.5094500295817852 180985.32051877162302844, 534070.93534209730569273 180988.37091345511726104, 534075.68040049390401691 180998.87782847607741132, 534054.99797940440475941 181035.08444935575244017, 534068.56281289900653064 181030.73750628152629361, 534096.52225887367967516 180994.37437144466093741, 534118.50570094562135637 180998.44537923578172922, 534120.13410406210459769 181012.28680572554003447, 534190.96963962737936527 181035.08444935575244017, 534233.56329029169864953 181041.4142344745923765, 534230.7365170813864097 181061.51134635950438678, 534425.65412626438774168 181087.91946370297227986, 534428.68984542321413755 181124.52763081435114145, 534418.41545121860690415 181314.94640340618207119, 534244.43570935411844403 181318.37120147436507978, 534082.24461821641307324 181331.92378598402137868, 534008.65777000458911061 181337.21434369860799052, 534003.03775836550630629 181356.73341751954285428, 533970.61429565714206547 181390.91446260787779465, 533908.72647818853147328 181354.13541679794434458, 533820.00587128894403577 181301.66338870135950856, 533762.7596401305636391 181265.19378197882906534, 533763.82057414436712861 181254.40761950571322814, 533775.00675160356331617 181229.54225989809492603, 533765.23515282932203263 181236.37174127201433294, 533750.68025846313685179 181246.3013364469516091, 533738.92612418869975954 181260.82114937415462919, 533558.01058455463498831 181157.44207860867027193, 533549.5142814606660977 181141.84867783010122366, 533537.31101294630207121 181133.86961764763691463, 533483.72784082207363099 181114.99530462495749816, 533375.88864138023927808 181117.98406295705353841, 533381.80025942670181394 181168.40668747131712735, 533323.37956343777477741 181201.44220008412958123, 533277.55680660111829638 181222.13016911473823711, 533325.81375910399947315 181204.22413798831985332, 533380.40929047460667789 181174.66604775583255105, 533399.53511356632225215 181212.91769393908907659, 533422.13835903815925121 181229.95706360254553147, 533476.03840593271888793 181291.15969749572104774, 533522.51176960719749331 181254.94408223693608306, 533527.5245621653739363 181246.81990119433612563, 533527.00599741796031594 181236.96717099371016957, 533512.83189432229846716 181222.62021298229228705, 533521.10348163370508701 181215.37559709040215239, 533538.7190823903074488 181185.9681870742351748, 533548.10621201666072011 181170.94877967197680846, 533562.65626293770037591 181116.50342783879023045, 533565.78408725361805409 181068.52103992408956401, 533568.11593338451348245 181052.2709871992119588, 533565.98876765870954841 181030.01686012774007395, 533550.6638780701905489 180995.96154993091477081, 533517.88564200571272522 180943.17581912584137172, 533527.8685909277992323 180932.10417117548058741, 533519.96954229823313653 180930.1110331111412961, 533540.88975644903257489 180852.93240523023996502, 533549.08821875147987157 180816.53405966371065006, 533554.74233068409375846 180784.02291605086065829, 533498.69594615150708705 180775.96580654679564759, 533473.25244245456997305 180751.37041963971569203, 533450.91870032052975148 180721.12092079993453808, 533451.20140591717790812 180708.11646335478872061, 533482.01631595019716769 180701.33152903561131097, 533556.93329905800055712 180708.68187454805593006, 533574.10766405356116593 180706.42022977498709224, 533632.91042815323453397 180723.09985997635521926, 533664.85616057284642011 180736.10431742150103673, 533657.22310946369543672 180723.94797676627058536, 533653.26523111085407436 180708.11646335478872061, 533628.66984420374501497 180717.16304244706407189, 533572.27007767534814775 180700.55408864485798404, 533556.72126986051443964 180706.77361177079728805, 533481.23887555941473693 180699.42326625832356513, 533449.2931431399192661 180706.77361177079728805, 533440.52926964417565614 180711.01419572028680705, 533410.70382919942494482 180714.40666287989006378, 533368.01528410776518285 180716.38560205633984879, 533344.26801399048417807 180714.68936847653822042, 533317.41098231042269617 180704.51196699772845022, 533298.32835453760344535 180707.05631736741634086, 533274.0156732271425426 180725.43218114858609624, 533214.36479233752470464 180758.22603035805514082, 533150.04926910332869738 180796.6033151010342408, 533131.95611091877799481 180803.10554382362170145, 533112.94415954523719847 180814.13106209231773391, 533032.09035890805535018 180821.19870200814330019, 533006.17641249333973974 180714.80543799756560475, 532992.55450278345961124 180708.59827885474078357, 533019.41655259137041867 180701.98867611197056249, 533047.67523066280409694 180678.44941610301611945, 533062.18958536896388978 180672.97919573029503226, 533115.1629428390879184 180663.2515109057421796, 533114.02687698940280825 180650.64306823158403859, 532992.54919304675422609 180668.21878358686808497, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531644.05815143184736371 180909.64867640155716799, 531643.0989445325685665 180988.84512792871100828, 531635.99518679245375097 181107.77244371830602176, 531600.40284548385534436 181102.74764259238145314, 531578.20997384435031563 181106.09751000965479761, 531580.30364098015706986 181147.13338587139151059, 531592.02817694062832743 181174.35105863682110794, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531133.39463505509775132 181279.42110962877632119, 531076.29551051347516477 181260.61487964406842366, 531131.04354967980179936 181113.15854730040882714, 531036.5176723989425227 181074.07573265538667329, 530995.61705242155585438 181020.45047535176854581, 530934.72057378862518817 181004.99913002699031495, 530807.47420052578672767 181052.26206866747816093, 530678.41002193070016801 181020.45047535176854581, 530547.98248933651484549 181092.25378597865346819, 530470.12182414066046476 180975.54759959221701138, 530510.45278707984834909 180923.94229928601998836, 530582.29576928459573537 180878.9198528709821403)</t>
+  </si>
+  <si>
+    <t>LineString (534150.19790721382014453 181658.82599177915835753, 534188.4078070386312902 181677.32008704933105037, 534295.39330477884504944 181748.67556176203652285, 534458.90044428419787437 181864.5233750130282715, 534483.31045287544839084 181802.6053044400177896, 534553.56364833330735564 181831.18287547372165136, 534581.15801056486088783 181763.96769404891529121, 534626.35794776398688555 181776.75086198319331743, 534797.74285306176170707 181843.92396450418164022, 535287.18371127475984395 182016.74360227302531712, 535232.17579299991484731 182019.72173797580762766, 535207.64996956521645188 182091.8977326549065765, 535091.50267715682275593 182197.53395787699264474, 535042.14986233541276306 182197.81197882973356172, 535028.73974128148984164 182224.41747152400785126, 535036.47778976988047361 182425.60673222184414044, 535003.97798611875623465 182543.22506924520712346, 534994.72957604483235627 182519.28562053974019364, 534911.66025196714326739 182500.88847403886029497, 534924.30123606591951102 182412.06298755903844722, 534860.19338813633657992 182410.70859640560229309, 534794.73114905343391001 182370.9797892379865516, 534781.76486209139693528 182416.81556864531012252, 534775.89833489886950701 182439.80761461149086244, 534733.01554672734346241 182433.42887881567003205, 534738.45721302484162152 182649.24169926377362572, 534730.12317419145256281 182691.18073339309194125, 534802.97880399296991527 182703.14411171845858917, 534809.85073587717488408 182706.20718782997573726, 534878.44964922510553151 182728.92067172401584685, 534874.50866161868907511 182753.88025989828747697, 534886.18912552238907665 182730.73464611344388686, 534960.41568882705178112 182744.27007824546308257, 534951.68315196770709008 182818.06001470709452406, 534939.02097352163400501 182880.93428009451599792, 534963.03544988483190536 182888.35693642497062683, 534944.24135854840278625 182963.83128923355252482, 534899.9714611767558381 182951.04220777060254477, 534891.78288685239385813 182949.51981309754773974, 534883.95649775443598628 182942.20384067995473742, 534838.18913542130030692 182939.14134059820207767, 534833.59538529859855771 182956.15522994138882495, 534728.87489639106206596 182935.52588911273051053, 534732.14552768925204873 182871.83970818307716399, 534649.52294641232583672 182862.46408719307510182, 534628.55294301128014922 182955.48487151082372293, 534493.18888259516097605 182880.20793622478959151, 534302.84577480040024966 182816.22254123163293116, 534284.02654097892809659 182859.77562521857907996, 534295.78345685871317983 182819.58610184054123238, 534296.67217820382211357 182816.26452868265914731, 534176.80159754795022309 182772.97793011250905693, 534076.9094470014097169 182756.3292383547523059, 534124.19173159345518798 182555.3795288386172615, 534016.13174477114807814 182513.80254928936483338, 534017.00426228798460215 182506.70794914639554918, 534125.32640601880848408 182535.96195105163496919, 534168.1666928093181923 182311.53897498786682263, 534269.44489237654488534 182341.85239916807040572, 534307.17684069508686662 182340.19748915411764756, 534331.33852689899504185 182328.77861005775048397, 534411.72237405984196812 182320.70818523829802871, 534383.0651157310931012 182118.86140918426099233, 534448.45756019873078912 182114.30714349748450331, 534385.02715628384612501 182112.14474336401326582, 534401.94695855455938727 182029.46270526901935227, 534197.29156851791776717 182037.41563493365538307, 534198.35195913992356509 182073.99911139099276625, 534075.34664699353743345 182084.07282229952397756, 533877.15337622561492026 182102.89926247851690277, 533881.96351368981413543 182166.63358387906919234, 533889.17871988611295819 182271.25407372525660321, 533665.51229002187028527 182282.44098327826941386, 533645.62510754854883999 182286.76606867561349645, 533618.567245963960886 182470.45983984900522046, 533632.33677199063822627 182516.43228964801528491, 533660.54209143260959536 182517.76482442481210455, 533676.7545978834386915 182542.63880692477687262, 533673.86743920051958412 182563.68175194147625007, 533708.19324949278961867 182577.78883584373397753, 533744.78147669287864119 182600.35388822320965119, 533719.61320557200815529 182691.0010928868141491, 533701.35989006015006453 182685.35125713315210305, 533696.14465705677866936 182787.91750619950471446, 533602.27046299609355628 182776.61783469218062237, 533604.152414740761742 182785.81231147074140608, 533629.6504362637642771 182783.13687594639486633, 533887.88424544327426702 182820.57441884058061987, 533896.32165873644407839 182796.25481581923668273, 533994.96494650165550411 182805.68486597036826424, 533958.97602709801867604 182864.08820365733117796, 534162.58751859271433204 183101.90006286397692747, 534151.45251515158452094 183143.85516511532478034, 534224.62539490743074566 183157.37624072236940265, 534242.12325745774433017 183214.64197270525619388, 534235.76864853664301336 183146.50009479920845479, 534422.34790956706274301 183189.51548639123211615, 534554.33143426640890539 183222.22614488427643664, 534560.58397974201943725 183245.53360263974172994, 534585.38740086904726923 183236.13562777847982943, 534839.23427885014098138 183312.35428325369139202, 534883.15689386974554509 183313.64612487191334367, 535342.64082826022058725 183415.18309037722065113, 535377.02339462761301547 183414.03198869159677997, 535729.61131596809718758 183230.43964716198388487, 535597.45816457970067859 183171.78773763249046169, 535493.01945444208104163 183163.06486600026255473)</t>
+  </si>
+  <si>
+    <t>LineString (533064.46897248667664826 183210.39921171619789675, 533076.87953593488782644 183044.4026491524418816, 533070.12536461430136114 182985.15014620366855524, 533045.871749417623505 182926.97217051047482528, 533058.76607648422941566 182947.23468447223422118, 533080.25662159512285143 182941.70854430084000342, 533168.98187212459743023 182947.23468447223422118, 533189.95457557367626578 182949.67927450055140071, 533190.07185356423724443 182932.90852184614050202, 533256.30459875019732863 182938.06875343210413121, 533270.02612364920787513 182934.78496969558182172, 533273.77901934809051454 182943.58081898986711167, 533263.22400019492488354 182991.66479513191734441, 533262.98944421380292624 183071.82430170045699924, 533364.55218406510539353 183067.83685002036509104, 533378.15643097355496138 183087.01180148191633634, 533393.87168171268422157 183066.6054311191837769, 533558.68779758946038783 183057.05841860847431235, 533558.68779758946038783 183104.32901793727069162, 533561.19678307115100324 183054.36769029102288187, 533513.35373550979420543 183055.70408826760831289, 533502.36358368746004999 182956.620714706776198, 533466.48049678211100399 182839.1161635409516748, 533430.95062767004128546 182843.6842895696463529, 533423.99112124263774604 182625.95366138272220269, 533418.28455447813030332 182579.59432971687056124, 533451.54715791763737798 182502.91214257484534755, 533464.75749999412801117 182467.34583698387723416, 533337.93821605830453336 182452.71284268359886482, 533337.78902459214441478 182368.47306541417492554, 533484.07380397082306445 182386.01211906579555944, 533490.69280884729232639 182350.24248738010646775, 533472.43150111590512097 182205.93442166002932936, 533583.10897760698571801 182063.8076075866993051, 533609.71995556121692061 182037.80142458603950217, 533610.24870057171210647 182016.33477542886976153, 533584.88456065976060927 182052.1574076684191823, 533535.1852201041765511 182057.86061068301205523, 533518.26287293271161616 181970.58373815898085013, 533484.19519956270232797 181975.12609460830572061, 533475.45617014251183718 181918.25283637543907389, 533396.87044996197801083 181921.33462932368274778, 533362.97072753123939037 181745.67243127315305173, 533383.00238169485237449 181921.33462932368274778, 533385.57218187116086483 181991.15361790888709947, 533400.75257761764805764 182035.04779862469877116, 533331.49939815502148122 182048.89843451723572798, 533234.54494690720457584 182081.48816602909937501, 533073.65851616964209825 182090.02078689282643609, 533085.33284421800635755 182215.89180190846673213, 533090.14230673655401915 182227.52340018114773557, 533155.84606537700165063 182220.5149992594961077, 533149.99286592833232135 182319.05148053923039697, 533156.54641778930090368 182323.96664443501504138, 533151.53487813088577241 182385.64713253875379451, 532980.57106288510840386 182377.64146055665332824, 532778.65285523270722479 182361.72131757129682228, 532755.6968509522266686 182366.02556837382144295, 532572.76619184156879783 182348.80856516343192197, 532552.88329151901416481 182350.97523911585449241, 532244.88995379093103111 182215.8126952207821887, 532262.60291642148513347 182168.39960261050146073, 532295.2441410442115739 182069.11680604351568036, 532305.37037298001814634 182028.61187830017297529, 532288.80017526680603623 182059.91114064730936661, 532220.90932479011826217 182025.71317250368883833, 532158.87452575471252203 182016.26025074589415453, 532107.4742636966984719 182011.53378986698226072, 532104.52022564737126231 181924.09426360743236728, 532086.79599735140800476 181928.63609710824675858, 532087.97761257109232247 181975.30989828731981106, 532092.70407344994600862 182022.86991088121430948, 532079.11549842311069369 182099.67490016322699375, 532046.62107988074421883 182161.70969919872004539, 532014.12666133837774396 182194.20411774111562409, 531972.17932103818748146 182188.88684925236157142, 531913.68936766183469445 182151.07516222121194005, 531908.60801759164314717 182163.45413967911736108, 531953.17571160080842674 182184.55127293791156262, 531987.59041022916790098 182199.51705184334423393, 532004.99554516770876944 182204.79133515805006027, 531983.10726941167376935 182243.55731752107385546, 531968.33927613054402173 182281.13658613828010857, 531944.07757288287393749 182371.59054498534533195, 531937.94260709825903177 182398.64015493713668548, 532011.93064753827638924 182423.87109960327506997, 532068.52979368122760206 182445.01053972897352651, 532086.94156411325093359 182440.23711776512209326, 532158.88385228300467134 182467.76953373529249802, 532152.40563676052261144 182502.8882810408831574, 532121.55289627402089536 182643.03526213087025099, 532075.0642949640750885 182863.25497264647856355, 532069.45360170258209109 182883.29316286626271904, 532082.41561907751020044 182888.00662372991791926, 532062.29523281508591026 182889.32744172037928365, 532066.95640396035742015 182915.35964283399516717, 531884.43796249642036855 182981.6259192216093652, 531767.99498561583459377 183028.33115369590814225, 531728.68198287941049784 182918.06297528900904581, 531725.87449492723681033 182910.13609254563925788, 531809.84689899394288659 182817.65547132669598795, 531837.40510237636044621 182760.1590255610353779, 531828.71498920442536473 182755.52429853595094755, 531814.23146725108381361 182767.69045697676483542, 531569.74961667892057449 182693.53482457570498809, 531563.95620789751410484 182754.94495765783358365, 531565.11488965386524796 182687.74141579438582994, 531616.09688692959025502 182577.66664894908899441, 531609.14479639194905758 182564.92114963015774265, 531628.84238624852150679 182534.7954239672399126, 531625.36634097970090806 182476.86133615393191576, 531747.02792538760695606 182513.93915235446183942, 531632.89777239540126175 182463.5364959568833001, 531625.94568185787647963 182421.82395273129804991, 531681.5624061586568132 182312.90786764226504602, 531703.57735952769871801 182270.0366426604159642, 531683.80043675052002072 182250.5687343017780222, 531595.88583471847232431 182183.28084469723398797, 531580.06645999138709158 182164.89640980056719854, 531555.2433897431474179 182143.27140381743083708, 531526.61310013174079359 182118.90519989278982393, 531515.64830836560577154 182136.41840896362555213, 531466.00216786901000887 182107.48354180311434902, 531411.63507536228280514 182149.7436767349136062, 531394.57873261498752981 182161.31762359911226667, 531354.5267849137308076 182200.07511671676184051, 531330.16058098908979446 182208.29871054133400321, 531333.2063564796699211 182193.06983308843336999, 531354.79575750709045678 182159.67430333484662697, 531334.90127811359707266 182155.04768022007192485, 531291.87368314596824348 182150.88371941674267873, 531265.96459370316006243 182135.15320082646212541, 531248.34037534287199378 182041.19192783226026222, 531270.21593675261829048 182040.14943936991039664, 531272.14963821833953261 182027.69603843480581418, 531291.66027387382928282 182000.88878809078596532, 531269.86458137142471969 182026.02942997106583789, 531260.89388385554775596 182036.66077076771762222, 531156.26423942053224891 182028.00196012531523593, 530992.96919284970499575 181971.66516905839671381, 530937.44887701561674476 182060.66096943948650733, 530881.5203235651133582 182170.88512587477453053, 530784.23736255615949631 182302.13991453754715621)</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,24 +685,24 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -714,7 +714,7 @@
         <v>10387.633383793</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -729,24 +729,24 @@
         <v>72.400000000000006</v>
       </c>
       <c r="M2">
-        <v>77.400000000000006</v>
+        <v>72.2</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>10135.874484428899</v>
+        <v>10324.6261671389</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -761,12 +761,12 @@
         <v>70.7</v>
       </c>
       <c r="M3">
-        <v>78.5</v>
+        <v>70.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -778,7 +778,7 @@
         <v>10889.6786160784</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -793,14 +793,14 @@
         <v>73</v>
       </c>
       <c r="M4">
-        <v>86.2</v>
+        <v>71.7</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -809,10 +809,10 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <v>10373.492909434601</v>
+        <v>9934.8314288458605</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -827,12 +827,12 @@
         <v>72.5</v>
       </c>
       <c r="M5">
-        <v>79.2</v>
+        <v>71.900000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -844,7 +844,7 @@
         <v>10047.75961035</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
@@ -859,14 +859,14 @@
         <v>71.8</v>
       </c>
       <c r="M6">
-        <v>79.5</v>
+        <v>71.7</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -878,10 +878,10 @@
         <v>10347.2332512455</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="J7">
         <f>AVERAGE(J2:J6)</f>
@@ -897,26 +897,26 @@
       </c>
       <c r="M7">
         <f>AVERAGE(M2:M6)</f>
-        <v>80.16</v>
+        <v>71.61999999999999</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>10260.484070139</v>
+        <v>10248.4265845503</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -924,11 +924,11 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" s="1">
         <f>SUM(D2:D8)</f>
-        <v>72442.156325469405</v>
+        <v>72180.189042001963</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -961,7 +961,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -973,12 +973,12 @@
         <v>10396.40561819</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -990,12 +990,12 @@
         <v>10050.3586120912</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1007,12 +1007,12 @@
         <v>10040.0307021154</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -1024,12 +1024,12 @@
         <v>10328.5537327765</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1041,29 +1041,29 @@
         <v>10468.1416395172</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>10473.764647815</v>
+        <v>10264.3029488128</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -1072,20 +1072,20 @@
         <v>29</v>
       </c>
       <c r="D18">
-        <v>8970.4012079409804</v>
+        <v>9061.0964137012907</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <f>SUM(C12:C18)</f>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" s="1">
         <f>SUM(D12:D18)</f>
-        <v>70727.656160446277</v>
+        <v>70608.889667204392</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1110,7 +1110,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1119,15 +1119,15 @@
         <v>24</v>
       </c>
       <c r="D22">
-        <v>10414.387040997</v>
+        <v>10351.5409177809</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1139,12 +1139,12 @@
         <v>10240.7485129782</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1153,15 +1153,15 @@
         <v>20</v>
       </c>
       <c r="D24">
-        <v>10322.5536861458</v>
+        <v>9758.4701712043206</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -1173,12 +1173,12 @@
         <v>10086.2297192444</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -1190,12 +1190,12 @@
         <v>10197.200793621199</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -1204,37 +1204,37 @@
         <v>22</v>
       </c>
       <c r="D27">
-        <v>10503.889210624</v>
+        <v>10363.8770276912</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
       <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <v>10746.090738475201</v>
+      </c>
+      <c r="E28" t="s">
         <v>31</v>
-      </c>
-      <c r="D28">
-        <v>11221.3477004749</v>
-      </c>
-      <c r="E28" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <f>SUM(C22:C28)</f>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D29" s="1">
         <f>SUM(D22:D28)</f>
-        <v>72986.356664085499</v>
+        <v>71744.157880995423</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1259,7 +1259,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1271,29 +1271,29 @@
         <v>10029.895474594299</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33">
-        <v>10369.6417108937</v>
+        <v>10424.143479610801</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1302,32 +1302,32 @@
         <v>19</v>
       </c>
       <c r="D34">
-        <v>10147.9934740517</v>
+        <v>10113.149431297201</v>
       </c>
       <c r="E34" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>17</v>
       </c>
       <c r="D35">
-        <v>10587.4904613938</v>
+        <v>10563.1611848091</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1339,12 +1339,12 @@
         <v>10263.725203550401</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -1353,15 +1353,15 @@
         <v>17</v>
       </c>
       <c r="D37">
-        <v>10124.7844637862</v>
+        <v>9995.7060506058697</v>
       </c>
       <c r="E37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38">
         <v>7</v>
@@ -1370,20 +1370,20 @@
         <v>27</v>
       </c>
       <c r="D38">
-        <v>11007.39364301</v>
+        <v>10492.952525106501</v>
       </c>
       <c r="E38" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C39" s="1">
         <f>SUM(C32:C38)</f>
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D39" s="1">
         <f>SUM(D32:D38)</f>
-        <v>72530.924431280087</v>
+        <v>71882.733349574162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1408,7 +1408,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>29</v>
       </c>
       <c r="D42">
-        <v>10275.7603419072</v>
+        <v>10267.3272148008</v>
       </c>
       <c r="E42" t="s">
         <v>14</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="B47">
         <v>6</v>
@@ -1502,36 +1502,37 @@
         <v>24</v>
       </c>
       <c r="D47">
-        <v>10185.2940832533</v>
+        <v>10124.1028846559</v>
       </c>
       <c r="E47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B48">
         <v>7</v>
       </c>
       <c r="C48">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48">
-        <v>9096.5507719182897</v>
+        <v>9062.0794277297991</v>
       </c>
       <c r="E48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" s="1">
-        <v>162</v>
+        <f>SUM(C42:C48)</f>
+        <v>161</v>
       </c>
       <c r="D49" s="1">
         <f>SUM(D42:D48)</f>
-        <v>71760.061292424696</v>
+        <v>71655.9656225324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ATD routes V4 - The ASICS London 10K edition
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Documents/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4601FF9A-9B59-3B4E-BA1C-E17141DD65ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAAA2ED-3DD8-234E-A771-8A02E6803040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>wkt_geom</t>
   </si>
@@ -71,9 +71,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>LineString (528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526810.75304763286840171 179467.00080663594417274, 526668.71815055573824793 179454.61404235597001389, 526438.77076674299314618 179425.46686823663185351, 526444.83039404929149896 179401.22835901146754622, 526429.857896420173347 179399.29642383340978995, 526400.95936604985035956 179579.61037377678439952, 526395.80753890855703503 179617.60509894342976622, 526400.31538765714503825 179630.4846667965175584, 526396.45151730126235634 179663.00557562557514757, 526429.93839371926151216 179670.41132714110426605, 526431.87032889726106077 179659.14170526966336183, 526400.31538765714503825 179655.59982411004602909, 526404.17925801302772015 179629.51869920754688792, 526481.13467593537643552 179644.97418063125223853, 526512.36762797913979739 179646.26213741654646583, 526515.90950913866981864 179639.17837509737000801, 526505.28386565984692425 179635.63649393775267527, 526386.30885761685203761 179621.30797470119432546, 526318.94980677636340261 179621.48525741521734744, 526215.34960218577180058 179626.84875574553734623, 526121.02660867478698492 179655.6876124200061895, 526113.32453510130289942 179686.26937513795564882, 526116.04291400965303183 179658.17945975257316604, 526072.0957883259980008 179674.03667005078750663, 526077.53254614258185029 179626.23850758047774434, 526092.24883591232355684 179409.14943758773733862, 526170.58646800776477903 179414.55203290464123711, 526170.91200886678416282 179254.77395809174049646, 526170.02756560104899108 179226.2506627686379943, 526170.69089805032126606 179197.28514581263880245, 526191.0330931645585224 179103.75527045089984313, 526208.50084766466170549 179068.1564290011592675, 526205.1700667041586712 179050.55107881623553112, 526215.6382354375673458 179000.58936440671095625, 526094.3026433001505211 178987.74206641569617204, 526096.78229620109777898 178934.34904740183264948, 526076.51597697660326958 178943.73160259836004116, 526090.02685645967721939 178944.10690480621997267, 526079.61222019151318818 179075.18120090151205659, 525857.43331313808448613 179086.440267137310002, 525822.15490559919271618 179081.18603622727096081, 525774.11622299312148243 179039.15218894690042362, 525789.9340731572592631 179008.44695039271027781, 525609.81218133552465588 178989.52756098052486777, 525584.06940557796042413 178987.97679135657381266, 525578.79678885661996901 179053.72942341200541705, 525579.54627333593089134 178986.48593813352636062, 525473.92217159015126526 178976.91720417744363658, 525356.52116651367396116 178940.85043772764038295, 525101.93763904797378927 178795.75530841300496832, 525143.89285716298036277 178740.55107405106537044, 525178.48751069651916623 178739.81501759291859344, 525136.90032081049866974 178734.29459415673045442, 525073.96749363793060184 178845.07109110968303867, 525050.22967286221683025 178837.15848418447421864, 524920.68373622617218643 178769.44129003383568488, 524812.24932546948548406 178896.28909129649400711, 524699.21156708616763353 179025.31069560500327498, 524681.6391244096448645 179051.25509521568892524, 524679.63010795961599797 179077.09913740976480767, 524788.97600055101793259 179149.0372246410115622, 524957.31112467218190432 179248.31178502010880038, 524889.31033757049590349 179366.96949636968201958, 524837.84125263791065663 179392.39398410747526214, 524751.64603811223059893 179345.88577483102562837, 524614.60184811090584844 179570.98550772908492945, 524703.84473427385091782 179436.35361285935505293, 524844.32857223774772137 179505.77558726171264425, 524810.43752961605787277 179598.63431089642108418, 524822.46338344959076494 179627.87900090057519265, 524845.42183167708572 179640.99811417344608344, 524954.20114589820150286 179688.82821464753942564, 524980.43937244394328445 179689.64815922707202844, 525145.27674076042603701 179339.90930881092208438, 525213.61852516769431531 179374.56420798628823832, 525206.26161919755395502 179390.0524310814216733, 525222.23384926444850862 179385.21236136413062923, 525351.1733065313892439 179466.91273819096386433, 525352.72212884086184204 179482.01375570870004594, 525369.8851592862047255 179479.95885097398422658, 525422.48737169418018311 179507.45546200548415072, 525366.53774576925206929 179596.40102116821799427, 525283.64405398862436414 179742.1564941595424898, 525384.085012789350003 179740.24697022794862278, 525418.45644355763215572 179681.43363313551526517, 525419.82130964624229819 179656.85948007801198401)</t>
-  </si>
-  <si>
     <t>LineString (525419.82130964624229819 179656.85948007801198401, 525441.752635522861965 179643.62505929038161412, 525473.17677637841552496 179595.26529158212360926, 525500.20750449819024652 179556.04433391022030264, 525550.45115803636144847 179584.76653285161592066, 525499.24060956016182899 179534.12816927468520589, 525517.26443388417828828 179487.20900754237663932, 525503.5319963040528819 179534.41426172424689867, 525559.32002397358883172 179590.48838184334454127, 525606.73984749265946448 179622.88835175908752717, 525629.34115101001225412 179599.42877089293324389, 525610.74514178687240928 179626.03536870455718599, 525658.80867331754416227 179674.95717758397222497, 525607.83047283766791224 179797.05819002352654934, 525605.59547769429627806 179802.41136387505684979, 525565.82862720161210746 179892.53048549505183473, 525542.10064045747276396 179969.00328062011976726, 525515.2065179068595171 180018.21411000256193802, 525579.59422428475227207 180050.68312432989478111, 525445.31558876170311123 180394.63454728861688636, 525379.27691555360797793 180350.05844287315267138, 525359.80384157912340015 180365.77170708231278695, 525341.08953253971412778 180458.30356844351626933, 525220.47356508939992636 180431.87263787462143227, 525220.06736415333580226 180443.37315647987998091, 525260.75858418515417725 180454.93051064651808701, 525259.69845210365019739 180479.84361456095939502, 525271.88997104053851217 180457.05077480943873525, 525349.58892509061843157 180481.27489107492147014, 525578.85862934240140021 180555.2543595980387181, 525838.78649172093719244 180589.91140791517682374, 525854.78205248259473592 180554.5878778996411711, 525882.10780211735982448 180593.2438164071936626, 525914.76540533918887377 180597.2427065976371523, 525856.11501587950624526 180869.16723954741610214, 525629.19645251578185707 180815.6728557784226723, 525607.69589158636517823 180896.01705714597483166, 525592.64245667064096779 180959.77655073793721385, 525465.21662881935480982 180928.60297152044950053, 525449.76506418350618333 180973.39663861988810822, 525471.05554088775534183 180869.10814367001876235, 525169.66690440021920949 180792.47538909091963433, 525168.57008813507854939 180716.41076266291202046, 525177.12844300922006369 180672.72679385205265135, 525198.13128985709045082 180518.01377174342633225, 525198.13128985709045082 180499.77590576437069103, 525216.49806978390552104 180422.86151518215774558, 525032.54404547775629908 180384.90800919375033118, 525042.54589259531348944 180329.57170285852043889, 525095.59916861017700285 180167.36783438673592173, 525073.85602270253002644 180201.72200492097181268, 524867.29613657889422029 180103.44298541796160862, 524783.80245629313867539 180254.77528093589353375, 524774.67033501190599054 180290.43404022458707914, 524644.64632248354610056 180224.76973958319285884, 524628.55639451183378696 180249.5569259180338122, 524615.48465062899049371 180279.87639951938763261, 524521.47936696978285909 180234.3491769400134217, 524548.17742959351744503 180180.49637430562870577, 524437.80201806232798845 180127.87308771314565092, 524428.80898644169792533 180134.89889366674469784, 524420.06375851028133184 180117.54754349653376266, 524132.30088686855742708 180008.73613583465339616, 524129.21403842425206676 179997.41769153883797117, 524165.22727027453947812 179939.45353741792496294, 524226.62125600024592131 179896.58064235807978548, 524270.18011738103814423 179878.40253485270659439, 524446.98793660791125149 179571.43260622417437844, 524457.27743142226245254 179530.78910170739982277, 524381.1351697959471494 179462.8784359325945843, 524348.89475271094124764 179388.7940732691786252, 524331.745594686944969 179384.67827534343814477, 524276.53971593477763236 179449.82277273709769361, 524251.3383856481523253 179421.85383848828496411, 524229.85877764469478279 179399.72832341972389258, 524389.1895376107422635 179207.66534497964312322, 524566.84597020875662565 179003.91686643939465284, 524369.1024815944256261 178938.00237023460795172, 524261.14581603015540168 178855.60790905589237809, 524505.73842157609760761 178619.25999807892367244, 524555.30119735538028181 178522.66434189284336753, 524557.56896609300747514 178478.6696283841447439, 524558.2010982601204887 178464.50738733183243312, 524415.99402974359691143 178486.72505095947417431, 524428.34983511443715543 178417.8673475687392056, 524415.57181855535600334 178400.8991837041976396, 524427.16849381849169731 178377.70583317801356316, 524578.50510600174311548 178422.93286670403904282, 524593.83628550986759365 178396.09239642595639452, 524646.92549005395267159 178410.17652391464798711, 524593.00095008069183677 178386.9831733884930145, 524606.6284040097380057 178344.01019967623869888, 524546.08097314718179405 178317.43756506184581667, 524547.72005947201978415 178302.13942603100440465, 524496.90838340518530458 178286.29492489190306515, 524414.95406716852448881 178274.27495851050480269, 524417.13951560144778341 178259.52318158789421432, 524399.10956602939404547 178272.63587218578322791, 524203.36645184078952298 178186.01344392789178528, 524150.09307708113919944 178297.58598351886030287, 524144.01900628820294514 178301.03496496815932915, 524016.37724255298962817 178317.86004791711457074, 524145.06728700950043276 178304.62208961919532157, 524127.89568292774492875 178629.52170006616506726, 524078.60595063568325713 178736.94340746355010197, 524002.99679681507404894 178712.5158346907410305, 523912.26581223041284829 178664.82390689619933255, 523906.44972347497241572 178456.60792945179855451, 523916.40600100060692057 178412.82588814571499825)</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>P7 Knightsbridge</t>
   </si>
   <si>
-    <t>LineString (530581.86556883039884269 180867.74445010567433201, 530619.76996912294998765 180831.70142661320278421, 530983.56856463546864688 180203.70454308946500532, 531002.70594172133132815 180167.18990898446645588, 531009.82027298887260258 180172.62735671561677009, 531014.84303175657987595 180179.2561260225775186, 531055.46903743746224791 180126.53966183957527392, 531062.93085470306687057 180082.20768867310835049, 531131.40400137600954622 180037.87571550664142706, 531230.60227796633262187 180072.55121927050640807, 531196.8046350572258234 180173.50521757037495263, 531180.12527881644200534 180209.05858218902722001, 531154.66731402778532356 180209.05858218902722001, 531173.54132240556646138 180223.10435586553649046, 531118.23608855437487364 180332.83696271321969107, 530929.62455369275994599 180270.64411783422110602, 530940.64358626771718264 180262.38647808227688074, 530923.9078333250945434 180242.84698136936640367, 530866.90213167306501418 180188.57442979663028382, 530842.303780960268341 180151.09122871042927727, 530862.94364999502431601 180139.18124142149463296, 530885.30430015258025378 180128.40685322834178805, 530835.31284910615067929 180139.32700893725268543, 530818.64858063124120235 180107.00842765255947597, 530746.94172840588726103 179903.50236112563288771, 530810.56893531011883169 179879.7684029946976807, 530845.41240575758274645 179870.67880200836225413, 530942.97500607429537922 180058.23076402678270824, 531005.72952298959717155 180026.85350556910270825, 531037.65725966589525342 180016.94489763511228375, 531078.94312605750747025 180004.28389860835159197, 531103.36682528315577656 179997.4820276228711009, 531123.39294299448374659 179985.6610553627833724, 531156.49166532268282026 179963.68795398517977446, 531181.76768542011268437 179933.82261524567729793, 531212.01546737970784307 179888.97245578825823031, 531103.54066311055794358 179763.39200930739752948, 531108.54719253838993609 179756.71663673696457408, 531135.1701887323288247 179781.81394092956907116, 531167.34841385786421597 179808.82066558845690452, 531194.06783293525222689 179811.40641582175157964, 531236.87636457534972578 179792.73155302571831271, 531253.82739388255868107 179784.97430232583428733, 531249.51781016041059047 179751.07224371147458442, 531230.84294736431911588 179747.62457673373864964, 531216.11277351365424693 179764.36885167972650379, 531081.64286881464067847 179671.73402844261727296, 531009.90093444765079767 179597.21122520481003448, 531009.90093444765079767 179597.21122520481003448, 530972.86260063934605569 179563.04264083271846175, 530945.78228133858647197 179595.62788598841871135, 530882.00223331130109727 179643.29507977730827406, 530842.39146664168220013 179630.53907017182791606, 530826.94998132972978055 179588.91419672238407657, 530809.49438923806883395 179516.40635264918091707, 530801.43796211876906455 179441.21303286953479983, 530771.22636042162775993 179379.44709162198705599, 530816.2080785040743649 179456.65451818142901175, 530938.3972231459338218 179398.91679049350204878, 530945.11091241205576807 179382.80393625498982146, 531051.18720281543210149 179331.77989783309749328, 531117.65272654918953776 179413.01553795216022991, 531106.23945479700341821 179449.94082891539437696, 531128.01335033809300512 179490.33879105054074898, 531145.9327949439175427 179489.53642785921692848, 531118.11753764539025724 179461.98862495779758319, 531170.3957165403990075 179433.66088251979090273, 531266.22342408250551671 179404.70195991088985465, 531313.87248040549457073 179407.3990763065230567, 531433.52216941397637129 179415.3352683637640439, 531469.58935155137442052 179427.35766240957309492, 531466.38337980583310127 179436.3744579438935034, 531357.78108692553360015 179511.91516719831270166, 531327.52472857688553631 179431.76587355969240889, 531318.50793304259423167 179389.48712116529350169, 531315.08669927902519703 179378.57198898226488382, 531298.67588855815120041 179338.66640459033078514, 531270.20679607603233308 179239.75740465606213547, 531274.79732766340021044 179226.52587243364541791, 531198.10844702739268541 179192.5019324331660755, 531219.62179134623147547 179127.21737543260678649, 531235.3105901419185102 179110.29808261376456358, 531240.33914468786679208 179077.35684370002127253, 531245.46363338397350162 178841.6303636806551367, 531233.0184465505881235 178844.00959057526779361, 531233.75051636435091496 178886.46963977129780687, 531226.42981822707224637 179085.22659419756382704, 531181.16885312169324607 179183.82010049920063466, 530988.59653849294409156 179108.14471807319205254, 530973.83061021461617202 179097.68551887612557039, 530832.78523280692752451 179038.00655875154188834, 530746.65065118379425257 179009.70519621824496426, 530660.53985221788752824 178980.90664574180846103, 530629.06085022771731019 178958.21248151632607915, 530596.23852397978771478 178935.36033985641552135, 530526.31339351984206587 178863.9934541292313952, 530506.84969741245731711 178868.31871993085951544, 530530.63865932147018611 178898.5955805424018763, 530534.24304748955182731 178938.24385039083426818, 530561.63639756664633751 178960.59105703269597143, 530637.84568799240514636 178901.11103604579693638, 530747.65616005111951381 178890.12998883993714117, 530829.64797918824478984 178865.23961517328280024, 530854.35533540148753673 178855.90572504830197431, 530871.92501093086320907 178861.03021374437958002, 530891.65204298356547952 178844.1667831186496187, 530965.44759355159476399 178788.4324741373420693, 530886.32739482226315886 178835.18531884101685137, 530876.4373699810821563 178823.49710766511270776, 530792.12940123490989208 178700.15787217835895717, 530743.08072371536400169 178626.95089080586330965, 530828.00082210742402822 178569.11737552162958309, 530830.19703154859598726 178562.52874719808460213, 530868.26466186228208244 178541.84777496033348143, 530837.15169477893505245 178458.75785110259312205, 530903.77004782785661519 178437.16179159769671969, 530958.67528385727200657 178408.9771037692844402, 530969.51906797324772924 178398.22482838027644902, 530903.17095182067714632 178270.43457464387756772, 530838.13083763618487865 178210.65022726217284799, 530867.03755505150184035 178124.58704586655949242, 531097.63432352372910827 178142.32525882596382871, 531169.9011170620797202 178195.53989770417683758, 531216.54604743677191436 178275.69034144666511565, 531215.56562907935585827 178356.32546967949019745, 531310.11752128496300429 178268.96068190585356206, 531365.33336403663270175 178240.15241612237878144, 531381.33795613853726536 178257.757467434508726, 531467.76275348896160722 178198.54047665739199147, 531466.96252388379070908 178187.33726218604715541, 531513.37584097939543426 178158.52899640260147862, 531625.40798569284379482 178357.78616807149956003, 531634.2105113489087671 178376.19144898871309124, 531471.76390151435043663 178477.02037923081661575, 531565.23039256664924324 178567.62021348648704588)</t>
-  </si>
-  <si>
     <t>S1 Lambeth</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>N6 Shoreditch</t>
   </si>
   <si>
-    <t>LineString (530580.2603085950249806 180875.74680006815469824, 530531.28659617097582668 180919.46416819942533039, 530563.88801023468840867 180944.97831833627424203, 530620.69896473211701959 180923.3214464345946908, 530631.52323099854402244 180940.26917490593041293, 530672.45004481147043407 181008.75894496028195135, 530717.5530641155783087 181038.41000394721049815, 530783.43270573788322508 181058.76900571642909199, 530778.00363859941717237 181104.28964556960272603, 530801.95612234645523131 181156.06284796763793565, 530751.4015138226095587 181178.39113339898176491, 530780.09174134500790387 181213.18420375051209703, 530814.09418500657193363 181239.43468773260246962, 530853.48855285136960447 181252.44053536702995189, 530912.3730502761900425 181206.08465441560838372, 531047.80579616781324148 181254.33936599228763953, 531131.03878337366040796 181286.03806058526970446, 531110.30965442163869739 181356.39285153028322384, 531197.1542466712417081 181376.88721254793927073, 531286.93602178571745753 181375.08379181567579508, 531305.25734407640993595 181583.75572135805850849, 531325.21203300100751221 181586.18808011634973809, 531388.88918386655859649 181572.61640889989212155, 531390.49493819230701774 181599.32936576748033985, 531367.26279260986484587 181685.65545662579825148, 531395.89248193160165101 181593.61920236010337248, 531412.32238542404957116 181591.09869188832817599, 531419.12145480117760599 181581.94767167716054246, 531385.41458384564612061 181534.11455342586850747, 531374.38023236603476107 181529.41130202304339036, 531413.36951656360179186 181525.26491641241591424, 531471.93530321691650897 181443.00015478587010875, 531489.86913823755457997 181396.66486753628123552, 531500.42645009863190353 181343.75654840667266399, 531561.43261282751336694 181271.18043218745151535, 531510.99066478840541095 181339.18317034683423117, 531566.52648988855071366 181353.74707860476337373, 531590.37191976455505937 181360.8123911606380716, 531583.52515332715120167 181463.7283773985109292, 531566.74728090583812445 181537.16921628548880108, 531557.91564021108206362 181566.97600363052333705, 531578.66999584389850497 181574.92448025586782023, 531607.15203708468470722 181582.43137484646285884, 531674.27250636543612927 181614.50127011956647038, 531688.84471351187676191 181590.65584024353302084, 531676.92199857381638139 181529.27593741449527442, 531692.81895182456355542 181520.00271468493156135, 531744.15286336338613182 181527.39921376685379073, 531827.17028589476831257 181517.68440900254063308, 531837.76825472852215171 181595.40284711701679043, 531873.09481750777922571 181627.19675361836561933, 531892.79980997554957867 181649.86393449633033015, 531906.87584316555876285 181666.05597267561824992, 532031.40197696257382631 181539.76351073960540816, 532080.85916485369671136 181575.09007351889158599, 532117.06889170245267451 181580.38905793579760939, 532140.91432157845702022 181599.81866746442392468, 532170.05873587145470083 181590.98702676958055235, 532184.18936098308768123 181559.19312026820261963, 532149.74596227332949638 181529.16554190579336137, 532138.2648293700767681 181394.04143927496625111, 532132.82734409463591874 181370.85496780133689754, 532125.90053239720873535 181323.38831371636479162, 532096.75611810432747006 181293.36073535395553336, 532017.27135185094084591 181313.67350895205163397, 532018.15451592043973505 181340.1684310365235433, 532031.40197696257382631 181369.31284532946301624, 532033.16830510157160461 181389.62561892755911686, 532057.23452599509619176 181405.74336319562280551, 532119.69996919808909297 181395.70321314127068035, 532140.79753599606920034 181364.76011517079314217, 532132.3034719011047855 181288.28254195442423224, 532160.56472212448716164 181242.35801034132600762, 532384.22602272103540599 181180.09494344278937206, 532424.85156991728581488 181173.91279495641356334, 532670.78084617818240076 181110.13770430514705367, 532818.19047775026410818 181176.80775713562616147, 532780.99707011831924319 181260.68462679820368066, 532688.27519202104303986 181257.87865509698167443, 532650.54560429917182773 181265.88190097737242468, 532436.45877699879929423 181308.18477205943781883, 532413.59236019768286496 181321.90462214010767639, 532414.73568103776779026 181427.0901394252141472, 532338.13318475405685604 181459.10312294677714817, 532350.7097139946417883 181509.40923990920418873, 532405.30328410735819489 181674.61910129722673446, 532528.63901972828898579 181635.46036252533667721, 532616.67472441249992698 181609.7356436240952462, 532545.63823982118628919 181643.35478146860259585, 532594.42826642119325697 181790.64542780804913491, 532462.787251255242154 181845.87942018534522504, 532437.01138814585283399 181871.65528329473454505, 532445.2964870025170967 181957.26797147953766398, 532616.5218633720651269 181942.53890684561338276, 532701.21398501726798713 181920.44530989468330517, 532802.42052498331759125 181910.09618882910581306, 532815.01476064522285014 182025.01858924416592345, 532915.61185974825639278 182009.02176296585821547, 532912.46310028480365872 181963.04987479909323156, 532924.13200544030405581 182009.18769421585602686, 532982.27383896452374756 182001.80460424453485757, 533061.71429885365068913 181990.75895807769848034, 533064.2333064244594425 181966.82838615524815395, 533035.89447125315200537 181858.51106061163591221, 532947.72920627577695996 181893.14741470987792127, 532880.60253748437389731 181721.24718533383565955, 532784.00711035938002169 181767.39149765466572717, 532747.24231199838686734 181784.20146203070180491, 532733.93556229211390018 181745.29988511741976254, 532713.1074947752058506 181674.74374392238678411, 532748.93080092582385987 181661.89110736449947581, 532742.91467317531351 181642.74888270380324684, 532713.65441547974478453 181552.64369662242825143, 532855.62877998419571668 181525.1299014599644579, 533071.32848995237145573 181469.8718779842602089, 533186.19458453194238245 181444.03007418513880111, 533181.16196181264240295 181435.64236965295276605, 533152.08458610100205988 181436.48114010615972802, 533186.47417468298226595 181432.28728784006671049, 533189.54966634477023035 181438.99745146580971777, 533257.37403261545114219 181533.14433782830019481, 533340.41452438081614673 181492.83427136726095341, 533338.70870435202959925 181483.54382457892643288, 533339.90022310265339911 181474.30955426144646481, 533358.96452311298344284 181468.35196050821105018, 533371.7733496823348105 181461.2028480043518357, 533421.18748124549165368 181431.14743276051012799, 533457.81188699707854539 181401.60169366677291691, 533466.42939423269126564 181399.13954874229966663, 533532.90730719361454248 181489.9311428323853761, 533627.23823461274150759 181537.48131668634596281, 533600.77017667470499873 181593.49511371820699424, 533571.96468304062727839 181647.30677931586978957, 533565.79550759738776833 181677.67810457508312538, 533571.43902549741324037 181761.11675010700128041, 533688.88424648460932076 181775.70174559103907086, 533695.46948461106512696 181806.18034129549050704, 533711.03833596489857882 181690.5134740429057274, 533774.42839107918553054 181698.56300485107931308, 533904.80115716229192913 181714.28477588956593536, 533897.61435122019611299 181746.38584243066725321, 534052.37023917213082314 181783.27811293312697671, 534085.0618540165014565 181674.51498261015512981, 534131.12462164927273989 181691.05033509369241074, 534139.47207866376265883 181655.85994260499137454, 534150.19790721382014453 181658.82599177915835753)</t>
-  </si>
-  <si>
     <t>Initial Draft</t>
   </si>
   <si>
@@ -254,9 +245,6 @@
     <t>v3 20230707</t>
   </si>
   <si>
-    <t>LineString (530577.23797894886229187 180877.97880632089800201, 530617.74819760688114911 180823.78270298111601733, 530460.08680607296992093 180724.14946249785134569, 530317.89046422939281911 180623.28449239319888875, 530146.54318801360204816 180467.81284240834065713, 530072.77626957895699888 180399.24656015267828479, 530035.55066324456129223 180349.42993991106050089, 529890.48028561775572598 180246.51208710417267866, 529825.74567924335133284 180200.98946149481344037, 529919.54799574031494558 180130.36585574291530065, 529957.12143912480678409 179966.409011882962659, 529911.86251868435647339 179845.57623372576199472, 529906.73886731371749192 179702.96793724340386689, 529926.37953090108931065 179692.72063450215500779, 529923.81770521576981992 179643.19200458613340743, 529919.54799574031494558 179631.23681805469095707, 529921.4103331834776327 179584.29027873513405211, 529930.04384519555605948 179550.71550979930907488, 529930.52348475181497633 179516.66110130725428462, 529941.07555498881265521 179505.62939151405589655, 529912.29718161525670439 179479.72885547782061622, 529902.96647088008467108 179374.86438768959487788, 529800.47367502108681947 179363.00662448359071277, 529739.62031473114620894 179333.45689976593712345, 529740.46023528114892542 179272.14269961469108239, 529760.61832848156336695 179193.19016791306785308, 529641.34961037908215076 179153.71390206224168651, 529568.27652252756524831 179120.95700061158277094, 529550.34316133812535554 179093.66307770530693233, 529617.62970972212497145 178970.86160351810394786, 529616.82995180855505168 178944.1724078263505362, 529593.97022081958130002 178995.33693686561309732, 529513.20162077283021063 179036.94500355634954758, 529526.79745115165133029 179077.07363828388042748, 529564.38437103840988129 179130.25138729959144257, 529513.81095916836056858 179152.52902801893651485, 529512.12165939807891846 179263.45971292795729823, 529524.55590479262173176 179301.70093485678080469, 529448.61280135076958686 179371.58212878205813468, 529385.91768299601972103 179410.16374007728882134, 529333.16189551877323538 179435.02868727562599815, 529281.9714767278637737 179374.53091961363679729, 529220.891999761457555 179328.57588456268422306, 529164.02991525223478675 179367.55040796031244099, 529081.42719402140937746 179391.9821987469040323, 529060.48565906146541238 179415.83228022902039811, 529027.32822870835661888 179419.32253605569712818, 528999.98789139953441918 179308.21605890721548349, 529003.47814722615294158 179297.74529142724350095, 529055.25027532153762877 179270.40495411845040508, 529084.33574054366908967 179209.47090447816299275, 529104.11385689466260374 179164.09757873168564402, 529351.77659326093271375 179225.75876500256708823, 529383.05599977204110473 179235.19909444704535417, 529373.87950731569435447 179284.14038754784269258, 529392.23249222850427032 179227.24613431817851961, 529266.2086624939693138 179192.37546298385132104, 529269.26749331271275878 179176.46954272608854808, 529304.13816464703995734 179174.63424423482501879, 529268.04396098526194692 179166.06951794217457063, 529196.15887484396807849 179120.03240704443305731, 529149.98932790081016719 179107.75948950258316472, 529203.17197058210149407 179134.6430231656995602, 529187.39250517124310136 179174.383899015490897, 529058.81908330414444208 179141.07169425903703086, 529011.0423685876885429 179146.33151606269530021, 528858.21532395936083049 179161.52655682878685184, 528770.55162723187822849 179211.78707628592383116, 528715.03128597105387598 179321.6589095177478157, 528618.60121957084629685 179477.9925020151422359, 528491.34275315469130874 179622.19928313192212954, 528388.04569717741105705 179719.06766801583580673, 528360.57773886946961284 179750.62659883772721514, 528302.13527438452001661 179698.61280544605688192, 528281.73319864494260401 179662.65391637163702399, 528262.13372618111316115 179565.91304187983041629, 528297.16959096642676741 179504.60027850553160533, 528354.10287124256137758 179445.47725668028579094, 528571.1610022954409942 179230.06143178927595727, 528461.67392484133597463 179117.28974201151868328, 528427.73293083056341857 179154.51534834591438994, 528270.83738425537012517 178995.94010165525833145, 528307.81268304819241166 178962.03991528681945056, 528251.02088932693004608 178905.98091890395153314, 528237.09773989859968424 178880.69941073132213205, 528445.48698298842646182 178680.18773902862449177, 528506.68087698111776263 178769.79506966570625082, 528622.96355511201545596 178714.21878967669908889, 528690.51011079095769674 178852.7319798031821847, 528629.80371264915447682 178709.94369121600175276, 528706.32797509559895843 178677.88045276078628376, 528675.97477602458093315 178675.74290353045216762, 528565.03597096959128976 178505.16647494878270663, 528591.54158142581582069 178459.85043126542586833, 528535.96530143683776259 178489.77612049027811736, 528478.67898206354584545 178502.6014158723410219, 528322.21037840214557946 178459.85043126542586833, 528311.95014209649525583 178498.3263174116727896, 528292.28468917729333043 178492.34117956669069827, 528227.69070692639797926 178577.5864321083354298, 528109.89053357648663223 178750.95101042950409465, 528057.58673679200001061 178714.85402391621028073, 528050.95667804463300854 178736.21754654651158489, 528039.90658013243228197 178798.09809485499863513, 528075.26689345156773925 178816.51492470869561657, 528057.36634973983746022 178881.49318986901198514, 528077.50150927738286555 178927.95894264802336693, 527957.20683819404803216 178903.17720783254480921, 527893.18735658738296479 178892.33519885077839717, 527901.3675460263621062 178842.38277947145979851, 527870.26802183757536113 178834.76434196019545197, 527853.8672185888281092 178819.73012841463787481, 527876.57178353331983089 178723.1521395173331257, 527822.2081079538911581 178692.29039585794089362, 527839.85880704678129405 178661.95543657644884661, 527875.91507322294637561 178584.04074644856154919, 527702.52480672812089324 178435.08524715233943425, 527673.89863282348960638 178393.55225022041122429)</t>
-  </si>
-  <si>
     <t>LineString (527158.31216002732980996 177000.8693951431196183, 527099.77578929206356406 176863.97566198912682012, 526993.89284357777796686 176974.11520853615365922, 526965.6928630608599633 177009.76424051032518037, 526918.33817879669368267 176978.37180936889490113, 526881.62499661440961063 176915.05487198193441145, 526809.33459098706953228 176814.57045149418991059, 526803.78523573139682412 176782.81458185013616458, 526837.9906987837748602 176724.64684572990518063, 526829.14218303072266281 176698.07787916850065812, 526713.59169160143937916 176585.58887918625259772, 526702.01159683079458773 176498.87495989364106208, 526728.35331819928251207 176459.47930909239221364, 526759.08459305611904711 176456.02855037362314761, 526877.73335154261440039 176444.22870948346098885, 526952.37421362893655896 176459.79166246333625168, 526957.30744241294451058 176431.45683538325829431, 527038.82798124512191862 176435.9939717588131316, 527098.5913686784915626 176454.87681948934914544, 527051.24293423152994365 176594.92815045249881223, 527174.99744662863668054 176650.61612686808803119, 527153.14015064027626067 176640.28990523278480396, 527205.55905537132639438 176487.71942607063101605, 527102.71056710940320045 176449.37945362422033213, 527080.02346470882184803 176442.65865531019517221, 527118.21201132400892675 176315.62328595775761642, 527136.13724749034736305 176310.16777929847012274, 527123.4023648789152503 176243.66339232763857581, 527158.08696234272792935 176237.9932378021767363, 527169.22996887960471213 176208.6499966005794704, 527150.43826302816160023 176186.18838753091404215, 527118.65549396350979805 176157.02174997527617961, 527093.6976608419790864 176147.4813768335734494, 527018.22708262107335031 176131.11693114246008918, 526849.86647974920924753 176114.85084184003062546, 526845.07710992521606386 176097.65762165782507509, 526857.65365130186546594 176044.64240146498195827, 526893.8380195926874876 176044.15844629961065948, 526858.37810308812186122 176039.0902959554514382, 526874.83542804175522178 175886.27227852959185839, 527054.69047931989189237 175862.7618143102445174, 527176.94489326048642397 175856.8841982554004062, 527195.27535622008144855 175822.70450227480614558, 527223.9658216992393136 175795.75699128504493274, 527224.12844125344417989 175773.97201046324335039, 527243.25712752784602344 175756.61424477020045742, 527267.78618826356250793 175718.31265972839901224, 527222.48707379773259163 175682.39379150536842644, 527195.04935412993654609 175648.09664192068157718, 527009.0825874931178987 175569.97535675560357049, 526824.66230209683999419 175469.42516340431757271, 526795.48152648622635752 175473.6317607709497679, 526758.33231608534697443 175456.72367672127438709, 526739.00449527858290821 175494.1876375125721097, 526659.79678197088651359 175453.90485760179581121, 526520.33526839537080377 175632.5364698740595486, 526494.29995637480169535 175591.88974311901256442, 526417.63095546839758754 175510.29328765845275484, 526347.42756016622297466 175447.95712626643944532, 526377.84023331629578024 175401.53346697887172922, 526474.02092083648312837 175290.30347386049106717, 526498.70052055746782571 175244.55399248562753201, 526475.29657367873005569 175230.89727244031382725, 526816.41278782673180103 175345.56198925705393776, 526851.47655176091939211 175305.71711282295291312, 526851.47655176091939211 175278.90286315878620371, 526865.43143400084227324 175215.89678796651423909, 526877.77642672799993306 175178.34743508807150647, 526907.09578445507213473 175139.25495811874861829, 526889.09267006127629429 175116.10809675537166186, 526973.96449506049975753 174912.93009145429823548, 526885.95633615972474217 174859.8365453231963329, 526909.64957838621921837 174789.88203135458752513, 526922.28532687691040337 174784.41939029871718958, 526957.33885194035246968 174894.75840272463392466, 526938.1368365534581244 174894.58398754562949762, 526918.67389838397502899 174882.02661713416455314, 526881.00047726207412779 174863.13230195376672782, 526645.98297396756242961 174831.60109246335923672, 526609.50912189844530076 174827.05741743353428319, 526567.45242367009632289 174822.48189269431168213, 526532.3543359829345718 174820.95671778128598817, 526511.19253406394273043 174818.36392042905208655, 526475.19840611529070884 174928.17651417059823871, 526482.59550444374326617 174953.18938274509855546, 526532.22763051942456514 174964.2464009866816923, 526571.62909553560893983 174894.99534126126673073, 526580.38497665035538375 174835.29615184283466078, 526489.64220873429439962 174815.59541933474247344, 526246.86550509929656982 174761.46815426199464127, 526221.64969290501903743 174759.09444567150785588, 526209.46505330502986908 174784.94649092113832012, 526160.02340298215858638 174854.23032570173381828, 526124.6438850344857201 174921.36244024016195908, 526014.36327163595706224 175074.63272621412761509, 526017.3072057357057929 175100.90490151091944426, 525993.2115238078404218 175089.59430634311866015, 525977.26344060234259814 175063.01416766727925278, 525818.40223485918249935 175038.85706352663692087, 525828.51382325252052397 174995.27803120561293326, 525849.7215751651674509 174948.58325841222540475, 525805.44013935560360551 174918.05182387726381421, 525814.23011417349334806 174839.56990586066967808, 525702.0009714097250253 174820.10639019258087501, 525698.8616946890251711 174722.78881185199134052, 525659.9346633527893573 174636.77262970581068657, 525565.36717306601349264 174664.02053710119798779, 525538.06676878000143915 174653.24728339188732207, 525493.99436724185943604 174553.83953325595939532, 525459.71583271224517375 174532.29302583733806387, 525496.93252734444104135 174407.42122147939517163, 525457.92714756459463388 174534.53035107266623527, 525490.77226448152214289 174556.32890400406904519, 525543.79577161197084934 174666.49996881955303252, 525536.72597066126763821 174676.51552016640198417, 525515.04797329346183687 174692.30743877869099379, 525500.11743205995298922 174748.58409419711097144, 525507.00845109077636153 174843.90985745683428831, 525596.59169849148020148 174873.7709399237355683, 525710.00638670718763024 174878.36495261095114984, 525777.76807384355925024 174928.89909217032254674, 525768.58004846912808716 175008.14581102479132824, 525718.31548450421541929 175117.9094939905917272, 525718.31548450421541929 175117.9094939905917272)</t>
   </si>
   <si>
@@ -266,37 +254,52 @@
     <t>LineString (538057.11912127735558897 181862.36995379574364051, 538053.62050980445928872 181858.87134232284734026, 538078.00283839902840555 181725.81349199247779325, 537941.46179826941806823 181703.52107727742986754, 537993.7096452577970922 181642.91357477093697526, 538053.69201395311392844 181543.8893257146992255, 537933.4239803443197161 181488.67192663639434613, 538057.85222895222250372 181541.24191616984899156, 538066.94687634671572596 181538.87918232899392024, 538082.506038723513484 181524.15319597572670318, 538090.42530879157129675 181509.20216024381807074, 538125.44152047054376453 181443.09396750494488515, 538174.66927109437528998 181352.78140245075337589, 538212.79301781801041216 181233.2282937929558102, 538225.66242323035839945 181199.85061172995483503, 538241.47548658237792552 181194.25015179277397692, 538274.4193685658974573 181215.99311390187358484, 538284.63197198079433292 181249.59587352504604496, 538292.94811339187435806 181286.28655660181539133, 538290.81553514266852289 181260.73360870234319009, 538312.43949847598560154 181260.35753977482090704, 538331.80704824393615127 181267.31481493418687023, 538327.67029004113283008 181291.66527799205505289, 538335.56773751927539706 181269.47721126751275733, 538339.14039233094081283 181284.1438994413765613, 538474.63447606388945132 181330.39465194242075086, 538488.79537792666815221 181288.87746238996624015, 538509.7148920422187075 181224.50972664973232895, 538549.53403901937417686 181124.09031605365453288, 538569.65582116693258286 181131.19212151752435602, 538573.00177168450318277 181118.41270654619438574, 538582.57363540562801063 181121.34447346715023741, 538588.59396907058544457 181104.41239674753160216, 538561.66629002010449767 181093.31582571024773642, 538598.21099730290006846 180963.41196743381442502, 538615.37369384057819843 180937.37201406632084399, 538635.46388516668230295 180855.08748821140034124, 538664.80175754404626787 180853.98271477461094037, 538664.80175754404626787 180848.70435279875528067, 538705.12598798738326877 180838.79208001849474385, 538708.31755569379311055 180833.63647064674296416, 538729.99642427545040846 180840.20523449187749065, 538707.07831848983187228 180830.60309832252096385, 538703.25330118928104639 180837.43348635928123258, 538663.36383505456615239 180847.26924513219273649, 538663.91026609751861542 180852.73355556160095148, 538660.24865216040052474 180844.65553881169762462, 538640.96016229398082942 180837.16027083780500107, 538544.24186769349034876 180802.73511513255652972, 538450.80215935071464628 180793.71900292404461652, 538430.0377797189867124 180786.06896832288475707, 538416.10378812404815108 180768.30995942730805837, 538405.72159830818418413 180775.6867785069916863, 538415.28414155961945653 180756.83490752556826919, 538418.01629677438177168 180719.40438108413945884, 538406.54124487261287868 180719.40438108413945884, 538409.000184565782547 180685.25244090033811517, 538395.33940849232021719 180678.69526838505407795, 538382.49827898317016661 180675.41668212742661126, 538362.28033039439469576 180657.65767323184991255, 538356.81601996498648077 180676.23632869182620198, 538348.34633879945613444 180663.94163022565771826, 538323.75694186717737466 180621.86643991924938746, 538322.93729530274868011 180593.17881016488536261, 538328.4016057321568951 180552.46969746579998173, 538322.6640797812724486 180530.61245574819622561, 538329.76768333942163736 180524.87492979731177911, 538343.42845941300038248 180540.99464556406019256, 538349.98563192831352353 180540.99464556406019256, 538343.97489045595284551 180555.74828372345655225, 538352.71778714295942336 180560.93937863138853572, 538365.01248560915701091 180534.98390409172861837, 538371.84287364582996815 180527.88030053349211812, 538376.48753751092590392 180495.36765347851905972, 538383.86435659055132419 180427.33698863245081156, 538397.2519171426538378 180335.26335789696895517, 538386.32329628383740783 180280.34703808143967763, 538356.54280444351024926 180181.98945035215001553, 538349.86702627711929381 180158.3111812362622004, 538333.93950255436357111 180158.96128424536436796, 538325.81321494071744382 180125.48097927699564025, 538338.16517211345490068 180121.9054127269773744, 538312.80498378432821482 180015.22765528378658928, 538309.48158343171235174 179915.05087322887266055, 538303.30955420562531799 179855.22966688327142037, 538278.62143730116076767 179762.64922849129652604, 538277.6718943432206288 179740.33496898142038845, 538278.14666582213249058 179706.15142249822383747, 538284.31869504833593965 179692.38304960916866548, 538274.34849399072118104 179684.31193446728866547, 538260.58012110169511288 179479.68542704707942903, 538283.84392356942407787 179380.45818795004743151, 538276.46764299820642918 179373.42610627005342394, 538286.21778096398338675 179367.16458653993322514, 538328.94721406803000718 179194.82253968715667725, 538373.10096160881221294 179125.98067524185171351, 538412.337829110911116 179066.10921436137869023, 538405.98546794115100056 179059.09686761553166434, 538415.39026240026578307 179061.24182073780684732, 538432.44739647547248751 179038.1479516392282676, 538557.31229543488007039 178855.83570372880785726, 538560.63569578749593347 178836.37007309254840948, 538544.49346550367772579 178770.85160899977199733, 538392.56659224512986839 178811.6819561880256515, 538328.48941097827628255 178579.7348779343010392, 538315.17884117900393903 178559.57830087453476153, 538294.47845585108734667 178453.40847317627049051, 538304.19587160169612616 178433.00190009997459128, 538253.66530969843734056 178404.8213944231683854, 538283.78929852542933077 178333.88425944367190823, 538307.11109632684383541 178343.60167519428068772, 538318.77199522766750306 178346.5168999194575008, 538335.11924329411704093 178348.77976422818028368, 538281.84581537533085793 178321.25161896785721183, 538252.69356812338810414 178330.96903471846599132, 538232.28699504712130874 178316.39291109255282208, 538044.79800434643402696 178261.3466268312477041, 538019.15639011771418154 178253.05674019930302165, 538025.32914176001213491 178211.08202903144410811, 537920.39236384036485106 178207.37837804603623226, 537794.46823033690452576 178227.13118330150609836, 537698.17330471647437662 178260.46404217008966953, 537658.66769420565105975 178275.27864611166296527, 537636.4457882932620123 178285.15504873939789832, 537613.32763770420569927 178298.05650823522591963, 537459.7524428729666397 178375.6691471713129431, 537456.14730042521841824 178381.81708270622766577, 537556.97021414036862552 178513.66243141060112976, 537678.42049946112092584 178674.65567737040692009, 537642.61853993555996567 178704.28488525358261541, 537655.49145826080348343 178726.26947054677293636, 537656.62345710769295692 178743.01280580330058001, 537645.11526750994380563 178749.34231008208007552, 537658.54148870729841292 178753.46607802127255127, 537643.36394558555912226 178764.38451038327184506, 537846.50558974756859243 178742.98746254466823302, 537864.34695504221599549 178732.03885750484187156, 537921.10559516295325011 178705.15133090259041637, 537929.97295804345048964 178681.03210386767750606, 537934.22929222602397203 178722.8860566635557916, 537931.391736104269512 178762.2571478528843727, 537923.27317417750600725 178793.5180244478979148, 537919.38620787719264627 178840.16162005084333941, 537924.24491575255524367 178882.91824935356271453, 537923.94315128470771015 178917.25865100373630412, 537939.79278095357585698 179148.20369934543850832, 537945.62323040387127548 179326.0324075817479752, 537596.7680049566552043 179354.21291325855418108, 537587.05058920604642481 179321.17369970644358546, 537583.16362290584947914 179361.01510428398614749, 537578.30491503048688173 179418.34785721261869185, 537345.08693701564334333 179405.71521673683309928, 537341.19997071544639766 179448.9577168270770926, 537339.25648756534792483 179477.62409329140791669, 537446.14806082216091454 179485.39802589188911952, 537438.37412822165060788 179644.76364420205936767, 537455.86547657276969403 179648.650610502314521, 537520.97216210188344121 179645.73538577710860409, 537523.7159856699872762 179645.73538577710860409, 537550.12440935370977968 179645.73538577710860409, 537546.72331384103745222 179683.14743641699897125, 537621.06154433323536068 179697.72356004291214049, 537630.77896008384414017 179799.27055463689612225, 537550.12440935370977968 179816.76190298801520839, 537528.26022391486912966 179825.02170637605013326, 537537.97763966547790915 179912.96431891914107837, 537544.29395990341436118 179930.94153805778478272, 537492.79165642510633916 179940.65895380839356221, 537507.85365083860233426 179979.04274602336226963, 537506.88190926343668252 180020.8276337510033045, 537501.05145981314126402 180022.28524611360626295, 537502.02320138819050044 180025.68634162630769424, 537416.05443968356121331 180037.57935224322136492, 537411.13920003117527813 180046.84167782287113369)</t>
   </si>
   <si>
-    <t>LineString (525327.85414873412810266 178420.77501689142081887, 525434.3555114408954978 178547.73350585880689323, 525347.43806628719903529 178651.24739231160492636, 525430.2491754493676126 178706.68292819705675356, 525486.36910066672135144 178623.18742970289895311, 525558.91436985018663108 178563.64555782591924071, 525601.34650842915289104 178515.0539152596029453, 525591.59441469295416027 178508.14618219647672959, 525612.31761388236191124 178515.8665897376195062, 525739.09483245271258056 178641.42479659095988609, 525767.53843918326310813 178664.58601921438821591, 525708.21320228814147413 178737.72672223576228134, 525731.62045715074054897 178716.68428954426781274, 525769.37393091234844178 178666.83504263576469384, 525806.39432751352433115 178612.95387134497286752, 526026.40911028429400176 178722.27400289245997556, 526144.43453311175107956 178765.52555535719147883, 526255.77580733434297144 178814.4714835460181348, 526271.20979337661992759 178817.35269416749360971, 526312.78246261400636286 178730.88154215391841717, 526431.85428454133216292 178507.28957353180157952, 526371.81847308482974768 178458.83962042655912228, 526552.97916730435099453 178570.48516453863703646, 526555.08568700461182743 178631.57423584524076432, 526525.59441120142582804 178796.93603231309680268, 526496.81081177107989788 178977.54604629526147619, 526531.73185393039602786 178797.25923736946424469, 526578.25740370713174343 178795.88277246299549006, 526808.88298217917326838 178842.85059796637506224, 526867.58985495707020164 178857.72481234182487242, 526887.47400313417892903 178869.08718272874830291, 526862.61881791288033128 179084.26207193068694323, 526876.82178089639637619 179026.0299236977880355, 526893.15518832765519619 179011.11681256498559378, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527768.86287219019141048 179171.7344985579547938, 527738.35830124607309699 179152.01631094136973843, 527772.52151037787552923 179165.95770141950924881, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528513.98412839835509658 179812.26687349064741284, 528529.45710146625060588 179823.30889789306093007, 528599.09828376933000982 179804.26158560626208782, 529067.56848417001310736 179787.9540786303114146, 529126.86850953719113022 179829.46409638732438907, 529184.68603427021298558 179833.91159828985109925, 529236.57355646649375558 179804.26158560626208782, 529461.54302770318463445 179967.33665536600165069, 529365.1804864815203473 180130.41172512577031739, 529330.03977657249197364 180104.57000673143193126, 529326.57823726569768041 180122.37220888037700206, 529506.08377560100052506 180233.14146669604815543, 529430.42441646789666265 180361.7129266606643796, 529518.94092159741558135 180419.07557802950032055, 529552.56730343436356634 180373.58106142663746141, 529648.71743816568050534 180427.49491339456290007, 529608.480220987345092 180501.82199512678198516, 529569.44679091090802103 180572.25595415246789344, 529667.74284364131744951 180629.72475247565307654, 529730.9295924516627565 180529.48919386579655111, 529787.31384936452377588 180567.2724588074197527, 529763.12702995492145419 180622.33490404754411429, 529706.82561028259806335 180576.71049719117581844, 529752.5037739867111668 180495.92673939117230475, 529740.29997511499095708 180487.27313655486796051, 529754.05698475218378007 180486.60747479822020978, 529800.36167021188884974 180412.51190174778457731, 529824.728592021856457 180415.94968910259194672, 529890.00781108462251723 180459.31649564448161982, 529865.28168949380051345 180503.69017882505431771, 529855.61934717127587646 180535.74483229906763881, 529894.55648332042619586 180548.55958596843993291, 529890.50570647965651006 180564.17520972224883735, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530050.41157349967397749 180610.86616918962681666, 530235.09162783063948154 180613.78033897408749908, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530441.01278525067027658 180758.81861569813918322, 530400.55581117747351527 180811.16401171206962317, 530508.37677010952029377 180901.19154505711048841, 530524.57064777321647853 180911.87319211009889841, 530583.04193836136255413 180879.49776674556778744)</t>
-  </si>
-  <si>
     <t>LineString (531565.23039256664924324 178567.62021348648704588, 531600.88228947878815234 178584.2162747971015051, 531772.37417057063430548 178639.05066937819356099, 531797.10340734256897122 178657.86639300896786153, 531837.96040722646284848 178713.77597179752774537, 531857.31372296100016683 178741.19316908807377331, 531868.06556503567844629 178749.79464274787460454, 531880.13844949356280267 178747.46484413990401663, 531893.87027424620464444 178732.70546787517378107, 531882.84744893456809223 178737.65639788802945986, 531874.82179012312553823 178745.74090769540634938, 531873.81108064437285066 178750.26503583858720958, 531928.47747769311536103 178812.55852085907827131, 531938.12053605390246958 178829.1566770619538147, 531932.74461501650512218 178852.9451276523177512, 531965.13453926669899374 178839.37092703295638785, 531981.7662949759978801 178846.35962438152637333, 532009.72108437039423734 178845.01564412217703648, 531981.39670040470082313 178850.0555700947297737, 531960.96820046263746917 178846.83001747232628986, 531933.5510031720623374 178860.26982006573234685, 531935.16377948329318315 178924.24328041044645943, 531930.32545054971706122 179009.45162885275203735, 531910.43454271147493273 179022.35383934245328419, 531885.70530593954026699 179057.83491818906622939, 531876.11210935655981302 179066.35873417466063984, 531831.93818780174478889 179086.51181359370821156, 531779.46893305156845599 179106.20686848048353568, 531672.18940927542280406 179157.81096578075084835, 531589.70353428379166871 179198.03799872964737006, 531556.67969205614645034 179124.41894058702746406, 531620.5699304185109213 179098.98690395732410252, 531635.7671230387641117 179139.9262799954158254, 531648.27035036904271692 179178.57474457612261176, 531695.00515957863535732 179157.60464692092500627, 531797.07743173581548035 179112.31386224390007555, 531810.86905931774526834 179106.1050852510088589, 531847.91815481544472277 179173.68914956544176675, 531891.07424407650250942 179215.21670715624350123, 531905.47685013443697244 179238.60377113270806149, 531919.96244928787928075 179292.40742513118311763, 531957.96748593868687749 179272.83832924981834367, 531967.94273236184380949 179364.63301262669847347, 531985.87575963942799717 179480.30103856680216268, 531979.93544435373041779 179495.99243743464467116, 531952.58757775544654578 179485.23262106810580008, 531939.54275271145161241 179490.46462862013140693, 531766.64450117154046893 179467.29959379057982005, 531761.71291867026593536 179464.16131401702295989, 531729.43346957070752978 179458.33308015181683004, 531718.67365320411045104 179473.57615333772264421, 531714.63872206665109843 179523.78862971480702981, 531716.09578053292352706 179527.48731659070472233, 531741.86680176388472319 179544.99216120038181543, 531751.2878118836088106 179549.55071448421222158, 531794.563677724217996 179583.10166665274300613, 531736.03185356059111655 179657.43647553340997547, 531711.23332369688432664 179690.98742770194076002, 531710.01770948793273419 179697.49096372016356327, 531768.36719152017030865 179689.71103278253576718, 531817.90347053715959191 179690.92664699154556729, 531827.62838420912157744 179689.71103278253576718, 531830.54585831076838076 179679.74299626867286861, 531848.91713031963445246 179689.19716539108776487, 531944.69973392877727747 179685.07748351542977616, 532042.54217847576364875 179713.40029641060391441, 532046.66186035145074129 179723.69950109976343811, 531964.78318307269364595 179783.43488829687703401, 531949.33437603886704892 179795.79393392385100015, 531887.02418766950722784 179851.66711936253705062, 531644.24913323228247464 179809.83732716954546049, 531648.01059164851903915 180039.80038389487890527, 531634.26440454111434519 180047.81851008319063112, 531623.9049881329992786 180054.69994857980054803, 531597.20816948893480003 180046.74794410250615329, 531509.86933764221612364 180049.32525078213075176, 531523.18559562193695456 180126.19637639203574508, 531515.31689772487152368 180157.06588352672406472, 531576.1272732806392014 180172.41316700863535516, 531565.55550737539306283 180212.44941103307064623, 531546.7916893131332472 180213.05469548667315394, 531534.08071578713133931 180378.90263577894074842, 531523.7637067319592461 180401.07970175734953955, 531452.49236999533604831 180382.73106677527539432, 531430.23252644832246006 180461.2673656364204362, 531482.0090381617192179 180489.08967605925863609, 531642.51904925843700767 180503.81476687197573483, 531641.9708823268301785 180395.39141782445949502, 531740.48138779681175947 180345.31959500885568559, 531899.45102110982406884 180269.32835973758483306, 531947.79937211831565946 180253.32166861725272611, 532077.03169044503010809 180211.29727531352546066, 532099.03156049200333655 180191.19724142824998125, 532036.57553188200108707 180178.45843636387144215, 532057.05969537724740803 180033.36227827219408937, 532071.14023115881718695 180019.57570919854333624, 532207.19135398743674159 180042.54381057742284611, 532098.64082088705617934 180352.62898129189852625, 532040.88056060869712383 180356.72434775123838335, 532096.3210087432526052 180363.38491236304980703, 532152.37729773903265595 180433.03831291184178554, 532202.94655013689771295 180431.75807867391267791, 532256.71638812962919474 180407.43362815340515226, 532374.97802585770841688 180393.35105153627227992, 532459.60804447636473924 180370.57185269574983977, 532461.19814912823494524 180285.76627126333187334, 532465.92665053717792034 180247.43457141483668238, 532493.4954023661557585 180222.92901423358125612, 532452.90807328466325998 180147.11494670400861651, 532527.19054349034558982 180142.52015473254141398, 532537.91172475717030466 180135.62796677529695444, 532618.38267560245003551 180157.40526832704199478, 532552.64666788431350142 180254.39529883849900216, 532628.93604597891680896 180260.83616025268565863, 532642.84987088851630688 180321.27857628939091228, 532664.46415251330472529 180368.25469532946590334, 532702.02634320827201009 180359.40188057228806429, 532839.63639755162876099 180333.20402154928888194, 532901.66608916665427387 180315.59065232524881139, 532923.87425036216154695 180282.66130986291682348, 533132.17148640297818929 180152.47553733742097393, 533126.72782159631606191 180120.77814802477951162, 533177.19047552125994116 179911.81100420773145743, 533177.19047552125994116 179911.81100420773145743, 533144.89093221118673682 179901.35225368669489399, 533108.5248437209520489 179872.42468329664552584, 533066.37324115261435509 179864.98616519634379074, 533049.84320092969574034 179750.92888765849056654, 533107.84760892775375396 179739.26681170516530983, 533140.86942005890887231 179734.16034606634639204, 533223.25373236555606127 179757.30965696240309626, 533248.27541399584151804 179688.03193979547359049, 533327.25541587651241571 179685.30849145477986895, 533413.72490069409832358 179664.20176681425073184, 533458.66179831593763083 179668.28693932530586608, 533460.88135104614775628 179717.44317431433591992, 533457.67475742171518505 179745.3986485997447744, 533465.68402344128116965 179805.36506646597990766, 533373.55403766862582415 179881.39677198612480424, 533374.91576183901634067 179946.07867007807362825, 533387.17127937218174338 180014.16487859591143206, 533381.73899602494202554 180032.14720059430692345, 533433.43858268216717988 179996.43141658138483763, 533486.57714380824472755 179980.80263642215868458, 533569.64231819997075945 179956.29160135574056767, 533665.64387221017386764 179901.82263454148778692, 533728.9640461317030713 179852.80056440862244926, 533763.00715039065107703 179912.03556581915472634, 533731.00663238728884608 179845.99194355684448965, 533825.00356353784445673 179775.30611803027568385, 533788.87545132858213037 179712.8257357390539255, 533730.70547138899564743 179746.56884022831218317, 533777.98611626459751278 179715.60685424524126574, 533886.92404989304486662 179672.03168079382157885, 534054.41612284700386226 179527.68891873603570275, 534134.50261897931341082 179505.72398318111663684)</t>
   </si>
   <si>
-    <t>LineString (530784.23736255615949631 182302.13991453754715621, 530778.6444442254723981 182309.68591545993695036, 530773.74559282837435603 182337.44607337698107585, 530858.50592793908435851 182423.17597282669157721, 530936.88755029300227761 182449.3031802780169528, 531037.31400393415242434 182542.38135682337451726, 531094.36521082976832986 182594.22753410961013287, 531155.37121963454410434 182521.76535719376988709, 531166.80187289451714605 182513.19236724881920964, 531203.95149598934222013 182472.57272441431996413, 531259.88004943984560668 182529.52187190589029342, 531326.62689972575753927 182604.63759332848712802, 531370.30832468345761299 182662.60733486112440005, 531384.59664125845301896 182683.83569091532262973, 531369.90008706704247743 182687.50982946317526512, 531339.69050345139112324 182687.10159184673102573, 531257.94092076190281659 182652.80963206687010825, 531233.85490139271132648 182679.95743355926242657, 531204.76797122228890657 182711.18761121592251584, 531182.72313993528950959 182813.24701532270410098, 531203.13502075662836432 182831.20947044549393468, 531268.45303938491269946 182871.21675685534137301, 531362.55180997133720666 182909.59109279947006144, 531365.40947328635957092 182920.61350844299886376, 531354.79529525921680033 182956.13018107216339558, 531444.90684366086497903 182988.57858534331899136, 531474.10273866006173193 182998.58689318058895878, 531486.5355991879478097 183012.4143484897504095, 531547.55104103893972933 183034.71440845559118316, 531569.85110100475139916 183061.97003730272990651, 531517.81762775115203112 183110.59655695044784807, 531527.72876551374793053 183131.65772469594958238, 531497.95239027438219637 183140.93648922778083943, 531508.4095920140389353 183177.7640257888706401, 531495.22442460327874869 183139.57250639220001176, 531524.09539462334942073 183130.25195701562915929, 531519.54878517135512084 183120.02208574867108837, 531516.59348902758210897 183111.38352778987609781, 531448.32344150589779019 183136.55978571731247939, 531241.26357583678327501 183121.43743597742286511, 531197.64141312555875629 183108.64160158214508556, 530715.12526052596513182 183043.21945667950785719, 530703.01725020399317145 183063.42695543030276895, 530695.13352120853960514 183041.84071603690972552, 530546.28326243243645877 183024.95802384099806659, 530541.22589214832987636 183004.5417986634420231, 530703.18488589045591652 182946.11745994322700426, 530775.51721857010852545 182908.57789488162961788, 530786.04660877038259059 182895.30170723787159659, 530795.49963942251633853 182875.6843990063352976, 530804.3135183157864958 182802.06196081181406043, 530806.59301448101177812 182793.73684438230702654, 530819.8735573566518724 182794.33149555584532209, 530807.31673856556881219 182782.83954266682849266, 530812.03824553836602718 182733.95805871355696581, 530761.76808306365273893 182714.23882370966020972, 530770.16958811797667295 182659.52488996647298336, 530712.95603303634561598 182638.97244784975191578, 530630.19079316093120724 182601.20039206769433804, 530615.74853653833270073 182603.42227770193130709, 530555.75762441393453628 182723.95957335943239741, 530539.09348215709906071 182717.29391645672149025, 530547.14781758119352162 182730.62523026211420074, 530461.60522066289559007 182906.15419536712579429, 530437.90885532670654356 182917.93718825542600825, 530382.0339413866167888 182876.71421071342774667, 530325.26406243664678186 182961.75723386157187633, 530268.29162278701551259 182922.72056224985863082, 530249.18178586428985 182908.73221319253207184, 530252.98490572301670909 182894.20538857823703438, 530184.08185019285883754 182852.74914162818458863, 530085.83308541483711451 182787.51840435751364566, 530111.18260209145955741 182744.29519918368896469, 529999.02136356220580637 182666.39424455061089247, 529961.66046464198734611 182715.15181299234973267, 529988.72742143063805997 182735.23374867427628487, 529986.10803851566743106 182740.763557050464442, 529932.80478152283467352 182814.59110673272516578, 529984.94386833114549518 182734.94270612817490473, 529957.00378390413243324 182716.02494063068297692, 530013.09155612858012319 182629.12904521985910833, 530018.17775851185433567 182621.49974164497689344, 530100.32880480831954628 182494.38274551162612624, 530104.0113532249815762 182482.84132467227755114, 530220.50368910923134536 182556.47051627180189826, 530255.09743770561181009 182478.63458192982943729, 530272.39431200386025012 182483.35191128388396464, 530279.47030603489838541 182470.7723663397191558, 530137.95042541308794171 182415.73685720900539309, 530133.8373461066512391 182413.51172491264878772, 530186.21162480069324374 182272.1011724385607522, 530075.7495097367791459 182226.86884083910263143, 530075.1733111577341333 182226.46204725949792191, 530187.16388441331218928 182265.91148495653760619, 530233.22869966924190521 182154.23642371431924403, 530357.8921046924078837 182201.72724467553780414, 530348.98757576220668852 182228.44083146619959734, 530358.86895656702108681 182231.0766534095746465, 530394.74696868821047246 182125.29837629428948276, 530508.99968287569936365 182165.49652313266415149, 530513.72136097133625299 182167.0985210579528939, 530567.86575565708335489 182188.16529536261805333, 530573.45622016047127545 182150.89553200689260848, 530664.76714038196951151 181926.34520778860314749, 530694.76100652059540153 181850.76066511913086288, 530759.06664636044297367 181869.87285391447949223, 530674.73822676041163504 181825.22436629422008991, 530573.75377231650054455 181777.63399121144902892, 530599.29007114132400602 181730.04361612870707177, 530646.88044622412417084 181748.21467864664737135, 530657.97477119497489184 181732.12790743884397671, 530724.74751764547545463 181760.6236275052651763, 530741.12779784575104713 181707.06197263259673491, 530773.19373494503088295 181600.7954151411249768, 530782.75100370426662266 181575.85406711159157567, 530688.89235894195735455 181552.28991476428927854, 530627.95015930733643472 181539.24596229381859303, 530599.01706093887332827 181486.621268884598976, 530600.06536160444375128 181482.63772635560599156, 530608.87108719476964325 181476.34792236247449182, 530639.82865497504826635 181423.25654537187074311, 530713.75870660948567092 181269.28719607146922499, 530693.84197932516690344 181263.16111494251526892, 530645.94210892508272082 181237.73285941511858255, 530707.03671619179658592 181120.0358954158728011, 530733.0917692908551544 181051.75368729417095892, 530735.53599696443416178 181033.12102656494244002, 530692.8715660268208012 181009.95126327298930846, 530547.98248933651484549 181092.25378597865346819, 530472.93963134801015258 180978.161691593733849, 530516.46695041528437287 180923.52303003016277216, 530552.73794393055140972 180906.14858023868873715, 530579.45680101704783738 180882.17122962352004834)</t>
-  </si>
-  <si>
     <t>N7 Kings Cross</t>
   </si>
   <si>
-    <t>LineString (530577.55627936229575425 180873.29039143532281741, 530508.03351007960736752 180921.27411260729422793, 530398.23249808500986546 181052.05378589619067498, 530335.04888452554587275 181096.60453780728857964, 530313.7541854988085106 181095.4837641742778942, 530277.88942924339789897 181128.54658634730731137, 530208.96185081487055868 181204.75919339017127641, 530146.19852736778557301 181259.11671458987984806, 530115.37725246080663055 181311.23268852362525649, 530089.44054251117631793 181304.94443834689445794, 529993.94726804597303271 181289.97907443816075101, 529966.154449358349666 181292.82961994459037669, 529944.77535806014202535 181334.87516616433276795, 529944.77535806014202535 181344.13943906020722352, 529926.36038226482924074 181394.46298536835820414, 529818.3114558468805626 181372.26115117289009504, 529660.9002180868992582 181353.18405782332411036, 529658.19050382054410875 181346.70498227514326572, 529687.50564937863964587 181285.67399781054700725, 529721.54846181173343211 181300.10519003760418855, 529759.29157994396518916 181225.35901491285767406, 529693.52337177516892552 181197.2517148221086245, 529775.50000859634019434 181018.70994359909673221, 529775.97546259185764939 181007.7745017017587088, 529781.20545654278248549 181022.98902955889934674, 529838.73539000260643661 181058.17262522855889983, 529856.80264183296822011 181056.27080924643087201, 529884.37897357402835041 181053.41808527320972644, 529884.37897357402835041 181040.5808273937436752, 529841.11265998031012714 181013.00449565265444107, 529793.09180643118452281 180981.03021445288322866, 529813.06087424361612648 180938.71480885017081164, 529693.24646736856084317 180862.64216956440941431, 529636.19198790425434709 180936.81299286801367998, 529605.88993830105755478 180991.46413140607182868, 529541.23135347885545343 180948.44746960292104632, 529492.06945427530445158 181030.20584545240853913, 529469.24634072056505829 181064.96606145869009197, 529432.46901320235338062 181041.241028774617007, 529404.33170837664511055 181030.67362469981890172, 529429.55946595408022404 180980.22139381090528332, 529341.93906022026203573 180918.15693974946043454, 529376.73622655984945595 180868.47114977936143987, 529404.34578149160370231 180829.45268785100779496, 529357.79744094552006572 180794.99778872131719254, 529292.81591668562032282 180885.3186391938070301, 529219.30587300169281662 180833.15022109559504315, 529297.55850014905445278 180694.72606625544722192, 529251.79900507966522127 180679.08758315991144627, 529252.95472623594105244 180654.80634892109083012, 529237.65350798552390188 180675.84590674249920994, 529186.38057327619753778 180657.79299018002348021, 529111.49788893118966371 180613.026168017211603, 529033.15595014626160264 180735.32098674381268211, 528988.79609909397549927 180702.76329789814190008, 529001.00523241108749062 180683.22868459072196856, 528968.42684971622657031 180655.33458768369746394, 528933.41540621093008667 180638.92297354058246128, 528917.00379206787329167 180629.07600505475420505, 528956.39166601130273193 180565.6177637014479842, 528889.09824919363018125 180520.36887541532632895, 529037.60859426553361118 180322.19037864034180529, 528980.81174594059120864 180277.24678561804466881, 528985.75060231669340283 180264.89964467784739099, 528967.47683372523169965 180262.43021648982539773, 528869.68747747887391597 180180.56867205633898266, 528753.13046700344420969 180299.10122508218046278, 528754.16503672057297081 180299.4973738573025912, 528770.91830490494612604 180309.96816647247760557, 528791.62720585486385971 180329.97901458147680387, 528777.89595665864180773 180339.10883718938566744, 528784.87936172517947853 180328.35022461912012659, 528766.49707728379871696 180311.67933983076363802, 528735.71864135982468724 180290.81664662051480263, 528713.38623358681797981 180285.77175626676762477, 528668.77996420615818352 180275.46013541670981795, 528678.81986454653088003 180236.4348891912959516, 528685.54394682915881276 180209.20438540610484779, 528648.68728152720723301 180200.38155767129501328, 528657.51626427297014743 180164.64456824841909111, 528561.08355491538532078 180139.08601459197234362, 528473.16496016969904304 180096.57592482483596541, 528471.71575256390497088 180078.58159705405705608, 528455.77446890133433044 180078.09852785218390636, 528452.87605368986260146 180092.59060390916420147, 528456.2575381031492725 180107.5657491680176463, 528445.63001566135790199 180136.06683208007598296, 528434.51942401775158942 180130.75307085920940153, 528435.00249321956653148 180119.15941001361352392, 528434.03635481582023203 180138.48217808958725072, 528458.18981491075828671 180158.28801536746323109, 528508.42901190835982561 180176.64464503963245079, 528492.97079744748771191 180232.19760325804236345, 528463.50357613165397197 180225.43463443146902137, 528442.73160045000258833 180280.1422215465863701, 528368.29083982005249709 180530.61085074103903025, 528399.42485451779793948 180540.37256290816003457, 528373.18561336421407759 180528.66321234643692151, 528398.20391442335676402 180451.73774791724281386, 528402.87839129334315658 180453.56406502836034633, 528495.6276780579937622 180483.51435554612544365, 528631.8531929935561493 180596.55254879055428319, 528664.70189872267656028 180554.04245902341790497, 528713.73342271556612104 180597.76022179532446899, 528701.17362346616573632 180617.08298987129819579, 528701.17362346616573632 180635.4396195434674155, 528716.6318379269214347 180666.35604846503701992, 528751.41282046365085989 180679.88198611821280792, 528786.19380300038028508 180647.03328038906329311, 528882.80764338024891913 180721.42593748154467903, 528908.89338028279598802 180749.44395119170076214, 528941.25901681010145694 180770.21592687338124961, 528984.08419391023926437 180821.70737133437069133, 528974.05492355371825397 180859.35868258221307769, 528989.1841545554343611 180829.86192138504702598, 529040.11857240251265466 180898.90430847753304988, 529112.31183115229941905 180989.06747418479062617, 529080.35383750754408538 181057.74321855726884678, 529150.25737489317543805 181094.96458261978114024, 529105.31938657385762781 181161.35024718247586861, 529063.5588317719521001 181143.64740329908090644, 529046.76382603647653013 181133.20726459860452451, 529038.72230120946187526 181129.90637958364095539, 529016.40501055552158505 181225.42438358269282617, 528860.85349469736684114 181191.94844760172418319, 528825.25553268182557076 181309.48477439771522768, 528674.92537136201281101 181261.00874411704717204, 528689.63158279552590102 181226.14957627476542257, 528640.0662035197019577 181213.07738833394250832, 528719.58868015988264233 181095.42769686627434567, 528668.38927739160135388 181063.29190151169314049, 528617.73454912076704204 181139.00165666910470463, 528598.12626720953267068 181160.78863657053443603, 528611.19845515035558492 181136.82295867896755226, 528206.1428879996528849 181051.66365116246743128, 528237.1932889255695045 180958.33994615747360513, 528214.42299491330049932 180950.7498481533548329, 527957.73968059255275875 180869.32879683657665737, 527979.60677813622169197 180868.6474805666366592, 527980.52286685828585178 180863.87237577338237315, 528002.11622184654697776 180796.95082105748588219, 528147.20215247070882469 180846.02662784914718941, 528143.09763044805731624 180858.87556635460350662, 528222.86812366941012442 180886.3580181579454802, 528226.97264569206163287 180877.07822923734784126, 528255.5258423708146438 180886.00110319946543314, 528274.28005263407249004 180832.49227053558570333, 528413.89659711671993136 180874.71776203761692159, 528440.4577933840919286 180872.67459309397963807, 528441.88889231265056878 180868.47956919606076553, 528480.12932370661292225 180756.38422738478402607, 528315.31369558570440859 180703.26183484998182394, 528079.46642620186321437 180632.41520988091360778)</t>
-  </si>
-  <si>
     <t>LineString (525813.62879803299438208 181444.3455462628044188, 525938.4894992244662717 181490.10516775862197392, 525950.2033640209119767 181472.33594733368954621, 525943.13234854943584651 181373.34173073348938487, 525962.06789837975520641 181288.70267443344346248, 526084.9407700706506148 181347.92177145567256957, 526141.85119377286173403 181374.63645114144310355, 526247.90762806567363441 181264.37710280925966799, 526196.01242155989166349 181214.6880689833778888, 526166.16735107859130949 181192.64317541586933658, 526187.1327016269788146 181205.25580382536281832, 526289.24206442979630083 181085.57761354133253917, 526304.73383384314365685 181090.14411224401555955, 526312.97320597257930785 181086.63195823784917593, 526423.70250916026998311 181197.57224821968702599, 526423.40014027606230229 181210.76514542126096785, 526440.61190727609209716 181208.4950954697560519, 526481.37747424189001322 181247.68218424991937354, 526436.7998225896153599 181292.98168183141387999, 526364.50886605237610638 181370.49790682113962248, 526315.65099693823140115 181327.24125062092207372, 526174.19306422164663672 181474.26841948175569996, 526118.98830004595220089 181451.55415104021085426, 526093.47386830300092697 181427.99858194089028984, 526147.53385363647248596 181372.97566176933469251, 526117.64916966739110649 181356.75464216282125562, 525896.63604345871135592 181252.18492163851624355, 525804.47871884633786976 181202.92109834335860796, 525674.52415049879346043 181177.43981043208623305, 525808.02069279435090721 181198.8358115378941875, 525864.59372291236650199 181229.60359984767274, 525899.00071198993828148 181072.78713039786089212, 525914.79815168655477464 180998.59706019930308685, 526038.20014135900419205 181021.09393767311121337, 526034.23010415781755 181034.3273950106522534, 526110.653320282115601 181059.4709639519569464, 526164.81034232175443321 180824.94568032599636354, 526232.31997911655344069 180857.46556634301668964, 526385.03995015844702721 180939.3827475757279899, 526403.75872426724527031 180965.03631317696999758, 526518.00100311415735632 180845.93953079267521389, 526544.3462272291071713 180802.71689747890923172, 526415.88937359000556171 180762.15805877896491438, 526543.08072616113349795 180799.48524305276805535, 526566.20990454801358283 180735.24582871556049213, 526773.2086006454192102 180792.2867543384199962, 526781.81037810200359672 180804.0292009754339233, 526876.82089265179820359 180898.32528518006438389, 526893.50918447971343994 180930.32612565089948475, 526924.34248529304750264 180944.76673002715688199, 526972.18770328722894192 180987.68083861388731748, 526822.07183925563003868 181156.94281222127028741, 526922.36106670461595058 181052.43190333811799064, 527056.51731256174389273 181181.75928882521111518, 527072.0604500574991107 181194.33582109218696132, 527105.36620856204535812 181208.59860649338224903, 527134.84456199198029935 181207.65720116312149912, 527141.67895267263520509 181237.20603345840936527, 527126.8461934340884909 181257.45282692171167582, 527004.39505052170716226 181384.53058732440695167, 526985.91159781138412654 181369.18001979179098271, 526928.28958167461678386 181432.30053406039951369, 526997.63798668433446437 181498.45083301386330277, 526991.12956032424699515 181511.24325723896618001, 526678.53803907369729131 181414.39224837144138291, 526667.31783640081994236 181399.6772284725739155, 526656.64944697415921837 181395.44666025164769962, 526645.98105754749849439 181403.90779669350013137, 526619.08016179490368813 181431.82035006419755518, 526630.85217771399766207 181442.85661498832632788, 526625.70192074938677251 181459.04313687709509395, 526679.9176372914807871 181475.29189143585972488, 526706.84188712364993989 181479.03970802802359685, 526704.67241586744785309 181483.81254479169729166, 526684.71328031027223915 181478.02728810845292173, 526671.31848243589047343 181522.68559793970780447, 526666.90397646627388895 181521.94984694477170706, 526673.52573542075697333 181504.29182306613074616, 526671.31848243589047343 181502.8203210762294475, 526664.32884798396844417 181521.58197144727455452, 526672.42210892832372338 181534.0897383613337297, 526664.69672348140738904 181552.11563773744273931, 526615.76928231760393828 181537.7684933360433206, 526607.67602137324865907 181540.71149731581681408, 526667.6397274611517787 181562.3241827923047822, 526633.51603102358058095 181673.21107818573364057, 526634.14788983517792076 181721.54827727310475893, 526750.40991116955410689 181719.96863024411140941, 526763.6789462132146582 181717.44119499769294634, 527047.06762321561109275 181716.49340678029693663, 527075.50126973760779947 181704.80401876571704634, 527090.57778861722908914 181720.29356452525826171, 527188.46480982354842126 181748.64203353796619922, 527263.33384336996823549 181773.11378883954603225, 527341.77672236878424883 181800.06906386234913953, 527457.35124988225288689 181828.41753287505707704, 527478.70498486375436187 181813.3316481038054917, 527501.72297252365387976 181756.39241547140409239, 527552.19019862043205649 181634.29178817657520995, 527576.96563832846004516 181539.9116470152803231, 527502.86533335037529469 181515.28355731410556473, 527511.7228042078204453 181503.83365596178919077, 527545.64043651556130499 181469.26791603030869737, 527474.56463378143962473 181422.82020299739087932, 527381.22077847318723798 181367.63679676040192135, 527435.71565961930900812 181312.86944120863336138, 527464.59794662659987807 181334.12244485557312146, 527517.74514231248758733 181280.34209467822802253, 527383.21302771475166082 181171.51255586085608229, 527413.66733776684850454 181131.1336214438197203, 527429.41461164352949709 181120.02025737526128069, 527508.38860920432489365 181143.15408535901224241, 527552.0115922475233674 181044.38326500484254211, 527617.38904907600954175 181065.27134975808439776, 527665.90049312810879201 181080.65138910515815951, 527880.71712640451733023 181139.95635454953298904, 527892.84981061285361648 181124.42310436989646405, 527898.57802572846412659 181147.61365187869523652, 528147.61506407021079212 181224.24573191639501601, 528390.99835214088670909 181293.8688241028576158, 528368.25337566784583032 181399.05101017700508237, 528327.16320699045900255 181385.98296514025423676, 528308.22175984270870686 181356.13857025865581818, 528284.80718849156983197 181340.66114173838286661, 528256.63033144187647849 181343.0422845876601059, 528236.78747436462435871 181362.88514166491222568, 528124.47690330736804754 181327.56485606741625816, 528078.36375248804688454 181310.06427945720497519)</t>
   </si>
   <si>
-    <t>LineString (528078.36375248804688454 181310.06427945720497519, 528120.39353655825834721 181328.79462172722560354, 528099.23992964578792453 181396.49718135065631941, 528083.2094619075069204 181447.06752287576091476, 527892.05577444343362004 181391.53930473059881479, 527886.54702264338266104 181381.62355149036739022, 527894.36945019953418523 181395.8361311347107403, 528096.21011615579482168 181454.44925028792931698, 528174.43439171742647886 181477.365657776419539, 528210.57180352613795549 181486.17966065660584718, 528186.33329560561105609 181562.09026046219514683, 528058.53025384293869138 181521.54584721333230846, 528025.91844318632502109 181610.126576159207616, 528008.71294296334963292 181668.53094684361713007, 527974.16629928222391754 181658.69760866125579923, 527946.58959034748841077 181751.49542285426286981, 527954.90637558174785227 181756.52926654869224876, 528111.16470766742713749 181801.12569479394005612, 528175.52004705951549113 181808.29031149361981079, 528172.01824275031685829 181825.36160750081762671, 528149.81553756294306368 182021.61447876173770055, 528104.60850979876704514 182012.27041250278125517, 528152.75831904984079301 182029.34170851000817493, 528168.07871290249750018 181874.8245933678408619, 528216.66624769219197333 181878.76412321566022001, 528233.97450602473691106 181880.77550011838320643, 528312.01526012923568487 181886.28911337567842565, 528336.83830706239677966 181958.7224278392677661, 528364.07657583232503384 181967.85795997321838513, 528398.32810312346555293 181877.94770083410548978, 528435.48417966347187757 181756.45373819654923864, 528556.93269398633856326 181793.33950502122752368, 528601.07048073236364871 181658.00311254803091288, 528462.81105602439492941 181615.32684191930457018, 528543.19771087332628667 181342.55578955341479741, 528848.09397080901544541 181432.12983202037867159, 528821.39401584293227643 181512.22969691874459386, 528869.62619255587924272 181528.59418544638901949, 528825.70046019228175282 181657.78751592763001099, 528781.18706770276185125 181829.79148424055892974, 528840.64356546348426491 181663.36835393149522133, 528928.19383570738136768 181689.65520411299075931, 528953.17121293372474611 181619.02951678325189278, 528997.95823416719213128 181634.5327164409973193, 529113.40120173222385347 181668.62010940056643449, 529255.4526879689656198 181785.48692165815737098, 529207.81271354551427066 181851.48813622404122725, 529209.79771247983444482 181862.901880096324021, 529201.85771674255374819 181846.52563888826989569, 529049.81566479301545769 181789.52457975188735873, 528954.52870295522734523 181766.80601999314967543, 529040.88659724884200841 181487.92052047938341275, 529208.07499765011016279 181542.65362748788902536, 529285.99421999289188534 181467.49755145219387487, 529296.60062423895578831 181467.17206752439960837, 529335.06877524114679545 181403.05848252086434513, 529397.35054353030864149 181423.20846637911745347, 529313.08697466843295842 181608.2219545322295744, 529347.89149224187713116 181631.11966346204280853, 529360.003021250362508 181638.69174143215059303, 529446.90093042538501322 181699.64433337154332548, 529416.11189753527287394 181753.80004300863947719, 529422.43464536091778427 181758.47337835803045891, 529443.87700755218975246 181711.74002486409153789, 529454.04838448914233595 181691.12236891090287827, 529472.12319620803464204 181661.08931673903134651, 529548.27107219526078552 181551.40338706798502244, 529523.80478713079355657 181530.78573111479636282, 529435.81869453191757202 181616.70519618046819232, 529478.4459440337959677 181645.69480029397527687, 529548.02589098876342177 181547.71293349421466701, 529541.20248039334546775 181540.13136616605333984, 529645.94890438881702721 181356.4556775517121423, 529665.98890690342523158 181359.0756422930280678, 529673.67560427926946431 181405.95077004205086268, 529767.56312223034910858 181439.16828370295115747, 529790.27442454162519425 181451.8257157189946156, 530012.95905668172053993 181535.92978279336239211, 530061.70118646346963942 181447.04707554430933669, 530133.46244322671554983 181459.83858795103151351, 530142.41057766624726355 181451.52960597147466615, 530121.31854648748412728 181417.01537313338485546, 530163.50260884512681514 181331.36894349814974703, 530208.22465636255219579 181366.63554168166592717, 530234.10646259249188006 181373.52784813527250662, 530191.7715905592776835 181481.05309050341020338, 530283.50257032876834273 181549.71721571101807058, 530311.93380967248231173 181491.24542158891563304, 530426.19520552584435791 181514.31227615085663274, 530446.77953103894833475 181528.09228405426256359, 530452.47980525041930377 181521.3478456501616165, 530415.45271119684912264 181496.96883923502173275, 530453.46287902258336544 181405.91857528948457912, 530484.62340791756287217 181368.68222978565609083, 530453.29358863539528102 181346.97811556659871712, 530395.29544163832906634 181277.22392895829398185, 530367.43655410828068852 181235.61759427358629182, 530392.94670032931026071 181209.0107060651644133, 530410.88688604242634028 181193.34473685521516018, 530334.12094446760602295 181103.43394227110547945, 530405.62894483865238726 181057.16405967809259892, 530486.81822421168908477 180959.05754400324076414, 530519.31806703854817897 180916.11851573517196812, 530582.29576928459573537 180878.9198528709821403, 530582.29576928459573537 180878.9198528709821403)</t>
-  </si>
-  <si>
-    <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529270.770087662152946 178758.30559268582146615, 529304.71750739659182727 178689.86743865112657659, 529337.70783226401545107 178657.27980173568357714, 529305.00792290433309972 178707.29236911991029046, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529684.84245063865091652 178849.14101684212801047, 529657.52491406002081931 178773.00064893162925728, 529696.44831980823073536 178755.84746999081107788, 529755.07401005295105278 178759.51157563112792559, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529980.5303832235513255 178971.74485745528363623, 529876.73172444535885006 178973.90732951316749677, 529877.37348464445676655 178984.43081074606743641, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530137.16457231086678803 179220.90265564562287182, 530137.2566814114106819 179287.56575694994535297, 530164.29013196483720094 179289.33844223213964142, 530181.6477391414809972 179297.81860453309491277, 530196.47771490353625268 179309.6297804182395339, 530192.14217540447134525 179370.16058188583701849, 530171.13148398592602462 179464.20843871153192595, 530148.2424291695933789 179574.15693386044586077, 530133.06942986708600074 179585.28380001557525247, 530072.88319930084981024 179599.95103267458034679, 530076.42356580472551286 179662.66609645792050287, 530120.93103042512666434 179669.24106282231514342, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530871.2405794725054875 180748.77793378444039263, 530884.09205942158587277 180795.04326160132768564, 530994.61478698416613042 180838.09571943094488233, 530982.23648845416028053 180885.78941204195143655, 531002.32567495363764465 180840.66601542077842169, 531087.78801661543548107 180857.37293935465277173, 531104.77522879175376147 180851.00402391061652452, 531115.93421733961440623 180802.8298538378730882, 531377.42735681601334363 180810.11179436542443, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531465.94281411881092936 180989.74318283077445813, 531389.47650842147413641 180987.01224334159633145, 531387.55785732087679207 181129.37252376566175371, 531386.90621243161149323 181168.05746712500695139, 531290.5201128131011501 181159.06143116063321941, 531142.08551940054167062 181108.94065935898106545, 531043.74918007606174797 181071.66004718522890471, 530997.40789101168047637 181015.41131011385004967, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530843.16896641999483109 180955.15571484464453533, 530745.85037270176690072 180904.40675493027083576, 530583.45370097586419433 180805.89406803768360987, 530578.08028169081080705 180813.05862708439235575, 530607.33556446491274983 180828.58183835234376602, 530580.2603085950249806 180875.74680006815469824, 530580.2603085950249806 180875.74680006815469824)</t>
-  </si>
-  <si>
-    <t>LineString (534494.76712749910075217 180197.82926488673547283, 534477.08958587038796395 180204.9261592309048865, 534466.10449469194281846 180201.48237478407099843, 534446.35375012725125998 180105.42193530994700268, 534275.77913797693327069 180170.50961626204662025, 534224.15787377348169684 180196.54468864286900498, 534203.5093680921709165 180212.25550818303599954, 534185.55414576060138643 180210.4599859498848673, 534171.14064759924076498 180237.33092047309037298, 534155.10926930524874479 180232.7692223628400825, 534110.10282780381385237 180227.94574123568600044, 534059.63022310636006296 180244.41244702640688047, 534045.56321658962406218 180253.93444574531167746, 534018.52404629567172378 180285.19719793670810759, 534005.14660858130082488 180295.44406237191287801, 533989.44804280833341181 180338.41282897180644795, 534003.21356487192679197 180354.3808345656725578, 534155.73554933757986873 180422.10720311899785884, 534135.36257668328471482 180462.85314842750085518, 534160.69113728043157607 180481.57425843409146182, 534211.8988793573807925 180382.46249957560212351, 534228.96812671632505953 180379.70939516284852289, 534265.3091049644863233 180416.35643082388560288, 534271.73921295220497996 180462.74348229306633584, 534252.4929513584356755 180455.64950213933479972, 534269.62446292664390057 180472.076978985540336, 534255.40823154035024345 180562.17560434373444878, 534234.92044681450352073 180597.79788426094455644, 534256.13046408852096647 180604.31816759763751179, 534251.89312430669087917 180626.73219362733652815, 534379.78553101746365428 180633.41155169066041708, 534352.34416242560837418 180636.5838860665098764, 534344.23650324332993478 180704.43507658550515771, 534297.84553046221844852 180708.00611733732512221, 534240.14221260114572942 180695.98651926324237138, 534189.34860979067161679 180672.75587819167412817, 534160.54824850801378489 180757.54946950945304707, 534160.5841055567143485 180757.22253176767844707, 534127.8658005315810442 180858.10397226159693673, 534111.99208847992122173 180939.00866548559861258, 534085.5094500295817852 180985.32051877162302844, 534070.93534209730569273 180988.37091345511726104, 534075.68040049390401691 180998.87782847607741132, 534054.99797940440475941 181035.08444935575244017, 534068.56281289900653064 181030.73750628152629361, 534096.52225887367967516 180994.37437144466093741, 534118.50570094562135637 180998.44537923578172922, 534120.13410406210459769 181012.28680572554003447, 534190.96963962737936527 181035.08444935575244017, 534233.56329029169864953 181041.4142344745923765, 534230.7365170813864097 181061.51134635950438678, 534425.65412626438774168 181087.91946370297227986, 534428.68984542321413755 181124.52763081435114145, 534418.41545121860690415 181314.94640340618207119, 534244.43570935411844403 181318.37120147436507978, 534082.24461821641307324 181331.92378598402137868, 534008.65777000458911061 181337.21434369860799052, 534003.03775836550630629 181356.73341751954285428, 533970.61429565714206547 181390.91446260787779465, 533908.72647818853147328 181354.13541679794434458, 533820.00587128894403577 181301.66338870135950856, 533762.7596401305636391 181265.19378197882906534, 533763.82057414436712861 181254.40761950571322814, 533775.00675160356331617 181229.54225989809492603, 533765.23515282932203263 181236.37174127201433294, 533750.68025846313685179 181246.3013364469516091, 533738.92612418869975954 181260.82114937415462919, 533558.01058455463498831 181157.44207860867027193, 533549.5142814606660977 181141.84867783010122366, 533537.31101294630207121 181133.86961764763691463, 533483.72784082207363099 181114.99530462495749816, 533375.88864138023927808 181117.98406295705353841, 533381.80025942670181394 181168.40668747131712735, 533323.37956343777477741 181201.44220008412958123, 533277.55680660111829638 181222.13016911473823711, 533325.81375910399947315 181204.22413798831985332, 533380.40929047460667789 181174.66604775583255105, 533399.53511356632225215 181212.91769393908907659, 533422.13835903815925121 181229.95706360254553147, 533476.03840593271888793 181291.15969749572104774, 533522.51176960719749331 181254.94408223693608306, 533527.5245621653739363 181246.81990119433612563, 533527.00599741796031594 181236.96717099371016957, 533512.83189432229846716 181222.62021298229228705, 533521.10348163370508701 181215.37559709040215239, 533538.7190823903074488 181185.9681870742351748, 533548.10621201666072011 181170.94877967197680846, 533562.65626293770037591 181116.50342783879023045, 533565.78408725361805409 181068.52103992408956401, 533568.11593338451348245 181052.2709871992119588, 533565.98876765870954841 181030.01686012774007395, 533550.6638780701905489 180995.96154993091477081, 533517.88564200571272522 180943.17581912584137172, 533527.8685909277992323 180932.10417117548058741, 533519.96954229823313653 180930.1110331111412961, 533540.88975644903257489 180852.93240523023996502, 533549.08821875147987157 180816.53405966371065006, 533554.74233068409375846 180784.02291605086065829, 533498.69594615150708705 180775.96580654679564759, 533473.25244245456997305 180751.37041963971569203, 533450.91870032052975148 180721.12092079993453808, 533451.20140591717790812 180708.11646335478872061, 533482.01631595019716769 180701.33152903561131097, 533556.93329905800055712 180708.68187454805593006, 533574.10766405356116593 180706.42022977498709224, 533632.91042815323453397 180723.09985997635521926, 533664.85616057284642011 180736.10431742150103673, 533657.22310946369543672 180723.94797676627058536, 533653.26523111085407436 180708.11646335478872061, 533628.66984420374501497 180717.16304244706407189, 533572.27007767534814775 180700.55408864485798404, 533556.72126986051443964 180706.77361177079728805, 533481.23887555941473693 180699.42326625832356513, 533449.2931431399192661 180706.77361177079728805, 533440.52926964417565614 180711.01419572028680705, 533410.70382919942494482 180714.40666287989006378, 533368.01528410776518285 180716.38560205633984879, 533344.26801399048417807 180714.68936847653822042, 533317.41098231042269617 180704.51196699772845022, 533298.32835453760344535 180707.05631736741634086, 533274.0156732271425426 180725.43218114858609624, 533214.36479233752470464 180758.22603035805514082, 533150.04926910332869738 180796.6033151010342408, 533131.95611091877799481 180803.10554382362170145, 533112.94415954523719847 180814.13106209231773391, 533032.09035890805535018 180821.19870200814330019, 533006.17641249333973974 180714.80543799756560475, 532992.55450278345961124 180708.59827885474078357, 533019.41655259137041867 180701.98867611197056249, 533047.67523066280409694 180678.44941610301611945, 533062.18958536896388978 180672.97919573029503226, 533115.1629428390879184 180663.2515109057421796, 533114.02687698940280825 180650.64306823158403859, 532992.54919304675422609 180668.21878358686808497, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531644.05815143184736371 180909.64867640155716799, 531643.0989445325685665 180988.84512792871100828, 531635.99518679245375097 181107.77244371830602176, 531600.40284548385534436 181102.74764259238145314, 531578.20997384435031563 181106.09751000965479761, 531580.30364098015706986 181147.13338587139151059, 531592.02817694062832743 181174.35105863682110794, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531133.39463505509775132 181279.42110962877632119, 531076.29551051347516477 181260.61487964406842366, 531131.04354967980179936 181113.15854730040882714, 531036.5176723989425227 181074.07573265538667329, 530995.61705242155585438 181020.45047535176854581, 530934.72057378862518817 181004.99913002699031495, 530807.47420052578672767 181052.26206866747816093, 530678.41002193070016801 181020.45047535176854581, 530547.98248933651484549 181092.25378597865346819, 530470.12182414066046476 180975.54759959221701138, 530510.45278707984834909 180923.94229928601998836, 530582.29576928459573537 180878.9198528709821403)</t>
-  </si>
-  <si>
     <t>LineString (534150.19790721382014453 181658.82599177915835753, 534188.4078070386312902 181677.32008704933105037, 534295.39330477884504944 181748.67556176203652285, 534458.90044428419787437 181864.5233750130282715, 534483.31045287544839084 181802.6053044400177896, 534553.56364833330735564 181831.18287547372165136, 534581.15801056486088783 181763.96769404891529121, 534626.35794776398688555 181776.75086198319331743, 534797.74285306176170707 181843.92396450418164022, 535287.18371127475984395 182016.74360227302531712, 535232.17579299991484731 182019.72173797580762766, 535207.64996956521645188 182091.8977326549065765, 535091.50267715682275593 182197.53395787699264474, 535042.14986233541276306 182197.81197882973356172, 535028.73974128148984164 182224.41747152400785126, 535036.47778976988047361 182425.60673222184414044, 535003.97798611875623465 182543.22506924520712346, 534994.72957604483235627 182519.28562053974019364, 534911.66025196714326739 182500.88847403886029497, 534924.30123606591951102 182412.06298755903844722, 534860.19338813633657992 182410.70859640560229309, 534794.73114905343391001 182370.9797892379865516, 534781.76486209139693528 182416.81556864531012252, 534775.89833489886950701 182439.80761461149086244, 534733.01554672734346241 182433.42887881567003205, 534738.45721302484162152 182649.24169926377362572, 534730.12317419145256281 182691.18073339309194125, 534802.97880399296991527 182703.14411171845858917, 534809.85073587717488408 182706.20718782997573726, 534878.44964922510553151 182728.92067172401584685, 534874.50866161868907511 182753.88025989828747697, 534886.18912552238907665 182730.73464611344388686, 534960.41568882705178112 182744.27007824546308257, 534951.68315196770709008 182818.06001470709452406, 534939.02097352163400501 182880.93428009451599792, 534963.03544988483190536 182888.35693642497062683, 534944.24135854840278625 182963.83128923355252482, 534899.9714611767558381 182951.04220777060254477, 534891.78288685239385813 182949.51981309754773974, 534883.95649775443598628 182942.20384067995473742, 534838.18913542130030692 182939.14134059820207767, 534833.59538529859855771 182956.15522994138882495, 534728.87489639106206596 182935.52588911273051053, 534732.14552768925204873 182871.83970818307716399, 534649.52294641232583672 182862.46408719307510182, 534628.55294301128014922 182955.48487151082372293, 534493.18888259516097605 182880.20793622478959151, 534302.84577480040024966 182816.22254123163293116, 534284.02654097892809659 182859.77562521857907996, 534295.78345685871317983 182819.58610184054123238, 534296.67217820382211357 182816.26452868265914731, 534176.80159754795022309 182772.97793011250905693, 534076.9094470014097169 182756.3292383547523059, 534124.19173159345518798 182555.3795288386172615, 534016.13174477114807814 182513.80254928936483338, 534017.00426228798460215 182506.70794914639554918, 534125.32640601880848408 182535.96195105163496919, 534168.1666928093181923 182311.53897498786682263, 534269.44489237654488534 182341.85239916807040572, 534307.17684069508686662 182340.19748915411764756, 534331.33852689899504185 182328.77861005775048397, 534411.72237405984196812 182320.70818523829802871, 534383.0651157310931012 182118.86140918426099233, 534448.45756019873078912 182114.30714349748450331, 534385.02715628384612501 182112.14474336401326582, 534401.94695855455938727 182029.46270526901935227, 534197.29156851791776717 182037.41563493365538307, 534198.35195913992356509 182073.99911139099276625, 534075.34664699353743345 182084.07282229952397756, 533877.15337622561492026 182102.89926247851690277, 533881.96351368981413543 182166.63358387906919234, 533889.17871988611295819 182271.25407372525660321, 533665.51229002187028527 182282.44098327826941386, 533645.62510754854883999 182286.76606867561349645, 533618.567245963960886 182470.45983984900522046, 533632.33677199063822627 182516.43228964801528491, 533660.54209143260959536 182517.76482442481210455, 533676.7545978834386915 182542.63880692477687262, 533673.86743920051958412 182563.68175194147625007, 533708.19324949278961867 182577.78883584373397753, 533744.78147669287864119 182600.35388822320965119, 533719.61320557200815529 182691.0010928868141491, 533701.35989006015006453 182685.35125713315210305, 533696.14465705677866936 182787.91750619950471446, 533602.27046299609355628 182776.61783469218062237, 533604.152414740761742 182785.81231147074140608, 533629.6504362637642771 182783.13687594639486633, 533887.88424544327426702 182820.57441884058061987, 533896.32165873644407839 182796.25481581923668273, 533994.96494650165550411 182805.68486597036826424, 533958.97602709801867604 182864.08820365733117796, 534162.58751859271433204 183101.90006286397692747, 534151.45251515158452094 183143.85516511532478034, 534224.62539490743074566 183157.37624072236940265, 534242.12325745774433017 183214.64197270525619388, 534235.76864853664301336 183146.50009479920845479, 534422.34790956706274301 183189.51548639123211615, 534554.33143426640890539 183222.22614488427643664, 534560.58397974201943725 183245.53360263974172994, 534585.38740086904726923 183236.13562777847982943, 534839.23427885014098138 183312.35428325369139202, 534883.15689386974554509 183313.64612487191334367, 535342.64082826022058725 183415.18309037722065113, 535377.02339462761301547 183414.03198869159677997, 535729.61131596809718758 183230.43964716198388487, 535597.45816457970067859 183171.78773763249046169, 535493.01945444208104163 183163.06486600026255473)</t>
   </si>
   <si>
     <t>LineString (533064.46897248667664826 183210.39921171619789675, 533076.87953593488782644 183044.4026491524418816, 533070.12536461430136114 182985.15014620366855524, 533045.871749417623505 182926.97217051047482528, 533058.76607648422941566 182947.23468447223422118, 533080.25662159512285143 182941.70854430084000342, 533168.98187212459743023 182947.23468447223422118, 533189.95457557367626578 182949.67927450055140071, 533190.07185356423724443 182932.90852184614050202, 533256.30459875019732863 182938.06875343210413121, 533270.02612364920787513 182934.78496969558182172, 533273.77901934809051454 182943.58081898986711167, 533263.22400019492488354 182991.66479513191734441, 533262.98944421380292624 183071.82430170045699924, 533364.55218406510539353 183067.83685002036509104, 533378.15643097355496138 183087.01180148191633634, 533393.87168171268422157 183066.6054311191837769, 533558.68779758946038783 183057.05841860847431235, 533558.68779758946038783 183104.32901793727069162, 533561.19678307115100324 183054.36769029102288187, 533513.35373550979420543 183055.70408826760831289, 533502.36358368746004999 182956.620714706776198, 533466.48049678211100399 182839.1161635409516748, 533430.95062767004128546 182843.6842895696463529, 533423.99112124263774604 182625.95366138272220269, 533418.28455447813030332 182579.59432971687056124, 533451.54715791763737798 182502.91214257484534755, 533464.75749999412801117 182467.34583698387723416, 533337.93821605830453336 182452.71284268359886482, 533337.78902459214441478 182368.47306541417492554, 533484.07380397082306445 182386.01211906579555944, 533490.69280884729232639 182350.24248738010646775, 533472.43150111590512097 182205.93442166002932936, 533583.10897760698571801 182063.8076075866993051, 533609.71995556121692061 182037.80142458603950217, 533610.24870057171210647 182016.33477542886976153, 533584.88456065976060927 182052.1574076684191823, 533535.1852201041765511 182057.86061068301205523, 533518.26287293271161616 181970.58373815898085013, 533484.19519956270232797 181975.12609460830572061, 533475.45617014251183718 181918.25283637543907389, 533396.87044996197801083 181921.33462932368274778, 533362.97072753123939037 181745.67243127315305173, 533383.00238169485237449 181921.33462932368274778, 533385.57218187116086483 181991.15361790888709947, 533400.75257761764805764 182035.04779862469877116, 533331.49939815502148122 182048.89843451723572798, 533234.54494690720457584 182081.48816602909937501, 533073.65851616964209825 182090.02078689282643609, 533085.33284421800635755 182215.89180190846673213, 533090.14230673655401915 182227.52340018114773557, 533155.84606537700165063 182220.5149992594961077, 533149.99286592833232135 182319.05148053923039697, 533156.54641778930090368 182323.96664443501504138, 533151.53487813088577241 182385.64713253875379451, 532980.57106288510840386 182377.64146055665332824, 532778.65285523270722479 182361.72131757129682228, 532755.6968509522266686 182366.02556837382144295, 532572.76619184156879783 182348.80856516343192197, 532552.88329151901416481 182350.97523911585449241, 532244.88995379093103111 182215.8126952207821887, 532262.60291642148513347 182168.39960261050146073, 532295.2441410442115739 182069.11680604351568036, 532305.37037298001814634 182028.61187830017297529, 532288.80017526680603623 182059.91114064730936661, 532220.90932479011826217 182025.71317250368883833, 532158.87452575471252203 182016.26025074589415453, 532107.4742636966984719 182011.53378986698226072, 532104.52022564737126231 181924.09426360743236728, 532086.79599735140800476 181928.63609710824675858, 532087.97761257109232247 181975.30989828731981106, 532092.70407344994600862 182022.86991088121430948, 532079.11549842311069369 182099.67490016322699375, 532046.62107988074421883 182161.70969919872004539, 532014.12666133837774396 182194.20411774111562409, 531972.17932103818748146 182188.88684925236157142, 531913.68936766183469445 182151.07516222121194005, 531908.60801759164314717 182163.45413967911736108, 531953.17571160080842674 182184.55127293791156262, 531987.59041022916790098 182199.51705184334423393, 532004.99554516770876944 182204.79133515805006027, 531983.10726941167376935 182243.55731752107385546, 531968.33927613054402173 182281.13658613828010857, 531944.07757288287393749 182371.59054498534533195, 531937.94260709825903177 182398.64015493713668548, 532011.93064753827638924 182423.87109960327506997, 532068.52979368122760206 182445.01053972897352651, 532086.94156411325093359 182440.23711776512209326, 532158.88385228300467134 182467.76953373529249802, 532152.40563676052261144 182502.8882810408831574, 532121.55289627402089536 182643.03526213087025099, 532075.0642949640750885 182863.25497264647856355, 532069.45360170258209109 182883.29316286626271904, 532082.41561907751020044 182888.00662372991791926, 532062.29523281508591026 182889.32744172037928365, 532066.95640396035742015 182915.35964283399516717, 531884.43796249642036855 182981.6259192216093652, 531767.99498561583459377 183028.33115369590814225, 531728.68198287941049784 182918.06297528900904581, 531725.87449492723681033 182910.13609254563925788, 531809.84689899394288659 182817.65547132669598795, 531837.40510237636044621 182760.1590255610353779, 531828.71498920442536473 182755.52429853595094755, 531814.23146725108381361 182767.69045697676483542, 531569.74961667892057449 182693.53482457570498809, 531563.95620789751410484 182754.94495765783358365, 531565.11488965386524796 182687.74141579438582994, 531616.09688692959025502 182577.66664894908899441, 531609.14479639194905758 182564.92114963015774265, 531628.84238624852150679 182534.7954239672399126, 531625.36634097970090806 182476.86133615393191576, 531747.02792538760695606 182513.93915235446183942, 531632.89777239540126175 182463.5364959568833001, 531625.94568185787647963 182421.82395273129804991, 531681.5624061586568132 182312.90786764226504602, 531703.57735952769871801 182270.0366426604159642, 531683.80043675052002072 182250.5687343017780222, 531595.88583471847232431 182183.28084469723398797, 531580.06645999138709158 182164.89640980056719854, 531555.2433897431474179 182143.27140381743083708, 531526.61310013174079359 182118.90519989278982393, 531515.64830836560577154 182136.41840896362555213, 531466.00216786901000887 182107.48354180311434902, 531411.63507536228280514 182149.7436767349136062, 531394.57873261498752981 182161.31762359911226667, 531354.5267849137308076 182200.07511671676184051, 531330.16058098908979446 182208.29871054133400321, 531333.2063564796699211 182193.06983308843336999, 531354.79575750709045678 182159.67430333484662697, 531334.90127811359707266 182155.04768022007192485, 531291.87368314596824348 182150.88371941674267873, 531265.96459370316006243 182135.15320082646212541, 531248.34037534287199378 182041.19192783226026222, 531270.21593675261829048 182040.14943936991039664, 531272.14963821833953261 182027.69603843480581418, 531291.66027387382928282 182000.88878809078596532, 531269.86458137142471969 182026.02942997106583789, 531260.89388385554775596 182036.66077076771762222, 531156.26423942053224891 182028.00196012531523593, 530992.96919284970499575 181971.66516905839671381, 530937.44887701561674476 182060.66096943948650733, 530881.5203235651133582 182170.88512587477453053, 530784.23736255615949631 182302.13991453754715621)</t>
+  </si>
+  <si>
+    <t>v4 20230708</t>
+  </si>
+  <si>
+    <t>LineString (528078.36375248804688454 181310.06427945720497519, 528120.39353655825834721 181328.79462172722560354, 528099.23992964578792453 181396.49718135065631941, 528083.2094619075069204 181447.06752287576091476, 527892.05577444343362004 181391.53930473059881479, 527886.54702264338266104 181381.62355149036739022, 527894.36945019953418523 181395.8361311347107403, 528096.21011615579482168 181454.44925028792931698, 528174.43439171742647886 181477.365657776419539, 528210.57180352613795549 181486.17966065660584718, 528186.33329560561105609 181562.09026046219514683, 528058.53025384293869138 181521.54584721333230846, 528025.91844318632502109 181610.126576159207616, 528008.71294296334963292 181668.53094684361713007, 527974.16629928222391754 181658.69760866125579923, 527946.58959034748841077 181751.49542285426286981, 527954.90637558174785227 181756.52926654869224876, 528111.16470766742713749 181801.12569479394005612, 528175.52004705951549113 181808.29031149361981079, 528172.01824275031685829 181825.36160750081762671, 528149.81553756294306368 182021.61447876173770055, 528104.60850979876704514 182012.27041250278125517, 528152.75831904984079301 182029.34170851000817493, 528168.07871290249750018 181874.8245933678408619, 528216.66624769219197333 181878.76412321566022001, 528233.97450602473691106 181880.77550011838320643, 528312.01526012923568487 181886.28911337567842565, 528336.83830706239677966 181958.7224278392677661, 528364.07657583232503384 181967.85795997321838513, 528398.32810312346555293 181877.94770083410548978, 528435.48417966347187757 181756.45373819654923864, 528556.93269398633856326 181793.33950502122752368, 528601.07048073236364871 181658.00311254803091288, 528462.81105602439492941 181615.32684191930457018, 528543.19771087332628667 181342.55578955341479741, 528848.09397080901544541 181432.12983202037867159, 528821.39401584293227643 181512.22969691874459386, 528869.62619255587924272 181528.59418544638901949, 528825.70046019228175282 181657.78751592763001099, 528781.18706770276185125 181829.79148424055892974, 528840.64356546348426491 181663.36835393149522133, 528928.19383570738136768 181689.65520411299075931, 528953.17121293372474611 181619.02951678325189278, 528997.95823416719213128 181634.5327164409973193, 529113.40120173222385347 181668.62010940056643449, 529255.4526879689656198 181785.48692165815737098, 529207.81271354551427066 181851.48813622404122725, 529209.79771247983444482 181862.901880096324021, 529201.85771674255374819 181846.52563888826989569, 529049.81566479301545769 181789.52457975188735873, 528954.52870295522734523 181766.80601999314967543, 529040.88659724884200841 181487.92052047938341275, 529208.07499765011016279 181542.65362748788902536, 529285.99421999289188534 181467.49755145219387487, 529296.60062423895578831 181467.17206752439960837, 529335.06877524114679545 181403.05848252086434513, 529397.35054353030864149 181423.20846637911745347, 529313.08697466843295842 181608.2219545322295744, 529347.89149224187713116 181631.11966346204280853, 529360.003021250362508 181638.69174143215059303, 529446.90093042538501322 181699.64433337154332548, 529416.11189753527287394 181753.80004300863947719, 529422.43464536091778427 181758.47337835803045891, 529443.87700755218975246 181711.74002486409153789, 529454.04838448914233595 181691.12236891090287827, 529472.12319620803464204 181661.08931673903134651, 529548.27107219526078552 181551.40338706798502244, 529523.80478713079355657 181530.78573111479636282, 529435.81869453191757202 181616.70519618046819232, 529478.4459440337959677 181645.69480029397527687, 529548.02589098876342177 181547.71293349421466701, 529541.20248039334546775 181540.13136616605333984, 529645.94890438881702721 181356.4556775517121423, 529665.98890690342523158 181359.0756422930280678, 529673.67560427926946431 181405.95077004205086268, 529767.56312223034910858 181439.16828370295115747, 529790.27442454162519425 181451.8257157189946156, 530012.95905668172053993 181535.92978279336239211, 530061.70118646346963942 181447.04707554430933669, 530133.46244322671554983 181459.83858795103151351, 530142.41057766624726355 181451.52960597147466615, 530121.31854648748412728 181417.01537313338485546, 530163.50260884512681514 181331.36894349814974703, 530208.22465636255219579 181366.63554168166592717, 530234.10646259249188006 181373.52784813527250662, 530191.7715905592776835 181481.05309050341020338, 530283.50257032876834273 181549.71721571101807058, 530311.93380967248231173 181491.24542158891563304, 530426.19520552584435791 181514.31227615085663274, 530446.77953103894833475 181528.09228405426256359, 530452.47980525041930377 181521.3478456501616165, 530415.45271119684912264 181496.96883923502173275, 530453.46287902258336544 181405.91857528948457912, 530484.62340791756287217 181368.68222978565609083, 530453.29358863539528102 181346.97811556659871712, 530395.29544163832906634 181277.22392895829398185, 530367.43655410828068852 181235.61759427358629182, 530392.94670032931026071 181209.0107060651644133, 530410.88688604242634028 181193.34473685521516018, 530334.12094446760602295 181103.43394227110547945, 530405.62894483865238726 181057.16405967809259892, 530486.81822421168908477 180959.05754400324076414, 530511.12097854469902813 180924.78276975522749126, 530505.35225721553433686 180900.45491703250445426, 530535.11384993349201977 180908.30573759670369327, 530582.29576928459573537 180878.9198528709821403, 530582.29576928459573537 180878.9198528709821403)</t>
+  </si>
+  <si>
+    <t>LineString (530784.23736255615949631 182302.13991453754715621, 530778.6444442254723981 182309.68591545993695036, 530773.74559282837435603 182337.44607337698107585, 530858.50592793908435851 182423.17597282669157721, 530936.88755029300227761 182449.3031802780169528, 531037.31400393415242434 182542.38135682337451726, 531094.36521082976832986 182594.22753410961013287, 531155.37121963454410434 182521.76535719376988709, 531166.80187289451714605 182513.19236724881920964, 531203.95149598934222013 182472.57272441431996413, 531259.88004943984560668 182529.52187190589029342, 531326.62689972575753927 182604.63759332848712802, 531370.30832468345761299 182662.60733486112440005, 531384.59664125845301896 182683.83569091532262973, 531369.90008706704247743 182687.50982946317526512, 531339.69050345139112324 182687.10159184673102573, 531257.94092076190281659 182652.80963206687010825, 531233.85490139271132648 182679.95743355926242657, 531204.76797122228890657 182711.18761121592251584, 531182.72313993528950959 182813.24701532270410098, 531203.13502075662836432 182831.20947044549393468, 531268.45303938491269946 182871.21675685534137301, 531362.55180997133720666 182909.59109279947006144, 531365.40947328635957092 182920.61350844299886376, 531354.79529525921680033 182956.13018107216339558, 531444.90684366086497903 182988.57858534331899136, 531474.10273866006173193 182998.58689318058895878, 531486.5355991879478097 183012.4143484897504095, 531547.55104103893972933 183034.71440845559118316, 531569.85110100475139916 183061.97003730272990651, 531517.81762775115203112 183110.59655695044784807, 531527.72876551374793053 183131.65772469594958238, 531497.95239027438219637 183140.93648922778083943, 531508.4095920140389353 183177.7640257888706401, 531495.22442460327874869 183139.57250639220001176, 531524.09539462334942073 183130.25195701562915929, 531519.54878517135512084 183120.02208574867108837, 531516.59348902758210897 183111.38352778987609781, 531448.32344150589779019 183136.55978571731247939, 531241.26357583678327501 183121.43743597742286511, 531197.64141312555875629 183108.64160158214508556, 530715.12526052596513182 183043.21945667950785719, 530703.01725020399317145 183063.42695543030276895, 530695.13352120853960514 183041.84071603690972552, 530546.28326243243645877 183024.95802384099806659, 530541.22589214832987636 183004.5417986634420231, 530703.18488589045591652 182946.11745994322700426, 530775.51721857010852545 182908.57789488162961788, 530786.04660877038259059 182895.30170723787159659, 530795.49963942251633853 182875.6843990063352976, 530804.3135183157864958 182802.06196081181406043, 530806.59301448101177812 182793.73684438230702654, 530819.8735573566518724 182794.33149555584532209, 530807.31673856556881219 182782.83954266682849266, 530812.03824553836602718 182733.95805871355696581, 530761.76808306365273893 182714.23882370966020972, 530770.16958811797667295 182659.52488996647298336, 530712.95603303634561598 182638.97244784975191578, 530630.19079316093120724 182601.20039206769433804, 530615.74853653833270073 182603.42227770193130709, 530555.75762441393453628 182723.95957335943239741, 530539.09348215709906071 182717.29391645672149025, 530547.14781758119352162 182730.62523026211420074, 530461.60522066289559007 182906.15419536712579429, 530437.90885532670654356 182917.93718825542600825, 530382.0339413866167888 182876.71421071342774667, 530325.26406243664678186 182961.75723386157187633, 530268.29162278701551259 182922.72056224985863082, 530249.18178586428985 182908.73221319253207184, 530252.98490572301670909 182894.20538857823703438, 530184.08185019285883754 182852.74914162818458863, 530085.83308541483711451 182787.51840435751364566, 530111.18260209145955741 182744.29519918368896469, 529999.02136356220580637 182666.39424455061089247, 529961.66046464198734611 182715.15181299234973267, 529988.72742143063805997 182735.23374867427628487, 529986.10803851566743106 182740.763557050464442, 529932.80478152283467352 182814.59110673272516578, 529984.94386833114549518 182734.94270612817490473, 529957.00378390413243324 182716.02494063068297692, 530013.09155612858012319 182629.12904521985910833, 530018.17775851185433567 182621.49974164497689344, 530100.32880480831954628 182494.38274551162612624, 530104.0113532249815762 182482.84132467227755114, 530220.50368910923134536 182556.47051627180189826, 530255.09743770561181009 182478.63458192982943729, 530272.39431200386025012 182483.35191128388396464, 530279.47030603489838541 182470.7723663397191558, 530137.95042541308794171 182415.73685720900539309, 530133.8373461066512391 182413.51172491264878772, 530186.21162480069324374 182272.1011724385607522, 530075.7495097367791459 182226.86884083910263143, 530075.1733111577341333 182226.46204725949792191, 530187.16388441331218928 182265.91148495653760619, 530233.22869966924190521 182154.23642371431924403, 530357.8921046924078837 182201.72724467553780414, 530348.98757576220668852 182228.44083146619959734, 530358.86895656702108681 182231.0766534095746465, 530394.74696868821047246 182125.29837629428948276, 530508.99968287569936365 182165.49652313266415149, 530513.72136097133625299 182167.0985210579528939, 530567.86575565708335489 182188.16529536261805333, 530573.45622016047127545 182150.89553200689260848, 530664.76714038196951151 181926.34520778860314749, 530694.76100652059540153 181850.76066511913086288, 530759.06664636044297367 181869.87285391447949223, 530674.73822676041163504 181825.22436629422008991, 530573.75377231650054455 181777.63399121144902892, 530599.29007114132400602 181730.04361612870707177, 530646.88044622412417084 181748.21467864664737135, 530657.97477119497489184 181732.12790743884397671, 530724.74751764547545463 181760.6236275052651763, 530741.12779784575104713 181707.06197263259673491, 530773.19373494503088295 181600.7954151411249768, 530782.75100370426662266 181575.85406711159157567, 530688.89235894195735455 181552.28991476428927854, 530627.95015930733643472 181539.24596229381859303, 530599.01706093887332827 181486.621268884598976, 530600.06536160444375128 181482.63772635560599156, 530608.87108719476964325 181476.34792236247449182, 530639.82865497504826635 181423.25654537187074311, 530713.75870660948567092 181269.28719607146922499, 530693.84197932516690344 181263.16111494251526892, 530645.94210892508272082 181237.73285941511858255, 530707.03671619179658592 181120.0358954158728011, 530733.0917692908551544 181051.75368729417095892, 530735.53599696443416178 181033.12102656494244002, 530692.8715660268208012 181009.95126327298930846, 530547.98248933651484549 181092.25378597865346819, 530472.93963134801015258 180978.161691593733849, 530509.50304127030540258 180927.1624389510252513, 530505.35225721553433686 180900.45491703250445426, 530541.06604016083292663 180904.23205514161963947, 530579.45680101704783738 180882.17122962352004834)</t>
+  </si>
+  <si>
+    <t>LineString (530531.28659617097582668 180919.46416819942533039, 530563.88801023468840867 180944.97831833627424203, 530620.69896473211701959 180923.3214464345946908, 530631.52323099854402244 180940.26917490593041293, 530672.45004481147043407 181008.75894496028195135, 530717.5530641155783087 181038.41000394721049815, 530783.43270573788322508 181058.76900571642909199, 530778.00363859941717237 181104.28964556960272603, 530801.95612234645523131 181156.06284796763793565, 530751.4015138226095587 181178.39113339898176491, 530780.09174134500790387 181213.18420375051209703, 530814.09418500657193363 181239.43468773260246962, 530853.48855285136960447 181252.44053536702995189, 530912.3730502761900425 181206.08465441560838372, 531047.80579616781324148 181254.33936599228763953, 531131.03878337366040796 181286.03806058526970446, 531110.30965442163869739 181356.39285153028322384, 531197.1542466712417081 181376.88721254793927073, 531286.93602178571745753 181375.08379181567579508, 531305.25734407640993595 181583.75572135805850849, 531325.21203300100751221 181586.18808011634973809, 531388.88918386655859649 181572.61640889989212155, 531390.49493819230701774 181599.32936576748033985, 531367.26279260986484587 181685.65545662579825148, 531395.89248193160165101 181593.61920236010337248, 531412.32238542404957116 181591.09869188832817599, 531419.12145480117760599 181581.94767167716054246, 531385.41458384564612061 181534.11455342586850747, 531374.38023236603476107 181529.41130202304339036, 531413.36951656360179186 181525.26491641241591424, 531471.93530321691650897 181443.00015478587010875, 531489.86913823755457997 181396.66486753628123552, 531500.42645009863190353 181343.75654840667266399, 531561.43261282751336694 181271.18043218745151535, 531510.99066478840541095 181339.18317034683423117, 531566.52648988855071366 181353.74707860476337373, 531590.37191976455505937 181360.8123911606380716, 531583.52515332715120167 181463.7283773985109292, 531566.74728090583812445 181537.16921628548880108, 531557.91564021108206362 181566.97600363052333705, 531578.66999584389850497 181574.92448025586782023, 531607.15203708468470722 181582.43137484646285884, 531674.27250636543612927 181614.50127011956647038, 531688.84471351187676191 181590.65584024353302084, 531676.92199857381638139 181529.27593741449527442, 531692.81895182456355542 181520.00271468493156135, 531744.15286336338613182 181527.39921376685379073, 531827.17028589476831257 181517.68440900254063308, 531837.76825472852215171 181595.40284711701679043, 531873.09481750777922571 181627.19675361836561933, 531892.79980997554957867 181649.86393449633033015, 531906.87584316555876285 181666.05597267561824992, 532031.40197696257382631 181539.76351073960540816, 532080.85916485369671136 181575.09007351889158599, 532117.06889170245267451 181580.38905793579760939, 532140.91432157845702022 181599.81866746442392468, 532170.05873587145470083 181590.98702676958055235, 532184.18936098308768123 181559.19312026820261963, 532149.74596227332949638 181529.16554190579336137, 532138.2648293700767681 181394.04143927496625111, 532132.82734409463591874 181370.85496780133689754, 532125.90053239720873535 181323.38831371636479162, 532096.75611810432747006 181293.36073535395553336, 532017.27135185094084591 181313.67350895205163397, 532018.15451592043973505 181340.1684310365235433, 532031.40197696257382631 181369.31284532946301624, 532033.16830510157160461 181389.62561892755911686, 532057.23452599509619176 181405.74336319562280551, 532119.69996919808909297 181395.70321314127068035, 532140.79753599606920034 181364.76011517079314217, 532132.3034719011047855 181288.28254195442423224, 532160.56472212448716164 181242.35801034132600762, 532384.22602272103540599 181180.09494344278937206, 532424.85156991728581488 181173.91279495641356334, 532670.78084617818240076 181110.13770430514705367, 532818.19047775026410818 181176.80775713562616147, 532780.99707011831924319 181260.68462679820368066, 532688.27519202104303986 181257.87865509698167443, 532650.54560429917182773 181265.88190097737242468, 532436.45877699879929423 181308.18477205943781883, 532413.59236019768286496 181321.90462214010767639, 532414.73568103776779026 181427.0901394252141472, 532338.13318475405685604 181459.10312294677714817, 532350.7097139946417883 181509.40923990920418873, 532405.30328410735819489 181674.61910129722673446, 532528.63901972828898579 181635.46036252533667721, 532616.67472441249992698 181609.7356436240952462, 532545.63823982118628919 181643.35478146860259585, 532594.42826642119325697 181790.64542780804913491, 532462.787251255242154 181845.87942018534522504, 532437.01138814585283399 181871.65528329473454505, 532445.2964870025170967 181957.26797147953766398, 532616.5218633720651269 181942.53890684561338276, 532701.21398501726798713 181920.44530989468330517, 532802.42052498331759125 181910.09618882910581306, 532815.01476064522285014 182025.01858924416592345, 532915.61185974825639278 182009.02176296585821547, 532912.46310028480365872 181963.04987479909323156, 532924.13200544030405581 182009.18769421585602686, 532982.27383896452374756 182001.80460424453485757, 533061.71429885365068913 181990.75895807769848034, 533064.2333064244594425 181966.82838615524815395, 533035.89447125315200537 181858.51106061163591221, 532947.72920627577695996 181893.14741470987792127, 532880.60253748437389731 181721.24718533383565955, 532784.00711035938002169 181767.39149765466572717, 532747.24231199838686734 181784.20146203070180491, 532733.93556229211390018 181745.29988511741976254, 532713.1074947752058506 181674.74374392238678411, 532748.93080092582385987 181661.89110736449947581, 532742.91467317531351 181642.74888270380324684, 532713.65441547974478453 181552.64369662242825143, 532855.62877998419571668 181525.1299014599644579, 533071.32848995237145573 181469.8718779842602089, 533186.19458453194238245 181444.03007418513880111, 533181.16196181264240295 181435.64236965295276605, 533152.08458610100205988 181436.48114010615972802, 533186.47417468298226595 181432.28728784006671049, 533189.54966634477023035 181438.99745146580971777, 533257.37403261545114219 181533.14433782830019481, 533340.41452438081614673 181492.83427136726095341, 533338.70870435202959925 181483.54382457892643288, 533339.90022310265339911 181474.30955426144646481, 533358.96452311298344284 181468.35196050821105018, 533371.7733496823348105 181461.2028480043518357, 533421.18748124549165368 181431.14743276051012799, 533457.81188699707854539 181401.60169366677291691, 533466.42939423269126564 181399.13954874229966663, 533532.90730719361454248 181489.9311428323853761, 533627.23823461274150759 181537.48131668634596281, 533600.77017667470499873 181593.49511371820699424, 533571.96468304062727839 181647.30677931586978957, 533565.79550759738776833 181677.67810457508312538, 533571.43902549741324037 181761.11675010700128041, 533688.88424648460932076 181775.70174559103907086, 533695.46948461106512696 181806.18034129549050704, 533711.03833596489857882 181690.5134740429057274, 533774.42839107918553054 181698.56300485107931308, 533904.80115716229192913 181714.28477588956593536, 533897.61435122019611299 181746.38584243066725321, 534052.37023917213082314 181783.27811293312697671, 534085.0618540165014565 181674.51498261015512981, 534131.12462164927273989 181691.05033509369241074, 534139.47207866376265883 181655.85994260499137454, 534150.19790721382014453 181658.82599177915835753)</t>
+  </si>
+  <si>
+    <t>LineString (534494.76712749910075217 180197.82926488673547283, 534477.08958587038796395 180204.9261592309048865, 534466.10449469194281846 180201.48237478407099843, 534446.35375012725125998 180105.42193530994700268, 534275.77913797693327069 180170.50961626204662025, 534224.15787377348169684 180196.54468864286900498, 534203.5093680921709165 180212.25550818303599954, 534185.55414576060138643 180210.4599859498848673, 534171.14064759924076498 180237.33092047309037298, 534155.10926930524874479 180232.7692223628400825, 534110.10282780381385237 180227.94574123568600044, 534059.63022310636006296 180244.41244702640688047, 534045.56321658962406218 180253.93444574531167746, 534018.52404629567172378 180285.19719793670810759, 534005.14660858130082488 180295.44406237191287801, 533989.44804280833341181 180338.41282897180644795, 534003.21356487192679197 180354.3808345656725578, 534155.73554933757986873 180422.10720311899785884, 534135.36257668328471482 180462.85314842750085518, 534160.69113728043157607 180481.57425843409146182, 534211.8988793573807925 180382.46249957560212351, 534228.96812671632505953 180379.70939516284852289, 534265.3091049644863233 180416.35643082388560288, 534271.73921295220497996 180462.74348229306633584, 534252.4929513584356755 180455.64950213933479972, 534269.62446292664390057 180472.076978985540336, 534255.40823154035024345 180562.17560434373444878, 534234.92044681450352073 180597.79788426094455644, 534256.13046408852096647 180604.31816759763751179, 534251.89312430669087917 180626.73219362733652815, 534379.78553101746365428 180633.41155169066041708, 534352.34416242560837418 180636.5838860665098764, 534344.23650324332993478 180704.43507658550515771, 534297.84553046221844852 180708.00611733732512221, 534240.14221260114572942 180695.98651926324237138, 534189.34860979067161679 180672.75587819167412817, 534160.54824850801378489 180757.54946950945304707, 534160.5841055567143485 180757.22253176767844707, 534127.8658005315810442 180858.10397226159693673, 534111.99208847992122173 180939.00866548559861258, 534085.5094500295817852 180985.32051877162302844, 534070.93534209730569273 180988.37091345511726104, 534075.68040049390401691 180998.87782847607741132, 534054.99797940440475941 181035.08444935575244017, 534068.56281289900653064 181030.73750628152629361, 534096.52225887367967516 180994.37437144466093741, 534118.50570094562135637 180998.44537923578172922, 534120.13410406210459769 181012.28680572554003447, 534190.96963962737936527 181035.08444935575244017, 534233.56329029169864953 181041.4142344745923765, 534230.7365170813864097 181061.51134635950438678, 534425.65412626438774168 181087.91946370297227986, 534428.68984542321413755 181124.52763081435114145, 534418.41545121860690415 181314.94640340618207119, 534244.43570935411844403 181318.37120147436507978, 534082.24461821641307324 181331.92378598402137868, 534008.65777000458911061 181337.21434369860799052, 534003.03775836550630629 181356.73341751954285428, 533970.61429565714206547 181390.91446260787779465, 533908.72647818853147328 181354.13541679794434458, 533820.00587128894403577 181301.66338870135950856, 533762.7596401305636391 181265.19378197882906534, 533763.82057414436712861 181254.40761950571322814, 533775.00675160356331617 181229.54225989809492603, 533765.23515282932203263 181236.37174127201433294, 533750.68025846313685179 181246.3013364469516091, 533738.92612418869975954 181260.82114937415462919, 533558.01058455463498831 181157.44207860867027193, 533549.5142814606660977 181141.84867783010122366, 533537.31101294630207121 181133.86961764763691463, 533483.72784082207363099 181114.99530462495749816, 533375.88864138023927808 181117.98406295705353841, 533381.80025942670181394 181168.40668747131712735, 533323.37956343777477741 181201.44220008412958123, 533277.55680660111829638 181222.13016911473823711, 533325.81375910399947315 181204.22413798831985332, 533380.40929047460667789 181174.66604775583255105, 533399.53511356632225215 181212.91769393908907659, 533422.13835903815925121 181229.95706360254553147, 533476.03840593271888793 181291.15969749572104774, 533522.51176960719749331 181254.94408223693608306, 533527.5245621653739363 181246.81990119433612563, 533527.00599741796031594 181236.96717099371016957, 533512.83189432229846716 181222.62021298229228705, 533521.10348163370508701 181215.37559709040215239, 533538.7190823903074488 181185.9681870742351748, 533548.10621201666072011 181170.94877967197680846, 533562.65626293770037591 181116.50342783879023045, 533565.78408725361805409 181068.52103992408956401, 533568.11593338451348245 181052.2709871992119588, 533565.98876765870954841 181030.01686012774007395, 533550.6638780701905489 180995.96154993091477081, 533517.88564200571272522 180943.17581912584137172, 533527.8685909277992323 180932.10417117548058741, 533519.96954229823313653 180930.1110331111412961, 533540.88975644903257489 180852.93240523023996502, 533549.08821875147987157 180816.53405966371065006, 533554.74233068409375846 180784.02291605086065829, 533498.69594615150708705 180775.96580654679564759, 533473.25244245456997305 180751.37041963971569203, 533450.91870032052975148 180721.12092079993453808, 533451.20140591717790812 180708.11646335478872061, 533482.01631595019716769 180701.33152903561131097, 533556.93329905800055712 180708.68187454805593006, 533574.10766405356116593 180706.42022977498709224, 533632.91042815323453397 180723.09985997635521926, 533664.85616057284642011 180736.10431742150103673, 533657.22310946369543672 180723.94797676627058536, 533653.26523111085407436 180708.11646335478872061, 533628.66984420374501497 180717.16304244706407189, 533572.27007767534814775 180700.55408864485798404, 533556.72126986051443964 180706.77361177079728805, 533481.23887555941473693 180699.42326625832356513, 533449.2931431399192661 180706.77361177079728805, 533440.52926964417565614 180711.01419572028680705, 533410.70382919942494482 180714.40666287989006378, 533368.01528410776518285 180716.38560205633984879, 533344.26801399048417807 180714.68936847653822042, 533317.41098231042269617 180704.51196699772845022, 533298.32835453760344535 180707.05631736741634086, 533274.0156732271425426 180725.43218114858609624, 533214.36479233752470464 180758.22603035805514082, 533150.04926910332869738 180796.6033151010342408, 533131.95611091877799481 180803.10554382362170145, 533112.94415954523719847 180814.13106209231773391, 533032.09035890805535018 180821.19870200814330019, 533006.17641249333973974 180714.80543799756560475, 532992.55450278345961124 180708.59827885474078357, 533019.41655259137041867 180701.98867611197056249, 533047.67523066280409694 180678.44941610301611945, 533062.18958536896388978 180672.97919573029503226, 533115.1629428390879184 180663.2515109057421796, 533114.02687698940280825 180650.64306823158403859, 532992.54919304675422609 180668.21878358686808497, 532965.16652780049480498 180676.47188869985984638, 532901.83528268674854189 180686.95517446676967666, 532903.8358352929353714 180700.17105029500089586, 532872.50304960866924375 180704.79467259434750304, 532805.92588160140439868 180717.79913003949332051, 532743.73065034206956625 180737.3058162071974948, 532629.94164769724011421 180778.72218611396965571, 532470.49569119606167078 180823.95508157531730831, 532430.91690766729880124 180829.60919350798940286, 532433.74396363366395235 180866.36092107032891363, 532438.69131157477386296 180904.80888221247005276, 532442.04758695687633008 180933.26225840556435287, 532376.49201568041462451 180946.49365811274037696, 532363.86204323265701532 180943.08557030936935917, 532329.07950006308965385 180951.90650344750611112, 532315.44714884960558265 180943.88747332192724571, 532301.01289462356362492 180966.34075767348986119, 532226.53615233255550265 180942.88509455622988753, 532187.1426668408093974 180935.66796744323801249, 532167.69651878625154495 180930.25512210847227834, 532139.09281037421897054 180929.8960797434556298, 532123.20177462184801698 180929.61217962004593574, 532123.33968604251276702 180942.71376458398299292, 532121.13310331176035106 180929.61217962004593574, 532080.40532022377010435 180931.02180181790026836, 532009.50720332562923431 180939.44211503997212276, 532008.18429834255948663 180956.0519220509158913, 532005.24450949102174491 180998.31138679117430001, 532006.05295142508111894 180940.76502002315828577, 531891.98914398706983775 180948.40847103702253662, 531794.97611188772134483 180950.17234434792771935, 531743.82378587161656469 180940.76502002315828577, 531728.53688384382985532 180937.82523117164964788, 531695.6112487071659416 180929.00586461715283804, 531644.05815143184736371 180909.64867640155716799, 531643.0989445325685665 180988.84512792871100828, 531635.99518679245375097 181107.77244371830602176, 531600.40284548385534436 181102.74764259238145314, 531578.20997384435031563 181106.09751000965479761, 531580.30364098015706986 181147.13338587139151059, 531592.02817694062832743 181174.35105863682110794, 531388.24308429716620594 181174.00195023015839979, 531284.22938067012000829 181163.10201389936264604, 531174.40470271790400147 181122.28725966333877295, 531157.88846834062132984 181171.61513478367123753, 531133.39463505509775132 181279.42110962877632119, 531076.29551051347516477 181260.61487964406842366, 531131.04354967980179936 181113.15854730040882714, 531036.5176723989425227 181074.07573265538667329, 530995.61705242155585438 181020.45047535176854581, 530934.72057378862518817 181004.99913002699031495, 530807.47420052578672767 181052.26206866747816093, 530678.41002193070016801 181020.45047535176854581, 530547.98248933651484549 181092.25378597865346819, 530470.12182414066046476 180975.54759959221701138, 530509.09838743833824992 180925.67870823395787738, 530505.35225721553433686 180900.45491703250445426, 530522.85661772394087166 180912.72978561217314564, 530582.29576928459573537 180878.9198528709821403)</t>
+  </si>
+  <si>
+    <t>LineString (530577.55627936229575425 180873.29039143532281741, 530508.03351007960736752 180921.27411260729422793, 530398.23249808500986546 181052.05378589619067498, 530335.04888452554587275 181096.60453780728857964, 530313.7541854988085106 181095.4837641742778942, 530277.88942924339789897 181128.54658634730731137, 530208.96185081487055868 181204.75919339017127641, 530146.19852736778557301 181259.11671458987984806, 530115.37725246080663055 181311.23268852362525649, 530089.44054251117631793 181304.94443834689445794, 529993.94726804597303271 181289.97907443816075101, 529966.154449358349666 181292.82961994459037669, 529944.77535806014202535 181334.87516616433276795, 529944.77535806014202535 181344.13943906020722352, 529926.36038226482924074 181394.46298536835820414, 529818.3114558468805626 181372.26115117289009504, 529660.9002180868992582 181353.18405782332411036, 529658.19050382054410875 181346.70498227514326572, 529687.50564937863964587 181285.67399781054700725, 529721.54846181173343211 181300.10519003760418855, 529759.29157994396518916 181225.35901491285767406, 529693.52337177516892552 181197.2517148221086245, 529775.50000859634019434 181018.70994359909673221, 529775.97546259185764939 181007.7745017017587088, 529781.20545654278248549 181022.98902955889934674, 529838.73539000260643661 181058.17262522855889983, 529856.80264183296822011 181056.27080924643087201, 529884.37897357402835041 181053.41808527320972644, 529884.37897357402835041 181040.5808273937436752, 529841.11265998031012714 181013.00449565265444107, 529793.09180643118452281 180981.03021445288322866, 529813.06087424361612648 180938.71480885017081164, 529693.24646736856084317 180862.64216956440941431, 529636.19198790425434709 180936.81299286801367998, 529605.88993830105755478 180991.46413140607182868, 529541.23135347885545343 180948.44746960292104632, 529492.06945427530445158 181030.20584545240853913, 529469.24634072056505829 181064.96606145869009197, 529432.46901320235338062 181041.241028774617007, 529404.33170837664511055 181030.67362469981890172, 529429.55946595408022404 180980.22139381090528332, 529341.93906022026203573 180918.15693974946043454, 529373.44581776950508356 180865.09463160243467428, 529338.10332967818249017 180918.10836373933125287, 529359.73536980303470045 180936.38896102792932652, 529323.421695526689291 180994.47477187277399935, 529276.82450287113897502 181091.04343665213673376, 529230.54867016489151865 181075.93951903271954507, 529206.7680339131038636 181060.51424146397039294, 529190.05731654691044241 181112.25319330915226601, 529147.47712325816974044 181094.25703614563099109, 529106.50156080489978194 181164.15282512898556888, 529059.30068865197245032 181142.16352662167628296, 529031.81018039816990495 181159.5481742657138966, 528861.2339281034655869 181105.69332964604836889, 528883.78786570683587343 181037.0717748103197664, 528922.69545664661563933 181033.7714086250634864, 528993.14916742767672986 180829.5977204886439722, 529045.82958481332752854 180895.76286042633000761, 529195.22303077194374055 180668.01108742074575275, 529239.74813623412046582 180680.31407708793994971, 529252.95472623594105244 180654.80634892109083012, 529237.65350798552390188 180675.84590674249920994, 529186.38057327619753778 180657.79299018002348021, 529111.49788893118966371 180613.026168017211603, 529033.15595014626160264 180735.32098674381268211, 528988.79609909397549927 180702.76329789814190008, 529001.00523241108749062 180683.22868459072196856, 528968.42684971622657031 180655.33458768369746394, 528933.41540621093008667 180638.92297354058246128, 528917.00379206787329167 180629.07600505475420505, 528956.39166601130273193 180565.6177637014479842, 528887.85708987119141966 180519.54143586705322377, 528863.23976127826608717 180540.43739942065440118, 528805.31899289903230965 180498.65170223280438222, 528842.96749234548769891 180432.87025814500520937, 528817.31686634896323085 180364.08934569478151388, 528801.18179515760857612 180348.78171405172906816, 528777.89595665864180773 180339.10883718938566744, 528784.87936172517947853 180328.35022461912012659, 528766.49707728379871696 180311.67933983076363802, 528735.71864135982468724 180290.81664662051480263, 528713.38623358681797981 180285.77175626676762477, 528668.77996420615818352 180275.46013541670981795, 528678.81986454653088003 180236.4348891912959516, 528685.54394682915881276 180209.20438540610484779, 528648.68728152720723301 180200.38155767129501328, 528657.51626427297014743 180164.64456824841909111, 528561.08355491538532078 180139.08601459197234362, 528473.16496016969904304 180096.57592482483596541, 528471.71575256390497088 180078.58159705405705608, 528455.77446890133433044 180078.09852785218390636, 528452.87605368986260146 180092.59060390916420147, 528456.2575381031492725 180107.5657491680176463, 528445.63001566135790199 180136.06683208007598296, 528434.51942401775158942 180130.75307085920940153, 528435.00249321956653148 180119.15941001361352392, 528434.03635481582023203 180138.48217808958725072, 528458.18981491075828671 180158.28801536746323109, 528508.42901190835982561 180176.64464503963245079, 528492.97079744748771191 180232.19760325804236345, 528463.50357613165397197 180225.43463443146902137, 528442.73160045000258833 180280.1422215465863701, 528368.29083982005249709 180530.61085074103903025, 528399.42485451779793948 180540.37256290816003457, 528373.18561336421407759 180528.66321234643692151, 528398.20391442335676402 180451.73774791724281386, 528402.87839129334315658 180453.56406502836034633, 528495.6276780579937622 180483.51435554612544365, 528631.8531929935561493 180596.55254879055428319, 528664.70189872267656028 180554.04245902341790497, 528713.73342271556612104 180597.76022179532446899, 528701.17362346616573632 180617.08298987129819579, 528701.17362346616573632 180635.4396195434674155, 528716.6318379269214347 180666.35604846503701992, 528751.41282046365085989 180679.88198611821280792, 528786.19380300038028508 180647.03328038906329311, 528882.80764338024891913 180721.42593748154467903, 528908.89338028279598802 180749.44395119170076214, 528941.25901681010145694 180770.21592687338124961, 528984.08419391023926437 180821.70737133437069133, 528974.05492355371825397 180859.35868258221307769, 528937.50480806769337505 180969.80595063656801358, 528905.95696268742904067 181031.40703499672235921, 528880.53527438559103757 181033.05660670524230227, 528856.86684315488673747 181104.10146333416923881, 528782.41271002357825637 181081.97650190588319674, 528728.68565749109257013 181158.32547129417071119, 528765.44627238169778138 181172.88833027009968646, 528732.9272669015917927 181276.59568035582196899, 528674.92537136201281101 181261.00874411704717204, 528689.63158279552590102 181226.14957627476542257, 528640.0662035197019577 181213.07738833394250832, 528719.58868015988264233 181095.42769686627434567, 528668.38927739160135388 181063.29190151169314049, 528617.73454912076704204 181139.00165666910470463, 528598.12626720953267068 181160.78863657053443603, 528611.19845515035558492 181136.82295867896755226, 528206.1428879996528849 181051.66365116246743128, 528237.1932889255695045 180958.33994615747360513, 528214.42299491330049932 180950.7498481533548329, 527957.73968059255275875 180869.32879683657665737, 527979.60677813622169197 180868.6474805666366592, 527980.52286685828585178 180863.87237577338237315, 528002.11622184654697776 180796.95082105748588219, 528147.20215247070882469 180846.02662784914718941, 528143.09763044805731624 180858.87556635460350662, 528222.86812366941012442 180886.3580181579454802, 528226.97264569206163287 180877.07822923734784126, 528255.5258423708146438 180886.00110319946543314, 528274.28005263407249004 180832.49227053558570333, 528413.89659711671993136 180874.71776203761692159, 528440.4577933840919286 180872.67459309397963807, 528441.88889231265056878 180868.47956919606076553, 528480.12932370661292225 180756.38422738478402607, 528315.31369558570440859 180703.26183484998182394, 528079.46642620186321437 180632.41520988091360778)</t>
+  </si>
+  <si>
+    <t>LineString (530581.86556883039884269 180867.74445010567433201, 530619.76996912294998765 180831.70142661320278421, 530983.56856463546864688 180203.70454308946500532, 531002.70594172133132815 180167.18990898446645588, 531009.82027298887260258 180172.62735671561677009, 531014.84303175657987595 180179.2561260225775186, 531055.46903743746224791 180126.53966183957527392, 531062.93085470306687057 180082.20768867310835049, 531131.40400137600954622 180037.87571550664142706, 531230.60227796633262187 180072.55121927050640807, 531196.8046350572258234 180173.50521757037495263, 531180.12527881644200534 180209.05858218902722001, 531154.66731402778532356 180209.05858218902722001, 531173.54132240556646138 180223.10435586553649046, 531118.23608855437487364 180332.83696271321969107, 530929.62455369275994599 180270.64411783422110602, 530940.64358626771718264 180262.38647808227688074, 530923.9078333250945434 180242.84698136936640367, 530866.90213167306501418 180188.57442979663028382, 530842.303780960268341 180151.09122871042927727, 530862.94364999502431601 180139.18124142149463296, 530885.30430015258025378 180128.40685322834178805, 530835.31284910615067929 180139.32700893725268543, 530818.64858063124120235 180107.00842765255947597, 530746.94172840588726103 179903.50236112563288771, 530810.56893531011883169 179879.7684029946976807, 530845.41240575758274645 179870.67880200836225413, 530942.97500607429537922 180058.23076402678270824, 531005.72952298959717155 180026.85350556910270825, 531037.65725966589525342 180016.94489763511228375, 531078.94312605750747025 180004.28389860835159197, 531103.36682528315577656 179997.4820276228711009, 531123.39294299448374659 179985.6610553627833724, 531156.49166532268282026 179963.68795398517977446, 531181.76768542011268437 179933.82261524567729793, 531212.01546737970784307 179888.97245578825823031, 531103.54066311055794358 179763.39200930739752948, 531108.54719253838993609 179756.71663673696457408, 531135.1701887323288247 179781.81394092956907116, 531167.34841385786421597 179808.82066558845690452, 531194.06783293525222689 179811.40641582175157964, 531236.87636457534972578 179792.73155302571831271, 531253.82739388255868107 179784.97430232583428733, 531249.51781016041059047 179751.07224371147458442, 531230.84294736431911588 179747.62457673373864964, 531216.11277351365424693 179764.36885167972650379, 531081.64286881464067847 179671.73402844261727296, 531009.90093444765079767 179597.21122520481003448, 531009.90093444765079767 179597.21122520481003448, 530978.82935859297867864 179566.08749107754556462, 531113.89855216781143099 179467.38308038824470714, 531145.9327949439175427 179489.53642785921692848, 531118.11753764539025724 179461.98862495779758319, 531170.3957165403990075 179433.66088251979090273, 531266.22342408250551671 179404.70195991088985465, 531313.87248040549457073 179407.3990763065230567, 531433.52216941397637129 179415.3352683637640439, 531469.58935155137442052 179427.35766240957309492, 531466.38337980583310127 179436.3744579438935034, 531357.78108692553360015 179511.91516719831270166, 531327.52472857688553631 179431.76587355969240889, 531318.50793304259423167 179389.48712116529350169, 531315.08669927902519703 179378.57198898226488382, 531298.67588855815120041 179338.66640459033078514, 531270.20679607603233308 179239.75740465606213547, 531274.79732766340021044 179226.52587243364541791, 531198.10844702739268541 179192.5019324331660755, 531219.62179134623147547 179127.21737543260678649, 531235.3105901419185102 179110.29808261376456358, 531240.33914468786679208 179077.35684370002127253, 531245.46363338397350162 178841.6303636806551367, 531233.0184465505881235 178844.00959057526779361, 531233.75051636435091496 178886.46963977129780687, 531226.42981822707224637 179085.22659419756382704, 531181.16885312169324607 179183.82010049920063466, 530988.59653849294409156 179108.14471807319205254, 530973.83061021461617202 179097.68551887612557039, 530832.78523280692752451 179038.00655875154188834, 530746.65065118379425257 179009.70519621824496426, 530660.53985221788752824 178980.90664574180846103, 530629.06085022771731019 178958.21248151632607915, 530596.23852397978771478 178935.36033985641552135, 530526.31339351984206587 178863.9934541292313952, 530506.84969741245731711 178868.31871993085951544, 530530.63865932147018611 178898.5955805424018763, 530534.24304748955182731 178938.24385039083426818, 530561.63639756664633751 178960.59105703269597143, 530637.84568799240514636 178901.11103604579693638, 530747.65616005111951381 178890.12998883993714117, 530829.64797918824478984 178865.23961517328280024, 530854.35533540148753673 178855.90572504830197431, 530871.92501093086320907 178861.03021374437958002, 530891.65204298356547952 178844.1667831186496187, 530965.44759355159476399 178788.4324741373420693, 530886.32739482226315886 178835.18531884101685137, 530876.4373699810821563 178823.49710766511270776, 530792.12940123490989208 178700.15787217835895717, 530743.08072371536400169 178626.95089080586330965, 530828.00082210742402822 178569.11737552162958309, 530830.19703154859598726 178562.52874719808460213, 530868.26466186228208244 178541.84777496033348143, 530837.15169477893505245 178458.75785110259312205, 530903.77004782785661519 178437.16179159769671969, 530958.67528385727200657 178408.9771037692844402, 530969.51906797324772924 178398.22482838027644902, 530903.17095182067714632 178270.43457464387756772, 530838.13083763618487865 178210.65022726217284799, 530867.03755505150184035 178124.58704586655949242, 531097.63432352372910827 178142.32525882596382871, 531169.9011170620797202 178195.53989770417683758, 531216.54604743677191436 178275.69034144666511565, 531215.56562907935585827 178356.32546967949019745, 531310.11752128496300429 178268.96068190585356206, 531365.33336403663270175 178240.15241612237878144, 531381.33795613853726536 178257.757467434508726, 531467.76275348896160722 178198.54047665739199147, 531466.96252388379070908 178187.33726218604715541, 531513.37584097939543426 178158.52899640260147862, 531625.40798569284379482 178357.78616807149956003, 531634.2105113489087671 178376.19144898871309124, 531471.76390151435043663 178477.02037923081661575, 531565.23039256664924324 178567.62021348648704588)</t>
+  </si>
+  <si>
+    <t>LineString (530577.23797894886229187 180877.97880632089800201, 530617.74819760688114911 180823.78270298111601733, 530843.57723920769058168 180435.41664124984527007, 531047.93121784145478159 180130.71107881036004983, 531054.34628752165008336 180080.99428878910839558, 530975.76168393960688263 180074.57921910894219764, 530900.78555705270264298 179951.08912776576471515, 530802.15386072010733187 179775.07565341630834155, 530805.36139556020498276 179738.18900275535997935, 530887.15353398234583437 179686.0665616040059831, 530865.50267381174489856 179648.37802723306231201, 530833.42732541100122035 179631.73894025012850761, 530823.80472089070826769 179592.44663845913601108, 530802.15386072010733187 179519.4752208472636994, 530780.50300054962281138 179416.03222225463832729, 530714.74853632797021419 179334.24008383255568333, 530639.37146758602466434 179282.9195263912260998, 530567.20193368417676538 179116.12771470696316101, 530551.16425948368851095 179003.86399530406924896, 530547.95672464370727539 178935.30293809733120725, 530268.09930984652601182 178972.18958875827956945, 530250.45786822598893195 178968.98205391821102239, 530211.96745014504995197 178975.39712359837722033, 529909.15843551640864462 178978.99828037086990662, 529880.44869170524179935 178978.50328478790470399, 529858.17389047238975763 178983.94823620040551759, 529736.00598863395862281 178985.05673808956635185, 529714.56382836180273443 179011.67757219314808026, 529647.12768985063303262 179156.00351349293487146, 529574.64959705818910152 179124.097396557132015, 529526.79745115165133029 179077.07363828388042748, 529564.38437103840988129 179130.25138729959144257, 529513.81095916836056858 179152.52902801893651485, 529512.12165939807891846 179263.45971292795729823, 529524.55590479262173176 179301.70093485678080469, 529448.61280135076958686 179371.58212878205813468, 529385.91768299601972103 179410.16374007728882134, 529333.16189551877323538 179435.02868727562599815, 529281.9714767278637737 179374.53091961363679729, 529220.891999761457555 179328.57588456268422306, 529164.02991525223478675 179367.55040796031244099, 529081.42719402140937746 179391.9821987469040323, 529060.48565906146541238 179415.83228022902039811, 529027.32822870835661888 179419.32253605569712818, 528999.98789139953441918 179308.21605890721548349, 529003.47814722615294158 179297.74529142724350095, 529055.25027532153762877 179270.40495411845040508, 529084.33574054366908967 179209.47090447816299275, 529104.11385689466260374 179164.09757873168564402, 529351.77659326093271375 179225.75876500256708823, 529383.05599977204110473 179235.19909444704535417, 529373.87950731569435447 179284.14038754784269258, 529392.23249222850427032 179227.24613431817851961, 529266.2086624939693138 179192.37546298385132104, 529269.26749331271275878 179176.46954272608854808, 529304.13816464703995734 179174.63424423482501879, 529268.04396098526194692 179166.06951794217457063, 529196.15887484396807849 179120.03240704443305731, 529149.98932790081016719 179107.75948950258316472, 529203.17197058210149407 179134.6430231656995602, 529187.39250517124310136 179174.383899015490897, 529058.81908330414444208 179141.07169425903703086, 529011.0423685876885429 179146.33151606269530021, 528858.21532395936083049 179161.52655682878685184, 528770.55162723187822849 179211.78707628592383116, 528715.03128597105387598 179321.6589095177478157, 528618.60121957084629685 179477.9925020151422359, 528491.34275315469130874 179622.19928313192212954, 528388.04569717741105705 179719.06766801583580673, 528360.57773886946961284 179750.62659883772721514, 528302.13527438452001661 179698.61280544605688192, 528281.73319864494260401 179662.65391637163702399, 528262.13372618111316115 179565.91304187983041629, 528297.16959096642676741 179504.60027850553160533, 528354.10287124256137758 179445.47725668028579094, 528571.1610022954409942 179230.06143178927595727, 528461.67392484133597463 179117.28974201151868328, 528427.73293083056341857 179154.51534834591438994, 528270.83738425537012517 178995.94010165525833145, 528307.81268304819241166 178962.03991528681945056, 528251.02088932693004608 178905.98091890395153314, 528237.09773989859968424 178880.69941073132213205, 528445.48698298842646182 178680.18773902862449177, 528506.68087698111776263 178769.79506966570625082, 528622.96355511201545596 178714.21878967669908889, 528690.51011079095769674 178852.7319798031821847, 528629.80371264915447682 178709.94369121600175276, 528706.32797509559895843 178677.88045276078628376, 528675.97477602458093315 178675.74290353045216762, 528565.03597096959128976 178505.16647494878270663, 528591.54158142581582069 178459.85043126542586833, 528535.96530143683776259 178489.77612049027811736, 528478.67898206354584545 178502.6014158723410219, 528322.21037840214557946 178459.85043126542586833, 528311.95014209649525583 178498.3263174116727896, 528292.28468917729333043 178492.34117956669069827, 528227.69070692639797926 178577.5864321083354298, 528109.89053357648663223 178750.95101042950409465, 528057.58673679200001061 178714.85402391621028073, 528050.95667804463300854 178736.21754654651158489, 528039.90658013243228197 178798.09809485499863513, 528075.26689345156773925 178816.51492470869561657, 528057.36634973983746022 178881.49318986901198514, 528077.50150927738286555 178927.95894264802336693, 527957.20683819404803216 178903.17720783254480921, 527893.18735658738296479 178892.33519885077839717, 527901.3675460263621062 178842.38277947145979851, 527870.26802183757536113 178834.76434196019545197, 527853.8672185888281092 178819.73012841463787481, 527876.57178353331983089 178723.1521395173331257, 527822.2081079538911581 178692.29039585794089362, 527839.85880704678129405 178661.95543657644884661, 527875.91507322294637561 178584.04074644856154919, 527702.52480672812089324 178435.08524715233943425, 527673.89863282348960638 178393.55225022041122429)</t>
+  </si>
+  <si>
+    <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529270.770087662152946 178758.30559268582146615, 529304.71750739659182727 178689.86743865112657659, 529337.70783226401545107 178657.27980173568357714, 529305.00792290433309972 178707.29236911991029046, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529619.5737125719897449 178946.00311593859805726, 529714.19555520184803754 179001.94307321662199683, 529732.04873305652290583 178984.08989536194712855, 529747.52148719725664705 178977.54373014855082147, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529975.09426932758651674 178984.62321261296165176, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530137.16457231086678803 179220.90265564562287182, 530137.2566814114106819 179287.56575694994535297, 530164.29013196483720094 179289.33844223213964142, 530181.6477391414809972 179297.81860453309491277, 530152.236118592787534 179291.25757650277228095, 530123.93161658430472016 179290.37801461422350258, 530010.93885788007173687 179324.27584222549921833, 529997.12863181624561548 179285.35611422738293186, 529943.14320265757851303 179272.8013632602232974, 529935.82251096051186323 179312.1535707954026293, 529909.83655243786051869 179337.6092036338231992, 529899.811406908207573 179372.55586857470916584, 529796.77445525978691876 179363.87907264640671201, 529750.2085215135011822 179339.20018068622448482, 529724.22256299096625298 179373.14102447082404979, 529924.43567383696790785 179499.69993192006950267, 529928.14961813052650541 179531.89329112289124168, 529927.0135171840665862 179569.76332267106045038, 529922.25843279552645981 179593.81102334667230025, 529914.26865162816829979 179631.81709465332096443, 529926.90485368797089905 179695.04491854083607905, 530056.77231763186864555 179684.35815048823133111, 530089.18110335676465183 179679.01476646191440523, 530121.47372855921275914 179675.29762974794721231, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530871.2405794725054875 180748.77793378444039263, 530884.09205942158587277 180795.04326160132768564, 530994.61478698416613042 180838.09571943094488233, 530982.23648845416028053 180885.78941204195143655, 531002.32567495363764465 180840.66601542077842169, 531087.78801661543548107 180857.37293935465277173, 531104.77522879175376147 180851.00402391061652452, 531115.93421733961440623 180802.8298538378730882, 531377.42735681601334363 180810.11179436542443, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531465.94281411881092936 180989.74318283077445813, 531389.47650842147413641 180987.01224334159633145, 531387.55785732087679207 181129.37252376566175371, 531386.90621243161149323 181168.05746712500695139, 531290.5201128131011501 181159.06143116063321941, 531142.08551940054167062 181108.94065935898106545, 531043.74918007606174797 181071.66004718522890471, 530997.40789101168047637 181015.41131011385004967, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530860.84877428377512842 180964.44244112810702063, 530839.77010409883223474 180962.68588527935207821, 530823.96110146003775299 180993.71837194060208276, 530827.47421315754763782 181054.02678941437625326, 530740.23193933628499508 181041.73089847312076017, 530692.21941280376631767 181014.7970421256031841, 530549.35287043871358037 181094.42757393565261737, 530472.93963134801015258 180978.161691593733849, 530513.05071623111143708 180924.627175223082304, 530505.35225721553433686 180900.45491703250445426, 530526.51764440489932895 180907.64713535181363113, 530581.55639433243777603 180875.44361145806033164)</t>
+  </si>
+  <si>
+    <t>LineString (528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526810.75304763286840171 179467.00080663594417274, 526668.71815055573824793 179454.61404235597001389, 526444.82263462664559484 179424.7408409794443287, 526441.88616490841377527 179401.24908323338604532, 526400.95936604985035956 179579.61037377678439952, 526395.80753890855703503 179617.60509894342976622, 526400.31538765714503825 179630.4846667965175584, 526396.45151730126235634 179663.00557562557514757, 526429.93839371926151216 179670.41132714110426605, 526431.87032889726106077 179659.14170526966336183, 526400.31538765714503825 179655.59982411004602909, 526404.17925801302772015 179629.51869920754688792, 526481.13467593537643552 179644.97418063125223853, 526512.36762797913979739 179646.26213741654646583, 526515.90950913866981864 179639.17837509737000801, 526505.28386565984692425 179635.63649393775267527, 526386.30885761685203761 179621.30797470119432546, 526318.94980677636340261 179621.48525741521734744, 526215.34960218577180058 179626.84875574553734623, 526121.02660867478698492 179655.6876124200061895, 526113.32453510130289942 179686.26937513795564882, 526116.04291400965303183 179658.17945975257316604, 526072.0957883259980008 179674.03667005078750663, 526077.53254614258185029 179626.23850758047774434, 526092.24883591232355684 179409.14943758773733862, 526170.58646800776477903 179414.55203290464123711, 526170.91200886678416282 179254.77395809174049646, 526170.02756560104899108 179226.2506627686379943, 526170.69089805032126606 179197.28514581263880245, 526191.0330931645585224 179103.75527045089984313, 526208.50084766466170549 179068.1564290011592675, 526190.95479760388843715 179087.37647593740257435, 526152.42256449558772147 179079.67002931574825197, 526079.61222019151318818 179075.18120090151205659, 525857.43331313808448613 179086.440267137310002, 525822.15490559919271618 179081.18603622727096081, 525774.11622299312148243 179039.15218894690042362, 525789.9340731572592631 179008.44695039271027781, 525608.18420976598281413 178985.48173996026162058, 525584.06940557796042413 178987.97679135657381266, 525573.85263970901723951 179052.99129645497305319, 525566.40184021822642535 179179.43401284626452252, 525539.12785214162431657 179262.48159250925527886, 525230.67203460761811584 179148.19059485456091352, 525218.00911157194059342 179136.66408798881457187, 525275.51739498809911311 178989.94413040805375203, 525288.82619905064348131 178973.64458385962643661, 525321.71609151223674417 178916.64969141795882024, 525110.25522415374871343 178791.72511747083626688, 525140.83571881789248437 178743.57710459540248848, 525170.6157625982305035 178737.53536503901705146, 525136.90032081049866974 178734.29459415673045442, 525073.96749363793060184 178845.07109110968303867, 525050.22967286221683025 178837.15848418447421864, 524920.68373622617218643 178769.44129003383568488, 524812.24932546948548406 178896.28909129649400711, 524699.21156708616763353 179025.31069560500327498, 524681.6391244096448645 179051.25509521568892524, 524679.63010795961599797 179077.09913740976480767, 524788.97600055101793259 179149.0372246410115622, 524957.31112467218190432 179248.31178502010880038, 524889.31033757049590349 179366.96949636968201958, 524837.84125263791065663 179392.39398410747526214, 524751.64603811223059893 179345.88577483102562837, 524614.60184811090584844 179570.98550772908492945, 524703.84473427385091782 179436.35361285935505293, 524844.32857223774772137 179505.77558726171264425, 524810.43752961605787277 179598.63431089642108418, 524822.46338344959076494 179627.87900090057519265, 524845.42183167708572 179640.99811417344608344, 524954.20114589820150286 179688.82821464753942564, 524980.43937244394328445 179689.64815922707202844, 525145.27674076042603701 179339.90930881092208438, 525213.61852516769431531 179374.56420798628823832, 525206.26161919755395502 179390.0524310814216733, 525222.23384926444850862 179385.21236136413062923, 525351.1733065313892439 179466.91273819096386433, 525352.72212884086184204 179482.01375570870004594, 525369.8851592862047255 179479.95885097398422658, 525422.48737169418018311 179507.45546200548415072, 525366.53774576925206929 179596.40102116821799427, 525283.64405398862436414 179742.1564941595424898, 525384.085012789350003 179740.24697022794862278, 525418.45644355763215572 179681.43363313551526517, 525419.82130964624229819 179656.85948007801198401)</t>
+  </si>
+  <si>
+    <t>LineString (525327.85414873412810266 178420.77501689142081887, 525435.54454665677621961 178546.54447064295527525, 525345.92272875038906932 178653.20884751385892741, 525429.15519386087544262 178703.14832658017985523, 525460.07010947330854833 178656.1814355535316281, 525501.7821286671096459 178615.87244897283380851, 525558.91436985018663108 178563.64555782591924071, 525601.34650842915289104 178515.0539152596029453, 525591.59441469295416027 178508.14618219647672959, 525612.31761388236191124 178515.8665897376195062, 525739.09483245271258056 178641.42479659095988609, 525767.53843918326310813 178664.58601921438821591, 525708.21320228814147413 178737.72672223576228134, 525731.62045715074054897 178716.68428954426781274, 525769.37393091234844178 178666.83504263576469384, 525806.39432751352433115 178612.95387134497286752, 526026.40911028429400176 178722.27400289245997556, 526144.43453311175107956 178765.52555535719147883, 526097.8322964139515534 178902.16469051572494209, 526093.05398678814526647 178927.64900852003484033, 526073.41744379187002778 178941.35436849229154177, 526098.01514758018311113 178929.59024928920553066, 526150.06246284244116396 178767.20975544024258852, 526255.77580733434297144 178814.4714835460181348, 526271.20979337661992759 178817.35269416749360971, 526312.78246261400636286 178730.88154215391841717, 526431.85428454133216292 178507.28957353180157952, 526371.81847308482974768 178458.83962042655912228, 526552.97916730435099453 178570.48516453863703646, 526555.08568700461182743 178631.57423584524076432, 526531.73185393039602786 178797.25923736946424469, 526501.3099303717026487 178977.1575194436009042, 526543.68378180800937116 178800.00690841992036439, 526578.25740370713174343 178795.88277246299549006, 526808.88298217917326838 178842.85059796637506224, 526867.58985495707020164 178857.72481234182487242, 526887.47400313417892903 178869.08718272874830291, 526862.61881791288033128 179084.26207193068694323, 526876.82178089639637619 179026.0299236977880355, 526893.15518832765519619 179011.11681256498559378, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527768.86287219019141048 179171.7344985579547938, 527738.35830124607309699 179152.01631094136973843, 527772.52151037787552923 179165.95770141950924881, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528513.98412839835509658 179812.26687349064741284, 528529.45710146625060588 179823.30889789306093007, 528522.1132692665560171 179877.67606056467047893, 528516.61473636329174042 179896.37107243580976501, 528982.89032656128983945 180285.39227534280507825, 528985.75060231669340283 180264.89964467784739099, 528997.18651210982352495 180296.38934114936273545, 529128.14837153907865286 180399.20853238902054727, 529260.66181104525458068 180474.31033623719122261, 529390.66158775170333683 180271.80423245803103782, 529460.4421130547998473 180310.72029464627848938, 529430.42441646789666265 180361.7129266606643796, 529518.94092159741558135 180419.07557802950032055, 529552.56730343436356634 180373.58106142663746141, 529648.71743816568050534 180427.49491339456290007, 529608.480220987345092 180501.82199512678198516, 529569.44679091090802103 180572.25595415246789344, 529667.74284364131744951 180629.72475247565307654, 529730.9295924516627565 180529.48919386579655111, 529787.31384936452377588 180567.2724588074197527, 529763.12702995492145419 180622.33490404754411429, 529706.82561028259806335 180576.71049719117581844, 529752.5037739867111668 180495.92673939117230475, 529740.29997511499095708 180487.27313655486796051, 529754.05698475218378007 180486.60747479822020978, 529800.36167021188884974 180412.51190174778457731, 529824.728592021856457 180415.94968910259194672, 529890.00781108462251723 180459.31649564448161982, 529865.28168949380051345 180503.69017882505431771, 529855.61934717127587646 180535.74483229906763881, 529894.55648332042619586 180548.55958596843993291, 529890.50570647965651006 180564.17520972224883735, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530054.15927445457782596 180611.80309442835277878, 530069.85973392939195037 180508.62456558644771576, 530160.12516808835789561 180516.73132610463653691, 530168.55684169579762965 180494.19840525725157931, 530148.45289235515519977 180461.23712512332713231, 530174.04404229309875518 180496.50880550872534513, 530161.336840910022147 180527.69920890356297605, 530154.59773694002069533 180615.4214020338258706, 530232.82974896696396172 180614.62270036846166477, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530441.01278525067027658 180758.81861569813918322, 530400.55581117747351527 180811.16401171206962317, 530524.57064777321647853 180911.87319211009889841, 530583.04193836136255413 180879.49776674556778744)</t>
   </si>
 </sst>
 </file>
@@ -340,9 +343,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +664,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,24 +689,27 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -711,10 +718,10 @@
         <v>36</v>
       </c>
       <c r="D2">
-        <v>10387.633383793</v>
+        <v>10321.9855903425</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
@@ -731,10 +738,13 @@
       <c r="M2">
         <v>72.2</v>
       </c>
+      <c r="N2">
+        <v>72.099999999999994</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -746,7 +756,7 @@
         <v>10324.6261671389</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
@@ -763,10 +773,13 @@
       <c r="M3">
         <v>70.599999999999994</v>
       </c>
+      <c r="N3">
+        <v>70.599999999999994</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -778,7 +791,7 @@
         <v>10889.6786160784</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -795,12 +808,14 @@
       <c r="M4">
         <v>71.7</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="2">
+        <v>72.900000000000006</v>
+      </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -812,7 +827,7 @@
         <v>9934.8314288458605</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -829,10 +844,13 @@
       <c r="M5">
         <v>71.900000000000006</v>
       </c>
+      <c r="N5">
+        <v>72.099999999999994</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -844,7 +862,7 @@
         <v>10047.75961035</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
@@ -861,12 +879,14 @@
       <c r="M6">
         <v>71.7</v>
       </c>
-      <c r="N6" s="1"/>
+      <c r="N6" s="2">
+        <v>72</v>
+      </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -878,10 +898,10 @@
         <v>10347.2332512455</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J7">
         <f>AVERAGE(J2:J6)</f>
@@ -899,24 +919,27 @@
         <f>AVERAGE(M2:M6)</f>
         <v>71.61999999999999</v>
       </c>
-      <c r="N7" s="1"/>
+      <c r="N7">
+        <f>AVERAGE(N2:N6)</f>
+        <v>71.94</v>
+      </c>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>10248.4265845503</v>
+        <v>10276.701746320599</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -924,11 +947,11 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D9" s="1">
         <f>SUM(D2:D8)</f>
-        <v>72180.189042001963</v>
+        <v>72142.816410321757</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -961,7 +984,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -973,12 +996,12 @@
         <v>10396.40561819</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -990,12 +1013,12 @@
         <v>10050.3586120912</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1007,12 +1030,12 @@
         <v>10040.0307021154</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -1024,12 +1047,12 @@
         <v>10328.5537327765</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1041,12 +1064,12 @@
         <v>10468.1416395172</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -1058,34 +1081,34 @@
         <v>10264.3029488128</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B18">
         <v>7</v>
       </c>
       <c r="C18">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>9061.0964137012907</v>
+        <v>9085.0926528498003</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <f>SUM(C12:C18)</f>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D19" s="1">
         <f>SUM(D12:D18)</f>
-        <v>70608.889667204392</v>
+        <v>70632.885906352894</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1110,7 +1133,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1119,15 +1142,15 @@
         <v>24</v>
       </c>
       <c r="D22">
-        <v>10351.5409177809</v>
+        <v>10957.430299309</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1139,12 +1162,12 @@
         <v>10240.7485129782</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1156,12 +1179,12 @@
         <v>9758.4701712043206</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -1173,12 +1196,12 @@
         <v>10086.2297192444</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -1190,12 +1213,12 @@
         <v>10197.200793621199</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -1207,34 +1230,34 @@
         <v>10363.8770276912</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
       <c r="C28">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>11251.3270744867</v>
+      </c>
+      <c r="E28" t="s">
         <v>30</v>
-      </c>
-      <c r="D28">
-        <v>10746.090738475201</v>
-      </c>
-      <c r="E28" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <f>SUM(C22:C28)</f>
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D29" s="1">
         <f>SUM(D22:D28)</f>
-        <v>71744.157880995423</v>
+        <v>72855.283598535025</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1259,24 +1282,24 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D32">
-        <v>10029.895474594299</v>
+        <v>9235.6509451020502</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1288,12 +1311,12 @@
         <v>10424.143479610801</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -1305,15 +1328,15 @@
         <v>10113.149431297201</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>17</v>
@@ -1322,12 +1345,12 @@
         <v>10563.1611848091</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1339,12 +1362,12 @@
         <v>10263.725203550401</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B37">
         <v>6</v>
@@ -1356,34 +1379,34 @@
         <v>9995.7060506058697</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B38">
         <v>7</v>
       </c>
       <c r="C38">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D38">
-        <v>10492.952525106501</v>
+        <v>11497.060436850301</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C39" s="1">
         <f>SUM(C32:C38)</f>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D39" s="1">
         <f>SUM(D32:D38)</f>
-        <v>71882.733349574162</v>
+        <v>72092.596731825717</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1408,41 +1431,41 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D42">
-        <v>10267.3272148008</v>
+        <v>10452.5931274209</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D43">
-        <v>10176.9320304295</v>
+        <v>10318.328776959301</v>
       </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -1454,12 +1477,12 @@
         <v>10601.066552067599</v>
       </c>
       <c r="E44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -1471,12 +1494,12 @@
         <v>11162.543933425801</v>
       </c>
       <c r="E45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -1488,12 +1511,12 @@
         <v>10261.913579423001</v>
       </c>
       <c r="E46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B47">
         <v>6</v>
@@ -1505,34 +1528,34 @@
         <v>10124.1028846559</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B48">
         <v>7</v>
       </c>
       <c r="C48">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D48">
-        <v>9062.0794277297991</v>
+        <v>9088.4678875283807</v>
       </c>
       <c r="E48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" s="1">
         <f>SUM(C42:C48)</f>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D49" s="1">
         <f>SUM(D42:D48)</f>
-        <v>71655.9656225324</v>
+        <v>72009.016741480882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix allocation error in v4
</commit_message>
<xml_diff>
--- a/allthedocks_summary.xlsx
+++ b/allthedocks_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/Documents/AllTheDocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAAA2ED-3DD8-234E-A771-8A02E6803040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D013F15-3C00-0D48-86C1-C58400848785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E10AA2E9-4849-4F4A-ADC4-EA73F101CC61}"/>
   </bookViews>
@@ -296,10 +296,10 @@
     <t>LineString (529972.73623576539102942 178260.44271802250295877, 529964.88981587113812566 178280.53501518818666227, 529736.19874976435676217 178449.42485077629680745, 529726.6756163917016238 178435.93374516512267292, 529667.15603281301446259 178374.03337824330083095, 529656.83930499281268567 178336.73443920066347346, 529656.83930499281268567 178318.48176690321997739, 529533.1423543622950092 178277.09763705841032788, 529545.88164580159354955 178234.77457293338375166, 529539.13281372934579849 178232.66417939844541252, 529526.46756790520157665 178272.0813878343324177, 529356.46380653255619109 178218.4888664910395164, 529209.25203648116439581 178181.18992744840215892, 529201.3160920039517805 178196.26822195498971269, 529174.33388078166171908 178213.72729980474105105, 529241.78940883744508028 178304.19706684432458133, 529096.56162490556016564 178405.77715615194756538, 529162.42996406590100378 178370.85900045244488865, 529265.59724226896651089 178509.73802880270523019, 529271.94599785073660314 178518.86436495141242631, 529255.28051444864831865 178531.56187611486529931, 529137.43173896288499236 178622.82523760217009112, 528935.58502973488066345 178770.48393843130907044, 528983.97178611240815371 178746.69013198197353631, 529038.32024148688651621 178787.730140567116905, 529134.25736117199994624 178678.3768489422800485, 529196.10179991333279759 178713.44813071331009269, 529262.83282760996371508 178758.27597455237992108, 529270.770087662152946 178758.30559268582146615, 529304.71750739659182727 178689.86743865112657659, 529337.70783226401545107 178657.27980173568357714, 529305.00792290433309972 178707.29236911991029046, 529360.72793802665546536 178737.71750709970365278, 529376.25811279006302357 178760.55599939869716763, 529432.8975736916763708 178872.92138151006656699, 529475.57562967715784907 178964.59189934626920149, 529598.9311413198010996 178898.89408748364076018, 529619.5737125719897449 178946.00311593859805726, 529714.19555520184803754 179001.94307321662199683, 529732.04873305652290583 178984.08989536194712855, 529747.52148719725664705 178977.54373014855082147, 529762.83693021174985915 178665.01042368449270725, 529763.44848158198874444 178762.70334927615476772, 529919.02978800015989691 178775.15741814990178682, 529920.62251020059920847 178777.0686847903416492, 529987.35757039557211101 178779.61704031089902855, 529990.88010893994942307 178704.02897236388525926, 529998.77212355576921254 178671.29172655026195571, 530029.46329150593373924 178652.58472894251463003, 529978.11976480018347502 178549.04879146168241277, 530142.89766389573924243 178470.78303775115637109, 530203.92096228688023984 178608.72268030606210232, 530221.91308957664296031 178657.90116156474687159, 530245.90259262965992093 178752.65969862419296987, 530245.56836481753271073 178793.74637619103305042, 530233.2973599269753322 178979.3297097270260565, 530129.87610972102265805 178980.12443667955812998, 530137.44476192351430655 178887.1381381907267496, 530084.32904200174380094 178884.16473911114735529, 529987.01779939723201096 178875.51485087964101695, 529975.09426932758651674 178984.62321261296165176, 530051.34281733946409076 178985.6960422565753106, 530038.8975292646791786 179035.15677982414490543, 530124.44105861149728298 179029.82073120991117321, 530118.77150695887394249 179077.09478690157993697, 530081.58591817854903638 179074.76026563285267912, 530075.24936044914647937 179088.10038716840790585, 530074.58235437236726284 179121.36731524771312252, 530086.42171223519835621 179134.04043070648913272, 530113.10195530625060201 179137.12533381159300916, 530104.43087630812078714 179218.41669941885629669, 530137.16457231086678803 179220.90265564562287182, 530137.2566814114106819 179287.56575694994535297, 530164.29013196483720094 179289.33844223213964142, 530181.6477391414809972 179297.81860453309491277, 530152.236118592787534 179291.25757650277228095, 530123.93161658430472016 179290.37801461422350258, 530010.93885788007173687 179324.27584222549921833, 529997.12863181624561548 179285.35611422738293186, 529943.14320265757851303 179272.8013632602232974, 529935.82251096051186323 179312.1535707954026293, 529909.83655243786051869 179337.6092036338231992, 529899.811406908207573 179372.55586857470916584, 529796.77445525978691876 179363.87907264640671201, 529750.2085215135011822 179339.20018068622448482, 529724.22256299096625298 179373.14102447082404979, 529924.43567383696790785 179499.69993192006950267, 529928.14961813052650541 179531.89329112289124168, 529927.0135171840665862 179569.76332267106045038, 529922.25843279552645981 179593.81102334667230025, 529914.26865162816829979 179631.81709465332096443, 529926.90485368797089905 179695.04491854083607905, 530056.77231763186864555 179684.35815048823133111, 530089.18110335676465183 179679.01476646191440523, 530121.47372855921275914 179675.29762974794721231, 530319.06511298276018351 179662.03388815367361531, 530319.76053756836336106 179732.32005187700269744, 530373.61476240970660001 180193.22727265988942236, 530412.24257195775862783 180279.92940676314174198, 530386.72824432235211134 180288.27955035289051011, 530352.16792779811657965 180294.54215804519481026, 530318.67950793809723109 180304.44907694679568522, 530311.60276080551557243 180320.70320951391477138, 530416.13335239037405699 180292.3420881467172876, 530487.0496485095936805 180440.21010984203894623, 530547.21533590857870877 180548.09341138508170843, 530636.23792039870750159 180625.04513696124195121, 530645.83293890720233321 180632.72962594628916122, 530635.93489812139887363 180644.80407832888886333, 530627.51556253083981574 180643.39991334360092878, 530637.0487118421588093 180647.8021944590145722, 530646.00271280272863805 180635.27623437941656448, 530647.50414836022537202 180636.20670148546923883, 530685.17803919909056276 180659.55390144197735935, 530739.10712194757070392 180685.53381026530405506, 530871.2405794725054875 180748.77793378444039263, 530884.09205942158587277 180795.04326160132768564, 530994.61478698416613042 180838.09571943094488233, 530982.23648845416028053 180885.78941204195143655, 531002.32567495363764465 180840.66601542077842169, 531087.78801661543548107 180857.37293935465277173, 531104.77522879175376147 180851.00402391061652452, 531115.93421733961440623 180802.8298538378730882, 531377.42735681601334363 180810.11179436542443, 531392.01873411587439477 180833.06676275972859003, 531387.64204643457196653 180913.19381415750831366, 531467.76909783226437867 180913.19381415750831366, 531465.94281411881092936 180989.74318283077445813, 531389.47650842147413641 180987.01224334159633145, 531387.55785732087679207 181129.37252376566175371, 531386.90621243161149323 181168.05746712500695139, 531290.5201128131011501 181159.06143116063321941, 531142.08551940054167062 181108.94065935898106545, 531043.74918007606174797 181071.66004718522890471, 530997.40789101168047637 181015.41131011385004967, 530934.34037396765779704 180999.47809187293751165, 530896.0915352045558393 180978.78303439042065293, 530860.84877428377512842 180964.44244112810702063, 530839.77010409883223474 180962.68588527935207821, 530823.96110146003775299 180993.71837194060208276, 530827.47421315754763782 181054.02678941437625326, 530740.23193933628499508 181041.73089847312076017, 530692.21941280376631767 181014.7970421256031841, 530549.35287043871358037 181094.42757393565261737, 530472.93963134801015258 180978.161691593733849, 530513.05071623111143708 180924.627175223082304, 530505.35225721553433686 180900.45491703250445426, 530526.51764440489932895 180907.64713535181363113, 530581.55639433243777603 180875.44361145806033164)</t>
   </si>
   <si>
-    <t>LineString (528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526810.75304763286840171 179467.00080663594417274, 526668.71815055573824793 179454.61404235597001389, 526444.82263462664559484 179424.7408409794443287, 526441.88616490841377527 179401.24908323338604532, 526400.95936604985035956 179579.61037377678439952, 526395.80753890855703503 179617.60509894342976622, 526400.31538765714503825 179630.4846667965175584, 526396.45151730126235634 179663.00557562557514757, 526429.93839371926151216 179670.41132714110426605, 526431.87032889726106077 179659.14170526966336183, 526400.31538765714503825 179655.59982411004602909, 526404.17925801302772015 179629.51869920754688792, 526481.13467593537643552 179644.97418063125223853, 526512.36762797913979739 179646.26213741654646583, 526515.90950913866981864 179639.17837509737000801, 526505.28386565984692425 179635.63649393775267527, 526386.30885761685203761 179621.30797470119432546, 526318.94980677636340261 179621.48525741521734744, 526215.34960218577180058 179626.84875574553734623, 526121.02660867478698492 179655.6876124200061895, 526113.32453510130289942 179686.26937513795564882, 526116.04291400965303183 179658.17945975257316604, 526072.0957883259980008 179674.03667005078750663, 526077.53254614258185029 179626.23850758047774434, 526092.24883591232355684 179409.14943758773733862, 526170.58646800776477903 179414.55203290464123711, 526170.91200886678416282 179254.77395809174049646, 526170.02756560104899108 179226.2506627686379943, 526170.69089805032126606 179197.28514581263880245, 526191.0330931645585224 179103.75527045089984313, 526208.50084766466170549 179068.1564290011592675, 526190.95479760388843715 179087.37647593740257435, 526152.42256449558772147 179079.67002931574825197, 526079.61222019151318818 179075.18120090151205659, 525857.43331313808448613 179086.440267137310002, 525822.15490559919271618 179081.18603622727096081, 525774.11622299312148243 179039.15218894690042362, 525789.9340731572592631 179008.44695039271027781, 525608.18420976598281413 178985.48173996026162058, 525584.06940557796042413 178987.97679135657381266, 525573.85263970901723951 179052.99129645497305319, 525566.40184021822642535 179179.43401284626452252, 525539.12785214162431657 179262.48159250925527886, 525230.67203460761811584 179148.19059485456091352, 525218.00911157194059342 179136.66408798881457187, 525275.51739498809911311 178989.94413040805375203, 525288.82619905064348131 178973.64458385962643661, 525321.71609151223674417 178916.64969141795882024, 525110.25522415374871343 178791.72511747083626688, 525140.83571881789248437 178743.57710459540248848, 525170.6157625982305035 178737.53536503901705146, 525136.90032081049866974 178734.29459415673045442, 525073.96749363793060184 178845.07109110968303867, 525050.22967286221683025 178837.15848418447421864, 524920.68373622617218643 178769.44129003383568488, 524812.24932546948548406 178896.28909129649400711, 524699.21156708616763353 179025.31069560500327498, 524681.6391244096448645 179051.25509521568892524, 524679.63010795961599797 179077.09913740976480767, 524788.97600055101793259 179149.0372246410115622, 524957.31112467218190432 179248.31178502010880038, 524889.31033757049590349 179366.96949636968201958, 524837.84125263791065663 179392.39398410747526214, 524751.64603811223059893 179345.88577483102562837, 524614.60184811090584844 179570.98550772908492945, 524703.84473427385091782 179436.35361285935505293, 524844.32857223774772137 179505.77558726171264425, 524810.43752961605787277 179598.63431089642108418, 524822.46338344959076494 179627.87900090057519265, 524845.42183167708572 179640.99811417344608344, 524954.20114589820150286 179688.82821464753942564, 524980.43937244394328445 179689.64815922707202844, 525145.27674076042603701 179339.90930881092208438, 525213.61852516769431531 179374.56420798628823832, 525206.26161919755395502 179390.0524310814216733, 525222.23384926444850862 179385.21236136413062923, 525351.1733065313892439 179466.91273819096386433, 525352.72212884086184204 179482.01375570870004594, 525369.8851592862047255 179479.95885097398422658, 525422.48737169418018311 179507.45546200548415072, 525366.53774576925206929 179596.40102116821799427, 525283.64405398862436414 179742.1564941595424898, 525384.085012789350003 179740.24697022794862278, 525418.45644355763215572 179681.43363313551526517, 525419.82130964624229819 179656.85948007801198401)</t>
-  </si>
-  <si>
-    <t>LineString (525327.85414873412810266 178420.77501689142081887, 525435.54454665677621961 178546.54447064295527525, 525345.92272875038906932 178653.20884751385892741, 525429.15519386087544262 178703.14832658017985523, 525460.07010947330854833 178656.1814355535316281, 525501.7821286671096459 178615.87244897283380851, 525558.91436985018663108 178563.64555782591924071, 525601.34650842915289104 178515.0539152596029453, 525591.59441469295416027 178508.14618219647672959, 525612.31761388236191124 178515.8665897376195062, 525739.09483245271258056 178641.42479659095988609, 525767.53843918326310813 178664.58601921438821591, 525708.21320228814147413 178737.72672223576228134, 525731.62045715074054897 178716.68428954426781274, 525769.37393091234844178 178666.83504263576469384, 525806.39432751352433115 178612.95387134497286752, 526026.40911028429400176 178722.27400289245997556, 526144.43453311175107956 178765.52555535719147883, 526097.8322964139515534 178902.16469051572494209, 526093.05398678814526647 178927.64900852003484033, 526073.41744379187002778 178941.35436849229154177, 526098.01514758018311113 178929.59024928920553066, 526150.06246284244116396 178767.20975544024258852, 526255.77580733434297144 178814.4714835460181348, 526271.20979337661992759 178817.35269416749360971, 526312.78246261400636286 178730.88154215391841717, 526431.85428454133216292 178507.28957353180157952, 526371.81847308482974768 178458.83962042655912228, 526552.97916730435099453 178570.48516453863703646, 526555.08568700461182743 178631.57423584524076432, 526531.73185393039602786 178797.25923736946424469, 526501.3099303717026487 178977.1575194436009042, 526543.68378180800937116 178800.00690841992036439, 526578.25740370713174343 178795.88277246299549006, 526808.88298217917326838 178842.85059796637506224, 526867.58985495707020164 178857.72481234182487242, 526887.47400313417892903 178869.08718272874830291, 526862.61881791288033128 179084.26207193068694323, 526876.82178089639637619 179026.0299236977880355, 526893.15518832765519619 179011.11681256498559378, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527768.86287219019141048 179171.7344985579547938, 527738.35830124607309699 179152.01631094136973843, 527772.52151037787552923 179165.95770141950924881, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528513.98412839835509658 179812.26687349064741284, 528529.45710146625060588 179823.30889789306093007, 528522.1132692665560171 179877.67606056467047893, 528516.61473636329174042 179896.37107243580976501, 528982.89032656128983945 180285.39227534280507825, 528985.75060231669340283 180264.89964467784739099, 528997.18651210982352495 180296.38934114936273545, 529128.14837153907865286 180399.20853238902054727, 529260.66181104525458068 180474.31033623719122261, 529390.66158775170333683 180271.80423245803103782, 529460.4421130547998473 180310.72029464627848938, 529430.42441646789666265 180361.7129266606643796, 529518.94092159741558135 180419.07557802950032055, 529552.56730343436356634 180373.58106142663746141, 529648.71743816568050534 180427.49491339456290007, 529608.480220987345092 180501.82199512678198516, 529569.44679091090802103 180572.25595415246789344, 529667.74284364131744951 180629.72475247565307654, 529730.9295924516627565 180529.48919386579655111, 529787.31384936452377588 180567.2724588074197527, 529763.12702995492145419 180622.33490404754411429, 529706.82561028259806335 180576.71049719117581844, 529752.5037739867111668 180495.92673939117230475, 529740.29997511499095708 180487.27313655486796051, 529754.05698475218378007 180486.60747479822020978, 529800.36167021188884974 180412.51190174778457731, 529824.728592021856457 180415.94968910259194672, 529890.00781108462251723 180459.31649564448161982, 529865.28168949380051345 180503.69017882505431771, 529855.61934717127587646 180535.74483229906763881, 529894.55648332042619586 180548.55958596843993291, 529890.50570647965651006 180564.17520972224883735, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530054.15927445457782596 180611.80309442835277878, 530069.85973392939195037 180508.62456558644771576, 530160.12516808835789561 180516.73132610463653691, 530168.55684169579762965 180494.19840525725157931, 530148.45289235515519977 180461.23712512332713231, 530174.04404229309875518 180496.50880550872534513, 530161.336840910022147 180527.69920890356297605, 530154.59773694002069533 180615.4214020338258706, 530232.82974896696396172 180614.62270036846166477, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530441.01278525067027658 180758.81861569813918322, 530400.55581117747351527 180811.16401171206962317, 530524.57064777321647853 180911.87319211009889841, 530583.04193836136255413 180879.49776674556778744)</t>
+    <t>LineString (525327.85414873412810266 178420.77501689142081887, 525435.54454665677621961 178546.54447064295527525, 525345.92272875038906932 178653.20884751385892741, 525429.15519386087544262 178703.14832658017985523, 525460.07010947330854833 178656.1814355535316281, 525501.7821286671096459 178615.87244897283380851, 525558.91436985018663108 178563.64555782591924071, 525601.34650842915289104 178515.0539152596029453, 525591.59441469295416027 178508.14618219647672959, 525612.31761388236191124 178515.8665897376195062, 525739.09483245271258056 178641.42479659095988609, 525767.53843918326310813 178664.58601921438821591, 525708.21320228814147413 178737.72672223576228134, 525731.62045715074054897 178716.68428954426781274, 525769.37393091234844178 178666.83504263576469384, 525806.39432751352433115 178612.95387134497286752, 526026.40911028429400176 178722.27400289245997556, 526144.43453311175107956 178765.52555535719147883, 526150.06246284244116396 178767.20975544024258852, 526255.77580733434297144 178814.4714835460181348, 526271.20979337661992759 178817.35269416749360971, 526312.78246261400636286 178730.88154215391841717, 526431.85428454133216292 178507.28957353180157952, 526371.81847308482974768 178458.83962042655912228, 526552.97916730435099453 178570.48516453863703646, 526555.08568700461182743 178631.57423584524076432, 526531.73185393039602786 178797.25923736946424469, 526501.3099303717026487 178977.1575194436009042, 526543.68378180800937116 178800.00690841992036439, 526578.25740370713174343 178795.88277246299549006, 526808.88298217917326838 178842.85059796637506224, 526867.58985495707020164 178857.72481234182487242, 526887.47400313417892903 178869.08718272874830291, 526862.61881791288033128 179084.26207193068694323, 526876.82178089639637619 179026.0299236977880355, 526893.15518832765519619 179011.11681256498559378, 526922.56527758203446865 179021.44788825331488624, 526976.82480131415650249 179026.93843529763398692, 527126.68443828821182251 179083.05505582402111031, 527206.78183046414051205 179136.0226861338596791, 527205.48993704188615084 179152.81730062235146761, 527216.03914421703666449 179145.72578124998835847, 527240.65396095986943692 179168.27212599763879552, 527356.07469829195179045 179281.62439133448060602, 527415.23299735458567739 179328.3718584259331692, 527437.15880050358828157 179344.91963438750826754, 527437.57249490264803171 179363.53588234429480508, 527448.74728261982090771 179356.647314573492622, 527504.23852299549616873 179398.66757797525497153, 527585.06438483926467597 179335.59891305171186104, 527665.89024668303318322 179312.33086191487382166, 527724.67269166023470461 179303.14610488718608394, 527769.37184252834413201 179306.82000769826117903, 527780.39355096162762493 179281.10268802070640959, 527792.02757653000298887 179222.32024304344668053, 527763.24867117661051452 179195.99060623071272857, 527768.86287219019141048 179171.7344985579547938, 527738.35830124607309699 179152.01631094136973843, 527772.52151037787552923 179165.95770141950924881, 527886.39517858054023236 179195.27266738505568355, 527822.45171340426895767 179520.46795567701337859, 527858.1322810254059732 179530.35083859681617469, 527891.88773283653426915 179539.25118037080392241, 527870.7807220573304221 179648.64833412505686283, 527868.61700371222104877 179658.18725142459152266, 527860.88046702521387488 179707.83289611263899133, 527871.11952563317026943 179673.40761047863634303, 527874.78819991135969758 179657.57498131820466369, 527913.67431851325090975 179664.11720327276270837, 527912.70541233289986849 179757.62383855623193085, 527908.07293678901623935 179798.69010824267752469, 527909.8863292447058484 179817.68885372436488979, 527912.46024989418219775 179831.26684675173601136, 527920.7886318500386551 179757.18808093448751606, 528047.62872848019469529 179774.55966792465187609, 528127.87066305975895375 179815.19500658992910758, 528096.22333193966187537 179801.94153121206909418, 528121.1935451285680756 179822.46549322339706123, 528115.72619099263101816 179848.85401823552092537, 528228.20267733931541443 179870.84723329346161336, 528232.45957181649282575 179854.12167384184431285, 528255.63412408879958093 179859.83663536846870556, 528233.04146977188065648 179858.24069136375328526, 528229.61167071235831827 179870.97432596748694777, 528256.6169783161021769 179876.28377280529821292, 528294.42466580052860081 179904.86705374554730952, 528301.72961289319209754 179899.58161686407402158, 528306.33070521731860936 179893.07007217648788355, 528319.42971817124634981 179870.80175015470013022, 528331.87378047755919397 179834.77946453119511716, 528377.07891597924754024 179802.95061608715332113, 528464.50208342960104346 179798.41427575697889552, 528500.39834169461391866 179812.81222550064558163, 528513.98412839835509658 179812.26687349064741284, 528529.45710146625060588 179823.30889789306093007, 528522.1132692665560171 179877.67606056467047893, 528516.61473636329174042 179896.37107243580976501, 528982.89032656128983945 180285.39227534280507825, 528985.75060231669340283 180264.89964467784739099, 528997.18651210982352495 180296.38934114936273545, 529128.14837153907865286 180399.20853238902054727, 529260.66181104525458068 180474.31033623719122261, 529390.66158775170333683 180271.80423245803103782, 529460.4421130547998473 180310.72029464627848938, 529430.42441646789666265 180361.7129266606643796, 529518.94092159741558135 180419.07557802950032055, 529552.56730343436356634 180373.58106142663746141, 529648.71743816568050534 180427.49491339456290007, 529608.480220987345092 180501.82199512678198516, 529569.44679091090802103 180572.25595415246789344, 529667.74284364131744951 180629.72475247565307654, 529730.9295924516627565 180529.48919386579655111, 529787.31384936452377588 180567.2724588074197527, 529763.12702995492145419 180622.33490404754411429, 529706.82561028259806335 180576.71049719117581844, 529752.5037739867111668 180495.92673939117230475, 529740.29997511499095708 180487.27313655486796051, 529754.05698475218378007 180486.60747479822020978, 529800.36167021188884974 180412.51190174778457731, 529824.728592021856457 180415.94968910259194672, 529890.00781108462251723 180459.31649564448161982, 529865.28168949380051345 180503.69017882505431771, 529855.61934717127587646 180535.74483229906763881, 529894.55648332042619586 180548.55958596843993291, 529890.50570647965651006 180564.17520972224883735, 529872.95531774952542037 180606.76134864933555946, 529915.37259634933434427 180613.59366198081988841, 529972.59322050062473863 180618.71789697947679088, 529975.86554363591130823 180653.11958405951736495, 529993.10341755871195346 180649.76780548423994333, 530003.82197457575239241 180653.6264860104129184, 530054.15927445457782596 180611.80309442835277878, 530069.85973392939195037 180508.62456558644771576, 530160.12516808835789561 180516.73132610463653691, 530168.55684169579762965 180494.19840525725157931, 530148.45289235515519977 180461.23712512332713231, 530174.04404229309875518 180496.50880550872534513, 530161.336840910022147 180527.69920890356297605, 530154.59773694002069533 180615.4214020338258706, 530232.82974896696396172 180614.62270036846166477, 530270.34142313164193183 180619.80239770526532084, 530278.97677504969760776 180605.4567557742993813, 530319.42912215983960778 180633.89190510252956301, 530452.98087174398824573 180736.21395450358977541, 530441.01278525067027658 180758.81861569813918322, 530400.55581117747351527 180811.16401171206962317, 530524.57064777321647853 180911.87319211009889841, 530583.04193836136255413 180879.49776674556778744)</t>
+  </si>
+  <si>
+    <t>LineString (528079.47067953646183014 180632.24651449063094333, 528074.47738231881521642 180628.91345400654245168, 528024.52704086224548519 180609.87107211141847074, 528002.13440979458391666 180610.44380836229538545, 527990.64072253345511854 180618.42097470845328644, 527972.56485775776673108 180621.4870105440786574, 527925.40382085286546499 180703.35145196394296363, 527902.95878737303428352 180701.55584928556345403, 527887.69616460683755577 180736.57010151402209885, 527757.73942075879313052 180828.59473878113203682, 527713.74715513840783387 180842.06175886897835881, 527632.04723327199462801 180837.57275217302958481, 527614.09120648819953203 180851.93757360009476542, 527504.55944310687482357 180858.22218297442304902, 527341.38404970872215927 180835.77714949465007521, 527227.36327963136136532 180809.74091065808897838, 527043.76290576683823019 180770.23765173368155956, 526939.61795042059384286 180763.05524102016352117, 526905.50149953132495284 180726.24538611332536675, 526911.78610890568234026 180702.90255129433353432, 526979.12120934505946934 180662.5014910307363607, 527036.5804950533201918 180622.10043076713918708, 527055.43432317627593875 180555.66313166698091663, 527077.87935665610712022 180308.3188627198105678, 527073.39034996007103473 180283.85377622683881782, 527108.40460218861699104 180190.48243695095879957, 527076.98155531683005393 180196.76704632528708316, 527017.72666693024802953 180212.92747043073177338, 526981.81461336265783757 180219.21207980506005697, 526955.77837452606763691 180225.49668917941744439, 526942.31135443819221109 180205.74505971721373498, 526901.91029417456593364 180116.8627271372533869, 526897.6457378133200109 180099.3556010230386164, 526888.66772442148067057 180050.87432870670454577, 526893.15673111740034074 180035.61170594047871418, 526880.58751236868556589 180035.61170594047871418, 526824.02602799970190972 179903.63490907935192809, 526802.70324619382154197 179852.90913341505802236, 526794.6230341411428526 179796.34764904601615854, 526794.26693146175239235 179743.8655021067825146, 526793.01302744331769645 179731.11747791964444332, 526790.71420340961776674 179729.23662189205060713, 526799.15176595037337393 179665.74589264905080199, 526810.75304763286840171 179467.00080663594417274, 526668.71815055573824793 179454.61404235597001389, 526444.82263462664559484 179424.7408409794443287, 526441.88616490841377527 179401.24908323338604532, 526400.95936604985035956 179579.61037377678439952, 526395.80753890855703503 179617.60509894342976622, 526400.31538765714503825 179630.4846667965175584, 526396.45151730126235634 179663.00557562557514757, 526429.93839371926151216 179670.41132714110426605, 526431.87032889726106077 179659.14170526966336183, 526400.31538765714503825 179655.59982411004602909, 526404.17925801302772015 179629.51869920754688792, 526481.13467593537643552 179644.97418063125223853, 526512.36762797913979739 179646.26213741654646583, 526515.90950913866981864 179639.17837509737000801, 526505.28386565984692425 179635.63649393775267527, 526386.30885761685203761 179621.30797470119432546, 526318.94980677636340261 179621.48525741521734744, 526215.34960218577180058 179626.84875574553734623, 526121.02660867478698492 179655.6876124200061895, 526113.32453510130289942 179686.26937513795564882, 526116.04291400965303183 179658.17945975257316604, 526072.0957883259980008 179674.03667005078750663, 526077.53254614258185029 179626.23850758047774434, 526092.24883591232355684 179409.14943758773733862, 526170.58646800776477903 179414.55203290464123711, 526170.91200886678416282 179254.77395809174049646, 526170.02756560104899108 179226.2506627686379943, 526170.69089805032126606 179197.28514581263880245, 526191.0330931645585224 179103.75527045089984313, 526208.50084766466170549 179068.1564290011592675, 526211.74739217478781939 179033.83077586514991708, 526212.5073481819126755 179000.39271154996822588, 526093.19425505725666881 178993.55310748549527489, 526096.23407908587250859 178919.83737479062983766, 526071.91548685671295971 178938.07631896255770698, 526089.39447502139955759 178936.55640694824978709, 526074.95531088532879949 179075.628356259141583, 525857.43331313808448613 179086.440267137310002, 525822.15490559919271618 179081.18603622727096081, 525774.11622299312148243 179039.15218894690042362, 525789.9340731572592631 179008.44695039271027781, 525608.18420976598281413 178985.48173996026162058, 525584.06940557796042413 178987.97679135657381266, 525573.85263970901723951 179052.99129645497305319, 525566.40184021822642535 179179.43401284626452252, 525539.12785214162431657 179262.48159250925527886, 525230.67203460761811584 179148.19059485456091352, 525218.00911157194059342 179136.66408798881457187, 525275.51739498809911311 178989.94413040805375203, 525288.82619905064348131 178973.64458385962643661, 525321.71609151223674417 178916.64969141795882024, 525110.25522415374871343 178791.72511747083626688, 525140.83571881789248437 178743.57710459540248848, 525170.6157625982305035 178737.53536503901705146, 525136.90032081049866974 178734.29459415673045442, 525073.96749363793060184 178845.07109110968303867, 525050.22967286221683025 178837.15848418447421864, 524920.68373622617218643 178769.44129003383568488, 524812.24932546948548406 178896.28909129649400711, 524699.21156708616763353 179025.31069560500327498, 524681.6391244096448645 179051.25509521568892524, 524679.63010795961599797 179077.09913740976480767, 524788.97600055101793259 179149.0372246410115622, 524957.31112467218190432 179248.31178502010880038, 524889.31033757049590349 179366.96949636968201958, 524837.84125263791065663 179392.39398410747526214, 524751.64603811223059893 179345.88577483102562837, 524614.60184811090584844 179570.98550772908492945, 524703.84473427385091782 179436.35361285935505293, 524844.32857223774772137 179505.77558726171264425, 524810.43752961605787277 179598.63431089642108418, 524822.46338344959076494 179627.87900090057519265, 524845.42183167708572 179640.99811417344608344, 524954.20114589820150286 179688.82821464753942564, 524980.43937244394328445 179689.64815922707202844, 525145.27674076042603701 179339.90930881092208438, 525213.61852516769431531 179374.56420798628823832, 525206.26161919755395502 179390.0524310814216733, 525222.23384926444850862 179385.21236136413062923, 525351.1733065313892439 179466.91273819096386433, 525352.72212884086184204 179482.01375570870004594, 525369.8851592862047255 179479.95885097398422658, 525422.48737169418018311 179507.45546200548415072, 525366.53774576925206929 179596.40102116821799427, 525283.64405398862436414 179742.1564941595424898, 525384.085012789350003 179740.24697022794862278, 525418.45644355763215572 179681.43363313551526517, 525419.82130964624229819 179656.85948007801198401)</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,7 +809,7 @@
         <v>71.7</v>
       </c>
       <c r="N4" s="2">
-        <v>72.900000000000006</v>
+        <v>72.5</v>
       </c>
       <c r="O4" s="1"/>
     </row>
@@ -880,7 +880,7 @@
         <v>71.7</v>
       </c>
       <c r="N6" s="2">
-        <v>72</v>
+        <v>72.3</v>
       </c>
       <c r="O6" s="1"/>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="N7">
         <f>AVERAGE(N2:N6)</f>
-        <v>71.94</v>
+        <v>71.919999999999987</v>
       </c>
       <c r="O7" s="1"/>
     </row>
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <v>10957.430299309</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28">
         <v>7</v>
@@ -1244,7 +1244,7 @@
         <v>32</v>
       </c>
       <c r="D28">
-        <v>11251.3270744867</v>
+        <v>10865.1751107169</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
@@ -1253,11 +1253,11 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <f>SUM(C22:C28)</f>
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" s="1">
         <f>SUM(D22:D28)</f>
-        <v>72855.283598535025</v>
+        <v>72469.131634765217</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1448,7 +1448,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1457,7 +1457,7 @@
         <v>25</v>
       </c>
       <c r="D43">
-        <v>10318.328776959301</v>
+        <v>10624.362508620899</v>
       </c>
       <c r="E43" t="s">
         <v>14</v>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D49" s="1">
         <f>SUM(D42:D48)</f>
-        <v>72009.016741480882</v>
+        <v>72315.050473142488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>